<commit_message>
28-Mar update (afternoon).  second update this evening
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B31BA94-4A4D-4522-B07E-98EF5B16CA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761A474C-B7A8-48E5-9BAE-5F86DDCB2E1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="27580" windowHeight="18000" tabRatio="685" activeTab="2" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
@@ -977,6 +977,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -995,8 +997,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1076,20 +1076,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47040D2C-B674-4C13-B6A3-34550FE96788}" name="dc" displayName="dc" ref="A1:CC5" totalsRowShown="0">
   <tableColumns count="81">
-    <tableColumn id="1" xr3:uid="{F7478CC8-05B3-43D3-A09E-A8CEC61508DC}" name="county" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{9F45BE28-05B7-422A-8E27-AA668258DF2E}" name="13-Mar" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{70A42E3E-AE1F-46EB-A473-4805986C1877}" name="14-Mar" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{E4737ADD-3E45-4AA8-A64F-0FE7CC869F0C}" name="15-Mar" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{C51A330C-2EAB-46EC-BF00-15CE343CCC9C}" name="16-Mar" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{6466DD8B-376E-45C8-88A2-BB70EB18C860}" name="17-Mar" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{A61C2E41-B744-4260-AA58-884D297C0997}" name="18-Mar" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{4CE3538A-8700-42B0-AF14-F16C83EE94BE}" name="19-Mar" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{D95DFEEA-CC3B-445F-87E0-FDAED4CFE20C}" name="20-Mar" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{BAA204A8-8ECE-468D-8B1D-CF29521BACD0}" name="21-Mar" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{951F0F95-00D8-483E-B217-8A463F80FEC0}" name="22-Mar" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{7C87B399-1E66-409E-875F-B104E1CE9E28}" name="23-Mar" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{0465D902-6D4E-468B-BEBE-1001F5CA5012}" name="24-Mar" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{21FCED83-89D6-40D0-9A78-518D6EFA4A18}" name="25-Mar" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{F7478CC8-05B3-43D3-A09E-A8CEC61508DC}" name="county" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{9F45BE28-05B7-422A-8E27-AA668258DF2E}" name="13-Mar" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{70A42E3E-AE1F-46EB-A473-4805986C1877}" name="14-Mar" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{E4737ADD-3E45-4AA8-A64F-0FE7CC869F0C}" name="15-Mar" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{C51A330C-2EAB-46EC-BF00-15CE343CCC9C}" name="16-Mar" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{6466DD8B-376E-45C8-88A2-BB70EB18C860}" name="17-Mar" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{A61C2E41-B744-4260-AA58-884D297C0997}" name="18-Mar" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{4CE3538A-8700-42B0-AF14-F16C83EE94BE}" name="19-Mar" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{D95DFEEA-CC3B-445F-87E0-FDAED4CFE20C}" name="20-Mar" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{BAA204A8-8ECE-468D-8B1D-CF29521BACD0}" name="21-Mar" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{951F0F95-00D8-483E-B217-8A463F80FEC0}" name="22-Mar" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{7C87B399-1E66-409E-875F-B104E1CE9E28}" name="23-Mar" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{0465D902-6D4E-468B-BEBE-1001F5CA5012}" name="24-Mar" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{21FCED83-89D6-40D0-9A78-518D6EFA4A18}" name="25-Mar" dataDxfId="5"/>
     <tableColumn id="67" xr3:uid="{56DC555E-518D-4235-BFD8-B8A8584EE11B}" name="26-Mar"/>
     <tableColumn id="68" xr3:uid="{B11B3509-C4D2-46EC-A429-0E887C921D54}" name="27-Mar"/>
     <tableColumn id="69" xr3:uid="{9A961F00-B3A3-490E-8480-8C22A4C7B5A9}" name="28-Mar"/>
@@ -1165,7 +1165,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{361921CA-3BCD-45E1-86C6-B187D95BF47D}" name="md" displayName="md" ref="A1:BP23" totalsRowShown="0">
   <tableColumns count="68">
-    <tableColumn id="1" xr3:uid="{068940A6-6829-484A-96AE-69D1D863098A}" name="county" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{068940A6-6829-484A-96AE-69D1D863098A}" name="county" dataDxfId="4"/>
     <tableColumn id="67" xr3:uid="{99D470F9-8EA1-4C62-91AE-00248DC05752}" name="26-Mar"/>
     <tableColumn id="68" xr3:uid="{2DA0F8D9-8B7F-4D19-A9B4-B6D2050FDE03}" name="27-Mar"/>
     <tableColumn id="69" xr3:uid="{252EC233-C118-46A1-94B6-EA5E71871C0C}" name="28-Mar"/>
@@ -1241,11 +1241,11 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6A2AD35F-60C9-437C-AA7B-C217E8DC7927}" name="va" displayName="va" ref="B1:BT134" totalsRowShown="0">
   <tableColumns count="71">
-    <tableColumn id="54" xr3:uid="{F1106E80-B529-4637-9194-7C9771A7B601}" name="Locality" dataDxfId="17"/>
-    <tableColumn id="1" xr3:uid="{179FB13D-5548-4710-AF18-46935F888BFD}" name="idx" dataDxfId="0"/>
+    <tableColumn id="54" xr3:uid="{F1106E80-B529-4637-9194-7C9771A7B601}" name="Locality" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{179FB13D-5548-4710-AF18-46935F888BFD}" name="idx" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{C0D66142-D221-4FA3-A5FB-E99400CCE2A8}" name="FIPS"/>
-    <tableColumn id="5" xr3:uid="{8F6126EE-1EBF-49BF-BDC7-699B4ED90A6F}" name="25-Mar" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{AE396216-533F-4C0B-B4EC-F4652803C9BC}" name="26-Mar" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{8F6126EE-1EBF-49BF-BDC7-699B4ED90A6F}" name="25-Mar" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{AE396216-533F-4C0B-B4EC-F4652803C9BC}" name="26-Mar" dataDxfId="0"/>
     <tableColumn id="30" xr3:uid="{EB534D48-6A11-43DB-B9A0-4420A0A688CF}" name="27-Mar"/>
     <tableColumn id="31" xr3:uid="{BFD96346-A4D2-42DF-B1D4-777D3555AEDC}" name="28-Mar"/>
     <tableColumn id="32" xr3:uid="{02DCCD2B-3EDF-4C63-B217-1513E5D52F49}" name="29-Mar"/>
@@ -1873,50 +1873,50 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:81" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="12">
         <v>69</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="12">
         <v>115</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="12">
         <v>120</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="12">
         <v>126</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="12">
         <v>170</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="12">
         <v>203</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="12">
         <v>573</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="12">
         <v>1055</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="12">
         <v>1229</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="12">
         <v>1344</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="12">
         <v>1609</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="12">
         <v>1858</v>
       </c>
-      <c r="O2" s="18">
+      <c r="O2" s="12">
         <v>2166</v>
       </c>
-      <c r="P2" s="18">
+      <c r="P2" s="12">
         <v>2516</v>
       </c>
     </row>
@@ -2161,7 +2161,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B685ED27-8882-4CE7-837C-253FB4ACFF90}">
   <dimension ref="A1:BP29"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2385,6 +2387,9 @@
       <c r="C2" s="10">
         <v>63</v>
       </c>
+      <c r="D2">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -2396,6 +2401,9 @@
       <c r="C3" s="10">
         <v>88</v>
       </c>
+      <c r="D3">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -2407,6 +2415,9 @@
       <c r="C4" s="10">
         <v>103</v>
       </c>
+      <c r="D4">
+        <v>141</v>
+      </c>
     </row>
     <row r="5" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -2418,6 +2429,9 @@
       <c r="C5" s="10">
         <v>9</v>
       </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -2429,6 +2443,9 @@
       <c r="C6" s="10">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -2440,6 +2457,9 @@
       <c r="C7" s="10">
         <v>9</v>
       </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -2451,6 +2471,9 @@
       <c r="C8" s="10">
         <v>9</v>
       </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -2462,6 +2485,9 @@
       <c r="C9" s="10">
         <v>17</v>
       </c>
+      <c r="D9">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -2473,6 +2499,9 @@
       <c r="C10" s="10">
         <v>15</v>
       </c>
+      <c r="D10">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -2484,6 +2513,9 @@
       <c r="C11" s="10">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -2495,6 +2527,9 @@
       <c r="C12" s="10">
         <v>18</v>
       </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -2506,6 +2541,9 @@
       <c r="C13" s="10">
         <v>62</v>
       </c>
+      <c r="D13">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -2517,6 +2555,9 @@
       <c r="C14" s="10">
         <v>2</v>
       </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -2528,6 +2569,9 @@
       <c r="C15" s="10">
         <v>208</v>
       </c>
+      <c r="D15">
+        <v>255</v>
+      </c>
     </row>
     <row r="16" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -2539,6 +2583,9 @@
       <c r="C16" s="10">
         <v>148</v>
       </c>
+      <c r="D16">
+        <v>196</v>
+      </c>
     </row>
     <row r="17" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -2550,6 +2597,9 @@
       <c r="C17" s="10">
         <v>1</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
@@ -2561,6 +2611,9 @@
       <c r="C18" s="10">
         <v>4</v>
       </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -2572,6 +2625,9 @@
       <c r="C19" s="10">
         <v>1</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
@@ -2583,6 +2639,9 @@
       <c r="C20" s="10">
         <v>1</v>
       </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -2594,6 +2653,9 @@
       <c r="C21" s="10">
         <v>5</v>
       </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -2605,6 +2667,9 @@
       <c r="C22" s="10">
         <v>5</v>
       </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -2616,6 +2681,9 @@
       <c r="C23" s="10">
         <v>2</v>
       </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -2626,10 +2694,11 @@
         <v>580</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <f>SUM(md[27-Mar])</f>
+        <v>774</v>
       </c>
       <c r="D25" s="10">
-        <v>0</v>
+        <v>992</v>
       </c>
       <c r="E25" s="10">
         <v>0</v>
@@ -2835,7 +2904,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>0</v>
+        <v>226</v>
       </c>
       <c r="E26" s="10">
         <v>0</v>
@@ -3038,10 +3107,10 @@
         <v>4</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D27" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E27" s="10">
         <v>0</v>
@@ -3309,7 +3378,7 @@
   <dimension ref="A1:BU141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M97" sqref="M97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3562,12 +3631,15 @@
       <c r="G2" s="10">
         <v>18</v>
       </c>
+      <c r="H2" s="10">
+        <v>20</v>
+      </c>
       <c r="BU2" s="2">
         <v>43915</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3588,12 +3660,15 @@
       <c r="G3" s="10">
         <v>0</v>
       </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
       <c r="BU3" s="2">
         <v>43916</v>
       </c>
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
         <v>97</v>
       </c>
@@ -3612,12 +3687,15 @@
       <c r="G4" s="10">
         <v>1</v>
       </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
       <c r="BU4" s="2">
         <v>43917</v>
       </c>
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
         <v>98</v>
       </c>
@@ -3636,12 +3714,15 @@
       <c r="G5" s="10">
         <v>0</v>
       </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
       <c r="BU5" s="2">
         <v>43918</v>
       </c>
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1" t="s">
         <v>122</v>
       </c>
@@ -3660,12 +3741,15 @@
       <c r="G6" s="10">
         <v>1</v>
       </c>
+      <c r="H6" s="10">
+        <v>2</v>
+      </c>
       <c r="BU6" s="2">
         <v>43919</v>
       </c>
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="1" t="s">
         <v>136</v>
       </c>
@@ -3684,12 +3768,15 @@
       <c r="G7" s="10">
         <v>0</v>
       </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
       <c r="BU7" s="2">
         <v>43920</v>
       </c>
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1" t="s">
         <v>89</v>
       </c>
@@ -3706,6 +3793,9 @@
         <v>0</v>
       </c>
       <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
         <v>0</v>
       </c>
       <c r="BU8" s="2">
@@ -3734,12 +3824,15 @@
       <c r="G9" s="10">
         <v>63</v>
       </c>
+      <c r="H9" s="10">
+        <v>75</v>
+      </c>
       <c r="BU9" s="2">
         <v>43922</v>
       </c>
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -3760,12 +3853,15 @@
       <c r="G10" s="10">
         <v>0</v>
       </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
       <c r="BU10" s="2">
         <v>43923</v>
       </c>
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
         <v>96</v>
       </c>
@@ -3784,12 +3880,15 @@
       <c r="G11" s="10">
         <v>0</v>
       </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
       <c r="BU11" s="2">
         <v>43924</v>
       </c>
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
@@ -3808,12 +3907,15 @@
       <c r="G12" s="10">
         <v>0</v>
       </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
       <c r="BU12" s="2">
         <v>43925</v>
       </c>
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
         <v>67</v>
       </c>
@@ -3832,12 +3934,15 @@
       <c r="G13" s="10">
         <v>1</v>
       </c>
+      <c r="H13" s="10">
+        <v>2</v>
+      </c>
       <c r="BU13" s="2">
         <v>43926</v>
       </c>
     </row>
     <row r="14" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
@@ -3856,12 +3961,15 @@
       <c r="G14" s="10">
         <v>4</v>
       </c>
+      <c r="H14" s="10">
+        <v>4</v>
+      </c>
       <c r="BU14" s="2">
         <v>43927</v>
       </c>
     </row>
     <row r="15" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="1" t="s">
         <v>133</v>
       </c>
@@ -3880,12 +3988,15 @@
       <c r="G15" s="10">
         <v>0</v>
       </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
       <c r="BU15" s="2">
         <v>43928</v>
       </c>
     </row>
     <row r="16" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="1" t="s">
         <v>83</v>
       </c>
@@ -3904,12 +4015,15 @@
       <c r="G16" s="10">
         <v>5</v>
       </c>
+      <c r="H16" s="10">
+        <v>5</v>
+      </c>
       <c r="BU16" s="2">
         <v>43929</v>
       </c>
     </row>
     <row r="17" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="1" t="s">
         <v>143</v>
       </c>
@@ -3928,12 +4042,15 @@
       <c r="G17" s="10">
         <v>0</v>
       </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
       <c r="BU17" s="2">
         <v>43930</v>
       </c>
     </row>
     <row r="18" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>154</v>
       </c>
@@ -3952,12 +4069,15 @@
       <c r="G18" s="10">
         <v>0</v>
       </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
       <c r="BU18" s="2">
         <v>43931</v>
       </c>
     </row>
     <row r="19" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>91</v>
       </c>
@@ -3976,12 +4096,15 @@
       <c r="G19" s="10">
         <v>0</v>
       </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
       <c r="BU19" s="2">
         <v>43932</v>
       </c>
     </row>
     <row r="20" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -4002,12 +4125,15 @@
       <c r="G20" s="10">
         <v>1</v>
       </c>
+      <c r="H20" s="10">
+        <v>2</v>
+      </c>
       <c r="BU20" s="2">
         <v>43933</v>
       </c>
     </row>
     <row r="21" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A21" s="15"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
@@ -4026,12 +4152,15 @@
       <c r="G21" s="10">
         <v>0</v>
       </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
       <c r="BU21" s="2">
         <v>43934</v>
       </c>
     </row>
     <row r="22" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
@@ -4050,12 +4179,15 @@
       <c r="G22" s="10">
         <v>2</v>
       </c>
+      <c r="H22" s="10">
+        <v>2</v>
+      </c>
       <c r="BU22" s="2">
         <v>43935</v>
       </c>
     </row>
     <row r="23" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A23" s="15"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
@@ -4074,12 +4206,15 @@
       <c r="G23" s="10">
         <v>0</v>
       </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
       <c r="BU23" s="2">
         <v>43936</v>
       </c>
     </row>
     <row r="24" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A24" s="16"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="1" t="s">
         <v>84</v>
       </c>
@@ -4096,6 +4231,9 @@
         <v>1</v>
       </c>
       <c r="G24" s="10">
+        <v>2</v>
+      </c>
+      <c r="H24" s="10">
         <v>2</v>
       </c>
       <c r="BU24" s="2">
@@ -4124,12 +4262,15 @@
       <c r="G25" s="10">
         <v>5</v>
       </c>
+      <c r="H25" s="10">
+        <v>7</v>
+      </c>
       <c r="BU25" s="2">
         <v>43938</v>
       </c>
     </row>
     <row r="26" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4150,12 +4291,15 @@
       <c r="G26" s="10">
         <v>12</v>
       </c>
+      <c r="H26" s="10">
+        <v>12</v>
+      </c>
       <c r="BU26" s="2">
         <v>43939</v>
       </c>
     </row>
     <row r="27" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A27" s="15"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>61</v>
       </c>
@@ -4174,12 +4318,15 @@
       <c r="G27" s="10">
         <v>0</v>
       </c>
+      <c r="H27" s="10">
+        <v>1</v>
+      </c>
       <c r="BU27" s="2">
         <v>43940</v>
       </c>
     </row>
     <row r="28" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A28" s="16"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="1" t="s">
         <v>135</v>
       </c>
@@ -4198,12 +4345,15 @@
       <c r="G28" s="10">
         <v>0</v>
       </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
       <c r="BU28" s="2">
         <v>43941</v>
       </c>
     </row>
     <row r="29" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -4224,12 +4374,15 @@
       <c r="G29" s="10">
         <v>1</v>
       </c>
+      <c r="H29" s="10">
+        <v>1</v>
+      </c>
       <c r="BU29" s="2">
         <v>43942</v>
       </c>
     </row>
     <row r="30" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="1" t="s">
         <v>107</v>
       </c>
@@ -4248,12 +4401,15 @@
       <c r="G30" s="10">
         <v>3</v>
       </c>
+      <c r="H30" s="10">
+        <v>5</v>
+      </c>
       <c r="BU30" s="2">
         <v>43943</v>
       </c>
     </row>
     <row r="31" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="1" t="s">
         <v>40</v>
       </c>
@@ -4272,12 +4428,15 @@
       <c r="G31" s="10">
         <v>2</v>
       </c>
+      <c r="H31" s="10">
+        <v>3</v>
+      </c>
       <c r="BU31" s="2">
         <v>43944</v>
       </c>
     </row>
     <row r="32" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
@@ -4296,12 +4455,15 @@
       <c r="G32" s="10">
         <v>0</v>
       </c>
+      <c r="H32" s="10">
+        <v>1</v>
+      </c>
       <c r="BU32" s="2">
         <v>43945</v>
       </c>
     </row>
     <row r="33" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -4322,12 +4484,15 @@
       <c r="G33" s="10">
         <v>0</v>
       </c>
+      <c r="H33" s="10">
+        <v>0</v>
+      </c>
       <c r="BU33" s="2">
         <v>43946</v>
       </c>
     </row>
     <row r="34" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A34" s="15"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
@@ -4346,12 +4511,15 @@
       <c r="G34" s="10">
         <v>0</v>
       </c>
+      <c r="H34" s="10">
+        <v>0</v>
+      </c>
       <c r="BU34" s="2">
         <v>43947</v>
       </c>
     </row>
     <row r="35" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A35" s="15"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="1" t="s">
         <v>63</v>
       </c>
@@ -4370,12 +4538,15 @@
       <c r="G35" s="10">
         <v>2</v>
       </c>
+      <c r="H35" s="10">
+        <v>2</v>
+      </c>
       <c r="BU35" s="2">
         <v>43948</v>
       </c>
     </row>
     <row r="36" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A36" s="15"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="1" t="s">
         <v>129</v>
       </c>
@@ -4394,12 +4565,15 @@
       <c r="G36" s="10">
         <v>0</v>
       </c>
+      <c r="H36" s="10">
+        <v>0</v>
+      </c>
       <c r="BU36" s="2">
         <v>43949</v>
       </c>
     </row>
     <row r="37" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A37" s="15"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="1" t="s">
         <v>130</v>
       </c>
@@ -4418,12 +4592,15 @@
       <c r="G37" s="10">
         <v>0</v>
       </c>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
       <c r="BU37" s="2">
         <v>43950</v>
       </c>
     </row>
     <row r="38" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A38" s="15"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="1" t="s">
         <v>137</v>
       </c>
@@ -4442,12 +4619,15 @@
       <c r="G38" s="10">
         <v>0</v>
       </c>
+      <c r="H38" s="10">
+        <v>0</v>
+      </c>
       <c r="BU38" s="2">
         <v>43951</v>
       </c>
     </row>
     <row r="39" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A39" s="15"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="1" t="s">
         <v>142</v>
       </c>
@@ -4466,12 +4646,15 @@
       <c r="G39" s="10">
         <v>0</v>
       </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
       <c r="BU39" s="2">
         <v>43952</v>
       </c>
     </row>
     <row r="40" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A40" s="16"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="1" t="s">
         <v>146</v>
       </c>
@@ -4490,12 +4673,15 @@
       <c r="G40" s="10">
         <v>0</v>
       </c>
+      <c r="H40" s="10">
+        <v>0</v>
+      </c>
       <c r="BU40" s="2">
         <v>43953</v>
       </c>
     </row>
     <row r="41" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -4516,12 +4702,15 @@
       <c r="G41" s="10">
         <v>0</v>
       </c>
+      <c r="H41" s="10">
+        <v>0</v>
+      </c>
       <c r="BU41" s="2">
         <v>43954</v>
       </c>
     </row>
     <row r="42" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="1" t="s">
         <v>99</v>
       </c>
@@ -4540,12 +4729,15 @@
       <c r="G42" s="10">
         <v>0</v>
       </c>
+      <c r="H42" s="10">
+        <v>0</v>
+      </c>
       <c r="BU42" s="2">
         <v>43955</v>
       </c>
     </row>
     <row r="43" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="1" t="s">
         <v>69</v>
       </c>
@@ -4564,12 +4756,15 @@
       <c r="G43" s="10">
         <v>0</v>
       </c>
+      <c r="H43" s="10">
+        <v>0</v>
+      </c>
       <c r="BU43" s="2">
         <v>43956</v>
       </c>
     </row>
     <row r="44" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="1" t="s">
         <v>70</v>
       </c>
@@ -4588,12 +4783,15 @@
       <c r="G44" s="10">
         <v>0</v>
       </c>
+      <c r="H44" s="10">
+        <v>0</v>
+      </c>
       <c r="BU44" s="2">
         <v>43957</v>
       </c>
     </row>
     <row r="45" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -4614,12 +4812,15 @@
       <c r="G45" s="10">
         <v>2</v>
       </c>
+      <c r="H45" s="10">
+        <v>2</v>
+      </c>
       <c r="BU45" s="2">
         <v>43958</v>
       </c>
     </row>
     <row r="46" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A46" s="16"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="1" t="s">
         <v>54</v>
       </c>
@@ -4638,12 +4839,15 @@
       <c r="G46" s="10">
         <v>1</v>
       </c>
+      <c r="H46" s="10">
+        <v>1</v>
+      </c>
       <c r="BU46" s="2">
         <v>43959</v>
       </c>
     </row>
     <row r="47" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="13" t="s">
         <v>81</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -4664,12 +4868,15 @@
       <c r="G47" s="10">
         <v>124</v>
       </c>
+      <c r="H47" s="10">
+        <v>156</v>
+      </c>
       <c r="BU47" s="2">
         <v>43960</v>
       </c>
     </row>
     <row r="48" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A48" s="12"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="1" t="s">
         <v>80</v>
       </c>
@@ -4688,12 +4895,15 @@
       <c r="G48" s="10">
         <v>0</v>
       </c>
+      <c r="H48" s="10">
+        <v>0</v>
+      </c>
       <c r="BU48" s="2">
         <v>43961</v>
       </c>
     </row>
     <row r="49" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A49" s="13"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1" t="s">
         <v>138</v>
       </c>
@@ -4710,6 +4920,9 @@
         <v>0</v>
       </c>
       <c r="G49" s="10">
+        <v>0</v>
+      </c>
+      <c r="H49" s="10">
         <v>0</v>
       </c>
       <c r="BU49" s="2">
@@ -4738,6 +4951,9 @@
       <c r="G50" s="10">
         <v>5</v>
       </c>
+      <c r="H50" s="10">
+        <v>7</v>
+      </c>
       <c r="BU50" s="2">
         <v>43963</v>
       </c>
@@ -4764,12 +4980,15 @@
       <c r="G51" s="10">
         <v>28</v>
       </c>
+      <c r="H51" s="10">
+        <v>31</v>
+      </c>
       <c r="BU51" s="2">
         <v>43964</v>
       </c>
     </row>
     <row r="52" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -4790,12 +5009,15 @@
       <c r="G52" s="10">
         <v>2</v>
       </c>
+      <c r="H52" s="10">
+        <v>2</v>
+      </c>
       <c r="BU52" s="2">
         <v>43965</v>
       </c>
     </row>
     <row r="53" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A53" s="15"/>
+      <c r="A53" s="17"/>
       <c r="B53" s="1" t="s">
         <v>123</v>
       </c>
@@ -4814,12 +5036,15 @@
       <c r="G53" s="10">
         <v>0</v>
       </c>
+      <c r="H53" s="10">
+        <v>0</v>
+      </c>
       <c r="BU53" s="2">
         <v>43966</v>
       </c>
     </row>
     <row r="54" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A54" s="15"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="1" t="s">
         <v>132</v>
       </c>
@@ -4838,12 +5063,15 @@
       <c r="G54" s="10">
         <v>0</v>
       </c>
+      <c r="H54" s="10">
+        <v>0</v>
+      </c>
       <c r="BU54" s="2">
         <v>43967</v>
       </c>
     </row>
     <row r="55" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A55" s="16"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="1" t="s">
         <v>145</v>
       </c>
@@ -4862,12 +5090,15 @@
       <c r="G55" s="10">
         <v>0</v>
       </c>
+      <c r="H55" s="10">
+        <v>0</v>
+      </c>
       <c r="BU55" s="2">
         <v>43968</v>
       </c>
     </row>
     <row r="56" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -4888,12 +5119,15 @@
       <c r="G56" s="10">
         <v>0</v>
       </c>
+      <c r="H56" s="10">
+        <v>0</v>
+      </c>
       <c r="BU56" s="2">
         <v>43969</v>
       </c>
     </row>
     <row r="57" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A57" s="12"/>
+      <c r="A57" s="14"/>
       <c r="B57" s="1" t="s">
         <v>104</v>
       </c>
@@ -4912,12 +5146,15 @@
       <c r="G57" s="10">
         <v>4</v>
       </c>
+      <c r="H57" s="10">
+        <v>4</v>
+      </c>
       <c r="BU57" s="2">
         <v>43970</v>
       </c>
     </row>
     <row r="58" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A58" s="12"/>
+      <c r="A58" s="14"/>
       <c r="B58" s="1" t="s">
         <v>119</v>
       </c>
@@ -4936,12 +5173,15 @@
       <c r="G58" s="10">
         <v>0</v>
       </c>
+      <c r="H58" s="10">
+        <v>0</v>
+      </c>
       <c r="BU58" s="2">
         <v>43971</v>
       </c>
     </row>
     <row r="59" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A59" s="12"/>
+      <c r="A59" s="14"/>
       <c r="B59" s="1" t="s">
         <v>124</v>
       </c>
@@ -4960,12 +5200,15 @@
       <c r="G59" s="10">
         <v>3</v>
       </c>
+      <c r="H59" s="10">
+        <v>3</v>
+      </c>
       <c r="BU59" s="2">
         <v>43972</v>
       </c>
     </row>
     <row r="60" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A60" s="12"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="1" t="s">
         <v>71</v>
       </c>
@@ -4984,12 +5227,15 @@
       <c r="G60" s="10">
         <v>2</v>
       </c>
+      <c r="H60" s="10">
+        <v>2</v>
+      </c>
       <c r="BU60" s="2">
         <v>43973</v>
       </c>
     </row>
     <row r="61" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A61" s="13"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="1" t="s">
         <v>93</v>
       </c>
@@ -5006,6 +5252,9 @@
         <v>0</v>
       </c>
       <c r="G61" s="10">
+        <v>0</v>
+      </c>
+      <c r="H61" s="10">
         <v>0</v>
       </c>
       <c r="BU61" s="2">
@@ -5034,12 +5283,15 @@
       <c r="G62" s="10">
         <v>43</v>
       </c>
+      <c r="H62" s="10">
+        <v>54</v>
+      </c>
       <c r="BU62" s="2">
         <v>43975</v>
       </c>
     </row>
     <row r="63" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -5060,12 +5312,15 @@
       <c r="G63" s="10">
         <v>0</v>
       </c>
+      <c r="H63" s="10">
+        <v>0</v>
+      </c>
       <c r="BU63" s="2">
         <v>43976</v>
       </c>
     </row>
     <row r="64" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A64" s="12"/>
+      <c r="A64" s="14"/>
       <c r="B64" s="1" t="s">
         <v>23</v>
       </c>
@@ -5084,12 +5339,15 @@
       <c r="G64" s="10">
         <v>0</v>
       </c>
+      <c r="H64" s="10">
+        <v>0</v>
+      </c>
       <c r="BU64" s="2">
         <v>43977</v>
       </c>
     </row>
     <row r="65" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A65" s="12"/>
+      <c r="A65" s="14"/>
       <c r="B65" s="1" t="s">
         <v>36</v>
       </c>
@@ -5108,12 +5366,15 @@
       <c r="G65" s="10">
         <v>0</v>
       </c>
+      <c r="H65" s="10">
+        <v>0</v>
+      </c>
       <c r="BU65" s="2">
         <v>43978</v>
       </c>
     </row>
     <row r="66" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A66" s="12"/>
+      <c r="A66" s="14"/>
       <c r="B66" s="1" t="s">
         <v>125</v>
       </c>
@@ -5132,12 +5393,15 @@
       <c r="G66" s="10">
         <v>0</v>
       </c>
+      <c r="H66" s="10">
+        <v>0</v>
+      </c>
       <c r="BU66" s="2">
         <v>43979</v>
       </c>
     </row>
     <row r="67" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A67" s="12"/>
+      <c r="A67" s="14"/>
       <c r="B67" s="1" t="s">
         <v>131</v>
       </c>
@@ -5156,12 +5420,15 @@
       <c r="G67" s="10">
         <v>1</v>
       </c>
+      <c r="H67" s="10">
+        <v>1</v>
+      </c>
       <c r="BU67" s="2">
         <v>43980</v>
       </c>
     </row>
     <row r="68" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A68" s="12"/>
+      <c r="A68" s="14"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
@@ -5180,12 +5447,15 @@
       <c r="G68" s="10">
         <v>0</v>
       </c>
+      <c r="H68" s="10">
+        <v>0</v>
+      </c>
       <c r="BU68" s="2">
         <v>43981</v>
       </c>
     </row>
     <row r="69" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A69" s="12"/>
+      <c r="A69" s="14"/>
       <c r="B69" s="1" t="s">
         <v>77</v>
       </c>
@@ -5204,12 +5474,15 @@
       <c r="G69" s="10">
         <v>1</v>
       </c>
+      <c r="H69" s="10">
+        <v>1</v>
+      </c>
       <c r="BU69" s="2">
         <v>43982</v>
       </c>
     </row>
     <row r="70" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A70" s="13"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="1" t="s">
         <v>140</v>
       </c>
@@ -5228,9 +5501,12 @@
       <c r="G70" s="10">
         <v>1</v>
       </c>
+      <c r="H70" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -5251,9 +5527,12 @@
       <c r="G71" s="10">
         <v>0</v>
       </c>
+      <c r="H71" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A72" s="15"/>
+      <c r="A72" s="17"/>
       <c r="B72" s="1" t="s">
         <v>105</v>
       </c>
@@ -5272,9 +5551,12 @@
       <c r="G72" s="10">
         <v>0</v>
       </c>
+      <c r="H72" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A73" s="15"/>
+      <c r="A73" s="17"/>
       <c r="B73" s="1" t="s">
         <v>115</v>
       </c>
@@ -5293,9 +5575,12 @@
       <c r="G73" s="10">
         <v>0</v>
       </c>
+      <c r="H73" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A74" s="15"/>
+      <c r="A74" s="17"/>
       <c r="B74" s="1" t="s">
         <v>65</v>
       </c>
@@ -5314,9 +5599,12 @@
       <c r="G74" s="10">
         <v>0</v>
       </c>
+      <c r="H74" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A75" s="16"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="1" t="s">
         <v>149</v>
       </c>
@@ -5333,6 +5621,9 @@
         <v>1</v>
       </c>
       <c r="G75" s="10">
+        <v>1</v>
+      </c>
+      <c r="H75" s="10">
         <v>1</v>
       </c>
     </row>
@@ -5358,9 +5649,12 @@
       <c r="G76" s="10">
         <v>8</v>
       </c>
+      <c r="H76" s="10">
+        <v>10</v>
+      </c>
     </row>
     <row r="77" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A77" s="14" t="s">
+      <c r="A77" s="16" t="s">
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -5381,9 +5675,12 @@
       <c r="G77" s="10">
         <v>55</v>
       </c>
+      <c r="H77" s="10">
+        <v>65</v>
+      </c>
     </row>
     <row r="78" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A78" s="15"/>
+      <c r="A78" s="17"/>
       <c r="B78" s="1" t="s">
         <v>74</v>
       </c>
@@ -5402,9 +5699,12 @@
       <c r="G78" s="10">
         <v>9</v>
       </c>
+      <c r="H78" s="10">
+        <v>9</v>
+      </c>
     </row>
     <row r="79" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A79" s="15"/>
+      <c r="A79" s="17"/>
       <c r="B79" s="1" t="s">
         <v>87</v>
       </c>
@@ -5423,9 +5723,12 @@
       <c r="G79" s="10">
         <v>12</v>
       </c>
+      <c r="H79" s="10">
+        <v>13</v>
+      </c>
     </row>
     <row r="80" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A80" s="15"/>
+      <c r="A80" s="17"/>
       <c r="B80" s="1" t="s">
         <v>147</v>
       </c>
@@ -5444,9 +5747,12 @@
       <c r="G80" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="16"/>
+      <c r="H80" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="18"/>
       <c r="B81" s="1" t="s">
         <v>92</v>
       </c>
@@ -5465,9 +5771,12 @@
       <c r="G81" s="10">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="11" t="s">
+      <c r="H81" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -5488,9 +5797,12 @@
       <c r="G82" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="12"/>
+      <c r="H82" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" s="14"/>
       <c r="B83" s="1" t="s">
         <v>18</v>
       </c>
@@ -5509,9 +5821,12 @@
       <c r="G83" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="12"/>
+      <c r="H83" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" s="14"/>
       <c r="B84" s="1" t="s">
         <v>26</v>
       </c>
@@ -5530,9 +5845,12 @@
       <c r="G84" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="12"/>
+      <c r="H84" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" s="14"/>
       <c r="B85" s="1" t="s">
         <v>31</v>
       </c>
@@ -5551,9 +5869,12 @@
       <c r="G85" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="12"/>
+      <c r="H85" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="14"/>
       <c r="B86" s="1" t="s">
         <v>49</v>
       </c>
@@ -5572,9 +5893,12 @@
       <c r="G86" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="12"/>
+      <c r="H86" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="14"/>
       <c r="B87" s="1" t="s">
         <v>117</v>
       </c>
@@ -5593,9 +5917,12 @@
       <c r="G87" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="13"/>
+      <c r="H87" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="15"/>
       <c r="B88" s="1" t="s">
         <v>120</v>
       </c>
@@ -5614,9 +5941,12 @@
       <c r="G88" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="14" t="s">
+      <c r="H88" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="16" t="s">
         <v>60</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -5637,9 +5967,12 @@
       <c r="G89" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="16"/>
+      <c r="H89" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="18"/>
       <c r="B90" s="1" t="s">
         <v>79</v>
       </c>
@@ -5658,8 +5991,11 @@
       <c r="G90" s="10">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H90" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>148</v>
       </c>
@@ -5681,9 +6017,12 @@
       <c r="G91" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="14" t="s">
+      <c r="H91" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -5704,9 +6043,12 @@
       <c r="G92" s="10">
         <v>44</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="15"/>
+      <c r="H92" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="17"/>
       <c r="B93" s="1" t="s">
         <v>144</v>
       </c>
@@ -5725,9 +6067,12 @@
       <c r="G93" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="16"/>
+      <c r="H93" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" s="18"/>
       <c r="B94" s="1" t="s">
         <v>85</v>
       </c>
@@ -5746,9 +6091,12 @@
       <c r="G94" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="11" t="s">
+      <c r="H94" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -5769,9 +6117,12 @@
       <c r="G95" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="12"/>
+      <c r="H95" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="14"/>
       <c r="B96" s="1" t="s">
         <v>110</v>
       </c>
@@ -5790,9 +6141,12 @@
       <c r="G96" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" s="12"/>
+      <c r="H96" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" s="14"/>
       <c r="B97" s="1" t="s">
         <v>127</v>
       </c>
@@ -5811,9 +6165,12 @@
       <c r="G97" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98" s="12"/>
+      <c r="H97" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" s="14"/>
       <c r="B98" s="1" t="s">
         <v>128</v>
       </c>
@@ -5832,9 +6189,12 @@
       <c r="G98" s="10">
         <v>11</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99" s="13"/>
+      <c r="H98" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" s="15"/>
       <c r="B99" s="1" t="s">
         <v>139</v>
       </c>
@@ -5853,9 +6213,12 @@
       <c r="G99" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" s="14" t="s">
+      <c r="H99" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -5876,9 +6239,12 @@
       <c r="G100" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101" s="15"/>
+      <c r="H100" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" s="17"/>
       <c r="B101" s="1" t="s">
         <v>100</v>
       </c>
@@ -5897,9 +6263,12 @@
       <c r="G101" s="10">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A102" s="15"/>
+      <c r="H101" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" s="17"/>
       <c r="B102" s="1" t="s">
         <v>50</v>
       </c>
@@ -5918,9 +6287,12 @@
       <c r="G102" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="15"/>
+      <c r="H102" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" s="17"/>
       <c r="B103" s="1" t="s">
         <v>118</v>
       </c>
@@ -5939,9 +6311,12 @@
       <c r="G103" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="16"/>
+      <c r="H103" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" s="18"/>
       <c r="B104" s="1" t="s">
         <v>22</v>
       </c>
@@ -5960,8 +6335,11 @@
       <c r="G104" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H104" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="7" t="s">
         <v>151</v>
       </c>
@@ -5983,8 +6361,11 @@
       <c r="G105" s="10">
         <v>17</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H105" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="6" t="s">
         <v>153</v>
       </c>
@@ -6006,9 +6387,12 @@
       <c r="G106" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A107" s="11" t="s">
+      <c r="H106" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A107" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -6029,9 +6413,12 @@
       <c r="G107" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" s="12"/>
+      <c r="H107" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A108" s="14"/>
       <c r="B108" s="1" t="s">
         <v>39</v>
       </c>
@@ -6050,9 +6437,12 @@
       <c r="G108" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" s="13"/>
+      <c r="H108" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A109" s="15"/>
       <c r="B109" s="1" t="s">
         <v>114</v>
       </c>
@@ -6071,9 +6461,12 @@
       <c r="G109" s="10">
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" s="14" t="s">
+      <c r="H109" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A110" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -6094,9 +6487,12 @@
       <c r="G110" s="10">
         <v>8</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A111" s="15"/>
+      <c r="H110" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" s="17"/>
       <c r="B111" s="1" t="s">
         <v>102</v>
       </c>
@@ -6115,9 +6511,12 @@
       <c r="G111" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112" s="15"/>
+      <c r="H111" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112" s="17"/>
       <c r="B112" s="1" t="s">
         <v>37</v>
       </c>
@@ -6136,9 +6535,12 @@
       <c r="G112" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A113" s="15"/>
+      <c r="H112" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" s="17"/>
       <c r="B113" s="1" t="s">
         <v>48</v>
       </c>
@@ -6157,9 +6559,12 @@
       <c r="G113" s="10">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="15"/>
+      <c r="H113" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A114" s="17"/>
       <c r="B114" s="1" t="s">
         <v>116</v>
       </c>
@@ -6178,9 +6583,12 @@
       <c r="G114" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="16"/>
+      <c r="H114" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A115" s="18"/>
       <c r="B115" s="1" t="s">
         <v>134</v>
       </c>
@@ -6199,9 +6607,12 @@
       <c r="G115" s="10">
         <v>11</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A116" s="11" t="s">
+      <c r="H115" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A116" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B116" s="1" t="s">
@@ -6222,9 +6633,12 @@
       <c r="G116" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A117" s="12"/>
+      <c r="H116" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A117" s="14"/>
       <c r="B117" s="1" t="s">
         <v>106</v>
       </c>
@@ -6243,9 +6657,12 @@
       <c r="G117" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A118" s="12"/>
+      <c r="H117" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" s="14"/>
       <c r="B118" s="1" t="s">
         <v>45</v>
       </c>
@@ -6264,9 +6681,12 @@
       <c r="G118" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A119" s="12"/>
+      <c r="H118" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A119" s="14"/>
       <c r="B119" s="1" t="s">
         <v>111</v>
       </c>
@@ -6285,9 +6705,12 @@
       <c r="G119" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="12"/>
+      <c r="H119" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" s="14"/>
       <c r="B120" s="1" t="s">
         <v>112</v>
       </c>
@@ -6306,9 +6729,12 @@
       <c r="G120" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="12"/>
+      <c r="H120" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" s="14"/>
       <c r="B121" s="1" t="s">
         <v>51</v>
       </c>
@@ -6327,9 +6753,12 @@
       <c r="G121" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A122" s="12"/>
+      <c r="H121" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" s="14"/>
       <c r="B122" s="1" t="s">
         <v>52</v>
       </c>
@@ -6348,9 +6777,12 @@
       <c r="G122" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A123" s="12"/>
+      <c r="H122" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A123" s="14"/>
       <c r="B123" s="1" t="s">
         <v>56</v>
       </c>
@@ -6369,9 +6801,12 @@
       <c r="G123" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A124" s="12"/>
+      <c r="H123" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A124" s="14"/>
       <c r="B124" s="1" t="s">
         <v>121</v>
       </c>
@@ -6390,9 +6825,12 @@
       <c r="G124" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A125" s="13"/>
+      <c r="H124" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A125" s="15"/>
       <c r="B125" s="1" t="s">
         <v>72</v>
       </c>
@@ -6411,8 +6849,11 @@
       <c r="G125" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H125" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
         <v>156</v>
       </c>
@@ -6434,9 +6875,12 @@
       <c r="G126" s="10">
         <v>29</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A127" s="11" t="s">
+      <c r="H126" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A127" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B127" s="1" t="s">
@@ -6457,9 +6901,12 @@
       <c r="G127" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A128" s="12"/>
+      <c r="H127" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A128" s="14"/>
       <c r="B128" s="1" t="s">
         <v>108</v>
       </c>
@@ -6478,9 +6925,12 @@
       <c r="G128" s="10">
         <v>0</v>
       </c>
+      <c r="H128" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A129" s="12"/>
+      <c r="A129" s="14"/>
       <c r="B129" s="1" t="s">
         <v>57</v>
       </c>
@@ -6499,9 +6949,12 @@
       <c r="G129" s="10">
         <v>0</v>
       </c>
+      <c r="H129" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A130" s="13"/>
+      <c r="A130" s="15"/>
       <c r="B130" s="1" t="s">
         <v>86</v>
       </c>
@@ -6520,9 +6973,12 @@
       <c r="G130" s="10">
         <v>0</v>
       </c>
+      <c r="H130" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A131" s="14" t="s">
+      <c r="A131" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -6543,9 +6999,12 @@
       <c r="G131" s="10">
         <v>2</v>
       </c>
+      <c r="H131" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="132" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A132" s="15"/>
+      <c r="A132" s="17"/>
       <c r="B132" s="1" t="s">
         <v>126</v>
       </c>
@@ -6564,9 +7023,12 @@
       <c r="G132" s="10">
         <v>1</v>
       </c>
+      <c r="H132" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A133" s="15"/>
+      <c r="A133" s="17"/>
       <c r="B133" s="1" t="s">
         <v>82</v>
       </c>
@@ -6585,9 +7047,12 @@
       <c r="G133" s="10">
         <v>0</v>
       </c>
+      <c r="H133" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A134" s="16"/>
+      <c r="A134" s="18"/>
       <c r="B134" s="1" t="s">
         <v>155</v>
       </c>
@@ -6604,6 +7069,9 @@
         <v>1</v>
       </c>
       <c r="G134" s="10">
+        <v>1</v>
+      </c>
+      <c r="H134" s="10">
         <v>1</v>
       </c>
     </row>
@@ -6625,7 +7093,7 @@
       </c>
       <c r="H136" s="10">
         <f>SUM(va[28-Mar])</f>
-        <v>0</v>
+        <v>739</v>
       </c>
       <c r="I136" s="10">
         <f>SUM(va[29-Mar])</f>
@@ -6898,7 +7366,7 @@
         <v>83</v>
       </c>
       <c r="H137" s="10">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="I137" s="10">
         <v>0</v>
@@ -7107,7 +7575,7 @@
         <v>14</v>
       </c>
       <c r="H138" s="10">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I138" s="10">
         <v>0</v>
@@ -7316,7 +7784,7 @@
         <v>7337</v>
       </c>
       <c r="H139" s="10">
-        <v>0</v>
+        <v>9166</v>
       </c>
       <c r="I139" s="10">
         <v>0</v>
@@ -7521,11 +7989,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="A110:A115"/>
-    <mergeCell ref="A116:A125"/>
-    <mergeCell ref="A127:A130"/>
     <mergeCell ref="A131:A134"/>
     <mergeCell ref="A71:A75"/>
     <mergeCell ref="A77:A81"/>
@@ -7533,11 +7996,11 @@
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="A92:A94"/>
     <mergeCell ref="A95:A99"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A56:A61"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A110:A115"/>
+    <mergeCell ref="A116:A125"/>
+    <mergeCell ref="A127:A130"/>
     <mergeCell ref="A63:A70"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A10:A19"/>
@@ -7545,6 +8008,11 @@
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A61"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:BB134 BS2:BS134">
     <cfRule type="colorScale" priority="6">

</xml_diff>

<commit_message>
corrected DC numbers from 28-mar
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79466BBD-FBE4-4CDD-9B5D-4B68AF3249C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2C6A67-10A6-4806-B068-A4EEE038441B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="27580" windowHeight="18000" tabRatio="685" activeTab="5" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="-110" yWindow="350" windowWidth="27580" windowHeight="18000" tabRatio="685" activeTab="3" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -3168,7 +3168,7 @@
   <dimension ref="A1:CC46"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3590,7 +3590,7 @@
         <v>4</v>
       </c>
       <c r="Q5" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R5" s="10">
         <v>9</v>
@@ -10201,7 +10201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F4047C-2E48-45D8-A0A4-C3935E342FF1}">
   <dimension ref="A1:CC8"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -11493,11 +11493,11 @@
       </c>
       <c r="Q5" s="12">
         <f>MAX(0, (dc!Q5-dc!P5))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="12">
         <f>MAX(0, (dc!R5-dc!Q5))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S5" s="12">
         <f>MAX(0, (dc!S5-dc!R5))</f>
@@ -19173,7 +19173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10B5AF9-8E42-4F8B-8F58-724C1869D2EC}">
   <dimension ref="A1:BU141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="T151" sqref="T151"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
mid-day update (MD & VA) for 31 March
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73629DB9-42F2-4999-9026-C5A237B3EA7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FD8689-A207-42DC-86EB-064306EC95A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="685" activeTab="5" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
@@ -3743,7 +3743,7 @@
   <dimension ref="A1:BP29"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="G2" sqref="G2:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,6 +3977,9 @@
       <c r="F2">
         <v>110</v>
       </c>
+      <c r="G2">
+        <v>127</v>
+      </c>
     </row>
     <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3997,6 +4000,9 @@
       <c r="F3">
         <v>152</v>
       </c>
+      <c r="G3">
+        <v>187</v>
+      </c>
     </row>
     <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -4017,6 +4023,9 @@
       <c r="F4">
         <v>186</v>
       </c>
+      <c r="G4">
+        <v>227</v>
+      </c>
     </row>
     <row r="5" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -4037,6 +4046,9 @@
       <c r="F5">
         <v>12</v>
       </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -4057,6 +4069,9 @@
       <c r="F6">
         <v>4</v>
       </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -4077,6 +4092,9 @@
       <c r="F7">
         <v>82</v>
       </c>
+      <c r="G7">
+        <v>92</v>
+      </c>
     </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -4097,6 +4115,9 @@
       <c r="F8">
         <v>13</v>
       </c>
+      <c r="G8">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -4117,6 +4138,9 @@
       <c r="F9">
         <v>33</v>
       </c>
+      <c r="G9">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -4137,6 +4161,9 @@
       <c r="F10">
         <v>26</v>
       </c>
+      <c r="G10">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -4157,6 +4184,9 @@
       <c r="F11">
         <v>3</v>
       </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -4177,6 +4207,9 @@
       <c r="F12">
         <v>24</v>
       </c>
+      <c r="G12">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -4197,6 +4230,9 @@
       <c r="F13">
         <v>96</v>
       </c>
+      <c r="G13">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -4217,6 +4253,9 @@
       <c r="F14">
         <v>3</v>
       </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -4237,6 +4276,9 @@
       <c r="F15">
         <v>341</v>
       </c>
+      <c r="G15">
+        <v>388</v>
+      </c>
     </row>
     <row r="16" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -4257,6 +4299,9 @@
       <c r="F16">
         <v>294</v>
       </c>
+      <c r="G16">
+        <v>341</v>
+      </c>
     </row>
     <row r="17" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -4277,6 +4322,9 @@
       <c r="F17">
         <v>4</v>
       </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -4297,6 +4345,9 @@
       <c r="F18">
         <v>9</v>
       </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -4317,6 +4368,9 @@
       <c r="F19">
         <v>1</v>
       </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -4337,6 +4391,9 @@
       <c r="F20">
         <v>4</v>
       </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -4357,6 +4414,9 @@
       <c r="F21">
         <v>7</v>
       </c>
+      <c r="G21">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -4377,6 +4437,9 @@
       <c r="F22">
         <v>6</v>
       </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -4397,6 +4460,9 @@
       <c r="F23">
         <v>3</v>
       </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -4423,8 +4489,7 @@
         <v>1413</v>
       </c>
       <c r="G25" s="10">
-        <f>SUM(md[31-Mar])</f>
-        <v>0</v>
+        <v>1660</v>
       </c>
       <c r="H25" s="10">
         <f>SUM(md[1-Apr])</f>
@@ -4691,7 +4756,7 @@
         <v>353</v>
       </c>
       <c r="G26" s="10">
-        <v>0</v>
+        <v>429</v>
       </c>
       <c r="H26" s="10">
         <v>0</v>
@@ -4897,7 +4962,7 @@
         <v>15</v>
       </c>
       <c r="G27" s="10">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H27" s="10">
         <v>0</v>
@@ -5155,8 +5220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289E8C7D-3613-4740-9288-5737AAA9BBA1}">
   <dimension ref="A1:BU141"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J141" sqref="J141"/>
+    <sheetView topLeftCell="A79" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5418,6 +5483,9 @@
       <c r="J2" s="10">
         <v>26</v>
       </c>
+      <c r="K2" s="10">
+        <v>30</v>
+      </c>
       <c r="BU2" s="2">
         <v>43915</v>
       </c>
@@ -5451,6 +5519,9 @@
         <v>1</v>
       </c>
       <c r="J3" s="10">
+        <v>1</v>
+      </c>
+      <c r="K3" s="10">
         <v>1</v>
       </c>
       <c r="BU3" s="2">
@@ -5486,6 +5557,9 @@
       <c r="J4" s="10">
         <v>5</v>
       </c>
+      <c r="K4" s="10">
+        <v>5</v>
+      </c>
       <c r="BU4" s="2">
         <v>43917</v>
       </c>
@@ -5519,6 +5593,9 @@
       <c r="J5" s="10">
         <v>0</v>
       </c>
+      <c r="K5" s="10">
+        <v>0</v>
+      </c>
       <c r="BU5" s="2">
         <v>43918</v>
       </c>
@@ -5552,6 +5629,9 @@
       <c r="J6" s="10">
         <v>2</v>
       </c>
+      <c r="K6" s="10">
+        <v>3</v>
+      </c>
       <c r="BU6" s="2">
         <v>43919</v>
       </c>
@@ -5585,6 +5665,9 @@
       <c r="J7" s="10">
         <v>0</v>
       </c>
+      <c r="K7" s="10">
+        <v>0</v>
+      </c>
       <c r="BU7" s="2">
         <v>43920</v>
       </c>
@@ -5618,6 +5701,9 @@
       <c r="J8" s="10">
         <v>0</v>
       </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
       <c r="BU8" s="2">
         <v>43921</v>
       </c>
@@ -5653,6 +5739,9 @@
       <c r="J9" s="10">
         <v>86</v>
       </c>
+      <c r="K9" s="10">
+        <v>104</v>
+      </c>
       <c r="BU9" s="2">
         <v>43922</v>
       </c>
@@ -5686,6 +5775,9 @@
         <v>0</v>
       </c>
       <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
         <v>0</v>
       </c>
       <c r="BU10" s="2">
@@ -5721,6 +5813,9 @@
       <c r="J11" s="10">
         <v>0</v>
       </c>
+      <c r="K11" s="10">
+        <v>0</v>
+      </c>
       <c r="BU11" s="2">
         <v>43924</v>
       </c>
@@ -5754,6 +5849,9 @@
       <c r="J12" s="10">
         <v>0</v>
       </c>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
       <c r="BU12" s="2">
         <v>43925</v>
       </c>
@@ -5787,6 +5885,9 @@
       <c r="J13" s="10">
         <v>2</v>
       </c>
+      <c r="K13" s="10">
+        <v>2</v>
+      </c>
       <c r="BU13" s="2">
         <v>43926</v>
       </c>
@@ -5820,6 +5921,9 @@
       <c r="J14" s="10">
         <v>5</v>
       </c>
+      <c r="K14" s="10">
+        <v>5</v>
+      </c>
       <c r="BU14" s="2">
         <v>43927</v>
       </c>
@@ -5853,6 +5957,9 @@
       <c r="J15" s="10">
         <v>0</v>
       </c>
+      <c r="K15" s="10">
+        <v>0</v>
+      </c>
       <c r="BU15" s="2">
         <v>43928</v>
       </c>
@@ -5886,6 +5993,9 @@
       <c r="J16" s="10">
         <v>6</v>
       </c>
+      <c r="K16" s="10">
+        <v>6</v>
+      </c>
       <c r="BU16" s="2">
         <v>43929</v>
       </c>
@@ -5919,6 +6029,9 @@
       <c r="J17" s="10">
         <v>0</v>
       </c>
+      <c r="K17" s="10">
+        <v>0</v>
+      </c>
       <c r="BU17" s="2">
         <v>43930</v>
       </c>
@@ -5952,6 +6065,9 @@
       <c r="J18" s="10">
         <v>0</v>
       </c>
+      <c r="K18" s="10">
+        <v>0</v>
+      </c>
       <c r="BU18" s="2">
         <v>43931</v>
       </c>
@@ -5985,6 +6101,9 @@
       <c r="J19" s="10">
         <v>0</v>
       </c>
+      <c r="K19" s="10">
+        <v>2</v>
+      </c>
       <c r="BU19" s="2">
         <v>43932</v>
       </c>
@@ -6018,6 +6137,9 @@
         <v>2</v>
       </c>
       <c r="J20" s="10">
+        <v>3</v>
+      </c>
+      <c r="K20" s="10">
         <v>3</v>
       </c>
       <c r="BU20" s="2">
@@ -6053,6 +6175,9 @@
       <c r="J21" s="10">
         <v>0</v>
       </c>
+      <c r="K21" s="10">
+        <v>0</v>
+      </c>
       <c r="BU21" s="2">
         <v>43934</v>
       </c>
@@ -6086,6 +6211,9 @@
       <c r="J22" s="10">
         <v>2</v>
       </c>
+      <c r="K22" s="10">
+        <v>2</v>
+      </c>
       <c r="BU22" s="2">
         <v>43935</v>
       </c>
@@ -6119,6 +6247,9 @@
       <c r="J23" s="10">
         <v>0</v>
       </c>
+      <c r="K23" s="10">
+        <v>1</v>
+      </c>
       <c r="BU23" s="2">
         <v>43936</v>
       </c>
@@ -6152,6 +6283,9 @@
       <c r="J24" s="10">
         <v>4</v>
       </c>
+      <c r="K24" s="10">
+        <v>5</v>
+      </c>
       <c r="BU24" s="2">
         <v>43937</v>
       </c>
@@ -6187,6 +6321,9 @@
       <c r="J25" s="10">
         <v>18</v>
       </c>
+      <c r="K25" s="10">
+        <v>23</v>
+      </c>
       <c r="BU25" s="2">
         <v>43938</v>
       </c>
@@ -6221,6 +6358,9 @@
       </c>
       <c r="J26" s="10">
         <v>21</v>
+      </c>
+      <c r="K26" s="10">
+        <v>43</v>
       </c>
       <c r="BU26" s="2">
         <v>43939</v>
@@ -6255,6 +6395,9 @@
       <c r="J27" s="10">
         <v>3</v>
       </c>
+      <c r="K27" s="10">
+        <v>4</v>
+      </c>
       <c r="BU27" s="2">
         <v>43940</v>
       </c>
@@ -6288,6 +6431,9 @@
       <c r="J28" s="10">
         <v>0</v>
       </c>
+      <c r="K28" s="10">
+        <v>0</v>
+      </c>
       <c r="BU28" s="2">
         <v>43941</v>
       </c>
@@ -6321,6 +6467,9 @@
         <v>1</v>
       </c>
       <c r="J29" s="10">
+        <v>1</v>
+      </c>
+      <c r="K29" s="10">
         <v>1</v>
       </c>
       <c r="BU29" s="2">
@@ -6356,6 +6505,9 @@
       <c r="J30" s="10">
         <v>6</v>
       </c>
+      <c r="K30" s="10">
+        <v>7</v>
+      </c>
       <c r="BU30" s="2">
         <v>43943</v>
       </c>
@@ -6389,6 +6541,9 @@
       <c r="J31" s="10">
         <v>5</v>
       </c>
+      <c r="K31" s="10">
+        <v>6</v>
+      </c>
       <c r="BU31" s="2">
         <v>43944</v>
       </c>
@@ -6422,6 +6577,9 @@
       <c r="J32" s="10">
         <v>1</v>
       </c>
+      <c r="K32" s="10">
+        <v>1</v>
+      </c>
       <c r="BU32" s="2">
         <v>43945</v>
       </c>
@@ -6455,6 +6613,9 @@
         <v>0</v>
       </c>
       <c r="J33" s="10">
+        <v>0</v>
+      </c>
+      <c r="K33" s="10">
         <v>0</v>
       </c>
       <c r="BU33" s="2">
@@ -6490,6 +6651,9 @@
       <c r="J34" s="10">
         <v>3</v>
       </c>
+      <c r="K34" s="10">
+        <v>3</v>
+      </c>
       <c r="BU34" s="2">
         <v>43947</v>
       </c>
@@ -6523,6 +6687,9 @@
       <c r="J35" s="10">
         <v>5</v>
       </c>
+      <c r="K35" s="10">
+        <v>7</v>
+      </c>
       <c r="BU35" s="2">
         <v>43948</v>
       </c>
@@ -6556,6 +6723,9 @@
       <c r="J36" s="10">
         <v>0</v>
       </c>
+      <c r="K36" s="10">
+        <v>1</v>
+      </c>
       <c r="BU36" s="2">
         <v>43949</v>
       </c>
@@ -6589,6 +6759,9 @@
       <c r="J37" s="10">
         <v>0</v>
       </c>
+      <c r="K37" s="10">
+        <v>0</v>
+      </c>
       <c r="BU37" s="2">
         <v>43950</v>
       </c>
@@ -6622,6 +6795,9 @@
       <c r="J38" s="10">
         <v>0</v>
       </c>
+      <c r="K38" s="10">
+        <v>0</v>
+      </c>
       <c r="BU38" s="2">
         <v>43951</v>
       </c>
@@ -6655,6 +6831,9 @@
       <c r="J39" s="10">
         <v>3</v>
       </c>
+      <c r="K39" s="10">
+        <v>4</v>
+      </c>
       <c r="BU39" s="2">
         <v>43952</v>
       </c>
@@ -6688,6 +6867,9 @@
       <c r="J40" s="10">
         <v>2</v>
       </c>
+      <c r="K40" s="10">
+        <v>2</v>
+      </c>
       <c r="BU40" s="2">
         <v>43953</v>
       </c>
@@ -6721,6 +6903,9 @@
         <v>0</v>
       </c>
       <c r="J41" s="10">
+        <v>0</v>
+      </c>
+      <c r="K41" s="10">
         <v>0</v>
       </c>
       <c r="BU41" s="2">
@@ -6756,6 +6941,9 @@
       <c r="J42" s="10">
         <v>0</v>
       </c>
+      <c r="K42" s="10">
+        <v>0</v>
+      </c>
       <c r="BU42" s="2">
         <v>43955</v>
       </c>
@@ -6789,6 +6977,9 @@
       <c r="J43" s="10">
         <v>0</v>
       </c>
+      <c r="K43" s="10">
+        <v>0</v>
+      </c>
       <c r="BU43" s="2">
         <v>43956</v>
       </c>
@@ -6822,6 +7013,9 @@
       <c r="J44" s="10">
         <v>2</v>
       </c>
+      <c r="K44" s="10">
+        <v>2</v>
+      </c>
       <c r="BU44" s="2">
         <v>43957</v>
       </c>
@@ -6856,6 +7050,9 @@
       </c>
       <c r="J45" s="10">
         <v>6</v>
+      </c>
+      <c r="K45" s="10">
+        <v>7</v>
       </c>
       <c r="BU45" s="2">
         <v>43958</v>
@@ -6890,6 +7087,9 @@
       <c r="J46" s="10">
         <v>1</v>
       </c>
+      <c r="K46" s="10">
+        <v>1</v>
+      </c>
       <c r="BU46" s="2">
         <v>43959</v>
       </c>
@@ -6924,6 +7124,9 @@
       </c>
       <c r="J47" s="10">
         <v>224</v>
+      </c>
+      <c r="K47" s="10">
+        <v>244</v>
       </c>
       <c r="BU47" s="2">
         <v>43960</v>
@@ -6958,6 +7161,9 @@
       <c r="J48" s="10">
         <v>1</v>
       </c>
+      <c r="K48" s="10">
+        <v>1</v>
+      </c>
       <c r="BU48" s="2">
         <v>43961</v>
       </c>
@@ -6991,6 +7197,9 @@
       <c r="J49" s="10">
         <v>0</v>
       </c>
+      <c r="K49" s="10">
+        <v>0</v>
+      </c>
       <c r="BU49" s="2">
         <v>43962</v>
       </c>
@@ -7026,6 +7235,9 @@
       <c r="J50" s="10">
         <v>9</v>
       </c>
+      <c r="K50" s="10">
+        <v>13</v>
+      </c>
       <c r="BU50" s="2">
         <v>43963</v>
       </c>
@@ -7061,6 +7273,9 @@
       <c r="J51" s="10">
         <v>44</v>
       </c>
+      <c r="K51" s="10">
+        <v>62</v>
+      </c>
       <c r="BU51" s="2">
         <v>43964</v>
       </c>
@@ -7094,6 +7309,9 @@
         <v>2</v>
       </c>
       <c r="J52" s="10">
+        <v>2</v>
+      </c>
+      <c r="K52" s="10">
         <v>2</v>
       </c>
       <c r="BU52" s="2">
@@ -7129,6 +7347,9 @@
       <c r="J53" s="10">
         <v>0</v>
       </c>
+      <c r="K53" s="10">
+        <v>0</v>
+      </c>
       <c r="BU53" s="2">
         <v>43966</v>
       </c>
@@ -7162,6 +7383,9 @@
       <c r="J54" s="10">
         <v>0</v>
       </c>
+      <c r="K54" s="10">
+        <v>0</v>
+      </c>
       <c r="BU54" s="2">
         <v>43967</v>
       </c>
@@ -7195,6 +7419,9 @@
       <c r="J55" s="10">
         <v>0</v>
       </c>
+      <c r="K55" s="10">
+        <v>0</v>
+      </c>
       <c r="BU55" s="2">
         <v>43968</v>
       </c>
@@ -7229,6 +7456,9 @@
       </c>
       <c r="J56" s="10">
         <v>0</v>
+      </c>
+      <c r="K56" s="10">
+        <v>1</v>
       </c>
       <c r="BU56" s="2">
         <v>43969</v>
@@ -7263,6 +7493,9 @@
       <c r="J57" s="10">
         <v>10</v>
       </c>
+      <c r="K57" s="10">
+        <v>12</v>
+      </c>
       <c r="BU57" s="2">
         <v>43970</v>
       </c>
@@ -7296,6 +7529,9 @@
       <c r="J58" s="10">
         <v>0</v>
       </c>
+      <c r="K58" s="10">
+        <v>1</v>
+      </c>
       <c r="BU58" s="2">
         <v>43971</v>
       </c>
@@ -7329,6 +7565,9 @@
       <c r="J59" s="10">
         <v>6</v>
       </c>
+      <c r="K59" s="10">
+        <v>7</v>
+      </c>
       <c r="BU59" s="2">
         <v>43972</v>
       </c>
@@ -7362,6 +7601,9 @@
       <c r="J60" s="10">
         <v>2</v>
       </c>
+      <c r="K60" s="10">
+        <v>3</v>
+      </c>
       <c r="BU60" s="2">
         <v>43973</v>
       </c>
@@ -7395,6 +7637,9 @@
       <c r="J61" s="10">
         <v>3</v>
       </c>
+      <c r="K61" s="10">
+        <v>3</v>
+      </c>
       <c r="BU61" s="2">
         <v>43974</v>
       </c>
@@ -7430,6 +7675,9 @@
       <c r="J62" s="10">
         <v>61</v>
       </c>
+      <c r="K62" s="10">
+        <v>87</v>
+      </c>
       <c r="BU62" s="2">
         <v>43975</v>
       </c>
@@ -7463,6 +7711,9 @@
         <v>0</v>
       </c>
       <c r="J63" s="10">
+        <v>0</v>
+      </c>
+      <c r="K63" s="10">
         <v>0</v>
       </c>
       <c r="BU63" s="2">
@@ -7498,6 +7749,9 @@
       <c r="J64" s="10">
         <v>0</v>
       </c>
+      <c r="K64" s="10">
+        <v>1</v>
+      </c>
       <c r="BU64" s="2">
         <v>43977</v>
       </c>
@@ -7531,6 +7785,9 @@
       <c r="J65" s="10">
         <v>0</v>
       </c>
+      <c r="K65" s="10">
+        <v>0</v>
+      </c>
       <c r="BU65" s="2">
         <v>43978</v>
       </c>
@@ -7564,6 +7821,9 @@
       <c r="J66" s="10">
         <v>1</v>
       </c>
+      <c r="K66" s="10">
+        <v>1</v>
+      </c>
       <c r="BU66" s="2">
         <v>43979</v>
       </c>
@@ -7597,6 +7857,9 @@
       <c r="J67" s="10">
         <v>2</v>
       </c>
+      <c r="K67" s="10">
+        <v>2</v>
+      </c>
       <c r="BU67" s="2">
         <v>43980</v>
       </c>
@@ -7630,6 +7893,9 @@
       <c r="J68" s="10">
         <v>1</v>
       </c>
+      <c r="K68" s="10">
+        <v>1</v>
+      </c>
       <c r="BU68" s="2">
         <v>43981</v>
       </c>
@@ -7663,6 +7929,9 @@
       <c r="J69" s="10">
         <v>1</v>
       </c>
+      <c r="K69" s="10">
+        <v>1</v>
+      </c>
       <c r="BU69" s="2">
         <v>43982</v>
       </c>
@@ -7696,6 +7965,9 @@
       <c r="J70" s="10">
         <v>1</v>
       </c>
+      <c r="K70" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
@@ -7726,6 +7998,9 @@
         <v>0</v>
       </c>
       <c r="J71" s="10">
+        <v>0</v>
+      </c>
+      <c r="K71" s="10">
         <v>0</v>
       </c>
     </row>
@@ -7758,6 +8033,9 @@
       <c r="J72" s="10">
         <v>0</v>
       </c>
+      <c r="K72" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
@@ -7788,6 +8066,9 @@
       <c r="J73" s="10">
         <v>1</v>
       </c>
+      <c r="K73" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
@@ -7818,6 +8099,9 @@
       <c r="J74" s="10">
         <v>0</v>
       </c>
+      <c r="K74" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A75" s="20"/>
@@ -7848,6 +8132,9 @@
       <c r="J75" s="10">
         <v>1</v>
       </c>
+      <c r="K75" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
@@ -7880,6 +8167,9 @@
       <c r="J76" s="10">
         <v>17</v>
       </c>
+      <c r="K76" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="77" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
@@ -7911,6 +8201,9 @@
       </c>
       <c r="J77" s="10">
         <v>73</v>
+      </c>
+      <c r="K77" s="10">
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="1:73" x14ac:dyDescent="0.25">
@@ -7942,6 +8235,9 @@
       <c r="J78" s="10">
         <v>11</v>
       </c>
+      <c r="K78" s="10">
+        <v>14</v>
+      </c>
     </row>
     <row r="79" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
@@ -7972,6 +8268,9 @@
       <c r="J79" s="10">
         <v>18</v>
       </c>
+      <c r="K79" s="10">
+        <v>23</v>
+      </c>
     </row>
     <row r="80" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
@@ -8002,8 +8301,11 @@
       <c r="J80" s="10">
         <v>2</v>
       </c>
+      <c r="K80" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
       <c r="B81" s="1" t="s">
         <v>92</v>
@@ -8032,8 +8334,11 @@
       <c r="J81" s="10">
         <v>7</v>
       </c>
+      <c r="K81" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
         <v>19</v>
       </c>
@@ -8064,8 +8369,11 @@
       <c r="J82" s="10">
         <v>1</v>
       </c>
+      <c r="K82" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
       <c r="B83" s="1" t="s">
         <v>18</v>
@@ -8094,8 +8402,11 @@
       <c r="J83" s="10">
         <v>0</v>
       </c>
+      <c r="K83" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
       <c r="B84" s="1" t="s">
         <v>26</v>
@@ -8124,8 +8435,11 @@
       <c r="J84" s="10">
         <v>0</v>
       </c>
+      <c r="K84" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
       <c r="B85" s="1" t="s">
         <v>31</v>
@@ -8154,8 +8468,11 @@
       <c r="J85" s="10">
         <v>0</v>
       </c>
+      <c r="K85" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="1" t="s">
         <v>49</v>
@@ -8184,8 +8501,11 @@
       <c r="J86" s="10">
         <v>0</v>
       </c>
+      <c r="K86" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="1" t="s">
         <v>117</v>
@@ -8214,8 +8534,11 @@
       <c r="J87" s="10">
         <v>1</v>
       </c>
+      <c r="K87" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="23"/>
       <c r="B88" s="1" t="s">
         <v>120</v>
@@ -8244,8 +8567,11 @@
       <c r="J88" s="10">
         <v>2</v>
       </c>
+      <c r="K88" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
         <v>60</v>
       </c>
@@ -8276,8 +8602,11 @@
       <c r="J89" s="10">
         <v>1</v>
       </c>
+      <c r="K89" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="20"/>
       <c r="B90" s="1" t="s">
         <v>79</v>
@@ -8306,8 +8635,11 @@
       <c r="J90" s="10">
         <v>4</v>
       </c>
+      <c r="K90" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>148</v>
       </c>
@@ -8338,8 +8670,11 @@
       <c r="J91" s="10">
         <v>4</v>
       </c>
+      <c r="K91" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
         <v>64</v>
       </c>
@@ -8370,8 +8705,11 @@
       <c r="J92" s="10">
         <v>79</v>
       </c>
+      <c r="K92" s="10">
+        <v>94</v>
+      </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="19"/>
       <c r="B93" s="1" t="s">
         <v>144</v>
@@ -8400,8 +8738,11 @@
       <c r="J93" s="10">
         <v>7</v>
       </c>
+      <c r="K93" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
       <c r="B94" s="1" t="s">
         <v>85</v>
@@ -8430,8 +8771,11 @@
       <c r="J94" s="10">
         <v>1</v>
       </c>
+      <c r="K94" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
         <v>22</v>
       </c>
@@ -8462,8 +8806,11 @@
       <c r="J95" s="10">
         <v>0</v>
       </c>
+      <c r="K95" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="22"/>
       <c r="B96" s="1" t="s">
         <v>110</v>
@@ -8492,8 +8839,11 @@
       <c r="J96" s="10">
         <v>3</v>
       </c>
+      <c r="K96" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
       <c r="B97" s="1" t="s">
         <v>127</v>
@@ -8522,8 +8872,11 @@
       <c r="J97" s="10">
         <v>6</v>
       </c>
+      <c r="K97" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="22"/>
       <c r="B98" s="1" t="s">
         <v>128</v>
@@ -8552,8 +8905,11 @@
       <c r="J98" s="10">
         <v>20</v>
       </c>
+      <c r="K98" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="23"/>
       <c r="B99" s="1" t="s">
         <v>139</v>
@@ -8582,8 +8938,11 @@
       <c r="J99" s="10">
         <v>1</v>
       </c>
+      <c r="K99" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
         <v>30</v>
       </c>
@@ -8614,8 +8973,11 @@
       <c r="J100" s="10">
         <v>3</v>
       </c>
+      <c r="K100" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="19"/>
       <c r="B101" s="1" t="s">
         <v>100</v>
@@ -8644,8 +9006,11 @@
       <c r="J101" s="10">
         <v>6</v>
       </c>
+      <c r="K101" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="19"/>
       <c r="B102" s="1" t="s">
         <v>50</v>
@@ -8674,8 +9039,11 @@
       <c r="J102" s="10">
         <v>3</v>
       </c>
+      <c r="K102" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="19"/>
       <c r="B103" s="1" t="s">
         <v>118</v>
@@ -8704,8 +9072,11 @@
       <c r="J103" s="10">
         <v>1</v>
       </c>
+      <c r="K103" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="20"/>
       <c r="B104" s="1" t="s">
         <v>22</v>
@@ -8734,8 +9105,11 @@
       <c r="J104" s="10">
         <v>0</v>
       </c>
+      <c r="K104" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>151</v>
       </c>
@@ -8766,8 +9140,11 @@
       <c r="J105" s="10">
         <v>25</v>
       </c>
+      <c r="K105" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>153</v>
       </c>
@@ -8798,8 +9175,11 @@
       <c r="J106" s="10">
         <v>6</v>
       </c>
+      <c r="K106" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="21" t="s">
         <v>15</v>
       </c>
@@ -8830,8 +9210,11 @@
       <c r="J107" s="10">
         <v>0</v>
       </c>
+      <c r="K107" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="22"/>
       <c r="B108" s="1" t="s">
         <v>39</v>
@@ -8860,8 +9243,11 @@
       <c r="J108" s="10">
         <v>1</v>
       </c>
+      <c r="K108" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="23"/>
       <c r="B109" s="1" t="s">
         <v>114</v>
@@ -8890,8 +9276,11 @@
       <c r="J109" s="10">
         <v>4</v>
       </c>
+      <c r="K109" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
         <v>4</v>
       </c>
@@ -8922,8 +9311,11 @@
       <c r="J110" s="10">
         <v>19</v>
       </c>
+      <c r="K110" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="19"/>
       <c r="B111" s="1" t="s">
         <v>102</v>
@@ -8952,8 +9344,11 @@
       <c r="J111" s="10">
         <v>3</v>
       </c>
+      <c r="K111" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="19"/>
       <c r="B112" s="1" t="s">
         <v>37</v>
@@ -8982,8 +9377,11 @@
       <c r="J112" s="10">
         <v>1</v>
       </c>
+      <c r="K112" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="19"/>
       <c r="B113" s="1" t="s">
         <v>48</v>
@@ -9012,8 +9410,11 @@
       <c r="J113" s="10">
         <v>8</v>
       </c>
+      <c r="K113" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="19"/>
       <c r="B114" s="1" t="s">
         <v>116</v>
@@ -9042,8 +9443,11 @@
       <c r="J114" s="10">
         <v>2</v>
       </c>
+      <c r="K114" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
       <c r="B115" s="1" t="s">
         <v>134</v>
@@ -9072,8 +9476,11 @@
       <c r="J115" s="10">
         <v>13</v>
       </c>
+      <c r="K115" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="21" t="s">
         <v>35</v>
       </c>
@@ -9104,8 +9511,11 @@
       <c r="J116" s="10">
         <v>0</v>
       </c>
+      <c r="K116" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="22"/>
       <c r="B117" s="1" t="s">
         <v>106</v>
@@ -9134,8 +9544,11 @@
       <c r="J117" s="10">
         <v>7</v>
       </c>
+      <c r="K117" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="22"/>
       <c r="B118" s="1" t="s">
         <v>45</v>
@@ -9164,8 +9577,11 @@
       <c r="J118" s="10">
         <v>0</v>
       </c>
+      <c r="K118" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="22"/>
       <c r="B119" s="1" t="s">
         <v>111</v>
@@ -9194,8 +9610,11 @@
       <c r="J119" s="10">
         <v>1</v>
       </c>
+      <c r="K119" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="22"/>
       <c r="B120" s="1" t="s">
         <v>112</v>
@@ -9224,8 +9643,11 @@
       <c r="J120" s="10">
         <v>1</v>
       </c>
+      <c r="K120" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="22"/>
       <c r="B121" s="1" t="s">
         <v>51</v>
@@ -9254,8 +9676,11 @@
       <c r="J121" s="10">
         <v>2</v>
       </c>
+      <c r="K121" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="22"/>
       <c r="B122" s="1" t="s">
         <v>52</v>
@@ -9284,8 +9709,11 @@
       <c r="J122" s="10">
         <v>0</v>
       </c>
+      <c r="K122" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="22"/>
       <c r="B123" s="1" t="s">
         <v>56</v>
@@ -9314,8 +9742,11 @@
       <c r="J123" s="10">
         <v>2</v>
       </c>
+      <c r="K123" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="22"/>
       <c r="B124" s="1" t="s">
         <v>121</v>
@@ -9344,8 +9775,11 @@
       <c r="J124" s="10">
         <v>0</v>
       </c>
+      <c r="K124" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="23"/>
       <c r="B125" s="1" t="s">
         <v>72</v>
@@ -9374,8 +9808,11 @@
       <c r="J125" s="10">
         <v>0</v>
       </c>
+      <c r="K125" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>156</v>
       </c>
@@ -9406,8 +9843,11 @@
       <c r="J126" s="10">
         <v>52</v>
       </c>
+      <c r="K126" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
         <v>58</v>
       </c>
@@ -9438,8 +9878,11 @@
       <c r="J127" s="10">
         <v>5</v>
       </c>
+      <c r="K127" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="22"/>
       <c r="B128" s="1" t="s">
         <v>108</v>
@@ -9466,6 +9909,9 @@
         <v>0</v>
       </c>
       <c r="J128" s="10">
+        <v>1</v>
+      </c>
+      <c r="K128" s="10">
         <v>1</v>
       </c>
     </row>
@@ -9498,6 +9944,9 @@
       <c r="J129" s="10">
         <v>0</v>
       </c>
+      <c r="K129" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A130" s="23"/>
@@ -9528,6 +9977,9 @@
       <c r="J130" s="10">
         <v>0</v>
       </c>
+      <c r="K130" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A131" s="18" t="s">
@@ -9559,6 +10011,9 @@
       </c>
       <c r="J131" s="10">
         <v>3</v>
+      </c>
+      <c r="K131" s="10">
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:72" x14ac:dyDescent="0.25">
@@ -9590,6 +10045,9 @@
       <c r="J132" s="10">
         <v>1</v>
       </c>
+      <c r="K132" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A133" s="19"/>
@@ -9620,6 +10078,9 @@
       <c r="J133" s="10">
         <v>0</v>
       </c>
+      <c r="K133" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="134" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A134" s="20"/>
@@ -9650,6 +10111,9 @@
       <c r="J134" s="10">
         <v>3</v>
       </c>
+      <c r="K134" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="136" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B136" s="10" t="s">
@@ -9681,7 +10145,7 @@
       </c>
       <c r="K136" s="10">
         <f>SUM(va[31-Mar])</f>
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="L136" s="10">
         <f>SUM(va[1-Apr])</f>
@@ -9951,7 +10415,7 @@
         <v>136</v>
       </c>
       <c r="K137" s="10">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="L137" s="10">
         <v>0</v>
@@ -10160,7 +10624,7 @@
         <v>25</v>
       </c>
       <c r="K138" s="10">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L138" s="10">
         <v>0</v>
@@ -10369,7 +10833,7 @@
         <v>12038</v>
       </c>
       <c r="K139" s="10">
-        <v>0</v>
+        <v>13401</v>
       </c>
       <c r="L139" s="10">
         <v>0</v>
@@ -12784,7 +13248,7 @@
       </c>
       <c r="G2" s="14">
         <f>MAX(0,(md!G2-md!F2))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H2" s="14">
         <f>MAX(0,(md!H2-md!G2))</f>
@@ -13056,7 +13520,7 @@
       </c>
       <c r="G3" s="14">
         <f>MAX(0,(md!G3-md!F3))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="H3" s="14">
         <f>MAX(0,(md!H3-md!G3))</f>
@@ -13328,7 +13792,7 @@
       </c>
       <c r="G4" s="14">
         <f>MAX(0,(md!G4-md!F4))</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="H4" s="14">
         <f>MAX(0,(md!H4-md!G4))</f>
@@ -13600,7 +14064,7 @@
       </c>
       <c r="G5" s="14">
         <f>MAX(0,(md!G5-md!F5))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="14">
         <f>MAX(0,(md!H5-md!G5))</f>
@@ -14144,7 +14608,7 @@
       </c>
       <c r="G7" s="14">
         <f>MAX(0,(md!G7-md!F7))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H7" s="14">
         <f>MAX(0,(md!H7-md!G7))</f>
@@ -14416,7 +14880,7 @@
       </c>
       <c r="G8" s="14">
         <f>MAX(0,(md!G8-md!F8))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="14">
         <f>MAX(0,(md!H8-md!G8))</f>
@@ -14688,7 +15152,7 @@
       </c>
       <c r="G9" s="14">
         <f>MAX(0,(md!G9-md!F9))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H9" s="14">
         <f>MAX(0,(md!H9-md!G9))</f>
@@ -14960,7 +15424,7 @@
       </c>
       <c r="G10" s="14">
         <f>MAX(0,(md!G10-md!F10))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H10" s="14">
         <f>MAX(0,(md!H10-md!G10))</f>
@@ -15504,7 +15968,7 @@
       </c>
       <c r="G12" s="14">
         <f>MAX(0,(md!G12-md!F12))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="14">
         <f>MAX(0,(md!H12-md!G12))</f>
@@ -15776,7 +16240,7 @@
       </c>
       <c r="G13" s="14">
         <f>MAX(0,(md!G13-md!F13))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H13" s="14">
         <f>MAX(0,(md!H13-md!G13))</f>
@@ -16320,7 +16784,7 @@
       </c>
       <c r="G15" s="14">
         <f>MAX(0,(md!G15-md!F15))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H15" s="14">
         <f>MAX(0,(md!H15-md!G15))</f>
@@ -16592,7 +17056,7 @@
       </c>
       <c r="G16" s="14">
         <f>MAX(0,(md!G16-md!F16))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H16" s="14">
         <f>MAX(0,(md!H16-md!G16))</f>
@@ -17136,7 +17600,7 @@
       </c>
       <c r="G18" s="14">
         <f>MAX(0,(md!G18-md!F18))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H18" s="14">
         <f>MAX(0,(md!H18-md!G18))</f>
@@ -17952,7 +18416,7 @@
       </c>
       <c r="G21" s="14">
         <f>MAX(0,(md!G21-md!F21))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="14">
         <f>MAX(0,(md!H21-md!G21))</f>
@@ -18224,7 +18688,7 @@
       </c>
       <c r="G22" s="14">
         <f>MAX(0,(md!G22-md!F22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="14">
         <f>MAX(0,(md!H22-md!G22))</f>
@@ -18771,7 +19235,7 @@
       </c>
       <c r="G25" s="14">
         <f>MAX(0,(md!G25-md!F25))</f>
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="H25" s="14">
         <f>MAX(0,(md!H25-md!G25))</f>
@@ -19043,7 +19507,7 @@
       </c>
       <c r="G26" s="14">
         <f>MAX(0,(md!G26-md!F26))</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="H26" s="14">
         <f>MAX(0,(md!H26-md!G26))</f>
@@ -19315,7 +19779,7 @@
       </c>
       <c r="G27" s="14">
         <f>MAX(0,(md!G27-md!F27))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27" s="14">
         <f>MAX(0,(md!H27-md!G27))</f>
@@ -19648,8 +20112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10B5AF9-8E42-4F8B-8F58-724C1869D2EC}">
   <dimension ref="A1:BU141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M147" sqref="M147"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19918,7 +20382,7 @@
       </c>
       <c r="K2" s="16">
         <f>MAX(0,(va!K2-va!J2))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L2" s="16">
         <f>MAX(0,(va!L2-va!K2))</f>
@@ -21064,7 +21528,7 @@
       </c>
       <c r="K6" s="16">
         <f>MAX(0,(va!K6-va!J6))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="16">
         <f>MAX(0,(va!L6-va!K6))</f>
@@ -21924,7 +22388,7 @@
       </c>
       <c r="K9" s="16">
         <f>MAX(0,(va!K9-va!J9))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L9" s="16">
         <f>MAX(0,(va!L9-va!K9))</f>
@@ -24786,7 +25250,7 @@
       </c>
       <c r="K19" s="16">
         <f>MAX(0,(va!K19-va!J19))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19" s="16">
         <f>MAX(0,(va!L19-va!K19))</f>
@@ -25932,7 +26396,7 @@
       </c>
       <c r="K23" s="16">
         <f>MAX(0,(va!K23-va!J23))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="16">
         <f>MAX(0,(va!L23-va!K23))</f>
@@ -26218,7 +26682,7 @@
       </c>
       <c r="K24" s="16">
         <f>MAX(0,(va!K24-va!J24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="16">
         <f>MAX(0,(va!L24-va!K24))</f>
@@ -26506,7 +26970,7 @@
       </c>
       <c r="K25" s="16">
         <f>MAX(0,(va!K25-va!J25))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L25" s="16">
         <f>MAX(0,(va!L25-va!K25))</f>
@@ -26794,7 +27258,7 @@
       </c>
       <c r="K26" s="16">
         <f>MAX(0,(va!K26-va!J26))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L26" s="16">
         <f>MAX(0,(va!L26-va!K26))</f>
@@ -27080,7 +27544,7 @@
       </c>
       <c r="K27" s="16">
         <f>MAX(0,(va!K27-va!J27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="16">
         <f>MAX(0,(va!L27-va!K27))</f>
@@ -27940,7 +28404,7 @@
       </c>
       <c r="K30" s="16">
         <f>MAX(0,(va!K30-va!J30))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="16">
         <f>MAX(0,(va!L30-va!K30))</f>
@@ -28226,7 +28690,7 @@
       </c>
       <c r="K31" s="16">
         <f>MAX(0,(va!K31-va!J31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" s="16">
         <f>MAX(0,(va!L31-va!K31))</f>
@@ -29372,7 +29836,7 @@
       </c>
       <c r="K35" s="16">
         <f>MAX(0,(va!K35-va!J35))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L35" s="16">
         <f>MAX(0,(va!L35-va!K35))</f>
@@ -29658,7 +30122,7 @@
       </c>
       <c r="K36" s="16">
         <f>MAX(0,(va!K36-va!J36))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" s="16">
         <f>MAX(0,(va!L36-va!K36))</f>
@@ -30516,7 +30980,7 @@
       </c>
       <c r="K39" s="16">
         <f>MAX(0,(va!K39-va!J39))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="16">
         <f>MAX(0,(va!L39-va!K39))</f>
@@ -32236,7 +32700,7 @@
       </c>
       <c r="K45" s="16">
         <f>MAX(0,(va!K45-va!J45))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" s="16">
         <f>MAX(0,(va!L45-va!K45))</f>
@@ -32810,7 +33274,7 @@
       </c>
       <c r="K47" s="16">
         <f>MAX(0,(va!K47-va!J47))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L47" s="16">
         <f>MAX(0,(va!L47-va!K47))</f>
@@ -33670,7 +34134,7 @@
       </c>
       <c r="K50" s="16">
         <f>MAX(0,(va!K50-va!J50))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L50" s="16">
         <f>MAX(0,(va!L50-va!K50))</f>
@@ -33958,7 +34422,7 @@
       </c>
       <c r="K51" s="16">
         <f>MAX(0,(va!K51-va!J51))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L51" s="16">
         <f>MAX(0,(va!L51-va!K51))</f>
@@ -35392,7 +35856,7 @@
       </c>
       <c r="K56" s="16">
         <f>MAX(0,(va!K56-va!J56))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" s="16">
         <f>MAX(0,(va!L56-va!K56))</f>
@@ -35678,7 +36142,7 @@
       </c>
       <c r="K57" s="16">
         <f>MAX(0,(va!K57-va!J57))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L57" s="16">
         <f>MAX(0,(va!L57-va!K57))</f>
@@ -35964,7 +36428,7 @@
       </c>
       <c r="K58" s="16">
         <f>MAX(0,(va!K58-va!J58))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" s="16">
         <f>MAX(0,(va!L58-va!K58))</f>
@@ -36250,7 +36714,7 @@
       </c>
       <c r="K59" s="16">
         <f>MAX(0,(va!K59-va!J59))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59" s="16">
         <f>MAX(0,(va!L59-va!K59))</f>
@@ -36536,7 +37000,7 @@
       </c>
       <c r="K60" s="16">
         <f>MAX(0,(va!K60-va!J60))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" s="16">
         <f>MAX(0,(va!L60-va!K60))</f>
@@ -37110,7 +37574,7 @@
       </c>
       <c r="K62" s="16">
         <f>MAX(0,(va!K62-va!J62))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="L62" s="16">
         <f>MAX(0,(va!L62-va!K62))</f>
@@ -37684,7 +38148,7 @@
       </c>
       <c r="K64" s="16">
         <f>MAX(0,(va!K64-va!J64))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L64" s="16">
         <f>MAX(0,(va!L64-va!K64))</f>
@@ -41102,7 +41566,7 @@
       </c>
       <c r="K76" s="16">
         <f>MAX(0,(va!K76-va!J76))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L76" s="16">
         <f>MAX(0,(va!L76-va!K76))</f>
@@ -41387,7 +41851,7 @@
       </c>
       <c r="K77" s="16">
         <f>MAX(0,(va!K77-va!J77))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L77" s="16">
         <f>MAX(0,(va!L77-va!K77))</f>
@@ -41670,7 +42134,7 @@
       </c>
       <c r="K78" s="16">
         <f>MAX(0,(va!K78-va!J78))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L78" s="16">
         <f>MAX(0,(va!L78-va!K78))</f>
@@ -41953,7 +42417,7 @@
       </c>
       <c r="K79" s="16">
         <f>MAX(0,(va!K79-va!J79))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L79" s="16">
         <f>MAX(0,(va!L79-va!K79))</f>
@@ -42519,7 +42983,7 @@
       </c>
       <c r="K81" s="16">
         <f>MAX(0,(va!K81-va!J81))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L81" s="16">
         <f>MAX(0,(va!L81-va!K81))</f>
@@ -42804,7 +43268,7 @@
       </c>
       <c r="K82" s="16">
         <f>MAX(0,(va!K82-va!J82))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L82" s="16">
         <f>MAX(0,(va!L82-va!K82))</f>
@@ -43087,7 +43551,7 @@
       </c>
       <c r="K83" s="16">
         <f>MAX(0,(va!K83-va!J83))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L83" s="16">
         <f>MAX(0,(va!L83-va!K83))</f>
@@ -45355,7 +45819,7 @@
       </c>
       <c r="K91" s="16">
         <f>MAX(0,(va!K91-va!J91))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L91" s="16">
         <f>MAX(0,(va!L91-va!K91))</f>
@@ -45640,7 +46104,7 @@
       </c>
       <c r="K92" s="16">
         <f>MAX(0,(va!K92-va!J92))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L92" s="16">
         <f>MAX(0,(va!L92-va!K92))</f>
@@ -45923,7 +46387,7 @@
       </c>
       <c r="K93" s="16">
         <f>MAX(0,(va!K93-va!J93))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L93" s="16">
         <f>MAX(0,(va!L93-va!K93))</f>
@@ -47057,7 +47521,7 @@
       </c>
       <c r="K97" s="16">
         <f>MAX(0,(va!K97-va!J97))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L97" s="16">
         <f>MAX(0,(va!L97-va!K97))</f>
@@ -47340,7 +47804,7 @@
       </c>
       <c r="K98" s="16">
         <f>MAX(0,(va!K98-va!J98))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L98" s="16">
         <f>MAX(0,(va!L98-va!K98))</f>
@@ -48191,7 +48655,7 @@
       </c>
       <c r="K101" s="16">
         <f>MAX(0,(va!K101-va!J101))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101" s="16">
         <f>MAX(0,(va!L101-va!K101))</f>
@@ -48757,7 +49221,7 @@
       </c>
       <c r="K103" s="16">
         <f>MAX(0,(va!K103-va!J103))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L103" s="16">
         <f>MAX(0,(va!L103-va!K103))</f>
@@ -49325,7 +49789,7 @@
       </c>
       <c r="K105" s="16">
         <f>MAX(0,(va!K105-va!J105))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L105" s="16">
         <f>MAX(0,(va!L105-va!K105))</f>
@@ -49895,7 +50359,7 @@
       </c>
       <c r="K107" s="16">
         <f>MAX(0,(va!K107-va!J107))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L107" s="16">
         <f>MAX(0,(va!L107-va!K107))</f>
@@ -50746,7 +51210,7 @@
       </c>
       <c r="K110" s="16">
         <f>MAX(0,(va!K110-va!J110))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L110" s="16">
         <f>MAX(0,(va!L110-va!K110))</f>
@@ -51595,7 +52059,7 @@
       </c>
       <c r="K113" s="16">
         <f>MAX(0,(va!K113-va!J113))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L113" s="16">
         <f>MAX(0,(va!L113-va!K113))</f>
@@ -52161,7 +52625,7 @@
       </c>
       <c r="K115" s="16">
         <f>MAX(0,(va!K115-va!J115))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L115" s="16">
         <f>MAX(0,(va!L115-va!K115))</f>
@@ -53012,7 +53476,7 @@
       </c>
       <c r="K118" s="16">
         <f>MAX(0,(va!K118-va!J118))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L118" s="16">
         <f>MAX(0,(va!L118-va!K118))</f>
@@ -54427,7 +54891,7 @@
       </c>
       <c r="K123" s="16">
         <f>MAX(0,(va!K123-va!J123))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L123" s="16">
         <f>MAX(0,(va!L123-va!K123))</f>
@@ -55278,7 +55742,7 @@
       </c>
       <c r="K126" s="16">
         <f>MAX(0,(va!K126-va!J126))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L126" s="16">
         <f>MAX(0,(va!L126-va!K126))</f>
@@ -56697,7 +57161,7 @@
       </c>
       <c r="K131" s="16">
         <f>MAX(0,(va!K131-va!J131))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L131" s="16">
         <f>MAX(0,(va!L131-va!K131))</f>
@@ -57263,7 +57727,7 @@
       </c>
       <c r="K133" s="16">
         <f>MAX(0,(va!K133-va!J133))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L133" s="16">
         <f>MAX(0,(va!L133-va!K133))</f>
@@ -57546,7 +58010,7 @@
       </c>
       <c r="K134" s="16">
         <f>MAX(0,(va!K134-va!J134))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L134" s="16">
         <f>MAX(0,(va!L134-va!K134))</f>
@@ -57823,7 +58287,7 @@
       </c>
       <c r="K136" s="14">
         <f>MAX(0,(va!K136-va!J136))</f>
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="L136" s="14">
         <f>MAX(0,(va!L136-va!K136))</f>
@@ -58100,7 +58564,7 @@
       </c>
       <c r="K137" s="14">
         <f>MAX(0,(va!K137-va!J137))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="L137" s="14">
         <f>MAX(0,(va!L137-va!K137))</f>
@@ -58377,7 +58841,7 @@
       </c>
       <c r="K138" s="14">
         <f>MAX(0,(va!K138-va!J138))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L138" s="14">
         <f>MAX(0,(va!L138-va!K138))</f>
@@ -58654,7 +59118,7 @@
       </c>
       <c r="K139" s="14">
         <f>MAX(0,(va!K139-va!J139))</f>
-        <v>0</v>
+        <v>1363</v>
       </c>
       <c r="L139" s="14">
         <f>MAX(0,(va!L139-va!K139))</f>

</xml_diff>

<commit_message>
06 April updt & std rows for easy ingest
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEBAB8E-C701-4575-99FF-59C4CC821BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392A7B96-2A12-4A72-8692-B02DACD8F35D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="27580" windowHeight="18000" tabRatio="685" activeTab="3" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="360" yWindow="1080" windowWidth="15980" windowHeight="11520" tabRatio="685" activeTab="5" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1047,6 +1047,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1054,15 +1063,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3700,9 +3700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B685ED27-8882-4CE7-837C-253FB4ACFF90}">
   <dimension ref="A1:BQ31"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:BQ31"/>
-    </sheetView>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3735,10 +3733,10 @@
         <v>11516</v>
       </c>
       <c r="F2" s="10">
-        <v>0</v>
+        <v>12354</v>
       </c>
       <c r="G2" s="10">
-        <v>0</v>
+        <v>13316</v>
       </c>
       <c r="H2" s="10">
         <v>14868</v>
@@ -4207,7 +4205,7 @@
         <v>132</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="E4" s="10">
         <v>226</v>
@@ -7168,7 +7166,7 @@
       </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="23" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -7221,7 +7219,7 @@
       </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -7272,7 +7270,7 @@
       </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -7323,7 +7321,7 @@
       </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -7374,7 +7372,7 @@
       </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -7425,7 +7423,7 @@
       </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -7529,7 +7527,7 @@
       </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -7582,7 +7580,7 @@
       </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -7633,7 +7631,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -7684,7 +7682,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -7735,7 +7733,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -7786,7 +7784,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -7837,7 +7835,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" s="27"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -7888,7 +7886,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A22" s="27"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -7939,7 +7937,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23" s="27"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -7990,7 +7988,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -8041,7 +8039,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="26" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -8094,7 +8092,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" s="24"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -8145,7 +8143,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A27" s="24"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -8196,7 +8194,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28" s="24"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -8247,7 +8245,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A29" s="25"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -8351,7 +8349,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="26" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -8404,7 +8402,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A32" s="24"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -8455,7 +8453,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -8506,7 +8504,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="23" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -8559,7 +8557,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -8610,7 +8608,7 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -8661,7 +8659,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="28"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -8712,7 +8710,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -8765,7 +8763,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A39" s="24"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -8816,7 +8814,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A40" s="24"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -8867,7 +8865,7 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" s="24"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -8918,7 +8916,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A42" s="24"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -8969,7 +8967,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A43" s="24"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -9020,7 +9018,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A44" s="24"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -9071,7 +9069,7 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A45" s="25"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -9122,7 +9120,7 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -9175,7 +9173,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A47" s="27"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -9226,7 +9224,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="27"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -9277,7 +9275,7 @@
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A49" s="28"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -9328,7 +9326,7 @@
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -9381,7 +9379,7 @@
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A51" s="25"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -9432,7 +9430,7 @@
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="23" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -9485,7 +9483,7 @@
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A53" s="27"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -9536,7 +9534,7 @@
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A54" s="28"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -9693,7 +9691,7 @@
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="26" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -9746,7 +9744,7 @@
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A58" s="24"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -9797,7 +9795,7 @@
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A59" s="24"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -9848,7 +9846,7 @@
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A60" s="25"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -9899,7 +9897,7 @@
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -9952,7 +9950,7 @@
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A62" s="27"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -10003,7 +10001,7 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A63" s="27"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -10054,7 +10052,7 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A64" s="27"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -10105,7 +10103,7 @@
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A65" s="27"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -10156,7 +10154,7 @@
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A66" s="28"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -10260,7 +10258,7 @@
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A68" s="26" t="s">
+      <c r="A68" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -10313,7 +10311,7 @@
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A69" s="27"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -10364,7 +10362,7 @@
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A70" s="27"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -10415,7 +10413,7 @@
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A71" s="27"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -10466,7 +10464,7 @@
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A72" s="27"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -10517,7 +10515,7 @@
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A73" s="27"/>
+      <c r="A73" s="24"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -10568,7 +10566,7 @@
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A74" s="27"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -10619,7 +10617,7 @@
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A75" s="28"/>
+      <c r="A75" s="25"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -10670,7 +10668,7 @@
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A76" s="23" t="s">
+      <c r="A76" s="26" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -10723,7 +10721,7 @@
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A77" s="24"/>
+      <c r="A77" s="27"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -10774,7 +10772,7 @@
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A78" s="24"/>
+      <c r="A78" s="27"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -10825,7 +10823,7 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A79" s="24"/>
+      <c r="A79" s="27"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -10876,7 +10874,7 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A80" s="25"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -10980,7 +10978,7 @@
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A82" s="23" t="s">
+      <c r="A82" s="26" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -11033,7 +11031,7 @@
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A83" s="24"/>
+      <c r="A83" s="27"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -11084,7 +11082,7 @@
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A84" s="24"/>
+      <c r="A84" s="27"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -11135,7 +11133,7 @@
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A85" s="24"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -11186,7 +11184,7 @@
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A86" s="25"/>
+      <c r="A86" s="28"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -11237,7 +11235,7 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A87" s="26" t="s">
+      <c r="A87" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -11290,7 +11288,7 @@
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A88" s="27"/>
+      <c r="A88" s="24"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -11341,7 +11339,7 @@
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A89" s="27"/>
+      <c r="A89" s="24"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -11392,7 +11390,7 @@
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A90" s="27"/>
+      <c r="A90" s="24"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -11443,7 +11441,7 @@
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A91" s="27"/>
+      <c r="A91" s="24"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -11494,7 +11492,7 @@
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A92" s="27"/>
+      <c r="A92" s="24"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -11545,7 +11543,7 @@
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A93" s="28"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -11596,7 +11594,7 @@
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A94" s="23" t="s">
+      <c r="A94" s="26" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -11649,7 +11647,7 @@
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A95" s="25"/>
+      <c r="A95" s="28"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -11753,7 +11751,7 @@
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A97" s="23" t="s">
+      <c r="A97" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -11806,7 +11804,7 @@
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A98" s="24"/>
+      <c r="A98" s="27"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -11857,7 +11855,7 @@
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A99" s="25"/>
+      <c r="A99" s="28"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -11908,7 +11906,7 @@
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A100" s="26" t="s">
+      <c r="A100" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -11961,7 +11959,7 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A101" s="27"/>
+      <c r="A101" s="24"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -12012,7 +12010,7 @@
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A102" s="27"/>
+      <c r="A102" s="24"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -12063,7 +12061,7 @@
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A103" s="27"/>
+      <c r="A103" s="24"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -12114,7 +12112,7 @@
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A104" s="28"/>
+      <c r="A104" s="25"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -12165,7 +12163,7 @@
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A105" s="23" t="s">
+      <c r="A105" s="26" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -12218,7 +12216,7 @@
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A106" s="24"/>
+      <c r="A106" s="27"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -12269,7 +12267,7 @@
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A107" s="24"/>
+      <c r="A107" s="27"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -12320,7 +12318,7 @@
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A108" s="24"/>
+      <c r="A108" s="27"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -12371,7 +12369,7 @@
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A109" s="25"/>
+      <c r="A109" s="28"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -12528,7 +12526,7 @@
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A112" s="26" t="s">
+      <c r="A112" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -12581,7 +12579,7 @@
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A113" s="27"/>
+      <c r="A113" s="24"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -12632,7 +12630,7 @@
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A114" s="28"/>
+      <c r="A114" s="25"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -12683,7 +12681,7 @@
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A115" s="23" t="s">
+      <c r="A115" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -12736,7 +12734,7 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A116" s="24"/>
+      <c r="A116" s="27"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -12787,7 +12785,7 @@
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A117" s="24"/>
+      <c r="A117" s="27"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -12838,7 +12836,7 @@
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A118" s="24"/>
+      <c r="A118" s="27"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -12889,7 +12887,7 @@
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A119" s="24"/>
+      <c r="A119" s="27"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -12940,7 +12938,7 @@
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A120" s="25"/>
+      <c r="A120" s="28"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -12991,7 +12989,7 @@
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A121" s="26" t="s">
+      <c r="A121" s="23" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -13044,7 +13042,7 @@
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A122" s="27"/>
+      <c r="A122" s="24"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -13095,7 +13093,7 @@
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A123" s="27"/>
+      <c r="A123" s="24"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -13146,7 +13144,7 @@
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A124" s="27"/>
+      <c r="A124" s="24"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -13197,7 +13195,7 @@
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A125" s="27"/>
+      <c r="A125" s="24"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -13248,7 +13246,7 @@
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A126" s="27"/>
+      <c r="A126" s="24"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -13299,7 +13297,7 @@
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A127" s="27"/>
+      <c r="A127" s="24"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -13350,7 +13348,7 @@
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A128" s="27"/>
+      <c r="A128" s="24"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -13401,7 +13399,7 @@
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A129" s="27"/>
+      <c r="A129" s="24"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -13452,7 +13450,7 @@
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A130" s="28"/>
+      <c r="A130" s="25"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -13556,7 +13554,7 @@
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A132" s="26" t="s">
+      <c r="A132" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -13609,7 +13607,7 @@
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A133" s="27"/>
+      <c r="A133" s="24"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -13660,7 +13658,7 @@
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A134" s="27"/>
+      <c r="A134" s="24"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -13711,7 +13709,7 @@
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A135" s="28"/>
+      <c r="A135" s="25"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -13762,7 +13760,7 @@
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A136" s="23" t="s">
+      <c r="A136" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -13815,7 +13813,7 @@
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A137" s="24"/>
+      <c r="A137" s="27"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -13866,7 +13864,7 @@
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A138" s="24"/>
+      <c r="A138" s="27"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -13917,7 +13915,7 @@
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A139" s="25"/>
+      <c r="A139" s="28"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -13969,6 +13967,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -13981,18 +13991,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -14080,7 +14078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F4047C-2E48-45D8-A0A4-C3935E342FF1}">
   <dimension ref="A1:CC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -14103,323 +14101,323 @@
         <v>270</v>
       </c>
       <c r="B2" s="19">
-        <f>(B7/MAX(B6,1))*100</f>
+        <f t="shared" ref="B2:AG2" si="0">(B7/MAX(B6,1))*100</f>
         <v>0</v>
       </c>
       <c r="C2" s="19">
-        <f>(C7/MAX(C6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>13.043478260869565</v>
       </c>
       <c r="D2" s="19">
-        <f>(D7/MAX(D6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="E2" s="19">
-        <f>(E7/MAX(E6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>83.333333333333343</v>
       </c>
       <c r="F2" s="19">
-        <f>(F7/MAX(F6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>20.454545454545457</v>
       </c>
       <c r="G2" s="19">
-        <f>(G7/MAX(G6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>24.242424242424242</v>
       </c>
       <c r="H2" s="19">
-        <f>(H7/MAX(H6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>8.6486486486486491</v>
       </c>
       <c r="I2" s="19">
-        <f>(I7/MAX(I6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="J2" s="19">
-        <f>(J7/MAX(J6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>1.9905213270142181</v>
       </c>
       <c r="K2" s="19">
-        <f>(K7/MAX(K6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>10.344827586206897</v>
       </c>
       <c r="L2" s="19">
-        <f>(L7/MAX(L6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>18.260869565217391</v>
       </c>
       <c r="M2" s="19">
-        <f>(M7/MAX(M6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>17.358490566037734</v>
       </c>
       <c r="N2" s="19">
-        <f>(N7/MAX(N6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>19.277108433734941</v>
       </c>
       <c r="O2" s="19">
-        <f>(O7/MAX(O6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>11.688311688311687</v>
       </c>
       <c r="P2" s="19">
-        <f>(P7/MAX(P6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>10.571428571428571</v>
       </c>
       <c r="Q2" s="19">
-        <f>(Q7/MAX(Q6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>12.837837837837837</v>
       </c>
       <c r="R2" s="19">
-        <f>(R7/MAX(R6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>21.611721611721613</v>
       </c>
       <c r="S2" s="19">
-        <f>(S7/MAX(S6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>13.94658753709199</v>
       </c>
       <c r="T2" s="19">
-        <f>(T7/MAX(T6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>14.241001564945227</v>
       </c>
       <c r="U2" s="19">
-        <f>(U7/MAX(U6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>9.9702380952380967</v>
       </c>
       <c r="V2" s="19">
-        <f>(V7/MAX(V6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>20.233463035019454</v>
       </c>
       <c r="W2" s="19">
-        <f>(W7/MAX(W6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>16.978922716627633</v>
       </c>
       <c r="X2" s="19">
-        <f>(X7/MAX(X6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>24.242424242424242</v>
       </c>
       <c r="Y2" s="19">
-        <f>(Y7/MAX(Y6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>15.993537964458804</v>
       </c>
       <c r="Z2" s="19">
-        <f>(Z7/MAX(Z6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA2" s="19">
-        <f>(AA7/MAX(AA6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB2" s="19">
-        <f>(AB7/MAX(AB6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC2" s="19">
-        <f>(AC7/MAX(AC6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD2" s="19">
-        <f>(AD7/MAX(AD6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE2" s="19">
-        <f>(AE7/MAX(AE6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF2" s="19">
-        <f>(AF7/MAX(AF6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG2" s="19">
-        <f>(AG7/MAX(AG6,1))*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH2" s="19">
-        <f>(AH7/MAX(AH6,1))*100</f>
+        <f t="shared" ref="AH2:BM2" si="1">(AH7/MAX(AH6,1))*100</f>
         <v>0</v>
       </c>
       <c r="AI2" s="19">
-        <f>(AI7/MAX(AI6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ2" s="19">
-        <f>(AJ7/MAX(AJ6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK2" s="19">
-        <f>(AK7/MAX(AK6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL2" s="19">
-        <f>(AL7/MAX(AL6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM2" s="19">
-        <f>(AM7/MAX(AM6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN2" s="19">
-        <f>(AN7/MAX(AN6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO2" s="19">
-        <f>(AO7/MAX(AO6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP2" s="19">
-        <f>(AP7/MAX(AP6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ2" s="19">
-        <f>(AQ7/MAX(AQ6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR2" s="19">
-        <f>(AR7/MAX(AR6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AS2" s="19">
-        <f>(AS7/MAX(AS6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AT2" s="19">
-        <f>(AT7/MAX(AT6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU2" s="19">
-        <f>(AU7/MAX(AU6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AV2" s="19">
-        <f>(AV7/MAX(AV6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AW2" s="19">
-        <f>(AW7/MAX(AW6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AX2" s="19">
-        <f>(AX7/MAX(AX6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AY2" s="19">
-        <f>(AY7/MAX(AY6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AZ2" s="19">
-        <f>(AZ7/MAX(AZ6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BA2" s="19">
-        <f>(BA7/MAX(BA6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BB2" s="19">
-        <f>(BB7/MAX(BB6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BC2" s="19">
-        <f>(BC7/MAX(BC6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BD2" s="19">
-        <f>(BD7/MAX(BD6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BE2" s="19">
-        <f>(BE7/MAX(BE6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BF2" s="19">
-        <f>(BF7/MAX(BF6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BG2" s="19">
-        <f>(BG7/MAX(BG6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BH2" s="19">
-        <f>(BH7/MAX(BH6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BI2" s="19">
-        <f>(BI7/MAX(BI6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BJ2" s="19">
-        <f>(BJ7/MAX(BJ6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BK2" s="19">
-        <f>(BK7/MAX(BK6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BL2" s="19">
-        <f>(BL7/MAX(BL6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BM2" s="19">
-        <f>(BM7/MAX(BM6,1))*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BN2" s="19">
-        <f>(BN7/MAX(BN6,1))*100</f>
+        <f t="shared" ref="BN2:CC2" si="2">(BN7/MAX(BN6,1))*100</f>
         <v>0</v>
       </c>
       <c r="BO2" s="19">
-        <f>(BO7/MAX(BO6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BP2" s="19">
-        <f>(BP7/MAX(BP6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BQ2" s="19">
-        <f>(BQ7/MAX(BQ6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BR2" s="19">
-        <f>(BR7/MAX(BR6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BS2" s="19">
-        <f>(BS7/MAX(BS6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BT2" s="19">
-        <f>(BT7/MAX(BT6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BU2" s="19">
-        <f>(BU7/MAX(BU6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BV2" s="19">
-        <f>(BV7/MAX(BV6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BW2" s="19">
-        <f>(BW7/MAX(BW6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BX2" s="19">
-        <f>(BX7/MAX(BX6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BY2" s="19">
-        <f>(BY7/MAX(BY6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BZ2" s="19">
-        <f>(BZ7/MAX(BZ6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CA2" s="19">
-        <f>(CA7/MAX(CA6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CB2" s="19">
-        <f>(CB7/MAX(CB6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CC2" s="19">
-        <f>(CC7/MAX(CC6,1))*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -14428,323 +14426,323 @@
         <v>271</v>
       </c>
       <c r="B3" s="22">
-        <f>(B8/MAX(1,B7))*100</f>
+        <f t="shared" ref="B3:AG3" si="3">(B8/MAX(1,B7))*100</f>
         <v>0</v>
       </c>
       <c r="C3" s="22">
-        <f>(C8/MAX(1,C7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D3" s="22">
-        <f>(D8/MAX(1,D7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E3" s="22">
-        <f>(E8/MAX(1,E7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F3" s="22">
-        <f>(F8/MAX(1,F7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G3" s="22">
-        <f>(G8/MAX(1,G7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H3" s="22">
-        <f>(H8/MAX(1,H7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I3" s="22">
-        <f>(I8/MAX(1,I7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J3" s="22">
-        <f>(J8/MAX(1,J7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K3" s="22">
-        <f>(K8/MAX(1,K7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L3" s="22">
-        <f>(L8/MAX(1,L7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M3" s="22">
-        <f>(M8/MAX(1,M7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N3" s="22">
-        <f>(N8/MAX(1,N7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O3" s="22">
-        <f>(O8/MAX(1,O7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P3" s="22">
-        <f>(P8/MAX(1,P7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q3" s="22">
-        <f>(Q8/MAX(1,Q7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R3" s="22">
-        <f>(R8/MAX(1,R7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S3" s="22">
-        <f>(S8/MAX(1,S7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T3" s="22">
-        <f>(T8/MAX(1,T7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U3" s="22">
-        <f>(U8/MAX(1,U7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V3" s="22">
-        <f>(V8/MAX(1,V7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W3" s="22">
-        <f>(W8/MAX(1,W7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X3" s="22">
-        <f>(X8/MAX(1,X7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y3" s="22">
-        <f>(Y8/MAX(1,Y7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z3" s="22">
-        <f>(Z8/MAX(1,Z7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA3" s="22">
-        <f>(AA8/MAX(1,AA7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB3" s="22">
-        <f>(AB8/MAX(1,AB7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC3" s="22">
-        <f>(AC8/MAX(1,AC7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD3" s="22">
-        <f>(AD8/MAX(1,AD7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE3" s="22">
-        <f>(AE8/MAX(1,AE7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF3" s="22">
-        <f>(AF8/MAX(1,AF7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG3" s="22">
-        <f>(AG8/MAX(1,AG7))*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH3" s="22">
-        <f>(AH8/MAX(1,AH7))*100</f>
+        <f t="shared" ref="AH3:BM3" si="4">(AH8/MAX(1,AH7))*100</f>
         <v>0</v>
       </c>
       <c r="AI3" s="22">
-        <f>(AI8/MAX(1,AI7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="22">
-        <f>(AJ8/MAX(1,AJ7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AK3" s="22">
-        <f>(AK8/MAX(1,AK7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AL3" s="22">
-        <f>(AL8/MAX(1,AL7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM3" s="22">
-        <f>(AM8/MAX(1,AM7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN3" s="22">
-        <f>(AN8/MAX(1,AN7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AO3" s="22">
-        <f>(AO8/MAX(1,AO7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AP3" s="22">
-        <f>(AP8/MAX(1,AP7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AQ3" s="22">
-        <f>(AQ8/MAX(1,AQ7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AR3" s="22">
-        <f>(AR8/MAX(1,AR7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AS3" s="22">
-        <f>(AS8/MAX(1,AS7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AT3" s="22">
-        <f>(AT8/MAX(1,AT7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU3" s="22">
-        <f>(AU8/MAX(1,AU7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AV3" s="22">
-        <f>(AV8/MAX(1,AV7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AW3" s="22">
-        <f>(AW8/MAX(1,AW7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AX3" s="22">
-        <f>(AX8/MAX(1,AX7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AY3" s="22">
-        <f>(AY8/MAX(1,AY7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AZ3" s="22">
-        <f>(AZ8/MAX(1,AZ7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BA3" s="22">
-        <f>(BA8/MAX(1,BA7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BB3" s="22">
-        <f>(BB8/MAX(1,BB7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BC3" s="22">
-        <f>(BC8/MAX(1,BC7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BD3" s="22">
-        <f>(BD8/MAX(1,BD7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BE3" s="22">
-        <f>(BE8/MAX(1,BE7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF3" s="22">
-        <f>(BF8/MAX(1,BF7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BG3" s="22">
-        <f>(BG8/MAX(1,BG7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH3" s="22">
-        <f>(BH8/MAX(1,BH7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BI3" s="22">
-        <f>(BI8/MAX(1,BI7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BJ3" s="22">
-        <f>(BJ8/MAX(1,BJ7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BK3" s="22">
-        <f>(BK8/MAX(1,BK7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BL3" s="22">
-        <f>(BL8/MAX(1,BL7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BM3" s="22">
-        <f>(BM8/MAX(1,BM7))*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BN3" s="22">
-        <f>(BN8/MAX(1,BN7))*100</f>
+        <f t="shared" ref="BN3:CC3" si="5">(BN8/MAX(1,BN7))*100</f>
         <v>0</v>
       </c>
       <c r="BO3" s="22">
-        <f>(BO8/MAX(1,BO7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BP3" s="22">
-        <f>(BP8/MAX(1,BP7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BQ3" s="22">
-        <f>(BQ8/MAX(1,BQ7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BR3" s="22">
-        <f>(BR8/MAX(1,BR7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BS3" s="22">
-        <f>(BS8/MAX(1,BS7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BT3" s="22">
-        <f>(BT8/MAX(1,BT7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BU3" s="22">
-        <f>(BU8/MAX(1,BU7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BV3" s="22">
-        <f>(BV8/MAX(1,BV7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BW3" s="22">
-        <f>(BW8/MAX(1,BW7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BX3" s="22">
-        <f>(BX8/MAX(1,BX7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BY3" s="22">
-        <f>(BY8/MAX(1,BY7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BZ3" s="22">
-        <f>(BZ8/MAX(1,BZ7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CA3" s="22">
-        <f>(CA8/MAX(1,CA7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CB3" s="22">
-        <f>(CB8/MAX(1,CB7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CC3" s="22">
-        <f>(CC8/MAX(1,CC7))*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -14753,323 +14751,323 @@
         <v>272</v>
       </c>
       <c r="B4" s="10">
-        <f>(B9/MAX(1,B7))*100</f>
+        <f t="shared" ref="B4:AG4" si="6">(B9/MAX(1,B7))*100</f>
         <v>0</v>
       </c>
       <c r="C4" s="10">
-        <f>(C9/MAX(1,C7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D4" s="10">
-        <f>(D9/MAX(1,D7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E4" s="10">
-        <f>(E9/MAX(1,E7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F4" s="10">
-        <f>(F9/MAX(1,F7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G4" s="10">
-        <f>(G9/MAX(1,G7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H4" s="10">
-        <f>(H9/MAX(1,H7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I4" s="10">
-        <f>(I9/MAX(1,I7))*100</f>
+        <f t="shared" si="6"/>
         <v>16.666666666666664</v>
       </c>
       <c r="J4" s="10">
-        <f>(J9/MAX(1,J7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K4" s="10">
-        <f>(K9/MAX(1,K7))*100</f>
+        <f t="shared" si="6"/>
         <v>5.5555555555555554</v>
       </c>
       <c r="L4" s="10">
-        <f>(L9/MAX(1,L7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M4" s="10">
-        <f>(M9/MAX(1,M7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N4" s="10">
-        <f>(N9/MAX(1,N7))*100</f>
+        <f t="shared" si="6"/>
         <v>2.083333333333333</v>
       </c>
       <c r="O4" s="10">
-        <f>(O9/MAX(1,O7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P4" s="10">
-        <f>(P9/MAX(1,P7))*100</f>
+        <f t="shared" si="6"/>
         <v>2.7027027027027026</v>
       </c>
       <c r="Q4" s="10">
-        <f>(Q9/MAX(1,Q7))*100</f>
+        <f t="shared" si="6"/>
         <v>2.6315789473684208</v>
       </c>
       <c r="R4" s="10">
-        <f>(R9/MAX(1,R7))*100</f>
+        <f t="shared" si="6"/>
         <v>6.7796610169491522</v>
       </c>
       <c r="S4" s="10">
-        <f>(S9/MAX(1,S7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T4" s="10">
-        <f>(T9/MAX(1,T7))*100</f>
+        <f t="shared" si="6"/>
         <v>2.197802197802198</v>
       </c>
       <c r="U4" s="10">
-        <f>(U9/MAX(1,U7))*100</f>
+        <f t="shared" si="6"/>
         <v>1.4925373134328357</v>
       </c>
       <c r="V4" s="10">
-        <f>(V9/MAX(1,V7))*100</f>
+        <f t="shared" si="6"/>
         <v>2.8846153846153846</v>
       </c>
       <c r="W4" s="10">
-        <f>(W9/MAX(1,W7))*100</f>
+        <f t="shared" si="6"/>
         <v>4.1379310344827589</v>
       </c>
       <c r="X4" s="10">
-        <f>(X9/MAX(1,X7))*100</f>
+        <f t="shared" si="6"/>
         <v>1.0416666666666665</v>
       </c>
       <c r="Y4" s="10">
-        <f>(Y9/MAX(1,Y7))*100</f>
+        <f t="shared" si="6"/>
         <v>2.0202020202020203</v>
       </c>
       <c r="Z4" s="10">
-        <f>(Z9/MAX(1,Z7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA4" s="10">
-        <f>(AA9/MAX(1,AA7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB4" s="10">
-        <f>(AB9/MAX(1,AB7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC4" s="10">
-        <f>(AC9/MAX(1,AC7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD4" s="10">
-        <f>(AD9/MAX(1,AD7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE4" s="10">
-        <f>(AE9/MAX(1,AE7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF4" s="10">
-        <f>(AF9/MAX(1,AF7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG4" s="10">
-        <f>(AG9/MAX(1,AG7))*100</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AH4" s="10">
-        <f>(AH9/MAX(1,AH7))*100</f>
+        <f t="shared" ref="AH4:BM4" si="7">(AH9/MAX(1,AH7))*100</f>
         <v>0</v>
       </c>
       <c r="AI4" s="10">
-        <f>(AI9/MAX(1,AI7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="10">
-        <f>(AJ9/MAX(1,AJ7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AK4" s="10">
-        <f>(AK9/MAX(1,AK7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AL4" s="10">
-        <f>(AL9/MAX(1,AL7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AM4" s="10">
-        <f>(AM9/MAX(1,AM7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AN4" s="10">
-        <f>(AN9/MAX(1,AN7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AO4" s="10">
-        <f>(AO9/MAX(1,AO7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AP4" s="10">
-        <f>(AP9/MAX(1,AP7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ4" s="10">
-        <f>(AQ9/MAX(1,AQ7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AR4" s="10">
-        <f>(AR9/MAX(1,AR7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AS4" s="10">
-        <f>(AS9/MAX(1,AS7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AT4" s="10">
-        <f>(AT9/MAX(1,AT7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AU4" s="10">
-        <f>(AU9/MAX(1,AU7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AV4" s="10">
-        <f>(AV9/MAX(1,AV7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AW4" s="10">
-        <f>(AW9/MAX(1,AW7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AX4" s="10">
-        <f>(AX9/MAX(1,AX7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AY4" s="10">
-        <f>(AY9/MAX(1,AY7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AZ4" s="10">
-        <f>(AZ9/MAX(1,AZ7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BA4" s="10">
-        <f>(BA9/MAX(1,BA7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BB4" s="10">
-        <f>(BB9/MAX(1,BB7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BC4" s="10">
-        <f>(BC9/MAX(1,BC7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BD4" s="10">
-        <f>(BD9/MAX(1,BD7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BE4" s="10">
-        <f>(BE9/MAX(1,BE7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BF4" s="10">
-        <f>(BF9/MAX(1,BF7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BG4" s="10">
-        <f>(BG9/MAX(1,BG7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BH4" s="10">
-        <f>(BH9/MAX(1,BH7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BI4" s="10">
-        <f>(BI9/MAX(1,BI7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BJ4" s="10">
-        <f>(BJ9/MAX(1,BJ7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BK4" s="10">
-        <f>(BK9/MAX(1,BK7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BL4" s="10">
-        <f>(BL9/MAX(1,BL7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BM4" s="10">
-        <f>(BM9/MAX(1,BM7))*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BN4" s="10">
-        <f>(BN9/MAX(1,BN7))*100</f>
+        <f t="shared" ref="BN4:CC4" si="8">(BN9/MAX(1,BN7))*100</f>
         <v>0</v>
       </c>
       <c r="BO4" s="10">
-        <f>(BO9/MAX(1,BO7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BP4" s="10">
-        <f>(BP9/MAX(1,BP7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BQ4" s="10">
-        <f>(BQ9/MAX(1,BQ7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BR4" s="10">
-        <f>(BR9/MAX(1,BR7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BS4" s="10">
-        <f>(BS9/MAX(1,BS7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BT4" s="10">
-        <f>(BT9/MAX(1,BT7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BU4" s="10">
-        <f>(BU9/MAX(1,BU7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BV4" s="10">
-        <f>(BV9/MAX(1,BV7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BW4" s="10">
-        <f>(BW9/MAX(1,BW7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BX4" s="10">
-        <f>(BX9/MAX(1,BX7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BY4" s="10">
-        <f>(BY9/MAX(1,BY7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BZ4" s="10">
-        <f>(BZ9/MAX(1,BZ7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CA4" s="10">
-        <f>(CA9/MAX(1,CA7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CB4" s="10">
-        <f>(CB9/MAX(1,CB7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CC4" s="10">
-        <f>(CC9/MAX(1,CC7))*100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -17165,11 +17163,11 @@
       </c>
       <c r="D3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>21.134020618556701</v>
       </c>
       <c r="E3" s="21">
         <f t="shared" si="2"/>
-        <v>103.6697247706422</v>
+        <v>24.311926605504588</v>
       </c>
       <c r="F3" s="21">
         <f t="shared" si="2"/>
@@ -18318,11 +18316,11 @@
       </c>
       <c r="D8" s="14">
         <f>MAX(0,(md!D4-md!C4))</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E8" s="14">
         <f>MAX(0,(md!E4-md!D4))</f>
-        <v>226</v>
+        <v>53</v>
       </c>
       <c r="F8" s="14">
         <f>MAX(0,(md!F4-md!E4))</f>
@@ -25863,7 +25861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10B5AF9-8E42-4F8B-8F58-724C1869D2EC}">
   <dimension ref="A1:BS143"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -25889,275 +25887,275 @@
         <v>270</v>
       </c>
       <c r="D2" s="20">
-        <f>(D7/(MAX(D6,1))*100)</f>
+        <f t="shared" ref="D2:AI2" si="0">(D7/(MAX(D6,1))*100)</f>
         <v>0</v>
       </c>
       <c r="E2" s="20">
-        <f>(E7/(MAX(E6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>9.8894706224549154</v>
       </c>
       <c r="F2" s="20">
-        <f>(F7/(MAX(F6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>12.543554006968641</v>
       </c>
       <c r="G2" s="20">
-        <f>(G7/(MAX(G6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>7.3810825587752866</v>
       </c>
       <c r="H2" s="20">
-        <f>(H7/(MAX(H6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>10.464310464310463</v>
       </c>
       <c r="I2" s="20">
-        <f>(I7/(MAX(I6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>9.0972708187543745</v>
       </c>
       <c r="J2" s="20">
-        <f>(J7/(MAX(J6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>16.874541452677917</v>
       </c>
       <c r="K2" s="20">
-        <f>(K7/(MAX(K6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>12.04323211528564</v>
       </c>
       <c r="L2" s="20">
-        <f>(L7/(MAX(L6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>9.8886414253897552</v>
       </c>
       <c r="M2" s="20">
-        <f>(M7/(MAX(M6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>21.610169491525426</v>
       </c>
       <c r="N2" s="20">
-        <f>(N7/(MAX(N6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>15.508441303494308</v>
       </c>
       <c r="O2" s="20">
-        <f>(O7/(MAX(O6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>10.854176498348277</v>
       </c>
       <c r="P2" s="20">
-        <f>(P7/(MAX(P6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>28.352941176470587</v>
       </c>
       <c r="Q2" s="20">
-        <f>(Q7/(MAX(Q6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R2" s="20">
-        <f>(R7/(MAX(R6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S2" s="20">
-        <f>(S7/(MAX(S6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T2" s="20">
-        <f>(T7/(MAX(T6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U2" s="20">
-        <f>(U7/(MAX(U6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V2" s="20">
-        <f>(V7/(MAX(V6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W2" s="20">
-        <f>(W7/(MAX(W6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X2" s="20">
-        <f>(X7/(MAX(X6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y2" s="20">
-        <f>(Y7/(MAX(Y6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z2" s="20">
-        <f>(Z7/(MAX(Z6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA2" s="20">
-        <f>(AA7/(MAX(AA6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB2" s="20">
-        <f>(AB7/(MAX(AB6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC2" s="20">
-        <f>(AC7/(MAX(AC6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD2" s="20">
-        <f>(AD7/(MAX(AD6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE2" s="20">
-        <f>(AE7/(MAX(AE6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF2" s="20">
-        <f>(AF7/(MAX(AF6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG2" s="20">
-        <f>(AG7/(MAX(AG6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH2" s="20">
-        <f>(AH7/(MAX(AH6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI2" s="20">
-        <f>(AI7/(MAX(AI6,1))*100)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ2" s="20">
-        <f>(AJ7/(MAX(AJ6,1))*100)</f>
+        <f t="shared" ref="AJ2:BS2" si="1">(AJ7/(MAX(AJ6,1))*100)</f>
         <v>0</v>
       </c>
       <c r="AK2" s="20">
-        <f>(AK7/(MAX(AK6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL2" s="20">
-        <f>(AL7/(MAX(AL6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM2" s="20">
-        <f>(AM7/(MAX(AM6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN2" s="20">
-        <f>(AN7/(MAX(AN6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO2" s="20">
-        <f>(AO7/(MAX(AO6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP2" s="20">
-        <f>(AP7/(MAX(AP6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ2" s="20">
-        <f>(AQ7/(MAX(AQ6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR2" s="20">
-        <f>(AR7/(MAX(AR6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AS2" s="20">
-        <f>(AS7/(MAX(AS6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AT2" s="20">
-        <f>(AT7/(MAX(AT6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU2" s="20">
-        <f>(AU7/(MAX(AU6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AV2" s="20">
-        <f>(AV7/(MAX(AV6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AW2" s="20">
-        <f>(AW7/(MAX(AW6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AX2" s="20">
-        <f>(AX7/(MAX(AX6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AY2" s="20">
-        <f>(AY7/(MAX(AY6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AZ2" s="20">
-        <f>(AZ7/(MAX(AZ6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BA2" s="20">
-        <f>(BA7/(MAX(BA6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BB2" s="20">
-        <f>(BB7/(MAX(BB6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BC2" s="20">
-        <f>(BC7/(MAX(BC6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BD2" s="20">
-        <f>(BD7/(MAX(BD6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BE2" s="20">
-        <f>(BE7/(MAX(BE6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BF2" s="20">
-        <f>(BF7/(MAX(BF6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BG2" s="20">
-        <f>(BG7/(MAX(BG6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BH2" s="20">
-        <f>(BH7/(MAX(BH6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BI2" s="20">
-        <f>(BI7/(MAX(BI6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BJ2" s="20">
-        <f>(BJ7/(MAX(BJ6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BK2" s="20">
-        <f>(BK7/(MAX(BK6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BL2" s="20">
-        <f>(BL7/(MAX(BL6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BM2" s="20">
-        <f>(BM7/(MAX(BM6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BN2" s="20">
-        <f>(BN7/(MAX(BN6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BO2" s="20">
-        <f>(BO7/(MAX(BO6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BP2" s="20">
-        <f>(BP7/(MAX(BP6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BQ2" s="20">
-        <f>(BQ7/(MAX(BQ6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BR2" s="20">
-        <f>(BR7/(MAX(BR6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BS2" s="20">
-        <f>(BS7/(MAX(BS6,1))*100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -26166,275 +26164,275 @@
         <v>271</v>
       </c>
       <c r="D3" s="20">
-        <f t="shared" ref="D3:AI3" si="0">(D8/MAX(1,D7))*100</f>
+        <f t="shared" ref="D3:AI3" si="2">(D8/MAX(1,D7))*100</f>
         <v>0</v>
       </c>
       <c r="E3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.76470588235294</v>
       </c>
       <c r="F3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="G3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.851851851851853</v>
       </c>
       <c r="H3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.6092715231788084</v>
       </c>
       <c r="I3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>18.461538461538463</v>
       </c>
       <c r="J3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.608695652173912</v>
       </c>
       <c r="K3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>18.376068376068378</v>
       </c>
       <c r="L3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>17.117117117117118</v>
       </c>
       <c r="M3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>21.568627450980394</v>
       </c>
       <c r="N3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>19.746835443037973</v>
       </c>
       <c r="O3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>17.826086956521738</v>
       </c>
       <c r="P3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>27.385892116182575</v>
       </c>
       <c r="Q3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="20">
-        <f t="shared" ref="AJ3:BS3" si="1">(AJ8/MAX(1,AJ7))*100</f>
+        <f t="shared" ref="AJ3:BS3" si="3">(AJ8/MAX(1,AJ7))*100</f>
         <v>0</v>
       </c>
       <c r="AK3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AL3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AN3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AO3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AP3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AQ3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AR3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AS3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AT3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AU3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AV3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AW3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AX3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AY3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AZ3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BA3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BB3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BC3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BD3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BE3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BF3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BG3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BH3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BI3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BJ3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BK3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BL3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BM3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BN3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BO3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BP3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BQ3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BR3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BS3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26443,275 +26441,275 @@
         <v>272</v>
       </c>
       <c r="D4" s="20">
-        <f t="shared" ref="D4:AI4" si="2">(D9/MAX(1,D7))*100</f>
+        <f t="shared" ref="D4:AI4" si="4">(D9/MAX(1,D7))*100</f>
         <v>0</v>
       </c>
       <c r="E4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5294117647058822</v>
       </c>
       <c r="F4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.69444444444444442</v>
       </c>
       <c r="G4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.2222222222222223</v>
       </c>
       <c r="H4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.3112582781456954</v>
       </c>
       <c r="I4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.3076923076923079</v>
       </c>
       <c r="J4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.86956521739130432</v>
       </c>
       <c r="K4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.9914529914529915</v>
       </c>
       <c r="L4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.1531531531531529</v>
       </c>
       <c r="M4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6339869281045754</v>
       </c>
       <c r="N4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5189873417721518</v>
       </c>
       <c r="O4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2448132780082988</v>
       </c>
       <c r="Q4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Y4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AA4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AB4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI4" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="20">
-        <f t="shared" ref="AJ4:BS4" si="3">(AJ9/MAX(1,AJ7))*100</f>
+        <f t="shared" ref="AJ4:BS4" si="5">(AJ9/MAX(1,AJ7))*100</f>
         <v>0</v>
       </c>
       <c r="AK4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AL4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AM4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AN4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AP4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AQ4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AR4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AS4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AT4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AU4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AV4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AW4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AX4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AY4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AZ4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BA4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BB4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BC4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BD4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BE4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BF4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BG4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BH4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BI4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BJ4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BK4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BL4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BM4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BN4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BO4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BP4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BQ4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BR4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BS4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
08 April update + corrections
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA593BFC-97A8-4878-9931-CDB49F50827A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D00094D-2048-4EB2-BB9A-5705DC27648A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="27580" windowHeight="18000" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="1520" yWindow="1980" windowWidth="20520" windowHeight="13130" tabRatio="685" activeTab="1" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="272">
   <si>
     <t>FIPS</t>
   </si>
@@ -841,9 +841,6 @@
     <t>Allegany</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>(-) tests</t>
   </si>
   <si>
@@ -1047,6 +1044,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1056,21 +1062,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="173">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1998,9 +1998,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2351,207 +2348,209 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3416EC88-0BC4-4758-A58D-187F9B999FB7}" name="delta_md" displayName="delta_md" ref="A10:BQ34" totalsRowShown="0">
   <tableColumns count="69">
-    <tableColumn id="1" xr3:uid="{BFB3F1B0-DE0E-4A75-8475-0AD52DEC3890}" name="county" dataDxfId="138">
-      <calculatedColumnFormula>T(md[[#This Row],[county]])</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{BFB3F1B0-DE0E-4A75-8475-0AD52DEC3890}" name="county" dataDxfId="0">
+      <calculatedColumnFormula>md!A7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F9092969-4B66-4A12-8600-89F79D327DA5}" name="FIPS" dataDxfId="137"/>
-    <tableColumn id="67" xr3:uid="{C1AF955F-BEA7-4320-9557-BB3EAECC72AE}" name="26-Mar" dataDxfId="136"/>
-    <tableColumn id="68" xr3:uid="{C7FF752A-8DC4-46FC-AF76-F1FF335EB014}" name="27-Mar" dataDxfId="135">
+    <tableColumn id="2" xr3:uid="{F9092969-4B66-4A12-8600-89F79D327DA5}" name="FIPS" dataDxfId="138">
+      <calculatedColumnFormula>md!B7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="67" xr3:uid="{C1AF955F-BEA7-4320-9557-BB3EAECC72AE}" name="26-Mar" dataDxfId="137"/>
+    <tableColumn id="68" xr3:uid="{C7FF752A-8DC4-46FC-AF76-F1FF335EB014}" name="27-Mar" dataDxfId="136">
       <calculatedColumnFormula>MAX(0,(md!D7-md!C7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="69" xr3:uid="{CF1FAAB0-7ED6-4840-A066-0E55CBEAF2B0}" name="28-Mar" dataDxfId="134">
+    <tableColumn id="69" xr3:uid="{CF1FAAB0-7ED6-4840-A066-0E55CBEAF2B0}" name="28-Mar" dataDxfId="135">
       <calculatedColumnFormula>MAX(0,(md!E7-md!D7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="70" xr3:uid="{C6B48FE5-0D82-4E66-879E-AD88448A92B0}" name="29-Mar" dataDxfId="133">
+    <tableColumn id="70" xr3:uid="{C6B48FE5-0D82-4E66-879E-AD88448A92B0}" name="29-Mar" dataDxfId="134">
       <calculatedColumnFormula>MAX(0,(md!F7-md!E7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="71" xr3:uid="{2FBAB02E-F400-450D-9DCA-14210AE3DFAC}" name="30-Mar" dataDxfId="132">
+    <tableColumn id="71" xr3:uid="{2FBAB02E-F400-450D-9DCA-14210AE3DFAC}" name="30-Mar" dataDxfId="133">
       <calculatedColumnFormula>MAX(0,(md!G7-md!F7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="72" xr3:uid="{760DFC79-3F68-4133-AD98-EC55B9CA5B60}" name="31-Mar" dataDxfId="131">
+    <tableColumn id="72" xr3:uid="{760DFC79-3F68-4133-AD98-EC55B9CA5B60}" name="31-Mar" dataDxfId="132">
       <calculatedColumnFormula>MAX(0,(md!H7-md!G7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{3A0DCBAA-0E39-4B12-BA9F-16EC890AE5D7}" name="1-Apr" dataDxfId="130">
+    <tableColumn id="73" xr3:uid="{3A0DCBAA-0E39-4B12-BA9F-16EC890AE5D7}" name="1-Apr" dataDxfId="131">
       <calculatedColumnFormula>MAX(0,(md!I7-md!H7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="74" xr3:uid="{E675B0EB-5084-45E1-B98F-33BBECE64BCA}" name="2-Apr" dataDxfId="129">
+    <tableColumn id="74" xr3:uid="{E675B0EB-5084-45E1-B98F-33BBECE64BCA}" name="2-Apr" dataDxfId="130">
       <calculatedColumnFormula>MAX(0,(md!J7-md!I7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{7D201D0E-7465-446D-96C8-6369C567BA17}" name="3-Apr" dataDxfId="128">
+    <tableColumn id="75" xr3:uid="{7D201D0E-7465-446D-96C8-6369C567BA17}" name="3-Apr" dataDxfId="129">
       <calculatedColumnFormula>MAX(0,(md!K7-md!J7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{28A6AB08-C7E3-44C7-8A67-CED2B8818875}" name="4-Apr" dataDxfId="127">
+    <tableColumn id="76" xr3:uid="{28A6AB08-C7E3-44C7-8A67-CED2B8818875}" name="4-Apr" dataDxfId="128">
       <calculatedColumnFormula>MAX(0,(md!L7-md!K7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DA52AE41-91C4-414C-BA03-812FFA287E17}" name="5-Apr" dataDxfId="126">
+    <tableColumn id="77" xr3:uid="{DA52AE41-91C4-414C-BA03-812FFA287E17}" name="5-Apr" dataDxfId="127">
       <calculatedColumnFormula>MAX(0,(md!M7-md!L7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{824BC17C-FABA-44FC-8DFD-B7D699B912DA}" name="6-Apr" dataDxfId="125">
+    <tableColumn id="78" xr3:uid="{824BC17C-FABA-44FC-8DFD-B7D699B912DA}" name="6-Apr" dataDxfId="126">
       <calculatedColumnFormula>MAX(0,(md!N7-md!M7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{ADAB64C4-87B8-4E71-A8BD-E5D36D0367A3}" name="7-Apr" dataDxfId="124">
+    <tableColumn id="79" xr3:uid="{ADAB64C4-87B8-4E71-A8BD-E5D36D0367A3}" name="7-Apr" dataDxfId="125">
       <calculatedColumnFormula>MAX(0,(md!O7-md!N7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{EFD25893-57FD-4F2A-B0A8-E74649945105}" name="8-Apr" dataDxfId="123">
+    <tableColumn id="80" xr3:uid="{EFD25893-57FD-4F2A-B0A8-E74649945105}" name="8-Apr" dataDxfId="124">
       <calculatedColumnFormula>MAX(0,(md!P7-md!O7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{CD753A3C-95EB-4785-B102-2C58EDAAE5EC}" name="9-Apr" dataDxfId="122">
+    <tableColumn id="81" xr3:uid="{CD753A3C-95EB-4785-B102-2C58EDAAE5EC}" name="9-Apr" dataDxfId="123">
       <calculatedColumnFormula>MAX(0,(md!Q7-md!P7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{996C1CCE-574A-49C4-9367-5B6F1CA045CA}" name="10-Apr" dataDxfId="121">
+    <tableColumn id="82" xr3:uid="{996C1CCE-574A-49C4-9367-5B6F1CA045CA}" name="10-Apr" dataDxfId="122">
       <calculatedColumnFormula>MAX(0,(md!R7-md!Q7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{40EF4BBD-F411-43F1-828D-4E3A9F1D9EA2}" name="11-Apr" dataDxfId="120">
+    <tableColumn id="83" xr3:uid="{40EF4BBD-F411-43F1-828D-4E3A9F1D9EA2}" name="11-Apr" dataDxfId="121">
       <calculatedColumnFormula>MAX(0,(md!S7-md!R7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="84" xr3:uid="{EB725643-C67D-4404-B5FD-5483B4E84D3F}" name="12-Apr" dataDxfId="119">
+    <tableColumn id="84" xr3:uid="{EB725643-C67D-4404-B5FD-5483B4E84D3F}" name="12-Apr" dataDxfId="120">
       <calculatedColumnFormula>MAX(0,(md!T7-md!S7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="85" xr3:uid="{5DA42EA3-77ED-4135-AFAA-FEFBF6C235B5}" name="13-Apr" dataDxfId="118">
+    <tableColumn id="85" xr3:uid="{5DA42EA3-77ED-4135-AFAA-FEFBF6C235B5}" name="13-Apr" dataDxfId="119">
       <calculatedColumnFormula>MAX(0,(md!U7-md!T7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{1AFEE08F-BD43-43C9-9F4D-D582447F1CBC}" name="14-Apr" dataDxfId="117">
+    <tableColumn id="86" xr3:uid="{1AFEE08F-BD43-43C9-9F4D-D582447F1CBC}" name="14-Apr" dataDxfId="118">
       <calculatedColumnFormula>MAX(0,(md!V7-md!U7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{8B04386D-D803-4517-ADE6-E3EB36F2B2CB}" name="15-Apr" dataDxfId="116">
+    <tableColumn id="87" xr3:uid="{8B04386D-D803-4517-ADE6-E3EB36F2B2CB}" name="15-Apr" dataDxfId="117">
       <calculatedColumnFormula>MAX(0,(md!W7-md!V7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{FB2ACEC4-C503-4985-BABF-2F3493F182BB}" name="16-Apr" dataDxfId="115">
+    <tableColumn id="88" xr3:uid="{FB2ACEC4-C503-4985-BABF-2F3493F182BB}" name="16-Apr" dataDxfId="116">
       <calculatedColumnFormula>MAX(0,(md!X7-md!W7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{7E3C269C-D7EB-4419-9DD2-B9360046FEDD}" name="17-Apr" dataDxfId="114">
+    <tableColumn id="89" xr3:uid="{7E3C269C-D7EB-4419-9DD2-B9360046FEDD}" name="17-Apr" dataDxfId="115">
       <calculatedColumnFormula>MAX(0,(md!Y7-md!X7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{54053764-3095-48BD-B0DC-FBAEA597B459}" name="18-Apr" dataDxfId="113">
+    <tableColumn id="90" xr3:uid="{54053764-3095-48BD-B0DC-FBAEA597B459}" name="18-Apr" dataDxfId="114">
       <calculatedColumnFormula>MAX(0,(md!Z7-md!Y7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{4377D20D-95DB-4908-82A3-A401AD129E61}" name="19-Apr" dataDxfId="112">
+    <tableColumn id="91" xr3:uid="{4377D20D-95DB-4908-82A3-A401AD129E61}" name="19-Apr" dataDxfId="113">
       <calculatedColumnFormula>MAX(0,(md!AA7-md!Z7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{51477B52-D4A6-4750-A535-A42BE77C5376}" name="20-Apr" dataDxfId="111">
+    <tableColumn id="92" xr3:uid="{51477B52-D4A6-4750-A535-A42BE77C5376}" name="20-Apr" dataDxfId="112">
       <calculatedColumnFormula>MAX(0,(md!AB7-md!AA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{6B62D812-8EC8-4A07-BB5C-0289C6388D63}" name="21-Apr" dataDxfId="110">
+    <tableColumn id="93" xr3:uid="{6B62D812-8EC8-4A07-BB5C-0289C6388D63}" name="21-Apr" dataDxfId="111">
       <calculatedColumnFormula>MAX(0,(md!AC7-md!AB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{13AE0503-9E29-41B3-B0E2-102AAB93EBC2}" name="22-Apr" dataDxfId="109">
+    <tableColumn id="94" xr3:uid="{13AE0503-9E29-41B3-B0E2-102AAB93EBC2}" name="22-Apr" dataDxfId="110">
       <calculatedColumnFormula>MAX(0,(md!AD7-md!AC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{9E427FAC-7198-4707-A673-7D2FBEE0AB05}" name="23-Apr" dataDxfId="108">
+    <tableColumn id="95" xr3:uid="{9E427FAC-7198-4707-A673-7D2FBEE0AB05}" name="23-Apr" dataDxfId="109">
       <calculatedColumnFormula>MAX(0,(md!AE7-md!AD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{C8AB402E-023F-43C2-9F84-B4F240B82255}" name="24-Apr" dataDxfId="107">
+    <tableColumn id="96" xr3:uid="{C8AB402E-023F-43C2-9F84-B4F240B82255}" name="24-Apr" dataDxfId="108">
       <calculatedColumnFormula>MAX(0,(md!AF7-md!AE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="97" xr3:uid="{49FBF307-99EC-4796-AC0B-FDB70D090EB3}" name="25-Apr" dataDxfId="106">
+    <tableColumn id="97" xr3:uid="{49FBF307-99EC-4796-AC0B-FDB70D090EB3}" name="25-Apr" dataDxfId="107">
       <calculatedColumnFormula>MAX(0,(md!AG7-md!AF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="98" xr3:uid="{97545A0F-D8FA-44BB-B126-7C82E5681E5B}" name="26-Apr" dataDxfId="105">
+    <tableColumn id="98" xr3:uid="{97545A0F-D8FA-44BB-B126-7C82E5681E5B}" name="26-Apr" dataDxfId="106">
       <calculatedColumnFormula>MAX(0,(md!AH7-md!AG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="99" xr3:uid="{A1EA2D07-F633-4D36-8126-F070310B936B}" name="27-Apr" dataDxfId="104">
+    <tableColumn id="99" xr3:uid="{A1EA2D07-F633-4D36-8126-F070310B936B}" name="27-Apr" dataDxfId="105">
       <calculatedColumnFormula>MAX(0,(md!AI7-md!AH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="100" xr3:uid="{6A49089B-958E-4670-BEE8-20D140F9DC00}" name="28-Apr" dataDxfId="103">
+    <tableColumn id="100" xr3:uid="{6A49089B-958E-4670-BEE8-20D140F9DC00}" name="28-Apr" dataDxfId="104">
       <calculatedColumnFormula>MAX(0,(md!AJ7-md!AI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="101" xr3:uid="{264A9134-7104-4DCB-922F-79C66B81E432}" name="29-Apr" dataDxfId="102">
+    <tableColumn id="101" xr3:uid="{264A9134-7104-4DCB-922F-79C66B81E432}" name="29-Apr" dataDxfId="103">
       <calculatedColumnFormula>MAX(0,(md!AK7-md!AJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="102" xr3:uid="{5FDD5894-EE0C-426E-BF3A-4C9D8D68BFA0}" name="30-Apr" dataDxfId="101">
+    <tableColumn id="102" xr3:uid="{5FDD5894-EE0C-426E-BF3A-4C9D8D68BFA0}" name="30-Apr" dataDxfId="102">
       <calculatedColumnFormula>MAX(0,(md!AL7-md!AK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="103" xr3:uid="{C43A5B5F-92CE-4F1C-952E-ABD6BB7341CE}" name="1-May" dataDxfId="100">
+    <tableColumn id="103" xr3:uid="{C43A5B5F-92CE-4F1C-952E-ABD6BB7341CE}" name="1-May" dataDxfId="101">
       <calculatedColumnFormula>MAX(0,(md!AM7-md!AL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="104" xr3:uid="{50B54D8A-B9E6-4CF6-A7B8-A5AB722D33DA}" name="2-May" dataDxfId="99">
+    <tableColumn id="104" xr3:uid="{50B54D8A-B9E6-4CF6-A7B8-A5AB722D33DA}" name="2-May" dataDxfId="100">
       <calculatedColumnFormula>MAX(0,(md!AN7-md!AM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="105" xr3:uid="{4B5FB437-BD09-44D9-925C-3E55C876D9CC}" name="3-May" dataDxfId="98">
+    <tableColumn id="105" xr3:uid="{4B5FB437-BD09-44D9-925C-3E55C876D9CC}" name="3-May" dataDxfId="99">
       <calculatedColumnFormula>MAX(0,(md!AO7-md!AN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="106" xr3:uid="{379072DC-0CD1-4E06-8C87-08A5F7FF2E05}" name="4-May" dataDxfId="97">
+    <tableColumn id="106" xr3:uid="{379072DC-0CD1-4E06-8C87-08A5F7FF2E05}" name="4-May" dataDxfId="98">
       <calculatedColumnFormula>MAX(0,(md!AP7-md!AO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="107" xr3:uid="{AEEEFF0B-566B-457E-B205-F55AEB13AD9E}" name="5-May" dataDxfId="96">
+    <tableColumn id="107" xr3:uid="{AEEEFF0B-566B-457E-B205-F55AEB13AD9E}" name="5-May" dataDxfId="97">
       <calculatedColumnFormula>MAX(0,(md!AQ7-md!AP7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="108" xr3:uid="{94C890F0-71FA-4374-8041-A9193FCE4E17}" name="6-May" dataDxfId="95">
+    <tableColumn id="108" xr3:uid="{94C890F0-71FA-4374-8041-A9193FCE4E17}" name="6-May" dataDxfId="96">
       <calculatedColumnFormula>MAX(0,(md!AR7-md!AQ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="109" xr3:uid="{33E6A0CC-1E42-4A87-B99D-E6A77E72126F}" name="7-May" dataDxfId="94">
+    <tableColumn id="109" xr3:uid="{33E6A0CC-1E42-4A87-B99D-E6A77E72126F}" name="7-May" dataDxfId="95">
       <calculatedColumnFormula>MAX(0,(md!AS7-md!AR7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="110" xr3:uid="{CD2CF375-F2D1-483D-8BD2-30D032E3CD04}" name="8-May" dataDxfId="93">
+    <tableColumn id="110" xr3:uid="{CD2CF375-F2D1-483D-8BD2-30D032E3CD04}" name="8-May" dataDxfId="94">
       <calculatedColumnFormula>MAX(0,(md!AT7-md!AS7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="111" xr3:uid="{E061025C-CDF7-4C91-AF64-42F835C57C96}" name="9-May" dataDxfId="92">
+    <tableColumn id="111" xr3:uid="{E061025C-CDF7-4C91-AF64-42F835C57C96}" name="9-May" dataDxfId="93">
       <calculatedColumnFormula>MAX(0,(md!AU7-md!AT7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="134" xr3:uid="{AE616B94-71FE-467D-86B4-667F51C6B88F}" name="10-May" dataDxfId="91">
+    <tableColumn id="134" xr3:uid="{AE616B94-71FE-467D-86B4-667F51C6B88F}" name="10-May" dataDxfId="92">
       <calculatedColumnFormula>MAX(0,(md!AV7-md!AU7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="135" xr3:uid="{6BB6B4AF-1198-44B7-83CE-176610757419}" name="11-May" dataDxfId="90">
+    <tableColumn id="135" xr3:uid="{6BB6B4AF-1198-44B7-83CE-176610757419}" name="11-May" dataDxfId="91">
       <calculatedColumnFormula>MAX(0,(md!AW7-md!AV7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="136" xr3:uid="{F8A39F33-5023-41AB-91DB-0BCFDE57C6C1}" name="12-May" dataDxfId="89">
+    <tableColumn id="136" xr3:uid="{F8A39F33-5023-41AB-91DB-0BCFDE57C6C1}" name="12-May" dataDxfId="90">
       <calculatedColumnFormula>MAX(0,(md!AX7-md!AW7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="137" xr3:uid="{0676A9AE-3A86-4158-9689-DD58082C1506}" name="13-May" dataDxfId="88">
+    <tableColumn id="137" xr3:uid="{0676A9AE-3A86-4158-9689-DD58082C1506}" name="13-May" dataDxfId="89">
       <calculatedColumnFormula>MAX(0,(md!AY7-md!AX7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="138" xr3:uid="{BE92BDB9-5A19-4036-B052-510BC75BF308}" name="14-May" dataDxfId="87">
+    <tableColumn id="138" xr3:uid="{BE92BDB9-5A19-4036-B052-510BC75BF308}" name="14-May" dataDxfId="88">
       <calculatedColumnFormula>MAX(0,(md!AZ7-md!AY7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="139" xr3:uid="{131F58F1-2C6B-4B17-ABD9-FC3D31544029}" name="15-May" dataDxfId="86">
+    <tableColumn id="139" xr3:uid="{131F58F1-2C6B-4B17-ABD9-FC3D31544029}" name="15-May" dataDxfId="87">
       <calculatedColumnFormula>MAX(0,(md!BA7-md!AZ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="140" xr3:uid="{F9D8DFE8-4BF8-498E-99E2-6B007456B7F4}" name="16-May" dataDxfId="85">
+    <tableColumn id="140" xr3:uid="{F9D8DFE8-4BF8-498E-99E2-6B007456B7F4}" name="16-May" dataDxfId="86">
       <calculatedColumnFormula>MAX(0,(md!BB7-md!BA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="141" xr3:uid="{850888F3-D54B-4B4C-99E1-BA7B9E46EE02}" name="17-May" dataDxfId="84">
+    <tableColumn id="141" xr3:uid="{850888F3-D54B-4B4C-99E1-BA7B9E46EE02}" name="17-May" dataDxfId="85">
       <calculatedColumnFormula>MAX(0,(md!BC7-md!BB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="142" xr3:uid="{4699F9BE-7F39-4078-AB3E-B50D7A10B837}" name="18-May" dataDxfId="83">
+    <tableColumn id="142" xr3:uid="{4699F9BE-7F39-4078-AB3E-B50D7A10B837}" name="18-May" dataDxfId="84">
       <calculatedColumnFormula>MAX(0,(md!BD7-md!BC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="143" xr3:uid="{8BFDF52E-6DAB-4C58-BC98-15836D8A7B57}" name="19-May" dataDxfId="82">
+    <tableColumn id="143" xr3:uid="{8BFDF52E-6DAB-4C58-BC98-15836D8A7B57}" name="19-May" dataDxfId="83">
       <calculatedColumnFormula>MAX(0,(md!BE7-md!BD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="144" xr3:uid="{688B7008-25D3-429E-886B-50AE8A87C074}" name="20-May" dataDxfId="81">
+    <tableColumn id="144" xr3:uid="{688B7008-25D3-429E-886B-50AE8A87C074}" name="20-May" dataDxfId="82">
       <calculatedColumnFormula>MAX(0,(md!BF7-md!BE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="145" xr3:uid="{A7814F0A-A83A-4398-B038-10389D9E6616}" name="21-May" dataDxfId="80">
+    <tableColumn id="145" xr3:uid="{A7814F0A-A83A-4398-B038-10389D9E6616}" name="21-May" dataDxfId="81">
       <calculatedColumnFormula>MAX(0,(md!BG7-md!BF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="146" xr3:uid="{E1B45AD0-EC1B-4E08-BFCF-ABEC66AEDA32}" name="22-May" dataDxfId="79">
+    <tableColumn id="146" xr3:uid="{E1B45AD0-EC1B-4E08-BFCF-ABEC66AEDA32}" name="22-May" dataDxfId="80">
       <calculatedColumnFormula>MAX(0,(md!BH7-md!BG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="147" xr3:uid="{2D30F07E-4A4C-44CC-9488-8B6A8CC75726}" name="23-May" dataDxfId="78">
+    <tableColumn id="147" xr3:uid="{2D30F07E-4A4C-44CC-9488-8B6A8CC75726}" name="23-May" dataDxfId="79">
       <calculatedColumnFormula>MAX(0,(md!BI7-md!BH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="148" xr3:uid="{78F7EC10-89A8-4EEB-9067-BE4A88B0565A}" name="24-May" dataDxfId="77">
+    <tableColumn id="148" xr3:uid="{78F7EC10-89A8-4EEB-9067-BE4A88B0565A}" name="24-May" dataDxfId="78">
       <calculatedColumnFormula>MAX(0,(md!BJ7-md!BI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="149" xr3:uid="{AC298BAD-F13B-4803-8CBB-7A22C58F269E}" name="25-May" dataDxfId="76">
+    <tableColumn id="149" xr3:uid="{AC298BAD-F13B-4803-8CBB-7A22C58F269E}" name="25-May" dataDxfId="77">
       <calculatedColumnFormula>MAX(0,(md!BK7-md!BJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="150" xr3:uid="{8BCAA082-E4E6-4619-8E56-A97B1FF4DA44}" name="26-May" dataDxfId="75">
+    <tableColumn id="150" xr3:uid="{8BCAA082-E4E6-4619-8E56-A97B1FF4DA44}" name="26-May" dataDxfId="76">
       <calculatedColumnFormula>MAX(0,(md!BL7-md!BK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="151" xr3:uid="{4B648A3F-3FCE-4C12-A50A-9BA09CA2697D}" name="27-May" dataDxfId="74">
+    <tableColumn id="151" xr3:uid="{4B648A3F-3FCE-4C12-A50A-9BA09CA2697D}" name="27-May" dataDxfId="75">
       <calculatedColumnFormula>MAX(0,(md!BM7-md!BL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="152" xr3:uid="{08604342-CE44-4618-A009-2731984B9556}" name="28-May" dataDxfId="73">
+    <tableColumn id="152" xr3:uid="{08604342-CE44-4618-A009-2731984B9556}" name="28-May" dataDxfId="74">
       <calculatedColumnFormula>MAX(0,(md!BN7-md!BM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="153" xr3:uid="{DC12CF48-1275-46AA-8DAC-6A196EDD8425}" name="29-May" dataDxfId="72">
+    <tableColumn id="153" xr3:uid="{DC12CF48-1275-46AA-8DAC-6A196EDD8425}" name="29-May" dataDxfId="73">
       <calculatedColumnFormula>MAX(0,(md!BO7-md!BN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="154" xr3:uid="{95A3B7F7-AC6C-4005-9B4D-70C3E3528929}" name="30-May" dataDxfId="71">
+    <tableColumn id="154" xr3:uid="{95A3B7F7-AC6C-4005-9B4D-70C3E3528929}" name="30-May" dataDxfId="72">
       <calculatedColumnFormula>MAX(0,(md!BP7-md!BO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="155" xr3:uid="{944A9E83-F75D-4D8B-AD2C-0A52AF055690}" name="31-May" dataDxfId="70">
+    <tableColumn id="155" xr3:uid="{944A9E83-F75D-4D8B-AD2C-0A52AF055690}" name="31-May" dataDxfId="71">
       <calculatedColumnFormula>MAX(0,(md!BQ7-md!BP7))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2562,209 +2561,209 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDE4BA6F-093B-443E-8276-7E7D049C5DE1}" name="delta_va" displayName="delta_va" ref="A10:BS143" totalsRowShown="0">
   <tableColumns count="71">
-    <tableColumn id="54" xr3:uid="{63B1A33A-0643-4DA3-8D65-E8A8D674C2E1}" name="Locality" dataDxfId="69"/>
-    <tableColumn id="1" xr3:uid="{FD33FE71-7C53-4ED0-99A2-CBB9B098FECC}" name="idx" dataDxfId="68"/>
+    <tableColumn id="54" xr3:uid="{63B1A33A-0643-4DA3-8D65-E8A8D674C2E1}" name="Locality" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{FD33FE71-7C53-4ED0-99A2-CBB9B098FECC}" name="idx" dataDxfId="69"/>
     <tableColumn id="2" xr3:uid="{76548448-4B06-473A-8C19-5749153B6A1D}" name="FIPS"/>
-    <tableColumn id="5" xr3:uid="{D127FF93-52D6-4EBE-92DB-D405A7B74D76}" name="25-Mar" dataDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{6A775A38-C028-4EC5-8C4E-7EBA81CA3009}" name="26-Mar" dataDxfId="66">
+    <tableColumn id="5" xr3:uid="{D127FF93-52D6-4EBE-92DB-D405A7B74D76}" name="25-Mar" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{6A775A38-C028-4EC5-8C4E-7EBA81CA3009}" name="26-Mar" dataDxfId="67">
       <calculatedColumnFormula>MAX(0,(va!F7-va!E7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{273C7511-9B33-45E4-A0E0-0B7D9493A13A}" name="27-Mar" dataDxfId="65">
+    <tableColumn id="30" xr3:uid="{273C7511-9B33-45E4-A0E0-0B7D9493A13A}" name="27-Mar" dataDxfId="66">
       <calculatedColumnFormula>MAX(0,(va!G7-va!F7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{ACC6CBDC-670D-4A3A-BEBD-B09E9FB43BC8}" name="28-Mar" dataDxfId="64">
+    <tableColumn id="31" xr3:uid="{ACC6CBDC-670D-4A3A-BEBD-B09E9FB43BC8}" name="28-Mar" dataDxfId="65">
       <calculatedColumnFormula>MAX(0,(va!H7-va!G7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{E53ECB20-6303-43A3-938C-9363F2920F4D}" name="29-Mar" dataDxfId="63">
+    <tableColumn id="32" xr3:uid="{E53ECB20-6303-43A3-938C-9363F2920F4D}" name="29-Mar" dataDxfId="64">
       <calculatedColumnFormula>MAX(0,(va!I7-va!H7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{4BD36DEA-292C-4095-8245-CFB513181126}" name="30-Mar" dataDxfId="62">
+    <tableColumn id="33" xr3:uid="{4BD36DEA-292C-4095-8245-CFB513181126}" name="30-Mar" dataDxfId="63">
       <calculatedColumnFormula>MAX(0,(va!J7-va!I7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{F1252424-C6F2-4FD1-A193-AC77B37E1DD7}" name="31-Mar" dataDxfId="61">
+    <tableColumn id="34" xr3:uid="{F1252424-C6F2-4FD1-A193-AC77B37E1DD7}" name="31-Mar" dataDxfId="62">
       <calculatedColumnFormula>MAX(0,(va!K7-va!J7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{CD743EF6-E0C5-4901-981D-2F27459CF468}" name="1-Apr" dataDxfId="60">
+    <tableColumn id="35" xr3:uid="{CD743EF6-E0C5-4901-981D-2F27459CF468}" name="1-Apr" dataDxfId="61">
       <calculatedColumnFormula>MAX(0,(va!L7-va!K7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{38ED5D84-2B28-479F-8C2D-B040039247F1}" name="2-Apr" dataDxfId="59">
+    <tableColumn id="36" xr3:uid="{38ED5D84-2B28-479F-8C2D-B040039247F1}" name="2-Apr" dataDxfId="60">
       <calculatedColumnFormula>MAX(0,(va!M7-va!L7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{CE521412-A311-433D-93C0-63BD7A514269}" name="3-Apr" dataDxfId="58">
+    <tableColumn id="37" xr3:uid="{CE521412-A311-433D-93C0-63BD7A514269}" name="3-Apr" dataDxfId="59">
       <calculatedColumnFormula>MAX(0,(va!N7-va!M7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{5D4C35B4-2054-4B4A-80F8-E9361CEA0ACC}" name="4-Apr" dataDxfId="57">
+    <tableColumn id="38" xr3:uid="{5D4C35B4-2054-4B4A-80F8-E9361CEA0ACC}" name="4-Apr" dataDxfId="58">
       <calculatedColumnFormula>MAX(0,(va!O7-va!N7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{10A2F446-2134-49BE-8AEF-2D84D9FA875B}" name="5-Apr" dataDxfId="56">
+    <tableColumn id="39" xr3:uid="{10A2F446-2134-49BE-8AEF-2D84D9FA875B}" name="5-Apr" dataDxfId="57">
       <calculatedColumnFormula>MAX(0,(va!P7-va!O7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{070AE366-CB37-4620-BA0C-1BE4F2C27279}" name="6-Apr" dataDxfId="55">
+    <tableColumn id="40" xr3:uid="{070AE366-CB37-4620-BA0C-1BE4F2C27279}" name="6-Apr" dataDxfId="56">
       <calculatedColumnFormula>MAX(0,(va!Q7-va!P7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{FBB50AAC-FF54-4926-8A78-E153DAC9F95B}" name="7-Apr" dataDxfId="54">
+    <tableColumn id="41" xr3:uid="{FBB50AAC-FF54-4926-8A78-E153DAC9F95B}" name="7-Apr" dataDxfId="55">
       <calculatedColumnFormula>MAX(0,(va!R7-va!Q7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{80F1496C-DB69-4C7F-9B80-445A59EF1B6D}" name="8-Apr" dataDxfId="53">
+    <tableColumn id="42" xr3:uid="{80F1496C-DB69-4C7F-9B80-445A59EF1B6D}" name="8-Apr" dataDxfId="54">
       <calculatedColumnFormula>MAX(0,(va!S7-va!R7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{B2D70650-881C-44FB-A51E-6DE0013D50F5}" name="9-Apr" dataDxfId="52">
+    <tableColumn id="43" xr3:uid="{B2D70650-881C-44FB-A51E-6DE0013D50F5}" name="9-Apr" dataDxfId="53">
       <calculatedColumnFormula>MAX(0,(va!T7-va!S7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{24972282-0E25-4AD5-A741-F9215388ABC2}" name="10-Apr" dataDxfId="51">
+    <tableColumn id="44" xr3:uid="{24972282-0E25-4AD5-A741-F9215388ABC2}" name="10-Apr" dataDxfId="52">
       <calculatedColumnFormula>MAX(0,(va!U7-va!T7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{6D9BB0E2-F429-49ED-BDB5-F356A4DC28CD}" name="11-Apr" dataDxfId="50">
+    <tableColumn id="45" xr3:uid="{6D9BB0E2-F429-49ED-BDB5-F356A4DC28CD}" name="11-Apr" dataDxfId="51">
       <calculatedColumnFormula>MAX(0,(va!V7-va!U7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{B7D6F42A-CE7F-4560-915A-2D75BB5FB9A7}" name="12-Apr" dataDxfId="49">
+    <tableColumn id="46" xr3:uid="{B7D6F42A-CE7F-4560-915A-2D75BB5FB9A7}" name="12-Apr" dataDxfId="50">
       <calculatedColumnFormula>MAX(0,(va!W7-va!V7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{D27C7A8C-BAA4-4A29-97DC-6D26B5399868}" name="13-Apr" dataDxfId="48">
+    <tableColumn id="47" xr3:uid="{D27C7A8C-BAA4-4A29-97DC-6D26B5399868}" name="13-Apr" dataDxfId="49">
       <calculatedColumnFormula>MAX(0,(va!X7-va!W7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{F892CCC7-B11E-4EF0-95BE-4BFE027CFFD1}" name="14-Apr" dataDxfId="47">
+    <tableColumn id="48" xr3:uid="{F892CCC7-B11E-4EF0-95BE-4BFE027CFFD1}" name="14-Apr" dataDxfId="48">
       <calculatedColumnFormula>MAX(0,(va!Y7-va!X7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{A3F0E963-9326-4555-ADE5-F4EFB83126F3}" name="15-Apr" dataDxfId="46">
+    <tableColumn id="49" xr3:uid="{A3F0E963-9326-4555-ADE5-F4EFB83126F3}" name="15-Apr" dataDxfId="47">
       <calculatedColumnFormula>MAX(0,(va!Z7-va!Y7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" xr3:uid="{3437FD4E-8616-4572-907D-5B33B199B617}" name="16-Apr" dataDxfId="45">
+    <tableColumn id="50" xr3:uid="{3437FD4E-8616-4572-907D-5B33B199B617}" name="16-Apr" dataDxfId="46">
       <calculatedColumnFormula>MAX(0,(va!AA7-va!Z7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{E6F99628-1312-41B6-A56A-B05C101DA0FB}" name="17-Apr" dataDxfId="44">
+    <tableColumn id="51" xr3:uid="{E6F99628-1312-41B6-A56A-B05C101DA0FB}" name="17-Apr" dataDxfId="45">
       <calculatedColumnFormula>MAX(0,(va!AB7-va!AA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{C7724E90-6B56-4650-A710-D3E539E48665}" name="18-Apr" dataDxfId="43">
+    <tableColumn id="52" xr3:uid="{C7724E90-6B56-4650-A710-D3E539E48665}" name="18-Apr" dataDxfId="44">
       <calculatedColumnFormula>MAX(0,(va!AC7-va!AB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{2321B68A-9B81-4AD5-BC7B-70E930711815}" name="19-Apr" dataDxfId="42">
+    <tableColumn id="53" xr3:uid="{2321B68A-9B81-4AD5-BC7B-70E930711815}" name="19-Apr" dataDxfId="43">
       <calculatedColumnFormula>MAX(0,(va!AD7-va!AC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{0909EDD8-E202-4043-8949-F6EA28E1C4AA}" name="20-Apr" dataDxfId="41">
+    <tableColumn id="22" xr3:uid="{0909EDD8-E202-4043-8949-F6EA28E1C4AA}" name="20-Apr" dataDxfId="42">
       <calculatedColumnFormula>MAX(0,(va!AE7-va!AD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{2367F62B-C6E4-48C7-81C9-530399CE2871}" name="21-Apr" dataDxfId="40">
+    <tableColumn id="23" xr3:uid="{2367F62B-C6E4-48C7-81C9-530399CE2871}" name="21-Apr" dataDxfId="41">
       <calculatedColumnFormula>MAX(0,(va!AF7-va!AE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{EB75A609-8DAC-42A0-990A-114C4750203C}" name="22-Apr" dataDxfId="39">
+    <tableColumn id="24" xr3:uid="{EB75A609-8DAC-42A0-990A-114C4750203C}" name="22-Apr" dataDxfId="40">
       <calculatedColumnFormula>MAX(0,(va!AG7-va!AF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{F23D1A1C-FDCB-42E7-BFFE-8860B35519AC}" name="23-Apr" dataDxfId="38">
+    <tableColumn id="25" xr3:uid="{F23D1A1C-FDCB-42E7-BFFE-8860B35519AC}" name="23-Apr" dataDxfId="39">
       <calculatedColumnFormula>MAX(0,(va!AH7-va!AG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{F5222424-7E21-47C9-A5EE-468D35C8D4D4}" name="24-Apr" dataDxfId="37">
+    <tableColumn id="26" xr3:uid="{F5222424-7E21-47C9-A5EE-468D35C8D4D4}" name="24-Apr" dataDxfId="38">
       <calculatedColumnFormula>MAX(0,(va!AI7-va!AH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{F5D517E5-C861-4DD4-A408-D023894C3440}" name="25-Apr" dataDxfId="36">
+    <tableColumn id="27" xr3:uid="{F5D517E5-C861-4DD4-A408-D023894C3440}" name="25-Apr" dataDxfId="37">
       <calculatedColumnFormula>MAX(0,(va!AJ7-va!AI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{6663E32B-51D1-4285-89F0-ADB6AC73C467}" name="26-Apr" dataDxfId="35">
+    <tableColumn id="28" xr3:uid="{6663E32B-51D1-4285-89F0-ADB6AC73C467}" name="26-Apr" dataDxfId="36">
       <calculatedColumnFormula>MAX(0,(va!AK7-va!AJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{F1067EAF-A27C-4330-9D36-8E8450545F45}" name="27-Apr" dataDxfId="34">
+    <tableColumn id="29" xr3:uid="{F1067EAF-A27C-4330-9D36-8E8450545F45}" name="27-Apr" dataDxfId="35">
       <calculatedColumnFormula>MAX(0,(va!AL7-va!AK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AC4610E3-C7C4-4914-AA0E-DB2D0357ED06}" name="28-Apr" dataDxfId="33">
+    <tableColumn id="14" xr3:uid="{AC4610E3-C7C4-4914-AA0E-DB2D0357ED06}" name="28-Apr" dataDxfId="34">
       <calculatedColumnFormula>MAX(0,(va!AM7-va!AL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{FF6B8433-3EC6-458E-89D7-5EB244B1F60B}" name="29-Apr" dataDxfId="32">
+    <tableColumn id="15" xr3:uid="{FF6B8433-3EC6-458E-89D7-5EB244B1F60B}" name="29-Apr" dataDxfId="33">
       <calculatedColumnFormula>MAX(0,(va!AN7-va!AM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{BA897434-B64A-4817-A3F9-46FF64B05E37}" name="30-Apr" dataDxfId="31">
+    <tableColumn id="16" xr3:uid="{BA897434-B64A-4817-A3F9-46FF64B05E37}" name="30-Apr" dataDxfId="32">
       <calculatedColumnFormula>MAX(0,(va!AO7-va!AN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{6AE0C639-A5DD-42D5-8FA4-8C9B3EA56006}" name="1-May" dataDxfId="30">
+    <tableColumn id="17" xr3:uid="{6AE0C639-A5DD-42D5-8FA4-8C9B3EA56006}" name="1-May" dataDxfId="31">
       <calculatedColumnFormula>MAX(0,(va!AP7-va!AO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{5E07F0EB-D30C-4867-AED9-8E88FBC08D77}" name="2-May" dataDxfId="29">
+    <tableColumn id="18" xr3:uid="{5E07F0EB-D30C-4867-AED9-8E88FBC08D77}" name="2-May" dataDxfId="30">
       <calculatedColumnFormula>MAX(0,(va!AQ7-va!AP7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{7E7DFBC2-6059-4A36-AF80-B77B98657554}" name="3-May" dataDxfId="28">
+    <tableColumn id="19" xr3:uid="{7E7DFBC2-6059-4A36-AF80-B77B98657554}" name="3-May" dataDxfId="29">
       <calculatedColumnFormula>MAX(0,(va!AR7-va!AQ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{04DF1446-184B-4D11-B3CA-CBA62452BF62}" name="4-May" dataDxfId="27">
+    <tableColumn id="20" xr3:uid="{04DF1446-184B-4D11-B3CA-CBA62452BF62}" name="4-May" dataDxfId="28">
       <calculatedColumnFormula>MAX(0,(va!AS7-va!AR7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{8B99FEA6-1FD6-49F9-9871-F98BDB596D5E}" name="5-May" dataDxfId="26">
+    <tableColumn id="21" xr3:uid="{8B99FEA6-1FD6-49F9-9871-F98BDB596D5E}" name="5-May" dataDxfId="27">
       <calculatedColumnFormula>MAX(0,(va!AT7-va!AS7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6658ADF8-B8F0-4C00-BEBC-CDE0466AF941}" name="6-May" dataDxfId="25">
+    <tableColumn id="10" xr3:uid="{6658ADF8-B8F0-4C00-BEBC-CDE0466AF941}" name="6-May" dataDxfId="26">
       <calculatedColumnFormula>MAX(0,(va!AU7-va!AT7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{3907184E-0754-43D6-A0B2-BA9FC1B11F9C}" name="7-May" dataDxfId="24">
+    <tableColumn id="11" xr3:uid="{3907184E-0754-43D6-A0B2-BA9FC1B11F9C}" name="7-May" dataDxfId="25">
       <calculatedColumnFormula>MAX(0,(va!AV7-va!AU7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F7EBE278-C13F-43E7-B6C5-146063646048}" name="8-May" dataDxfId="23">
+    <tableColumn id="12" xr3:uid="{F7EBE278-C13F-43E7-B6C5-146063646048}" name="8-May" dataDxfId="24">
       <calculatedColumnFormula>MAX(0,(va!AW7-va!AV7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{B169461D-64D3-4BF0-BD2E-EC9669326BEF}" name="9-May" dataDxfId="22">
+    <tableColumn id="13" xr3:uid="{B169461D-64D3-4BF0-BD2E-EC9669326BEF}" name="9-May" dataDxfId="23">
       <calculatedColumnFormula>MAX(0,(va!AX7-va!AW7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD44E28B-08BF-4D2B-BEE3-9536EEE5373F}" name="10-May" dataDxfId="21">
+    <tableColumn id="8" xr3:uid="{CD44E28B-08BF-4D2B-BEE3-9536EEE5373F}" name="10-May" dataDxfId="22">
       <calculatedColumnFormula>MAX(0,(va!AY7-va!AX7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A4B9A93-0725-4010-A087-30E03FE5D7BA}" name="11-May" dataDxfId="20">
+    <tableColumn id="9" xr3:uid="{4A4B9A93-0725-4010-A087-30E03FE5D7BA}" name="11-May" dataDxfId="21">
       <calculatedColumnFormula>MAX(0,(va!AZ7-va!AY7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2E62BF37-C2F6-4728-B7D3-D5351C180DB1}" name="12-May" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{2E62BF37-C2F6-4728-B7D3-D5351C180DB1}" name="12-May" dataDxfId="20">
       <calculatedColumnFormula>MAX(0,(va!BA7-va!AZ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33AAE041-9853-4118-9ABB-D3E20ADE0CDA}" name="13-May" dataDxfId="18">
+    <tableColumn id="4" xr3:uid="{33AAE041-9853-4118-9ABB-D3E20ADE0CDA}" name="13-May" dataDxfId="19">
       <calculatedColumnFormula>MAX(0,(va!BB7-va!BA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{84C1D2A4-6A91-4756-BB95-DBFFFC7C0C27}" name="14-May" dataDxfId="17">
+    <tableColumn id="55" xr3:uid="{84C1D2A4-6A91-4756-BB95-DBFFFC7C0C27}" name="14-May" dataDxfId="18">
       <calculatedColumnFormula>MAX(0,(va!BC7-va!BB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="56" xr3:uid="{6A194ED5-9BB1-440C-A0AC-25E5553948E0}" name="15-May" dataDxfId="16">
+    <tableColumn id="56" xr3:uid="{6A194ED5-9BB1-440C-A0AC-25E5553948E0}" name="15-May" dataDxfId="17">
       <calculatedColumnFormula>MAX(0,(va!BD7-va!BC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="57" xr3:uid="{E4944CC5-EA4C-4102-87EC-2BBD05DEB3CC}" name="16-May" dataDxfId="15">
+    <tableColumn id="57" xr3:uid="{E4944CC5-EA4C-4102-87EC-2BBD05DEB3CC}" name="16-May" dataDxfId="16">
       <calculatedColumnFormula>MAX(0,(va!BE7-va!BD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="58" xr3:uid="{80518BBE-DB7B-456F-BA3F-098675345342}" name="17-May" dataDxfId="14">
+    <tableColumn id="58" xr3:uid="{80518BBE-DB7B-456F-BA3F-098675345342}" name="17-May" dataDxfId="15">
       <calculatedColumnFormula>MAX(0,(va!BF7-va!BE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" xr3:uid="{8890D892-2DB0-4294-B2B0-F0E35897244B}" name="18-May" dataDxfId="13">
+    <tableColumn id="59" xr3:uid="{8890D892-2DB0-4294-B2B0-F0E35897244B}" name="18-May" dataDxfId="14">
       <calculatedColumnFormula>MAX(0,(va!BG7-va!BF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="60" xr3:uid="{3C7B710E-EE82-4733-8595-B3558286C4A4}" name="19-May" dataDxfId="12">
+    <tableColumn id="60" xr3:uid="{3C7B710E-EE82-4733-8595-B3558286C4A4}" name="19-May" dataDxfId="13">
       <calculatedColumnFormula>MAX(0,(va!BH7-va!BG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="61" xr3:uid="{15806639-509B-4998-B1F9-4D768A2A4FF8}" name="20-May" dataDxfId="11">
+    <tableColumn id="61" xr3:uid="{15806639-509B-4998-B1F9-4D768A2A4FF8}" name="20-May" dataDxfId="12">
       <calculatedColumnFormula>MAX(0,(va!BI7-va!BH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{979C3098-F4F8-4A51-B7AF-115BE23F8E36}" name="21-May" dataDxfId="10">
+    <tableColumn id="62" xr3:uid="{979C3098-F4F8-4A51-B7AF-115BE23F8E36}" name="21-May" dataDxfId="11">
       <calculatedColumnFormula>MAX(0,(va!BJ7-va!BI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{581E410D-1F56-463B-A79B-39C309A32AD5}" name="22-May" dataDxfId="9">
+    <tableColumn id="63" xr3:uid="{581E410D-1F56-463B-A79B-39C309A32AD5}" name="22-May" dataDxfId="10">
       <calculatedColumnFormula>MAX(0,(va!BK7-va!BJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{7DEACC7F-9EE9-4ECB-9078-A7DFE44015D5}" name="23-May" dataDxfId="8">
+    <tableColumn id="64" xr3:uid="{7DEACC7F-9EE9-4ECB-9078-A7DFE44015D5}" name="23-May" dataDxfId="9">
       <calculatedColumnFormula>MAX(0,(va!BL7-va!BK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{F4060BBB-E4ED-4A58-A557-430AD718B5CB}" name="24-May" dataDxfId="7">
+    <tableColumn id="65" xr3:uid="{F4060BBB-E4ED-4A58-A557-430AD718B5CB}" name="24-May" dataDxfId="8">
       <calculatedColumnFormula>MAX(0,(va!BM7-va!BL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{DFA30D74-C0ED-439F-B66D-B8802D5CB693}" name="25-May" dataDxfId="6">
+    <tableColumn id="66" xr3:uid="{DFA30D74-C0ED-439F-B66D-B8802D5CB693}" name="25-May" dataDxfId="7">
       <calculatedColumnFormula>MAX(0,(va!BN7-va!BM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{81E9478F-D6B4-4B44-B1E3-77E1D6C58E52}" name="26-May" dataDxfId="5">
+    <tableColumn id="67" xr3:uid="{81E9478F-D6B4-4B44-B1E3-77E1D6C58E52}" name="26-May" dataDxfId="6">
       <calculatedColumnFormula>MAX(0,(va!BO7-va!BN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="68" xr3:uid="{28BE5C31-58B2-4EB9-875C-DB12815ABB54}" name="27-May" dataDxfId="4">
+    <tableColumn id="68" xr3:uid="{28BE5C31-58B2-4EB9-875C-DB12815ABB54}" name="27-May" dataDxfId="5">
       <calculatedColumnFormula>MAX(0,(va!BP7-va!BO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="69" xr3:uid="{C8F214AC-38D3-49D8-A4C1-772682FA80C7}" name="28-May" dataDxfId="3">
+    <tableColumn id="69" xr3:uid="{C8F214AC-38D3-49D8-A4C1-772682FA80C7}" name="28-May" dataDxfId="4">
       <calculatedColumnFormula>MAX(0,(va!BQ7-va!BP7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="70" xr3:uid="{EE1980CC-3CC5-46F1-BA70-2D4487917FFD}" name="29-May" dataDxfId="2">
+    <tableColumn id="70" xr3:uid="{EE1980CC-3CC5-46F1-BA70-2D4487917FFD}" name="29-May" dataDxfId="3">
       <calculatedColumnFormula>MAX(0,(va!BR7-va!BQ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="71" xr3:uid="{05E114EA-2EEA-46AA-92A0-906C6A3D082F}" name="30-May" dataDxfId="1">
+    <tableColumn id="71" xr3:uid="{05E114EA-2EEA-46AA-92A0-906C6A3D082F}" name="30-May" dataDxfId="2">
       <calculatedColumnFormula>MAX(0,(va!BS7-va!BR7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="72" xr3:uid="{55F28C38-AF0C-4D02-AC6A-D856844BFEF1}" name="31-May" dataDxfId="0">
+    <tableColumn id="72" xr3:uid="{55F28C38-AF0C-4D02-AC6A-D856844BFEF1}" name="31-May" dataDxfId="1">
       <calculatedColumnFormula>MAX(0,(va!BT7-va!BS7))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3071,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E207B2A-317D-4660-A7D7-5B9F35994222}">
   <dimension ref="A1:CC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3170,7 +3169,7 @@
       <c r="Z2" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="18" t="s">
         <v>191</v>
       </c>
       <c r="AB2" s="3" t="s">
@@ -3412,10 +3411,13 @@
       <c r="Z3" s="12">
         <v>7823</v>
       </c>
+      <c r="AA3" s="12">
+        <v>8283</v>
+      </c>
     </row>
     <row r="4" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B4" s="10">
         <v>10</v>
@@ -3494,6 +3496,9 @@
       </c>
       <c r="Z4" s="10">
         <v>1211</v>
+      </c>
+      <c r="AA4" s="10">
+        <v>1440</v>
       </c>
     </row>
     <row r="5" spans="1:81" x14ac:dyDescent="0.35">
@@ -3579,6 +3584,9 @@
       </c>
       <c r="Z6" s="10">
         <v>22</v>
+      </c>
+      <c r="AA6" s="10">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.35">
@@ -3709,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B685ED27-8882-4CE7-837C-253FB4ACFF90}">
   <dimension ref="A1:BQ31"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3724,14 +3732,13 @@
       <c r="A1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="9" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="10">
@@ -3774,7 +3781,7 @@
         <v>27256</v>
       </c>
       <c r="P2" s="10">
-        <v>0</v>
+        <v>32933</v>
       </c>
       <c r="Q2" s="10">
         <v>0</v>
@@ -3938,7 +3945,7 @@
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C3">
         <f>SUM(md[26-Mar])</f>
@@ -3989,11 +3996,11 @@
       </c>
       <c r="O3" s="10">
         <f>SUM(md[7-Apr])</f>
-        <v>3352</v>
+        <v>4371</v>
       </c>
       <c r="P3" s="10">
         <f>SUM(md[8-Apr])</f>
-        <v>0</v>
+        <v>5529</v>
       </c>
       <c r="Q3" s="10">
         <f>SUM(md[9-Apr])</f>
@@ -4252,7 +4259,7 @@
         <v>1106</v>
       </c>
       <c r="P4" s="10">
-        <v>0</v>
+        <v>1210</v>
       </c>
       <c r="Q4" s="10">
         <v>0</v>
@@ -4458,7 +4465,7 @@
         <v>103</v>
       </c>
       <c r="P5" s="10">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="Q5" s="10">
         <v>0</v>
@@ -4666,7 +4673,7 @@
       <c r="O6" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="18" t="s">
         <v>192</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -4875,6 +4882,9 @@
       <c r="O7">
         <v>7</v>
       </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -4922,6 +4932,9 @@
       <c r="O8" s="10">
         <v>370</v>
       </c>
+      <c r="P8" s="10">
+        <v>466</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -4969,6 +4982,9 @@
       <c r="O9">
         <v>459</v>
       </c>
+      <c r="P9">
+        <v>571</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -5016,6 +5032,9 @@
       <c r="O10">
         <v>652</v>
       </c>
+      <c r="P10">
+        <v>866</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -5063,6 +5082,9 @@
       <c r="O11">
         <v>41</v>
       </c>
+      <c r="P11">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -5110,6 +5132,9 @@
       <c r="O12">
         <v>11</v>
       </c>
+      <c r="P12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -5157,6 +5182,9 @@
       <c r="O13">
         <v>159</v>
       </c>
+      <c r="P13">
+        <v>186</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -5204,6 +5232,9 @@
       <c r="O14">
         <v>41</v>
       </c>
+      <c r="P14">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -5251,6 +5282,9 @@
       <c r="O15">
         <v>136</v>
       </c>
+      <c r="P15">
+        <v>164</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -5298,8 +5332,11 @@
       <c r="O16" s="10">
         <v>3</v>
       </c>
+      <c r="P16" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -5345,8 +5382,11 @@
       <c r="O17">
         <v>151</v>
       </c>
+      <c r="P17">
+        <v>199</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -5392,8 +5432,11 @@
       <c r="O18">
         <v>3</v>
       </c>
+      <c r="P18">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -5439,8 +5482,11 @@
       <c r="O19">
         <v>59</v>
       </c>
+      <c r="P19">
+        <v>86</v>
+      </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -5486,8 +5532,11 @@
       <c r="O20">
         <v>236</v>
       </c>
+      <c r="P20">
+        <v>274</v>
+      </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -5533,8 +5582,11 @@
       <c r="O21">
         <v>8</v>
       </c>
+      <c r="P21">
+        <v>9</v>
+      </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -5580,8 +5632,11 @@
       <c r="O22">
         <v>871</v>
       </c>
+      <c r="P22">
+        <v>1088</v>
+      </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -5625,10 +5680,13 @@
         <v>916</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>1020</v>
+      </c>
+      <c r="P23">
+        <v>1310</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -5674,8 +5732,11 @@
       <c r="O24">
         <v>15</v>
       </c>
+      <c r="P24">
+        <v>16</v>
+      </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -5721,8 +5782,11 @@
       <c r="O25">
         <v>46</v>
       </c>
+      <c r="P25">
+        <v>62</v>
+      </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -5768,8 +5832,11 @@
       <c r="O26">
         <v>4</v>
       </c>
+      <c r="P26">
+        <v>4</v>
+      </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -5815,8 +5882,11 @@
       <c r="O27">
         <v>8</v>
       </c>
+      <c r="P27">
+        <v>10</v>
+      </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -5862,8 +5932,11 @@
       <c r="O28">
         <v>44</v>
       </c>
+      <c r="P28">
+        <v>57</v>
+      </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -5909,8 +5982,11 @@
       <c r="O29">
         <v>17</v>
       </c>
+      <c r="P29">
+        <v>20</v>
+      </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -5956,14 +6032,17 @@
       <c r="O30">
         <v>10</v>
       </c>
+      <c r="P30">
+        <v>10</v>
+      </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C1:BQ2">
+  <conditionalFormatting sqref="C2:BQ2 D1:BQ1 B1">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -6036,7 +6115,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{EB21EFCC-2A79-4CFF-97FA-7077A84411CA}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{EB21EFCC-2A79-4CFF-97FA-7077A84411CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6051,7 +6130,7 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6077,7 +6156,7 @@
     </row>
     <row r="2" spans="1:72" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E2" s="10">
         <f>SUM(va[25-Mar])</f>
@@ -6137,7 +6216,7 @@
       </c>
       <c r="S2" s="10">
         <f>SUM(va[8-Apr])</f>
-        <v>0</v>
+        <v>3645</v>
       </c>
       <c r="T2" s="10">
         <f>SUM(va[9-Apr])</f>
@@ -6399,7 +6478,7 @@
         <v>563</v>
       </c>
       <c r="S3" s="10">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="T3" s="10">
         <v>0</v>
@@ -6608,7 +6687,7 @@
         <v>63</v>
       </c>
       <c r="S4" s="10">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="T4" s="10">
         <v>0</v>
@@ -6817,7 +6896,7 @@
         <v>28645</v>
       </c>
       <c r="S5" s="10">
-        <v>0</v>
+        <v>30645</v>
       </c>
       <c r="T5" s="10">
         <v>0</v>
@@ -7252,9 +7331,12 @@
       <c r="R7" s="10">
         <v>126</v>
       </c>
+      <c r="S7" s="10">
+        <v>143</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -7308,9 +7390,12 @@
       <c r="R8" s="10">
         <v>2</v>
       </c>
+      <c r="S8" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -7362,9 +7447,12 @@
       <c r="R9" s="10">
         <v>18</v>
       </c>
+      <c r="S9" s="10">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A10" s="24"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -7416,9 +7504,12 @@
       <c r="R10" s="10">
         <v>2</v>
       </c>
+      <c r="S10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -7470,9 +7561,12 @@
       <c r="R11" s="10">
         <v>8</v>
       </c>
+      <c r="S11" s="10">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A12" s="24"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -7524,9 +7618,12 @@
       <c r="R12" s="10">
         <v>1</v>
       </c>
+      <c r="S12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -7576,6 +7673,9 @@
         <v>1</v>
       </c>
       <c r="R13" s="10">
+        <v>1</v>
+      </c>
+      <c r="S13" s="10">
         <v>1</v>
       </c>
     </row>
@@ -7634,9 +7734,12 @@
       <c r="R14" s="10">
         <v>237</v>
       </c>
+      <c r="S14" s="10">
+        <v>254</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -7690,9 +7793,12 @@
       <c r="R15" s="10">
         <v>10</v>
       </c>
+      <c r="S15" s="10">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A16" s="24"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -7744,9 +7850,12 @@
       <c r="R16" s="10">
         <v>0</v>
       </c>
+      <c r="S16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="24"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -7798,9 +7907,12 @@
       <c r="R17" s="10">
         <v>0</v>
       </c>
+      <c r="S17" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="24"/>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -7852,9 +7964,12 @@
       <c r="R18" s="10">
         <v>3</v>
       </c>
+      <c r="S18" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="24"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -7906,9 +8021,12 @@
       <c r="R19" s="10">
         <v>16</v>
       </c>
+      <c r="S19" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="24"/>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -7960,9 +8078,12 @@
       <c r="R20" s="10">
         <v>4</v>
       </c>
+      <c r="S20" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="27"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -8014,9 +8135,12 @@
       <c r="R21" s="10">
         <v>27</v>
       </c>
+      <c r="S21" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="24"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="27"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -8068,9 +8192,12 @@
       <c r="R22" s="10">
         <v>3</v>
       </c>
+      <c r="S22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="24"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="27"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -8122,9 +8249,12 @@
       <c r="R23" s="10">
         <v>1</v>
       </c>
+      <c r="S23" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="28"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -8176,9 +8306,12 @@
       <c r="R24" s="10">
         <v>2</v>
       </c>
+      <c r="S24" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A25" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -8232,9 +8365,12 @@
       <c r="R25" s="10">
         <v>8</v>
       </c>
+      <c r="S25" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A26" s="24"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -8286,9 +8422,12 @@
       <c r="R26" s="10">
         <v>3</v>
       </c>
+      <c r="S26" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A27" s="24"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -8340,9 +8479,12 @@
       <c r="R27" s="10">
         <v>8</v>
       </c>
+      <c r="S27" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="27"/>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A28" s="24"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -8394,9 +8536,12 @@
       <c r="R28" s="10">
         <v>3</v>
       </c>
+      <c r="S28" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29" s="25"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -8448,8 +8593,11 @@
       <c r="R29" s="10">
         <v>20</v>
       </c>
+      <c r="S29" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -8504,9 +8652,12 @@
       <c r="R30" s="10">
         <v>80</v>
       </c>
+      <c r="S30" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A31" s="26" t="s">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -8560,9 +8711,12 @@
       <c r="R31" s="10">
         <v>128</v>
       </c>
+      <c r="S31" s="10">
+        <v>145</v>
+      </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A32" s="27"/>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" s="24"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -8614,9 +8768,12 @@
       <c r="R32" s="10">
         <v>4</v>
       </c>
+      <c r="S32" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A33" s="25"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -8668,9 +8825,12 @@
       <c r="R33" s="10">
         <v>0</v>
       </c>
+      <c r="S33" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A34" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -8724,9 +8884,12 @@
       <c r="R34" s="10">
         <v>4</v>
       </c>
+      <c r="S34" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="24"/>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -8778,9 +8941,12 @@
       <c r="R35" s="10">
         <v>22</v>
       </c>
+      <c r="S35" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="24"/>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -8832,9 +8998,12 @@
       <c r="R36" s="10">
         <v>19</v>
       </c>
+      <c r="S36" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A37" s="25"/>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A37" s="28"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -8886,9 +9055,12 @@
       <c r="R37" s="10">
         <v>12</v>
       </c>
+      <c r="S37" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A38" s="26" t="s">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A38" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -8942,9 +9114,12 @@
       <c r="R38" s="10">
         <v>1</v>
       </c>
+      <c r="S38" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A39" s="27"/>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39" s="24"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -8996,9 +9171,12 @@
       <c r="R39" s="10">
         <v>5</v>
       </c>
+      <c r="S39" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A40" s="27"/>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A40" s="24"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -9050,9 +9228,12 @@
       <c r="R40" s="10">
         <v>21</v>
       </c>
+      <c r="S40" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A41" s="27"/>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41" s="24"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -9104,9 +9285,12 @@
       <c r="R41" s="10">
         <v>3</v>
       </c>
+      <c r="S41" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A42" s="27"/>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A42" s="24"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -9158,9 +9342,12 @@
       <c r="R42" s="10">
         <v>5</v>
       </c>
+      <c r="S42" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A43" s="27"/>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A43" s="24"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -9212,9 +9399,12 @@
       <c r="R43" s="10">
         <v>2</v>
       </c>
+      <c r="S43" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A44" s="27"/>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44" s="24"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -9266,9 +9456,12 @@
       <c r="R44" s="10">
         <v>13</v>
       </c>
+      <c r="S44" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A45" s="28"/>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A45" s="25"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -9320,9 +9513,12 @@
       <c r="R45" s="10">
         <v>10</v>
       </c>
+      <c r="S45" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A46" s="23" t="s">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A46" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -9376,9 +9572,12 @@
       <c r="R46" s="10">
         <v>1</v>
       </c>
+      <c r="S46" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A47" s="24"/>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A47" s="27"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -9430,9 +9629,12 @@
       <c r="R47" s="10">
         <v>0</v>
       </c>
+      <c r="S47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A48" s="24"/>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A48" s="27"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -9484,9 +9686,12 @@
       <c r="R48" s="10">
         <v>1</v>
       </c>
+      <c r="S48" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A49" s="25"/>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A49" s="28"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -9538,9 +9743,12 @@
       <c r="R49" s="10">
         <v>4</v>
       </c>
+      <c r="S49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A50" s="26" t="s">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A50" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -9594,9 +9802,12 @@
       <c r="R50" s="10">
         <v>11</v>
       </c>
+      <c r="S50" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A51" s="28"/>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A51" s="25"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -9648,9 +9859,12 @@
       <c r="R51" s="10">
         <v>2</v>
       </c>
+      <c r="S51" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A52" s="23" t="s">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A52" s="26" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -9704,9 +9918,12 @@
       <c r="R52" s="10">
         <v>532</v>
       </c>
+      <c r="S52" s="10">
+        <v>570</v>
+      </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A53" s="24"/>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A53" s="27"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -9758,9 +9975,12 @@
       <c r="R53" s="10">
         <v>0</v>
       </c>
+      <c r="S53" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A54" s="25"/>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A54" s="28"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -9812,8 +10032,11 @@
       <c r="R54" s="10">
         <v>0</v>
       </c>
+      <c r="S54" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -9868,8 +10091,11 @@
       <c r="R55" s="10">
         <v>43</v>
       </c>
+      <c r="S55" s="10">
+        <v>53</v>
+      </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -9924,9 +10150,12 @@
       <c r="R56" s="10">
         <v>267</v>
       </c>
+      <c r="S56" s="10">
+        <v>291</v>
+      </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A57" s="26" t="s">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A57" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -9980,9 +10209,12 @@
       <c r="R57" s="10">
         <v>2</v>
       </c>
+      <c r="S57" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A58" s="27"/>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A58" s="24"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -10034,9 +10266,12 @@
       <c r="R58" s="10">
         <v>0</v>
       </c>
+      <c r="S58" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A59" s="27"/>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A59" s="24"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -10088,9 +10323,12 @@
       <c r="R59" s="10">
         <v>3</v>
       </c>
+      <c r="S59" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A60" s="28"/>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A60" s="25"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -10142,9 +10380,12 @@
       <c r="R60" s="10">
         <v>0</v>
       </c>
+      <c r="S60" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A61" s="23" t="s">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A61" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -10198,9 +10439,12 @@
       <c r="R61" s="10">
         <v>2</v>
       </c>
+      <c r="S61" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A62" s="24"/>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A62" s="27"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -10252,9 +10496,12 @@
       <c r="R62" s="10">
         <v>43</v>
       </c>
+      <c r="S62" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A63" s="24"/>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A63" s="27"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -10306,9 +10553,12 @@
       <c r="R63" s="10">
         <v>3</v>
       </c>
+      <c r="S63" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A64" s="24"/>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A64" s="27"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -10360,9 +10610,12 @@
       <c r="R64" s="10">
         <v>12</v>
       </c>
+      <c r="S64" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A65" s="24"/>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A65" s="27"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -10414,9 +10667,12 @@
       <c r="R65" s="10">
         <v>6</v>
       </c>
+      <c r="S65" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A66" s="25"/>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A66" s="28"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -10468,8 +10724,11 @@
       <c r="R66" s="10">
         <v>14</v>
       </c>
+      <c r="S66" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -10524,9 +10783,12 @@
       <c r="R67" s="10">
         <v>209</v>
       </c>
+      <c r="S67" s="10">
+        <v>238</v>
+      </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A68" s="23" t="s">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A68" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -10580,9 +10842,12 @@
       <c r="R68" s="10">
         <v>0</v>
       </c>
+      <c r="S68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A69" s="24"/>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A69" s="27"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -10634,9 +10899,12 @@
       <c r="R69" s="10">
         <v>2</v>
       </c>
+      <c r="S69" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A70" s="24"/>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A70" s="27"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -10688,9 +10956,12 @@
       <c r="R70" s="10">
         <v>0</v>
       </c>
+      <c r="S70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A71" s="24"/>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A71" s="27"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -10742,9 +11013,12 @@
       <c r="R71" s="10">
         <v>3</v>
       </c>
+      <c r="S71" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A72" s="24"/>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A72" s="27"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -10796,9 +11070,12 @@
       <c r="R72" s="10">
         <v>10</v>
       </c>
+      <c r="S72" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A73" s="24"/>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A73" s="27"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -10850,9 +11127,12 @@
       <c r="R73" s="10">
         <v>3</v>
       </c>
+      <c r="S73" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A74" s="24"/>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A74" s="27"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -10904,9 +11184,12 @@
       <c r="R74" s="10">
         <v>1</v>
       </c>
+      <c r="S74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A75" s="25"/>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A75" s="28"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -10958,9 +11241,12 @@
       <c r="R75" s="10">
         <v>1</v>
       </c>
+      <c r="S75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A76" s="26" t="s">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A76" s="23" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -11014,9 +11300,12 @@
       <c r="R76" s="10">
         <v>0</v>
       </c>
+      <c r="S76" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A77" s="27"/>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A77" s="24"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -11068,9 +11357,12 @@
       <c r="R77" s="10">
         <v>2</v>
       </c>
+      <c r="S77" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A78" s="27"/>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A78" s="24"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -11122,9 +11414,12 @@
       <c r="R78" s="10">
         <v>16</v>
       </c>
+      <c r="S78" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A79" s="27"/>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A79" s="24"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -11176,9 +11471,12 @@
       <c r="R79" s="10">
         <v>2</v>
       </c>
+      <c r="S79" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A80" s="28"/>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A80" s="25"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -11230,8 +11528,11 @@
       <c r="R80" s="10">
         <v>1</v>
       </c>
+      <c r="S80" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -11286,9 +11587,12 @@
       <c r="R81" s="10">
         <v>72</v>
       </c>
+      <c r="S81" s="10">
+        <v>77</v>
+      </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A82" s="26" t="s">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A82" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -11342,9 +11646,12 @@
       <c r="R82" s="10">
         <v>119</v>
       </c>
+      <c r="S82" s="10">
+        <v>122</v>
+      </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A83" s="27"/>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A83" s="24"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -11396,9 +11703,12 @@
       <c r="R83" s="10">
         <v>25</v>
       </c>
+      <c r="S83" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A84" s="27"/>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A84" s="24"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -11450,9 +11760,12 @@
       <c r="R84" s="10">
         <v>57</v>
       </c>
+      <c r="S84" s="10">
+        <v>60</v>
+      </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A85" s="27"/>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A85" s="24"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -11504,9 +11817,12 @@
       <c r="R85" s="10">
         <v>4</v>
       </c>
+      <c r="S85" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A86" s="28"/>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A86" s="25"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -11558,9 +11874,12 @@
       <c r="R86" s="10">
         <v>14</v>
       </c>
+      <c r="S86" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A87" s="23" t="s">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A87" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -11614,9 +11933,12 @@
       <c r="R87" s="10">
         <v>7</v>
       </c>
+      <c r="S87" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A88" s="24"/>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A88" s="27"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -11668,9 +11990,12 @@
       <c r="R88" s="10">
         <v>6</v>
       </c>
+      <c r="S88" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A89" s="24"/>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A89" s="27"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -11722,9 +12047,12 @@
       <c r="R89" s="10">
         <v>1</v>
       </c>
+      <c r="S89" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A90" s="24"/>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A90" s="27"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -11776,9 +12104,12 @@
       <c r="R90" s="10">
         <v>6</v>
       </c>
+      <c r="S90" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A91" s="24"/>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A91" s="27"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -11830,9 +12161,12 @@
       <c r="R91" s="10">
         <v>2</v>
       </c>
+      <c r="S91" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A92" s="24"/>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A92" s="27"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -11884,9 +12218,12 @@
       <c r="R92" s="10">
         <v>3</v>
       </c>
+      <c r="S92" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A93" s="25"/>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A93" s="28"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -11938,9 +12275,12 @@
       <c r="R93" s="10">
         <v>3</v>
       </c>
+      <c r="S93" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A94" s="26" t="s">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A94" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -11994,9 +12334,12 @@
       <c r="R94" s="10">
         <v>3</v>
       </c>
+      <c r="S94" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A95" s="28"/>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A95" s="25"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -12048,8 +12391,11 @@
       <c r="R95" s="10">
         <v>15</v>
       </c>
+      <c r="S95" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -12104,9 +12450,12 @@
       <c r="R96" s="10">
         <v>36</v>
       </c>
+      <c r="S96" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A97" s="26" t="s">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A97" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -12160,9 +12509,12 @@
       <c r="R97" s="10">
         <v>236</v>
       </c>
+      <c r="S97" s="10">
+        <v>263</v>
+      </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A98" s="27"/>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A98" s="24"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -12214,9 +12566,12 @@
       <c r="R98" s="10">
         <v>20</v>
       </c>
+      <c r="S98" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A99" s="28"/>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A99" s="25"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -12268,9 +12623,12 @@
       <c r="R99" s="10">
         <v>4</v>
       </c>
+      <c r="S99" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A100" s="23" t="s">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A100" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -12324,9 +12682,12 @@
       <c r="R100" s="10">
         <v>4</v>
       </c>
+      <c r="S100" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A101" s="24"/>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A101" s="27"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -12378,9 +12739,12 @@
       <c r="R101" s="10">
         <v>10</v>
       </c>
+      <c r="S101" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A102" s="24"/>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A102" s="27"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -12432,9 +12796,12 @@
       <c r="R102" s="10">
         <v>29</v>
       </c>
+      <c r="S102" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A103" s="24"/>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A103" s="27"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -12486,9 +12853,12 @@
       <c r="R103" s="10">
         <v>49</v>
       </c>
+      <c r="S103" s="10">
+        <v>48</v>
+      </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A104" s="25"/>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A104" s="28"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -12540,9 +12910,12 @@
       <c r="R104" s="10">
         <v>8</v>
       </c>
+      <c r="S104" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A105" s="26" t="s">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A105" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -12596,9 +12969,12 @@
       <c r="R105" s="10">
         <v>9</v>
       </c>
+      <c r="S105" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A106" s="27"/>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A106" s="24"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -12650,9 +13026,12 @@
       <c r="R106" s="10">
         <v>18</v>
       </c>
+      <c r="S106" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A107" s="27"/>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A107" s="24"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -12704,9 +13083,12 @@
       <c r="R107" s="10">
         <v>4</v>
       </c>
+      <c r="S107" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A108" s="27"/>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A108" s="24"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -12758,9 +13140,12 @@
       <c r="R108" s="10">
         <v>7</v>
       </c>
+      <c r="S108" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A109" s="28"/>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A109" s="25"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -12812,8 +13197,11 @@
       <c r="R109" s="10">
         <v>1</v>
       </c>
+      <c r="S109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -12868,8 +13256,11 @@
       <c r="R110" s="10">
         <v>110</v>
       </c>
+      <c r="S110" s="10">
+        <v>119</v>
+      </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -12924,9 +13315,12 @@
       <c r="R111" s="10">
         <v>12</v>
       </c>
+      <c r="S111" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A112" s="23" t="s">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A112" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -12980,9 +13374,12 @@
       <c r="R112" s="10">
         <v>1</v>
       </c>
+      <c r="S112" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A113" s="24"/>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A113" s="27"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -13034,9 +13431,12 @@
       <c r="R113" s="10">
         <v>2</v>
       </c>
+      <c r="S113" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A114" s="25"/>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A114" s="28"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -13088,9 +13488,12 @@
       <c r="R114" s="10">
         <v>12</v>
       </c>
+      <c r="S114" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A115" s="26" t="s">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A115" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -13144,9 +13547,12 @@
       <c r="R115" s="10">
         <v>38</v>
       </c>
+      <c r="S115" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A116" s="27"/>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A116" s="24"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -13198,9 +13604,12 @@
       <c r="R116" s="10">
         <v>9</v>
       </c>
+      <c r="S116" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A117" s="27"/>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A117" s="24"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -13252,9 +13661,12 @@
       <c r="R117" s="10">
         <v>4</v>
       </c>
+      <c r="S117" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A118" s="27"/>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A118" s="24"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -13306,9 +13718,12 @@
       <c r="R118" s="10">
         <v>14</v>
       </c>
+      <c r="S118" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A119" s="27"/>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A119" s="24"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -13360,9 +13775,12 @@
       <c r="R119" s="10">
         <v>2</v>
       </c>
+      <c r="S119" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A120" s="28"/>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A120" s="25"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -13414,9 +13832,12 @@
       <c r="R120" s="10">
         <v>23</v>
       </c>
+      <c r="S120" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A121" s="23" t="s">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A121" s="26" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -13470,9 +13891,12 @@
       <c r="R121" s="10">
         <v>0</v>
       </c>
+      <c r="S121" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A122" s="24"/>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A122" s="27"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -13524,9 +13948,12 @@
       <c r="R122" s="10">
         <v>15</v>
       </c>
+      <c r="S122" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A123" s="24"/>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A123" s="27"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -13578,9 +14005,12 @@
       <c r="R123" s="10">
         <v>1</v>
       </c>
+      <c r="S123" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A124" s="24"/>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A124" s="27"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -13632,9 +14062,12 @@
       <c r="R124" s="10">
         <v>2</v>
       </c>
+      <c r="S124" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A125" s="24"/>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A125" s="27"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -13686,9 +14119,12 @@
       <c r="R125" s="10">
         <v>1</v>
       </c>
+      <c r="S125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A126" s="24"/>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A126" s="27"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -13740,9 +14176,12 @@
       <c r="R126" s="10">
         <v>2</v>
       </c>
+      <c r="S126" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A127" s="24"/>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A127" s="27"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -13794,9 +14233,12 @@
       <c r="R127" s="10">
         <v>0</v>
       </c>
+      <c r="S127" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A128" s="24"/>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A128" s="27"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -13848,9 +14290,12 @@
       <c r="R128" s="10">
         <v>3</v>
       </c>
+      <c r="S128" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A129" s="24"/>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A129" s="27"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -13902,9 +14347,12 @@
       <c r="R129" s="10">
         <v>2</v>
       </c>
+      <c r="S129" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A130" s="25"/>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A130" s="28"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -13956,8 +14404,11 @@
       <c r="R130" s="10">
         <v>3</v>
       </c>
+      <c r="S130" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -14012,9 +14463,12 @@
       <c r="R131" s="10">
         <v>200</v>
       </c>
+      <c r="S131" s="10">
+        <v>207</v>
+      </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A132" s="23" t="s">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A132" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -14068,9 +14522,12 @@
       <c r="R132" s="10">
         <v>11</v>
       </c>
+      <c r="S132" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A133" s="24"/>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A133" s="27"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -14122,9 +14579,12 @@
       <c r="R133" s="10">
         <v>4</v>
       </c>
+      <c r="S133" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A134" s="24"/>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A134" s="27"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -14176,9 +14636,12 @@
       <c r="R134" s="10">
         <v>0</v>
       </c>
+      <c r="S134" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A135" s="25"/>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A135" s="28"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -14230,9 +14693,12 @@
       <c r="R135" s="10">
         <v>0</v>
       </c>
+      <c r="S135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A136" s="26" t="s">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A136" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -14286,9 +14752,12 @@
       <c r="R136" s="10">
         <v>23</v>
       </c>
+      <c r="S136" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A137" s="27"/>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A137" s="24"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -14340,9 +14809,12 @@
       <c r="R137" s="10">
         <v>5</v>
       </c>
+      <c r="S137" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A138" s="27"/>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A138" s="24"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -14394,9 +14866,12 @@
       <c r="R138" s="10">
         <v>4</v>
       </c>
+      <c r="S138" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A139" s="28"/>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A139" s="25"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -14447,10 +14922,25 @@
       </c>
       <c r="R139" s="10">
         <v>30</v>
+      </c>
+      <c r="S139" s="10">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -14463,18 +14953,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -14582,7 +15060,7 @@
     </row>
     <row r="2" spans="1:81" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" s="19">
         <f t="shared" ref="B2:AG2" si="0">(B7/MAX(B6,1))*100</f>
@@ -14686,7 +15164,7 @@
       </c>
       <c r="AA2" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>49.782608695652172</v>
       </c>
       <c r="AB2" s="19">
         <f t="shared" si="0"/>
@@ -14907,7 +15385,7 @@
     </row>
     <row r="3" spans="1:81" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" s="22">
         <f t="shared" ref="B3:AG3" si="3">(B8/MAX(1,B7))*100</f>
@@ -15232,7 +15710,7 @@
     </row>
     <row r="4" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B4" s="10">
         <f t="shared" ref="B4:AG4" si="6">(B9/MAX(1,B7))*100</f>
@@ -15336,7 +15814,7 @@
       </c>
       <c r="AA4" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.1834061135371177</v>
       </c>
       <c r="AB4" s="10">
         <f t="shared" si="6"/>
@@ -15661,7 +16139,7 @@
       </c>
       <c r="AA6" s="12">
         <f>MAX(0, (dc!AA3-dc!Z3))</f>
-        <v>0</v>
+        <v>460</v>
       </c>
       <c r="AB6" s="12">
         <f>MAX(0, (dc!AB3-dc!AA3))</f>
@@ -15882,7 +16360,7 @@
     </row>
     <row r="7" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7" s="12">
         <v>0</v>
@@ -15985,7 +16463,7 @@
       </c>
       <c r="AA7" s="12">
         <f>MAX(0, (dc!AA4-dc!Z4))</f>
-        <v>0</v>
+        <v>229</v>
       </c>
       <c r="AB7" s="12">
         <f>MAX(0, (dc!AB4-dc!AA4))</f>
@@ -16633,7 +17111,7 @@
       </c>
       <c r="AA9" s="12">
         <f>MAX(0, (dc!AA6-dc!Z6))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB9" s="12">
         <f>MAX(0, (dc!AB6-dc!AA6))</f>
@@ -17351,7 +17829,7 @@
   <dimension ref="A1:BQ70"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AB70" sqref="AB70"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17371,7 +17849,7 @@
     </row>
     <row r="2" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" s="21">
         <f>(C7/MAX(C6,1))*100</f>
@@ -17418,11 +17896,11 @@
       </c>
       <c r="O2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.218905472636816</v>
       </c>
       <c r="P2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.942209217264082</v>
       </c>
       <c r="Q2" s="21">
         <f t="shared" si="0"/>
@@ -17639,7 +18117,7 @@
     </row>
     <row r="3" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="21">
         <f t="shared" ref="C3:AH3" si="2">(C8/MAX(1,C7))*100</f>
@@ -17691,11 +18169,11 @@
       </c>
       <c r="O3" s="21">
         <f t="shared" si="2"/>
-        <v>4700</v>
+        <v>14.417177914110429</v>
       </c>
       <c r="P3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.9810017271157179</v>
       </c>
       <c r="Q3" s="21">
         <f t="shared" si="2"/>
@@ -17912,7 +18390,7 @@
     </row>
     <row r="4" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C4" s="21">
         <f t="shared" ref="C4:AH4" si="4">(C9/MAX(1,C7))*100</f>
@@ -17964,11 +18442,11 @@
       </c>
       <c r="O4" s="21">
         <f t="shared" si="4"/>
-        <v>1200</v>
+        <v>3.6809815950920246</v>
       </c>
       <c r="P4" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.8134715025906734</v>
       </c>
       <c r="Q4" s="21">
         <f t="shared" si="4"/>
@@ -18300,11 +18778,11 @@
       </c>
       <c r="O6" s="14">
         <f>MAX(0,(md!O2-md!N2)+(md!O3-md!N3))</f>
-        <v>991</v>
+        <v>2010</v>
       </c>
       <c r="P6" s="14">
         <f>MAX(0,(md!P2-md!O2)+(md!P3-md!O3))</f>
-        <v>0</v>
+        <v>6835</v>
       </c>
       <c r="Q6" s="14">
         <f>MAX(0,(md!Q2-md!P2)+(md!Q3-md!P3))</f>
@@ -18521,7 +18999,7 @@
     </row>
     <row r="7" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="14">
         <v>0</v>
@@ -18572,11 +19050,11 @@
       </c>
       <c r="O7" s="14">
         <f>MAX(0,(md!O3-md!N3))</f>
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="P7" s="14">
         <f>MAX(0,(md!P3-md!O3))</f>
-        <v>0</v>
+        <v>1158</v>
       </c>
       <c r="Q7" s="14">
         <f>MAX(0,(md!Q3-md!P3))</f>
@@ -18848,7 +19326,7 @@
       </c>
       <c r="P8" s="14">
         <f>MAX(0,(md!P4-md!O4))</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="Q8" s="14">
         <f>MAX(0,(md!Q4-md!P4))</f>
@@ -19120,7 +19598,7 @@
       </c>
       <c r="P9" s="14">
         <f>MAX(0,(md!P5-md!O5))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="Q9" s="14">
         <f>MAX(0,(md!Q5-md!P5))</f>
@@ -19546,11 +20024,12 @@
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Calvert</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>267</v>
+        <f>md!A7</f>
+        <v>Allegany</v>
+      </c>
+      <c r="B11" s="1">
+        <f>md!B7</f>
+        <v>24001</v>
       </c>
       <c r="C11" s="14">
         <v>0</v>
@@ -19822,10 +20301,11 @@
     </row>
     <row r="12" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Caroline</v>
+        <f>md!A8</f>
+        <v>Anne Arundel</v>
       </c>
       <c r="B12" s="1">
+        <f>md!B8</f>
         <v>24003</v>
       </c>
       <c r="C12" s="14">
@@ -19881,7 +20361,7 @@
       </c>
       <c r="P12" s="14">
         <f>MAX(0,(md!P9-md!O9))</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="Q12" s="14">
         <f>MAX(0,(md!Q9-md!P9))</f>
@@ -20098,10 +20578,11 @@
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Carroll</v>
+        <f>md!A9</f>
+        <v>Baltimore City</v>
       </c>
       <c r="B13" s="1">
+        <f>md!B9</f>
         <v>24510</v>
       </c>
       <c r="C13" s="14">
@@ -20157,7 +20638,7 @@
       </c>
       <c r="P13" s="14">
         <f>MAX(0,(md!P9-md!O9))</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="Q13" s="14">
         <f>MAX(0,(md!Q9-md!P9))</f>
@@ -20374,10 +20855,11 @@
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Cecil</v>
+        <f>md!A10</f>
+        <v>Baltimore County</v>
       </c>
       <c r="B14" s="1">
+        <f>md!B10</f>
         <v>24005</v>
       </c>
       <c r="C14" s="14">
@@ -20433,7 +20915,7 @@
       </c>
       <c r="P14" s="14">
         <f>MAX(0,(md!P10-md!O10))</f>
-        <v>0</v>
+        <v>214</v>
       </c>
       <c r="Q14" s="14">
         <f>MAX(0,(md!Q10-md!P10))</f>
@@ -20650,10 +21132,11 @@
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Charles</v>
+        <f>md!A11</f>
+        <v>Calvert</v>
       </c>
       <c r="B15" s="1">
+        <f>md!B11</f>
         <v>24009</v>
       </c>
       <c r="C15" s="14">
@@ -20709,7 +21192,7 @@
       </c>
       <c r="P15" s="14">
         <f>MAX(0,(md!P11-md!O11))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q15" s="14">
         <f>MAX(0,(md!Q11-md!P11))</f>
@@ -20926,10 +21409,11 @@
     </row>
     <row r="16" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Dorchester</v>
+        <f>md!A12</f>
+        <v>Caroline</v>
       </c>
       <c r="B16" s="1">
+        <f>md!B12</f>
         <v>24011</v>
       </c>
       <c r="C16" s="14">
@@ -21202,10 +21686,11 @@
     </row>
     <row r="17" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Frederick</v>
+        <f>md!A13</f>
+        <v>Carroll</v>
       </c>
       <c r="B17" s="1">
+        <f>md!B13</f>
         <v>24013</v>
       </c>
       <c r="C17" s="14">
@@ -21261,7 +21746,7 @@
       </c>
       <c r="P17" s="14">
         <f>MAX(0,(md!P13-md!O13))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q17" s="14">
         <f>MAX(0,(md!Q13-md!P13))</f>
@@ -21478,10 +21963,11 @@
     </row>
     <row r="18" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Garrett</v>
+        <f>md!A14</f>
+        <v>Cecil</v>
       </c>
       <c r="B18" s="1">
+        <f>md!B14</f>
         <v>24015</v>
       </c>
       <c r="C18" s="14">
@@ -21537,7 +22023,7 @@
       </c>
       <c r="P18" s="14">
         <f>MAX(0,(md!P14-md!O14))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q18" s="14">
         <f>MAX(0,(md!Q14-md!P14))</f>
@@ -21754,10 +22240,11 @@
     </row>
     <row r="19" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Harford</v>
+        <f>md!A15</f>
+        <v>Charles</v>
       </c>
       <c r="B19" s="1">
+        <f>md!B15</f>
         <v>24017</v>
       </c>
       <c r="C19" s="14">
@@ -21813,7 +22300,7 @@
       </c>
       <c r="P19" s="14">
         <f>MAX(0,(md!P15-md!O15))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="Q19" s="14">
         <f>MAX(0,(md!Q15-md!P15))</f>
@@ -22030,10 +22517,11 @@
     </row>
     <row r="20" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Howard</v>
+        <f>md!A16</f>
+        <v>Dorchester</v>
       </c>
       <c r="B20" s="1">
+        <f>md!B16</f>
         <v>24019</v>
       </c>
       <c r="C20" s="14">
@@ -22089,7 +22577,7 @@
       </c>
       <c r="P20" s="14">
         <f>MAX(0,(md!P16-md!O16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="14">
         <f>MAX(0,(md!Q16-md!P16))</f>
@@ -22306,10 +22794,11 @@
     </row>
     <row r="21" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Kent</v>
+        <f>md!A17</f>
+        <v>Frederick</v>
       </c>
       <c r="B21" s="1">
+        <f>md!B17</f>
         <v>24021</v>
       </c>
       <c r="C21" s="14">
@@ -22365,7 +22854,7 @@
       </c>
       <c r="P21" s="14">
         <f>MAX(0,(md!P17-md!O17))</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="Q21" s="14">
         <f>MAX(0,(md!Q17-md!P17))</f>
@@ -22582,10 +23071,11 @@
     </row>
     <row r="22" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Montgomery</v>
+        <f>md!A18</f>
+        <v>Garrett</v>
       </c>
       <c r="B22" s="1">
+        <f>md!B18</f>
         <v>24023</v>
       </c>
       <c r="C22" s="14">
@@ -22641,7 +23131,7 @@
       </c>
       <c r="P22" s="14">
         <f>MAX(0,(md!P18-md!O18))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="14">
         <f>MAX(0,(md!Q18-md!P18))</f>
@@ -22858,10 +23348,11 @@
     </row>
     <row r="23" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Prince George's</v>
+        <f>md!A19</f>
+        <v>Harford</v>
       </c>
       <c r="B23" s="1">
+        <f>md!B19</f>
         <v>24025</v>
       </c>
       <c r="C23" s="14">
@@ -22917,7 +23408,7 @@
       </c>
       <c r="P23" s="14">
         <f>MAX(0,(md!P19-md!O19))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q23" s="14">
         <f>MAX(0,(md!Q19-md!P19))</f>
@@ -23134,10 +23625,11 @@
     </row>
     <row r="24" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Queen Anne's</v>
+        <f>md!A20</f>
+        <v>Howard</v>
       </c>
       <c r="B24" s="1">
+        <f>md!B20</f>
         <v>24027</v>
       </c>
       <c r="C24" s="14">
@@ -23193,7 +23685,7 @@
       </c>
       <c r="P24" s="14">
         <f>MAX(0,(md!P20-md!O20))</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="Q24" s="14">
         <f>MAX(0,(md!Q20-md!P20))</f>
@@ -23410,10 +23902,11 @@
     </row>
     <row r="25" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>St. Mary's</v>
+        <f>md!A21</f>
+        <v>Kent</v>
       </c>
       <c r="B25" s="1">
+        <f>md!B21</f>
         <v>24029</v>
       </c>
       <c r="C25" s="14">
@@ -23469,7 +23962,7 @@
       </c>
       <c r="P25" s="14">
         <f>MAX(0,(md!P21-md!O21))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="14">
         <f>MAX(0,(md!Q21-md!P21))</f>
@@ -23686,10 +24179,11 @@
     </row>
     <row r="26" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Somerset</v>
+        <f>md!A22</f>
+        <v>Montgomery</v>
       </c>
       <c r="B26" s="1">
+        <f>md!B22</f>
         <v>24031</v>
       </c>
       <c r="C26" s="14">
@@ -23745,7 +24239,7 @@
       </c>
       <c r="P26" s="14">
         <f>MAX(0,(md!P22-md!O22))</f>
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="Q26" s="14">
         <f>MAX(0,(md!Q22-md!P22))</f>
@@ -23962,10 +24456,11 @@
     </row>
     <row r="27" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Talbot</v>
+        <f>md!A23</f>
+        <v>Prince George's</v>
       </c>
       <c r="B27" s="1">
+        <f>md!B23</f>
         <v>24033</v>
       </c>
       <c r="C27" s="14">
@@ -24017,11 +24512,11 @@
       </c>
       <c r="O27" s="14">
         <f>MAX(0,(md!O23-md!N23))</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="P27" s="14">
         <f>MAX(0,(md!P23-md!O23))</f>
-        <v>0</v>
+        <v>290</v>
       </c>
       <c r="Q27" s="14">
         <f>MAX(0,(md!Q23-md!P23))</f>
@@ -24238,10 +24733,11 @@
     </row>
     <row r="28" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Washington</v>
+        <f>md!A24</f>
+        <v>Queen Anne's</v>
       </c>
       <c r="B28" s="1">
+        <f>md!B24</f>
         <v>24035</v>
       </c>
       <c r="C28" s="14">
@@ -24297,7 +24793,7 @@
       </c>
       <c r="P28" s="14">
         <f>MAX(0,(md!P24-md!O24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="14">
         <f>MAX(0,(md!Q24-md!P24))</f>
@@ -24514,10 +25010,11 @@
     </row>
     <row r="29" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Wicomico</v>
+        <f>md!A25</f>
+        <v>St. Mary's</v>
       </c>
       <c r="B29" s="1">
+        <f>md!B25</f>
         <v>24039</v>
       </c>
       <c r="C29" s="14">
@@ -24573,7 +25070,7 @@
       </c>
       <c r="P29" s="14">
         <f>MAX(0,(md!P25-md!O25))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q29" s="14">
         <f>MAX(0,(md!Q25-md!P25))</f>
@@ -24790,10 +25287,11 @@
     </row>
     <row r="30" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>Worcester</v>
+        <f>md!A26</f>
+        <v>Somerset</v>
       </c>
       <c r="B30" s="1">
+        <f>md!B26</f>
         <v>24037</v>
       </c>
       <c r="C30" s="14">
@@ -25066,10 +25564,11 @@
     </row>
     <row r="31" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v/>
+        <f>md!A27</f>
+        <v>Talbot</v>
       </c>
       <c r="B31" s="1">
+        <f>md!B27</f>
         <v>24041</v>
       </c>
       <c r="C31" s="14">
@@ -25125,7 +25624,7 @@
       </c>
       <c r="P31" s="14">
         <f>MAX(0,(md!P27-md!O27))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q31" s="14">
         <f>MAX(0,(md!Q27-md!P27))</f>
@@ -25342,10 +25841,11 @@
     </row>
     <row r="32" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="str">
-        <f>T(md[[#This Row],[county]])</f>
-        <v/>
+        <f>md!A28</f>
+        <v>Washington</v>
       </c>
       <c r="B32" s="1">
+        <f>md!B28</f>
         <v>24043</v>
       </c>
       <c r="C32" s="14">
@@ -25401,7 +25901,7 @@
       </c>
       <c r="P32" s="14">
         <f>MAX(0,(md!P28-md!O28))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="Q32" s="14">
         <f>MAX(0,(md!Q28-md!P28))</f>
@@ -25617,11 +26117,12 @@
       </c>
     </row>
     <row r="33" spans="1:69" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="e">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>#VALUE!</v>
+      <c r="A33" s="1" t="str">
+        <f>md!A29</f>
+        <v>Wicomico</v>
       </c>
       <c r="B33" s="1">
+        <f>md!B29</f>
         <v>24045</v>
       </c>
       <c r="C33" s="14">
@@ -25677,7 +26178,7 @@
       </c>
       <c r="P33" s="14">
         <f>MAX(0,(md!P29-md!O29))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q33" s="14">
         <f>MAX(0,(md!Q29-md!P29))</f>
@@ -25893,11 +26394,12 @@
       </c>
     </row>
     <row r="34" spans="1:69" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="e">
-        <f>T(md[[#This Row],[county]])</f>
-        <v>#VALUE!</v>
+      <c r="A34" s="1" t="str">
+        <f>md!A30</f>
+        <v>Worcester</v>
       </c>
       <c r="B34" s="1">
+        <f>md!B30</f>
         <v>24047</v>
       </c>
       <c r="C34" s="14">
@@ -26247,6 +26749,7 @@
       <c r="D70" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C11:BQ34">
     <cfRule type="colorScale" priority="9">
       <colorScale>
@@ -26368,7 +26871,7 @@
     </row>
     <row r="2" spans="1:71" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D2" s="20">
         <f t="shared" ref="D2:AI2" si="0">(D7/(MAX(D6,1))*100)</f>
@@ -26428,7 +26931,7 @@
       </c>
       <c r="R2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15.6</v>
       </c>
       <c r="S2" s="20">
         <f t="shared" si="0"/>
@@ -26645,7 +27148,7 @@
     </row>
     <row r="3" spans="1:71" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D3" s="20">
         <f t="shared" ref="D3:AI3" si="2">(D8/MAX(1,D7))*100</f>
@@ -26705,7 +27208,7 @@
       </c>
       <c r="R3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="S3" s="20">
         <f t="shared" si="2"/>
@@ -26922,7 +27425,7 @@
     </row>
     <row r="4" spans="1:71" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="20">
         <f t="shared" ref="D4:AI4" si="4">(D9/MAX(1,D7))*100</f>
@@ -26982,7 +27485,7 @@
       </c>
       <c r="R4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.8461538461538463</v>
       </c>
       <c r="S4" s="20">
         <f t="shared" si="4"/>
@@ -27259,7 +27762,7 @@
       </c>
       <c r="R6" s="14">
         <f>MAX(0,(va!S5-va!R5))</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="S6" s="14">
         <f>MAX(0,(va!T5-va!S5))</f>
@@ -27476,7 +27979,7 @@
     </row>
     <row r="7" spans="1:71" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D7" s="14">
         <f>SUM(delta_va[25-Mar])</f>
@@ -27536,7 +28039,7 @@
       </c>
       <c r="R7" s="14">
         <f>MAX(0,(va!S2-va!R2))</f>
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="S7" s="14">
         <f>MAX(0,(va!T2-va!S2))</f>
@@ -27813,7 +28316,7 @@
       </c>
       <c r="R8" s="14">
         <f>MAX(0,(va!S3-va!R3))</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="S8" s="14">
         <f>MAX(0,(va!T3-va!S3))</f>
@@ -28090,7 +28593,7 @@
       </c>
       <c r="R9" s="14">
         <f>MAX(0,(va!S4-va!R4))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="S9" s="14">
         <f>MAX(0,(va!T4-va!S4))</f>
@@ -28587,7 +29090,7 @@
       </c>
       <c r="R11" s="16">
         <f>MAX(0,(va!S7-va!R7))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="S11" s="16">
         <f>MAX(0,(va!T7-va!S7))</f>
@@ -29715,7 +30218,7 @@
       </c>
       <c r="R15" s="16">
         <f>MAX(0,(va!S11-va!R11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" s="16">
         <f>MAX(0,(va!T11-va!S11))</f>
@@ -30561,7 +31064,7 @@
       </c>
       <c r="R18" s="16">
         <f>MAX(0,(va!S14-va!R14))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="S18" s="16">
         <f>MAX(0,(va!T14-va!S14))</f>
@@ -30843,7 +31346,7 @@
       </c>
       <c r="R19" s="16">
         <f>MAX(0,(va!S15-va!R15))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S19" s="16">
         <f>MAX(0,(va!T15-va!S15))</f>
@@ -31971,7 +32474,7 @@
       </c>
       <c r="R23" s="16">
         <f>MAX(0,(va!S19-va!R19))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S23" s="16">
         <f>MAX(0,(va!T19-va!S19))</f>
@@ -32535,7 +33038,7 @@
       </c>
       <c r="R25" s="16">
         <f>MAX(0,(va!S21-va!R21))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S25" s="16">
         <f>MAX(0,(va!T21-va!S21))</f>
@@ -34227,7 +34730,7 @@
       </c>
       <c r="R31" s="16">
         <f>MAX(0,(va!S27-va!R27))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S31" s="16">
         <f>MAX(0,(va!T27-va!S27))</f>
@@ -34509,7 +35012,7 @@
       </c>
       <c r="R32" s="16">
         <f>MAX(0,(va!S28-va!R28))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S32" s="16">
         <f>MAX(0,(va!T28-va!S28))</f>
@@ -35073,7 +35576,7 @@
       </c>
       <c r="R34" s="16">
         <f>MAX(0,(va!S30-va!R30))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="S34" s="16">
         <f>MAX(0,(va!T30-va!S30))</f>
@@ -35355,7 +35858,7 @@
       </c>
       <c r="R35" s="16">
         <f>MAX(0,(va!S31-va!R31))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="S35" s="16">
         <f>MAX(0,(va!T31-va!S31))</f>
@@ -35919,7 +36422,7 @@
       </c>
       <c r="R37" s="16">
         <f>MAX(0,(va!S33-va!R33))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S37" s="16">
         <f>MAX(0,(va!T33-va!S33))</f>
@@ -36201,7 +36704,7 @@
       </c>
       <c r="R38" s="16">
         <f>MAX(0,(va!S34-va!R34))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S38" s="16">
         <f>MAX(0,(va!T34-va!S34))</f>
@@ -36483,7 +36986,7 @@
       </c>
       <c r="R39" s="16">
         <f>MAX(0,(va!S35-va!R35))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S39" s="16">
         <f>MAX(0,(va!T35-va!S35))</f>
@@ -36765,7 +37268,7 @@
       </c>
       <c r="R40" s="16">
         <f>MAX(0,(va!S36-va!R36))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S40" s="16">
         <f>MAX(0,(va!T36-va!S36))</f>
@@ -37329,7 +37832,7 @@
       </c>
       <c r="R42" s="16">
         <f>MAX(0,(va!S38-va!R38))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S42" s="16">
         <f>MAX(0,(va!T38-va!S38))</f>
@@ -37893,7 +38396,7 @@
       </c>
       <c r="R44" s="16">
         <f>MAX(0,(va!S40-va!R40))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S44" s="16">
         <f>MAX(0,(va!T40-va!S40))</f>
@@ -38457,7 +38960,7 @@
       </c>
       <c r="R46" s="16">
         <f>MAX(0,(va!S42-va!R42))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S46" s="16">
         <f>MAX(0,(va!T42-va!S42))</f>
@@ -38739,7 +39242,7 @@
       </c>
       <c r="R47" s="16">
         <f>MAX(0,(va!S43-va!R43))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S47" s="16">
         <f>MAX(0,(va!T43-va!S43))</f>
@@ -41277,7 +41780,7 @@
       </c>
       <c r="R56" s="16">
         <f>MAX(0,(va!S52-va!R52))</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="S56" s="16">
         <f>MAX(0,(va!T52-va!S52))</f>
@@ -42123,7 +42626,7 @@
       </c>
       <c r="R59" s="16">
         <f>MAX(0,(va!S55-va!R55))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S59" s="16">
         <f>MAX(0,(va!T55-va!S55))</f>
@@ -42405,7 +42908,7 @@
       </c>
       <c r="R60" s="16">
         <f>MAX(0,(va!S56-va!R56))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="S60" s="16">
         <f>MAX(0,(va!T56-va!S56))</f>
@@ -42687,7 +43190,7 @@
       </c>
       <c r="R61" s="16">
         <f>MAX(0,(va!S57-va!R57))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S61" s="16">
         <f>MAX(0,(va!T57-va!S57))</f>
@@ -43251,7 +43754,7 @@
       </c>
       <c r="R63" s="16">
         <f>MAX(0,(va!S59-va!R59))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S63" s="16">
         <f>MAX(0,(va!T59-va!S59))</f>
@@ -43815,7 +44318,7 @@
       </c>
       <c r="R65" s="16">
         <f>MAX(0,(va!S61-va!R61))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S65" s="16">
         <f>MAX(0,(va!T61-va!S61))</f>
@@ -44097,7 +44600,7 @@
       </c>
       <c r="R66" s="16">
         <f>MAX(0,(va!S62-va!R62))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S66" s="16">
         <f>MAX(0,(va!T62-va!S62))</f>
@@ -44661,7 +45164,7 @@
       </c>
       <c r="R68" s="16">
         <f>MAX(0,(va!S64-va!R64))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S68" s="16">
         <f>MAX(0,(va!T64-va!S64))</f>
@@ -44943,7 +45446,7 @@
       </c>
       <c r="R69" s="16">
         <f>MAX(0,(va!S65-va!R65))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S69" s="16">
         <f>MAX(0,(va!T65-va!S65))</f>
@@ -45225,7 +45728,7 @@
       </c>
       <c r="R70" s="16">
         <f>MAX(0,(va!S66-va!R66))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S70" s="16">
         <f>MAX(0,(va!T66-va!S66))</f>
@@ -45507,7 +46010,7 @@
       </c>
       <c r="R71" s="16">
         <f>MAX(0,(va!S67-va!R67))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="S71" s="16">
         <f>MAX(0,(va!T67-va!S67))</f>
@@ -46635,7 +47138,7 @@
       </c>
       <c r="R75" s="16">
         <f>MAX(0,(va!S71-va!R71))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S75" s="16">
         <f>MAX(0,(va!T71-va!S71))</f>
@@ -46917,7 +47420,7 @@
       </c>
       <c r="R76" s="16">
         <f>MAX(0,(va!S72-va!R72))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S76" s="16">
         <f>MAX(0,(va!T72-va!S72))</f>
@@ -47199,7 +47702,7 @@
       </c>
       <c r="R77" s="16">
         <f>MAX(0,(va!S73-va!R73))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S77" s="16">
         <f>MAX(0,(va!T73-va!S73))</f>
@@ -49455,7 +49958,7 @@
       </c>
       <c r="R85" s="16">
         <f>MAX(0,(va!S81-va!R81))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S85" s="16">
         <f>MAX(0,(va!T81-va!S81))</f>
@@ -49737,7 +50240,7 @@
       </c>
       <c r="R86" s="16">
         <f>MAX(0,(va!S82-va!R82))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S86" s="16">
         <f>MAX(0,(va!T82-va!S82))</f>
@@ -50301,7 +50804,7 @@
       </c>
       <c r="R88" s="16">
         <f>MAX(0,(va!S84-va!R84))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S88" s="16">
         <f>MAX(0,(va!T84-va!S84))</f>
@@ -50865,7 +51368,7 @@
       </c>
       <c r="R90" s="16">
         <f>MAX(0,(va!S86-va!R86))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S90" s="16">
         <f>MAX(0,(va!T86-va!S86))</f>
@@ -51147,7 +51650,7 @@
       </c>
       <c r="R91" s="16">
         <f>MAX(0,(va!S87-va!R87))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S91" s="16">
         <f>MAX(0,(va!T87-va!S87))</f>
@@ -51429,7 +51932,7 @@
       </c>
       <c r="R92" s="16">
         <f>MAX(0,(va!S88-va!R88))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S92" s="16">
         <f>MAX(0,(va!T88-va!S88))</f>
@@ -53685,7 +54188,7 @@
       </c>
       <c r="R100" s="16">
         <f>MAX(0,(va!S96-va!R96))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S100" s="16">
         <f>MAX(0,(va!T96-va!S96))</f>
@@ -53967,7 +54470,7 @@
       </c>
       <c r="R101" s="16">
         <f>MAX(0,(va!S97-va!R97))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S101" s="16">
         <f>MAX(0,(va!T97-va!S97))</f>
@@ -54531,7 +55034,7 @@
       </c>
       <c r="R103" s="16">
         <f>MAX(0,(va!S99-va!R99))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S103" s="16">
         <f>MAX(0,(va!T99-va!S99))</f>
@@ -55095,7 +55598,7 @@
       </c>
       <c r="R105" s="16">
         <f>MAX(0,(va!S101-va!R101))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S105" s="16">
         <f>MAX(0,(va!T101-va!S101))</f>
@@ -55377,7 +55880,7 @@
       </c>
       <c r="R106" s="16">
         <f>MAX(0,(va!S102-va!R102))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S106" s="16">
         <f>MAX(0,(va!T102-va!S102))</f>
@@ -56223,7 +56726,7 @@
       </c>
       <c r="R109" s="16">
         <f>MAX(0,(va!S105-va!R105))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S109" s="16">
         <f>MAX(0,(va!T105-va!S105))</f>
@@ -56787,7 +57290,7 @@
       </c>
       <c r="R111" s="16">
         <f>MAX(0,(va!S107-va!R107))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S111" s="16">
         <f>MAX(0,(va!T107-va!S107))</f>
@@ -57633,7 +58136,7 @@
       </c>
       <c r="R114" s="16">
         <f>MAX(0,(va!S110-va!R110))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S114" s="16">
         <f>MAX(0,(va!T110-va!S110))</f>
@@ -57915,7 +58418,7 @@
       </c>
       <c r="R115" s="16">
         <f>MAX(0,(va!S111-va!R111))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S115" s="16">
         <f>MAX(0,(va!T111-va!S111))</f>
@@ -58761,7 +59264,7 @@
       </c>
       <c r="R118" s="16">
         <f>MAX(0,(va!S114-va!R114))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S118" s="16">
         <f>MAX(0,(va!T114-va!S114))</f>
@@ -59043,7 +59546,7 @@
       </c>
       <c r="R119" s="16">
         <f>MAX(0,(va!S115-va!R115))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S119" s="16">
         <f>MAX(0,(va!T115-va!S115))</f>
@@ -59325,7 +59828,7 @@
       </c>
       <c r="R120" s="16">
         <f>MAX(0,(va!S116-va!R116))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S120" s="16">
         <f>MAX(0,(va!T116-va!S116))</f>
@@ -59889,7 +60392,7 @@
       </c>
       <c r="R122" s="16">
         <f>MAX(0,(va!S118-va!R118))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S122" s="16">
         <f>MAX(0,(va!T118-va!S118))</f>
@@ -60171,7 +60674,7 @@
       </c>
       <c r="R123" s="16">
         <f>MAX(0,(va!S119-va!R119))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S123" s="16">
         <f>MAX(0,(va!T119-va!S119))</f>
@@ -61017,7 +61520,7 @@
       </c>
       <c r="R126" s="16">
         <f>MAX(0,(va!S122-va!R122))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S126" s="16">
         <f>MAX(0,(va!T122-va!S122))</f>
@@ -63273,7 +63776,7 @@
       </c>
       <c r="R134" s="16">
         <f>MAX(0,(va!S130-va!R130))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S134" s="16">
         <f>MAX(0,(va!T130-va!S130))</f>
@@ -63555,7 +64058,7 @@
       </c>
       <c r="R135" s="16">
         <f>MAX(0,(va!S131-va!R131))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S135" s="16">
         <f>MAX(0,(va!T131-va!S131))</f>
@@ -63837,7 +64340,7 @@
       </c>
       <c r="R136" s="16">
         <f>MAX(0,(va!S132-va!R132))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S136" s="16">
         <f>MAX(0,(va!T132-va!S132))</f>
@@ -65529,7 +66032,7 @@
       </c>
       <c r="R142" s="16">
         <f>MAX(0,(va!S138-va!R138))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S142" s="16">
         <f>MAX(0,(va!T138-va!S138))</f>
@@ -65811,7 +66314,7 @@
       </c>
       <c r="R143" s="16">
         <f>MAX(0,(va!S139-va!R139))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S143" s="16">
         <f>MAX(0,(va!T139-va!S139))</f>

</xml_diff>

<commit_message>
12 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FCAC77-21A3-469E-9642-D2D624FD1CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B47491-BFBD-42AA-ACBF-185CA19C1E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="27580" windowHeight="18000" tabRatio="685" activeTab="3" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="6780" yWindow="4980" windowWidth="20520" windowHeight="13130" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1060,6 +1060,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1069,24 +1078,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="190">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1908,6 +1906,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3105,7 +3106,7 @@
     <tableColumn id="70" xr3:uid="{BF0F6EA4-D03C-4B39-B744-A10BFAA808B6}" name="29-Mar"/>
     <tableColumn id="71" xr3:uid="{6EB11E5A-C3AA-4AD8-8662-DC535BE6403E}" name="30-Mar"/>
     <tableColumn id="72" xr3:uid="{59784BA3-1B79-4BA6-9B04-532097E0A8B9}" name="31-Mar"/>
-    <tableColumn id="73" xr3:uid="{80588F27-312F-4CA9-8F43-744439C924D9}" name="1-Apr" dataDxfId="0">
+    <tableColumn id="73" xr3:uid="{80588F27-312F-4CA9-8F43-744439C924D9}" name="1-Apr" dataDxfId="139">
       <calculatedColumnFormula>MAX(0,(dc!U7-dc!T7))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="74" xr3:uid="{84813A08-755C-4060-8A53-4CAD927C68AF}" name="2-Apr">
@@ -3296,209 +3297,209 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3416EC88-0BC4-4758-A58D-187F9B999FB7}" name="delta_md" displayName="delta_md" ref="A10:BQ34" totalsRowShown="0">
   <tableColumns count="69">
-    <tableColumn id="1" xr3:uid="{BFB3F1B0-DE0E-4A75-8475-0AD52DEC3890}" name="county" dataDxfId="139">
+    <tableColumn id="1" xr3:uid="{BFB3F1B0-DE0E-4A75-8475-0AD52DEC3890}" name="county" dataDxfId="138">
       <calculatedColumnFormula>md!A7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F9092969-4B66-4A12-8600-89F79D327DA5}" name="FIPS" dataDxfId="138">
+    <tableColumn id="2" xr3:uid="{F9092969-4B66-4A12-8600-89F79D327DA5}" name="FIPS" dataDxfId="137">
       <calculatedColumnFormula>md!B7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{C1AF955F-BEA7-4320-9557-BB3EAECC72AE}" name="26-Mar" dataDxfId="137"/>
-    <tableColumn id="68" xr3:uid="{C7FF752A-8DC4-46FC-AF76-F1FF335EB014}" name="27-Mar" dataDxfId="136">
+    <tableColumn id="67" xr3:uid="{C1AF955F-BEA7-4320-9557-BB3EAECC72AE}" name="26-Mar" dataDxfId="136"/>
+    <tableColumn id="68" xr3:uid="{C7FF752A-8DC4-46FC-AF76-F1FF335EB014}" name="27-Mar" dataDxfId="135">
       <calculatedColumnFormula>MAX(0,(md!D7-md!C7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="69" xr3:uid="{CF1FAAB0-7ED6-4840-A066-0E55CBEAF2B0}" name="28-Mar" dataDxfId="135">
+    <tableColumn id="69" xr3:uid="{CF1FAAB0-7ED6-4840-A066-0E55CBEAF2B0}" name="28-Mar" dataDxfId="134">
       <calculatedColumnFormula>MAX(0,(md!E7-md!D7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="70" xr3:uid="{C6B48FE5-0D82-4E66-879E-AD88448A92B0}" name="29-Mar" dataDxfId="134">
+    <tableColumn id="70" xr3:uid="{C6B48FE5-0D82-4E66-879E-AD88448A92B0}" name="29-Mar" dataDxfId="133">
       <calculatedColumnFormula>MAX(0,(md!F7-md!E7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="71" xr3:uid="{2FBAB02E-F400-450D-9DCA-14210AE3DFAC}" name="30-Mar" dataDxfId="133">
+    <tableColumn id="71" xr3:uid="{2FBAB02E-F400-450D-9DCA-14210AE3DFAC}" name="30-Mar" dataDxfId="132">
       <calculatedColumnFormula>MAX(0,(md!G7-md!F7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="72" xr3:uid="{760DFC79-3F68-4133-AD98-EC55B9CA5B60}" name="31-Mar" dataDxfId="132">
+    <tableColumn id="72" xr3:uid="{760DFC79-3F68-4133-AD98-EC55B9CA5B60}" name="31-Mar" dataDxfId="131">
       <calculatedColumnFormula>MAX(0,(md!H7-md!G7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{3A0DCBAA-0E39-4B12-BA9F-16EC890AE5D7}" name="1-Apr" dataDxfId="131">
+    <tableColumn id="73" xr3:uid="{3A0DCBAA-0E39-4B12-BA9F-16EC890AE5D7}" name="1-Apr" dataDxfId="130">
       <calculatedColumnFormula>MAX(0,(md!I7-md!H7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="74" xr3:uid="{E675B0EB-5084-45E1-B98F-33BBECE64BCA}" name="2-Apr" dataDxfId="130">
+    <tableColumn id="74" xr3:uid="{E675B0EB-5084-45E1-B98F-33BBECE64BCA}" name="2-Apr" dataDxfId="129">
       <calculatedColumnFormula>MAX(0,(md!J7-md!I7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{7D201D0E-7465-446D-96C8-6369C567BA17}" name="3-Apr" dataDxfId="129">
+    <tableColumn id="75" xr3:uid="{7D201D0E-7465-446D-96C8-6369C567BA17}" name="3-Apr" dataDxfId="128">
       <calculatedColumnFormula>MAX(0,(md!K7-md!J7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{28A6AB08-C7E3-44C7-8A67-CED2B8818875}" name="4-Apr" dataDxfId="128">
+    <tableColumn id="76" xr3:uid="{28A6AB08-C7E3-44C7-8A67-CED2B8818875}" name="4-Apr" dataDxfId="127">
       <calculatedColumnFormula>MAX(0,(md!L7-md!K7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DA52AE41-91C4-414C-BA03-812FFA287E17}" name="5-Apr" dataDxfId="127">
+    <tableColumn id="77" xr3:uid="{DA52AE41-91C4-414C-BA03-812FFA287E17}" name="5-Apr" dataDxfId="126">
       <calculatedColumnFormula>MAX(0,(md!M7-md!L7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{824BC17C-FABA-44FC-8DFD-B7D699B912DA}" name="6-Apr" dataDxfId="126">
+    <tableColumn id="78" xr3:uid="{824BC17C-FABA-44FC-8DFD-B7D699B912DA}" name="6-Apr" dataDxfId="125">
       <calculatedColumnFormula>MAX(0,(md!N7-md!M7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{ADAB64C4-87B8-4E71-A8BD-E5D36D0367A3}" name="7-Apr" dataDxfId="125">
+    <tableColumn id="79" xr3:uid="{ADAB64C4-87B8-4E71-A8BD-E5D36D0367A3}" name="7-Apr" dataDxfId="124">
       <calculatedColumnFormula>MAX(0,(md!O7-md!N7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{EFD25893-57FD-4F2A-B0A8-E74649945105}" name="8-Apr" dataDxfId="124">
+    <tableColumn id="80" xr3:uid="{EFD25893-57FD-4F2A-B0A8-E74649945105}" name="8-Apr" dataDxfId="123">
       <calculatedColumnFormula>MAX(0,(md!P7-md!O7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{CD753A3C-95EB-4785-B102-2C58EDAAE5EC}" name="9-Apr" dataDxfId="123">
+    <tableColumn id="81" xr3:uid="{CD753A3C-95EB-4785-B102-2C58EDAAE5EC}" name="9-Apr" dataDxfId="122">
       <calculatedColumnFormula>MAX(0,(md!Q7-md!P7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{996C1CCE-574A-49C4-9367-5B6F1CA045CA}" name="10-Apr" dataDxfId="122">
+    <tableColumn id="82" xr3:uid="{996C1CCE-574A-49C4-9367-5B6F1CA045CA}" name="10-Apr" dataDxfId="121">
       <calculatedColumnFormula>MAX(0,(md!R7-md!Q7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{40EF4BBD-F411-43F1-828D-4E3A9F1D9EA2}" name="11-Apr" dataDxfId="121">
+    <tableColumn id="83" xr3:uid="{40EF4BBD-F411-43F1-828D-4E3A9F1D9EA2}" name="11-Apr" dataDxfId="120">
       <calculatedColumnFormula>MAX(0,(md!S7-md!R7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="84" xr3:uid="{EB725643-C67D-4404-B5FD-5483B4E84D3F}" name="12-Apr" dataDxfId="120">
+    <tableColumn id="84" xr3:uid="{EB725643-C67D-4404-B5FD-5483B4E84D3F}" name="12-Apr" dataDxfId="119">
       <calculatedColumnFormula>MAX(0,(md!T7-md!S7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="85" xr3:uid="{5DA42EA3-77ED-4135-AFAA-FEFBF6C235B5}" name="13-Apr" dataDxfId="119">
+    <tableColumn id="85" xr3:uid="{5DA42EA3-77ED-4135-AFAA-FEFBF6C235B5}" name="13-Apr" dataDxfId="118">
       <calculatedColumnFormula>MAX(0,(md!U7-md!T7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{1AFEE08F-BD43-43C9-9F4D-D582447F1CBC}" name="14-Apr" dataDxfId="118">
+    <tableColumn id="86" xr3:uid="{1AFEE08F-BD43-43C9-9F4D-D582447F1CBC}" name="14-Apr" dataDxfId="117">
       <calculatedColumnFormula>MAX(0,(md!V7-md!U7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{8B04386D-D803-4517-ADE6-E3EB36F2B2CB}" name="15-Apr" dataDxfId="117">
+    <tableColumn id="87" xr3:uid="{8B04386D-D803-4517-ADE6-E3EB36F2B2CB}" name="15-Apr" dataDxfId="116">
       <calculatedColumnFormula>MAX(0,(md!W7-md!V7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{FB2ACEC4-C503-4985-BABF-2F3493F182BB}" name="16-Apr" dataDxfId="116">
+    <tableColumn id="88" xr3:uid="{FB2ACEC4-C503-4985-BABF-2F3493F182BB}" name="16-Apr" dataDxfId="115">
       <calculatedColumnFormula>MAX(0,(md!X7-md!W7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{7E3C269C-D7EB-4419-9DD2-B9360046FEDD}" name="17-Apr" dataDxfId="115">
+    <tableColumn id="89" xr3:uid="{7E3C269C-D7EB-4419-9DD2-B9360046FEDD}" name="17-Apr" dataDxfId="114">
       <calculatedColumnFormula>MAX(0,(md!Y7-md!X7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{54053764-3095-48BD-B0DC-FBAEA597B459}" name="18-Apr" dataDxfId="114">
+    <tableColumn id="90" xr3:uid="{54053764-3095-48BD-B0DC-FBAEA597B459}" name="18-Apr" dataDxfId="113">
       <calculatedColumnFormula>MAX(0,(md!Z7-md!Y7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{4377D20D-95DB-4908-82A3-A401AD129E61}" name="19-Apr" dataDxfId="113">
+    <tableColumn id="91" xr3:uid="{4377D20D-95DB-4908-82A3-A401AD129E61}" name="19-Apr" dataDxfId="112">
       <calculatedColumnFormula>MAX(0,(md!AA7-md!Z7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{51477B52-D4A6-4750-A535-A42BE77C5376}" name="20-Apr" dataDxfId="112">
+    <tableColumn id="92" xr3:uid="{51477B52-D4A6-4750-A535-A42BE77C5376}" name="20-Apr" dataDxfId="111">
       <calculatedColumnFormula>MAX(0,(md!AB7-md!AA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{6B62D812-8EC8-4A07-BB5C-0289C6388D63}" name="21-Apr" dataDxfId="111">
+    <tableColumn id="93" xr3:uid="{6B62D812-8EC8-4A07-BB5C-0289C6388D63}" name="21-Apr" dataDxfId="110">
       <calculatedColumnFormula>MAX(0,(md!AC7-md!AB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{13AE0503-9E29-41B3-B0E2-102AAB93EBC2}" name="22-Apr" dataDxfId="110">
+    <tableColumn id="94" xr3:uid="{13AE0503-9E29-41B3-B0E2-102AAB93EBC2}" name="22-Apr" dataDxfId="109">
       <calculatedColumnFormula>MAX(0,(md!AD7-md!AC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{9E427FAC-7198-4707-A673-7D2FBEE0AB05}" name="23-Apr" dataDxfId="109">
+    <tableColumn id="95" xr3:uid="{9E427FAC-7198-4707-A673-7D2FBEE0AB05}" name="23-Apr" dataDxfId="108">
       <calculatedColumnFormula>MAX(0,(md!AE7-md!AD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{C8AB402E-023F-43C2-9F84-B4F240B82255}" name="24-Apr" dataDxfId="108">
+    <tableColumn id="96" xr3:uid="{C8AB402E-023F-43C2-9F84-B4F240B82255}" name="24-Apr" dataDxfId="107">
       <calculatedColumnFormula>MAX(0,(md!AF7-md!AE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="97" xr3:uid="{49FBF307-99EC-4796-AC0B-FDB70D090EB3}" name="25-Apr" dataDxfId="107">
+    <tableColumn id="97" xr3:uid="{49FBF307-99EC-4796-AC0B-FDB70D090EB3}" name="25-Apr" dataDxfId="106">
       <calculatedColumnFormula>MAX(0,(md!AG7-md!AF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="98" xr3:uid="{97545A0F-D8FA-44BB-B126-7C82E5681E5B}" name="26-Apr" dataDxfId="106">
+    <tableColumn id="98" xr3:uid="{97545A0F-D8FA-44BB-B126-7C82E5681E5B}" name="26-Apr" dataDxfId="105">
       <calculatedColumnFormula>MAX(0,(md!AH7-md!AG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="99" xr3:uid="{A1EA2D07-F633-4D36-8126-F070310B936B}" name="27-Apr" dataDxfId="105">
+    <tableColumn id="99" xr3:uid="{A1EA2D07-F633-4D36-8126-F070310B936B}" name="27-Apr" dataDxfId="104">
       <calculatedColumnFormula>MAX(0,(md!AI7-md!AH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="100" xr3:uid="{6A49089B-958E-4670-BEE8-20D140F9DC00}" name="28-Apr" dataDxfId="104">
+    <tableColumn id="100" xr3:uid="{6A49089B-958E-4670-BEE8-20D140F9DC00}" name="28-Apr" dataDxfId="103">
       <calculatedColumnFormula>MAX(0,(md!AJ7-md!AI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="101" xr3:uid="{264A9134-7104-4DCB-922F-79C66B81E432}" name="29-Apr" dataDxfId="103">
+    <tableColumn id="101" xr3:uid="{264A9134-7104-4DCB-922F-79C66B81E432}" name="29-Apr" dataDxfId="102">
       <calculatedColumnFormula>MAX(0,(md!AK7-md!AJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="102" xr3:uid="{5FDD5894-EE0C-426E-BF3A-4C9D8D68BFA0}" name="30-Apr" dataDxfId="102">
+    <tableColumn id="102" xr3:uid="{5FDD5894-EE0C-426E-BF3A-4C9D8D68BFA0}" name="30-Apr" dataDxfId="101">
       <calculatedColumnFormula>MAX(0,(md!AL7-md!AK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="103" xr3:uid="{C43A5B5F-92CE-4F1C-952E-ABD6BB7341CE}" name="1-May" dataDxfId="101">
+    <tableColumn id="103" xr3:uid="{C43A5B5F-92CE-4F1C-952E-ABD6BB7341CE}" name="1-May" dataDxfId="100">
       <calculatedColumnFormula>MAX(0,(md!AM7-md!AL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="104" xr3:uid="{50B54D8A-B9E6-4CF6-A7B8-A5AB722D33DA}" name="2-May" dataDxfId="100">
+    <tableColumn id="104" xr3:uid="{50B54D8A-B9E6-4CF6-A7B8-A5AB722D33DA}" name="2-May" dataDxfId="99">
       <calculatedColumnFormula>MAX(0,(md!AN7-md!AM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="105" xr3:uid="{4B5FB437-BD09-44D9-925C-3E55C876D9CC}" name="3-May" dataDxfId="99">
+    <tableColumn id="105" xr3:uid="{4B5FB437-BD09-44D9-925C-3E55C876D9CC}" name="3-May" dataDxfId="98">
       <calculatedColumnFormula>MAX(0,(md!AO7-md!AN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="106" xr3:uid="{379072DC-0CD1-4E06-8C87-08A5F7FF2E05}" name="4-May" dataDxfId="98">
+    <tableColumn id="106" xr3:uid="{379072DC-0CD1-4E06-8C87-08A5F7FF2E05}" name="4-May" dataDxfId="97">
       <calculatedColumnFormula>MAX(0,(md!AP7-md!AO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="107" xr3:uid="{AEEEFF0B-566B-457E-B205-F55AEB13AD9E}" name="5-May" dataDxfId="97">
+    <tableColumn id="107" xr3:uid="{AEEEFF0B-566B-457E-B205-F55AEB13AD9E}" name="5-May" dataDxfId="96">
       <calculatedColumnFormula>MAX(0,(md!AQ7-md!AP7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="108" xr3:uid="{94C890F0-71FA-4374-8041-A9193FCE4E17}" name="6-May" dataDxfId="96">
+    <tableColumn id="108" xr3:uid="{94C890F0-71FA-4374-8041-A9193FCE4E17}" name="6-May" dataDxfId="95">
       <calculatedColumnFormula>MAX(0,(md!AR7-md!AQ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="109" xr3:uid="{33E6A0CC-1E42-4A87-B99D-E6A77E72126F}" name="7-May" dataDxfId="95">
+    <tableColumn id="109" xr3:uid="{33E6A0CC-1E42-4A87-B99D-E6A77E72126F}" name="7-May" dataDxfId="94">
       <calculatedColumnFormula>MAX(0,(md!AS7-md!AR7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="110" xr3:uid="{CD2CF375-F2D1-483D-8BD2-30D032E3CD04}" name="8-May" dataDxfId="94">
+    <tableColumn id="110" xr3:uid="{CD2CF375-F2D1-483D-8BD2-30D032E3CD04}" name="8-May" dataDxfId="93">
       <calculatedColumnFormula>MAX(0,(md!AT7-md!AS7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="111" xr3:uid="{E061025C-CDF7-4C91-AF64-42F835C57C96}" name="9-May" dataDxfId="93">
+    <tableColumn id="111" xr3:uid="{E061025C-CDF7-4C91-AF64-42F835C57C96}" name="9-May" dataDxfId="92">
       <calculatedColumnFormula>MAX(0,(md!AU7-md!AT7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="134" xr3:uid="{AE616B94-71FE-467D-86B4-667F51C6B88F}" name="10-May" dataDxfId="92">
+    <tableColumn id="134" xr3:uid="{AE616B94-71FE-467D-86B4-667F51C6B88F}" name="10-May" dataDxfId="91">
       <calculatedColumnFormula>MAX(0,(md!AV7-md!AU7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="135" xr3:uid="{6BB6B4AF-1198-44B7-83CE-176610757419}" name="11-May" dataDxfId="91">
+    <tableColumn id="135" xr3:uid="{6BB6B4AF-1198-44B7-83CE-176610757419}" name="11-May" dataDxfId="90">
       <calculatedColumnFormula>MAX(0,(md!AW7-md!AV7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="136" xr3:uid="{F8A39F33-5023-41AB-91DB-0BCFDE57C6C1}" name="12-May" dataDxfId="90">
+    <tableColumn id="136" xr3:uid="{F8A39F33-5023-41AB-91DB-0BCFDE57C6C1}" name="12-May" dataDxfId="89">
       <calculatedColumnFormula>MAX(0,(md!AX7-md!AW7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="137" xr3:uid="{0676A9AE-3A86-4158-9689-DD58082C1506}" name="13-May" dataDxfId="89">
+    <tableColumn id="137" xr3:uid="{0676A9AE-3A86-4158-9689-DD58082C1506}" name="13-May" dataDxfId="88">
       <calculatedColumnFormula>MAX(0,(md!AY7-md!AX7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="138" xr3:uid="{BE92BDB9-5A19-4036-B052-510BC75BF308}" name="14-May" dataDxfId="88">
+    <tableColumn id="138" xr3:uid="{BE92BDB9-5A19-4036-B052-510BC75BF308}" name="14-May" dataDxfId="87">
       <calculatedColumnFormula>MAX(0,(md!AZ7-md!AY7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="139" xr3:uid="{131F58F1-2C6B-4B17-ABD9-FC3D31544029}" name="15-May" dataDxfId="87">
+    <tableColumn id="139" xr3:uid="{131F58F1-2C6B-4B17-ABD9-FC3D31544029}" name="15-May" dataDxfId="86">
       <calculatedColumnFormula>MAX(0,(md!BA7-md!AZ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="140" xr3:uid="{F9D8DFE8-4BF8-498E-99E2-6B007456B7F4}" name="16-May" dataDxfId="86">
+    <tableColumn id="140" xr3:uid="{F9D8DFE8-4BF8-498E-99E2-6B007456B7F4}" name="16-May" dataDxfId="85">
       <calculatedColumnFormula>MAX(0,(md!BB7-md!BA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="141" xr3:uid="{850888F3-D54B-4B4C-99E1-BA7B9E46EE02}" name="17-May" dataDxfId="85">
+    <tableColumn id="141" xr3:uid="{850888F3-D54B-4B4C-99E1-BA7B9E46EE02}" name="17-May" dataDxfId="84">
       <calculatedColumnFormula>MAX(0,(md!BC7-md!BB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="142" xr3:uid="{4699F9BE-7F39-4078-AB3E-B50D7A10B837}" name="18-May" dataDxfId="84">
+    <tableColumn id="142" xr3:uid="{4699F9BE-7F39-4078-AB3E-B50D7A10B837}" name="18-May" dataDxfId="83">
       <calculatedColumnFormula>MAX(0,(md!BD7-md!BC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="143" xr3:uid="{8BFDF52E-6DAB-4C58-BC98-15836D8A7B57}" name="19-May" dataDxfId="83">
+    <tableColumn id="143" xr3:uid="{8BFDF52E-6DAB-4C58-BC98-15836D8A7B57}" name="19-May" dataDxfId="82">
       <calculatedColumnFormula>MAX(0,(md!BE7-md!BD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="144" xr3:uid="{688B7008-25D3-429E-886B-50AE8A87C074}" name="20-May" dataDxfId="82">
+    <tableColumn id="144" xr3:uid="{688B7008-25D3-429E-886B-50AE8A87C074}" name="20-May" dataDxfId="81">
       <calculatedColumnFormula>MAX(0,(md!BF7-md!BE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="145" xr3:uid="{A7814F0A-A83A-4398-B038-10389D9E6616}" name="21-May" dataDxfId="81">
+    <tableColumn id="145" xr3:uid="{A7814F0A-A83A-4398-B038-10389D9E6616}" name="21-May" dataDxfId="80">
       <calculatedColumnFormula>MAX(0,(md!BG7-md!BF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="146" xr3:uid="{E1B45AD0-EC1B-4E08-BFCF-ABEC66AEDA32}" name="22-May" dataDxfId="80">
+    <tableColumn id="146" xr3:uid="{E1B45AD0-EC1B-4E08-BFCF-ABEC66AEDA32}" name="22-May" dataDxfId="79">
       <calculatedColumnFormula>MAX(0,(md!BH7-md!BG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="147" xr3:uid="{2D30F07E-4A4C-44CC-9488-8B6A8CC75726}" name="23-May" dataDxfId="79">
+    <tableColumn id="147" xr3:uid="{2D30F07E-4A4C-44CC-9488-8B6A8CC75726}" name="23-May" dataDxfId="78">
       <calculatedColumnFormula>MAX(0,(md!BI7-md!BH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="148" xr3:uid="{78F7EC10-89A8-4EEB-9067-BE4A88B0565A}" name="24-May" dataDxfId="78">
+    <tableColumn id="148" xr3:uid="{78F7EC10-89A8-4EEB-9067-BE4A88B0565A}" name="24-May" dataDxfId="77">
       <calculatedColumnFormula>MAX(0,(md!BJ7-md!BI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="149" xr3:uid="{AC298BAD-F13B-4803-8CBB-7A22C58F269E}" name="25-May" dataDxfId="77">
+    <tableColumn id="149" xr3:uid="{AC298BAD-F13B-4803-8CBB-7A22C58F269E}" name="25-May" dataDxfId="76">
       <calculatedColumnFormula>MAX(0,(md!BK7-md!BJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="150" xr3:uid="{8BCAA082-E4E6-4619-8E56-A97B1FF4DA44}" name="26-May" dataDxfId="76">
+    <tableColumn id="150" xr3:uid="{8BCAA082-E4E6-4619-8E56-A97B1FF4DA44}" name="26-May" dataDxfId="75">
       <calculatedColumnFormula>MAX(0,(md!BL7-md!BK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="151" xr3:uid="{4B648A3F-3FCE-4C12-A50A-9BA09CA2697D}" name="27-May" dataDxfId="75">
+    <tableColumn id="151" xr3:uid="{4B648A3F-3FCE-4C12-A50A-9BA09CA2697D}" name="27-May" dataDxfId="74">
       <calculatedColumnFormula>MAX(0,(md!BM7-md!BL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="152" xr3:uid="{08604342-CE44-4618-A009-2731984B9556}" name="28-May" dataDxfId="74">
+    <tableColumn id="152" xr3:uid="{08604342-CE44-4618-A009-2731984B9556}" name="28-May" dataDxfId="73">
       <calculatedColumnFormula>MAX(0,(md!BN7-md!BM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="153" xr3:uid="{DC12CF48-1275-46AA-8DAC-6A196EDD8425}" name="29-May" dataDxfId="73">
+    <tableColumn id="153" xr3:uid="{DC12CF48-1275-46AA-8DAC-6A196EDD8425}" name="29-May" dataDxfId="72">
       <calculatedColumnFormula>MAX(0,(md!BO7-md!BN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="154" xr3:uid="{95A3B7F7-AC6C-4005-9B4D-70C3E3528929}" name="30-May" dataDxfId="72">
+    <tableColumn id="154" xr3:uid="{95A3B7F7-AC6C-4005-9B4D-70C3E3528929}" name="30-May" dataDxfId="71">
       <calculatedColumnFormula>MAX(0,(md!BP7-md!BO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="155" xr3:uid="{944A9E83-F75D-4D8B-AD2C-0A52AF055690}" name="31-May" dataDxfId="71">
+    <tableColumn id="155" xr3:uid="{944A9E83-F75D-4D8B-AD2C-0A52AF055690}" name="31-May" dataDxfId="70">
       <calculatedColumnFormula>MAX(0,(md!BQ7-md!BP7))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3509,209 +3510,209 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDE4BA6F-093B-443E-8276-7E7D049C5DE1}" name="delta_va" displayName="delta_va" ref="A10:BS143" totalsRowShown="0">
   <tableColumns count="71">
-    <tableColumn id="54" xr3:uid="{63B1A33A-0643-4DA3-8D65-E8A8D674C2E1}" name="Locality" dataDxfId="70"/>
-    <tableColumn id="1" xr3:uid="{FD33FE71-7C53-4ED0-99A2-CBB9B098FECC}" name="idx" dataDxfId="69"/>
+    <tableColumn id="54" xr3:uid="{63B1A33A-0643-4DA3-8D65-E8A8D674C2E1}" name="Locality" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{FD33FE71-7C53-4ED0-99A2-CBB9B098FECC}" name="idx" dataDxfId="68"/>
     <tableColumn id="2" xr3:uid="{76548448-4B06-473A-8C19-5749153B6A1D}" name="FIPS"/>
-    <tableColumn id="5" xr3:uid="{D127FF93-52D6-4EBE-92DB-D405A7B74D76}" name="25-Mar" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{6A775A38-C028-4EC5-8C4E-7EBA81CA3009}" name="26-Mar" dataDxfId="67">
+    <tableColumn id="5" xr3:uid="{D127FF93-52D6-4EBE-92DB-D405A7B74D76}" name="25-Mar" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{6A775A38-C028-4EC5-8C4E-7EBA81CA3009}" name="26-Mar" dataDxfId="66">
       <calculatedColumnFormula>MAX(0,(va!F7-va!E7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{273C7511-9B33-45E4-A0E0-0B7D9493A13A}" name="27-Mar" dataDxfId="66">
+    <tableColumn id="30" xr3:uid="{273C7511-9B33-45E4-A0E0-0B7D9493A13A}" name="27-Mar" dataDxfId="65">
       <calculatedColumnFormula>MAX(0,(va!G7-va!F7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{ACC6CBDC-670D-4A3A-BEBD-B09E9FB43BC8}" name="28-Mar" dataDxfId="65">
+    <tableColumn id="31" xr3:uid="{ACC6CBDC-670D-4A3A-BEBD-B09E9FB43BC8}" name="28-Mar" dataDxfId="64">
       <calculatedColumnFormula>MAX(0,(va!H7-va!G7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{E53ECB20-6303-43A3-938C-9363F2920F4D}" name="29-Mar" dataDxfId="64">
+    <tableColumn id="32" xr3:uid="{E53ECB20-6303-43A3-938C-9363F2920F4D}" name="29-Mar" dataDxfId="63">
       <calculatedColumnFormula>MAX(0,(va!I7-va!H7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{4BD36DEA-292C-4095-8245-CFB513181126}" name="30-Mar" dataDxfId="63">
+    <tableColumn id="33" xr3:uid="{4BD36DEA-292C-4095-8245-CFB513181126}" name="30-Mar" dataDxfId="62">
       <calculatedColumnFormula>MAX(0,(va!J7-va!I7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{F1252424-C6F2-4FD1-A193-AC77B37E1DD7}" name="31-Mar" dataDxfId="62">
+    <tableColumn id="34" xr3:uid="{F1252424-C6F2-4FD1-A193-AC77B37E1DD7}" name="31-Mar" dataDxfId="61">
       <calculatedColumnFormula>MAX(0,(va!K7-va!J7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{CD743EF6-E0C5-4901-981D-2F27459CF468}" name="1-Apr" dataDxfId="61">
+    <tableColumn id="35" xr3:uid="{CD743EF6-E0C5-4901-981D-2F27459CF468}" name="1-Apr" dataDxfId="60">
       <calculatedColumnFormula>MAX(0,(va!L7-va!K7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{38ED5D84-2B28-479F-8C2D-B040039247F1}" name="2-Apr" dataDxfId="60">
+    <tableColumn id="36" xr3:uid="{38ED5D84-2B28-479F-8C2D-B040039247F1}" name="2-Apr" dataDxfId="59">
       <calculatedColumnFormula>MAX(0,(va!M7-va!L7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{CE521412-A311-433D-93C0-63BD7A514269}" name="3-Apr" dataDxfId="59">
+    <tableColumn id="37" xr3:uid="{CE521412-A311-433D-93C0-63BD7A514269}" name="3-Apr" dataDxfId="58">
       <calculatedColumnFormula>MAX(0,(va!N7-va!M7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{5D4C35B4-2054-4B4A-80F8-E9361CEA0ACC}" name="4-Apr" dataDxfId="58">
+    <tableColumn id="38" xr3:uid="{5D4C35B4-2054-4B4A-80F8-E9361CEA0ACC}" name="4-Apr" dataDxfId="57">
       <calculatedColumnFormula>MAX(0,(va!O7-va!N7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{10A2F446-2134-49BE-8AEF-2D84D9FA875B}" name="5-Apr" dataDxfId="57">
+    <tableColumn id="39" xr3:uid="{10A2F446-2134-49BE-8AEF-2D84D9FA875B}" name="5-Apr" dataDxfId="56">
       <calculatedColumnFormula>MAX(0,(va!P7-va!O7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{070AE366-CB37-4620-BA0C-1BE4F2C27279}" name="6-Apr" dataDxfId="56">
+    <tableColumn id="40" xr3:uid="{070AE366-CB37-4620-BA0C-1BE4F2C27279}" name="6-Apr" dataDxfId="55">
       <calculatedColumnFormula>MAX(0,(va!Q7-va!P7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{FBB50AAC-FF54-4926-8A78-E153DAC9F95B}" name="7-Apr" dataDxfId="55">
+    <tableColumn id="41" xr3:uid="{FBB50AAC-FF54-4926-8A78-E153DAC9F95B}" name="7-Apr" dataDxfId="54">
       <calculatedColumnFormula>MAX(0,(va!R7-va!Q7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{80F1496C-DB69-4C7F-9B80-445A59EF1B6D}" name="8-Apr" dataDxfId="54">
+    <tableColumn id="42" xr3:uid="{80F1496C-DB69-4C7F-9B80-445A59EF1B6D}" name="8-Apr" dataDxfId="53">
       <calculatedColumnFormula>MAX(0,(va!S7-va!R7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{B2D70650-881C-44FB-A51E-6DE0013D50F5}" name="9-Apr" dataDxfId="53">
+    <tableColumn id="43" xr3:uid="{B2D70650-881C-44FB-A51E-6DE0013D50F5}" name="9-Apr" dataDxfId="52">
       <calculatedColumnFormula>MAX(0,(va!T7-va!S7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{24972282-0E25-4AD5-A741-F9215388ABC2}" name="10-Apr" dataDxfId="52">
+    <tableColumn id="44" xr3:uid="{24972282-0E25-4AD5-A741-F9215388ABC2}" name="10-Apr" dataDxfId="51">
       <calculatedColumnFormula>MAX(0,(va!U7-va!T7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{6D9BB0E2-F429-49ED-BDB5-F356A4DC28CD}" name="11-Apr" dataDxfId="51">
+    <tableColumn id="45" xr3:uid="{6D9BB0E2-F429-49ED-BDB5-F356A4DC28CD}" name="11-Apr" dataDxfId="50">
       <calculatedColumnFormula>MAX(0,(va!V7-va!U7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{B7D6F42A-CE7F-4560-915A-2D75BB5FB9A7}" name="12-Apr" dataDxfId="50">
+    <tableColumn id="46" xr3:uid="{B7D6F42A-CE7F-4560-915A-2D75BB5FB9A7}" name="12-Apr" dataDxfId="49">
       <calculatedColumnFormula>MAX(0,(va!W7-va!V7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{D27C7A8C-BAA4-4A29-97DC-6D26B5399868}" name="13-Apr" dataDxfId="49">
+    <tableColumn id="47" xr3:uid="{D27C7A8C-BAA4-4A29-97DC-6D26B5399868}" name="13-Apr" dataDxfId="48">
       <calculatedColumnFormula>MAX(0,(va!X7-va!W7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{F892CCC7-B11E-4EF0-95BE-4BFE027CFFD1}" name="14-Apr" dataDxfId="48">
+    <tableColumn id="48" xr3:uid="{F892CCC7-B11E-4EF0-95BE-4BFE027CFFD1}" name="14-Apr" dataDxfId="47">
       <calculatedColumnFormula>MAX(0,(va!Y7-va!X7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{A3F0E963-9326-4555-ADE5-F4EFB83126F3}" name="15-Apr" dataDxfId="47">
+    <tableColumn id="49" xr3:uid="{A3F0E963-9326-4555-ADE5-F4EFB83126F3}" name="15-Apr" dataDxfId="46">
       <calculatedColumnFormula>MAX(0,(va!Z7-va!Y7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" xr3:uid="{3437FD4E-8616-4572-907D-5B33B199B617}" name="16-Apr" dataDxfId="46">
+    <tableColumn id="50" xr3:uid="{3437FD4E-8616-4572-907D-5B33B199B617}" name="16-Apr" dataDxfId="45">
       <calculatedColumnFormula>MAX(0,(va!AA7-va!Z7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{E6F99628-1312-41B6-A56A-B05C101DA0FB}" name="17-Apr" dataDxfId="45">
+    <tableColumn id="51" xr3:uid="{E6F99628-1312-41B6-A56A-B05C101DA0FB}" name="17-Apr" dataDxfId="44">
       <calculatedColumnFormula>MAX(0,(va!AB7-va!AA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{C7724E90-6B56-4650-A710-D3E539E48665}" name="18-Apr" dataDxfId="44">
+    <tableColumn id="52" xr3:uid="{C7724E90-6B56-4650-A710-D3E539E48665}" name="18-Apr" dataDxfId="43">
       <calculatedColumnFormula>MAX(0,(va!AC7-va!AB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{2321B68A-9B81-4AD5-BC7B-70E930711815}" name="19-Apr" dataDxfId="43">
+    <tableColumn id="53" xr3:uid="{2321B68A-9B81-4AD5-BC7B-70E930711815}" name="19-Apr" dataDxfId="42">
       <calculatedColumnFormula>MAX(0,(va!AD7-va!AC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{0909EDD8-E202-4043-8949-F6EA28E1C4AA}" name="20-Apr" dataDxfId="42">
+    <tableColumn id="22" xr3:uid="{0909EDD8-E202-4043-8949-F6EA28E1C4AA}" name="20-Apr" dataDxfId="41">
       <calculatedColumnFormula>MAX(0,(va!AE7-va!AD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{2367F62B-C6E4-48C7-81C9-530399CE2871}" name="21-Apr" dataDxfId="41">
+    <tableColumn id="23" xr3:uid="{2367F62B-C6E4-48C7-81C9-530399CE2871}" name="21-Apr" dataDxfId="40">
       <calculatedColumnFormula>MAX(0,(va!AF7-va!AE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{EB75A609-8DAC-42A0-990A-114C4750203C}" name="22-Apr" dataDxfId="40">
+    <tableColumn id="24" xr3:uid="{EB75A609-8DAC-42A0-990A-114C4750203C}" name="22-Apr" dataDxfId="39">
       <calculatedColumnFormula>MAX(0,(va!AG7-va!AF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{F23D1A1C-FDCB-42E7-BFFE-8860B35519AC}" name="23-Apr" dataDxfId="39">
+    <tableColumn id="25" xr3:uid="{F23D1A1C-FDCB-42E7-BFFE-8860B35519AC}" name="23-Apr" dataDxfId="38">
       <calculatedColumnFormula>MAX(0,(va!AH7-va!AG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{F5222424-7E21-47C9-A5EE-468D35C8D4D4}" name="24-Apr" dataDxfId="38">
+    <tableColumn id="26" xr3:uid="{F5222424-7E21-47C9-A5EE-468D35C8D4D4}" name="24-Apr" dataDxfId="37">
       <calculatedColumnFormula>MAX(0,(va!AI7-va!AH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{F5D517E5-C861-4DD4-A408-D023894C3440}" name="25-Apr" dataDxfId="37">
+    <tableColumn id="27" xr3:uid="{F5D517E5-C861-4DD4-A408-D023894C3440}" name="25-Apr" dataDxfId="36">
       <calculatedColumnFormula>MAX(0,(va!AJ7-va!AI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{6663E32B-51D1-4285-89F0-ADB6AC73C467}" name="26-Apr" dataDxfId="36">
+    <tableColumn id="28" xr3:uid="{6663E32B-51D1-4285-89F0-ADB6AC73C467}" name="26-Apr" dataDxfId="35">
       <calculatedColumnFormula>MAX(0,(va!AK7-va!AJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{F1067EAF-A27C-4330-9D36-8E8450545F45}" name="27-Apr" dataDxfId="35">
+    <tableColumn id="29" xr3:uid="{F1067EAF-A27C-4330-9D36-8E8450545F45}" name="27-Apr" dataDxfId="34">
       <calculatedColumnFormula>MAX(0,(va!AL7-va!AK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AC4610E3-C7C4-4914-AA0E-DB2D0357ED06}" name="28-Apr" dataDxfId="34">
+    <tableColumn id="14" xr3:uid="{AC4610E3-C7C4-4914-AA0E-DB2D0357ED06}" name="28-Apr" dataDxfId="33">
       <calculatedColumnFormula>MAX(0,(va!AM7-va!AL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{FF6B8433-3EC6-458E-89D7-5EB244B1F60B}" name="29-Apr" dataDxfId="33">
+    <tableColumn id="15" xr3:uid="{FF6B8433-3EC6-458E-89D7-5EB244B1F60B}" name="29-Apr" dataDxfId="32">
       <calculatedColumnFormula>MAX(0,(va!AN7-va!AM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{BA897434-B64A-4817-A3F9-46FF64B05E37}" name="30-Apr" dataDxfId="32">
+    <tableColumn id="16" xr3:uid="{BA897434-B64A-4817-A3F9-46FF64B05E37}" name="30-Apr" dataDxfId="31">
       <calculatedColumnFormula>MAX(0,(va!AO7-va!AN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{6AE0C639-A5DD-42D5-8FA4-8C9B3EA56006}" name="1-May" dataDxfId="31">
+    <tableColumn id="17" xr3:uid="{6AE0C639-A5DD-42D5-8FA4-8C9B3EA56006}" name="1-May" dataDxfId="30">
       <calculatedColumnFormula>MAX(0,(va!AP7-va!AO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{5E07F0EB-D30C-4867-AED9-8E88FBC08D77}" name="2-May" dataDxfId="30">
+    <tableColumn id="18" xr3:uid="{5E07F0EB-D30C-4867-AED9-8E88FBC08D77}" name="2-May" dataDxfId="29">
       <calculatedColumnFormula>MAX(0,(va!AQ7-va!AP7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{7E7DFBC2-6059-4A36-AF80-B77B98657554}" name="3-May" dataDxfId="29">
+    <tableColumn id="19" xr3:uid="{7E7DFBC2-6059-4A36-AF80-B77B98657554}" name="3-May" dataDxfId="28">
       <calculatedColumnFormula>MAX(0,(va!AR7-va!AQ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{04DF1446-184B-4D11-B3CA-CBA62452BF62}" name="4-May" dataDxfId="28">
+    <tableColumn id="20" xr3:uid="{04DF1446-184B-4D11-B3CA-CBA62452BF62}" name="4-May" dataDxfId="27">
       <calculatedColumnFormula>MAX(0,(va!AS7-va!AR7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{8B99FEA6-1FD6-49F9-9871-F98BDB596D5E}" name="5-May" dataDxfId="27">
+    <tableColumn id="21" xr3:uid="{8B99FEA6-1FD6-49F9-9871-F98BDB596D5E}" name="5-May" dataDxfId="26">
       <calculatedColumnFormula>MAX(0,(va!AT7-va!AS7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6658ADF8-B8F0-4C00-BEBC-CDE0466AF941}" name="6-May" dataDxfId="26">
+    <tableColumn id="10" xr3:uid="{6658ADF8-B8F0-4C00-BEBC-CDE0466AF941}" name="6-May" dataDxfId="25">
       <calculatedColumnFormula>MAX(0,(va!AU7-va!AT7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{3907184E-0754-43D6-A0B2-BA9FC1B11F9C}" name="7-May" dataDxfId="25">
+    <tableColumn id="11" xr3:uid="{3907184E-0754-43D6-A0B2-BA9FC1B11F9C}" name="7-May" dataDxfId="24">
       <calculatedColumnFormula>MAX(0,(va!AV7-va!AU7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F7EBE278-C13F-43E7-B6C5-146063646048}" name="8-May" dataDxfId="24">
+    <tableColumn id="12" xr3:uid="{F7EBE278-C13F-43E7-B6C5-146063646048}" name="8-May" dataDxfId="23">
       <calculatedColumnFormula>MAX(0,(va!AW7-va!AV7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{B169461D-64D3-4BF0-BD2E-EC9669326BEF}" name="9-May" dataDxfId="23">
+    <tableColumn id="13" xr3:uid="{B169461D-64D3-4BF0-BD2E-EC9669326BEF}" name="9-May" dataDxfId="22">
       <calculatedColumnFormula>MAX(0,(va!AX7-va!AW7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD44E28B-08BF-4D2B-BEE3-9536EEE5373F}" name="10-May" dataDxfId="22">
+    <tableColumn id="8" xr3:uid="{CD44E28B-08BF-4D2B-BEE3-9536EEE5373F}" name="10-May" dataDxfId="21">
       <calculatedColumnFormula>MAX(0,(va!AY7-va!AX7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A4B9A93-0725-4010-A087-30E03FE5D7BA}" name="11-May" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{4A4B9A93-0725-4010-A087-30E03FE5D7BA}" name="11-May" dataDxfId="20">
       <calculatedColumnFormula>MAX(0,(va!AZ7-va!AY7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2E62BF37-C2F6-4728-B7D3-D5351C180DB1}" name="12-May" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{2E62BF37-C2F6-4728-B7D3-D5351C180DB1}" name="12-May" dataDxfId="19">
       <calculatedColumnFormula>MAX(0,(va!BA7-va!AZ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33AAE041-9853-4118-9ABB-D3E20ADE0CDA}" name="13-May" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{33AAE041-9853-4118-9ABB-D3E20ADE0CDA}" name="13-May" dataDxfId="18">
       <calculatedColumnFormula>MAX(0,(va!BB7-va!BA7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{84C1D2A4-6A91-4756-BB95-DBFFFC7C0C27}" name="14-May" dataDxfId="18">
+    <tableColumn id="55" xr3:uid="{84C1D2A4-6A91-4756-BB95-DBFFFC7C0C27}" name="14-May" dataDxfId="17">
       <calculatedColumnFormula>MAX(0,(va!BC7-va!BB7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="56" xr3:uid="{6A194ED5-9BB1-440C-A0AC-25E5553948E0}" name="15-May" dataDxfId="17">
+    <tableColumn id="56" xr3:uid="{6A194ED5-9BB1-440C-A0AC-25E5553948E0}" name="15-May" dataDxfId="16">
       <calculatedColumnFormula>MAX(0,(va!BD7-va!BC7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="57" xr3:uid="{E4944CC5-EA4C-4102-87EC-2BBD05DEB3CC}" name="16-May" dataDxfId="16">
+    <tableColumn id="57" xr3:uid="{E4944CC5-EA4C-4102-87EC-2BBD05DEB3CC}" name="16-May" dataDxfId="15">
       <calculatedColumnFormula>MAX(0,(va!BE7-va!BD7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="58" xr3:uid="{80518BBE-DB7B-456F-BA3F-098675345342}" name="17-May" dataDxfId="15">
+    <tableColumn id="58" xr3:uid="{80518BBE-DB7B-456F-BA3F-098675345342}" name="17-May" dataDxfId="14">
       <calculatedColumnFormula>MAX(0,(va!BF7-va!BE7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" xr3:uid="{8890D892-2DB0-4294-B2B0-F0E35897244B}" name="18-May" dataDxfId="14">
+    <tableColumn id="59" xr3:uid="{8890D892-2DB0-4294-B2B0-F0E35897244B}" name="18-May" dataDxfId="13">
       <calculatedColumnFormula>MAX(0,(va!BG7-va!BF7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="60" xr3:uid="{3C7B710E-EE82-4733-8595-B3558286C4A4}" name="19-May" dataDxfId="13">
+    <tableColumn id="60" xr3:uid="{3C7B710E-EE82-4733-8595-B3558286C4A4}" name="19-May" dataDxfId="12">
       <calculatedColumnFormula>MAX(0,(va!BH7-va!BG7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="61" xr3:uid="{15806639-509B-4998-B1F9-4D768A2A4FF8}" name="20-May" dataDxfId="12">
+    <tableColumn id="61" xr3:uid="{15806639-509B-4998-B1F9-4D768A2A4FF8}" name="20-May" dataDxfId="11">
       <calculatedColumnFormula>MAX(0,(va!BI7-va!BH7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{979C3098-F4F8-4A51-B7AF-115BE23F8E36}" name="21-May" dataDxfId="11">
+    <tableColumn id="62" xr3:uid="{979C3098-F4F8-4A51-B7AF-115BE23F8E36}" name="21-May" dataDxfId="10">
       <calculatedColumnFormula>MAX(0,(va!BJ7-va!BI7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{581E410D-1F56-463B-A79B-39C309A32AD5}" name="22-May" dataDxfId="10">
+    <tableColumn id="63" xr3:uid="{581E410D-1F56-463B-A79B-39C309A32AD5}" name="22-May" dataDxfId="9">
       <calculatedColumnFormula>MAX(0,(va!BK7-va!BJ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{7DEACC7F-9EE9-4ECB-9078-A7DFE44015D5}" name="23-May" dataDxfId="9">
+    <tableColumn id="64" xr3:uid="{7DEACC7F-9EE9-4ECB-9078-A7DFE44015D5}" name="23-May" dataDxfId="8">
       <calculatedColumnFormula>MAX(0,(va!BL7-va!BK7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{F4060BBB-E4ED-4A58-A557-430AD718B5CB}" name="24-May" dataDxfId="8">
+    <tableColumn id="65" xr3:uid="{F4060BBB-E4ED-4A58-A557-430AD718B5CB}" name="24-May" dataDxfId="7">
       <calculatedColumnFormula>MAX(0,(va!BM7-va!BL7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{DFA30D74-C0ED-439F-B66D-B8802D5CB693}" name="25-May" dataDxfId="7">
+    <tableColumn id="66" xr3:uid="{DFA30D74-C0ED-439F-B66D-B8802D5CB693}" name="25-May" dataDxfId="6">
       <calculatedColumnFormula>MAX(0,(va!BN7-va!BM7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{81E9478F-D6B4-4B44-B1E3-77E1D6C58E52}" name="26-May" dataDxfId="6">
+    <tableColumn id="67" xr3:uid="{81E9478F-D6B4-4B44-B1E3-77E1D6C58E52}" name="26-May" dataDxfId="5">
       <calculatedColumnFormula>MAX(0,(va!BO7-va!BN7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="68" xr3:uid="{28BE5C31-58B2-4EB9-875C-DB12815ABB54}" name="27-May" dataDxfId="5">
+    <tableColumn id="68" xr3:uid="{28BE5C31-58B2-4EB9-875C-DB12815ABB54}" name="27-May" dataDxfId="4">
       <calculatedColumnFormula>MAX(0,(va!BP7-va!BO7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="69" xr3:uid="{C8F214AC-38D3-49D8-A4C1-772682FA80C7}" name="28-May" dataDxfId="4">
+    <tableColumn id="69" xr3:uid="{C8F214AC-38D3-49D8-A4C1-772682FA80C7}" name="28-May" dataDxfId="3">
       <calculatedColumnFormula>MAX(0,(va!BQ7-va!BP7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="70" xr3:uid="{EE1980CC-3CC5-46F1-BA70-2D4487917FFD}" name="29-May" dataDxfId="3">
+    <tableColumn id="70" xr3:uid="{EE1980CC-3CC5-46F1-BA70-2D4487917FFD}" name="29-May" dataDxfId="2">
       <calculatedColumnFormula>MAX(0,(va!BR7-va!BQ7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="71" xr3:uid="{05E114EA-2EEA-46AA-92A0-906C6A3D082F}" name="30-May" dataDxfId="2">
+    <tableColumn id="71" xr3:uid="{05E114EA-2EEA-46AA-92A0-906C6A3D082F}" name="30-May" dataDxfId="1">
       <calculatedColumnFormula>MAX(0,(va!BS7-va!BR7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="72" xr3:uid="{55F28C38-AF0C-4D02-AC6A-D856844BFEF1}" name="31-May" dataDxfId="1">
+    <tableColumn id="72" xr3:uid="{55F28C38-AF0C-4D02-AC6A-D856844BFEF1}" name="31-May" dataDxfId="0">
       <calculatedColumnFormula>MAX(0,(va!BT7-va!BS7))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4018,8 +4019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E207B2A-317D-4660-A7D7-5B9F35994222}">
   <dimension ref="A1:CC46"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4126,6 +4127,9 @@
       <c r="AD2" s="12">
         <v>10039</v>
       </c>
+      <c r="AE2" s="12">
+        <v>10640</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -4234,7 +4238,7 @@
       </c>
       <c r="AE3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1875</v>
       </c>
       <c r="AF3" s="10">
         <f t="shared" si="0"/>
@@ -4533,6 +4537,9 @@
       <c r="AD5" s="10">
         <v>47</v>
       </c>
+      <c r="AE5" s="10">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -4625,7 +4632,7 @@
       <c r="AD6" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AE6" s="18" t="s">
         <v>195</v>
       </c>
       <c r="AF6" s="3" t="s">
@@ -4869,6 +4876,9 @@
       </c>
       <c r="AD7" s="10">
         <v>202</v>
+      </c>
+      <c r="AE7" s="35">
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.35">
@@ -4962,6 +4972,9 @@
       <c r="AD8" s="10">
         <v>151</v>
       </c>
+      <c r="AE8" s="35">
+        <v>160</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A9" s="25">
@@ -5054,6 +5067,9 @@
       <c r="AD9" s="10">
         <v>139</v>
       </c>
+      <c r="AE9" s="35">
+        <v>143</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A10" s="27">
@@ -5146,6 +5162,9 @@
       <c r="AD10" s="10">
         <v>288</v>
       </c>
+      <c r="AE10" s="35">
+        <v>303</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A11" s="25">
@@ -5238,6 +5257,9 @@
       <c r="AD11" s="10">
         <v>231</v>
       </c>
+      <c r="AE11" s="35">
+        <v>250</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A12" s="27">
@@ -5330,6 +5352,9 @@
       <c r="AD12" s="10">
         <v>266</v>
       </c>
+      <c r="AE12" s="35">
+        <v>281</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
@@ -5422,6 +5447,9 @@
       <c r="AD13" s="10">
         <v>266</v>
       </c>
+      <c r="AE13" s="35">
+        <v>284</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A14" s="27">
@@ -5514,6 +5542,9 @@
       <c r="AD14" s="10">
         <v>202</v>
       </c>
+      <c r="AE14" s="35">
+        <v>218</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
@@ -5605,6 +5636,9 @@
       </c>
       <c r="AD15" s="10">
         <v>33</v>
+      </c>
+      <c r="AE15" s="35">
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.35">
@@ -5760,7 +5794,7 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5835,7 +5869,7 @@
         <v>39544</v>
       </c>
       <c r="T2" s="10">
-        <v>0</v>
+        <v>41539</v>
       </c>
       <c r="U2" s="10">
         <v>0</v>
@@ -6058,7 +6092,7 @@
       </c>
       <c r="T3" s="10">
         <f>SUM(md[12-Apr])</f>
-        <v>0</v>
+        <v>8225</v>
       </c>
       <c r="U3" s="10">
         <f>SUM(md[13-Apr])</f>
@@ -6313,7 +6347,7 @@
         <v>1709</v>
       </c>
       <c r="T4" s="10">
-        <v>0</v>
+        <v>1860</v>
       </c>
       <c r="U4" s="10">
         <v>0</v>
@@ -6519,7 +6553,7 @@
         <v>206</v>
       </c>
       <c r="T5" s="10">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="U5" s="10">
         <v>0</v>
@@ -6727,7 +6761,7 @@
       <c r="S6" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="18" t="s">
         <v>196</v>
       </c>
       <c r="U6" s="3" t="s">
@@ -6936,6 +6970,9 @@
       <c r="S7">
         <v>11</v>
       </c>
+      <c r="T7">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -6995,6 +7032,9 @@
       <c r="S8" s="10">
         <v>615</v>
       </c>
+      <c r="T8" s="10">
+        <v>659</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -7054,6 +7094,9 @@
       <c r="S9">
         <v>756</v>
       </c>
+      <c r="T9">
+        <v>812</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -7113,6 +7156,9 @@
       <c r="S10">
         <v>1173</v>
       </c>
+      <c r="T10">
+        <v>1257</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -7172,6 +7218,9 @@
       <c r="S11">
         <v>82</v>
       </c>
+      <c r="T11">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -7231,6 +7280,9 @@
       <c r="S12">
         <v>15</v>
       </c>
+      <c r="T12">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -7290,6 +7342,9 @@
       <c r="S13">
         <v>214</v>
       </c>
+      <c r="T13">
+        <v>236</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -7349,6 +7404,9 @@
       <c r="S14">
         <v>66</v>
       </c>
+      <c r="T14">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -7408,6 +7466,9 @@
       <c r="S15">
         <v>235</v>
       </c>
+      <c r="T15">
+        <v>253</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -7467,8 +7528,11 @@
       <c r="S16" s="10">
         <v>8</v>
       </c>
+      <c r="T16" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -7526,8 +7590,11 @@
       <c r="S17">
         <v>341</v>
       </c>
+      <c r="T17">
+        <v>368</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -7585,8 +7652,11 @@
       <c r="S18">
         <v>4</v>
       </c>
+      <c r="T18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -7644,8 +7714,11 @@
       <c r="S19">
         <v>120</v>
       </c>
+      <c r="T19">
+        <v>129</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -7703,8 +7776,11 @@
       <c r="S20">
         <v>351</v>
       </c>
+      <c r="T20">
+        <v>371</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -7762,8 +7838,11 @@
       <c r="S21">
         <v>10</v>
       </c>
+      <c r="T21">
+        <v>11</v>
+      </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -7821,8 +7900,11 @@
       <c r="S22">
         <v>1537</v>
       </c>
+      <c r="T22">
+        <v>1631</v>
+      </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -7880,8 +7962,11 @@
       <c r="S23">
         <v>1923</v>
       </c>
+      <c r="T23">
+        <v>2035</v>
+      </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -7939,8 +8024,11 @@
       <c r="S24">
         <v>19</v>
       </c>
+      <c r="T24">
+        <v>19</v>
+      </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -7998,8 +8086,11 @@
       <c r="S25">
         <v>73</v>
       </c>
+      <c r="T25">
+        <v>82</v>
+      </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -8057,8 +8148,11 @@
       <c r="S26">
         <v>4</v>
       </c>
+      <c r="T26">
+        <v>4</v>
+      </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -8116,8 +8210,11 @@
       <c r="S27">
         <v>13</v>
       </c>
+      <c r="T27">
+        <v>14</v>
+      </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -8175,8 +8272,11 @@
       <c r="S28">
         <v>72</v>
       </c>
+      <c r="T28">
+        <v>75</v>
+      </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -8234,8 +8334,11 @@
       <c r="S29">
         <v>33</v>
       </c>
+      <c r="T29">
+        <v>42</v>
+      </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -8293,8 +8396,11 @@
       <c r="S30">
         <v>19</v>
       </c>
+      <c r="T30">
+        <v>20</v>
+      </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -8388,7 +8494,7 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8490,7 +8596,7 @@
       </c>
       <c r="W2" s="10">
         <f>SUM(va[12-Apr])</f>
-        <v>0</v>
+        <v>5274</v>
       </c>
       <c r="X2" s="10">
         <f>SUM(va[13-Apr])</f>
@@ -8748,7 +8854,7 @@
         <v>837</v>
       </c>
       <c r="W3" s="10">
-        <v>0</v>
+        <v>872</v>
       </c>
       <c r="X3" s="10">
         <v>0</v>
@@ -8957,7 +9063,7 @@
         <v>130</v>
       </c>
       <c r="W4" s="10">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="X4" s="10">
         <v>0</v>
@@ -9166,7 +9272,7 @@
         <v>37999</v>
       </c>
       <c r="W5" s="10">
-        <v>0</v>
+        <v>39985</v>
       </c>
       <c r="X5" s="10">
         <v>0</v>
@@ -9383,7 +9489,7 @@
       <c r="V6" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="18" t="s">
         <v>196</v>
       </c>
       <c r="X6" s="3" t="s">
@@ -9601,9 +9707,12 @@
       <c r="V7" s="10">
         <v>188</v>
       </c>
+      <c r="W7" s="10">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="29" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -9669,9 +9778,12 @@
       <c r="V8" s="10">
         <v>4</v>
       </c>
+      <c r="W8" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A9" s="33"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -9735,9 +9847,12 @@
       <c r="V9" s="10">
         <v>22</v>
       </c>
+      <c r="W9" s="10">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -9801,9 +9916,12 @@
       <c r="V10" s="10">
         <v>2</v>
       </c>
+      <c r="W10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -9867,9 +9985,12 @@
       <c r="V11" s="10">
         <v>13</v>
       </c>
+      <c r="W11" s="10">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -9933,9 +10054,12 @@
       <c r="V12" s="10">
         <v>1</v>
       </c>
+      <c r="W12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A13" s="34"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -9997,6 +10121,9 @@
         <v>1</v>
       </c>
       <c r="V13" s="10">
+        <v>1</v>
+      </c>
+      <c r="W13" s="10">
         <v>1</v>
       </c>
     </row>
@@ -10067,9 +10194,12 @@
       <c r="V14" s="10">
         <v>349</v>
       </c>
+      <c r="W14" s="10">
+        <v>366</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -10135,9 +10265,12 @@
       <c r="V15" s="10">
         <v>17</v>
       </c>
+      <c r="W15" s="10">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -10201,9 +10334,12 @@
       <c r="V16" s="10">
         <v>0</v>
       </c>
+      <c r="W16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A17" s="33"/>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A17" s="30"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -10267,9 +10403,12 @@
       <c r="V17" s="10">
         <v>0</v>
       </c>
+      <c r="W17" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A18" s="33"/>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A18" s="30"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -10333,9 +10472,12 @@
       <c r="V18" s="10">
         <v>3</v>
       </c>
+      <c r="W18" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A19" s="33"/>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19" s="30"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -10399,9 +10541,12 @@
       <c r="V19" s="10">
         <v>44</v>
       </c>
+      <c r="W19" s="10">
+        <v>43</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A20" s="33"/>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A20" s="30"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -10465,9 +10610,12 @@
       <c r="V20" s="10">
         <v>4</v>
       </c>
+      <c r="W20" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A21" s="33"/>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A21" s="30"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -10531,9 +10679,12 @@
       <c r="V21" s="10">
         <v>79</v>
       </c>
+      <c r="W21" s="10">
+        <v>81</v>
+      </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A22" s="33"/>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A22" s="30"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -10597,9 +10748,12 @@
       <c r="V22" s="10">
         <v>3</v>
       </c>
+      <c r="W22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A23" s="33"/>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A23" s="30"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -10663,9 +10817,12 @@
       <c r="V23" s="10">
         <v>1</v>
       </c>
+      <c r="W23" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A24" s="34"/>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A24" s="31"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -10729,9 +10886,12 @@
       <c r="V24" s="10">
         <v>5</v>
       </c>
+      <c r="W24" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A25" s="29" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A25" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -10797,9 +10957,12 @@
       <c r="V25" s="10">
         <v>10</v>
       </c>
+      <c r="W25" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A26" s="33"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -10863,9 +11026,12 @@
       <c r="V26" s="10">
         <v>7</v>
       </c>
+      <c r="W26" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A27" s="33"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -10929,9 +11095,12 @@
       <c r="V27" s="10">
         <v>15</v>
       </c>
+      <c r="W27" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A28" s="30"/>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A28" s="33"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -10995,9 +11164,12 @@
       <c r="V28" s="10">
         <v>9</v>
       </c>
+      <c r="W28" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A29" s="31"/>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A29" s="34"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -11061,8 +11233,11 @@
       <c r="V29" s="10">
         <v>31</v>
       </c>
+      <c r="W29" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -11129,9 +11304,12 @@
       <c r="V30" s="10">
         <v>115</v>
       </c>
+      <c r="W30" s="10">
+        <v>121</v>
+      </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A31" s="29" t="s">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A31" s="32" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -11197,9 +11375,12 @@
       <c r="V31" s="10">
         <v>203</v>
       </c>
+      <c r="W31" s="10">
+        <v>209</v>
+      </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A32" s="30"/>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A32" s="33"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -11263,9 +11444,12 @@
       <c r="V32" s="10">
         <v>5</v>
       </c>
+      <c r="W32" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A33" s="31"/>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A33" s="34"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -11329,9 +11513,12 @@
       <c r="V33" s="10">
         <v>6</v>
       </c>
+      <c r="W33" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A34" s="32" t="s">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A34" s="29" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -11397,9 +11584,12 @@
       <c r="V34" s="10">
         <v>8</v>
       </c>
+      <c r="W34" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A35" s="33"/>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A35" s="30"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -11463,9 +11653,12 @@
       <c r="V35" s="10">
         <v>26</v>
       </c>
+      <c r="W35" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A36" s="33"/>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A36" s="30"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -11529,9 +11722,12 @@
       <c r="V36" s="10">
         <v>38</v>
       </c>
+      <c r="W36" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A37" s="34"/>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A37" s="31"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -11595,9 +11791,12 @@
       <c r="V37" s="10">
         <v>12</v>
       </c>
+      <c r="W37" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A38" s="29" t="s">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A38" s="32" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -11663,9 +11862,12 @@
       <c r="V38" s="10">
         <v>6</v>
       </c>
+      <c r="W38" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A39" s="30"/>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A39" s="33"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -11729,9 +11931,12 @@
       <c r="V39" s="10">
         <v>8</v>
       </c>
+      <c r="W39" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A40" s="30"/>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A40" s="33"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -11795,9 +12000,12 @@
       <c r="V40" s="10">
         <v>26</v>
       </c>
+      <c r="W40" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A41" s="30"/>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A41" s="33"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -11861,9 +12069,12 @@
       <c r="V41" s="10">
         <v>3</v>
       </c>
+      <c r="W41" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A42" s="30"/>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A42" s="33"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -11927,9 +12138,12 @@
       <c r="V42" s="10">
         <v>8</v>
       </c>
+      <c r="W42" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A43" s="30"/>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A43" s="33"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -11993,9 +12207,12 @@
       <c r="V43" s="10">
         <v>7</v>
       </c>
+      <c r="W43" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A44" s="30"/>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A44" s="33"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -12059,9 +12276,12 @@
       <c r="V44" s="10">
         <v>14</v>
       </c>
+      <c r="W44" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A45" s="31"/>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A45" s="34"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -12125,9 +12345,12 @@
       <c r="V45" s="10">
         <v>17</v>
       </c>
+      <c r="W45" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A46" s="32" t="s">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A46" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -12193,9 +12416,12 @@
       <c r="V46" s="10">
         <v>2</v>
       </c>
+      <c r="W46" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A47" s="33"/>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A47" s="30"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -12259,9 +12485,12 @@
       <c r="V47" s="10">
         <v>0</v>
       </c>
+      <c r="W47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A48" s="33"/>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A48" s="30"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -12325,9 +12554,12 @@
       <c r="V48" s="10">
         <v>1</v>
       </c>
+      <c r="W48" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A49" s="34"/>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A49" s="31"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -12391,9 +12623,12 @@
       <c r="V49" s="10">
         <v>4</v>
       </c>
+      <c r="W49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A50" s="29" t="s">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A50" s="32" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -12459,9 +12694,12 @@
       <c r="V50" s="10">
         <v>15</v>
       </c>
+      <c r="W50" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A51" s="31"/>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A51" s="34"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -12525,9 +12763,12 @@
       <c r="V51" s="10">
         <v>4</v>
       </c>
+      <c r="W51" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A52" s="32" t="s">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A52" s="29" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -12593,9 +12834,12 @@
       <c r="V52" s="10">
         <v>946</v>
       </c>
+      <c r="W52" s="10">
+        <v>1008</v>
+      </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A53" s="33"/>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A53" s="30"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -12659,9 +12903,12 @@
       <c r="V53" s="10">
         <v>1</v>
       </c>
+      <c r="W53" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A54" s="34"/>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A54" s="31"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -12725,8 +12972,11 @@
       <c r="V54" s="10">
         <v>0</v>
       </c>
+      <c r="W54" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -12793,8 +13043,11 @@
       <c r="V55" s="10">
         <v>64</v>
       </c>
+      <c r="W55" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -12861,9 +13114,12 @@
       <c r="V56" s="10">
         <v>368</v>
       </c>
+      <c r="W56" s="10">
+        <v>379</v>
+      </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A57" s="29" t="s">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A57" s="32" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -12929,9 +13185,12 @@
       <c r="V57" s="10">
         <v>6</v>
       </c>
+      <c r="W57" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A58" s="30"/>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A58" s="33"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -12995,9 +13254,12 @@
       <c r="V58" s="10">
         <v>3</v>
       </c>
+      <c r="W58" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A59" s="30"/>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A59" s="33"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -13061,9 +13323,12 @@
       <c r="V59" s="10">
         <v>8</v>
       </c>
+      <c r="W59" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A60" s="31"/>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A60" s="34"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -13127,9 +13392,12 @@
       <c r="V60" s="10">
         <v>0</v>
       </c>
+      <c r="W60" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A61" s="32" t="s">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A61" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -13195,9 +13463,12 @@
       <c r="V61" s="10">
         <v>3</v>
       </c>
+      <c r="W61" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A62" s="33"/>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A62" s="30"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -13261,9 +13532,12 @@
       <c r="V62" s="10">
         <v>63</v>
       </c>
+      <c r="W62" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A63" s="33"/>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A63" s="30"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -13327,9 +13601,12 @@
       <c r="V63" s="10">
         <v>6</v>
       </c>
+      <c r="W63" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A64" s="33"/>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A64" s="30"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -13393,9 +13670,12 @@
       <c r="V64" s="10">
         <v>16</v>
       </c>
+      <c r="W64" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A65" s="33"/>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A65" s="30"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -13459,9 +13739,12 @@
       <c r="V65" s="10">
         <v>15</v>
       </c>
+      <c r="W65" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A66" s="34"/>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A66" s="31"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -13525,8 +13808,11 @@
       <c r="V66" s="10">
         <v>19</v>
       </c>
+      <c r="W66" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -13593,9 +13879,12 @@
       <c r="V67" s="10">
         <v>296</v>
       </c>
+      <c r="W67" s="10">
+        <v>309</v>
+      </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A68" s="32" t="s">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A68" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -13661,9 +13950,12 @@
       <c r="V68" s="10">
         <v>0</v>
       </c>
+      <c r="W68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A69" s="33"/>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A69" s="30"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -13727,9 +14019,12 @@
       <c r="V69" s="10">
         <v>3</v>
       </c>
+      <c r="W69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A70" s="33"/>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A70" s="30"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -13793,9 +14088,12 @@
       <c r="V70" s="10">
         <v>0</v>
       </c>
+      <c r="W70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A71" s="33"/>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A71" s="30"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -13859,9 +14157,12 @@
       <c r="V71" s="10">
         <v>9</v>
       </c>
+      <c r="W71" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A72" s="33"/>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A72" s="30"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -13925,9 +14226,12 @@
       <c r="V72" s="10">
         <v>24</v>
       </c>
+      <c r="W72" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A73" s="33"/>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A73" s="30"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -13991,9 +14295,12 @@
       <c r="V73" s="10">
         <v>7</v>
       </c>
+      <c r="W73" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A74" s="33"/>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A74" s="30"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -14057,9 +14364,12 @@
       <c r="V74" s="10">
         <v>1</v>
       </c>
+      <c r="W74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A75" s="34"/>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A75" s="31"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -14123,9 +14433,12 @@
       <c r="V75" s="10">
         <v>1</v>
       </c>
+      <c r="W75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A76" s="29" t="s">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A76" s="32" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -14191,9 +14504,12 @@
       <c r="V76" s="10">
         <v>1</v>
       </c>
+      <c r="W76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A77" s="30"/>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A77" s="33"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -14257,9 +14573,12 @@
       <c r="V77" s="10">
         <v>2</v>
       </c>
+      <c r="W77" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A78" s="30"/>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A78" s="33"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -14323,9 +14642,12 @@
       <c r="V78" s="10">
         <v>31</v>
       </c>
+      <c r="W78" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A79" s="30"/>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A79" s="33"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -14389,9 +14711,12 @@
       <c r="V79" s="10">
         <v>4</v>
       </c>
+      <c r="W79" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A80" s="31"/>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A80" s="34"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -14455,8 +14780,11 @@
       <c r="V80" s="10">
         <v>1</v>
       </c>
+      <c r="W80" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -14523,9 +14851,12 @@
       <c r="V81" s="10">
         <v>90</v>
       </c>
+      <c r="W81" s="10">
+        <v>90</v>
+      </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A82" s="29" t="s">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A82" s="32" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -14591,9 +14922,12 @@
       <c r="V82" s="10">
         <v>126</v>
       </c>
+      <c r="W82" s="10">
+        <v>126</v>
+      </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A83" s="30"/>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A83" s="33"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -14657,9 +14991,12 @@
       <c r="V83" s="10">
         <v>27</v>
       </c>
+      <c r="W83" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A84" s="30"/>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A84" s="33"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -14723,9 +15060,12 @@
       <c r="V84" s="10">
         <v>75</v>
       </c>
+      <c r="W84" s="10">
+        <v>78</v>
+      </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A85" s="30"/>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A85" s="33"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -14789,9 +15129,12 @@
       <c r="V85" s="10">
         <v>6</v>
       </c>
+      <c r="W85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A86" s="31"/>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A86" s="34"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -14855,9 +15198,12 @@
       <c r="V86" s="10">
         <v>17</v>
       </c>
+      <c r="W86" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A87" s="32" t="s">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A87" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -14923,9 +15269,12 @@
       <c r="V87" s="10">
         <v>9</v>
       </c>
+      <c r="W87" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A88" s="33"/>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A88" s="30"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -14989,9 +15338,12 @@
       <c r="V88" s="10">
         <v>14</v>
       </c>
+      <c r="W88" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A89" s="33"/>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A89" s="30"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -15055,9 +15407,12 @@
       <c r="V89" s="10">
         <v>2</v>
       </c>
+      <c r="W89" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A90" s="33"/>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A90" s="30"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -15121,9 +15476,12 @@
       <c r="V90" s="10">
         <v>8</v>
       </c>
+      <c r="W90" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A91" s="33"/>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A91" s="30"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -15187,9 +15545,12 @@
       <c r="V91" s="10">
         <v>3</v>
       </c>
+      <c r="W91" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A92" s="33"/>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A92" s="30"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -15253,9 +15614,12 @@
       <c r="V92" s="10">
         <v>4</v>
       </c>
+      <c r="W92" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A93" s="34"/>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A93" s="31"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -15319,9 +15683,12 @@
       <c r="V93" s="10">
         <v>8</v>
       </c>
+      <c r="W93" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A94" s="29" t="s">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A94" s="32" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -15387,9 +15754,12 @@
       <c r="V94" s="10">
         <v>4</v>
       </c>
+      <c r="W94" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A95" s="31"/>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A95" s="34"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -15453,8 +15823,11 @@
       <c r="V95" s="10">
         <v>20</v>
       </c>
+      <c r="W95" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -15521,9 +15894,12 @@
       <c r="V96" s="10">
         <v>49</v>
       </c>
+      <c r="W96" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A97" s="29" t="s">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A97" s="32" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -15589,9 +15965,12 @@
       <c r="V97" s="10">
         <v>390</v>
       </c>
+      <c r="W97" s="10">
+        <v>389</v>
+      </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A98" s="30"/>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A98" s="33"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -15655,9 +16034,12 @@
       <c r="V98" s="10">
         <v>34</v>
       </c>
+      <c r="W98" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A99" s="31"/>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A99" s="34"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -15721,9 +16103,12 @@
       <c r="V99" s="10">
         <v>10</v>
       </c>
+      <c r="W99" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A100" s="32" t="s">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A100" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -15789,9 +16174,12 @@
       <c r="V100" s="10">
         <v>6</v>
       </c>
+      <c r="W100" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A101" s="33"/>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A101" s="30"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -15855,9 +16243,12 @@
       <c r="V101" s="10">
         <v>13</v>
       </c>
+      <c r="W101" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A102" s="33"/>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A102" s="30"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -15921,9 +16312,12 @@
       <c r="V102" s="10">
         <v>47</v>
       </c>
+      <c r="W102" s="10">
+        <v>50</v>
+      </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A103" s="33"/>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A103" s="30"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -15987,9 +16381,12 @@
       <c r="V103" s="10">
         <v>67</v>
       </c>
+      <c r="W103" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A104" s="34"/>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A104" s="31"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -16053,9 +16450,12 @@
       <c r="V104" s="10">
         <v>11</v>
       </c>
+      <c r="W104" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A105" s="29" t="s">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A105" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -16121,9 +16521,12 @@
       <c r="V105" s="10">
         <v>17</v>
       </c>
+      <c r="W105" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A106" s="30"/>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A106" s="33"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -16187,9 +16590,12 @@
       <c r="V106" s="10">
         <v>25</v>
       </c>
+      <c r="W106" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A107" s="30"/>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A107" s="33"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -16253,9 +16659,12 @@
       <c r="V107" s="10">
         <v>6</v>
       </c>
+      <c r="W107" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A108" s="30"/>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A108" s="33"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -16319,9 +16728,12 @@
       <c r="V108" s="10">
         <v>13</v>
       </c>
+      <c r="W108" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A109" s="31"/>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A109" s="34"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -16385,8 +16797,11 @@
       <c r="V109" s="10">
         <v>1</v>
       </c>
+      <c r="W109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -16453,8 +16868,11 @@
       <c r="V110" s="10">
         <v>148</v>
       </c>
+      <c r="W110" s="10">
+        <v>154</v>
+      </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -16521,9 +16939,12 @@
       <c r="V111" s="10">
         <v>17</v>
       </c>
+      <c r="W111" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A112" s="32" t="s">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A112" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -16589,9 +17010,12 @@
       <c r="V112" s="10">
         <v>3</v>
       </c>
+      <c r="W112" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A113" s="33"/>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A113" s="30"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -16655,9 +17079,12 @@
       <c r="V113" s="10">
         <v>7</v>
       </c>
+      <c r="W113" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A114" s="34"/>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A114" s="31"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -16721,9 +17148,12 @@
       <c r="V114" s="10">
         <v>53</v>
       </c>
+      <c r="W114" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A115" s="29" t="s">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A115" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -16789,9 +17219,12 @@
       <c r="V115" s="10">
         <v>46</v>
       </c>
+      <c r="W115" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A116" s="30"/>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A116" s="33"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -16855,9 +17288,12 @@
       <c r="V116" s="10">
         <v>19</v>
       </c>
+      <c r="W116" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A117" s="30"/>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A117" s="33"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -16921,9 +17357,12 @@
       <c r="V117" s="10">
         <v>4</v>
       </c>
+      <c r="W117" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A118" s="30"/>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A118" s="33"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -16987,9 +17426,12 @@
       <c r="V118" s="10">
         <v>25</v>
       </c>
+      <c r="W118" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A119" s="30"/>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A119" s="33"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -17053,9 +17495,12 @@
       <c r="V119" s="10">
         <v>4</v>
       </c>
+      <c r="W119" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A120" s="31"/>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A120" s="34"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -17119,9 +17564,12 @@
       <c r="V120" s="10">
         <v>31</v>
       </c>
+      <c r="W120" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A121" s="32" t="s">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A121" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -17187,9 +17635,12 @@
       <c r="V121" s="10">
         <v>0</v>
       </c>
+      <c r="W121" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A122" s="33"/>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A122" s="30"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -17253,9 +17704,12 @@
       <c r="V122" s="10">
         <v>20</v>
       </c>
+      <c r="W122" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A123" s="33"/>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A123" s="30"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -17319,9 +17773,12 @@
       <c r="V123" s="10">
         <v>2</v>
       </c>
+      <c r="W123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A124" s="33"/>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A124" s="30"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -17385,9 +17842,12 @@
       <c r="V124" s="10">
         <v>2</v>
       </c>
+      <c r="W124" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A125" s="33"/>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A125" s="30"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -17451,9 +17911,12 @@
       <c r="V125" s="10">
         <v>1</v>
       </c>
+      <c r="W125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A126" s="33"/>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A126" s="30"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -17517,9 +17980,12 @@
       <c r="V126" s="10">
         <v>2</v>
       </c>
+      <c r="W126" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A127" s="33"/>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A127" s="30"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -17583,9 +18049,12 @@
       <c r="V127" s="10">
         <v>3</v>
       </c>
+      <c r="W127" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A128" s="33"/>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A128" s="30"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -17649,9 +18118,12 @@
       <c r="V128" s="10">
         <v>4</v>
       </c>
+      <c r="W128" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A129" s="33"/>
+    <row r="129" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A129" s="30"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -17715,9 +18187,12 @@
       <c r="V129" s="10">
         <v>5</v>
       </c>
+      <c r="W129" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A130" s="34"/>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A130" s="31"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -17781,8 +18256,11 @@
       <c r="V130" s="10">
         <v>8</v>
       </c>
+      <c r="W130" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -17849,9 +18327,12 @@
       <c r="V131" s="10">
         <v>236</v>
       </c>
+      <c r="W131" s="10">
+        <v>243</v>
+      </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A132" s="32" t="s">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A132" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -17917,9 +18398,12 @@
       <c r="V132" s="10">
         <v>14</v>
       </c>
+      <c r="W132" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A133" s="33"/>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A133" s="30"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -17983,9 +18467,12 @@
       <c r="V133" s="10">
         <v>8</v>
       </c>
+      <c r="W133" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A134" s="33"/>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A134" s="30"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -18049,9 +18536,12 @@
       <c r="V134" s="10">
         <v>0</v>
       </c>
+      <c r="W134" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A135" s="34"/>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A135" s="31"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -18115,9 +18605,12 @@
       <c r="V135" s="10">
         <v>0</v>
       </c>
+      <c r="W135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A136" s="29" t="s">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A136" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -18183,9 +18676,12 @@
       <c r="V136" s="10">
         <v>28</v>
       </c>
+      <c r="W136" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A137" s="30"/>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A137" s="33"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -18249,9 +18745,12 @@
       <c r="V137" s="10">
         <v>5</v>
       </c>
+      <c r="W137" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A138" s="30"/>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A138" s="33"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -18315,9 +18814,12 @@
       <c r="V138" s="10">
         <v>6</v>
       </c>
+      <c r="W138" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A139" s="31"/>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A139" s="34"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -18380,10 +18882,25 @@
       </c>
       <c r="V139" s="10">
         <v>40</v>
+      </c>
+      <c r="W139" s="10">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -18396,18 +18913,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -18498,7 +19003,7 @@
   </sheetPr>
   <dimension ref="A1:CC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
@@ -18638,7 +19143,7 @@
       </c>
       <c r="AE2" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.139767054908486</v>
       </c>
       <c r="AF2" s="19">
         <f t="shared" si="0"/>
@@ -19288,7 +19793,7 @@
       </c>
       <c r="AE4" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.0927835051546393</v>
       </c>
       <c r="AF4" s="10">
         <f t="shared" si="6"/>
@@ -19613,7 +20118,7 @@
       </c>
       <c r="AE6" s="12">
         <f>MAX(0, (dc!AE2-dc!AD2))</f>
-        <v>0</v>
+        <v>601</v>
       </c>
       <c r="AF6" s="12">
         <f>MAX(0, (dc!AF2-dc!AE2))</f>
@@ -19937,7 +20442,7 @@
       </c>
       <c r="AE7" s="12">
         <f>MAX(0, (dc!AE3-dc!AD3))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="AF7" s="12">
         <f>MAX(0, (dc!AF3-dc!AE3))</f>
@@ -20585,7 +21090,7 @@
       </c>
       <c r="AE9" s="12">
         <f>MAX(0, (dc!AE5-dc!AD5))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF9" s="12">
         <f>MAX(0, (dc!AF5-dc!AE5))</f>
@@ -21137,7 +21642,7 @@
       </c>
       <c r="AE11" s="10">
         <f>MAX(0,(dc!AE7-dc!AD7))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AF11" s="10">
         <f>MAX(0,(dc!AF7-dc!AE7))</f>
@@ -21444,7 +21949,7 @@
       </c>
       <c r="AE12" s="10">
         <f>MAX(0,(dc!AE8-dc!AD8))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AF12" s="10">
         <f>MAX(0,(dc!AF8-dc!AE8))</f>
@@ -21751,7 +22256,7 @@
       </c>
       <c r="AE13" s="10">
         <f>MAX(0,(dc!AE9-dc!AD9))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AF13" s="10">
         <f>MAX(0,(dc!AF9-dc!AE9))</f>
@@ -22058,7 +22563,7 @@
       </c>
       <c r="AE14" s="10">
         <f>MAX(0,(dc!AE10-dc!AD10))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF14" s="10">
         <f>MAX(0,(dc!AF10-dc!AE10))</f>
@@ -22365,7 +22870,7 @@
       </c>
       <c r="AE15" s="10">
         <f>MAX(0,(dc!AE11-dc!AD11))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AF15" s="10">
         <f>MAX(0,(dc!AF11-dc!AE11))</f>
@@ -22672,7 +23177,7 @@
       </c>
       <c r="AE16" s="10">
         <f>MAX(0,(dc!AE12-dc!AD12))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF16" s="10">
         <f>MAX(0,(dc!AF12-dc!AE12))</f>
@@ -22979,7 +23484,7 @@
       </c>
       <c r="AE17" s="10">
         <f>MAX(0,(dc!AE13-dc!AD13))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AF17" s="10">
         <f>MAX(0,(dc!AF13-dc!AE13))</f>
@@ -23286,7 +23791,7 @@
       </c>
       <c r="AE18" s="10">
         <f>MAX(0,(dc!AE14-dc!AD14))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AF18" s="10">
         <f>MAX(0,(dc!AF14-dc!AE14))</f>
@@ -23987,7 +24492,7 @@
       </c>
       <c r="T2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21.021377672209027</v>
       </c>
       <c r="U2" s="21">
         <f t="shared" si="0"/>
@@ -24260,7 +24765,7 @@
       </c>
       <c r="T3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28.436911487758948</v>
       </c>
       <c r="U3" s="21">
         <f t="shared" si="2"/>
@@ -24533,7 +25038,7 @@
       </c>
       <c r="T4" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.4613935969868175</v>
       </c>
       <c r="U4" s="21">
         <f t="shared" si="4"/>
@@ -24869,7 +25374,7 @@
       </c>
       <c r="T6" s="14">
         <f>MAX(0,(md!T2-md!S2)+(md!T3-md!S3))</f>
-        <v>0</v>
+        <v>2526</v>
       </c>
       <c r="U6" s="14">
         <f>MAX(0,(md!U2-md!T2)+(md!U3-md!T3))</f>
@@ -25141,7 +25646,7 @@
       </c>
       <c r="T7" s="14">
         <f>MAX(0,(md!T3-md!S3))</f>
-        <v>0</v>
+        <v>531</v>
       </c>
       <c r="U7" s="14">
         <f>MAX(0,(md!U3-md!T3))</f>
@@ -25413,7 +25918,7 @@
       </c>
       <c r="T8" s="14">
         <f>MAX(0,(md!T4-md!S4))</f>
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="U8" s="14">
         <f>MAX(0,(md!U4-md!T4))</f>
@@ -25685,7 +26190,7 @@
       </c>
       <c r="T9" s="14">
         <f>MAX(0,(md!T5-md!S5))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="U9" s="14">
         <f>MAX(0,(md!U5-md!T5))</f>
@@ -26171,7 +26676,7 @@
       </c>
       <c r="T11" s="14">
         <f>MAX(0,(md!T7-md!S7))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U11" s="14">
         <f>MAX(0,(md!U7-md!T7))</f>
@@ -26448,7 +26953,7 @@
       </c>
       <c r="T12" s="14">
         <f>MAX(0,(md!T9-md!S9))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="U12" s="14">
         <f>MAX(0,(md!U9-md!T9))</f>
@@ -26725,7 +27230,7 @@
       </c>
       <c r="T13" s="14">
         <f>MAX(0,(md!T9-md!S9))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="U13" s="14">
         <f>MAX(0,(md!U9-md!T9))</f>
@@ -27002,7 +27507,7 @@
       </c>
       <c r="T14" s="14">
         <f>MAX(0,(md!T10-md!S10))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="U14" s="14">
         <f>MAX(0,(md!U10-md!T10))</f>
@@ -27279,7 +27784,7 @@
       </c>
       <c r="T15" s="14">
         <f>MAX(0,(md!T11-md!S11))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U15" s="14">
         <f>MAX(0,(md!U11-md!T11))</f>
@@ -27556,7 +28061,7 @@
       </c>
       <c r="T16" s="14">
         <f>MAX(0,(md!T12-md!S12))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U16" s="14">
         <f>MAX(0,(md!U12-md!T12))</f>
@@ -27833,7 +28338,7 @@
       </c>
       <c r="T17" s="14">
         <f>MAX(0,(md!T13-md!S13))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="U17" s="14">
         <f>MAX(0,(md!U13-md!T13))</f>
@@ -28110,7 +28615,7 @@
       </c>
       <c r="T18" s="14">
         <f>MAX(0,(md!T14-md!S14))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U18" s="14">
         <f>MAX(0,(md!U14-md!T14))</f>
@@ -28387,7 +28892,7 @@
       </c>
       <c r="T19" s="14">
         <f>MAX(0,(md!T15-md!S15))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="U19" s="14">
         <f>MAX(0,(md!U15-md!T15))</f>
@@ -28664,7 +29169,7 @@
       </c>
       <c r="T20" s="14">
         <f>MAX(0,(md!T16-md!S16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" s="14">
         <f>MAX(0,(md!U16-md!T16))</f>
@@ -28941,7 +29446,7 @@
       </c>
       <c r="T21" s="14">
         <f>MAX(0,(md!T17-md!S17))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U21" s="14">
         <f>MAX(0,(md!U17-md!T17))</f>
@@ -29495,7 +30000,7 @@
       </c>
       <c r="T23" s="14">
         <f>MAX(0,(md!T19-md!S19))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U23" s="14">
         <f>MAX(0,(md!U19-md!T19))</f>
@@ -29772,7 +30277,7 @@
       </c>
       <c r="T24" s="14">
         <f>MAX(0,(md!T20-md!S20))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U24" s="14">
         <f>MAX(0,(md!U20-md!T20))</f>
@@ -30049,7 +30554,7 @@
       </c>
       <c r="T25" s="14">
         <f>MAX(0,(md!T21-md!S21))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25" s="14">
         <f>MAX(0,(md!U21-md!T21))</f>
@@ -30326,7 +30831,7 @@
       </c>
       <c r="T26" s="14">
         <f>MAX(0,(md!T22-md!S22))</f>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="U26" s="14">
         <f>MAX(0,(md!U22-md!T22))</f>
@@ -30603,7 +31108,7 @@
       </c>
       <c r="T27" s="14">
         <f>MAX(0,(md!T23-md!S23))</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="U27" s="14">
         <f>MAX(0,(md!U23-md!T23))</f>
@@ -31157,7 +31662,7 @@
       </c>
       <c r="T29" s="14">
         <f>MAX(0,(md!T25-md!S25))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U29" s="14">
         <f>MAX(0,(md!U25-md!T25))</f>
@@ -31711,7 +32216,7 @@
       </c>
       <c r="T31" s="14">
         <f>MAX(0,(md!T27-md!S27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31" s="14">
         <f>MAX(0,(md!U27-md!T27))</f>
@@ -31988,7 +32493,7 @@
       </c>
       <c r="T32" s="14">
         <f>MAX(0,(md!T28-md!S28))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U32" s="14">
         <f>MAX(0,(md!U28-md!T28))</f>
@@ -32265,7 +32770,7 @@
       </c>
       <c r="T33" s="14">
         <f>MAX(0,(md!T29-md!S29))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U33" s="14">
         <f>MAX(0,(md!U29-md!T29))</f>
@@ -32542,7 +33047,7 @@
       </c>
       <c r="T34" s="14">
         <f>MAX(0,(md!T30-md!S30))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34" s="14">
         <f>MAX(0,(md!U30-md!T30))</f>
@@ -33021,7 +33526,7 @@
       </c>
       <c r="V2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.9194360523665654</v>
       </c>
       <c r="W2" s="20">
         <f t="shared" si="0"/>
@@ -33298,7 +33803,7 @@
       </c>
       <c r="V3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17.766497461928935</v>
       </c>
       <c r="W3" s="20">
         <f t="shared" si="2"/>
@@ -33575,7 +34080,7 @@
       </c>
       <c r="V4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.5837563451776653</v>
       </c>
       <c r="W4" s="20">
         <f t="shared" si="4"/>
@@ -33852,7 +34357,7 @@
       </c>
       <c r="V6" s="14">
         <f>MAX(0,(va!W5-va!V5))</f>
-        <v>0</v>
+        <v>1986</v>
       </c>
       <c r="W6" s="14">
         <f>MAX(0,(va!X5-va!W5))</f>
@@ -34129,7 +34634,7 @@
       </c>
       <c r="V7" s="14">
         <f>MAX(0,(va!W2-va!V2))</f>
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="W7" s="14">
         <f>MAX(0,(va!X2-va!W2))</f>
@@ -34406,7 +34911,7 @@
       </c>
       <c r="V8" s="14">
         <f>MAX(0,(va!W3-va!V3))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="W8" s="14">
         <f>MAX(0,(va!X3-va!W3))</f>
@@ -34683,7 +35188,7 @@
       </c>
       <c r="V9" s="14">
         <f>MAX(0,(va!W4-va!V4))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="W9" s="14">
         <f>MAX(0,(va!X4-va!W4))</f>
@@ -35180,7 +35685,7 @@
       </c>
       <c r="V11" s="16">
         <f>MAX(0,(va!W7-va!V7))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W11" s="16">
         <f>MAX(0,(va!X7-va!W7))</f>
@@ -35744,7 +36249,7 @@
       </c>
       <c r="V13" s="16">
         <f>MAX(0,(va!W9-va!V9))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="16">
         <f>MAX(0,(va!X9-va!W9))</f>
@@ -36308,7 +36813,7 @@
       </c>
       <c r="V15" s="16">
         <f>MAX(0,(va!W11-va!V11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" s="16">
         <f>MAX(0,(va!X11-va!W11))</f>
@@ -37154,7 +37659,7 @@
       </c>
       <c r="V18" s="16">
         <f>MAX(0,(va!W14-va!V14))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="W18" s="16">
         <f>MAX(0,(va!X14-va!W14))</f>
@@ -39128,7 +39633,7 @@
       </c>
       <c r="V25" s="16">
         <f>MAX(0,(va!W21-va!V21))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W25" s="16">
         <f>MAX(0,(va!X21-va!W21))</f>
@@ -41666,7 +42171,7 @@
       </c>
       <c r="V34" s="16">
         <f>MAX(0,(va!W30-va!V30))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W34" s="16">
         <f>MAX(0,(va!X30-va!W30))</f>
@@ -41948,7 +42453,7 @@
       </c>
       <c r="V35" s="16">
         <f>MAX(0,(va!W31-va!V31))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W35" s="16">
         <f>MAX(0,(va!X31-va!W31))</f>
@@ -42794,7 +43299,7 @@
       </c>
       <c r="V38" s="16">
         <f>MAX(0,(va!W34-va!V34))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W38" s="16">
         <f>MAX(0,(va!X34-va!W34))</f>
@@ -43076,7 +43581,7 @@
       </c>
       <c r="V39" s="16">
         <f>MAX(0,(va!W35-va!V35))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W39" s="16">
         <f>MAX(0,(va!X35-va!W35))</f>
@@ -47870,7 +48375,7 @@
       </c>
       <c r="V56" s="16">
         <f>MAX(0,(va!W52-va!V52))</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="W56" s="16">
         <f>MAX(0,(va!X52-va!W52))</f>
@@ -48434,7 +48939,7 @@
       </c>
       <c r="V58" s="16">
         <f>MAX(0,(va!W54-va!V54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W58" s="16">
         <f>MAX(0,(va!X54-va!W54))</f>
@@ -48716,7 +49221,7 @@
       </c>
       <c r="V59" s="16">
         <f>MAX(0,(va!W55-va!V55))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W59" s="16">
         <f>MAX(0,(va!X55-va!W55))</f>
@@ -48998,7 +49503,7 @@
       </c>
       <c r="V60" s="16">
         <f>MAX(0,(va!W56-va!V56))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="W60" s="16">
         <f>MAX(0,(va!X56-va!W56))</f>
@@ -50690,7 +51195,7 @@
       </c>
       <c r="V66" s="16">
         <f>MAX(0,(va!W62-va!V62))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W66" s="16">
         <f>MAX(0,(va!X62-va!W62))</f>
@@ -51254,7 +51759,7 @@
       </c>
       <c r="V68" s="16">
         <f>MAX(0,(va!W64-va!V64))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W68" s="16">
         <f>MAX(0,(va!X64-va!W64))</f>
@@ -52100,7 +52605,7 @@
       </c>
       <c r="V71" s="16">
         <f>MAX(0,(va!W67-va!V67))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="W71" s="16">
         <f>MAX(0,(va!X67-va!W67))</f>
@@ -54920,7 +55425,7 @@
       </c>
       <c r="V81" s="16">
         <f>MAX(0,(va!W77-va!V77))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W81" s="16">
         <f>MAX(0,(va!X77-va!W77))</f>
@@ -55202,7 +55707,7 @@
       </c>
       <c r="V82" s="16">
         <f>MAX(0,(va!W78-va!V78))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W82" s="16">
         <f>MAX(0,(va!X78-va!W78))</f>
@@ -56612,7 +57117,7 @@
       </c>
       <c r="V87" s="16">
         <f>MAX(0,(va!W83-va!V83))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W87" s="16">
         <f>MAX(0,(va!X83-va!W83))</f>
@@ -56894,7 +57399,7 @@
       </c>
       <c r="V88" s="16">
         <f>MAX(0,(va!W84-va!V84))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W88" s="16">
         <f>MAX(0,(va!X84-va!W84))</f>
@@ -58304,7 +58809,7 @@
       </c>
       <c r="V93" s="16">
         <f>MAX(0,(va!W89-va!V89))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W93" s="16">
         <f>MAX(0,(va!X89-va!W89))</f>
@@ -59150,7 +59655,7 @@
       </c>
       <c r="V96" s="16">
         <f>MAX(0,(va!W92-va!V92))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W96" s="16">
         <f>MAX(0,(va!X92-va!W92))</f>
@@ -59432,7 +59937,7 @@
       </c>
       <c r="V97" s="16">
         <f>MAX(0,(va!W93-va!V93))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W97" s="16">
         <f>MAX(0,(va!X93-va!W93))</f>
@@ -60278,7 +60783,7 @@
       </c>
       <c r="V100" s="16">
         <f>MAX(0,(va!W96-va!V96))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W100" s="16">
         <f>MAX(0,(va!X96-va!W96))</f>
@@ -61688,7 +62193,7 @@
       </c>
       <c r="V105" s="16">
         <f>MAX(0,(va!W101-va!V101))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W105" s="16">
         <f>MAX(0,(va!X101-va!W101))</f>
@@ -61970,7 +62475,7 @@
       </c>
       <c r="V106" s="16">
         <f>MAX(0,(va!W102-va!V102))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W106" s="16">
         <f>MAX(0,(va!X102-va!W102))</f>
@@ -62252,7 +62757,7 @@
       </c>
       <c r="V107" s="16">
         <f>MAX(0,(va!W103-va!V103))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W107" s="16">
         <f>MAX(0,(va!X103-va!W103))</f>
@@ -62534,7 +63039,7 @@
       </c>
       <c r="V108" s="16">
         <f>MAX(0,(va!W104-va!V104))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W108" s="16">
         <f>MAX(0,(va!X104-va!W104))</f>
@@ -62816,7 +63321,7 @@
       </c>
       <c r="V109" s="16">
         <f>MAX(0,(va!W105-va!V105))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W109" s="16">
         <f>MAX(0,(va!X105-va!W105))</f>
@@ -64226,7 +64731,7 @@
       </c>
       <c r="V114" s="16">
         <f>MAX(0,(va!W110-va!V110))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W114" s="16">
         <f>MAX(0,(va!X110-va!W110))</f>
@@ -64508,7 +65013,7 @@
       </c>
       <c r="V115" s="16">
         <f>MAX(0,(va!W111-va!V111))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W115" s="16">
         <f>MAX(0,(va!X111-va!W111))</f>
@@ -65354,7 +65859,7 @@
       </c>
       <c r="V118" s="16">
         <f>MAX(0,(va!W114-va!V114))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W118" s="16">
         <f>MAX(0,(va!X114-va!W114))</f>
@@ -65918,7 +66423,7 @@
       </c>
       <c r="V120" s="16">
         <f>MAX(0,(va!W116-va!V116))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W120" s="16">
         <f>MAX(0,(va!X116-va!W116))</f>
@@ -66764,7 +67269,7 @@
       </c>
       <c r="V123" s="16">
         <f>MAX(0,(va!W119-va!V119))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W123" s="16">
         <f>MAX(0,(va!X119-va!W119))</f>
@@ -70148,7 +70653,7 @@
       </c>
       <c r="V135" s="16">
         <f>MAX(0,(va!W131-va!V131))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="W135" s="16">
         <f>MAX(0,(va!X131-va!W131))</f>
@@ -71558,7 +72063,7 @@
       </c>
       <c r="V140" s="16">
         <f>MAX(0,(va!W136-va!V136))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W140" s="16">
         <f>MAX(0,(va!X136-va!W136))</f>
@@ -72404,7 +72909,7 @@
       </c>
       <c r="V143" s="16">
         <f>MAX(0,(va!W139-va!V139))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W143" s="16">
         <f>MAX(0,(va!X139-va!W139))</f>

</xml_diff>

<commit_message>
13 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B47491-BFBD-42AA-ACBF-185CA19C1E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E8756-744F-4CF3-810D-F366AD1A6F2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="4980" windowWidth="20520" windowHeight="13130" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="6780" yWindow="4980" windowWidth="20520" windowHeight="13130" tabRatio="685" activeTab="2" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="md_delta" sheetId="10" r:id="rId5"/>
     <sheet name="va_delta" sheetId="11" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">va!$D$1:$BT$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1060,6 +1063,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1069,16 +1082,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4019,8 +4022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E207B2A-317D-4660-A7D7-5B9F35994222}">
   <dimension ref="A1:CC46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4130,6 +4133,9 @@
       <c r="AE2" s="12">
         <v>10640</v>
       </c>
+      <c r="AF2" s="12">
+        <v>10934</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -4242,7 +4248,7 @@
       </c>
       <c r="AF3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1955</v>
       </c>
       <c r="AG3" s="10">
         <f t="shared" si="0"/>
@@ -4540,6 +4546,9 @@
       <c r="AE5" s="10">
         <v>50</v>
       </c>
+      <c r="AF5" s="10">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -4635,7 +4644,7 @@
       <c r="AE6" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" s="18" t="s">
         <v>196</v>
       </c>
       <c r="AG6" s="3" t="s">
@@ -4877,8 +4886,11 @@
       <c r="AD7" s="10">
         <v>202</v>
       </c>
-      <c r="AE7" s="35">
+      <c r="AE7" s="29">
         <v>218</v>
+      </c>
+      <c r="AF7" s="10">
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.35">
@@ -4972,8 +4984,11 @@
       <c r="AD8" s="10">
         <v>151</v>
       </c>
-      <c r="AE8" s="35">
+      <c r="AE8" s="29">
         <v>160</v>
+      </c>
+      <c r="AF8" s="10">
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.35">
@@ -5067,8 +5082,11 @@
       <c r="AD9" s="10">
         <v>139</v>
       </c>
-      <c r="AE9" s="35">
+      <c r="AE9" s="29">
         <v>143</v>
+      </c>
+      <c r="AF9" s="10">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.35">
@@ -5162,8 +5180,11 @@
       <c r="AD10" s="10">
         <v>288</v>
       </c>
-      <c r="AE10" s="35">
+      <c r="AE10" s="29">
         <v>303</v>
+      </c>
+      <c r="AF10" s="10">
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.35">
@@ -5257,8 +5278,11 @@
       <c r="AD11" s="10">
         <v>231</v>
       </c>
-      <c r="AE11" s="35">
+      <c r="AE11" s="29">
         <v>250</v>
+      </c>
+      <c r="AF11" s="10">
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.35">
@@ -5352,8 +5376,11 @@
       <c r="AD12" s="10">
         <v>266</v>
       </c>
-      <c r="AE12" s="35">
+      <c r="AE12" s="29">
         <v>281</v>
+      </c>
+      <c r="AF12" s="10">
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.35">
@@ -5447,8 +5474,11 @@
       <c r="AD13" s="10">
         <v>266</v>
       </c>
-      <c r="AE13" s="35">
+      <c r="AE13" s="29">
         <v>284</v>
+      </c>
+      <c r="AF13" s="10">
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.35">
@@ -5542,8 +5572,11 @@
       <c r="AD14" s="10">
         <v>202</v>
       </c>
-      <c r="AE14" s="35">
+      <c r="AE14" s="29">
         <v>218</v>
+      </c>
+      <c r="AF14" s="10">
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.35">
@@ -5637,8 +5670,11 @@
       <c r="AD15" s="10">
         <v>33</v>
       </c>
-      <c r="AE15" s="35">
+      <c r="AE15" s="29">
         <v>18</v>
+      </c>
+      <c r="AF15" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.35">
@@ -5794,7 +5830,7 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5872,7 +5908,7 @@
         <v>41539</v>
       </c>
       <c r="U2" s="10">
-        <v>0</v>
+        <v>42815</v>
       </c>
       <c r="V2" s="10">
         <v>0</v>
@@ -6096,7 +6132,7 @@
       </c>
       <c r="U3" s="10">
         <f>SUM(md[13-Apr])</f>
-        <v>0</v>
+        <v>8936</v>
       </c>
       <c r="V3" s="10">
         <f>SUM(md[14-Apr])</f>
@@ -6350,7 +6386,7 @@
         <v>1860</v>
       </c>
       <c r="U4" s="10">
-        <v>0</v>
+        <v>1975</v>
       </c>
       <c r="V4" s="10">
         <v>0</v>
@@ -6556,7 +6592,7 @@
         <v>235</v>
       </c>
       <c r="U5" s="10">
-        <v>0</v>
+        <v>262</v>
       </c>
       <c r="V5" s="10">
         <v>0</v>
@@ -6764,7 +6800,7 @@
       <c r="T6" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U6" s="18" t="s">
         <v>197</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -6973,6 +7009,9 @@
       <c r="T7">
         <v>13</v>
       </c>
+      <c r="U7">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -7035,6 +7074,9 @@
       <c r="T8" s="10">
         <v>659</v>
       </c>
+      <c r="U8" s="10">
+        <v>724</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -7097,6 +7139,9 @@
       <c r="T9">
         <v>812</v>
       </c>
+      <c r="U9">
+        <v>873</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -7159,6 +7204,9 @@
       <c r="T10">
         <v>1257</v>
       </c>
+      <c r="U10">
+        <v>1361</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -7221,6 +7269,9 @@
       <c r="T11">
         <v>90</v>
       </c>
+      <c r="U11">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -7283,6 +7334,9 @@
       <c r="T12">
         <v>17</v>
       </c>
+      <c r="U12">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -7345,6 +7399,9 @@
       <c r="T13">
         <v>236</v>
       </c>
+      <c r="U13">
+        <v>250</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -7407,6 +7464,9 @@
       <c r="T14">
         <v>74</v>
       </c>
+      <c r="U14">
+        <v>83</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -7469,6 +7529,9 @@
       <c r="T15">
         <v>253</v>
       </c>
+      <c r="U15">
+        <v>274</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -7531,8 +7594,11 @@
       <c r="T16" s="10">
         <v>9</v>
       </c>
+      <c r="U16" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -7593,8 +7659,11 @@
       <c r="T17">
         <v>368</v>
       </c>
+      <c r="U17">
+        <v>417</v>
+      </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -7655,8 +7724,11 @@
       <c r="T18">
         <v>4</v>
       </c>
+      <c r="U18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -7717,8 +7789,11 @@
       <c r="T19">
         <v>129</v>
       </c>
+      <c r="U19">
+        <v>142</v>
+      </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -7779,8 +7854,11 @@
       <c r="T20">
         <v>371</v>
       </c>
+      <c r="U20">
+        <v>386</v>
+      </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -7841,8 +7919,11 @@
       <c r="T21">
         <v>11</v>
       </c>
+      <c r="U21">
+        <v>11</v>
+      </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -7903,8 +7984,11 @@
       <c r="T22">
         <v>1631</v>
       </c>
+      <c r="U22">
+        <v>1756</v>
+      </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -7965,8 +8049,11 @@
       <c r="T23">
         <v>2035</v>
       </c>
+      <c r="U23">
+        <v>2205</v>
+      </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -8027,8 +8114,11 @@
       <c r="T24">
         <v>19</v>
       </c>
+      <c r="U24">
+        <v>19</v>
+      </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -8089,8 +8179,11 @@
       <c r="T25">
         <v>82</v>
       </c>
+      <c r="U25">
+        <v>95</v>
+      </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -8151,8 +8244,11 @@
       <c r="T26">
         <v>4</v>
       </c>
+      <c r="U26">
+        <v>6</v>
+      </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -8213,8 +8309,11 @@
       <c r="T27">
         <v>14</v>
       </c>
+      <c r="U27">
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -8275,8 +8374,11 @@
       <c r="T28">
         <v>75</v>
       </c>
+      <c r="U28">
+        <v>93</v>
+      </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -8337,8 +8439,11 @@
       <c r="T29">
         <v>42</v>
       </c>
+      <c r="U29">
+        <v>58</v>
+      </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -8399,8 +8504,11 @@
       <c r="T30">
         <v>20</v>
       </c>
+      <c r="U30">
+        <v>21</v>
+      </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -8493,8 +8601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289E8C7D-3613-4740-9288-5737AAA9BBA1}">
   <dimension ref="A1:BT139"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8600,7 +8708,7 @@
       </c>
       <c r="X2" s="10">
         <f>SUM(va[13-Apr])</f>
-        <v>0</v>
+        <v>5747</v>
       </c>
       <c r="Y2" s="10">
         <f>SUM(va[14-Apr])</f>
@@ -8857,7 +8965,7 @@
         <v>872</v>
       </c>
       <c r="X3" s="10">
-        <v>0</v>
+        <v>903</v>
       </c>
       <c r="Y3" s="10">
         <v>0</v>
@@ -9066,7 +9174,7 @@
         <v>141</v>
       </c>
       <c r="X4" s="10">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="Y4" s="10">
         <v>0</v>
@@ -9275,7 +9383,7 @@
         <v>39985</v>
       </c>
       <c r="X5" s="10">
-        <v>0</v>
+        <v>41401</v>
       </c>
       <c r="Y5" s="10">
         <v>0</v>
@@ -9492,7 +9600,7 @@
       <c r="W6" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="X6" s="18" t="s">
         <v>197</v>
       </c>
       <c r="Y6" s="3" t="s">
@@ -9710,9 +9818,12 @@
       <c r="W7" s="10">
         <v>198</v>
       </c>
+      <c r="X7" s="10">
+        <v>235</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -9781,9 +9892,12 @@
       <c r="W8" s="10">
         <v>4</v>
       </c>
+      <c r="X8" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -9850,9 +9964,12 @@
       <c r="W9" s="10">
         <v>23</v>
       </c>
+      <c r="X9" s="10">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A10" s="30"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -9919,9 +10036,12 @@
       <c r="W10" s="10">
         <v>2</v>
       </c>
+      <c r="X10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A11" s="30"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -9988,9 +10108,12 @@
       <c r="W11" s="10">
         <v>14</v>
       </c>
+      <c r="X11" s="10">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A12" s="30"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -10057,9 +10180,12 @@
       <c r="W12" s="10">
         <v>1</v>
       </c>
+      <c r="X12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -10124,6 +10250,9 @@
         <v>1</v>
       </c>
       <c r="W13" s="10">
+        <v>1</v>
+      </c>
+      <c r="X13" s="10">
         <v>1</v>
       </c>
     </row>
@@ -10197,9 +10326,12 @@
       <c r="W14" s="10">
         <v>366</v>
       </c>
+      <c r="X14" s="10">
+        <v>390</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -10268,9 +10400,12 @@
       <c r="W15" s="10">
         <v>17</v>
       </c>
+      <c r="X15" s="10">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A16" s="30"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -10337,9 +10472,12 @@
       <c r="W16" s="10">
         <v>0</v>
       </c>
+      <c r="X16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A17" s="30"/>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -10406,9 +10544,12 @@
       <c r="W17" s="10">
         <v>0</v>
       </c>
+      <c r="X17" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A18" s="30"/>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -10475,9 +10616,12 @@
       <c r="W18" s="10">
         <v>3</v>
       </c>
+      <c r="X18" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A19" s="30"/>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -10544,9 +10688,12 @@
       <c r="W19" s="10">
         <v>43</v>
       </c>
+      <c r="X19" s="10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A20" s="30"/>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -10613,9 +10760,12 @@
       <c r="W20" s="10">
         <v>4</v>
       </c>
+      <c r="X20" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -10682,9 +10832,12 @@
       <c r="W21" s="10">
         <v>81</v>
       </c>
+      <c r="X21" s="10">
+        <v>87</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A22" s="30"/>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -10751,9 +10904,12 @@
       <c r="W22" s="10">
         <v>3</v>
       </c>
+      <c r="X22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A23" s="30"/>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -10820,9 +10976,12 @@
       <c r="W23" s="10">
         <v>1</v>
       </c>
+      <c r="X23" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -10889,9 +11048,12 @@
       <c r="W24" s="10">
         <v>5</v>
       </c>
+      <c r="X24" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A25" s="32" t="s">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -10960,9 +11122,12 @@
       <c r="W25" s="10">
         <v>10</v>
       </c>
+      <c r="X25" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A26" s="33"/>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -11029,9 +11194,12 @@
       <c r="W26" s="10">
         <v>7</v>
       </c>
+      <c r="X26" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A27" s="33"/>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -11098,9 +11266,12 @@
       <c r="W27" s="10">
         <v>15</v>
       </c>
+      <c r="X27" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -11167,9 +11338,12 @@
       <c r="W28" s="10">
         <v>9</v>
       </c>
+      <c r="X28" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A29" s="34"/>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -11236,8 +11410,11 @@
       <c r="W29" s="10">
         <v>31</v>
       </c>
+      <c r="X29" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -11307,9 +11484,12 @@
       <c r="W30" s="10">
         <v>121</v>
       </c>
+      <c r="X30" s="10">
+        <v>126</v>
+      </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A31" s="32" t="s">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -11378,9 +11558,12 @@
       <c r="W31" s="10">
         <v>209</v>
       </c>
+      <c r="X31" s="10">
+        <v>211</v>
+      </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A32" s="33"/>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -11447,9 +11630,12 @@
       <c r="W32" s="10">
         <v>5</v>
       </c>
+      <c r="X32" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A33" s="34"/>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -11516,9 +11702,12 @@
       <c r="W33" s="10">
         <v>6</v>
       </c>
+      <c r="X33" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A34" s="29" t="s">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -11587,9 +11776,12 @@
       <c r="W34" s="10">
         <v>9</v>
       </c>
+      <c r="X34" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -11656,9 +11848,12 @@
       <c r="W35" s="10">
         <v>32</v>
       </c>
+      <c r="X35" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A36" s="30"/>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -11725,9 +11920,12 @@
       <c r="W36" s="10">
         <v>38</v>
       </c>
+      <c r="X36" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A37" s="31"/>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -11794,9 +11992,12 @@
       <c r="W37" s="10">
         <v>12</v>
       </c>
+      <c r="X37" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A38" s="32" t="s">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -11865,9 +12066,12 @@
       <c r="W38" s="10">
         <v>6</v>
       </c>
+      <c r="X38" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A39" s="33"/>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -11934,9 +12138,12 @@
       <c r="W39" s="10">
         <v>8</v>
       </c>
+      <c r="X39" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A40" s="33"/>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -12003,9 +12210,12 @@
       <c r="W40" s="10">
         <v>26</v>
       </c>
+      <c r="X40" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A41" s="33"/>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -12072,9 +12282,12 @@
       <c r="W41" s="10">
         <v>3</v>
       </c>
+      <c r="X41" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A42" s="33"/>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -12141,9 +12354,12 @@
       <c r="W42" s="10">
         <v>8</v>
       </c>
+      <c r="X42" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A43" s="33"/>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -12210,9 +12426,12 @@
       <c r="W43" s="10">
         <v>7</v>
       </c>
+      <c r="X43" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A44" s="33"/>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -12279,9 +12498,12 @@
       <c r="W44" s="10">
         <v>14</v>
       </c>
+      <c r="X44" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A45" s="34"/>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -12348,9 +12570,12 @@
       <c r="W45" s="10">
         <v>17</v>
       </c>
+      <c r="X45" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A46" s="29" t="s">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -12419,9 +12644,12 @@
       <c r="W46" s="10">
         <v>2</v>
       </c>
+      <c r="X46" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A47" s="30"/>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -12488,9 +12716,12 @@
       <c r="W47" s="10">
         <v>0</v>
       </c>
+      <c r="X47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A48" s="30"/>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -12557,9 +12788,12 @@
       <c r="W48" s="10">
         <v>1</v>
       </c>
+      <c r="X48" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A49" s="31"/>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -12626,9 +12860,12 @@
       <c r="W49" s="10">
         <v>4</v>
       </c>
+      <c r="X49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A50" s="32" t="s">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -12697,9 +12934,12 @@
       <c r="W50" s="10">
         <v>15</v>
       </c>
+      <c r="X50" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A51" s="34"/>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -12766,9 +13006,12 @@
       <c r="W51" s="10">
         <v>4</v>
       </c>
+      <c r="X51" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A52" s="29" t="s">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -12837,9 +13080,12 @@
       <c r="W52" s="10">
         <v>1008</v>
       </c>
+      <c r="X52" s="10">
+        <v>1164</v>
+      </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A53" s="30"/>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -12906,9 +13152,12 @@
       <c r="W53" s="10">
         <v>1</v>
       </c>
+      <c r="X53" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A54" s="31"/>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -12975,8 +13224,11 @@
       <c r="W54" s="10">
         <v>2</v>
       </c>
+      <c r="X54" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -13046,8 +13298,11 @@
       <c r="W55" s="10">
         <v>65</v>
       </c>
+      <c r="X55" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -13117,9 +13372,12 @@
       <c r="W56" s="10">
         <v>379</v>
       </c>
+      <c r="X56" s="10">
+        <v>397</v>
+      </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A57" s="32" t="s">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -13188,9 +13446,12 @@
       <c r="W57" s="10">
         <v>6</v>
       </c>
+      <c r="X57" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A58" s="33"/>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -13257,9 +13518,12 @@
       <c r="W58" s="10">
         <v>3</v>
       </c>
+      <c r="X58" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A59" s="33"/>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -13326,9 +13590,12 @@
       <c r="W59" s="10">
         <v>8</v>
       </c>
+      <c r="X59" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A60" s="34"/>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -13395,9 +13662,12 @@
       <c r="W60" s="10">
         <v>0</v>
       </c>
+      <c r="X60" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A61" s="29" t="s">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -13466,9 +13736,12 @@
       <c r="W61" s="10">
         <v>3</v>
       </c>
+      <c r="X61" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A62" s="30"/>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -13535,9 +13808,12 @@
       <c r="W62" s="10">
         <v>65</v>
       </c>
+      <c r="X62" s="10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A63" s="30"/>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -13604,9 +13880,12 @@
       <c r="W63" s="10">
         <v>6</v>
       </c>
+      <c r="X63" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A64" s="30"/>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -13673,9 +13952,12 @@
       <c r="W64" s="10">
         <v>17</v>
       </c>
+      <c r="X64" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A65" s="30"/>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -13742,9 +14024,12 @@
       <c r="W65" s="10">
         <v>15</v>
       </c>
+      <c r="X65" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A66" s="31"/>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -13811,8 +14096,11 @@
       <c r="W66" s="10">
         <v>19</v>
       </c>
+      <c r="X66" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -13882,9 +14170,12 @@
       <c r="W67" s="10">
         <v>309</v>
       </c>
+      <c r="X67" s="10">
+        <v>324</v>
+      </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A68" s="29" t="s">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -13953,9 +14244,12 @@
       <c r="W68" s="10">
         <v>0</v>
       </c>
+      <c r="X68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A69" s="30"/>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -14022,9 +14316,12 @@
       <c r="W69" s="10">
         <v>3</v>
       </c>
+      <c r="X69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A70" s="30"/>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -14091,9 +14388,12 @@
       <c r="W70" s="10">
         <v>0</v>
       </c>
+      <c r="X70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A71" s="30"/>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -14160,9 +14460,12 @@
       <c r="W71" s="10">
         <v>9</v>
       </c>
+      <c r="X71" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A72" s="30"/>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -14229,9 +14532,12 @@
       <c r="W72" s="10">
         <v>24</v>
       </c>
+      <c r="X72" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A73" s="30"/>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -14298,9 +14604,12 @@
       <c r="W73" s="10">
         <v>7</v>
       </c>
+      <c r="X73" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A74" s="30"/>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -14367,9 +14676,12 @@
       <c r="W74" s="10">
         <v>1</v>
       </c>
+      <c r="X74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A75" s="31"/>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -14436,9 +14748,12 @@
       <c r="W75" s="10">
         <v>1</v>
       </c>
+      <c r="X75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A76" s="32" t="s">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -14507,9 +14822,12 @@
       <c r="W76" s="10">
         <v>1</v>
       </c>
+      <c r="X76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A77" s="33"/>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -14576,9 +14894,12 @@
       <c r="W77" s="10">
         <v>3</v>
       </c>
+      <c r="X77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A78" s="33"/>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -14645,9 +14966,12 @@
       <c r="W78" s="10">
         <v>32</v>
       </c>
+      <c r="X78" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A79" s="33"/>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -14714,9 +15038,12 @@
       <c r="W79" s="10">
         <v>4</v>
       </c>
+      <c r="X79" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A80" s="34"/>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -14783,8 +15110,11 @@
       <c r="W80" s="10">
         <v>1</v>
       </c>
+      <c r="X80" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -14854,9 +15184,12 @@
       <c r="W81" s="10">
         <v>90</v>
       </c>
+      <c r="X81" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A82" s="32" t="s">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -14925,9 +15258,12 @@
       <c r="W82" s="10">
         <v>126</v>
       </c>
+      <c r="X82" s="10">
+        <v>126</v>
+      </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A83" s="33"/>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -14994,9 +15330,12 @@
       <c r="W83" s="10">
         <v>29</v>
       </c>
+      <c r="X83" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A84" s="33"/>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -15063,9 +15402,12 @@
       <c r="W84" s="10">
         <v>78</v>
       </c>
+      <c r="X84" s="10">
+        <v>88</v>
+      </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A85" s="33"/>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -15132,9 +15474,12 @@
       <c r="W85" s="10">
         <v>6</v>
       </c>
+      <c r="X85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A86" s="34"/>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -15201,9 +15546,12 @@
       <c r="W86" s="10">
         <v>17</v>
       </c>
+      <c r="X86" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A87" s="29" t="s">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -15272,9 +15620,12 @@
       <c r="W87" s="10">
         <v>9</v>
       </c>
+      <c r="X87" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A88" s="30"/>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -15341,9 +15692,12 @@
       <c r="W88" s="10">
         <v>14</v>
       </c>
+      <c r="X88" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A89" s="30"/>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -15410,9 +15764,12 @@
       <c r="W89" s="10">
         <v>4</v>
       </c>
+      <c r="X89" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A90" s="30"/>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -15479,9 +15836,12 @@
       <c r="W90" s="10">
         <v>8</v>
       </c>
+      <c r="X90" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A91" s="30"/>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -15548,9 +15908,12 @@
       <c r="W91" s="10">
         <v>3</v>
       </c>
+      <c r="X91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A92" s="30"/>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -15617,9 +15980,12 @@
       <c r="W92" s="10">
         <v>5</v>
       </c>
+      <c r="X92" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A93" s="31"/>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -15686,9 +16052,12 @@
       <c r="W93" s="10">
         <v>9</v>
       </c>
+      <c r="X93" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A94" s="32" t="s">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -15757,9 +16126,12 @@
       <c r="W94" s="10">
         <v>4</v>
       </c>
+      <c r="X94" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A95" s="34"/>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -15826,8 +16198,11 @@
       <c r="W95" s="10">
         <v>20</v>
       </c>
+      <c r="X95" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -15897,9 +16272,12 @@
       <c r="W96" s="10">
         <v>51</v>
       </c>
+      <c r="X96" s="10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A97" s="32" t="s">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -15968,9 +16346,12 @@
       <c r="W97" s="10">
         <v>389</v>
       </c>
+      <c r="X97" s="10">
+        <v>434</v>
+      </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A98" s="33"/>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -16037,9 +16418,12 @@
       <c r="W98" s="10">
         <v>34</v>
       </c>
+      <c r="X98" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A99" s="34"/>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -16106,9 +16490,12 @@
       <c r="W99" s="10">
         <v>10</v>
       </c>
+      <c r="X99" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A100" s="29" t="s">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -16177,9 +16564,12 @@
       <c r="W100" s="10">
         <v>6</v>
       </c>
+      <c r="X100" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A101" s="30"/>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -16246,9 +16636,12 @@
       <c r="W101" s="10">
         <v>14</v>
       </c>
+      <c r="X101" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A102" s="30"/>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -16315,9 +16708,12 @@
       <c r="W102" s="10">
         <v>50</v>
       </c>
+      <c r="X102" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A103" s="30"/>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -16384,9 +16780,12 @@
       <c r="W103" s="10">
         <v>72</v>
       </c>
+      <c r="X103" s="10">
+        <v>87</v>
+      </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A104" s="31"/>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -16453,9 +16852,12 @@
       <c r="W104" s="10">
         <v>12</v>
       </c>
+      <c r="X104" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A105" s="32" t="s">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -16524,9 +16926,12 @@
       <c r="W105" s="10">
         <v>19</v>
       </c>
+      <c r="X105" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A106" s="33"/>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -16593,9 +16998,12 @@
       <c r="W106" s="10">
         <v>25</v>
       </c>
+      <c r="X106" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A107" s="33"/>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -16662,9 +17070,12 @@
       <c r="W107" s="10">
         <v>6</v>
       </c>
+      <c r="X107" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A108" s="33"/>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -16731,9 +17142,12 @@
       <c r="W108" s="10">
         <v>13</v>
       </c>
+      <c r="X108" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A109" s="34"/>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -16800,8 +17214,11 @@
       <c r="W109" s="10">
         <v>1</v>
       </c>
+      <c r="X109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -16871,8 +17288,11 @@
       <c r="W110" s="10">
         <v>154</v>
       </c>
+      <c r="X110" s="10">
+        <v>167</v>
+      </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -16942,9 +17362,12 @@
       <c r="W111" s="10">
         <v>20</v>
       </c>
+      <c r="X111" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A112" s="29" t="s">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -17013,9 +17436,12 @@
       <c r="W112" s="10">
         <v>3</v>
       </c>
+      <c r="X112" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A113" s="30"/>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -17082,9 +17508,12 @@
       <c r="W113" s="10">
         <v>7</v>
       </c>
+      <c r="X113" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A114" s="31"/>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -17151,9 +17580,12 @@
       <c r="W114" s="10">
         <v>55</v>
       </c>
+      <c r="X114" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A115" s="32" t="s">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -17222,9 +17654,12 @@
       <c r="W115" s="10">
         <v>46</v>
       </c>
+      <c r="X115" s="10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A116" s="33"/>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -17291,9 +17726,12 @@
       <c r="W116" s="10">
         <v>21</v>
       </c>
+      <c r="X116" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A117" s="33"/>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -17360,9 +17798,12 @@
       <c r="W117" s="10">
         <v>4</v>
       </c>
+      <c r="X117" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A118" s="33"/>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -17429,9 +17870,12 @@
       <c r="W118" s="10">
         <v>25</v>
       </c>
+      <c r="X118" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A119" s="33"/>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -17498,9 +17942,12 @@
       <c r="W119" s="10">
         <v>5</v>
       </c>
+      <c r="X119" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A120" s="34"/>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -17567,9 +18014,12 @@
       <c r="W120" s="10">
         <v>31</v>
       </c>
+      <c r="X120" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A121" s="29" t="s">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -17638,9 +18088,12 @@
       <c r="W121" s="10">
         <v>0</v>
       </c>
+      <c r="X121" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A122" s="30"/>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -17707,9 +18160,12 @@
       <c r="W122" s="10">
         <v>20</v>
       </c>
+      <c r="X122" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A123" s="30"/>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -17776,9 +18232,12 @@
       <c r="W123" s="10">
         <v>2</v>
       </c>
+      <c r="X123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A124" s="30"/>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -17845,9 +18304,12 @@
       <c r="W124" s="10">
         <v>2</v>
       </c>
+      <c r="X124" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A125" s="30"/>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -17914,9 +18376,12 @@
       <c r="W125" s="10">
         <v>1</v>
       </c>
+      <c r="X125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A126" s="30"/>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -17983,9 +18448,12 @@
       <c r="W126" s="10">
         <v>2</v>
       </c>
+      <c r="X126" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A127" s="30"/>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -18052,9 +18520,12 @@
       <c r="W127" s="10">
         <v>3</v>
       </c>
+      <c r="X127" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A128" s="30"/>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -18121,9 +18592,12 @@
       <c r="W128" s="10">
         <v>4</v>
       </c>
+      <c r="X128" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A129" s="30"/>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -18190,9 +18664,12 @@
       <c r="W129" s="10">
         <v>5</v>
       </c>
+      <c r="X129" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A130" s="31"/>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -18259,8 +18736,11 @@
       <c r="W130" s="10">
         <v>8</v>
       </c>
+      <c r="X130" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -18330,9 +18810,12 @@
       <c r="W131" s="10">
         <v>243</v>
       </c>
+      <c r="X131" s="10">
+        <v>251</v>
+      </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A132" s="29" t="s">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -18401,9 +18884,12 @@
       <c r="W132" s="10">
         <v>14</v>
       </c>
+      <c r="X132" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A133" s="30"/>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -18470,9 +18956,12 @@
       <c r="W133" s="10">
         <v>8</v>
       </c>
+      <c r="X133" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A134" s="30"/>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -18539,9 +19028,12 @@
       <c r="W134" s="10">
         <v>0</v>
       </c>
+      <c r="X134" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A135" s="31"/>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -18608,9 +19100,12 @@
       <c r="W135" s="10">
         <v>0</v>
       </c>
+      <c r="X135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A136" s="32" t="s">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -18679,9 +19174,12 @@
       <c r="W136" s="10">
         <v>31</v>
       </c>
+      <c r="X136" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A137" s="33"/>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -18748,9 +19246,12 @@
       <c r="W137" s="10">
         <v>5</v>
       </c>
+      <c r="X137" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A138" s="33"/>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -18817,9 +19318,12 @@
       <c r="W138" s="10">
         <v>6</v>
       </c>
+      <c r="X138" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A139" s="34"/>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -18885,10 +19389,25 @@
       </c>
       <c r="W139" s="10">
         <v>48</v>
+      </c>
+      <c r="X139" s="10">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -18901,18 +19420,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -19147,7 +19654,7 @@
       </c>
       <c r="AF2" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27.210884353741498</v>
       </c>
       <c r="AG2" s="19">
         <f t="shared" si="0"/>
@@ -19797,7 +20304,7 @@
       </c>
       <c r="AF4" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="AG4" s="10">
         <f t="shared" si="6"/>
@@ -20122,7 +20629,7 @@
       </c>
       <c r="AF6" s="12">
         <f>MAX(0, (dc!AF2-dc!AE2))</f>
-        <v>0</v>
+        <v>294</v>
       </c>
       <c r="AG6" s="12">
         <f>MAX(0, (dc!AG2-dc!AF2))</f>
@@ -20446,7 +20953,7 @@
       </c>
       <c r="AF7" s="12">
         <f>MAX(0, (dc!AF3-dc!AE3))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="AG7" s="12">
         <f>MAX(0, (dc!AG3-dc!AF3))</f>
@@ -21094,7 +21601,7 @@
       </c>
       <c r="AF9" s="12">
         <f>MAX(0, (dc!AF5-dc!AE5))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG9" s="12">
         <f>MAX(0, (dc!AG5-dc!AF5))</f>
@@ -21646,7 +22153,7 @@
       </c>
       <c r="AF11" s="10">
         <f>MAX(0,(dc!AF7-dc!AE7))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG11" s="10">
         <f>MAX(0,(dc!AG7-dc!AF7))</f>
@@ -21953,7 +22460,7 @@
       </c>
       <c r="AF12" s="10">
         <f>MAX(0,(dc!AF8-dc!AE8))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AG12" s="10">
         <f>MAX(0,(dc!AG8-dc!AF8))</f>
@@ -22260,7 +22767,7 @@
       </c>
       <c r="AF13" s="10">
         <f>MAX(0,(dc!AF9-dc!AE9))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG13" s="10">
         <f>MAX(0,(dc!AG9-dc!AF9))</f>
@@ -22567,7 +23074,7 @@
       </c>
       <c r="AF14" s="10">
         <f>MAX(0,(dc!AF10-dc!AE10))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AG14" s="10">
         <f>MAX(0,(dc!AG10-dc!AF10))</f>
@@ -22874,7 +23381,7 @@
       </c>
       <c r="AF15" s="10">
         <f>MAX(0,(dc!AF11-dc!AE11))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG15" s="10">
         <f>MAX(0,(dc!AG11-dc!AF11))</f>
@@ -23181,7 +23688,7 @@
       </c>
       <c r="AF16" s="10">
         <f>MAX(0,(dc!AF12-dc!AE12))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG16" s="10">
         <f>MAX(0,(dc!AG12-dc!AF12))</f>
@@ -23488,7 +23995,7 @@
       </c>
       <c r="AF17" s="10">
         <f>MAX(0,(dc!AF13-dc!AE13))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG17" s="10">
         <f>MAX(0,(dc!AG13-dc!AF13))</f>
@@ -23795,7 +24302,7 @@
       </c>
       <c r="AF18" s="10">
         <f>MAX(0,(dc!AF14-dc!AE14))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG18" s="10">
         <f>MAX(0,(dc!AG14-dc!AF14))</f>
@@ -24102,7 +24609,7 @@
       </c>
       <c r="AF19" s="10">
         <f>MAX(0,(dc!AF15-dc!AE15))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AG19" s="10">
         <f>MAX(0,(dc!AG15-dc!AF15))</f>
@@ -24496,7 +25003,7 @@
       </c>
       <c r="U2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35.782586814292905</v>
       </c>
       <c r="V2" s="21">
         <f t="shared" si="0"/>
@@ -24769,7 +25276,7 @@
       </c>
       <c r="U3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16.174402250351619</v>
       </c>
       <c r="V3" s="21">
         <f t="shared" si="2"/>
@@ -25042,7 +25549,7 @@
       </c>
       <c r="U4" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.79746835443038</v>
       </c>
       <c r="V4" s="21">
         <f t="shared" si="4"/>
@@ -25378,7 +25885,7 @@
       </c>
       <c r="U6" s="14">
         <f>MAX(0,(md!U2-md!T2)+(md!U3-md!T3))</f>
-        <v>0</v>
+        <v>1987</v>
       </c>
       <c r="V6" s="14">
         <f>MAX(0,(md!V2-md!U2)+(md!V3-md!U3))</f>
@@ -25650,7 +26157,7 @@
       </c>
       <c r="U7" s="14">
         <f>MAX(0,(md!U3-md!T3))</f>
-        <v>0</v>
+        <v>711</v>
       </c>
       <c r="V7" s="14">
         <f>MAX(0,(md!V3-md!U3))</f>
@@ -25922,7 +26429,7 @@
       </c>
       <c r="U8" s="14">
         <f>MAX(0,(md!U4-md!T4))</f>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="V8" s="14">
         <f>MAX(0,(md!V4-md!U4))</f>
@@ -26194,7 +26701,7 @@
       </c>
       <c r="U9" s="14">
         <f>MAX(0,(md!U5-md!T5))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V9" s="14">
         <f>MAX(0,(md!V5-md!U5))</f>
@@ -26680,7 +27187,7 @@
       </c>
       <c r="U11" s="14">
         <f>MAX(0,(md!U7-md!T7))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11" s="14">
         <f>MAX(0,(md!V7-md!U7))</f>
@@ -26957,7 +27464,7 @@
       </c>
       <c r="U12" s="14">
         <f>MAX(0,(md!U9-md!T9))</f>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="V12" s="14">
         <f>MAX(0,(md!V9-md!U9))</f>
@@ -27234,7 +27741,7 @@
       </c>
       <c r="U13" s="14">
         <f>MAX(0,(md!U9-md!T9))</f>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="V13" s="14">
         <f>MAX(0,(md!V9-md!U9))</f>
@@ -27511,7 +28018,7 @@
       </c>
       <c r="U14" s="14">
         <f>MAX(0,(md!U10-md!T10))</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="V14" s="14">
         <f>MAX(0,(md!V10-md!U10))</f>
@@ -27788,7 +28295,7 @@
       </c>
       <c r="U15" s="14">
         <f>MAX(0,(md!U11-md!T11))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V15" s="14">
         <f>MAX(0,(md!V11-md!U11))</f>
@@ -28065,7 +28572,7 @@
       </c>
       <c r="U16" s="14">
         <f>MAX(0,(md!U12-md!T12))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V16" s="14">
         <f>MAX(0,(md!V12-md!U12))</f>
@@ -28342,7 +28849,7 @@
       </c>
       <c r="U17" s="14">
         <f>MAX(0,(md!U13-md!T13))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="V17" s="14">
         <f>MAX(0,(md!V13-md!U13))</f>
@@ -28619,7 +29126,7 @@
       </c>
       <c r="U18" s="14">
         <f>MAX(0,(md!U14-md!T14))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V18" s="14">
         <f>MAX(0,(md!V14-md!U14))</f>
@@ -28896,7 +29403,7 @@
       </c>
       <c r="U19" s="14">
         <f>MAX(0,(md!U15-md!T15))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="V19" s="14">
         <f>MAX(0,(md!V15-md!U15))</f>
@@ -29173,7 +29680,7 @@
       </c>
       <c r="U20" s="14">
         <f>MAX(0,(md!U16-md!T16))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V20" s="14">
         <f>MAX(0,(md!V16-md!U16))</f>
@@ -29450,7 +29957,7 @@
       </c>
       <c r="U21" s="14">
         <f>MAX(0,(md!U17-md!T17))</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="V21" s="14">
         <f>MAX(0,(md!V17-md!U17))</f>
@@ -30004,7 +30511,7 @@
       </c>
       <c r="U23" s="14">
         <f>MAX(0,(md!U19-md!T19))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="V23" s="14">
         <f>MAX(0,(md!V19-md!U19))</f>
@@ -30281,7 +30788,7 @@
       </c>
       <c r="U24" s="14">
         <f>MAX(0,(md!U20-md!T20))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V24" s="14">
         <f>MAX(0,(md!V20-md!U20))</f>
@@ -30835,7 +31342,7 @@
       </c>
       <c r="U26" s="14">
         <f>MAX(0,(md!U22-md!T22))</f>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="V26" s="14">
         <f>MAX(0,(md!V22-md!U22))</f>
@@ -31112,7 +31619,7 @@
       </c>
       <c r="U27" s="14">
         <f>MAX(0,(md!U23-md!T23))</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V27" s="14">
         <f>MAX(0,(md!V23-md!U23))</f>
@@ -31666,7 +32173,7 @@
       </c>
       <c r="U29" s="14">
         <f>MAX(0,(md!U25-md!T25))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="V29" s="14">
         <f>MAX(0,(md!V25-md!U25))</f>
@@ -31943,7 +32450,7 @@
       </c>
       <c r="U30" s="14">
         <f>MAX(0,(md!U26-md!T26))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V30" s="14">
         <f>MAX(0,(md!V26-md!U26))</f>
@@ -32220,7 +32727,7 @@
       </c>
       <c r="U31" s="14">
         <f>MAX(0,(md!U27-md!T27))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V31" s="14">
         <f>MAX(0,(md!V27-md!U27))</f>
@@ -32497,7 +33004,7 @@
       </c>
       <c r="U32" s="14">
         <f>MAX(0,(md!U28-md!T28))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="V32" s="14">
         <f>MAX(0,(md!V28-md!U28))</f>
@@ -32774,7 +33281,7 @@
       </c>
       <c r="U33" s="14">
         <f>MAX(0,(md!U29-md!T29))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V33" s="14">
         <f>MAX(0,(md!V29-md!U29))</f>
@@ -33051,7 +33558,7 @@
       </c>
       <c r="U34" s="14">
         <f>MAX(0,(md!U30-md!T30))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V34" s="14">
         <f>MAX(0,(md!V30-md!U30))</f>
@@ -33530,7 +34037,7 @@
       </c>
       <c r="W2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33.403954802259889</v>
       </c>
       <c r="X2" s="20">
         <f t="shared" si="0"/>
@@ -33807,7 +34314,7 @@
       </c>
       <c r="W3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5539112050739963</v>
       </c>
       <c r="X3" s="20">
         <f t="shared" si="2"/>
@@ -34084,7 +34591,7 @@
       </c>
       <c r="W4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.6913319238900635</v>
       </c>
       <c r="X4" s="20">
         <f t="shared" si="4"/>
@@ -34361,7 +34868,7 @@
       </c>
       <c r="W6" s="14">
         <f>MAX(0,(va!X5-va!W5))</f>
-        <v>0</v>
+        <v>1416</v>
       </c>
       <c r="X6" s="14">
         <f>MAX(0,(va!Y5-va!X5))</f>
@@ -34638,7 +35145,7 @@
       </c>
       <c r="W7" s="14">
         <f>MAX(0,(va!X2-va!W2))</f>
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="X7" s="14">
         <f>MAX(0,(va!Y2-va!X2))</f>
@@ -34915,7 +35422,7 @@
       </c>
       <c r="W8" s="14">
         <f>MAX(0,(va!X3-va!W3))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="X8" s="14">
         <f>MAX(0,(va!Y3-va!X3))</f>
@@ -35192,7 +35699,7 @@
       </c>
       <c r="W9" s="14">
         <f>MAX(0,(va!X4-va!W4))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="14">
         <f>MAX(0,(va!Y4-va!X4))</f>
@@ -35689,7 +36196,7 @@
       </c>
       <c r="W11" s="16">
         <f>MAX(0,(va!X7-va!W7))</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="X11" s="16">
         <f>MAX(0,(va!Y7-va!X7))</f>
@@ -36253,7 +36760,7 @@
       </c>
       <c r="W13" s="16">
         <f>MAX(0,(va!X9-va!W9))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" s="16">
         <f>MAX(0,(va!Y9-va!X9))</f>
@@ -36817,7 +37324,7 @@
       </c>
       <c r="W15" s="16">
         <f>MAX(0,(va!X11-va!W11))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X15" s="16">
         <f>MAX(0,(va!Y11-va!X11))</f>
@@ -37663,7 +38170,7 @@
       </c>
       <c r="W18" s="16">
         <f>MAX(0,(va!X14-va!W14))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="X18" s="16">
         <f>MAX(0,(va!Y14-va!X14))</f>
@@ -39073,7 +39580,7 @@
       </c>
       <c r="W23" s="16">
         <f>MAX(0,(va!X19-va!W19))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X23" s="16">
         <f>MAX(0,(va!Y19-va!X19))</f>
@@ -39637,7 +40144,7 @@
       </c>
       <c r="W25" s="16">
         <f>MAX(0,(va!X21-va!W21))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X25" s="16">
         <f>MAX(0,(va!Y21-va!X21))</f>
@@ -40201,7 +40708,7 @@
       </c>
       <c r="W27" s="16">
         <f>MAX(0,(va!X23-va!W23))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X27" s="16">
         <f>MAX(0,(va!Y23-va!X23))</f>
@@ -40483,7 +40990,7 @@
       </c>
       <c r="W28" s="16">
         <f>MAX(0,(va!X24-va!W24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X28" s="16">
         <f>MAX(0,(va!Y24-va!X24))</f>
@@ -41329,7 +41836,7 @@
       </c>
       <c r="W31" s="16">
         <f>MAX(0,(va!X27-va!W27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X31" s="16">
         <f>MAX(0,(va!Y27-va!X27))</f>
@@ -41611,7 +42118,7 @@
       </c>
       <c r="W32" s="16">
         <f>MAX(0,(va!X28-va!W28))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X32" s="16">
         <f>MAX(0,(va!Y28-va!X28))</f>
@@ -41893,7 +42400,7 @@
       </c>
       <c r="W33" s="16">
         <f>MAX(0,(va!X29-va!W29))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X33" s="16">
         <f>MAX(0,(va!Y29-va!X29))</f>
@@ -42175,7 +42682,7 @@
       </c>
       <c r="W34" s="16">
         <f>MAX(0,(va!X30-va!W30))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X34" s="16">
         <f>MAX(0,(va!Y30-va!X30))</f>
@@ -42457,7 +42964,7 @@
       </c>
       <c r="W35" s="16">
         <f>MAX(0,(va!X31-va!W31))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X35" s="16">
         <f>MAX(0,(va!Y31-va!X31))</f>
@@ -43021,7 +43528,7 @@
       </c>
       <c r="W37" s="16">
         <f>MAX(0,(va!X33-va!W33))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X37" s="16">
         <f>MAX(0,(va!Y33-va!X33))</f>
@@ -43585,7 +44092,7 @@
       </c>
       <c r="W39" s="16">
         <f>MAX(0,(va!X35-va!W35))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X39" s="16">
         <f>MAX(0,(va!Y35-va!X35))</f>
@@ -43867,7 +44374,7 @@
       </c>
       <c r="W40" s="16">
         <f>MAX(0,(va!X36-va!W36))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X40" s="16">
         <f>MAX(0,(va!Y36-va!X36))</f>
@@ -44149,7 +44656,7 @@
       </c>
       <c r="W41" s="16">
         <f>MAX(0,(va!X37-va!W37))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X41" s="16">
         <f>MAX(0,(va!Y37-va!X37))</f>
@@ -44713,7 +45220,7 @@
       </c>
       <c r="W43" s="16">
         <f>MAX(0,(va!X39-va!W39))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X43" s="16">
         <f>MAX(0,(va!Y39-va!X39))</f>
@@ -44995,7 +45502,7 @@
       </c>
       <c r="W44" s="16">
         <f>MAX(0,(va!X40-va!W40))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X44" s="16">
         <f>MAX(0,(va!Y40-va!X40))</f>
@@ -46405,7 +46912,7 @@
       </c>
       <c r="W49" s="16">
         <f>MAX(0,(va!X45-va!W45))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X49" s="16">
         <f>MAX(0,(va!Y45-va!X45))</f>
@@ -48379,7 +48886,7 @@
       </c>
       <c r="W56" s="16">
         <f>MAX(0,(va!X52-va!W52))</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="X56" s="16">
         <f>MAX(0,(va!Y52-va!X52))</f>
@@ -49225,7 +49732,7 @@
       </c>
       <c r="W59" s="16">
         <f>MAX(0,(va!X55-va!W55))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="X59" s="16">
         <f>MAX(0,(va!Y55-va!X55))</f>
@@ -49507,7 +50014,7 @@
       </c>
       <c r="W60" s="16">
         <f>MAX(0,(va!X56-va!W56))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="X60" s="16">
         <f>MAX(0,(va!Y56-va!X56))</f>
@@ -49789,7 +50296,7 @@
       </c>
       <c r="W61" s="16">
         <f>MAX(0,(va!X57-va!W57))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X61" s="16">
         <f>MAX(0,(va!Y57-va!X57))</f>
@@ -50353,7 +50860,7 @@
       </c>
       <c r="W63" s="16">
         <f>MAX(0,(va!X59-va!W59))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X63" s="16">
         <f>MAX(0,(va!Y59-va!X59))</f>
@@ -51199,7 +51706,7 @@
       </c>
       <c r="W66" s="16">
         <f>MAX(0,(va!X62-va!W62))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X66" s="16">
         <f>MAX(0,(va!Y62-va!X62))</f>
@@ -52045,7 +52552,7 @@
       </c>
       <c r="W69" s="16">
         <f>MAX(0,(va!X65-va!W65))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X69" s="16">
         <f>MAX(0,(va!Y65-va!X65))</f>
@@ -52327,7 +52834,7 @@
       </c>
       <c r="W70" s="16">
         <f>MAX(0,(va!X66-va!W66))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X70" s="16">
         <f>MAX(0,(va!Y66-va!X66))</f>
@@ -52609,7 +53116,7 @@
       </c>
       <c r="W71" s="16">
         <f>MAX(0,(va!X67-va!W67))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="X71" s="16">
         <f>MAX(0,(va!Y67-va!X67))</f>
@@ -53737,7 +54244,7 @@
       </c>
       <c r="W75" s="16">
         <f>MAX(0,(va!X71-va!W71))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X75" s="16">
         <f>MAX(0,(va!Y71-va!X71))</f>
@@ -54019,7 +54526,7 @@
       </c>
       <c r="W76" s="16">
         <f>MAX(0,(va!X72-va!W72))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X76" s="16">
         <f>MAX(0,(va!Y72-va!X72))</f>
@@ -55429,7 +55936,7 @@
       </c>
       <c r="W81" s="16">
         <f>MAX(0,(va!X77-va!W77))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X81" s="16">
         <f>MAX(0,(va!Y77-va!X77))</f>
@@ -56557,7 +57064,7 @@
       </c>
       <c r="W85" s="16">
         <f>MAX(0,(va!X81-va!W81))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="X85" s="16">
         <f>MAX(0,(va!Y81-va!X81))</f>
@@ -57121,7 +57628,7 @@
       </c>
       <c r="W87" s="16">
         <f>MAX(0,(va!X83-va!W83))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X87" s="16">
         <f>MAX(0,(va!Y83-va!X83))</f>
@@ -57403,7 +57910,7 @@
       </c>
       <c r="W88" s="16">
         <f>MAX(0,(va!X84-va!W84))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X88" s="16">
         <f>MAX(0,(va!Y84-va!X84))</f>
@@ -57967,7 +58474,7 @@
       </c>
       <c r="W90" s="16">
         <f>MAX(0,(va!X86-va!W86))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X90" s="16">
         <f>MAX(0,(va!Y86-va!X86))</f>
@@ -58531,7 +59038,7 @@
       </c>
       <c r="W92" s="16">
         <f>MAX(0,(va!X88-va!W88))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X92" s="16">
         <f>MAX(0,(va!Y88-va!X88))</f>
@@ -59377,7 +59884,7 @@
       </c>
       <c r="W95" s="16">
         <f>MAX(0,(va!X91-va!W91))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X95" s="16">
         <f>MAX(0,(va!Y91-va!X91))</f>
@@ -59941,7 +60448,7 @@
       </c>
       <c r="W97" s="16">
         <f>MAX(0,(va!X93-va!W93))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X97" s="16">
         <f>MAX(0,(va!Y93-va!X93))</f>
@@ -60505,7 +61012,7 @@
       </c>
       <c r="W99" s="16">
         <f>MAX(0,(va!X95-va!W95))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X99" s="16">
         <f>MAX(0,(va!Y95-va!X95))</f>
@@ -60787,7 +61294,7 @@
       </c>
       <c r="W100" s="16">
         <f>MAX(0,(va!X96-va!W96))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X100" s="16">
         <f>MAX(0,(va!Y96-va!X96))</f>
@@ -61069,7 +61576,7 @@
       </c>
       <c r="W101" s="16">
         <f>MAX(0,(va!X97-va!W97))</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="X101" s="16">
         <f>MAX(0,(va!Y97-va!X97))</f>
@@ -61351,7 +61858,7 @@
       </c>
       <c r="W102" s="16">
         <f>MAX(0,(va!X98-va!W98))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="X102" s="16">
         <f>MAX(0,(va!Y98-va!X98))</f>
@@ -62479,7 +62986,7 @@
       </c>
       <c r="W106" s="16">
         <f>MAX(0,(va!X102-va!W102))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X106" s="16">
         <f>MAX(0,(va!Y102-va!X102))</f>
@@ -62761,7 +63268,7 @@
       </c>
       <c r="W107" s="16">
         <f>MAX(0,(va!X103-va!W103))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="X107" s="16">
         <f>MAX(0,(va!Y103-va!X103))</f>
@@ -63043,7 +63550,7 @@
       </c>
       <c r="W108" s="16">
         <f>MAX(0,(va!X104-va!W104))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X108" s="16">
         <f>MAX(0,(va!Y104-va!X104))</f>
@@ -63325,7 +63832,7 @@
       </c>
       <c r="W109" s="16">
         <f>MAX(0,(va!X105-va!W105))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X109" s="16">
         <f>MAX(0,(va!Y105-va!X105))</f>
@@ -63607,7 +64114,7 @@
       </c>
       <c r="W110" s="16">
         <f>MAX(0,(va!X106-va!W106))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X110" s="16">
         <f>MAX(0,(va!Y106-va!X106))</f>
@@ -64171,7 +64678,7 @@
       </c>
       <c r="W112" s="16">
         <f>MAX(0,(va!X108-va!W108))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X112" s="16">
         <f>MAX(0,(va!Y108-va!X108))</f>
@@ -64735,7 +65242,7 @@
       </c>
       <c r="W114" s="16">
         <f>MAX(0,(va!X110-va!W110))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="X114" s="16">
         <f>MAX(0,(va!Y110-va!X110))</f>
@@ -65017,7 +65524,7 @@
       </c>
       <c r="W115" s="16">
         <f>MAX(0,(va!X111-va!W111))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X115" s="16">
         <f>MAX(0,(va!Y111-va!X111))</f>
@@ -65863,7 +66370,7 @@
       </c>
       <c r="W118" s="16">
         <f>MAX(0,(va!X114-va!W114))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X118" s="16">
         <f>MAX(0,(va!Y114-va!X114))</f>
@@ -66145,7 +66652,7 @@
       </c>
       <c r="W119" s="16">
         <f>MAX(0,(va!X115-va!W115))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X119" s="16">
         <f>MAX(0,(va!Y115-va!X115))</f>
@@ -66427,7 +66934,7 @@
       </c>
       <c r="W120" s="16">
         <f>MAX(0,(va!X116-va!W116))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X120" s="16">
         <f>MAX(0,(va!Y116-va!X116))</f>
@@ -66709,7 +67216,7 @@
       </c>
       <c r="W121" s="16">
         <f>MAX(0,(va!X117-va!W117))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X121" s="16">
         <f>MAX(0,(va!Y117-va!X117))</f>
@@ -66991,7 +67498,7 @@
       </c>
       <c r="W122" s="16">
         <f>MAX(0,(va!X118-va!W118))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X122" s="16">
         <f>MAX(0,(va!Y118-va!X118))</f>
@@ -67555,7 +68062,7 @@
       </c>
       <c r="W124" s="16">
         <f>MAX(0,(va!X120-va!W120))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X124" s="16">
         <f>MAX(0,(va!Y120-va!X120))</f>
@@ -69247,7 +69754,7 @@
       </c>
       <c r="W130" s="16">
         <f>MAX(0,(va!X126-va!W126))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X130" s="16">
         <f>MAX(0,(va!Y126-va!X126))</f>
@@ -70657,7 +71164,7 @@
       </c>
       <c r="W135" s="16">
         <f>MAX(0,(va!X131-va!W131))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X135" s="16">
         <f>MAX(0,(va!Y131-va!X131))</f>
@@ -72067,7 +72574,7 @@
       </c>
       <c r="W140" s="16">
         <f>MAX(0,(va!X136-va!W136))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X140" s="16">
         <f>MAX(0,(va!Y136-va!X136))</f>
@@ -72631,7 +73138,7 @@
       </c>
       <c r="W142" s="16">
         <f>MAX(0,(va!X138-va!W138))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X142" s="16">
         <f>MAX(0,(va!Y138-va!X138))</f>
@@ -72913,7 +73420,7 @@
       </c>
       <c r="W143" s="16">
         <f>MAX(0,(va!X139-va!W139))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X143" s="16">
         <f>MAX(0,(va!Y139-va!X139))</f>

</xml_diff>

<commit_message>
15 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6CFAE9-0973-4BF5-8E0E-B93BB8DEA8D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543C408D-629C-4EAD-A759-C739563D44AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="5130" windowWidth="21600" windowHeight="12855" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="7185" yWindow="5130" windowWidth="21600" windowHeight="12855" tabRatio="685" activeTab="5" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1003,7 +1003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1064,6 +1064,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1073,15 +1082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4022,8 +4023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E207B2A-317D-4660-A7D7-5B9F35994222}">
   <dimension ref="A1:CC46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4139,6 +4140,9 @@
       <c r="AG2" s="12">
         <v>11518</v>
       </c>
+      <c r="AH2" s="12">
+        <v>11525</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4259,7 +4263,7 @@
       </c>
       <c r="AH3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2197</v>
       </c>
       <c r="AI3" s="10">
         <f t="shared" si="0"/>
@@ -4555,8 +4559,11 @@
       <c r="AG5" s="10">
         <v>67</v>
       </c>
+      <c r="AH5" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="6" spans="1:81" ht="39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>272</v>
       </c>
@@ -4900,6 +4907,9 @@
       </c>
       <c r="AG7" s="10">
         <v>230</v>
+      </c>
+      <c r="AH7" s="36">
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
@@ -5002,6 +5012,9 @@
       <c r="AG8" s="10">
         <v>182</v>
       </c>
+      <c r="AH8" s="36">
+        <v>183</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
@@ -5103,6 +5116,9 @@
       <c r="AG9" s="10">
         <v>149</v>
       </c>
+      <c r="AH9" s="36">
+        <v>161</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
@@ -5204,6 +5220,9 @@
       <c r="AG10" s="10">
         <v>326</v>
       </c>
+      <c r="AH10" s="36">
+        <v>361</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
@@ -5305,6 +5324,9 @@
       <c r="AG11" s="10">
         <v>262</v>
       </c>
+      <c r="AH11" s="36">
+        <v>278</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
@@ -5406,6 +5428,9 @@
       <c r="AG12" s="10">
         <v>290</v>
       </c>
+      <c r="AH12" s="36">
+        <v>298</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
@@ -5507,6 +5532,9 @@
       <c r="AG13" s="10">
         <v>296</v>
       </c>
+      <c r="AH13" s="36">
+        <v>322</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
@@ -5608,6 +5636,9 @@
       <c r="AG14" s="10">
         <v>237</v>
       </c>
+      <c r="AH14" s="36">
+        <v>259</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
@@ -5708,6 +5739,9 @@
       </c>
       <c r="AG15" s="10">
         <v>86</v>
+      </c>
+      <c r="AH15" s="36">
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -5863,7 +5897,7 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5947,7 +5981,7 @@
         <v>44261</v>
       </c>
       <c r="W2" s="10">
-        <v>0</v>
+        <v>45731</v>
       </c>
       <c r="X2" s="10">
         <v>0</v>
@@ -6173,7 +6207,7 @@
       </c>
       <c r="W3" s="10">
         <f>SUM(md[15-Apr])</f>
-        <v>0</v>
+        <v>10032</v>
       </c>
       <c r="X3" s="10">
         <f>SUM(md[16-Apr])</f>
@@ -6425,7 +6459,7 @@
         <v>2122</v>
       </c>
       <c r="W4" s="10">
-        <v>0</v>
+        <v>2231</v>
       </c>
       <c r="X4" s="10">
         <v>0</v>
@@ -6631,7 +6665,7 @@
         <v>302</v>
       </c>
       <c r="W5" s="10">
-        <v>0</v>
+        <v>349</v>
       </c>
       <c r="X5" s="10">
         <v>0</v>
@@ -6839,7 +6873,7 @@
       <c r="V6" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="18" t="s">
         <v>199</v>
       </c>
       <c r="X6" s="3" t="s">
@@ -7048,6 +7082,9 @@
       <c r="V7">
         <v>17</v>
       </c>
+      <c r="W7">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7116,6 +7153,9 @@
       <c r="V8" s="10">
         <v>783</v>
       </c>
+      <c r="W8" s="10">
+        <v>845</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7184,6 +7224,9 @@
       <c r="V9">
         <v>962</v>
       </c>
+      <c r="W9">
+        <v>1060</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7252,6 +7295,9 @@
       <c r="V10">
         <v>1377</v>
       </c>
+      <c r="W10">
+        <v>1485</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -7320,6 +7366,9 @@
       <c r="V11">
         <v>99</v>
       </c>
+      <c r="W11">
+        <v>102</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -7388,6 +7437,9 @@
       <c r="V12">
         <v>21</v>
       </c>
+      <c r="W12">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -7456,6 +7508,9 @@
       <c r="V13">
         <v>259</v>
       </c>
+      <c r="W13">
+        <v>262</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -7524,6 +7579,9 @@
       <c r="V14">
         <v>85</v>
       </c>
+      <c r="W14">
+        <v>90</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -7592,6 +7650,9 @@
       <c r="V15">
         <v>292</v>
       </c>
+      <c r="W15">
+        <v>310</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -7660,8 +7721,11 @@
       <c r="V16" s="10">
         <v>14</v>
       </c>
+      <c r="W16" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -7728,8 +7792,11 @@
       <c r="V17">
         <v>441</v>
       </c>
+      <c r="W17">
+        <v>442</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -7796,8 +7863,11 @@
       <c r="V18">
         <v>4</v>
       </c>
+      <c r="W18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -7864,8 +7934,11 @@
       <c r="V19">
         <v>147</v>
       </c>
+      <c r="W19">
+        <v>152</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -7932,8 +8005,11 @@
       <c r="V20">
         <v>403</v>
       </c>
+      <c r="W20">
+        <v>424</v>
+      </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -8000,8 +8076,11 @@
       <c r="V21">
         <v>11</v>
       </c>
+      <c r="W21">
+        <v>11</v>
+      </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -8068,8 +8147,11 @@
       <c r="V22">
         <v>1883</v>
       </c>
+      <c r="W22">
+        <v>1933</v>
+      </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -8136,8 +8218,11 @@
       <c r="V23">
         <v>2356</v>
       </c>
+      <c r="W23">
+        <v>2516</v>
+      </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -8204,8 +8289,11 @@
       <c r="V24">
         <v>19</v>
       </c>
+      <c r="W24">
+        <v>19</v>
+      </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -8272,8 +8360,11 @@
       <c r="V25">
         <v>98</v>
       </c>
+      <c r="W25">
+        <v>99</v>
+      </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -8340,8 +8431,11 @@
       <c r="V26">
         <v>5</v>
       </c>
+      <c r="W26">
+        <v>5</v>
+      </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -8408,8 +8502,11 @@
       <c r="V27">
         <v>16</v>
       </c>
+      <c r="W27">
+        <v>14</v>
+      </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -8476,8 +8573,11 @@
       <c r="V28">
         <v>96</v>
       </c>
+      <c r="W28">
+        <v>106</v>
+      </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -8544,8 +8644,11 @@
       <c r="V29">
         <v>63</v>
       </c>
+      <c r="W29">
+        <v>76</v>
+      </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -8612,8 +8715,11 @@
       <c r="V30">
         <v>21</v>
       </c>
+      <c r="W30">
+        <v>22</v>
+      </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -8707,7 +8813,7 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8821,7 +8927,7 @@
       </c>
       <c r="Z2" s="10">
         <f>SUM(va[15-Apr])</f>
-        <v>0</v>
+        <v>6500</v>
       </c>
       <c r="AA2" s="10">
         <f>SUM(va[16-Apr])</f>
@@ -9076,7 +9182,7 @@
         <v>978</v>
       </c>
       <c r="Z3" s="10">
-        <v>0</v>
+        <v>1048</v>
       </c>
       <c r="AA3" s="10">
         <v>0</v>
@@ -9285,7 +9391,7 @@
         <v>154</v>
       </c>
       <c r="Z4" s="10">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="AA4" s="10">
         <v>0</v>
@@ -9494,7 +9600,7 @@
         <v>42763</v>
       </c>
       <c r="Z5" s="10">
-        <v>0</v>
+        <v>44169</v>
       </c>
       <c r="AA5" s="10">
         <v>0</v>
@@ -9711,7 +9817,7 @@
       <c r="Y6" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="18" t="s">
         <v>199</v>
       </c>
       <c r="AA6" s="3" t="s">
@@ -9929,9 +10035,12 @@
       <c r="Y7" s="10">
         <v>247</v>
       </c>
+      <c r="Z7" s="10">
+        <v>254</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -10006,9 +10115,12 @@
       <c r="Y8" s="10">
         <v>4</v>
       </c>
+      <c r="Z8" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -10081,9 +10193,12 @@
       <c r="Y9" s="10">
         <v>23</v>
       </c>
+      <c r="Z9" s="10">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -10156,9 +10271,12 @@
       <c r="Y10" s="10">
         <v>2</v>
       </c>
+      <c r="Z10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -10231,9 +10349,12 @@
       <c r="Y11" s="10">
         <v>16</v>
       </c>
+      <c r="Z11" s="10">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -10306,9 +10427,12 @@
       <c r="Y12" s="10">
         <v>1</v>
       </c>
+      <c r="Z12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -10379,6 +10503,9 @@
         <v>1</v>
       </c>
       <c r="Y13" s="10">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="10">
         <v>3</v>
       </c>
     </row>
@@ -10458,9 +10585,12 @@
       <c r="Y14" s="10">
         <v>401</v>
       </c>
+      <c r="Z14" s="10">
+        <v>420</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -10535,9 +10665,12 @@
       <c r="Y15" s="10">
         <v>17</v>
       </c>
+      <c r="Z15" s="10">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -10610,9 +10743,12 @@
       <c r="Y16" s="10">
         <v>0</v>
       </c>
+      <c r="Z16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -10685,9 +10821,12 @@
       <c r="Y17" s="10">
         <v>0</v>
       </c>
+      <c r="Z17" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -10760,9 +10899,12 @@
       <c r="Y18" s="10">
         <v>3</v>
       </c>
+      <c r="Z18" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -10835,9 +10977,12 @@
       <c r="Y19" s="10">
         <v>56</v>
       </c>
+      <c r="Z19" s="10">
+        <v>67</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -10910,9 +11055,12 @@
       <c r="Y20" s="10">
         <v>4</v>
       </c>
+      <c r="Z20" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -10985,9 +11133,12 @@
       <c r="Y21" s="10">
         <v>95</v>
       </c>
+      <c r="Z21" s="10">
+        <v>101</v>
+      </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -11060,9 +11211,12 @@
       <c r="Y22" s="10">
         <v>3</v>
       </c>
+      <c r="Z22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -11135,9 +11289,12 @@
       <c r="Y23" s="10">
         <v>2</v>
       </c>
+      <c r="Z23" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -11210,9 +11367,12 @@
       <c r="Y24" s="10">
         <v>6</v>
       </c>
+      <c r="Z24" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -11287,9 +11447,12 @@
       <c r="Y25" s="10">
         <v>10</v>
       </c>
+      <c r="Z25" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -11362,9 +11525,12 @@
       <c r="Y26" s="10">
         <v>7</v>
       </c>
+      <c r="Z26" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -11437,9 +11603,12 @@
       <c r="Y27" s="10">
         <v>16</v>
       </c>
+      <c r="Z27" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -11512,9 +11681,12 @@
       <c r="Y28" s="10">
         <v>11</v>
       </c>
+      <c r="Z28" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -11587,8 +11759,11 @@
       <c r="Y29" s="10">
         <v>33</v>
       </c>
+      <c r="Z29" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -11664,9 +11839,12 @@
       <c r="Y30" s="10">
         <v>136</v>
       </c>
+      <c r="Z30" s="10">
+        <v>140</v>
+      </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -11741,9 +11919,12 @@
       <c r="Y31" s="10">
         <v>241</v>
       </c>
+      <c r="Z31" s="10">
+        <v>254</v>
+      </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -11816,9 +11997,12 @@
       <c r="Y32" s="10">
         <v>5</v>
       </c>
+      <c r="Z32" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -11891,9 +12075,12 @@
       <c r="Y33" s="10">
         <v>16</v>
       </c>
+      <c r="Z33" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -11968,9 +12155,12 @@
       <c r="Y34" s="10">
         <v>9</v>
       </c>
+      <c r="Z34" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -12043,9 +12233,12 @@
       <c r="Y35" s="10">
         <v>39</v>
       </c>
+      <c r="Z35" s="10">
+        <v>40</v>
+      </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -12118,9 +12311,12 @@
       <c r="Y36" s="10">
         <v>52</v>
       </c>
+      <c r="Z36" s="10">
+        <v>53</v>
+      </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -12193,9 +12389,12 @@
       <c r="Y37" s="10">
         <v>15</v>
       </c>
+      <c r="Z37" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -12270,9 +12469,12 @@
       <c r="Y38" s="10">
         <v>7</v>
       </c>
+      <c r="Z38" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -12345,9 +12547,12 @@
       <c r="Y39" s="10">
         <v>15</v>
       </c>
+      <c r="Z39" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -12420,9 +12625,12 @@
       <c r="Y40" s="10">
         <v>27</v>
       </c>
+      <c r="Z40" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -12495,9 +12703,12 @@
       <c r="Y41" s="10">
         <v>3</v>
       </c>
+      <c r="Z41" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -12570,9 +12781,12 @@
       <c r="Y42" s="10">
         <v>8</v>
       </c>
+      <c r="Z42" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -12645,9 +12859,12 @@
       <c r="Y43" s="10">
         <v>8</v>
       </c>
+      <c r="Z43" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -12720,9 +12937,12 @@
       <c r="Y44" s="10">
         <v>14</v>
       </c>
+      <c r="Z44" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -12795,9 +13015,12 @@
       <c r="Y45" s="10">
         <v>19</v>
       </c>
+      <c r="Z45" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -12872,9 +13095,12 @@
       <c r="Y46" s="10">
         <v>12</v>
       </c>
+      <c r="Z46" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -12947,9 +13173,12 @@
       <c r="Y47" s="10">
         <v>0</v>
       </c>
+      <c r="Z47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -13022,9 +13251,12 @@
       <c r="Y48" s="10">
         <v>2</v>
       </c>
+      <c r="Z48" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -13097,9 +13329,12 @@
       <c r="Y49" s="10">
         <v>4</v>
       </c>
+      <c r="Z49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -13174,9 +13409,12 @@
       <c r="Y50" s="10">
         <v>15</v>
       </c>
+      <c r="Z50" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -13249,9 +13487,12 @@
       <c r="Y51" s="10">
         <v>4</v>
       </c>
+      <c r="Z51" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -13326,9 +13567,12 @@
       <c r="Y52" s="10">
         <v>1207</v>
       </c>
+      <c r="Z52" s="10">
+        <v>1298</v>
+      </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -13401,9 +13645,12 @@
       <c r="Y53" s="10">
         <v>0</v>
       </c>
+      <c r="Z53" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -13476,8 +13723,11 @@
       <c r="Y54" s="10">
         <v>0</v>
       </c>
+      <c r="Z54" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -13553,8 +13803,11 @@
       <c r="Y55" s="10">
         <v>73</v>
       </c>
+      <c r="Z55" s="10">
+        <v>75</v>
+      </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -13630,9 +13883,12 @@
       <c r="Y56" s="10">
         <v>432</v>
       </c>
+      <c r="Z56" s="10">
+        <v>453</v>
+      </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -13707,9 +13963,12 @@
       <c r="Y57" s="10">
         <v>6</v>
       </c>
+      <c r="Z57" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -13782,9 +14041,12 @@
       <c r="Y58" s="10">
         <v>3</v>
       </c>
+      <c r="Z58" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -13857,9 +14119,12 @@
       <c r="Y59" s="10">
         <v>14</v>
       </c>
+      <c r="Z59" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -13932,9 +14197,12 @@
       <c r="Y60" s="10">
         <v>0</v>
       </c>
+      <c r="Z60" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -14009,9 +14277,12 @@
       <c r="Y61" s="10">
         <v>5</v>
       </c>
+      <c r="Z61" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -14084,9 +14355,12 @@
       <c r="Y62" s="10">
         <v>71</v>
       </c>
+      <c r="Z62" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -14159,9 +14433,12 @@
       <c r="Y63" s="10">
         <v>6</v>
       </c>
+      <c r="Z63" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -14234,9 +14511,12 @@
       <c r="Y64" s="10">
         <v>23</v>
       </c>
+      <c r="Z64" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -14309,9 +14589,12 @@
       <c r="Y65" s="10">
         <v>19</v>
       </c>
+      <c r="Z65" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -14384,8 +14667,11 @@
       <c r="Y66" s="10">
         <v>20</v>
       </c>
+      <c r="Z66" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -14461,9 +14747,12 @@
       <c r="Y67" s="10">
         <v>344</v>
       </c>
+      <c r="Z67" s="10">
+        <v>367</v>
+      </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -14538,9 +14827,12 @@
       <c r="Y68" s="10">
         <v>0</v>
       </c>
+      <c r="Z68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -14613,9 +14905,12 @@
       <c r="Y69" s="10">
         <v>3</v>
       </c>
+      <c r="Z69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -14688,9 +14983,12 @@
       <c r="Y70" s="10">
         <v>0</v>
       </c>
+      <c r="Z70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -14763,9 +15061,12 @@
       <c r="Y71" s="10">
         <v>11</v>
       </c>
+      <c r="Z71" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -14838,9 +15139,12 @@
       <c r="Y72" s="10">
         <v>27</v>
       </c>
+      <c r="Z72" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -14913,9 +15217,12 @@
       <c r="Y73" s="10">
         <v>7</v>
       </c>
+      <c r="Z73" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -14988,9 +15295,12 @@
       <c r="Y74" s="10">
         <v>1</v>
       </c>
+      <c r="Z74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -15063,9 +15373,12 @@
       <c r="Y75" s="10">
         <v>1</v>
       </c>
+      <c r="Z75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -15140,9 +15453,12 @@
       <c r="Y76" s="10">
         <v>1</v>
       </c>
+      <c r="Z76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -15215,9 +15531,12 @@
       <c r="Y77" s="10">
         <v>4</v>
       </c>
+      <c r="Z77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -15290,9 +15609,12 @@
       <c r="Y78" s="10">
         <v>33</v>
       </c>
+      <c r="Z78" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -15365,9 +15687,12 @@
       <c r="Y79" s="10">
         <v>4</v>
       </c>
+      <c r="Z79" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -15440,8 +15765,11 @@
       <c r="Y80" s="10">
         <v>1</v>
       </c>
+      <c r="Z80" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -15517,9 +15845,12 @@
       <c r="Y81" s="10">
         <v>97</v>
       </c>
+      <c r="Z81" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -15594,9 +15925,12 @@
       <c r="Y82" s="10">
         <v>128</v>
       </c>
+      <c r="Z82" s="10">
+        <v>132</v>
+      </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -15669,9 +16003,12 @@
       <c r="Y83" s="10">
         <v>35</v>
       </c>
+      <c r="Z83" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -15744,9 +16081,12 @@
       <c r="Y84" s="10">
         <v>93</v>
       </c>
+      <c r="Z84" s="10">
+        <v>95</v>
+      </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -15819,9 +16159,12 @@
       <c r="Y85" s="10">
         <v>6</v>
       </c>
+      <c r="Z85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -15894,9 +16237,12 @@
       <c r="Y86" s="10">
         <v>20</v>
       </c>
+      <c r="Z86" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A87" s="30" t="s">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -15971,9 +16317,12 @@
       <c r="Y87" s="10">
         <v>9</v>
       </c>
+      <c r="Z87" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -16046,9 +16395,12 @@
       <c r="Y88" s="10">
         <v>18</v>
       </c>
+      <c r="Z88" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -16121,9 +16473,12 @@
       <c r="Y89" s="10">
         <v>4</v>
       </c>
+      <c r="Z89" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -16196,9 +16551,12 @@
       <c r="Y90" s="10">
         <v>8</v>
       </c>
+      <c r="Z90" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -16271,9 +16629,12 @@
       <c r="Y91" s="10">
         <v>3</v>
       </c>
+      <c r="Z91" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A92" s="31"/>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -16346,9 +16707,12 @@
       <c r="Y92" s="10">
         <v>5</v>
       </c>
+      <c r="Z92" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -16421,9 +16785,12 @@
       <c r="Y93" s="10">
         <v>13</v>
       </c>
+      <c r="Z93" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -16498,9 +16865,12 @@
       <c r="Y94" s="10">
         <v>4</v>
       </c>
+      <c r="Z94" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -16573,8 +16943,11 @@
       <c r="Y95" s="10">
         <v>22</v>
       </c>
+      <c r="Z95" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -16650,9 +17023,12 @@
       <c r="Y96" s="10">
         <v>59</v>
       </c>
+      <c r="Z96" s="10">
+        <v>59</v>
+      </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A97" s="33" t="s">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -16727,9 +17103,12 @@
       <c r="Y97" s="10">
         <v>508</v>
       </c>
+      <c r="Z97" s="10">
+        <v>536</v>
+      </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -16802,9 +17181,12 @@
       <c r="Y98" s="10">
         <v>49</v>
       </c>
+      <c r="Z98" s="10">
+        <v>53</v>
+      </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A99" s="35"/>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -16877,9 +17259,12 @@
       <c r="Y99" s="10">
         <v>13</v>
       </c>
+      <c r="Z99" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -16954,9 +17339,12 @@
       <c r="Y100" s="10">
         <v>7</v>
       </c>
+      <c r="Z100" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -17029,9 +17417,12 @@
       <c r="Y101" s="10">
         <v>16</v>
       </c>
+      <c r="Z101" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -17104,9 +17495,12 @@
       <c r="Y102" s="10">
         <v>56</v>
       </c>
+      <c r="Z102" s="10">
+        <v>60</v>
+      </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -17179,9 +17573,12 @@
       <c r="Y103" s="10">
         <v>95</v>
       </c>
+      <c r="Z103" s="10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -17254,9 +17651,12 @@
       <c r="Y104" s="10">
         <v>14</v>
       </c>
+      <c r="Z104" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -17331,9 +17731,12 @@
       <c r="Y105" s="10">
         <v>24</v>
       </c>
+      <c r="Z105" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -17406,9 +17809,12 @@
       <c r="Y106" s="10">
         <v>28</v>
       </c>
+      <c r="Z106" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -17481,9 +17887,12 @@
       <c r="Y107" s="10">
         <v>7</v>
       </c>
+      <c r="Z107" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -17556,9 +17965,12 @@
       <c r="Y108" s="10">
         <v>15</v>
       </c>
+      <c r="Z108" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -17631,8 +18043,11 @@
       <c r="Y109" s="10">
         <v>1</v>
       </c>
+      <c r="Z109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -17708,8 +18123,11 @@
       <c r="Y110" s="10">
         <v>175</v>
       </c>
+      <c r="Z110" s="10">
+        <v>177</v>
+      </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -17785,9 +18203,12 @@
       <c r="Y111" s="10">
         <v>21</v>
       </c>
+      <c r="Z111" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -17862,9 +18283,12 @@
       <c r="Y112" s="10">
         <v>9</v>
       </c>
+      <c r="Z112" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -17937,9 +18361,12 @@
       <c r="Y113" s="10">
         <v>7</v>
       </c>
+      <c r="Z113" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A114" s="32"/>
+    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -18012,9 +18439,12 @@
       <c r="Y114" s="10">
         <v>57</v>
       </c>
+      <c r="Z114" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A115" s="33" t="s">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -18089,9 +18519,12 @@
       <c r="Y115" s="10">
         <v>50</v>
       </c>
+      <c r="Z115" s="10">
+        <v>53</v>
+      </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -18164,9 +18597,12 @@
       <c r="Y116" s="10">
         <v>40</v>
       </c>
+      <c r="Z116" s="10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -18239,9 +18675,12 @@
       <c r="Y117" s="10">
         <v>5</v>
       </c>
+      <c r="Z117" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
+    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -18314,9 +18753,12 @@
       <c r="Y118" s="10">
         <v>27</v>
       </c>
+      <c r="Z118" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -18389,9 +18831,12 @@
       <c r="Y119" s="10">
         <v>5</v>
       </c>
+      <c r="Z119" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -18464,9 +18909,12 @@
       <c r="Y120" s="10">
         <v>36</v>
       </c>
+      <c r="Z120" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="s">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -18541,9 +18989,12 @@
       <c r="Y121" s="10">
         <v>0</v>
       </c>
+      <c r="Z121" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
+    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -18616,9 +19067,12 @@
       <c r="Y122" s="10">
         <v>20</v>
       </c>
+      <c r="Z122" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A123" s="31"/>
+    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -18691,9 +19145,12 @@
       <c r="Y123" s="10">
         <v>2</v>
       </c>
+      <c r="Z123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A124" s="31"/>
+    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -18766,9 +19223,12 @@
       <c r="Y124" s="10">
         <v>2</v>
       </c>
+      <c r="Z124" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A125" s="31"/>
+    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -18841,9 +19301,12 @@
       <c r="Y125" s="10">
         <v>1</v>
       </c>
+      <c r="Z125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A126" s="31"/>
+    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -18916,9 +19379,12 @@
       <c r="Y126" s="10">
         <v>3</v>
       </c>
+      <c r="Z126" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A127" s="31"/>
+    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -18991,9 +19457,12 @@
       <c r="Y127" s="10">
         <v>3</v>
       </c>
+      <c r="Z127" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A128" s="31"/>
+    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -19066,9 +19535,12 @@
       <c r="Y128" s="10">
         <v>4</v>
       </c>
+      <c r="Z128" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A129" s="31"/>
+    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -19141,9 +19613,12 @@
       <c r="Y129" s="10">
         <v>7</v>
       </c>
+      <c r="Z129" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -19216,8 +19691,11 @@
       <c r="Y130" s="10">
         <v>8</v>
       </c>
+      <c r="Z130" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -19293,9 +19771,12 @@
       <c r="Y131" s="10">
         <v>252</v>
       </c>
+      <c r="Z131" s="10">
+        <v>256</v>
+      </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="s">
+    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -19370,9 +19851,12 @@
       <c r="Y132" s="10">
         <v>15</v>
       </c>
+      <c r="Z132" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A133" s="31"/>
+    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -19445,9 +19929,12 @@
       <c r="Y133" s="10">
         <v>8</v>
       </c>
+      <c r="Z133" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A134" s="31"/>
+    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -19520,9 +20007,12 @@
       <c r="Y134" s="10">
         <v>0</v>
       </c>
+      <c r="Z134" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A135" s="32"/>
+    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -19595,9 +20085,12 @@
       <c r="Y135" s="10">
         <v>0</v>
       </c>
+      <c r="Z135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="s">
+    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -19672,9 +20165,12 @@
       <c r="Y136" s="10">
         <v>60</v>
       </c>
+      <c r="Z136" s="10">
+        <v>60</v>
+      </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
+    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -19747,9 +20243,12 @@
       <c r="Y137" s="10">
         <v>6</v>
       </c>
+      <c r="Z137" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -19822,9 +20321,12 @@
       <c r="Y138" s="10">
         <v>7</v>
       </c>
+      <c r="Z138" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A139" s="35"/>
+    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -19896,10 +20398,25 @@
       </c>
       <c r="Y139" s="10">
         <v>57</v>
+      </c>
+      <c r="Z139" s="10">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -19912,18 +20429,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -20015,7 +20520,7 @@
   <dimension ref="A1:CC19"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20166,7 +20671,7 @@
       </c>
       <c r="AH2" s="19">
         <f t="shared" ref="AH2:BM2" si="1">(AH7/MAX(AH6,1))*100</f>
-        <v>0</v>
+        <v>1985.7142857142858</v>
       </c>
       <c r="AI2" s="19">
         <f t="shared" si="1"/>
@@ -20816,7 +21321,7 @@
       </c>
       <c r="AH4" s="10">
         <f t="shared" ref="AH4:BM4" si="7">(AH9/MAX(1,AH7))*100</f>
-        <v>0</v>
+        <v>3.5971223021582732</v>
       </c>
       <c r="AI4" s="10">
         <f t="shared" si="7"/>
@@ -21141,7 +21646,7 @@
       </c>
       <c r="AH6" s="12">
         <f>MAX(0, (dc!AH2-dc!AG2))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI6" s="12">
         <f>MAX(0, (dc!AI2-dc!AH2))</f>
@@ -21465,7 +21970,7 @@
       </c>
       <c r="AH7" s="12">
         <f>MAX(0, (dc!AH3-dc!AG3))</f>
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="AI7" s="12">
         <f>MAX(0, (dc!AI3-dc!AH3))</f>
@@ -22113,7 +22618,7 @@
       </c>
       <c r="AH9" s="12">
         <f>MAX(0, (dc!AH5-dc!AG5))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI9" s="12">
         <f>MAX(0, (dc!AI5-dc!AH5))</f>
@@ -22665,7 +23170,7 @@
       </c>
       <c r="AH11" s="10">
         <f>MAX(0,(dc!AH7-dc!AG7))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AI11" s="10">
         <f>MAX(0,(dc!AI7-dc!AH7))</f>
@@ -22972,7 +23477,7 @@
       </c>
       <c r="AH12" s="10">
         <f>MAX(0,(dc!AH8-dc!AG8))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI12" s="10">
         <f>MAX(0,(dc!AI8-dc!AH8))</f>
@@ -23279,7 +23784,7 @@
       </c>
       <c r="AH13" s="10">
         <f>MAX(0,(dc!AH9-dc!AG9))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AI13" s="10">
         <f>MAX(0,(dc!AI9-dc!AH9))</f>
@@ -23586,7 +24091,7 @@
       </c>
       <c r="AH14" s="10">
         <f>MAX(0,(dc!AH10-dc!AG10))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AI14" s="10">
         <f>MAX(0,(dc!AI10-dc!AH10))</f>
@@ -23893,7 +24398,7 @@
       </c>
       <c r="AH15" s="10">
         <f>MAX(0,(dc!AH11-dc!AG11))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AI15" s="10">
         <f>MAX(0,(dc!AI11-dc!AH11))</f>
@@ -24200,7 +24705,7 @@
       </c>
       <c r="AH16" s="10">
         <f>MAX(0,(dc!AH12-dc!AG12))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI16" s="10">
         <f>MAX(0,(dc!AI12-dc!AH12))</f>
@@ -24507,7 +25012,7 @@
       </c>
       <c r="AH17" s="10">
         <f>MAX(0,(dc!AH13-dc!AG13))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AI17" s="10">
         <f>MAX(0,(dc!AI13-dc!AH13))</f>
@@ -24814,7 +25319,7 @@
       </c>
       <c r="AH18" s="10">
         <f>MAX(0,(dc!AH14-dc!AG14))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AI18" s="10">
         <f>MAX(0,(dc!AI14-dc!AH14))</f>
@@ -25121,7 +25626,7 @@
       </c>
       <c r="AH19" s="10">
         <f>MAX(0,(dc!AH15-dc!AG15))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AI19" s="10">
         <f>MAX(0,(dc!AI15-dc!AH15))</f>
@@ -25515,7 +26020,7 @@
       </c>
       <c r="W2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27.586206896551722</v>
       </c>
       <c r="X2" s="21">
         <f t="shared" si="0"/>
@@ -25788,7 +26293,7 @@
       </c>
       <c r="W3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19.464285714285715</v>
       </c>
       <c r="X3" s="21">
         <f t="shared" si="2"/>
@@ -26061,7 +26566,7 @@
       </c>
       <c r="W4" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.3928571428571423</v>
       </c>
       <c r="X4" s="21">
         <f t="shared" si="4"/>
@@ -26397,7 +26902,7 @@
       </c>
       <c r="W6" s="14">
         <f>MAX(0,(md!W2-md!V2)+(md!W3-md!V3))</f>
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="X6" s="14">
         <f>MAX(0,(md!X2-md!W2)+(md!X3-md!W3))</f>
@@ -26669,7 +27174,7 @@
       </c>
       <c r="W7" s="14">
         <f>MAX(0,(md!W3-md!V3))</f>
-        <v>0</v>
+        <v>560</v>
       </c>
       <c r="X7" s="14">
         <f>MAX(0,(md!X3-md!W3))</f>
@@ -26941,7 +27446,7 @@
       </c>
       <c r="W8" s="14">
         <f>MAX(0,(md!W4-md!V4))</f>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="X8" s="14">
         <f>MAX(0,(md!X4-md!W4))</f>
@@ -27213,7 +27718,7 @@
       </c>
       <c r="W9" s="14">
         <f>MAX(0,(md!W5-md!V5))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="X9" s="14">
         <f>MAX(0,(md!X5-md!W5))</f>
@@ -27976,7 +28481,7 @@
       </c>
       <c r="W12" s="14">
         <f>MAX(0,(md!W9-md!V9))</f>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="X12" s="14">
         <f>MAX(0,(md!X9-md!W9))</f>
@@ -28253,7 +28758,7 @@
       </c>
       <c r="W13" s="14">
         <f>MAX(0,(md!W9-md!V9))</f>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="X13" s="14">
         <f>MAX(0,(md!X9-md!W9))</f>
@@ -28530,7 +29035,7 @@
       </c>
       <c r="W14" s="14">
         <f>MAX(0,(md!W10-md!V10))</f>
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="X14" s="14">
         <f>MAX(0,(md!X10-md!W10))</f>
@@ -28807,7 +29312,7 @@
       </c>
       <c r="W15" s="14">
         <f>MAX(0,(md!W11-md!V11))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X15" s="14">
         <f>MAX(0,(md!X11-md!W11))</f>
@@ -29084,7 +29589,7 @@
       </c>
       <c r="W16" s="14">
         <f>MAX(0,(md!W12-md!V12))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16" s="14">
         <f>MAX(0,(md!X12-md!W12))</f>
@@ -29361,7 +29866,7 @@
       </c>
       <c r="W17" s="14">
         <f>MAX(0,(md!W13-md!V13))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X17" s="14">
         <f>MAX(0,(md!X13-md!W13))</f>
@@ -29638,7 +30143,7 @@
       </c>
       <c r="W18" s="14">
         <f>MAX(0,(md!W14-md!V14))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X18" s="14">
         <f>MAX(0,(md!X14-md!W14))</f>
@@ -29915,7 +30420,7 @@
       </c>
       <c r="W19" s="14">
         <f>MAX(0,(md!W15-md!V15))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="X19" s="14">
         <f>MAX(0,(md!X15-md!W15))</f>
@@ -30192,7 +30697,7 @@
       </c>
       <c r="W20" s="14">
         <f>MAX(0,(md!W16-md!V16))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X20" s="14">
         <f>MAX(0,(md!X16-md!W16))</f>
@@ -30469,7 +30974,7 @@
       </c>
       <c r="W21" s="14">
         <f>MAX(0,(md!W17-md!V17))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21" s="14">
         <f>MAX(0,(md!X17-md!W17))</f>
@@ -31023,7 +31528,7 @@
       </c>
       <c r="W23" s="14">
         <f>MAX(0,(md!W19-md!V19))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X23" s="14">
         <f>MAX(0,(md!X19-md!W19))</f>
@@ -31300,7 +31805,7 @@
       </c>
       <c r="W24" s="14">
         <f>MAX(0,(md!W20-md!V20))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="X24" s="14">
         <f>MAX(0,(md!X20-md!W20))</f>
@@ -31854,7 +32359,7 @@
       </c>
       <c r="W26" s="14">
         <f>MAX(0,(md!W22-md!V22))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="X26" s="14">
         <f>MAX(0,(md!X22-md!W22))</f>
@@ -32131,7 +32636,7 @@
       </c>
       <c r="W27" s="14">
         <f>MAX(0,(md!W23-md!V23))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="X27" s="14">
         <f>MAX(0,(md!X23-md!W23))</f>
@@ -32685,7 +33190,7 @@
       </c>
       <c r="W29" s="14">
         <f>MAX(0,(md!W25-md!V25))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X29" s="14">
         <f>MAX(0,(md!X25-md!W25))</f>
@@ -33516,7 +34021,7 @@
       </c>
       <c r="W32" s="14">
         <f>MAX(0,(md!W28-md!V28))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X32" s="14">
         <f>MAX(0,(md!X28-md!W28))</f>
@@ -33793,7 +34298,7 @@
       </c>
       <c r="W33" s="14">
         <f>MAX(0,(md!W29-md!V29))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="X33" s="14">
         <f>MAX(0,(md!X29-md!W29))</f>
@@ -34070,7 +34575,7 @@
       </c>
       <c r="W34" s="14">
         <f>MAX(0,(md!W30-md!V30))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X34" s="14">
         <f>MAX(0,(md!X30-md!W30))</f>
@@ -34438,8 +34943,8 @@
   </sheetPr>
   <dimension ref="A1:BS143"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="X66" sqref="X66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34549,7 +35054,7 @@
       </c>
       <c r="Y2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23.399715504978662</v>
       </c>
       <c r="Z2" s="20">
         <f t="shared" si="0"/>
@@ -34826,7 +35331,7 @@
       </c>
       <c r="Y3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>21.276595744680851</v>
       </c>
       <c r="Z3" s="20">
         <f t="shared" si="2"/>
@@ -35103,7 +35608,7 @@
       </c>
       <c r="Y4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>12.462006079027356</v>
       </c>
       <c r="Z4" s="20">
         <f t="shared" si="4"/>
@@ -35380,7 +35885,7 @@
       </c>
       <c r="Y6" s="14">
         <f>MAX(0,(va!Z5-va!Y5))</f>
-        <v>0</v>
+        <v>1406</v>
       </c>
       <c r="Z6" s="14">
         <f>MAX(0,(va!AA5-va!Z5))</f>
@@ -35657,7 +36162,7 @@
       </c>
       <c r="Y7" s="14">
         <f>MAX(0,(va!Z2-va!Y2))</f>
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="Z7" s="14">
         <f>MAX(0,(va!AA2-va!Z2))</f>
@@ -35934,7 +36439,7 @@
       </c>
       <c r="Y8" s="14">
         <f>MAX(0,(va!Z3-va!Y3))</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="Z8" s="14">
         <f>MAX(0,(va!AA3-va!Z3))</f>
@@ -36211,7 +36716,7 @@
       </c>
       <c r="Y9" s="14">
         <f>MAX(0,(va!Z4-va!Y4))</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="Z9" s="14">
         <f>MAX(0,(va!AA4-va!Z4))</f>
@@ -36708,7 +37213,7 @@
       </c>
       <c r="Y11" s="16">
         <f>MAX(0,(va!Z7-va!Y7))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Z11" s="16">
         <f>MAX(0,(va!AA7-va!Z7))</f>
@@ -37836,7 +38341,7 @@
       </c>
       <c r="Y15" s="16">
         <f>MAX(0,(va!Z11-va!Y11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15" s="16">
         <f>MAX(0,(va!AA11-va!Z11))</f>
@@ -38682,7 +39187,7 @@
       </c>
       <c r="Y18" s="16">
         <f>MAX(0,(va!Z14-va!Y14))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="Z18" s="16">
         <f>MAX(0,(va!AA14-va!Z14))</f>
@@ -38964,7 +39469,7 @@
       </c>
       <c r="Y19" s="16">
         <f>MAX(0,(va!Z15-va!Y15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19" s="16">
         <f>MAX(0,(va!AA15-va!Z15))</f>
@@ -40092,7 +40597,7 @@
       </c>
       <c r="Y23" s="16">
         <f>MAX(0,(va!Z19-va!Y19))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Z23" s="16">
         <f>MAX(0,(va!AA19-va!Z19))</f>
@@ -40656,7 +41161,7 @@
       </c>
       <c r="Y25" s="16">
         <f>MAX(0,(va!Z21-va!Y21))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Z25" s="16">
         <f>MAX(0,(va!AA21-va!Z21))</f>
@@ -42912,7 +43417,7 @@
       </c>
       <c r="Y33" s="16">
         <f>MAX(0,(va!Z29-va!Y29))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z33" s="16">
         <f>MAX(0,(va!AA29-va!Z29))</f>
@@ -43194,7 +43699,7 @@
       </c>
       <c r="Y34" s="16">
         <f>MAX(0,(va!Z30-va!Y30))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z34" s="16">
         <f>MAX(0,(va!AA30-va!Z30))</f>
@@ -43476,7 +43981,7 @@
       </c>
       <c r="Y35" s="16">
         <f>MAX(0,(va!Z31-va!Y31))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="Z35" s="16">
         <f>MAX(0,(va!AA31-va!Z31))</f>
@@ -44040,7 +44545,7 @@
       </c>
       <c r="Y37" s="16">
         <f>MAX(0,(va!Z33-va!Y33))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z37" s="16">
         <f>MAX(0,(va!AA33-va!Z33))</f>
@@ -44604,7 +45109,7 @@
       </c>
       <c r="Y39" s="16">
         <f>MAX(0,(va!Z35-va!Y35))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z39" s="16">
         <f>MAX(0,(va!AA35-va!Z35))</f>
@@ -44886,7 +45391,7 @@
       </c>
       <c r="Y40" s="16">
         <f>MAX(0,(va!Z36-va!Y36))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z40" s="16">
         <f>MAX(0,(va!AA36-va!Z36))</f>
@@ -45168,7 +45673,7 @@
       </c>
       <c r="Y41" s="16">
         <f>MAX(0,(va!Z37-va!Y37))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z41" s="16">
         <f>MAX(0,(va!AA37-va!Z37))</f>
@@ -45732,7 +46237,7 @@
       </c>
       <c r="Y43" s="16">
         <f>MAX(0,(va!Z39-va!Y39))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z43" s="16">
         <f>MAX(0,(va!AA39-va!Z39))</f>
@@ -46578,7 +47083,7 @@
       </c>
       <c r="Y46" s="16">
         <f>MAX(0,(va!Z42-va!Y42))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z46" s="16">
         <f>MAX(0,(va!AA42-va!Z42))</f>
@@ -49398,7 +49903,7 @@
       </c>
       <c r="Y56" s="16">
         <f>MAX(0,(va!Z52-va!Y52))</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="Z56" s="16">
         <f>MAX(0,(va!AA52-va!Z52))</f>
@@ -50244,7 +50749,7 @@
       </c>
       <c r="Y59" s="16">
         <f>MAX(0,(va!Z55-va!Y55))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z59" s="16">
         <f>MAX(0,(va!AA55-va!Z55))</f>
@@ -50526,7 +51031,7 @@
       </c>
       <c r="Y60" s="16">
         <f>MAX(0,(va!Z56-va!Y56))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="Z60" s="16">
         <f>MAX(0,(va!AA56-va!Z56))</f>
@@ -51372,7 +51877,7 @@
       </c>
       <c r="Y63" s="16">
         <f>MAX(0,(va!Z59-va!Y59))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z63" s="16">
         <f>MAX(0,(va!AA59-va!Z59))</f>
@@ -51936,7 +52441,7 @@
       </c>
       <c r="Y65" s="16">
         <f>MAX(0,(va!Z61-va!Y61))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z65" s="16">
         <f>MAX(0,(va!AA61-va!Z61))</f>
@@ -52218,7 +52723,7 @@
       </c>
       <c r="Y66" s="16">
         <f>MAX(0,(va!Z62-va!Y62))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z66" s="16">
         <f>MAX(0,(va!AA62-va!Z62))</f>
@@ -52782,7 +53287,7 @@
       </c>
       <c r="Y68" s="16">
         <f>MAX(0,(va!Z64-va!Y64))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z68" s="16">
         <f>MAX(0,(va!AA64-va!Z64))</f>
@@ -53064,7 +53569,7 @@
       </c>
       <c r="Y69" s="16">
         <f>MAX(0,(va!Z65-va!Y65))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z69" s="16">
         <f>MAX(0,(va!AA65-va!Z65))</f>
@@ -53346,7 +53851,7 @@
       </c>
       <c r="Y70" s="16">
         <f>MAX(0,(va!Z66-va!Y66))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z70" s="16">
         <f>MAX(0,(va!AA66-va!Z66))</f>
@@ -53628,7 +54133,7 @@
       </c>
       <c r="Y71" s="16">
         <f>MAX(0,(va!Z67-va!Y67))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Z71" s="16">
         <f>MAX(0,(va!AA67-va!Z67))</f>
@@ -56730,7 +57235,7 @@
       </c>
       <c r="Y82" s="16">
         <f>MAX(0,(va!Z78-va!Y78))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z82" s="16">
         <f>MAX(0,(va!AA78-va!Z78))</f>
@@ -57576,7 +58081,7 @@
       </c>
       <c r="Y85" s="16">
         <f>MAX(0,(va!Z81-va!Y81))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z85" s="16">
         <f>MAX(0,(va!AA81-va!Z81))</f>
@@ -57858,7 +58363,7 @@
       </c>
       <c r="Y86" s="16">
         <f>MAX(0,(va!Z82-va!Y82))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z86" s="16">
         <f>MAX(0,(va!AA82-va!Z82))</f>
@@ -58422,7 +58927,7 @@
       </c>
       <c r="Y88" s="16">
         <f>MAX(0,(va!Z84-va!Y84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z88" s="16">
         <f>MAX(0,(va!AA84-va!Z84))</f>
@@ -59268,7 +59773,7 @@
       </c>
       <c r="Y91" s="16">
         <f>MAX(0,(va!Z87-va!Y87))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z91" s="16">
         <f>MAX(0,(va!AA87-va!Z87))</f>
@@ -59550,7 +60055,7 @@
       </c>
       <c r="Y92" s="16">
         <f>MAX(0,(va!Z88-va!Y88))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z92" s="16">
         <f>MAX(0,(va!AA88-va!Z88))</f>
@@ -59832,7 +60337,7 @@
       </c>
       <c r="Y93" s="16">
         <f>MAX(0,(va!Z89-va!Y89))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z93" s="16">
         <f>MAX(0,(va!AA89-va!Z89))</f>
@@ -60960,7 +61465,7 @@
       </c>
       <c r="Y97" s="16">
         <f>MAX(0,(va!Z93-va!Y93))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z97" s="16">
         <f>MAX(0,(va!AA93-va!Z93))</f>
@@ -62088,7 +62593,7 @@
       </c>
       <c r="Y101" s="16">
         <f>MAX(0,(va!Z97-va!Y97))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="Z101" s="16">
         <f>MAX(0,(va!AA97-va!Z97))</f>
@@ -62370,7 +62875,7 @@
       </c>
       <c r="Y102" s="16">
         <f>MAX(0,(va!Z98-va!Y98))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z102" s="16">
         <f>MAX(0,(va!AA98-va!Z98))</f>
@@ -62652,7 +63157,7 @@
       </c>
       <c r="Y103" s="16">
         <f>MAX(0,(va!Z99-va!Y99))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z103" s="16">
         <f>MAX(0,(va!AA99-va!Z99))</f>
@@ -62934,7 +63439,7 @@
       </c>
       <c r="Y104" s="16">
         <f>MAX(0,(va!Z100-va!Y100))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z104" s="16">
         <f>MAX(0,(va!AA100-va!Z100))</f>
@@ -63216,7 +63721,7 @@
       </c>
       <c r="Y105" s="16">
         <f>MAX(0,(va!Z101-va!Y101))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z105" s="16">
         <f>MAX(0,(va!AA101-va!Z101))</f>
@@ -63498,7 +64003,7 @@
       </c>
       <c r="Y106" s="16">
         <f>MAX(0,(va!Z102-va!Y102))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z106" s="16">
         <f>MAX(0,(va!AA102-va!Z102))</f>
@@ -63780,7 +64285,7 @@
       </c>
       <c r="Y107" s="16">
         <f>MAX(0,(va!Z103-va!Y103))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="Z107" s="16">
         <f>MAX(0,(va!AA103-va!Z103))</f>
@@ -64062,7 +64567,7 @@
       </c>
       <c r="Y108" s="16">
         <f>MAX(0,(va!Z104-va!Y104))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z108" s="16">
         <f>MAX(0,(va!AA104-va!Z104))</f>
@@ -64344,7 +64849,7 @@
       </c>
       <c r="Y109" s="16">
         <f>MAX(0,(va!Z105-va!Y105))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z109" s="16">
         <f>MAX(0,(va!AA105-va!Z105))</f>
@@ -64626,7 +65131,7 @@
       </c>
       <c r="Y110" s="16">
         <f>MAX(0,(va!Z106-va!Y106))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z110" s="16">
         <f>MAX(0,(va!AA106-va!Z106))</f>
@@ -64908,7 +65413,7 @@
       </c>
       <c r="Y111" s="16">
         <f>MAX(0,(va!Z107-va!Y107))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z111" s="16">
         <f>MAX(0,(va!AA107-va!Z107))</f>
@@ -65190,7 +65695,7 @@
       </c>
       <c r="Y112" s="16">
         <f>MAX(0,(va!Z108-va!Y108))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z112" s="16">
         <f>MAX(0,(va!AA108-va!Z108))</f>
@@ -65754,7 +66259,7 @@
       </c>
       <c r="Y114" s="16">
         <f>MAX(0,(va!Z110-va!Y110))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z114" s="16">
         <f>MAX(0,(va!AA110-va!Z110))</f>
@@ -66036,7 +66541,7 @@
       </c>
       <c r="Y115" s="16">
         <f>MAX(0,(va!Z111-va!Y111))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z115" s="16">
         <f>MAX(0,(va!AA111-va!Z111))</f>
@@ -67164,7 +67669,7 @@
       </c>
       <c r="Y119" s="16">
         <f>MAX(0,(va!Z115-va!Y115))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z119" s="16">
         <f>MAX(0,(va!AA115-va!Z115))</f>
@@ -67446,7 +67951,7 @@
       </c>
       <c r="Y120" s="16">
         <f>MAX(0,(va!Z116-va!Y116))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Z120" s="16">
         <f>MAX(0,(va!AA116-va!Z116))</f>
@@ -68010,7 +68515,7 @@
       </c>
       <c r="Y122" s="16">
         <f>MAX(0,(va!Z118-va!Y118))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z122" s="16">
         <f>MAX(0,(va!AA118-va!Z118))</f>
@@ -68574,7 +69079,7 @@
       </c>
       <c r="Y124" s="16">
         <f>MAX(0,(va!Z120-va!Y120))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z124" s="16">
         <f>MAX(0,(va!AA120-va!Z120))</f>
@@ -71676,7 +72181,7 @@
       </c>
       <c r="Y135" s="16">
         <f>MAX(0,(va!Z131-va!Y131))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z135" s="16">
         <f>MAX(0,(va!AA131-va!Z131))</f>
@@ -73932,7 +74437,7 @@
       </c>
       <c r="Y143" s="16">
         <f>MAX(0,(va!Z139-va!Y139))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z143" s="16">
         <f>MAX(0,(va!AA139-va!Z139))</f>

</xml_diff>

<commit_message>
16 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543C408D-629C-4EAD-A759-C739563D44AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD61F543-0B35-4B07-813D-7A3451317AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="5130" windowWidth="21600" windowHeight="12855" tabRatio="685" activeTab="5" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1003,7 +1003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1064,6 +1064,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1071,15 +1081,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4023,8 +4024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E207B2A-317D-4660-A7D7-5B9F35994222}">
   <dimension ref="A1:CC46"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4143,6 +4144,9 @@
       <c r="AH2" s="12">
         <v>11525</v>
       </c>
+      <c r="AI2" s="12">
+        <v>12150</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4267,7 +4271,7 @@
       </c>
       <c r="AI3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="AJ3" s="10">
         <f t="shared" si="0"/>
@@ -4562,6 +4566,9 @@
       <c r="AH5" s="10">
         <v>72</v>
       </c>
+      <c r="AI5" s="10">
+        <v>81</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -4663,10 +4670,10 @@
       <c r="AG6" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AH6" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="AI6" s="3" t="s">
+      <c r="AI6" s="18" t="s">
         <v>199</v>
       </c>
       <c r="AJ6" s="3" t="s">
@@ -4908,8 +4915,11 @@
       <c r="AG7" s="10">
         <v>230</v>
       </c>
-      <c r="AH7" s="36">
+      <c r="AH7" s="30">
         <v>243</v>
+      </c>
+      <c r="AI7" s="37">
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
@@ -5012,8 +5022,11 @@
       <c r="AG8" s="10">
         <v>182</v>
       </c>
-      <c r="AH8" s="36">
+      <c r="AH8" s="30">
         <v>183</v>
+      </c>
+      <c r="AI8" s="37">
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
@@ -5116,8 +5129,11 @@
       <c r="AG9" s="10">
         <v>149</v>
       </c>
-      <c r="AH9" s="36">
+      <c r="AH9" s="30">
         <v>161</v>
+      </c>
+      <c r="AI9" s="37">
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
@@ -5220,8 +5236,11 @@
       <c r="AG10" s="10">
         <v>326</v>
       </c>
-      <c r="AH10" s="36">
+      <c r="AH10" s="30">
         <v>361</v>
+      </c>
+      <c r="AI10" s="37">
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
@@ -5324,8 +5343,11 @@
       <c r="AG11" s="10">
         <v>262</v>
       </c>
-      <c r="AH11" s="36">
+      <c r="AH11" s="30">
         <v>278</v>
+      </c>
+      <c r="AI11" s="37">
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
@@ -5428,8 +5450,11 @@
       <c r="AG12" s="10">
         <v>290</v>
       </c>
-      <c r="AH12" s="36">
+      <c r="AH12" s="30">
         <v>298</v>
+      </c>
+      <c r="AI12" s="37">
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
@@ -5532,8 +5557,11 @@
       <c r="AG13" s="10">
         <v>296</v>
       </c>
-      <c r="AH13" s="36">
+      <c r="AH13" s="30">
         <v>322</v>
+      </c>
+      <c r="AI13" s="37">
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
@@ -5636,8 +5664,11 @@
       <c r="AG14" s="10">
         <v>237</v>
       </c>
-      <c r="AH14" s="36">
+      <c r="AH14" s="30">
         <v>259</v>
+      </c>
+      <c r="AI14" s="37">
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
@@ -5740,8 +5771,11 @@
       <c r="AG15" s="10">
         <v>86</v>
       </c>
-      <c r="AH15" s="36">
+      <c r="AH15" s="30">
         <v>92</v>
+      </c>
+      <c r="AI15" s="37">
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -5897,7 +5931,7 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5984,7 +6018,7 @@
         <v>45731</v>
       </c>
       <c r="X2" s="10">
-        <v>0</v>
+        <v>48059</v>
       </c>
       <c r="Y2" s="10">
         <v>0</v>
@@ -6211,7 +6245,7 @@
       </c>
       <c r="X3" s="10">
         <f>SUM(md[16-Apr])</f>
-        <v>0</v>
+        <v>10784</v>
       </c>
       <c r="Y3" s="10">
         <f>SUM(md[17-Apr])</f>
@@ -6462,7 +6496,7 @@
         <v>2231</v>
       </c>
       <c r="X4" s="10">
-        <v>0</v>
+        <v>2451</v>
       </c>
       <c r="Y4" s="10">
         <v>0</v>
@@ -6668,7 +6702,7 @@
         <v>349</v>
       </c>
       <c r="X5" s="10">
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="Y5" s="10">
         <v>0</v>
@@ -6876,7 +6910,7 @@
       <c r="W6" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="X6" s="18" t="s">
         <v>200</v>
       </c>
       <c r="Y6" s="3" t="s">
@@ -7085,6 +7119,9 @@
       <c r="W7">
         <v>17</v>
       </c>
+      <c r="X7">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7156,6 +7193,9 @@
       <c r="W8" s="10">
         <v>845</v>
       </c>
+      <c r="X8" s="10">
+        <v>896</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7227,6 +7267,9 @@
       <c r="W9">
         <v>1060</v>
       </c>
+      <c r="X9">
+        <v>1160</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7298,6 +7341,9 @@
       <c r="W10">
         <v>1485</v>
       </c>
+      <c r="X10">
+        <v>1516</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -7369,6 +7415,9 @@
       <c r="W11">
         <v>102</v>
       </c>
+      <c r="X11">
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -7440,6 +7489,9 @@
       <c r="W12">
         <v>22</v>
       </c>
+      <c r="X12">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -7511,6 +7563,9 @@
       <c r="W13">
         <v>262</v>
       </c>
+      <c r="X13">
+        <v>283</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -7582,6 +7637,9 @@
       <c r="W14">
         <v>90</v>
       </c>
+      <c r="X14">
+        <v>101</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -7653,6 +7711,9 @@
       <c r="W15">
         <v>310</v>
       </c>
+      <c r="X15">
+        <v>327</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -7724,8 +7785,11 @@
       <c r="W16" s="10">
         <v>16</v>
       </c>
+      <c r="X16" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -7795,8 +7859,11 @@
       <c r="W17">
         <v>442</v>
       </c>
+      <c r="X17">
+        <v>497</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -7866,8 +7933,11 @@
       <c r="W18">
         <v>4</v>
       </c>
+      <c r="X18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -7937,8 +8007,11 @@
       <c r="W19">
         <v>152</v>
       </c>
+      <c r="X19">
+        <v>161</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -8008,8 +8081,11 @@
       <c r="W20">
         <v>424</v>
       </c>
+      <c r="X20">
+        <v>451</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -8079,8 +8155,11 @@
       <c r="W21">
         <v>11</v>
       </c>
+      <c r="X21">
+        <v>11</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -8150,8 +8229,11 @@
       <c r="W22">
         <v>1933</v>
       </c>
+      <c r="X22">
+        <v>2133</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -8221,8 +8303,11 @@
       <c r="W23">
         <v>2516</v>
       </c>
+      <c r="X23">
+        <v>2722</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -8292,8 +8377,11 @@
       <c r="W24">
         <v>19</v>
       </c>
+      <c r="X24">
+        <v>19</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -8363,8 +8451,11 @@
       <c r="W25">
         <v>99</v>
       </c>
+      <c r="X25">
+        <v>98</v>
+      </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -8434,8 +8525,11 @@
       <c r="W26">
         <v>5</v>
       </c>
+      <c r="X26">
+        <v>6</v>
+      </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -8505,8 +8599,11 @@
       <c r="W27">
         <v>14</v>
       </c>
+      <c r="X27">
+        <v>14</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -8576,8 +8673,11 @@
       <c r="W28">
         <v>106</v>
       </c>
+      <c r="X28">
+        <v>109</v>
+      </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -8647,8 +8747,11 @@
       <c r="W29">
         <v>76</v>
       </c>
+      <c r="X29">
+        <v>87</v>
+      </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -8718,8 +8821,11 @@
       <c r="W30">
         <v>22</v>
       </c>
+      <c r="X30">
+        <v>25</v>
+      </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -8813,7 +8919,7 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8931,7 +9037,7 @@
       </c>
       <c r="AA2" s="10">
         <f>SUM(va[16-Apr])</f>
-        <v>0</v>
+        <v>6889</v>
       </c>
       <c r="AB2" s="10">
         <f>SUM(va[17-Apr])</f>
@@ -9185,7 +9291,7 @@
         <v>1048</v>
       </c>
       <c r="AA3" s="10">
-        <v>0</v>
+        <v>1114</v>
       </c>
       <c r="AB3" s="10">
         <v>0</v>
@@ -9394,7 +9500,7 @@
         <v>195</v>
       </c>
       <c r="AA4" s="10">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="AB4" s="10">
         <v>0</v>
@@ -9603,7 +9709,7 @@
         <v>44169</v>
       </c>
       <c r="AA5" s="10">
-        <v>0</v>
+        <v>46444</v>
       </c>
       <c r="AB5" s="10">
         <v>0</v>
@@ -9820,7 +9926,7 @@
       <c r="Z6" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AA6" s="18" t="s">
         <v>200</v>
       </c>
       <c r="AB6" s="3" t="s">
@@ -10038,9 +10144,12 @@
       <c r="Z7" s="10">
         <v>254</v>
       </c>
+      <c r="AA7" s="10">
+        <v>275</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -10118,9 +10227,12 @@
       <c r="Z8" s="10">
         <v>4</v>
       </c>
+      <c r="AA8" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -10196,9 +10308,12 @@
       <c r="Z9" s="10">
         <v>23</v>
       </c>
+      <c r="AA9" s="10">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -10274,9 +10389,12 @@
       <c r="Z10" s="10">
         <v>2</v>
       </c>
+      <c r="AA10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -10352,9 +10470,12 @@
       <c r="Z11" s="10">
         <v>17</v>
       </c>
+      <c r="AA11" s="10">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -10430,9 +10551,12 @@
       <c r="Z12" s="10">
         <v>1</v>
       </c>
+      <c r="AA12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -10507,6 +10631,9 @@
       </c>
       <c r="Z13" s="10">
         <v>3</v>
+      </c>
+      <c r="AA13" s="10">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
@@ -10588,9 +10715,12 @@
       <c r="Z14" s="10">
         <v>420</v>
       </c>
+      <c r="AA14" s="10">
+        <v>453</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -10668,9 +10798,12 @@
       <c r="Z15" s="10">
         <v>18</v>
       </c>
+      <c r="AA15" s="10">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -10746,9 +10879,12 @@
       <c r="Z16" s="10">
         <v>0</v>
       </c>
+      <c r="AA16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -10824,9 +10960,12 @@
       <c r="Z17" s="10">
         <v>0</v>
       </c>
+      <c r="AA17" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -10902,9 +11041,12 @@
       <c r="Z18" s="10">
         <v>3</v>
       </c>
+      <c r="AA18" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -10980,9 +11122,12 @@
       <c r="Z19" s="10">
         <v>67</v>
       </c>
+      <c r="AA19" s="10">
+        <v>69</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -11058,9 +11203,12 @@
       <c r="Z20" s="10">
         <v>4</v>
       </c>
+      <c r="AA20" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -11136,9 +11284,12 @@
       <c r="Z21" s="10">
         <v>101</v>
       </c>
+      <c r="AA21" s="10">
+        <v>119</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -11214,9 +11365,12 @@
       <c r="Z22" s="10">
         <v>3</v>
       </c>
+      <c r="AA22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -11292,9 +11446,12 @@
       <c r="Z23" s="10">
         <v>2</v>
       </c>
+      <c r="AA23" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -11370,9 +11527,12 @@
       <c r="Z24" s="10">
         <v>6</v>
       </c>
+      <c r="AA24" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -11450,9 +11610,12 @@
       <c r="Z25" s="10">
         <v>10</v>
       </c>
+      <c r="AA25" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="35"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -11528,9 +11691,12 @@
       <c r="Z26" s="10">
         <v>7</v>
       </c>
+      <c r="AA26" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -11606,9 +11772,12 @@
       <c r="Z27" s="10">
         <v>16</v>
       </c>
+      <c r="AA27" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="35"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -11684,9 +11853,12 @@
       <c r="Z28" s="10">
         <v>11</v>
       </c>
+      <c r="AA28" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -11762,8 +11934,11 @@
       <c r="Z29" s="10">
         <v>34</v>
       </c>
+      <c r="AA29" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -11842,9 +12017,12 @@
       <c r="Z30" s="10">
         <v>140</v>
       </c>
+      <c r="AA30" s="10">
+        <v>143</v>
+      </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -11922,9 +12100,12 @@
       <c r="Z31" s="10">
         <v>254</v>
       </c>
+      <c r="AA31" s="10">
+        <v>267</v>
+      </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="35"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -12000,9 +12181,12 @@
       <c r="Z32" s="10">
         <v>5</v>
       </c>
+      <c r="AA32" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -12078,9 +12262,12 @@
       <c r="Z33" s="10">
         <v>17</v>
       </c>
+      <c r="AA33" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -12158,9 +12345,12 @@
       <c r="Z34" s="10">
         <v>9</v>
       </c>
+      <c r="AA34" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -12236,9 +12426,12 @@
       <c r="Z35" s="10">
         <v>40</v>
       </c>
+      <c r="AA35" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -12314,9 +12507,12 @@
       <c r="Z36" s="10">
         <v>53</v>
       </c>
+      <c r="AA36" s="10">
+        <v>61</v>
+      </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -12392,9 +12588,12 @@
       <c r="Z37" s="10">
         <v>16</v>
       </c>
+      <c r="AA37" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -12472,9 +12671,12 @@
       <c r="Z38" s="10">
         <v>7</v>
       </c>
+      <c r="AA38" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -12550,9 +12752,12 @@
       <c r="Z39" s="10">
         <v>16</v>
       </c>
+      <c r="AA39" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" s="35"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -12628,9 +12833,12 @@
       <c r="Z40" s="10">
         <v>27</v>
       </c>
+      <c r="AA40" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" s="35"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -12706,9 +12914,12 @@
       <c r="Z41" s="10">
         <v>3</v>
       </c>
+      <c r="AA41" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A42" s="35"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -12784,9 +12995,12 @@
       <c r="Z42" s="10">
         <v>10</v>
       </c>
+      <c r="AA42" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A43" s="35"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -12862,9 +13076,12 @@
       <c r="Z43" s="10">
         <v>7</v>
       </c>
+      <c r="AA43" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A44" s="35"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -12940,9 +13157,12 @@
       <c r="Z44" s="10">
         <v>14</v>
       </c>
+      <c r="AA44" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A45" s="36"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -13018,9 +13238,12 @@
       <c r="Z45" s="10">
         <v>19</v>
       </c>
+      <c r="AA45" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -13098,9 +13321,12 @@
       <c r="Z46" s="10">
         <v>12</v>
       </c>
+      <c r="AA46" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A47" s="32"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -13176,9 +13402,12 @@
       <c r="Z47" s="10">
         <v>0</v>
       </c>
+      <c r="AA47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -13254,9 +13483,12 @@
       <c r="Z48" s="10">
         <v>2</v>
       </c>
+      <c r="AA48" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A49" s="33"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -13332,9 +13564,12 @@
       <c r="Z49" s="10">
         <v>4</v>
       </c>
+      <c r="AA49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A50" s="34" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -13412,9 +13647,12 @@
       <c r="Z50" s="10">
         <v>15</v>
       </c>
+      <c r="AA50" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A51" s="36"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -13490,9 +13728,12 @@
       <c r="Z51" s="10">
         <v>4</v>
       </c>
+      <c r="AA51" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -13570,9 +13811,12 @@
       <c r="Z52" s="10">
         <v>1298</v>
       </c>
+      <c r="AA52" s="10">
+        <v>1375</v>
+      </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A53" s="32"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -13648,9 +13892,12 @@
       <c r="Z53" s="10">
         <v>0</v>
       </c>
+      <c r="AA53" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A54" s="33"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -13726,8 +13973,11 @@
       <c r="Z54" s="10">
         <v>0</v>
       </c>
+      <c r="AA54" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -13806,8 +14056,11 @@
       <c r="Z55" s="10">
         <v>75</v>
       </c>
+      <c r="AA55" s="10">
+        <v>77</v>
+      </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -13886,9 +14139,12 @@
       <c r="Z56" s="10">
         <v>453</v>
       </c>
+      <c r="AA56" s="10">
+        <v>497</v>
+      </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A57" s="34" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -13966,9 +14222,12 @@
       <c r="Z57" s="10">
         <v>6</v>
       </c>
+      <c r="AA57" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A58" s="35"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -14044,9 +14303,12 @@
       <c r="Z58" s="10">
         <v>3</v>
       </c>
+      <c r="AA58" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A59" s="35"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -14122,9 +14384,12 @@
       <c r="Z59" s="10">
         <v>15</v>
       </c>
+      <c r="AA59" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A60" s="36"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -14200,9 +14465,12 @@
       <c r="Z60" s="10">
         <v>0</v>
       </c>
+      <c r="AA60" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A61" s="31" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -14280,9 +14548,12 @@
       <c r="Z61" s="10">
         <v>6</v>
       </c>
+      <c r="AA61" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A62" s="32"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -14358,9 +14629,12 @@
       <c r="Z62" s="10">
         <v>73</v>
       </c>
+      <c r="AA62" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A63" s="32"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -14436,9 +14710,12 @@
       <c r="Z63" s="10">
         <v>6</v>
       </c>
+      <c r="AA63" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A64" s="32"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -14514,9 +14791,12 @@
       <c r="Z64" s="10">
         <v>27</v>
       </c>
+      <c r="AA64" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A65" s="32"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -14592,9 +14872,12 @@
       <c r="Z65" s="10">
         <v>20</v>
       </c>
+      <c r="AA65" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A66" s="33"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -14670,8 +14953,11 @@
       <c r="Z66" s="10">
         <v>21</v>
       </c>
+      <c r="AA66" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -14750,9 +15036,12 @@
       <c r="Z67" s="10">
         <v>367</v>
       </c>
+      <c r="AA67" s="10">
+        <v>378</v>
+      </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A68" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -14830,9 +15119,12 @@
       <c r="Z68" s="10">
         <v>0</v>
       </c>
+      <c r="AA68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A69" s="32"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -14908,9 +15200,12 @@
       <c r="Z69" s="10">
         <v>3</v>
       </c>
+      <c r="AA69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A70" s="32"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -14986,9 +15281,12 @@
       <c r="Z70" s="10">
         <v>0</v>
       </c>
+      <c r="AA70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A71" s="32"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -15064,9 +15362,12 @@
       <c r="Z71" s="10">
         <v>11</v>
       </c>
+      <c r="AA71" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A72" s="32"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -15142,9 +15443,12 @@
       <c r="Z72" s="10">
         <v>27</v>
       </c>
+      <c r="AA72" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A73" s="32"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -15220,9 +15524,12 @@
       <c r="Z73" s="10">
         <v>7</v>
       </c>
+      <c r="AA73" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A74" s="32"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -15298,9 +15605,12 @@
       <c r="Z74" s="10">
         <v>1</v>
       </c>
+      <c r="AA74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A75" s="33"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -15376,9 +15686,12 @@
       <c r="Z75" s="10">
         <v>1</v>
       </c>
+      <c r="AA75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A76" s="34" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -15456,9 +15769,12 @@
       <c r="Z76" s="10">
         <v>1</v>
       </c>
+      <c r="AA76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A77" s="35"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -15534,9 +15850,12 @@
       <c r="Z77" s="10">
         <v>4</v>
       </c>
+      <c r="AA77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A78" s="35"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -15612,9 +15931,12 @@
       <c r="Z78" s="10">
         <v>34</v>
       </c>
+      <c r="AA78" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A79" s="35"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -15690,9 +16012,12 @@
       <c r="Z79" s="10">
         <v>4</v>
       </c>
+      <c r="AA79" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A80" s="36"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -15768,8 +16093,11 @@
       <c r="Z80" s="10">
         <v>1</v>
       </c>
+      <c r="AA80" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -15848,9 +16176,12 @@
       <c r="Z81" s="10">
         <v>99</v>
       </c>
+      <c r="AA81" s="10">
+        <v>105</v>
+      </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A82" s="30" t="s">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A82" s="34" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -15928,9 +16259,12 @@
       <c r="Z82" s="10">
         <v>132</v>
       </c>
+      <c r="AA82" s="10">
+        <v>135</v>
+      </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A83" s="35"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -16006,9 +16340,12 @@
       <c r="Z83" s="10">
         <v>35</v>
       </c>
+      <c r="AA83" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A84" s="35"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -16084,9 +16421,12 @@
       <c r="Z84" s="10">
         <v>95</v>
       </c>
+      <c r="AA84" s="10">
+        <v>97</v>
+      </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A85" s="35"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -16162,9 +16502,12 @@
       <c r="Z85" s="10">
         <v>6</v>
       </c>
+      <c r="AA85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A86" s="36"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -16240,9 +16583,12 @@
       <c r="Z86" s="10">
         <v>19</v>
       </c>
+      <c r="AA86" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A87" s="31" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -16320,9 +16666,12 @@
       <c r="Z87" s="10">
         <v>10</v>
       </c>
+      <c r="AA87" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A88" s="32"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -16398,9 +16747,12 @@
       <c r="Z88" s="10">
         <v>22</v>
       </c>
+      <c r="AA88" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A89" s="32"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -16476,9 +16828,12 @@
       <c r="Z89" s="10">
         <v>5</v>
       </c>
+      <c r="AA89" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A90" s="32"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -16554,9 +16909,12 @@
       <c r="Z90" s="10">
         <v>8</v>
       </c>
+      <c r="AA90" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A91" s="32"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -16632,9 +16990,12 @@
       <c r="Z91" s="10">
         <v>3</v>
       </c>
+      <c r="AA91" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A92" s="32"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -16710,9 +17071,12 @@
       <c r="Z92" s="10">
         <v>5</v>
       </c>
+      <c r="AA92" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A93" s="33"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -16788,9 +17152,12 @@
       <c r="Z93" s="10">
         <v>15</v>
       </c>
+      <c r="AA93" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A94" s="34" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -16868,9 +17235,12 @@
       <c r="Z94" s="10">
         <v>4</v>
       </c>
+      <c r="AA94" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A95" s="36"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -16946,8 +17316,11 @@
       <c r="Z95" s="10">
         <v>22</v>
       </c>
+      <c r="AA95" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -17026,9 +17399,12 @@
       <c r="Z96" s="10">
         <v>59</v>
       </c>
+      <c r="AA96" s="10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A97" s="34" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -17106,9 +17482,12 @@
       <c r="Z97" s="10">
         <v>536</v>
       </c>
+      <c r="AA97" s="10">
+        <v>582</v>
+      </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A98" s="35"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -17184,9 +17563,12 @@
       <c r="Z98" s="10">
         <v>53</v>
       </c>
+      <c r="AA98" s="10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A99" s="36"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -17262,9 +17644,12 @@
       <c r="Z99" s="10">
         <v>14</v>
       </c>
+      <c r="AA99" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A100" s="31" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -17342,9 +17727,12 @@
       <c r="Z100" s="10">
         <v>9</v>
       </c>
+      <c r="AA100" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A101" s="32"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -17420,9 +17808,12 @@
       <c r="Z101" s="10">
         <v>17</v>
       </c>
+      <c r="AA101" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A102" s="32"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -17498,9 +17889,12 @@
       <c r="Z102" s="10">
         <v>60</v>
       </c>
+      <c r="AA102" s="10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A103" s="32"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -17576,9 +17970,12 @@
       <c r="Z103" s="10">
         <v>108</v>
       </c>
+      <c r="AA103" s="10">
+        <v>120</v>
+      </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A104" s="33"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -17654,9 +18051,12 @@
       <c r="Z104" s="10">
         <v>15</v>
       </c>
+      <c r="AA104" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A105" s="34" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -17734,9 +18134,12 @@
       <c r="Z105" s="10">
         <v>25</v>
       </c>
+      <c r="AA105" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A106" s="35"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -17812,9 +18215,12 @@
       <c r="Z106" s="10">
         <v>29</v>
       </c>
+      <c r="AA106" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A107" s="35"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -17890,9 +18296,12 @@
       <c r="Z107" s="10">
         <v>8</v>
       </c>
+      <c r="AA107" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A108" s="35"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -17968,9 +18377,12 @@
       <c r="Z108" s="10">
         <v>17</v>
       </c>
+      <c r="AA108" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A109" s="32"/>
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A109" s="36"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -18046,8 +18458,11 @@
       <c r="Z109" s="10">
         <v>1</v>
       </c>
+      <c r="AA109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -18126,8 +18541,11 @@
       <c r="Z110" s="10">
         <v>177</v>
       </c>
+      <c r="AA110" s="10">
+        <v>188</v>
+      </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -18206,9 +18624,12 @@
       <c r="Z111" s="10">
         <v>22</v>
       </c>
+      <c r="AA111" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A112" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -18286,9 +18707,12 @@
       <c r="Z112" s="10">
         <v>9</v>
       </c>
+      <c r="AA112" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A113" s="32"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -18364,9 +18788,12 @@
       <c r="Z113" s="10">
         <v>7</v>
       </c>
+      <c r="AA113" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A114" s="33"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -18442,9 +18869,12 @@
       <c r="Z114" s="10">
         <v>57</v>
       </c>
+      <c r="AA114" s="10">
+        <v>61</v>
+      </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A115" s="30" t="s">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A115" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -18522,9 +18952,12 @@
       <c r="Z115" s="10">
         <v>53</v>
       </c>
+      <c r="AA115" s="10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A116" s="31"/>
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A116" s="35"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -18600,9 +19033,12 @@
       <c r="Z116" s="10">
         <v>62</v>
       </c>
+      <c r="AA116" s="10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A117" s="35"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -18678,9 +19114,12 @@
       <c r="Z117" s="10">
         <v>5</v>
       </c>
+      <c r="AA117" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A118" s="35"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -18756,9 +19195,12 @@
       <c r="Z118" s="10">
         <v>29</v>
       </c>
+      <c r="AA118" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A119" s="35"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -18834,9 +19276,12 @@
       <c r="Z119" s="10">
         <v>5</v>
       </c>
+      <c r="AA119" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A120" s="36"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -18912,9 +19357,12 @@
       <c r="Z120" s="10">
         <v>38</v>
       </c>
+      <c r="AA120" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A121" s="33" t="s">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A121" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -18992,9 +19440,12 @@
       <c r="Z121" s="10">
         <v>0</v>
       </c>
+      <c r="AA121" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A122" s="32"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -19070,9 +19521,12 @@
       <c r="Z122" s="10">
         <v>20</v>
       </c>
+      <c r="AA122" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A123" s="32"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -19148,9 +19602,12 @@
       <c r="Z123" s="10">
         <v>2</v>
       </c>
+      <c r="AA123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A124" s="32"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -19226,9 +19683,12 @@
       <c r="Z124" s="10">
         <v>2</v>
       </c>
+      <c r="AA124" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A125" s="32"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -19304,9 +19764,12 @@
       <c r="Z125" s="10">
         <v>1</v>
       </c>
+      <c r="AA125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A126" s="32"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -19382,9 +19845,12 @@
       <c r="Z126" s="10">
         <v>3</v>
       </c>
+      <c r="AA126" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A127" s="32"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -19460,9 +19926,12 @@
       <c r="Z127" s="10">
         <v>3</v>
       </c>
+      <c r="AA127" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A128" s="32"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -19538,9 +20007,12 @@
       <c r="Z128" s="10">
         <v>4</v>
       </c>
+      <c r="AA128" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A129" s="32"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -19616,9 +20088,12 @@
       <c r="Z129" s="10">
         <v>7</v>
       </c>
+      <c r="AA129" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A130" s="33"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -19694,8 +20169,11 @@
       <c r="Z130" s="10">
         <v>8</v>
       </c>
+      <c r="AA130" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -19774,9 +20252,12 @@
       <c r="Z131" s="10">
         <v>256</v>
       </c>
+      <c r="AA131" s="10">
+        <v>258</v>
+      </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A132" s="33" t="s">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A132" s="31" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -19854,9 +20335,12 @@
       <c r="Z132" s="10">
         <v>15</v>
       </c>
+      <c r="AA132" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A133" s="32"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -19932,9 +20416,12 @@
       <c r="Z133" s="10">
         <v>8</v>
       </c>
+      <c r="AA133" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A134" s="32"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -20010,9 +20497,12 @@
       <c r="Z134" s="10">
         <v>0</v>
       </c>
+      <c r="AA134" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A135" s="35"/>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A135" s="33"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -20088,9 +20578,12 @@
       <c r="Z135" s="10">
         <v>0</v>
       </c>
+      <c r="AA135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A136" s="34" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -20168,9 +20661,12 @@
       <c r="Z136" s="10">
         <v>60</v>
       </c>
+      <c r="AA136" s="10">
+        <v>63</v>
+      </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A137" s="35"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -20246,9 +20742,12 @@
       <c r="Z137" s="10">
         <v>6</v>
       </c>
+      <c r="AA137" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A138" s="35"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -20324,9 +20823,12 @@
       <c r="Z138" s="10">
         <v>7</v>
       </c>
+      <c r="AA138" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A139" s="32"/>
+    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A139" s="36"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -20401,10 +20903,25 @@
       </c>
       <c r="Z139" s="10">
         <v>59</v>
+      </c>
+      <c r="AA139" s="10">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -20417,18 +20934,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -20675,7 +21180,7 @@
       </c>
       <c r="AI2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24.48</v>
       </c>
       <c r="AJ2" s="19">
         <f t="shared" si="1"/>
@@ -21325,7 +21830,7 @@
       </c>
       <c r="AI4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.8823529411764701</v>
       </c>
       <c r="AJ4" s="10">
         <f t="shared" si="7"/>
@@ -21650,7 +22155,7 @@
       </c>
       <c r="AI6" s="12">
         <f>MAX(0, (dc!AI2-dc!AH2))</f>
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="AJ6" s="12">
         <f>MAX(0, (dc!AJ2-dc!AI2))</f>
@@ -21974,7 +22479,7 @@
       </c>
       <c r="AI7" s="12">
         <f>MAX(0, (dc!AI3-dc!AH3))</f>
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="AJ7" s="12">
         <f>MAX(0, (dc!AJ3-dc!AI3))</f>
@@ -22622,7 +23127,7 @@
       </c>
       <c r="AI9" s="12">
         <f>MAX(0, (dc!AI5-dc!AH5))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AJ9" s="12">
         <f>MAX(0, (dc!AJ5-dc!AI5))</f>
@@ -23174,7 +23679,7 @@
       </c>
       <c r="AI11" s="10">
         <f>MAX(0,(dc!AI7-dc!AH7))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AJ11" s="10">
         <f>MAX(0,(dc!AJ7-dc!AI7))</f>
@@ -23481,7 +23986,7 @@
       </c>
       <c r="AI12" s="10">
         <f>MAX(0,(dc!AI8-dc!AH8))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AJ12" s="10">
         <f>MAX(0,(dc!AJ8-dc!AI8))</f>
@@ -23788,7 +24293,7 @@
       </c>
       <c r="AI13" s="10">
         <f>MAX(0,(dc!AI9-dc!AH9))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AJ13" s="10">
         <f>MAX(0,(dc!AJ9-dc!AI9))</f>
@@ -24095,7 +24600,7 @@
       </c>
       <c r="AI14" s="10">
         <f>MAX(0,(dc!AI10-dc!AH10))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AJ14" s="10">
         <f>MAX(0,(dc!AJ10-dc!AI10))</f>
@@ -24402,7 +24907,7 @@
       </c>
       <c r="AI15" s="10">
         <f>MAX(0,(dc!AI11-dc!AH11))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ15" s="10">
         <f>MAX(0,(dc!AJ11-dc!AI11))</f>
@@ -24709,7 +25214,7 @@
       </c>
       <c r="AI16" s="10">
         <f>MAX(0,(dc!AI12-dc!AH12))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AJ16" s="10">
         <f>MAX(0,(dc!AJ12-dc!AI12))</f>
@@ -25016,7 +25521,7 @@
       </c>
       <c r="AI17" s="10">
         <f>MAX(0,(dc!AI13-dc!AH13))</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AJ17" s="10">
         <f>MAX(0,(dc!AJ13-dc!AI13))</f>
@@ -25323,7 +25828,7 @@
       </c>
       <c r="AI18" s="10">
         <f>MAX(0,(dc!AI14-dc!AH14))</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AJ18" s="10">
         <f>MAX(0,(dc!AJ14-dc!AI14))</f>
@@ -26024,7 +26529,7 @@
       </c>
       <c r="X2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24.415584415584416</v>
       </c>
       <c r="Y2" s="21">
         <f t="shared" si="0"/>
@@ -26297,7 +26802,7 @@
       </c>
       <c r="X3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>29.25531914893617</v>
       </c>
       <c r="Y3" s="21">
         <f t="shared" si="2"/>
@@ -26570,7 +27075,7 @@
       </c>
       <c r="X4" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.7180851063829783</v>
       </c>
       <c r="Y4" s="21">
         <f t="shared" si="4"/>
@@ -26906,7 +27411,7 @@
       </c>
       <c r="X6" s="14">
         <f>MAX(0,(md!X2-md!W2)+(md!X3-md!W3))</f>
-        <v>0</v>
+        <v>3080</v>
       </c>
       <c r="Y6" s="14">
         <f>MAX(0,(md!Y2-md!X2)+(md!Y3-md!X3))</f>
@@ -27178,7 +27683,7 @@
       </c>
       <c r="X7" s="14">
         <f>MAX(0,(md!X3-md!W3))</f>
-        <v>0</v>
+        <v>752</v>
       </c>
       <c r="Y7" s="14">
         <f>MAX(0,(md!Y3-md!X3))</f>
@@ -27450,7 +27955,7 @@
       </c>
       <c r="X8" s="14">
         <f>MAX(0,(md!X4-md!W4))</f>
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="Y8" s="14">
         <f>MAX(0,(md!Y4-md!X4))</f>
@@ -27722,7 +28227,7 @@
       </c>
       <c r="X9" s="14">
         <f>MAX(0,(md!X5-md!W5))</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="Y9" s="14">
         <f>MAX(0,(md!Y5-md!X5))</f>
@@ -28208,7 +28713,7 @@
       </c>
       <c r="X11" s="14">
         <f>MAX(0,(md!X7-md!W7))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="14">
         <f>MAX(0,(md!Y7-md!X7))</f>
@@ -28485,7 +28990,7 @@
       </c>
       <c r="X12" s="14">
         <f>MAX(0,(md!X9-md!W9))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y12" s="14">
         <f>MAX(0,(md!Y9-md!X9))</f>
@@ -28762,7 +29267,7 @@
       </c>
       <c r="X13" s="14">
         <f>MAX(0,(md!X9-md!W9))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y13" s="14">
         <f>MAX(0,(md!Y9-md!X9))</f>
@@ -29039,7 +29544,7 @@
       </c>
       <c r="X14" s="14">
         <f>MAX(0,(md!X10-md!W10))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="Y14" s="14">
         <f>MAX(0,(md!Y10-md!X10))</f>
@@ -29316,7 +29821,7 @@
       </c>
       <c r="X15" s="14">
         <f>MAX(0,(md!X11-md!W11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="14">
         <f>MAX(0,(md!Y11-md!X11))</f>
@@ -29593,7 +30098,7 @@
       </c>
       <c r="X16" s="14">
         <f>MAX(0,(md!X12-md!W12))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="14">
         <f>MAX(0,(md!Y12-md!X12))</f>
@@ -29870,7 +30375,7 @@
       </c>
       <c r="X17" s="14">
         <f>MAX(0,(md!X13-md!W13))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="Y17" s="14">
         <f>MAX(0,(md!Y13-md!X13))</f>
@@ -30147,7 +30652,7 @@
       </c>
       <c r="X18" s="14">
         <f>MAX(0,(md!X14-md!W14))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Y18" s="14">
         <f>MAX(0,(md!Y14-md!X14))</f>
@@ -30424,7 +30929,7 @@
       </c>
       <c r="X19" s="14">
         <f>MAX(0,(md!X15-md!W15))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="Y19" s="14">
         <f>MAX(0,(md!Y15-md!X15))</f>
@@ -30701,7 +31206,7 @@
       </c>
       <c r="X20" s="14">
         <f>MAX(0,(md!X16-md!W16))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y20" s="14">
         <f>MAX(0,(md!Y16-md!X16))</f>
@@ -30978,7 +31483,7 @@
       </c>
       <c r="X21" s="14">
         <f>MAX(0,(md!X17-md!W17))</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="Y21" s="14">
         <f>MAX(0,(md!Y17-md!X17))</f>
@@ -31532,7 +32037,7 @@
       </c>
       <c r="X23" s="14">
         <f>MAX(0,(md!X19-md!W19))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Y23" s="14">
         <f>MAX(0,(md!Y19-md!X19))</f>
@@ -31809,7 +32314,7 @@
       </c>
       <c r="X24" s="14">
         <f>MAX(0,(md!X20-md!W20))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Y24" s="14">
         <f>MAX(0,(md!Y20-md!X20))</f>
@@ -32363,7 +32868,7 @@
       </c>
       <c r="X26" s="14">
         <f>MAX(0,(md!X22-md!W22))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Y26" s="14">
         <f>MAX(0,(md!Y22-md!X22))</f>
@@ -32640,7 +33145,7 @@
       </c>
       <c r="X27" s="14">
         <f>MAX(0,(md!X23-md!W23))</f>
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="Y27" s="14">
         <f>MAX(0,(md!Y23-md!X23))</f>
@@ -33471,7 +33976,7 @@
       </c>
       <c r="X30" s="14">
         <f>MAX(0,(md!X26-md!W26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y30" s="14">
         <f>MAX(0,(md!Y26-md!X26))</f>
@@ -34025,7 +34530,7 @@
       </c>
       <c r="X32" s="14">
         <f>MAX(0,(md!X28-md!W28))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y32" s="14">
         <f>MAX(0,(md!Y28-md!X28))</f>
@@ -34302,7 +34807,7 @@
       </c>
       <c r="X33" s="14">
         <f>MAX(0,(md!X29-md!W29))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Y33" s="14">
         <f>MAX(0,(md!Y29-md!X29))</f>
@@ -34579,7 +35084,7 @@
       </c>
       <c r="X34" s="14">
         <f>MAX(0,(md!X30-md!W30))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y34" s="14">
         <f>MAX(0,(md!Y30-md!X30))</f>
@@ -34943,8 +35448,8 @@
   </sheetPr>
   <dimension ref="A1:BS143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="X66" sqref="X66"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35058,7 +35563,7 @@
       </c>
       <c r="Z2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.098901098901099</v>
       </c>
       <c r="AA2" s="20">
         <f t="shared" si="0"/>
@@ -35335,7 +35840,7 @@
       </c>
       <c r="Z3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16.966580976863753</v>
       </c>
       <c r="AA3" s="20">
         <f t="shared" si="2"/>
@@ -35612,7 +36117,7 @@
       </c>
       <c r="Z4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.3419023136246784</v>
       </c>
       <c r="AA4" s="20">
         <f t="shared" si="4"/>
@@ -35889,7 +36394,7 @@
       </c>
       <c r="Z6" s="14">
         <f>MAX(0,(va!AA5-va!Z5))</f>
-        <v>0</v>
+        <v>2275</v>
       </c>
       <c r="AA6" s="14">
         <f>MAX(0,(va!AB5-va!AA5))</f>
@@ -36166,7 +36671,7 @@
       </c>
       <c r="Z7" s="14">
         <f>MAX(0,(va!AA2-va!Z2))</f>
-        <v>0</v>
+        <v>389</v>
       </c>
       <c r="AA7" s="14">
         <f>MAX(0,(va!AB2-va!AA2))</f>
@@ -36443,7 +36948,7 @@
       </c>
       <c r="Z8" s="14">
         <f>MAX(0,(va!AA3-va!Z3))</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AA8" s="14">
         <f>MAX(0,(va!AB3-va!AA3))</f>
@@ -36720,7 +37225,7 @@
       </c>
       <c r="Z9" s="14">
         <f>MAX(0,(va!AA4-va!Z4))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AA9" s="14">
         <f>MAX(0,(va!AB4-va!AA4))</f>
@@ -37217,7 +37722,7 @@
       </c>
       <c r="Z11" s="16">
         <f>MAX(0,(va!AA7-va!Z7))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AA11" s="16">
         <f>MAX(0,(va!AB7-va!AA7))</f>
@@ -38345,7 +38850,7 @@
       </c>
       <c r="Z15" s="16">
         <f>MAX(0,(va!AA11-va!Z11))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA15" s="16">
         <f>MAX(0,(va!AB11-va!AA11))</f>
@@ -38909,7 +39414,7 @@
       </c>
       <c r="Z17" s="16">
         <f>MAX(0,(va!AA13-va!Z13))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17" s="16">
         <f>MAX(0,(va!AB13-va!AA13))</f>
@@ -39191,7 +39696,7 @@
       </c>
       <c r="Z18" s="16">
         <f>MAX(0,(va!AA14-va!Z14))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AA18" s="16">
         <f>MAX(0,(va!AB14-va!AA14))</f>
@@ -39473,7 +39978,7 @@
       </c>
       <c r="Z19" s="16">
         <f>MAX(0,(va!AA15-va!Z15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19" s="16">
         <f>MAX(0,(va!AB15-va!AA15))</f>
@@ -40601,7 +41106,7 @@
       </c>
       <c r="Z23" s="16">
         <f>MAX(0,(va!AA19-va!Z19))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA23" s="16">
         <f>MAX(0,(va!AB19-va!AA19))</f>
@@ -41165,7 +41670,7 @@
       </c>
       <c r="Z25" s="16">
         <f>MAX(0,(va!AA21-va!Z21))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AA25" s="16">
         <f>MAX(0,(va!AB21-va!AA21))</f>
@@ -41729,7 +42234,7 @@
       </c>
       <c r="Z27" s="16">
         <f>MAX(0,(va!AA23-va!Z23))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA27" s="16">
         <f>MAX(0,(va!AB23-va!AA23))</f>
@@ -43703,7 +44208,7 @@
       </c>
       <c r="Z34" s="16">
         <f>MAX(0,(va!AA30-va!Z30))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA34" s="16">
         <f>MAX(0,(va!AB30-va!AA30))</f>
@@ -43985,7 +44490,7 @@
       </c>
       <c r="Z35" s="16">
         <f>MAX(0,(va!AA31-va!Z31))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AA35" s="16">
         <f>MAX(0,(va!AB31-va!AA31))</f>
@@ -44549,7 +45054,7 @@
       </c>
       <c r="Z37" s="16">
         <f>MAX(0,(va!AA33-va!Z33))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA37" s="16">
         <f>MAX(0,(va!AB33-va!AA33))</f>
@@ -45113,7 +45618,7 @@
       </c>
       <c r="Z39" s="16">
         <f>MAX(0,(va!AA35-va!Z35))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA39" s="16">
         <f>MAX(0,(va!AB35-va!AA35))</f>
@@ -45395,7 +45900,7 @@
       </c>
       <c r="Z40" s="16">
         <f>MAX(0,(va!AA36-va!Z36))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA40" s="16">
         <f>MAX(0,(va!AB36-va!AA36))</f>
@@ -49343,7 +49848,7 @@
       </c>
       <c r="Z54" s="16">
         <f>MAX(0,(va!AA50-va!Z50))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA54" s="16">
         <f>MAX(0,(va!AB50-va!AA50))</f>
@@ -49907,7 +50412,7 @@
       </c>
       <c r="Z56" s="16">
         <f>MAX(0,(va!AA52-va!Z52))</f>
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="AA56" s="16">
         <f>MAX(0,(va!AB52-va!AA52))</f>
@@ -50753,7 +51258,7 @@
       </c>
       <c r="Z59" s="16">
         <f>MAX(0,(va!AA55-va!Z55))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA59" s="16">
         <f>MAX(0,(va!AB55-va!AA55))</f>
@@ -51035,7 +51540,7 @@
       </c>
       <c r="Z60" s="16">
         <f>MAX(0,(va!AA56-va!Z56))</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="AA60" s="16">
         <f>MAX(0,(va!AB56-va!AA56))</f>
@@ -51881,7 +52386,7 @@
       </c>
       <c r="Z63" s="16">
         <f>MAX(0,(va!AA59-va!Z59))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA63" s="16">
         <f>MAX(0,(va!AB59-va!AA59))</f>
@@ -53009,7 +53514,7 @@
       </c>
       <c r="Z67" s="16">
         <f>MAX(0,(va!AA63-va!Z63))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA67" s="16">
         <f>MAX(0,(va!AB63-va!AA63))</f>
@@ -53291,7 +53796,7 @@
       </c>
       <c r="Z68" s="16">
         <f>MAX(0,(va!AA64-va!Z64))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA68" s="16">
         <f>MAX(0,(va!AB64-va!AA64))</f>
@@ -53573,7 +54078,7 @@
       </c>
       <c r="Z69" s="16">
         <f>MAX(0,(va!AA65-va!Z65))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA69" s="16">
         <f>MAX(0,(va!AB65-va!AA65))</f>
@@ -54137,7 +54642,7 @@
       </c>
       <c r="Z71" s="16">
         <f>MAX(0,(va!AA67-va!Z67))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AA71" s="16">
         <f>MAX(0,(va!AB67-va!AA67))</f>
@@ -57521,7 +58026,7 @@
       </c>
       <c r="Z83" s="16">
         <f>MAX(0,(va!AA79-va!Z79))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA83" s="16">
         <f>MAX(0,(va!AB79-va!AA79))</f>
@@ -58085,7 +58590,7 @@
       </c>
       <c r="Z85" s="16">
         <f>MAX(0,(va!AA81-va!Z81))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA85" s="16">
         <f>MAX(0,(va!AB81-va!AA81))</f>
@@ -58367,7 +58872,7 @@
       </c>
       <c r="Z86" s="16">
         <f>MAX(0,(va!AA82-va!Z82))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA86" s="16">
         <f>MAX(0,(va!AB82-va!AA82))</f>
@@ -58649,7 +59154,7 @@
       </c>
       <c r="Z87" s="16">
         <f>MAX(0,(va!AA83-va!Z83))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA87" s="16">
         <f>MAX(0,(va!AB83-va!AA83))</f>
@@ -58931,7 +59436,7 @@
       </c>
       <c r="Z88" s="16">
         <f>MAX(0,(va!AA84-va!Z84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA88" s="16">
         <f>MAX(0,(va!AB84-va!AA84))</f>
@@ -59777,7 +60282,7 @@
       </c>
       <c r="Z91" s="16">
         <f>MAX(0,(va!AA87-va!Z87))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA91" s="16">
         <f>MAX(0,(va!AB87-va!AA87))</f>
@@ -60059,7 +60564,7 @@
       </c>
       <c r="Z92" s="16">
         <f>MAX(0,(va!AA88-va!Z88))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA92" s="16">
         <f>MAX(0,(va!AB88-va!AA88))</f>
@@ -60341,7 +60846,7 @@
       </c>
       <c r="Z93" s="16">
         <f>MAX(0,(va!AA89-va!Z89))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA93" s="16">
         <f>MAX(0,(va!AB89-va!AA89))</f>
@@ -61751,7 +62256,7 @@
       </c>
       <c r="Z98" s="16">
         <f>MAX(0,(va!AA94-va!Z94))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA98" s="16">
         <f>MAX(0,(va!AB94-va!AA94))</f>
@@ -62315,7 +62820,7 @@
       </c>
       <c r="Z100" s="16">
         <f>MAX(0,(va!AA96-va!Z96))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA100" s="16">
         <f>MAX(0,(va!AB96-va!AA96))</f>
@@ -62597,7 +63102,7 @@
       </c>
       <c r="Z101" s="16">
         <f>MAX(0,(va!AA97-va!Z97))</f>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AA101" s="16">
         <f>MAX(0,(va!AB97-va!AA97))</f>
@@ -62879,7 +63384,7 @@
       </c>
       <c r="Z102" s="16">
         <f>MAX(0,(va!AA98-va!Z98))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AA102" s="16">
         <f>MAX(0,(va!AB98-va!AA98))</f>
@@ -63161,7 +63666,7 @@
       </c>
       <c r="Z103" s="16">
         <f>MAX(0,(va!AA99-va!Z99))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA103" s="16">
         <f>MAX(0,(va!AB99-va!AA99))</f>
@@ -63443,7 +63948,7 @@
       </c>
       <c r="Z104" s="16">
         <f>MAX(0,(va!AA100-va!Z100))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA104" s="16">
         <f>MAX(0,(va!AB100-va!AA100))</f>
@@ -63725,7 +64230,7 @@
       </c>
       <c r="Z105" s="16">
         <f>MAX(0,(va!AA101-va!Z101))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA105" s="16">
         <f>MAX(0,(va!AB101-va!AA101))</f>
@@ -64007,7 +64512,7 @@
       </c>
       <c r="Z106" s="16">
         <f>MAX(0,(va!AA102-va!Z102))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA106" s="16">
         <f>MAX(0,(va!AB102-va!AA102))</f>
@@ -64289,7 +64794,7 @@
       </c>
       <c r="Z107" s="16">
         <f>MAX(0,(va!AA103-va!Z103))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AA107" s="16">
         <f>MAX(0,(va!AB103-va!AA103))</f>
@@ -64853,7 +65358,7 @@
       </c>
       <c r="Z109" s="16">
         <f>MAX(0,(va!AA105-va!Z105))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA109" s="16">
         <f>MAX(0,(va!AB105-va!AA105))</f>
@@ -65135,7 +65640,7 @@
       </c>
       <c r="Z110" s="16">
         <f>MAX(0,(va!AA106-va!Z106))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA110" s="16">
         <f>MAX(0,(va!AB106-va!AA106))</f>
@@ -65699,7 +66204,7 @@
       </c>
       <c r="Z112" s="16">
         <f>MAX(0,(va!AA108-va!Z108))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA112" s="16">
         <f>MAX(0,(va!AB108-va!AA108))</f>
@@ -66263,7 +66768,7 @@
       </c>
       <c r="Z114" s="16">
         <f>MAX(0,(va!AA110-va!Z110))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AA114" s="16">
         <f>MAX(0,(va!AB110-va!AA110))</f>
@@ -66545,7 +67050,7 @@
       </c>
       <c r="Z115" s="16">
         <f>MAX(0,(va!AA111-va!Z111))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA115" s="16">
         <f>MAX(0,(va!AB111-va!AA111))</f>
@@ -66827,7 +67332,7 @@
       </c>
       <c r="Z116" s="16">
         <f>MAX(0,(va!AA112-va!Z112))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA116" s="16">
         <f>MAX(0,(va!AB112-va!AA112))</f>
@@ -67391,7 +67896,7 @@
       </c>
       <c r="Z118" s="16">
         <f>MAX(0,(va!AA114-va!Z114))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA118" s="16">
         <f>MAX(0,(va!AB114-va!AA114))</f>
@@ -67673,7 +68178,7 @@
       </c>
       <c r="Z119" s="16">
         <f>MAX(0,(va!AA115-va!Z115))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA119" s="16">
         <f>MAX(0,(va!AB115-va!AA115))</f>
@@ -67955,7 +68460,7 @@
       </c>
       <c r="Z120" s="16">
         <f>MAX(0,(va!AA116-va!Z116))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA120" s="16">
         <f>MAX(0,(va!AB116-va!AA116))</f>
@@ -68519,7 +69024,7 @@
       </c>
       <c r="Z122" s="16">
         <f>MAX(0,(va!AA118-va!Z118))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA122" s="16">
         <f>MAX(0,(va!AB118-va!AA118))</f>
@@ -69365,7 +69870,7 @@
       </c>
       <c r="Z125" s="16">
         <f>MAX(0,(va!AA121-va!Z121))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA125" s="16">
         <f>MAX(0,(va!AB121-va!AA121))</f>
@@ -71339,7 +71844,7 @@
       </c>
       <c r="Z132" s="16">
         <f>MAX(0,(va!AA128-va!Z128))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA132" s="16">
         <f>MAX(0,(va!AB128-va!AA128))</f>
@@ -71903,7 +72408,7 @@
       </c>
       <c r="Z134" s="16">
         <f>MAX(0,(va!AA130-va!Z130))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA134" s="16">
         <f>MAX(0,(va!AB130-va!AA130))</f>
@@ -72185,7 +72690,7 @@
       </c>
       <c r="Z135" s="16">
         <f>MAX(0,(va!AA131-va!Z131))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA135" s="16">
         <f>MAX(0,(va!AB131-va!AA131))</f>
@@ -73595,7 +74100,7 @@
       </c>
       <c r="Z140" s="16">
         <f>MAX(0,(va!AA136-va!Z136))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA140" s="16">
         <f>MAX(0,(va!AB136-va!AA136))</f>
@@ -74159,7 +74664,7 @@
       </c>
       <c r="Z142" s="16">
         <f>MAX(0,(va!AA138-va!Z138))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA142" s="16">
         <f>MAX(0,(va!AB138-va!AA138))</f>
@@ -74441,7 +74946,7 @@
       </c>
       <c r="Z143" s="16">
         <f>MAX(0,(va!AA139-va!Z139))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA143" s="16">
         <f>MAX(0,(va!AB139-va!AA139))</f>

</xml_diff>

<commit_message>
18 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127C18EC-D546-47F4-8E64-10AA1331D5B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1EA7E9-70D6-4319-B314-6AF6C53EAF68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="5120" windowWidth="20520" windowHeight="13130" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="6840" yWindow="5110" windowWidth="20520" windowHeight="13130" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1066,6 +1066,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1075,17 +1086,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4027,7 +4027,7 @@
   <dimension ref="A1:CC46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4152,6 +4152,9 @@
       <c r="AJ2" s="12">
         <v>12643</v>
       </c>
+      <c r="AK2" s="12">
+        <v>13268</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -4284,7 +4287,7 @@
       </c>
       <c r="AK3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2666</v>
       </c>
       <c r="AL3" s="10">
         <f t="shared" si="0"/>
@@ -4577,6 +4580,9 @@
       <c r="AJ5" s="10">
         <v>86</v>
       </c>
+      <c r="AK5" s="10">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -4929,8 +4935,11 @@
       <c r="AI7" s="31">
         <v>264</v>
       </c>
-      <c r="AJ7" s="39">
+      <c r="AJ7" s="33">
         <v>282</v>
+      </c>
+      <c r="AK7" s="10">
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.35">
@@ -5039,8 +5048,11 @@
       <c r="AI8" s="31">
         <v>193</v>
       </c>
-      <c r="AJ8" s="39">
+      <c r="AJ8" s="33">
         <v>207</v>
+      </c>
+      <c r="AK8" s="10">
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.35">
@@ -5149,8 +5161,11 @@
       <c r="AI9" s="31">
         <v>169</v>
       </c>
-      <c r="AJ9" s="39">
+      <c r="AJ9" s="33">
         <v>176</v>
+      </c>
+      <c r="AK9" s="10">
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.35">
@@ -5259,8 +5274,11 @@
       <c r="AI10" s="31">
         <v>389</v>
       </c>
-      <c r="AJ10" s="39">
+      <c r="AJ10" s="33">
         <v>423</v>
+      </c>
+      <c r="AK10" s="10">
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.35">
@@ -5369,8 +5387,11 @@
       <c r="AI11" s="31">
         <v>311</v>
       </c>
-      <c r="AJ11" s="39">
+      <c r="AJ11" s="33">
         <v>328</v>
+      </c>
+      <c r="AK11" s="10">
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.35">
@@ -5479,8 +5500,11 @@
       <c r="AI12" s="31">
         <v>313</v>
       </c>
-      <c r="AJ12" s="39">
+      <c r="AJ12" s="33">
         <v>337</v>
+      </c>
+      <c r="AK12" s="10">
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.35">
@@ -5589,8 +5613,11 @@
       <c r="AI13" s="31">
         <v>361</v>
       </c>
-      <c r="AJ13" s="39">
+      <c r="AJ13" s="33">
         <v>382</v>
+      </c>
+      <c r="AK13" s="10">
+        <v>402</v>
       </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.35">
@@ -5699,8 +5726,11 @@
       <c r="AI14" s="31">
         <v>293</v>
       </c>
-      <c r="AJ14" s="39">
+      <c r="AJ14" s="33">
         <v>316</v>
+      </c>
+      <c r="AK14" s="10">
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.35">
@@ -5809,8 +5839,11 @@
       <c r="AI15" s="31">
         <v>57</v>
       </c>
-      <c r="AJ15" s="39">
+      <c r="AJ15" s="33">
         <v>25</v>
+      </c>
+      <c r="AK15" s="10">
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.35">
@@ -5966,7 +5999,7 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6059,7 +6092,7 @@
         <v>50437</v>
       </c>
       <c r="Z2" s="10">
-        <v>0</v>
+        <v>53062</v>
       </c>
       <c r="AA2" s="10">
         <v>0</v>
@@ -6288,7 +6321,7 @@
       </c>
       <c r="Z3" s="10">
         <f>SUM(md[18-Apr])</f>
-        <v>0</v>
+        <v>12308</v>
       </c>
       <c r="AA3" s="10">
         <f>SUM(md[19-Apr])</f>
@@ -6537,7 +6570,7 @@
         <v>2612</v>
       </c>
       <c r="Z4" s="10">
-        <v>0</v>
+        <v>2757</v>
       </c>
       <c r="AA4" s="10">
         <v>0</v>
@@ -6743,7 +6776,7 @@
         <v>425</v>
       </c>
       <c r="Z5" s="10">
-        <v>0</v>
+        <v>463</v>
       </c>
       <c r="AA5" s="10">
         <v>0</v>
@@ -6951,7 +6984,7 @@
       <c r="Y6" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="18" t="s">
         <v>202</v>
       </c>
       <c r="AA6" s="3" t="s">
@@ -7160,6 +7193,9 @@
       <c r="Y7" s="31">
         <v>26</v>
       </c>
+      <c r="Z7">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -7237,6 +7273,9 @@
       <c r="Y8" s="31">
         <v>966</v>
       </c>
+      <c r="Z8" s="10">
+        <v>1005</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -7311,8 +7350,11 @@
       <c r="X9">
         <v>1160</v>
       </c>
-      <c r="Y9" s="38">
+      <c r="Y9" s="32">
         <v>1273</v>
+      </c>
+      <c r="Z9">
+        <v>1378</v>
       </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.35">
@@ -7388,8 +7430,11 @@
       <c r="X10">
         <v>1516</v>
       </c>
-      <c r="Y10" s="38">
+      <c r="Y10" s="32">
         <v>1569</v>
+      </c>
+      <c r="Z10">
+        <v>1664</v>
       </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.35">
@@ -7468,6 +7513,9 @@
       <c r="Y11" s="31">
         <v>109</v>
       </c>
+      <c r="Z11">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -7545,6 +7593,9 @@
       <c r="Y12" s="31">
         <v>28</v>
       </c>
+      <c r="Z12">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -7622,6 +7673,9 @@
       <c r="Y13" s="31">
         <v>288</v>
       </c>
+      <c r="Z13">
+        <v>308</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -7699,6 +7753,9 @@
       <c r="Y14" s="31">
         <v>127</v>
       </c>
+      <c r="Z14">
+        <v>131</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -7776,6 +7833,9 @@
       <c r="Y15" s="31">
         <v>337</v>
       </c>
+      <c r="Z15">
+        <v>347</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -7853,8 +7913,11 @@
       <c r="Y16" s="31">
         <v>20</v>
       </c>
+      <c r="Z16" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -7930,8 +7993,11 @@
       <c r="Y17" s="31">
         <v>525</v>
       </c>
+      <c r="Z17">
+        <v>557</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8007,8 +8073,11 @@
       <c r="Y18" s="31">
         <v>4</v>
       </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8084,8 +8153,11 @@
       <c r="Y19" s="31">
         <v>176</v>
       </c>
+      <c r="Z19">
+        <v>195</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -8161,8 +8233,11 @@
       <c r="Y20" s="31">
         <v>475</v>
       </c>
+      <c r="Z20">
+        <v>508</v>
+      </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -8238,8 +8313,11 @@
       <c r="Y21" s="31">
         <v>14</v>
       </c>
+      <c r="Z21">
+        <v>16</v>
+      </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -8312,11 +8390,14 @@
       <c r="X22">
         <v>2133</v>
       </c>
-      <c r="Y22" s="38">
+      <c r="Y22" s="32">
         <v>2280</v>
       </c>
+      <c r="Z22">
+        <v>2404</v>
+      </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -8389,11 +8470,14 @@
       <c r="X23">
         <v>2722</v>
       </c>
-      <c r="Y23" s="38">
+      <c r="Y23" s="32">
         <v>2966</v>
       </c>
+      <c r="Z23">
+        <v>3160</v>
+      </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -8469,8 +8553,11 @@
       <c r="Y24" s="31">
         <v>19</v>
       </c>
+      <c r="Z24">
+        <v>24</v>
+      </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -8546,8 +8633,11 @@
       <c r="Y25" s="31">
         <v>100</v>
       </c>
+      <c r="Z25">
+        <v>101</v>
+      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -8623,8 +8713,11 @@
       <c r="Y26" s="31">
         <v>9</v>
       </c>
+      <c r="Z26">
+        <v>10</v>
+      </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -8700,8 +8793,11 @@
       <c r="Y27" s="31">
         <v>14</v>
       </c>
+      <c r="Z27">
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -8777,8 +8873,11 @@
       <c r="Y28" s="31">
         <v>116</v>
       </c>
+      <c r="Z28">
+        <v>116</v>
+      </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -8854,8 +8953,11 @@
       <c r="Y29" s="31">
         <v>103</v>
       </c>
+      <c r="Z29">
+        <v>138</v>
+      </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -8931,8 +9033,11 @@
       <c r="Y30" s="31">
         <v>28</v>
       </c>
+      <c r="Z30">
+        <v>31</v>
+      </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -9026,7 +9131,7 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9152,7 +9257,7 @@
       </c>
       <c r="AC2" s="10">
         <f>SUM(va[18-Apr])</f>
-        <v>0</v>
+        <v>8053</v>
       </c>
       <c r="AD2" s="10">
         <f>SUM(va[19-Apr])</f>
@@ -9404,7 +9509,7 @@
         <v>1221</v>
       </c>
       <c r="AC3" s="10">
-        <v>0</v>
+        <v>1296</v>
       </c>
       <c r="AD3" s="10">
         <v>0</v>
@@ -9613,7 +9718,7 @@
         <v>231</v>
       </c>
       <c r="AC4" s="10">
-        <v>0</v>
+        <v>258</v>
       </c>
       <c r="AD4" s="10">
         <v>0</v>
@@ -9822,7 +9927,7 @@
         <v>48997</v>
       </c>
       <c r="AC5" s="10">
-        <v>0</v>
+        <v>51931</v>
       </c>
       <c r="AD5" s="10">
         <v>0</v>
@@ -10039,7 +10144,7 @@
       <c r="AB6" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AC6" s="18" t="s">
         <v>202</v>
       </c>
       <c r="AD6" s="3" t="s">
@@ -10257,9 +10362,12 @@
       <c r="AB7" s="10">
         <v>321</v>
       </c>
+      <c r="AC7" s="10">
+        <v>354</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -10343,9 +10451,12 @@
       <c r="AB8" s="10">
         <v>4</v>
       </c>
+      <c r="AC8" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A9" s="36"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -10427,9 +10538,12 @@
       <c r="AB9" s="10">
         <v>23</v>
       </c>
+      <c r="AC9" s="10">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -10511,9 +10625,12 @@
       <c r="AB10" s="10">
         <v>2</v>
       </c>
+      <c r="AC10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A11" s="36"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -10595,9 +10712,12 @@
       <c r="AB11" s="10">
         <v>20</v>
       </c>
+      <c r="AC11" s="10">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A12" s="36"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -10679,9 +10799,12 @@
       <c r="AB12" s="10">
         <v>1</v>
       </c>
+      <c r="AC12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -10761,6 +10884,9 @@
         <v>4</v>
       </c>
       <c r="AB13" s="10">
+        <v>6</v>
+      </c>
+      <c r="AC13" s="10">
         <v>6</v>
       </c>
     </row>
@@ -10849,9 +10975,12 @@
       <c r="AB14" s="10">
         <v>485</v>
       </c>
+      <c r="AC14" s="10">
+        <v>520</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -10935,9 +11064,12 @@
       <c r="AB15" s="10">
         <v>19</v>
       </c>
+      <c r="AC15" s="10">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A16" s="36"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -11019,9 +11151,12 @@
       <c r="AB16" s="10">
         <v>0</v>
       </c>
+      <c r="AC16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A17" s="36"/>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A17" s="35"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -11103,9 +11238,12 @@
       <c r="AB17" s="10">
         <v>0</v>
       </c>
+      <c r="AC17" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A18" s="35"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -11187,9 +11325,12 @@
       <c r="AB18" s="10">
         <v>5</v>
       </c>
+      <c r="AC18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A19" s="35"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -11271,9 +11412,12 @@
       <c r="AB19" s="10">
         <v>83</v>
       </c>
+      <c r="AC19" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A20" s="35"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -11355,9 +11499,12 @@
       <c r="AB20" s="10">
         <v>5</v>
       </c>
+      <c r="AC20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A21" s="35"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -11439,9 +11586,12 @@
       <c r="AB21" s="10">
         <v>214</v>
       </c>
+      <c r="AC21" s="10">
+        <v>233</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A22" s="36"/>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A22" s="35"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -11523,9 +11673,12 @@
       <c r="AB22" s="10">
         <v>3</v>
       </c>
+      <c r="AC22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A23" s="36"/>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A23" s="35"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -11607,9 +11760,12 @@
       <c r="AB23" s="10">
         <v>4</v>
       </c>
+      <c r="AC23" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A24" s="36"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -11691,9 +11847,12 @@
       <c r="AB24" s="10">
         <v>7</v>
       </c>
+      <c r="AC24" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A25" s="32" t="s">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A25" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -11777,9 +11936,12 @@
       <c r="AB25" s="10">
         <v>10</v>
       </c>
+      <c r="AC25" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A26" s="33"/>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A26" s="38"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -11861,9 +12023,12 @@
       <c r="AB26" s="10">
         <v>7</v>
       </c>
+      <c r="AC26" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A27" s="33"/>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A27" s="38"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -11945,9 +12110,12 @@
       <c r="AB27" s="10">
         <v>17</v>
       </c>
+      <c r="AC27" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A28" s="38"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -12029,9 +12197,12 @@
       <c r="AB28" s="10">
         <v>9</v>
       </c>
+      <c r="AC28" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A29" s="34"/>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A29" s="39"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -12113,8 +12284,11 @@
       <c r="AB29" s="10">
         <v>38</v>
       </c>
+      <c r="AC29" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -12199,9 +12373,12 @@
       <c r="AB30" s="10">
         <v>147</v>
       </c>
+      <c r="AC30" s="10">
+        <v>154</v>
+      </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A31" s="32" t="s">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A31" s="37" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -12285,9 +12462,12 @@
       <c r="AB31" s="10">
         <v>291</v>
       </c>
+      <c r="AC31" s="10">
+        <v>310</v>
+      </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A32" s="33"/>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A32" s="38"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -12369,9 +12549,12 @@
       <c r="AB32" s="10">
         <v>7</v>
       </c>
+      <c r="AC32" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A33" s="34"/>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A33" s="39"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -12453,9 +12636,12 @@
       <c r="AB33" s="10">
         <v>19</v>
       </c>
+      <c r="AC33" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A34" s="35" t="s">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A34" s="34" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -12539,9 +12725,12 @@
       <c r="AB34" s="10">
         <v>10</v>
       </c>
+      <c r="AC34" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A35" s="36"/>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A35" s="35"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -12623,9 +12812,12 @@
       <c r="AB35" s="10">
         <v>52</v>
       </c>
+      <c r="AC35" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A36" s="36"/>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A36" s="35"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -12707,9 +12899,12 @@
       <c r="AB36" s="10">
         <v>70</v>
       </c>
+      <c r="AC36" s="10">
+        <v>79</v>
+      </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A37" s="37"/>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A37" s="36"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -12791,9 +12986,12 @@
       <c r="AB37" s="10">
         <v>17</v>
       </c>
+      <c r="AC37" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A38" s="32" t="s">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A38" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -12877,9 +13075,12 @@
       <c r="AB38" s="10">
         <v>7</v>
       </c>
+      <c r="AC38" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A39" s="33"/>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A39" s="38"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -12961,9 +13162,12 @@
       <c r="AB39" s="10">
         <v>18</v>
       </c>
+      <c r="AC39" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A40" s="33"/>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A40" s="38"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -13045,9 +13249,12 @@
       <c r="AB40" s="10">
         <v>28</v>
       </c>
+      <c r="AC40" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A41" s="33"/>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A41" s="38"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -13129,9 +13336,12 @@
       <c r="AB41" s="10">
         <v>3</v>
       </c>
+      <c r="AC41" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A42" s="33"/>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A42" s="38"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -13213,9 +13423,12 @@
       <c r="AB42" s="10">
         <v>11</v>
       </c>
+      <c r="AC42" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A43" s="33"/>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A43" s="38"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -13297,9 +13510,12 @@
       <c r="AB43" s="10">
         <v>7</v>
       </c>
+      <c r="AC43" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A44" s="33"/>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A44" s="38"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -13381,9 +13597,12 @@
       <c r="AB44" s="10">
         <v>14</v>
       </c>
+      <c r="AC44" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A45" s="34"/>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A45" s="39"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -13465,9 +13684,12 @@
       <c r="AB45" s="10">
         <v>21</v>
       </c>
+      <c r="AC45" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A46" s="35" t="s">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A46" s="34" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -13551,9 +13773,12 @@
       <c r="AB46" s="10">
         <v>12</v>
       </c>
+      <c r="AC46" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A47" s="36"/>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A47" s="35"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -13635,9 +13860,12 @@
       <c r="AB47" s="10">
         <v>0</v>
       </c>
+      <c r="AC47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A48" s="36"/>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A48" s="35"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -13719,9 +13947,12 @@
       <c r="AB48" s="10">
         <v>2</v>
       </c>
+      <c r="AC48" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A49" s="37"/>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A49" s="36"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -13803,9 +14034,12 @@
       <c r="AB49" s="10">
         <v>4</v>
       </c>
+      <c r="AC49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A50" s="32" t="s">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A50" s="37" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -13889,9 +14123,12 @@
       <c r="AB50" s="10">
         <v>28</v>
       </c>
+      <c r="AC50" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A51" s="34"/>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A51" s="39"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -13973,9 +14210,12 @@
       <c r="AB51" s="10">
         <v>5</v>
       </c>
+      <c r="AC51" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A52" s="35" t="s">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A52" s="34" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -14059,9 +14299,12 @@
       <c r="AB52" s="10">
         <v>1476</v>
       </c>
+      <c r="AC52" s="10">
+        <v>1633</v>
+      </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A53" s="36"/>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A53" s="35"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -14143,9 +14386,12 @@
       <c r="AB53" s="10">
         <v>2</v>
       </c>
+      <c r="AC53" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A54" s="37"/>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A54" s="36"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -14227,8 +14473,11 @@
       <c r="AB54" s="10">
         <v>0</v>
       </c>
+      <c r="AC54" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -14313,8 +14562,11 @@
       <c r="AB55" s="10">
         <v>78</v>
       </c>
+      <c r="AC55" s="10">
+        <v>79</v>
+      </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -14399,9 +14651,12 @@
       <c r="AB56" s="10">
         <v>532</v>
       </c>
+      <c r="AC56" s="10">
+        <v>559</v>
+      </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A57" s="32" t="s">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A57" s="37" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -14485,9 +14740,12 @@
       <c r="AB57" s="10">
         <v>7</v>
       </c>
+      <c r="AC57" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A58" s="33"/>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A58" s="38"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -14569,9 +14827,12 @@
       <c r="AB58" s="10">
         <v>3</v>
       </c>
+      <c r="AC58" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A59" s="33"/>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A59" s="38"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -14653,9 +14914,12 @@
       <c r="AB59" s="10">
         <v>17</v>
       </c>
+      <c r="AC59" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A60" s="34"/>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A60" s="39"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -14737,9 +15001,12 @@
       <c r="AB60" s="10">
         <v>0</v>
       </c>
+      <c r="AC60" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A61" s="35" t="s">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A61" s="34" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -14823,9 +15090,12 @@
       <c r="AB61" s="10">
         <v>6</v>
       </c>
+      <c r="AC61" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A62" s="36"/>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A62" s="35"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -14907,9 +15177,12 @@
       <c r="AB62" s="10">
         <v>76</v>
       </c>
+      <c r="AC62" s="10">
+        <v>81</v>
+      </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A63" s="36"/>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A63" s="35"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -14991,9 +15264,12 @@
       <c r="AB63" s="10">
         <v>10</v>
       </c>
+      <c r="AC63" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A64" s="36"/>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A64" s="35"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -15075,9 +15351,12 @@
       <c r="AB64" s="10">
         <v>33</v>
       </c>
+      <c r="AC64" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A65" s="36"/>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A65" s="35"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -15159,9 +15438,12 @@
       <c r="AB65" s="10">
         <v>22</v>
       </c>
+      <c r="AC65" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A66" s="37"/>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A66" s="36"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -15243,8 +15525,11 @@
       <c r="AB66" s="10">
         <v>22</v>
       </c>
+      <c r="AC66" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -15329,9 +15614,12 @@
       <c r="AB67" s="10">
         <v>385</v>
       </c>
+      <c r="AC67" s="10">
+        <v>413</v>
+      </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A68" s="35" t="s">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A68" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -15415,9 +15703,12 @@
       <c r="AB68" s="10">
         <v>0</v>
       </c>
+      <c r="AC68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A69" s="36"/>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A69" s="35"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -15499,9 +15790,12 @@
       <c r="AB69" s="10">
         <v>3</v>
       </c>
+      <c r="AC69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A70" s="36"/>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A70" s="35"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -15583,9 +15877,12 @@
       <c r="AB70" s="10">
         <v>0</v>
       </c>
+      <c r="AC70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A71" s="36"/>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A71" s="35"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -15667,9 +15964,12 @@
       <c r="AB71" s="10">
         <v>11</v>
       </c>
+      <c r="AC71" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A72" s="36"/>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A72" s="35"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -15751,9 +16051,12 @@
       <c r="AB72" s="10">
         <v>28</v>
       </c>
+      <c r="AC72" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A73" s="36"/>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A73" s="35"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -15835,9 +16138,12 @@
       <c r="AB73" s="10">
         <v>8</v>
       </c>
+      <c r="AC73" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A74" s="36"/>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A74" s="35"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -15919,9 +16225,12 @@
       <c r="AB74" s="10">
         <v>1</v>
       </c>
+      <c r="AC74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A75" s="37"/>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A75" s="36"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -16003,9 +16312,12 @@
       <c r="AB75" s="10">
         <v>1</v>
       </c>
+      <c r="AC75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A76" s="32" t="s">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A76" s="37" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -16089,9 +16401,12 @@
       <c r="AB76" s="10">
         <v>1</v>
       </c>
+      <c r="AC76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A77" s="33"/>
+    <row r="77" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A77" s="38"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -16173,9 +16488,12 @@
       <c r="AB77" s="10">
         <v>4</v>
       </c>
+      <c r="AC77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A78" s="33"/>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A78" s="38"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -16257,9 +16575,12 @@
       <c r="AB78" s="10">
         <v>40</v>
       </c>
+      <c r="AC78" s="10">
+        <v>42</v>
+      </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A79" s="33"/>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A79" s="38"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -16341,9 +16662,12 @@
       <c r="AB79" s="10">
         <v>8</v>
       </c>
+      <c r="AC79" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A80" s="34"/>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A80" s="39"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -16425,8 +16749,11 @@
       <c r="AB80" s="10">
         <v>1</v>
       </c>
+      <c r="AC80" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -16511,9 +16838,12 @@
       <c r="AB81" s="10">
         <v>108</v>
       </c>
+      <c r="AC81" s="10">
+        <v>109</v>
+      </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A82" s="32" t="s">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A82" s="37" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -16597,9 +16927,12 @@
       <c r="AB82" s="10">
         <v>138</v>
       </c>
+      <c r="AC82" s="10">
+        <v>139</v>
+      </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A83" s="33"/>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A83" s="38"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -16681,9 +17014,12 @@
       <c r="AB83" s="10">
         <v>38</v>
       </c>
+      <c r="AC83" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A84" s="33"/>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A84" s="38"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -16765,9 +17101,12 @@
       <c r="AB84" s="10">
         <v>100</v>
       </c>
+      <c r="AC84" s="10">
+        <v>102</v>
+      </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A85" s="33"/>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A85" s="38"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -16849,9 +17188,12 @@
       <c r="AB85" s="10">
         <v>6</v>
       </c>
+      <c r="AC85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A86" s="34"/>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A86" s="39"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -16933,9 +17275,12 @@
       <c r="AB86" s="10">
         <v>19</v>
       </c>
+      <c r="AC86" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A87" s="35" t="s">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A87" s="34" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -17019,9 +17364,12 @@
       <c r="AB87" s="10">
         <v>13</v>
       </c>
+      <c r="AC87" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A88" s="36"/>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A88" s="35"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -17103,9 +17451,12 @@
       <c r="AB88" s="10">
         <v>24</v>
       </c>
+      <c r="AC88" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A89" s="36"/>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A89" s="35"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -17187,9 +17538,12 @@
       <c r="AB89" s="10">
         <v>8</v>
       </c>
+      <c r="AC89" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A90" s="36"/>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A90" s="35"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -17271,9 +17625,12 @@
       <c r="AB90" s="10">
         <v>8</v>
       </c>
+      <c r="AC90" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A91" s="36"/>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A91" s="35"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -17355,9 +17712,12 @@
       <c r="AB91" s="10">
         <v>3</v>
       </c>
+      <c r="AC91" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A92" s="36"/>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A92" s="35"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -17439,9 +17799,12 @@
       <c r="AB92" s="10">
         <v>5</v>
       </c>
+      <c r="AC92" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A93" s="37"/>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A93" s="36"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -17523,9 +17886,12 @@
       <c r="AB93" s="10">
         <v>17</v>
       </c>
+      <c r="AC93" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A94" s="32" t="s">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A94" s="37" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -17609,9 +17975,12 @@
       <c r="AB94" s="10">
         <v>6</v>
       </c>
+      <c r="AC94" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A95" s="34"/>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A95" s="39"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -17693,8 +18062,11 @@
       <c r="AB95" s="10">
         <v>22</v>
       </c>
+      <c r="AC95" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -17779,9 +18151,12 @@
       <c r="AB96" s="10">
         <v>63</v>
       </c>
+      <c r="AC96" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A97" s="32" t="s">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A97" s="37" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -17865,9 +18240,12 @@
       <c r="AB97" s="10">
         <v>644</v>
       </c>
+      <c r="AC97" s="10">
+        <v>700</v>
+      </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A98" s="33"/>
+    <row r="98" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A98" s="38"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -17949,9 +18327,12 @@
       <c r="AB98" s="10">
         <v>72</v>
       </c>
+      <c r="AC98" s="10">
+        <v>82</v>
+      </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A99" s="34"/>
+    <row r="99" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A99" s="39"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -18033,9 +18414,12 @@
       <c r="AB99" s="10">
         <v>21</v>
       </c>
+      <c r="AC99" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A100" s="35" t="s">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A100" s="34" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -18119,9 +18503,12 @@
       <c r="AB100" s="10">
         <v>11</v>
       </c>
+      <c r="AC100" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A101" s="36"/>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A101" s="35"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -18203,9 +18590,12 @@
       <c r="AB101" s="10">
         <v>18</v>
       </c>
+      <c r="AC101" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A102" s="36"/>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A102" s="35"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -18287,9 +18677,12 @@
       <c r="AB102" s="10">
         <v>69</v>
       </c>
+      <c r="AC102" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A103" s="36"/>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A103" s="35"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -18371,9 +18764,12 @@
       <c r="AB103" s="10">
         <v>128</v>
       </c>
+      <c r="AC103" s="10">
+        <v>143</v>
+      </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A104" s="37"/>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A104" s="36"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -18455,9 +18851,12 @@
       <c r="AB104" s="10">
         <v>15</v>
       </c>
+      <c r="AC104" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A105" s="32" t="s">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A105" s="37" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -18541,9 +18940,12 @@
       <c r="AB105" s="10">
         <v>32</v>
       </c>
+      <c r="AC105" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A106" s="33"/>
+    <row r="106" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A106" s="38"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -18625,9 +19027,12 @@
       <c r="AB106" s="10">
         <v>35</v>
       </c>
+      <c r="AC106" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A107" s="33"/>
+    <row r="107" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A107" s="38"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -18709,9 +19114,12 @@
       <c r="AB107" s="10">
         <v>8</v>
       </c>
+      <c r="AC107" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A108" s="33"/>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A108" s="38"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -18793,9 +19201,12 @@
       <c r="AB108" s="10">
         <v>19</v>
       </c>
+      <c r="AC108" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A109" s="34"/>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A109" s="39"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -18877,8 +19288,11 @@
       <c r="AB109" s="10">
         <v>1</v>
       </c>
+      <c r="AC109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -18963,8 +19377,11 @@
       <c r="AB110" s="10">
         <v>201</v>
       </c>
+      <c r="AC110" s="10">
+        <v>211</v>
+      </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -19049,9 +19466,12 @@
       <c r="AB111" s="10">
         <v>24</v>
       </c>
+      <c r="AC111" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A112" s="35" t="s">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A112" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -19135,9 +19555,12 @@
       <c r="AB112" s="10">
         <v>10</v>
       </c>
+      <c r="AC112" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A113" s="36"/>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A113" s="35"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -19219,9 +19642,12 @@
       <c r="AB113" s="10">
         <v>7</v>
       </c>
+      <c r="AC113" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A114" s="37"/>
+    <row r="114" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A114" s="36"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -19303,9 +19729,12 @@
       <c r="AB114" s="10">
         <v>62</v>
       </c>
+      <c r="AC114" s="10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A115" s="32" t="s">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A115" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -19389,9 +19818,12 @@
       <c r="AB115" s="10">
         <v>56</v>
       </c>
+      <c r="AC115" s="10">
+        <v>56</v>
+      </c>
     </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A116" s="33"/>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A116" s="38"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -19473,9 +19905,12 @@
       <c r="AB116" s="10">
         <v>64</v>
       </c>
+      <c r="AC116" s="10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A117" s="33"/>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A117" s="38"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -19557,9 +19992,12 @@
       <c r="AB117" s="10">
         <v>7</v>
       </c>
+      <c r="AC117" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A118" s="33"/>
+    <row r="118" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A118" s="38"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -19641,9 +20079,12 @@
       <c r="AB118" s="10">
         <v>33</v>
       </c>
+      <c r="AC118" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A119" s="33"/>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A119" s="38"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -19725,9 +20166,12 @@
       <c r="AB119" s="10">
         <v>5</v>
       </c>
+      <c r="AC119" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A120" s="34"/>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A120" s="39"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -19809,9 +20253,12 @@
       <c r="AB120" s="10">
         <v>40</v>
       </c>
+      <c r="AC120" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A121" s="35" t="s">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A121" s="34" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -19895,9 +20342,12 @@
       <c r="AB121" s="10">
         <v>2</v>
       </c>
+      <c r="AC121" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A122" s="36"/>
+    <row r="122" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A122" s="35"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -19979,9 +20429,12 @@
       <c r="AB122" s="10">
         <v>20</v>
       </c>
+      <c r="AC122" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A123" s="36"/>
+    <row r="123" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A123" s="35"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -20063,9 +20516,12 @@
       <c r="AB123" s="10">
         <v>2</v>
       </c>
+      <c r="AC123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A124" s="36"/>
+    <row r="124" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A124" s="35"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -20147,9 +20603,12 @@
       <c r="AB124" s="10">
         <v>2</v>
       </c>
+      <c r="AC124" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A125" s="36"/>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A125" s="35"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -20231,9 +20690,12 @@
       <c r="AB125" s="10">
         <v>1</v>
       </c>
+      <c r="AC125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A126" s="36"/>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A126" s="35"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -20315,9 +20777,12 @@
       <c r="AB126" s="10">
         <v>3</v>
       </c>
+      <c r="AC126" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A127" s="36"/>
+    <row r="127" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A127" s="35"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -20399,9 +20864,12 @@
       <c r="AB127" s="10">
         <v>3</v>
       </c>
+      <c r="AC127" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A128" s="36"/>
+    <row r="128" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A128" s="35"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -20483,9 +20951,12 @@
       <c r="AB128" s="10">
         <v>5</v>
       </c>
+      <c r="AC128" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A129" s="36"/>
+    <row r="129" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A129" s="35"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -20567,9 +21038,12 @@
       <c r="AB129" s="10">
         <v>8</v>
       </c>
+      <c r="AC129" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A130" s="37"/>
+    <row r="130" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A130" s="36"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -20651,8 +21125,11 @@
       <c r="AB130" s="10">
         <v>9</v>
       </c>
+      <c r="AC130" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -20737,9 +21214,12 @@
       <c r="AB131" s="10">
         <v>265</v>
       </c>
+      <c r="AC131" s="10">
+        <v>271</v>
+      </c>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A132" s="35" t="s">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A132" s="34" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -20823,9 +21303,12 @@
       <c r="AB132" s="10">
         <v>15</v>
       </c>
+      <c r="AC132" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A133" s="36"/>
+    <row r="133" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A133" s="35"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -20907,9 +21390,12 @@
       <c r="AB133" s="10">
         <v>10</v>
       </c>
+      <c r="AC133" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A134" s="36"/>
+    <row r="134" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A134" s="35"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -20991,9 +21477,12 @@
       <c r="AB134" s="10">
         <v>0</v>
       </c>
+      <c r="AC134" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A135" s="37"/>
+    <row r="135" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A135" s="36"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -21075,9 +21564,12 @@
       <c r="AB135" s="10">
         <v>0</v>
       </c>
+      <c r="AC135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A136" s="32" t="s">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A136" s="37" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -21161,9 +21653,12 @@
       <c r="AB136" s="10">
         <v>69</v>
       </c>
+      <c r="AC136" s="10">
+        <v>83</v>
+      </c>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A137" s="33"/>
+    <row r="137" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A137" s="38"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -21245,9 +21740,12 @@
       <c r="AB137" s="10">
         <v>7</v>
       </c>
+      <c r="AC137" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A138" s="33"/>
+    <row r="138" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A138" s="38"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -21329,9 +21827,12 @@
       <c r="AB138" s="10">
         <v>9</v>
       </c>
+      <c r="AC138" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A139" s="34"/>
+    <row r="139" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A139" s="39"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -21412,10 +21913,25 @@
       </c>
       <c r="AB139" s="10">
         <v>70</v>
+      </c>
+      <c r="AC139" s="10">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -21428,18 +21944,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -21694,7 +22198,7 @@
       </c>
       <c r="AK2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30.4</v>
       </c>
       <c r="AL2" s="19">
         <f t="shared" si="1"/>
@@ -22344,7 +22848,7 @@
       </c>
       <c r="AK4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.6315789473684208</v>
       </c>
       <c r="AL4" s="10">
         <f t="shared" si="7"/>
@@ -22669,7 +23173,7 @@
       </c>
       <c r="AK6" s="12">
         <f>MAX(0, (dc!AK2-dc!AJ2))</f>
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="AL6" s="12">
         <f>MAX(0, (dc!AL2-dc!AK2))</f>
@@ -22993,7 +23497,7 @@
       </c>
       <c r="AK7" s="12">
         <f>MAX(0, (dc!AK3-dc!AJ3))</f>
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="AL7" s="12">
         <f>MAX(0, (dc!AL3-dc!AK3))</f>
@@ -23641,7 +24145,7 @@
       </c>
       <c r="AK9" s="12">
         <f>MAX(0, (dc!AK5-dc!AJ5))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL9" s="12">
         <f>MAX(0, (dc!AL5-dc!AK5))</f>
@@ -24193,7 +24697,7 @@
       </c>
       <c r="AK11" s="10">
         <f>MAX(0,(dc!AK7-dc!AJ7))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AL11" s="10">
         <f>MAX(0,(dc!AL7-dc!AK7))</f>
@@ -24500,7 +25004,7 @@
       </c>
       <c r="AK12" s="10">
         <f>MAX(0,(dc!AK8-dc!AJ8))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AL12" s="10">
         <f>MAX(0,(dc!AL8-dc!AK8))</f>
@@ -24807,7 +25311,7 @@
       </c>
       <c r="AK13" s="10">
         <f>MAX(0,(dc!AK9-dc!AJ9))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AL13" s="10">
         <f>MAX(0,(dc!AL9-dc!AK9))</f>
@@ -25114,7 +25618,7 @@
       </c>
       <c r="AK14" s="10">
         <f>MAX(0,(dc!AK10-dc!AJ10))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AL14" s="10">
         <f>MAX(0,(dc!AL10-dc!AK10))</f>
@@ -25421,7 +25925,7 @@
       </c>
       <c r="AK15" s="10">
         <f>MAX(0,(dc!AK11-dc!AJ11))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AL15" s="10">
         <f>MAX(0,(dc!AL11-dc!AK11))</f>
@@ -25728,7 +26232,7 @@
       </c>
       <c r="AK16" s="10">
         <f>MAX(0,(dc!AK12-dc!AJ12))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AL16" s="10">
         <f>MAX(0,(dc!AL12-dc!AK12))</f>
@@ -26035,7 +26539,7 @@
       </c>
       <c r="AK17" s="10">
         <f>MAX(0,(dc!AK13-dc!AJ13))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AL17" s="10">
         <f>MAX(0,(dc!AL13-dc!AK13))</f>
@@ -26342,7 +26846,7 @@
       </c>
       <c r="AK18" s="10">
         <f>MAX(0,(dc!AK14-dc!AJ14))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AL18" s="10">
         <f>MAX(0,(dc!AL14-dc!AK14))</f>
@@ -26649,7 +27153,7 @@
       </c>
       <c r="AK19" s="10">
         <f>MAX(0,(dc!AK15-dc!AJ15))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL19" s="10">
         <f>MAX(0,(dc!AL15-dc!AK15))</f>
@@ -27043,7 +27547,7 @@
       </c>
       <c r="Z2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21.898244570068432</v>
       </c>
       <c r="AA2" s="21">
         <f t="shared" si="0"/>
@@ -27316,7 +27820,7 @@
       </c>
       <c r="Z3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19.701086956521738</v>
       </c>
       <c r="AA3" s="21">
         <f t="shared" si="2"/>
@@ -27589,7 +28093,7 @@
       </c>
       <c r="Z4" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.1630434782608692</v>
       </c>
       <c r="AA4" s="21">
         <f t="shared" si="4"/>
@@ -27925,7 +28429,7 @@
       </c>
       <c r="Z6" s="14">
         <f>MAX(0,(md!Z2-md!Y2)+(md!Z3-md!Y3))</f>
-        <v>0</v>
+        <v>3361</v>
       </c>
       <c r="AA6" s="14">
         <f>MAX(0,(md!AA2-md!Z2)+(md!AA3-md!Z3))</f>
@@ -28197,7 +28701,7 @@
       </c>
       <c r="Z7" s="14">
         <f>MAX(0,(md!Z3-md!Y3))</f>
-        <v>0</v>
+        <v>736</v>
       </c>
       <c r="AA7" s="14">
         <f>MAX(0,(md!AA3-md!Z3))</f>
@@ -28469,7 +28973,7 @@
       </c>
       <c r="Z8" s="14">
         <f>MAX(0,(md!Z4-md!Y4))</f>
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="AA8" s="14">
         <f>MAX(0,(md!AA4-md!Z4))</f>
@@ -28741,7 +29245,7 @@
       </c>
       <c r="Z9" s="14">
         <f>MAX(0,(md!Z5-md!Y5))</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AA9" s="14">
         <f>MAX(0,(md!AA5-md!Z5))</f>
@@ -29227,7 +29731,7 @@
       </c>
       <c r="Z11" s="14">
         <f>MAX(0,(md!Z7-md!Y7))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AA11" s="14">
         <f>MAX(0,(md!AA7-md!Z7))</f>
@@ -29504,7 +30008,7 @@
       </c>
       <c r="Z12" s="14">
         <f>MAX(0,(md!Z9-md!Y9))</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="AA12" s="14">
         <f>MAX(0,(md!AA9-md!Z9))</f>
@@ -29781,7 +30285,7 @@
       </c>
       <c r="Z13" s="14">
         <f>MAX(0,(md!Z9-md!Y9))</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="AA13" s="14">
         <f>MAX(0,(md!AA9-md!Z9))</f>
@@ -30058,7 +30562,7 @@
       </c>
       <c r="Z14" s="14">
         <f>MAX(0,(md!Z10-md!Y10))</f>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="AA14" s="14">
         <f>MAX(0,(md!AA10-md!Z10))</f>
@@ -30612,7 +31116,7 @@
       </c>
       <c r="Z16" s="14">
         <f>MAX(0,(md!Z12-md!Y12))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA16" s="14">
         <f>MAX(0,(md!AA12-md!Z12))</f>
@@ -30889,7 +31393,7 @@
       </c>
       <c r="Z17" s="14">
         <f>MAX(0,(md!Z13-md!Y13))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA17" s="14">
         <f>MAX(0,(md!AA13-md!Z13))</f>
@@ -31166,7 +31670,7 @@
       </c>
       <c r="Z18" s="14">
         <f>MAX(0,(md!Z14-md!Y14))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA18" s="14">
         <f>MAX(0,(md!AA14-md!Z14))</f>
@@ -31443,7 +31947,7 @@
       </c>
       <c r="Z19" s="14">
         <f>MAX(0,(md!Z15-md!Y15))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA19" s="14">
         <f>MAX(0,(md!AA15-md!Z15))</f>
@@ -31997,7 +32501,7 @@
       </c>
       <c r="Z21" s="14">
         <f>MAX(0,(md!Z17-md!Y17))</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AA21" s="14">
         <f>MAX(0,(md!AA17-md!Z17))</f>
@@ -32551,7 +33055,7 @@
       </c>
       <c r="Z23" s="14">
         <f>MAX(0,(md!Z19-md!Y19))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AA23" s="14">
         <f>MAX(0,(md!AA19-md!Z19))</f>
@@ -32828,7 +33332,7 @@
       </c>
       <c r="Z24" s="14">
         <f>MAX(0,(md!Z20-md!Y20))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AA24" s="14">
         <f>MAX(0,(md!AA20-md!Z20))</f>
@@ -33105,7 +33609,7 @@
       </c>
       <c r="Z25" s="14">
         <f>MAX(0,(md!Z21-md!Y21))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA25" s="14">
         <f>MAX(0,(md!AA21-md!Z21))</f>
@@ -33382,7 +33886,7 @@
       </c>
       <c r="Z26" s="14">
         <f>MAX(0,(md!Z22-md!Y22))</f>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="AA26" s="14">
         <f>MAX(0,(md!AA22-md!Z22))</f>
@@ -33659,7 +34163,7 @@
       </c>
       <c r="Z27" s="14">
         <f>MAX(0,(md!Z23-md!Y23))</f>
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="AA27" s="14">
         <f>MAX(0,(md!AA23-md!Z23))</f>
@@ -33936,7 +34440,7 @@
       </c>
       <c r="Z28" s="14">
         <f>MAX(0,(md!Z24-md!Y24))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA28" s="14">
         <f>MAX(0,(md!AA24-md!Z24))</f>
@@ -34213,7 +34717,7 @@
       </c>
       <c r="Z29" s="14">
         <f>MAX(0,(md!Z25-md!Y25))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA29" s="14">
         <f>MAX(0,(md!AA25-md!Z25))</f>
@@ -34490,7 +34994,7 @@
       </c>
       <c r="Z30" s="14">
         <f>MAX(0,(md!Z26-md!Y26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA30" s="14">
         <f>MAX(0,(md!AA26-md!Z26))</f>
@@ -34767,7 +35271,7 @@
       </c>
       <c r="Z31" s="14">
         <f>MAX(0,(md!Z27-md!Y27))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA31" s="14">
         <f>MAX(0,(md!AA27-md!Z27))</f>
@@ -35321,7 +35825,7 @@
       </c>
       <c r="Z33" s="14">
         <f>MAX(0,(md!Z29-md!Y29))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AA33" s="14">
         <f>MAX(0,(md!AA29-md!Z29))</f>
@@ -35598,7 +36102,7 @@
       </c>
       <c r="Z34" s="14">
         <f>MAX(0,(md!Z30-md!Y30))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA34" s="14">
         <f>MAX(0,(md!AA30-md!Z30))</f>
@@ -36077,7 +36581,7 @@
       </c>
       <c r="AB2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19.154737559645536</v>
       </c>
       <c r="AC2" s="20">
         <f t="shared" si="0"/>
@@ -36354,7 +36858,7 @@
       </c>
       <c r="AB3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.345195729537366</v>
       </c>
       <c r="AC3" s="20">
         <f t="shared" si="2"/>
@@ -36631,7 +37135,7 @@
       </c>
       <c r="AB4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.8042704626334514</v>
       </c>
       <c r="AC4" s="20">
         <f t="shared" si="4"/>
@@ -36908,7 +37412,7 @@
       </c>
       <c r="AB6" s="14">
         <f>MAX(0,(va!AC5-va!AB5))</f>
-        <v>0</v>
+        <v>2934</v>
       </c>
       <c r="AC6" s="14">
         <f>MAX(0,(va!AD5-va!AC5))</f>
@@ -37185,7 +37689,7 @@
       </c>
       <c r="AB7" s="14">
         <f>MAX(0,(va!AC2-va!AB2))</f>
-        <v>0</v>
+        <v>562</v>
       </c>
       <c r="AC7" s="14">
         <f>MAX(0,(va!AD2-va!AC2))</f>
@@ -37462,7 +37966,7 @@
       </c>
       <c r="AB8" s="14">
         <f>MAX(0,(va!AC3-va!AB3))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AC8" s="14">
         <f>MAX(0,(va!AD3-va!AC3))</f>
@@ -37739,7 +38243,7 @@
       </c>
       <c r="AB9" s="14">
         <f>MAX(0,(va!AC4-va!AB4))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AC9" s="14">
         <f>MAX(0,(va!AD4-va!AC4))</f>
@@ -38236,7 +38740,7 @@
       </c>
       <c r="AB11" s="16">
         <f>MAX(0,(va!AC7-va!AB7))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AC11" s="16">
         <f>MAX(0,(va!AD7-va!AC7))</f>
@@ -40210,7 +40714,7 @@
       </c>
       <c r="AB18" s="16">
         <f>MAX(0,(va!AC14-va!AB14))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AC18" s="16">
         <f>MAX(0,(va!AD14-va!AC14))</f>
@@ -40492,7 +40996,7 @@
       </c>
       <c r="AB19" s="16">
         <f>MAX(0,(va!AC15-va!AB15))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC19" s="16">
         <f>MAX(0,(va!AD15-va!AC15))</f>
@@ -41620,7 +42124,7 @@
       </c>
       <c r="AB23" s="16">
         <f>MAX(0,(va!AC19-va!AB19))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AC23" s="16">
         <f>MAX(0,(va!AD19-va!AC19))</f>
@@ -42184,7 +42688,7 @@
       </c>
       <c r="AB25" s="16">
         <f>MAX(0,(va!AC21-va!AB21))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC25" s="16">
         <f>MAX(0,(va!AD21-va!AC21))</f>
@@ -42748,7 +43252,7 @@
       </c>
       <c r="AB27" s="16">
         <f>MAX(0,(va!AC23-va!AB23))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC27" s="16">
         <f>MAX(0,(va!AD23-va!AC23))</f>
@@ -44722,7 +45226,7 @@
       </c>
       <c r="AB34" s="16">
         <f>MAX(0,(va!AC30-va!AB30))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC34" s="16">
         <f>MAX(0,(va!AD30-va!AC30))</f>
@@ -45004,7 +45508,7 @@
       </c>
       <c r="AB35" s="16">
         <f>MAX(0,(va!AC31-va!AB31))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC35" s="16">
         <f>MAX(0,(va!AD31-va!AC31))</f>
@@ -45286,7 +45790,7 @@
       </c>
       <c r="AB36" s="16">
         <f>MAX(0,(va!AC32-va!AB32))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC36" s="16">
         <f>MAX(0,(va!AD32-va!AC32))</f>
@@ -45568,7 +46072,7 @@
       </c>
       <c r="AB37" s="16">
         <f>MAX(0,(va!AC33-va!AB33))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AC37" s="16">
         <f>MAX(0,(va!AD33-va!AC33))</f>
@@ -45850,7 +46354,7 @@
       </c>
       <c r="AB38" s="16">
         <f>MAX(0,(va!AC34-va!AB34))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC38" s="16">
         <f>MAX(0,(va!AD34-va!AC34))</f>
@@ -46132,7 +46636,7 @@
       </c>
       <c r="AB39" s="16">
         <f>MAX(0,(va!AC35-va!AB35))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC39" s="16">
         <f>MAX(0,(va!AD35-va!AC35))</f>
@@ -46414,7 +46918,7 @@
       </c>
       <c r="AB40" s="16">
         <f>MAX(0,(va!AC36-va!AB36))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AC40" s="16">
         <f>MAX(0,(va!AD36-va!AC36))</f>
@@ -48670,7 +49174,7 @@
       </c>
       <c r="AB48" s="16">
         <f>MAX(0,(va!AC44-va!AB44))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC48" s="16">
         <f>MAX(0,(va!AD44-va!AC44))</f>
@@ -50362,7 +50866,7 @@
       </c>
       <c r="AB54" s="16">
         <f>MAX(0,(va!AC50-va!AB50))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC54" s="16">
         <f>MAX(0,(va!AD50-va!AC50))</f>
@@ -50926,7 +51430,7 @@
       </c>
       <c r="AB56" s="16">
         <f>MAX(0,(va!AC52-va!AB52))</f>
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="AC56" s="16">
         <f>MAX(0,(va!AD52-va!AC52))</f>
@@ -51208,7 +51712,7 @@
       </c>
       <c r="AB57" s="16">
         <f>MAX(0,(va!AC53-va!AB53))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC57" s="16">
         <f>MAX(0,(va!AD53-va!AC53))</f>
@@ -51772,7 +52276,7 @@
       </c>
       <c r="AB59" s="16">
         <f>MAX(0,(va!AC55-va!AB55))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC59" s="16">
         <f>MAX(0,(va!AD55-va!AC55))</f>
@@ -52054,7 +52558,7 @@
       </c>
       <c r="AB60" s="16">
         <f>MAX(0,(va!AC56-va!AB56))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AC60" s="16">
         <f>MAX(0,(va!AD56-va!AC56))</f>
@@ -52618,7 +53122,7 @@
       </c>
       <c r="AB62" s="16">
         <f>MAX(0,(va!AC58-va!AB58))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC62" s="16">
         <f>MAX(0,(va!AD58-va!AC58))</f>
@@ -52900,7 +53404,7 @@
       </c>
       <c r="AB63" s="16">
         <f>MAX(0,(va!AC59-va!AB59))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC63" s="16">
         <f>MAX(0,(va!AD59-va!AC59))</f>
@@ -53182,7 +53686,7 @@
       </c>
       <c r="AB64" s="16">
         <f>MAX(0,(va!AC60-va!AB60))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC64" s="16">
         <f>MAX(0,(va!AD60-va!AC60))</f>
@@ -53746,7 +54250,7 @@
       </c>
       <c r="AB66" s="16">
         <f>MAX(0,(va!AC62-va!AB62))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC66" s="16">
         <f>MAX(0,(va!AD62-va!AC62))</f>
@@ -54028,7 +54532,7 @@
       </c>
       <c r="AB67" s="16">
         <f>MAX(0,(va!AC63-va!AB63))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC67" s="16">
         <f>MAX(0,(va!AD63-va!AC63))</f>
@@ -54310,7 +54814,7 @@
       </c>
       <c r="AB68" s="16">
         <f>MAX(0,(va!AC64-va!AB64))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AC68" s="16">
         <f>MAX(0,(va!AD64-va!AC64))</f>
@@ -54592,7 +55096,7 @@
       </c>
       <c r="AB69" s="16">
         <f>MAX(0,(va!AC65-va!AB65))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC69" s="16">
         <f>MAX(0,(va!AD65-va!AC65))</f>
@@ -54874,7 +55378,7 @@
       </c>
       <c r="AB70" s="16">
         <f>MAX(0,(va!AC66-va!AB66))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC70" s="16">
         <f>MAX(0,(va!AD66-va!AC66))</f>
@@ -55156,7 +55660,7 @@
       </c>
       <c r="AB71" s="16">
         <f>MAX(0,(va!AC67-va!AB67))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AC71" s="16">
         <f>MAX(0,(va!AD67-va!AC67))</f>
@@ -56284,7 +56788,7 @@
       </c>
       <c r="AB75" s="16">
         <f>MAX(0,(va!AC71-va!AB71))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC75" s="16">
         <f>MAX(0,(va!AD71-va!AC71))</f>
@@ -58258,7 +58762,7 @@
       </c>
       <c r="AB82" s="16">
         <f>MAX(0,(va!AC78-va!AB78))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC82" s="16">
         <f>MAX(0,(va!AD78-va!AC78))</f>
@@ -59104,7 +59608,7 @@
       </c>
       <c r="AB85" s="16">
         <f>MAX(0,(va!AC81-va!AB81))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC85" s="16">
         <f>MAX(0,(va!AD81-va!AC81))</f>
@@ -59386,7 +59890,7 @@
       </c>
       <c r="AB86" s="16">
         <f>MAX(0,(va!AC82-va!AB82))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC86" s="16">
         <f>MAX(0,(va!AD82-va!AC82))</f>
@@ -59950,7 +60454,7 @@
       </c>
       <c r="AB88" s="16">
         <f>MAX(0,(va!AC84-va!AB84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC88" s="16">
         <f>MAX(0,(va!AD84-va!AC84))</f>
@@ -61078,7 +61582,7 @@
       </c>
       <c r="AB92" s="16">
         <f>MAX(0,(va!AC88-va!AB88))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC92" s="16">
         <f>MAX(0,(va!AD88-va!AC88))</f>
@@ -61642,7 +62146,7 @@
       </c>
       <c r="AB94" s="16">
         <f>MAX(0,(va!AC90-va!AB90))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC94" s="16">
         <f>MAX(0,(va!AD90-va!AC90))</f>
@@ -62206,7 +62710,7 @@
       </c>
       <c r="AB96" s="16">
         <f>MAX(0,(va!AC92-va!AB92))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC96" s="16">
         <f>MAX(0,(va!AD92-va!AC92))</f>
@@ -63052,7 +63556,7 @@
       </c>
       <c r="AB99" s="16">
         <f>MAX(0,(va!AC95-va!AB95))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC99" s="16">
         <f>MAX(0,(va!AD95-va!AC95))</f>
@@ -63334,7 +63838,7 @@
       </c>
       <c r="AB100" s="16">
         <f>MAX(0,(va!AC96-va!AB96))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC100" s="16">
         <f>MAX(0,(va!AD96-va!AC96))</f>
@@ -63616,7 +64120,7 @@
       </c>
       <c r="AB101" s="16">
         <f>MAX(0,(va!AC97-va!AB97))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AC101" s="16">
         <f>MAX(0,(va!AD97-va!AC97))</f>
@@ -63898,7 +64402,7 @@
       </c>
       <c r="AB102" s="16">
         <f>MAX(0,(va!AC98-va!AB98))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC102" s="16">
         <f>MAX(0,(va!AD98-va!AC98))</f>
@@ -64462,7 +64966,7 @@
       </c>
       <c r="AB104" s="16">
         <f>MAX(0,(va!AC100-va!AB100))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC104" s="16">
         <f>MAX(0,(va!AD100-va!AC100))</f>
@@ -65026,7 +65530,7 @@
       </c>
       <c r="AB106" s="16">
         <f>MAX(0,(va!AC102-va!AB102))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC106" s="16">
         <f>MAX(0,(va!AD102-va!AC102))</f>
@@ -65308,7 +65812,7 @@
       </c>
       <c r="AB107" s="16">
         <f>MAX(0,(va!AC103-va!AB103))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC107" s="16">
         <f>MAX(0,(va!AD103-va!AC103))</f>
@@ -65872,7 +66376,7 @@
       </c>
       <c r="AB109" s="16">
         <f>MAX(0,(va!AC105-va!AB105))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC109" s="16">
         <f>MAX(0,(va!AD105-va!AC105))</f>
@@ -66154,7 +66658,7 @@
       </c>
       <c r="AB110" s="16">
         <f>MAX(0,(va!AC106-va!AB106))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC110" s="16">
         <f>MAX(0,(va!AD106-va!AC106))</f>
@@ -66718,7 +67222,7 @@
       </c>
       <c r="AB112" s="16">
         <f>MAX(0,(va!AC108-va!AB108))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC112" s="16">
         <f>MAX(0,(va!AD108-va!AC108))</f>
@@ -67282,7 +67786,7 @@
       </c>
       <c r="AB114" s="16">
         <f>MAX(0,(va!AC110-va!AB110))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC114" s="16">
         <f>MAX(0,(va!AD110-va!AC110))</f>
@@ -67846,7 +68350,7 @@
       </c>
       <c r="AB116" s="16">
         <f>MAX(0,(va!AC112-va!AB112))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC116" s="16">
         <f>MAX(0,(va!AD112-va!AC112))</f>
@@ -68128,7 +68632,7 @@
       </c>
       <c r="AB117" s="16">
         <f>MAX(0,(va!AC113-va!AB113))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC117" s="16">
         <f>MAX(0,(va!AD113-va!AC113))</f>
@@ -68410,7 +68914,7 @@
       </c>
       <c r="AB118" s="16">
         <f>MAX(0,(va!AC114-va!AB114))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC118" s="16">
         <f>MAX(0,(va!AD114-va!AC114))</f>
@@ -68974,7 +69478,7 @@
       </c>
       <c r="AB120" s="16">
         <f>MAX(0,(va!AC116-va!AB116))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC120" s="16">
         <f>MAX(0,(va!AD116-va!AC116))</f>
@@ -69256,7 +69760,7 @@
       </c>
       <c r="AB121" s="16">
         <f>MAX(0,(va!AC117-va!AB117))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC121" s="16">
         <f>MAX(0,(va!AD117-va!AC117))</f>
@@ -70102,7 +70606,7 @@
       </c>
       <c r="AB124" s="16">
         <f>MAX(0,(va!AC120-va!AB120))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC124" s="16">
         <f>MAX(0,(va!AD120-va!AC120))</f>
@@ -70666,7 +71170,7 @@
       </c>
       <c r="AB126" s="16">
         <f>MAX(0,(va!AC122-va!AB122))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC126" s="16">
         <f>MAX(0,(va!AD122-va!AC122))</f>
@@ -72922,7 +73426,7 @@
       </c>
       <c r="AB134" s="16">
         <f>MAX(0,(va!AC130-va!AB130))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC134" s="16">
         <f>MAX(0,(va!AD130-va!AC130))</f>
@@ -73204,7 +73708,7 @@
       </c>
       <c r="AB135" s="16">
         <f>MAX(0,(va!AC131-va!AB131))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AC135" s="16">
         <f>MAX(0,(va!AD131-va!AC131))</f>
@@ -74614,7 +75118,7 @@
       </c>
       <c r="AB140" s="16">
         <f>MAX(0,(va!AC136-va!AB136))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AC140" s="16">
         <f>MAX(0,(va!AD136-va!AC136))</f>
@@ -74896,7 +75400,7 @@
       </c>
       <c r="AB141" s="16">
         <f>MAX(0,(va!AC137-va!AB137))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC141" s="16">
         <f>MAX(0,(va!AD137-va!AC137))</f>
@@ -75178,7 +75682,7 @@
       </c>
       <c r="AB142" s="16">
         <f>MAX(0,(va!AC138-va!AB138))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC142" s="16">
         <f>MAX(0,(va!AD138-va!AC138))</f>
@@ -75460,7 +75964,7 @@
       </c>
       <c r="AB143" s="16">
         <f>MAX(0,(va!AC139-va!AB139))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AC143" s="16">
         <f>MAX(0,(va!AD139-va!AC139))</f>

</xml_diff>

<commit_message>
19 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1EA7E9-70D6-4319-B314-6AF6C53EAF68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DA08DB-7E7F-4A54-9A0C-C2317C8F9B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="5110" windowWidth="20520" windowHeight="13130" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="6830" yWindow="5130" windowWidth="20520" windowHeight="13130" tabRatio="685" activeTab="5" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1003,7 +1003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1064,10 +1064,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1077,15 +1082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4026,8 +4023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E207B2A-317D-4660-A7D7-5B9F35994222}">
   <dimension ref="A1:CC46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AI22" sqref="AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4143,17 +4140,20 @@
       <c r="AG2" s="12">
         <v>11518</v>
       </c>
-      <c r="AH2" s="12">
+      <c r="AH2" s="36">
         <v>11525</v>
       </c>
-      <c r="AI2" s="12">
+      <c r="AI2" s="36">
         <v>12150</v>
       </c>
-      <c r="AJ2" s="12">
+      <c r="AJ2" s="36">
         <v>12643</v>
       </c>
-      <c r="AK2" s="12">
+      <c r="AK2" s="36">
         <v>13268</v>
+      </c>
+      <c r="AL2" s="12">
+        <v>13699</v>
       </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.35">
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AL3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2793</v>
       </c>
       <c r="AM3" s="10">
         <f t="shared" si="0"/>
@@ -4571,17 +4571,20 @@
       <c r="AG5" s="10">
         <v>67</v>
       </c>
-      <c r="AH5" s="10">
+      <c r="AH5" s="29">
         <v>72</v>
       </c>
-      <c r="AI5" s="10">
+      <c r="AI5" s="29">
         <v>81</v>
       </c>
-      <c r="AJ5" s="10">
+      <c r="AJ5" s="29">
         <v>86</v>
       </c>
-      <c r="AK5" s="10">
+      <c r="AK5" s="29">
         <v>91</v>
+      </c>
+      <c r="AL5" s="10">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:81" ht="39" x14ac:dyDescent="0.35">
@@ -4693,10 +4696,10 @@
       <c r="AJ6" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AK6" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AL6" s="18" t="s">
         <v>202</v>
       </c>
       <c r="AM6" s="3" t="s">
@@ -4929,17 +4932,20 @@
       <c r="AG7" s="10">
         <v>230</v>
       </c>
-      <c r="AH7" s="30">
+      <c r="AH7" s="29">
         <v>243</v>
       </c>
-      <c r="AI7" s="31">
+      <c r="AI7" s="29">
         <v>264</v>
       </c>
-      <c r="AJ7" s="33">
+      <c r="AJ7" s="29">
         <v>282</v>
       </c>
-      <c r="AK7" s="10">
+      <c r="AK7" s="29">
         <v>309</v>
+      </c>
+      <c r="AL7" s="10">
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.35">
@@ -5042,17 +5048,20 @@
       <c r="AG8" s="10">
         <v>182</v>
       </c>
-      <c r="AH8" s="30">
+      <c r="AH8" s="29">
         <v>183</v>
       </c>
-      <c r="AI8" s="31">
+      <c r="AI8" s="29">
         <v>193</v>
       </c>
-      <c r="AJ8" s="33">
+      <c r="AJ8" s="29">
         <v>207</v>
       </c>
-      <c r="AK8" s="10">
+      <c r="AK8" s="29">
         <v>215</v>
+      </c>
+      <c r="AL8" s="10">
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.35">
@@ -5155,17 +5164,20 @@
       <c r="AG9" s="10">
         <v>149</v>
       </c>
-      <c r="AH9" s="30">
+      <c r="AH9" s="29">
         <v>161</v>
       </c>
-      <c r="AI9" s="31">
+      <c r="AI9" s="29">
         <v>169</v>
       </c>
-      <c r="AJ9" s="33">
+      <c r="AJ9" s="29">
         <v>176</v>
       </c>
-      <c r="AK9" s="10">
+      <c r="AK9" s="29">
         <v>205</v>
+      </c>
+      <c r="AL9" s="10">
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.35">
@@ -5268,17 +5280,20 @@
       <c r="AG10" s="10">
         <v>326</v>
       </c>
-      <c r="AH10" s="30">
+      <c r="AH10" s="29">
         <v>361</v>
       </c>
-      <c r="AI10" s="31">
+      <c r="AI10" s="29">
         <v>389</v>
       </c>
-      <c r="AJ10" s="33">
+      <c r="AJ10" s="29">
         <v>423</v>
       </c>
-      <c r="AK10" s="10">
+      <c r="AK10" s="29">
         <v>459</v>
+      </c>
+      <c r="AL10" s="10">
+        <v>477</v>
       </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.35">
@@ -5381,17 +5396,20 @@
       <c r="AG11" s="10">
         <v>262</v>
       </c>
-      <c r="AH11" s="30">
+      <c r="AH11" s="29">
         <v>278</v>
       </c>
-      <c r="AI11" s="31">
+      <c r="AI11" s="29">
         <v>311</v>
       </c>
-      <c r="AJ11" s="33">
+      <c r="AJ11" s="29">
         <v>328</v>
       </c>
-      <c r="AK11" s="10">
+      <c r="AK11" s="29">
         <v>350</v>
+      </c>
+      <c r="AL11" s="10">
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.35">
@@ -5494,17 +5512,20 @@
       <c r="AG12" s="10">
         <v>290</v>
       </c>
-      <c r="AH12" s="30">
+      <c r="AH12" s="29">
         <v>298</v>
       </c>
-      <c r="AI12" s="31">
+      <c r="AI12" s="29">
         <v>313</v>
       </c>
-      <c r="AJ12" s="33">
+      <c r="AJ12" s="29">
         <v>337</v>
       </c>
-      <c r="AK12" s="10">
+      <c r="AK12" s="29">
         <v>353</v>
+      </c>
+      <c r="AL12" s="10">
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.35">
@@ -5607,17 +5628,20 @@
       <c r="AG13" s="10">
         <v>296</v>
       </c>
-      <c r="AH13" s="30">
+      <c r="AH13" s="29">
         <v>322</v>
       </c>
-      <c r="AI13" s="31">
+      <c r="AI13" s="29">
         <v>361</v>
       </c>
-      <c r="AJ13" s="33">
+      <c r="AJ13" s="29">
         <v>382</v>
       </c>
-      <c r="AK13" s="10">
+      <c r="AK13" s="29">
         <v>402</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.35">
@@ -5720,17 +5744,20 @@
       <c r="AG14" s="10">
         <v>237</v>
       </c>
-      <c r="AH14" s="30">
+      <c r="AH14" s="29">
         <v>259</v>
       </c>
-      <c r="AI14" s="31">
+      <c r="AI14" s="29">
         <v>293</v>
       </c>
-      <c r="AJ14" s="33">
+      <c r="AJ14" s="29">
         <v>316</v>
       </c>
-      <c r="AK14" s="10">
+      <c r="AK14" s="29">
         <v>339</v>
+      </c>
+      <c r="AL14" s="10">
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.35">
@@ -5833,17 +5860,20 @@
       <c r="AG15" s="10">
         <v>86</v>
       </c>
-      <c r="AH15" s="30">
+      <c r="AH15" s="29">
         <v>92</v>
       </c>
-      <c r="AI15" s="31">
+      <c r="AI15" s="29">
         <v>57</v>
       </c>
-      <c r="AJ15" s="33">
+      <c r="AJ15" s="29">
         <v>25</v>
       </c>
-      <c r="AK15" s="10">
+      <c r="AK15" s="29">
         <v>34</v>
+      </c>
+      <c r="AL15" s="10">
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.35">
@@ -5888,6 +5918,114 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O3:CC3">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:CC4">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:AG5 AL5:CC5">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:CC3">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:AG5 AL5:CC5">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:AG2 AL2:CC2">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD16:CC16 B7:AC15 AD8:AG15 AL8:CC15">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T7:AG15 AL7:CC15">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH8:AK15">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH7:AK15">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -5899,7 +6037,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:CC4">
+  <conditionalFormatting sqref="AH2:AK2">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -5911,7 +6049,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O5:CC5">
+  <conditionalFormatting sqref="AH5:AK5">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -5923,7 +6061,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:CC3">
+  <conditionalFormatting sqref="AH5:AK5">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -5959,19 +6097,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD8:CC16 B7:AC15">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T7:CC15">
+  <conditionalFormatting sqref="B7:CC15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5999,7 +6125,7 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6095,7 +6221,7 @@
         <v>53062</v>
       </c>
       <c r="AA2" s="10">
-        <v>0</v>
+        <v>55061</v>
       </c>
       <c r="AB2" s="10">
         <v>0</v>
@@ -6325,7 +6451,7 @@
       </c>
       <c r="AA3" s="10">
         <f>SUM(md[19-Apr])</f>
-        <v>0</v>
+        <v>12830</v>
       </c>
       <c r="AB3" s="10">
         <f>SUM(md[20-Apr])</f>
@@ -6573,7 +6699,7 @@
         <v>2757</v>
       </c>
       <c r="AA4" s="10">
-        <v>0</v>
+        <v>2886</v>
       </c>
       <c r="AB4" s="10">
         <v>0</v>
@@ -6779,7 +6905,7 @@
         <v>463</v>
       </c>
       <c r="AA5" s="10">
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="AB5" s="10">
         <v>0</v>
@@ -6987,7 +7113,7 @@
       <c r="Z6" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AA6" s="18" t="s">
         <v>203</v>
       </c>
       <c r="AB6" s="3" t="s">
@@ -7190,10 +7316,13 @@
       <c r="X7">
         <v>20</v>
       </c>
-      <c r="Y7" s="31">
+      <c r="Y7">
         <v>26</v>
       </c>
       <c r="Z7">
+        <v>33</v>
+      </c>
+      <c r="AA7">
         <v>33</v>
       </c>
     </row>
@@ -7270,11 +7399,14 @@
       <c r="X8" s="10">
         <v>896</v>
       </c>
-      <c r="Y8" s="31">
+      <c r="Y8" s="10">
         <v>966</v>
       </c>
       <c r="Z8" s="10">
         <v>1005</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>1047</v>
       </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.35">
@@ -7350,11 +7482,14 @@
       <c r="X9">
         <v>1160</v>
       </c>
-      <c r="Y9" s="32">
+      <c r="Y9">
         <v>1273</v>
       </c>
       <c r="Z9">
         <v>1378</v>
+      </c>
+      <c r="AA9">
+        <v>1392</v>
       </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.35">
@@ -7430,11 +7565,14 @@
       <c r="X10">
         <v>1516</v>
       </c>
-      <c r="Y10" s="32">
+      <c r="Y10">
         <v>1569</v>
       </c>
       <c r="Z10">
         <v>1664</v>
+      </c>
+      <c r="AA10">
+        <v>1733</v>
       </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.35">
@@ -7510,11 +7648,14 @@
       <c r="X11">
         <v>103</v>
       </c>
-      <c r="Y11" s="31">
+      <c r="Y11">
         <v>109</v>
       </c>
       <c r="Z11">
         <v>109</v>
+      </c>
+      <c r="AA11">
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.35">
@@ -7590,10 +7731,13 @@
       <c r="X12">
         <v>23</v>
       </c>
-      <c r="Y12" s="31">
+      <c r="Y12">
         <v>28</v>
       </c>
       <c r="Z12">
+        <v>33</v>
+      </c>
+      <c r="AA12">
         <v>33</v>
       </c>
     </row>
@@ -7670,11 +7814,14 @@
       <c r="X13">
         <v>283</v>
       </c>
-      <c r="Y13" s="31">
+      <c r="Y13">
         <v>288</v>
       </c>
       <c r="Z13">
         <v>308</v>
+      </c>
+      <c r="AA13">
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.35">
@@ -7750,10 +7897,13 @@
       <c r="X14">
         <v>101</v>
       </c>
-      <c r="Y14" s="31">
+      <c r="Y14">
         <v>127</v>
       </c>
       <c r="Z14">
+        <v>131</v>
+      </c>
+      <c r="AA14">
         <v>131</v>
       </c>
     </row>
@@ -7830,11 +7980,14 @@
       <c r="X15">
         <v>327</v>
       </c>
-      <c r="Y15" s="31">
+      <c r="Y15">
         <v>337</v>
       </c>
       <c r="Z15">
         <v>347</v>
+      </c>
+      <c r="AA15">
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -7910,14 +8063,17 @@
       <c r="X16" s="10">
         <v>18</v>
       </c>
-      <c r="Y16" s="31">
+      <c r="Y16" s="10">
         <v>20</v>
       </c>
       <c r="Z16" s="10">
         <v>20</v>
       </c>
+      <c r="AA16" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -7990,14 +8146,17 @@
       <c r="X17">
         <v>497</v>
       </c>
-      <c r="Y17" s="31">
+      <c r="Y17">
         <v>525</v>
       </c>
       <c r="Z17">
         <v>557</v>
       </c>
+      <c r="AA17">
+        <v>591</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8070,14 +8229,17 @@
       <c r="X18">
         <v>4</v>
       </c>
-      <c r="Y18" s="31">
+      <c r="Y18">
         <v>4</v>
       </c>
       <c r="Z18">
         <v>4</v>
       </c>
+      <c r="AA18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8150,14 +8312,17 @@
       <c r="X19">
         <v>161</v>
       </c>
-      <c r="Y19" s="31">
+      <c r="Y19">
         <v>176</v>
       </c>
       <c r="Z19">
         <v>195</v>
       </c>
+      <c r="AA19">
+        <v>210</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -8230,14 +8395,17 @@
       <c r="X20">
         <v>451</v>
       </c>
-      <c r="Y20" s="31">
+      <c r="Y20">
         <v>475</v>
       </c>
       <c r="Z20">
         <v>508</v>
       </c>
+      <c r="AA20">
+        <v>515</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -8310,14 +8478,17 @@
       <c r="X21">
         <v>11</v>
       </c>
-      <c r="Y21" s="31">
+      <c r="Y21">
         <v>14</v>
       </c>
       <c r="Z21">
         <v>16</v>
       </c>
+      <c r="AA21">
+        <v>18</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -8390,14 +8561,17 @@
       <c r="X22">
         <v>2133</v>
       </c>
-      <c r="Y22" s="32">
+      <c r="Y22">
         <v>2280</v>
       </c>
       <c r="Z22">
         <v>2404</v>
       </c>
+      <c r="AA22">
+        <v>2507</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -8470,14 +8644,17 @@
       <c r="X23">
         <v>2722</v>
       </c>
-      <c r="Y23" s="32">
+      <c r="Y23">
         <v>2966</v>
       </c>
       <c r="Z23">
         <v>3160</v>
       </c>
+      <c r="AA23">
+        <v>3345</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -8550,14 +8727,17 @@
       <c r="X24">
         <v>19</v>
       </c>
-      <c r="Y24" s="31">
+      <c r="Y24">
         <v>19</v>
       </c>
       <c r="Z24">
         <v>24</v>
       </c>
+      <c r="AA24">
+        <v>25</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -8630,14 +8810,17 @@
       <c r="X25">
         <v>98</v>
       </c>
-      <c r="Y25" s="31">
+      <c r="Y25">
         <v>100</v>
       </c>
       <c r="Z25">
         <v>101</v>
       </c>
+      <c r="AA25">
+        <v>105</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -8710,14 +8893,17 @@
       <c r="X26">
         <v>6</v>
       </c>
-      <c r="Y26" s="31">
+      <c r="Y26">
         <v>9</v>
       </c>
       <c r="Z26">
         <v>10</v>
       </c>
+      <c r="AA26">
+        <v>10</v>
+      </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -8790,14 +8976,17 @@
       <c r="X27">
         <v>14</v>
       </c>
-      <c r="Y27" s="31">
+      <c r="Y27">
         <v>14</v>
       </c>
       <c r="Z27">
         <v>16</v>
       </c>
+      <c r="AA27">
+        <v>19</v>
+      </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -8870,14 +9059,17 @@
       <c r="X28">
         <v>109</v>
       </c>
-      <c r="Y28" s="31">
+      <c r="Y28">
         <v>116</v>
       </c>
       <c r="Z28">
         <v>116</v>
       </c>
+      <c r="AA28">
+        <v>117</v>
+      </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -8950,14 +9142,17 @@
       <c r="X29">
         <v>87</v>
       </c>
-      <c r="Y29" s="31">
+      <c r="Y29">
         <v>103</v>
       </c>
       <c r="Z29">
         <v>138</v>
       </c>
+      <c r="AA29">
+        <v>145</v>
+      </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -9030,14 +9225,17 @@
       <c r="X30">
         <v>25</v>
       </c>
-      <c r="Y30" s="31">
+      <c r="Y30">
         <v>28</v>
       </c>
       <c r="Z30">
         <v>31</v>
       </c>
+      <c r="AA30">
+        <v>33</v>
+      </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -9131,7 +9329,7 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9261,7 +9459,7 @@
       </c>
       <c r="AD2" s="10">
         <f>SUM(va[19-Apr])</f>
-        <v>0</v>
+        <v>8537</v>
       </c>
       <c r="AE2" s="10">
         <f>SUM(va[20-Apr])</f>
@@ -9512,7 +9710,7 @@
         <v>1296</v>
       </c>
       <c r="AD3" s="10">
-        <v>0</v>
+        <v>1422</v>
       </c>
       <c r="AE3" s="10">
         <v>0</v>
@@ -9721,7 +9919,7 @@
         <v>258</v>
       </c>
       <c r="AD4" s="10">
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="AE4" s="10">
         <v>0</v>
@@ -9930,7 +10128,7 @@
         <v>51931</v>
       </c>
       <c r="AD5" s="10">
-        <v>0</v>
+        <v>54733</v>
       </c>
       <c r="AE5" s="10">
         <v>0</v>
@@ -10147,7 +10345,7 @@
       <c r="AC6" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AD6" s="18" t="s">
         <v>203</v>
       </c>
       <c r="AE6" s="3" t="s">
@@ -10365,9 +10563,12 @@
       <c r="AC7" s="10">
         <v>354</v>
       </c>
+      <c r="AD7" s="10">
+        <v>383</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -10454,9 +10655,12 @@
       <c r="AC8" s="10">
         <v>4</v>
       </c>
+      <c r="AD8" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A9" s="35"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -10541,9 +10745,12 @@
       <c r="AC9" s="10">
         <v>23</v>
       </c>
+      <c r="AD9" s="10">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -10628,9 +10835,12 @@
       <c r="AC10" s="10">
         <v>2</v>
       </c>
+      <c r="AD10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A11" s="35"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -10715,9 +10925,12 @@
       <c r="AC11" s="10">
         <v>20</v>
       </c>
+      <c r="AD11" s="10">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A12" s="35"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -10802,9 +11015,12 @@
       <c r="AC12" s="10">
         <v>1</v>
       </c>
+      <c r="AD12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A13" s="36"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -10887,6 +11103,9 @@
         <v>6</v>
       </c>
       <c r="AC13" s="10">
+        <v>6</v>
+      </c>
+      <c r="AD13" s="10">
         <v>6</v>
       </c>
     </row>
@@ -10978,9 +11197,12 @@
       <c r="AC14" s="10">
         <v>520</v>
       </c>
+      <c r="AD14" s="10">
+        <v>575</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -11067,9 +11289,12 @@
       <c r="AC15" s="10">
         <v>22</v>
       </c>
+      <c r="AD15" s="10">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -11154,9 +11379,12 @@
       <c r="AC16" s="10">
         <v>0</v>
       </c>
+      <c r="AD16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -11241,9 +11469,12 @@
       <c r="AC17" s="10">
         <v>0</v>
       </c>
+      <c r="AD17" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -11328,9 +11559,12 @@
       <c r="AC18" s="10">
         <v>5</v>
       </c>
+      <c r="AD18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A19" s="35"/>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -11415,9 +11649,12 @@
       <c r="AC19" s="10">
         <v>100</v>
       </c>
+      <c r="AD19" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A20" s="35"/>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -11502,9 +11739,12 @@
       <c r="AC20" s="10">
         <v>5</v>
       </c>
+      <c r="AD20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A21" s="35"/>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -11589,9 +11829,12 @@
       <c r="AC21" s="10">
         <v>233</v>
       </c>
+      <c r="AD21" s="10">
+        <v>236</v>
+      </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A22" s="35"/>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -11676,9 +11919,12 @@
       <c r="AC22" s="10">
         <v>3</v>
       </c>
+      <c r="AD22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A23" s="35"/>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -11763,9 +12009,12 @@
       <c r="AC23" s="10">
         <v>5</v>
       </c>
+      <c r="AD23" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A24" s="36"/>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -11850,9 +12099,12 @@
       <c r="AC24" s="10">
         <v>7</v>
       </c>
+      <c r="AD24" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A25" s="37" t="s">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -11939,9 +12191,12 @@
       <c r="AC25" s="10">
         <v>10</v>
       </c>
+      <c r="AD25" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A26" s="38"/>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -12026,9 +12281,12 @@
       <c r="AC26" s="10">
         <v>7</v>
       </c>
+      <c r="AD26" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A27" s="38"/>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -12113,9 +12371,12 @@
       <c r="AC27" s="10">
         <v>17</v>
       </c>
+      <c r="AD27" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A28" s="38"/>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -12200,9 +12461,12 @@
       <c r="AC28" s="10">
         <v>9</v>
       </c>
+      <c r="AD28" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A29" s="39"/>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -12287,8 +12551,11 @@
       <c r="AC29" s="10">
         <v>38</v>
       </c>
+      <c r="AD29" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -12376,9 +12643,12 @@
       <c r="AC30" s="10">
         <v>154</v>
       </c>
+      <c r="AD30" s="10">
+        <v>162</v>
+      </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A31" s="37" t="s">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -12465,9 +12735,12 @@
       <c r="AC31" s="10">
         <v>310</v>
       </c>
+      <c r="AD31" s="10">
+        <v>311</v>
+      </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A32" s="38"/>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -12552,9 +12825,12 @@
       <c r="AC32" s="10">
         <v>9</v>
       </c>
+      <c r="AD32" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -12639,9 +12915,12 @@
       <c r="AC33" s="10">
         <v>23</v>
       </c>
+      <c r="AD33" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -12728,9 +13007,12 @@
       <c r="AC34" s="10">
         <v>11</v>
       </c>
+      <c r="AD34" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A35" s="35"/>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -12815,9 +13097,12 @@
       <c r="AC35" s="10">
         <v>55</v>
       </c>
+      <c r="AD35" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A36" s="35"/>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -12902,9 +13187,12 @@
       <c r="AC36" s="10">
         <v>79</v>
       </c>
+      <c r="AD36" s="10">
+        <v>84</v>
+      </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A37" s="36"/>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -12989,9 +13277,12 @@
       <c r="AC37" s="10">
         <v>17</v>
       </c>
+      <c r="AD37" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A38" s="37" t="s">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -13078,9 +13369,12 @@
       <c r="AC38" s="10">
         <v>7</v>
       </c>
+      <c r="AD38" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A39" s="38"/>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -13165,9 +13459,12 @@
       <c r="AC39" s="10">
         <v>18</v>
       </c>
+      <c r="AD39" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A40" s="38"/>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -13252,9 +13549,12 @@
       <c r="AC40" s="10">
         <v>28</v>
       </c>
+      <c r="AD40" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A41" s="38"/>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -13339,9 +13639,12 @@
       <c r="AC41" s="10">
         <v>3</v>
       </c>
+      <c r="AD41" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A42" s="38"/>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -13426,9 +13729,12 @@
       <c r="AC42" s="10">
         <v>11</v>
       </c>
+      <c r="AD42" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A43" s="38"/>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -13513,9 +13819,12 @@
       <c r="AC43" s="10">
         <v>7</v>
       </c>
+      <c r="AD43" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A44" s="38"/>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -13600,9 +13909,12 @@
       <c r="AC44" s="10">
         <v>16</v>
       </c>
+      <c r="AD44" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A45" s="39"/>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -13687,9 +13999,12 @@
       <c r="AC45" s="10">
         <v>21</v>
       </c>
+      <c r="AD45" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A46" s="34" t="s">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -13776,9 +14091,12 @@
       <c r="AC46" s="10">
         <v>12</v>
       </c>
+      <c r="AD46" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A47" s="35"/>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -13863,9 +14181,12 @@
       <c r="AC47" s="10">
         <v>0</v>
       </c>
+      <c r="AD47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A48" s="35"/>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -13950,9 +14271,12 @@
       <c r="AC48" s="10">
         <v>2</v>
       </c>
+      <c r="AD48" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A49" s="36"/>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -14037,9 +14361,12 @@
       <c r="AC49" s="10">
         <v>4</v>
       </c>
+      <c r="AD49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A50" s="37" t="s">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -14126,9 +14453,12 @@
       <c r="AC50" s="10">
         <v>33</v>
       </c>
+      <c r="AD50" s="10">
+        <v>42</v>
+      </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A51" s="39"/>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -14213,9 +14543,12 @@
       <c r="AC51" s="10">
         <v>5</v>
       </c>
+      <c r="AD51" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A52" s="34" t="s">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -14302,9 +14635,12 @@
       <c r="AC52" s="10">
         <v>1633</v>
       </c>
+      <c r="AD52" s="10">
+        <v>1809</v>
+      </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A53" s="35"/>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -14389,9 +14725,12 @@
       <c r="AC53" s="10">
         <v>3</v>
       </c>
+      <c r="AD53" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A54" s="36"/>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -14476,8 +14815,11 @@
       <c r="AC54" s="10">
         <v>0</v>
       </c>
+      <c r="AD54" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -14565,8 +14907,11 @@
       <c r="AC55" s="10">
         <v>79</v>
       </c>
+      <c r="AD55" s="10">
+        <v>83</v>
+      </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -14654,9 +14999,12 @@
       <c r="AC56" s="10">
         <v>559</v>
       </c>
+      <c r="AD56" s="10">
+        <v>584</v>
+      </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A57" s="37" t="s">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -14743,9 +15091,12 @@
       <c r="AC57" s="10">
         <v>7</v>
       </c>
+      <c r="AD57" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A58" s="38"/>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -14830,9 +15181,12 @@
       <c r="AC58" s="10">
         <v>4</v>
       </c>
+      <c r="AD58" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A59" s="38"/>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -14917,9 +15271,12 @@
       <c r="AC59" s="10">
         <v>18</v>
       </c>
+      <c r="AD59" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A60" s="39"/>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -15004,9 +15361,12 @@
       <c r="AC60" s="10">
         <v>1</v>
       </c>
+      <c r="AD60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A61" s="34" t="s">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -15093,9 +15453,12 @@
       <c r="AC61" s="10">
         <v>6</v>
       </c>
+      <c r="AD61" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A62" s="35"/>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -15180,9 +15543,12 @@
       <c r="AC62" s="10">
         <v>81</v>
       </c>
+      <c r="AD62" s="10">
+        <v>81</v>
+      </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A63" s="35"/>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -15267,9 +15633,12 @@
       <c r="AC63" s="10">
         <v>13</v>
       </c>
+      <c r="AD63" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A64" s="35"/>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -15354,9 +15723,12 @@
       <c r="AC64" s="10">
         <v>39</v>
       </c>
+      <c r="AD64" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A65" s="35"/>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -15441,9 +15813,12 @@
       <c r="AC65" s="10">
         <v>24</v>
       </c>
+      <c r="AD65" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A66" s="36"/>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -15528,8 +15903,11 @@
       <c r="AC66" s="10">
         <v>25</v>
       </c>
+      <c r="AD66" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -15617,9 +15995,12 @@
       <c r="AC67" s="10">
         <v>413</v>
       </c>
+      <c r="AD67" s="10">
+        <v>425</v>
+      </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A68" s="34" t="s">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -15706,9 +16087,12 @@
       <c r="AC68" s="10">
         <v>0</v>
       </c>
+      <c r="AD68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A69" s="35"/>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -15793,9 +16177,12 @@
       <c r="AC69" s="10">
         <v>3</v>
       </c>
+      <c r="AD69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A70" s="35"/>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -15880,9 +16267,12 @@
       <c r="AC70" s="10">
         <v>0</v>
       </c>
+      <c r="AD70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A71" s="35"/>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -15967,9 +16357,12 @@
       <c r="AC71" s="10">
         <v>12</v>
       </c>
+      <c r="AD71" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A72" s="35"/>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -16054,9 +16447,12 @@
       <c r="AC72" s="10">
         <v>27</v>
       </c>
+      <c r="AD72" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A73" s="35"/>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -16141,9 +16537,12 @@
       <c r="AC73" s="10">
         <v>8</v>
       </c>
+      <c r="AD73" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A74" s="35"/>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -16228,9 +16627,12 @@
       <c r="AC74" s="10">
         <v>1</v>
       </c>
+      <c r="AD74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A75" s="36"/>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -16315,9 +16717,12 @@
       <c r="AC75" s="10">
         <v>1</v>
       </c>
+      <c r="AD75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A76" s="37" t="s">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -16404,9 +16809,12 @@
       <c r="AC76" s="10">
         <v>1</v>
       </c>
+      <c r="AD76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A77" s="38"/>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -16491,9 +16899,12 @@
       <c r="AC77" s="10">
         <v>4</v>
       </c>
+      <c r="AD77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A78" s="38"/>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -16578,9 +16989,12 @@
       <c r="AC78" s="10">
         <v>42</v>
       </c>
+      <c r="AD78" s="10">
+        <v>42</v>
+      </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A79" s="38"/>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -16665,9 +17079,12 @@
       <c r="AC79" s="10">
         <v>8</v>
       </c>
+      <c r="AD79" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A80" s="39"/>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -16752,8 +17169,11 @@
       <c r="AC80" s="10">
         <v>1</v>
       </c>
+      <c r="AD80" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -16841,9 +17261,12 @@
       <c r="AC81" s="10">
         <v>109</v>
       </c>
+      <c r="AD81" s="10">
+        <v>111</v>
+      </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A82" s="37" t="s">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -16930,9 +17353,12 @@
       <c r="AC82" s="10">
         <v>139</v>
       </c>
+      <c r="AD82" s="10">
+        <v>141</v>
+      </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A83" s="38"/>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -17017,9 +17443,12 @@
       <c r="AC83" s="10">
         <v>38</v>
       </c>
+      <c r="AD83" s="10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A84" s="38"/>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -17104,9 +17533,12 @@
       <c r="AC84" s="10">
         <v>102</v>
       </c>
+      <c r="AD84" s="10">
+        <v>101</v>
+      </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A85" s="38"/>
+    <row r="85" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -17191,9 +17623,12 @@
       <c r="AC85" s="10">
         <v>6</v>
       </c>
+      <c r="AD85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A86" s="39"/>
+    <row r="86" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -17278,9 +17713,12 @@
       <c r="AC86" s="10">
         <v>19</v>
       </c>
+      <c r="AD86" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A87" s="34" t="s">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -17367,9 +17805,12 @@
       <c r="AC87" s="10">
         <v>13</v>
       </c>
+      <c r="AD87" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A88" s="35"/>
+    <row r="88" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -17454,9 +17895,12 @@
       <c r="AC88" s="10">
         <v>25</v>
       </c>
+      <c r="AD88" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A89" s="35"/>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -17541,9 +17985,12 @@
       <c r="AC89" s="10">
         <v>8</v>
       </c>
+      <c r="AD89" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A90" s="35"/>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -17628,9 +18075,12 @@
       <c r="AC90" s="10">
         <v>10</v>
       </c>
+      <c r="AD90" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A91" s="35"/>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -17715,9 +18165,12 @@
       <c r="AC91" s="10">
         <v>3</v>
       </c>
+      <c r="AD91" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A92" s="35"/>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -17802,9 +18255,12 @@
       <c r="AC92" s="10">
         <v>6</v>
       </c>
+      <c r="AD92" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A93" s="36"/>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -17889,9 +18345,12 @@
       <c r="AC93" s="10">
         <v>17</v>
       </c>
+      <c r="AD93" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A94" s="37" t="s">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -17978,9 +18437,12 @@
       <c r="AC94" s="10">
         <v>6</v>
       </c>
+      <c r="AD94" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A95" s="39"/>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -18065,8 +18527,11 @@
       <c r="AC95" s="10">
         <v>24</v>
       </c>
+      <c r="AD95" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -18154,9 +18619,12 @@
       <c r="AC96" s="10">
         <v>65</v>
       </c>
+      <c r="AD96" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A97" s="37" t="s">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -18243,9 +18711,12 @@
       <c r="AC97" s="10">
         <v>700</v>
       </c>
+      <c r="AD97" s="10">
+        <v>742</v>
+      </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A98" s="38"/>
+    <row r="98" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -18330,9 +18801,12 @@
       <c r="AC98" s="10">
         <v>82</v>
       </c>
+      <c r="AD98" s="10">
+        <v>93</v>
+      </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A99" s="39"/>
+    <row r="99" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -18417,9 +18891,12 @@
       <c r="AC99" s="10">
         <v>21</v>
       </c>
+      <c r="AD99" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A100" s="34" t="s">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -18506,9 +18983,12 @@
       <c r="AC100" s="10">
         <v>13</v>
       </c>
+      <c r="AD100" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A101" s="35"/>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -18593,9 +19073,12 @@
       <c r="AC101" s="10">
         <v>18</v>
       </c>
+      <c r="AD101" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A102" s="35"/>
+    <row r="102" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -18680,9 +19163,12 @@
       <c r="AC102" s="10">
         <v>72</v>
       </c>
+      <c r="AD102" s="10">
+        <v>74</v>
+      </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A103" s="35"/>
+    <row r="103" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -18767,9 +19253,12 @@
       <c r="AC103" s="10">
         <v>143</v>
       </c>
+      <c r="AD103" s="10">
+        <v>152</v>
+      </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A104" s="36"/>
+    <row r="104" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -18854,9 +19343,12 @@
       <c r="AC104" s="10">
         <v>15</v>
       </c>
+      <c r="AD104" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A105" s="37" t="s">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -18943,9 +19435,12 @@
       <c r="AC105" s="10">
         <v>39</v>
       </c>
+      <c r="AD105" s="10">
+        <v>43</v>
+      </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A106" s="38"/>
+    <row r="106" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -19030,9 +19525,12 @@
       <c r="AC106" s="10">
         <v>36</v>
       </c>
+      <c r="AD106" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A107" s="38"/>
+    <row r="107" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -19117,9 +19615,12 @@
       <c r="AC107" s="10">
         <v>8</v>
       </c>
+      <c r="AD107" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A108" s="38"/>
+    <row r="108" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -19204,9 +19705,12 @@
       <c r="AC108" s="10">
         <v>20</v>
       </c>
+      <c r="AD108" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A109" s="39"/>
+    <row r="109" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -19291,8 +19795,11 @@
       <c r="AC109" s="10">
         <v>1</v>
       </c>
+      <c r="AD109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -19380,8 +19887,11 @@
       <c r="AC110" s="10">
         <v>211</v>
       </c>
+      <c r="AD110" s="10">
+        <v>231</v>
+      </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -19469,9 +19979,12 @@
       <c r="AC111" s="10">
         <v>24</v>
       </c>
+      <c r="AD111" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A112" s="34" t="s">
+    <row r="112" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -19558,9 +20071,12 @@
       <c r="AC112" s="10">
         <v>12</v>
       </c>
+      <c r="AD112" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A113" s="35"/>
+    <row r="113" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -19645,9 +20161,12 @@
       <c r="AC113" s="10">
         <v>8</v>
       </c>
+      <c r="AD113" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A114" s="36"/>
+    <row r="114" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -19732,9 +20251,12 @@
       <c r="AC114" s="10">
         <v>64</v>
       </c>
+      <c r="AD114" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A115" s="37" t="s">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -19821,9 +20343,12 @@
       <c r="AC115" s="10">
         <v>56</v>
       </c>
+      <c r="AD115" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A116" s="38"/>
+    <row r="116" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -19908,9 +20433,12 @@
       <c r="AC116" s="10">
         <v>66</v>
       </c>
+      <c r="AD116" s="10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A117" s="38"/>
+    <row r="117" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -19995,9 +20523,12 @@
       <c r="AC117" s="10">
         <v>8</v>
       </c>
+      <c r="AD117" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A118" s="38"/>
+    <row r="118" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -20082,9 +20613,12 @@
       <c r="AC118" s="10">
         <v>33</v>
       </c>
+      <c r="AD118" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A119" s="38"/>
+    <row r="119" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -20169,9 +20703,12 @@
       <c r="AC119" s="10">
         <v>5</v>
       </c>
+      <c r="AD119" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A120" s="39"/>
+    <row r="120" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -20256,9 +20793,12 @@
       <c r="AC120" s="10">
         <v>41</v>
       </c>
+      <c r="AD120" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A121" s="34" t="s">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -20345,9 +20885,12 @@
       <c r="AC121" s="10">
         <v>2</v>
       </c>
+      <c r="AD121" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A122" s="35"/>
+    <row r="122" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -20432,9 +20975,12 @@
       <c r="AC122" s="10">
         <v>21</v>
       </c>
+      <c r="AD122" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A123" s="35"/>
+    <row r="123" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -20519,9 +21065,12 @@
       <c r="AC123" s="10">
         <v>2</v>
       </c>
+      <c r="AD123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A124" s="35"/>
+    <row r="124" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -20606,9 +21155,12 @@
       <c r="AC124" s="10">
         <v>2</v>
       </c>
+      <c r="AD124" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A125" s="35"/>
+    <row r="125" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -20693,9 +21245,12 @@
       <c r="AC125" s="10">
         <v>1</v>
       </c>
+      <c r="AD125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A126" s="35"/>
+    <row r="126" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -20780,9 +21335,12 @@
       <c r="AC126" s="10">
         <v>3</v>
       </c>
+      <c r="AD126" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A127" s="35"/>
+    <row r="127" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -20867,9 +21425,12 @@
       <c r="AC127" s="10">
         <v>3</v>
       </c>
+      <c r="AD127" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A128" s="35"/>
+    <row r="128" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -20954,9 +21515,12 @@
       <c r="AC128" s="10">
         <v>5</v>
       </c>
+      <c r="AD128" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A129" s="35"/>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -21041,9 +21605,12 @@
       <c r="AC129" s="10">
         <v>8</v>
       </c>
+      <c r="AD129" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A130" s="36"/>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -21128,8 +21695,11 @@
       <c r="AC130" s="10">
         <v>10</v>
       </c>
+      <c r="AD130" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -21217,9 +21787,12 @@
       <c r="AC131" s="10">
         <v>271</v>
       </c>
+      <c r="AD131" s="10">
+        <v>273</v>
+      </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A132" s="34" t="s">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -21306,9 +21879,12 @@
       <c r="AC132" s="10">
         <v>15</v>
       </c>
+      <c r="AD132" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A133" s="35"/>
+    <row r="133" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -21393,9 +21969,12 @@
       <c r="AC133" s="10">
         <v>10</v>
       </c>
+      <c r="AD133" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A134" s="35"/>
+    <row r="134" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -21480,9 +22059,12 @@
       <c r="AC134" s="10">
         <v>0</v>
       </c>
+      <c r="AD134" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A135" s="36"/>
+    <row r="135" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -21567,9 +22149,12 @@
       <c r="AC135" s="10">
         <v>0</v>
       </c>
+      <c r="AD135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A136" s="37" t="s">
+    <row r="136" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -21656,9 +22241,12 @@
       <c r="AC136" s="10">
         <v>83</v>
       </c>
+      <c r="AD136" s="10">
+        <v>86</v>
+      </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A137" s="38"/>
+    <row r="137" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -21743,9 +22331,12 @@
       <c r="AC137" s="10">
         <v>9</v>
       </c>
+      <c r="AD137" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A138" s="38"/>
+    <row r="138" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -21830,9 +22421,12 @@
       <c r="AC138" s="10">
         <v>12</v>
       </c>
+      <c r="AD138" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A139" s="39"/>
+    <row r="139" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -21916,10 +22510,25 @@
       </c>
       <c r="AC139" s="10">
         <v>81</v>
+      </c>
+      <c r="AD139" s="10">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -21932,18 +22541,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:BB139 E1:BB1 BS7:BS139 BS1">
     <cfRule type="colorScale" priority="6">
@@ -22035,7 +22632,7 @@
   <dimension ref="A1:CC19"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22202,7 +22799,7 @@
       </c>
       <c r="AL2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.466357308584683</v>
       </c>
       <c r="AM2" s="19">
         <f t="shared" si="1"/>
@@ -22852,7 +23449,7 @@
       </c>
       <c r="AL4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.9370078740157481</v>
       </c>
       <c r="AM4" s="10">
         <f t="shared" si="7"/>
@@ -23177,7 +23774,7 @@
       </c>
       <c r="AL6" s="12">
         <f>MAX(0, (dc!AL2-dc!AK2))</f>
-        <v>0</v>
+        <v>431</v>
       </c>
       <c r="AM6" s="12">
         <f>MAX(0, (dc!AM2-dc!AL2))</f>
@@ -23501,7 +24098,7 @@
       </c>
       <c r="AL7" s="12">
         <f>MAX(0, (dc!AL3-dc!AK3))</f>
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="AM7" s="12">
         <f>MAX(0, (dc!AM3-dc!AL3))</f>
@@ -24149,7 +24746,7 @@
       </c>
       <c r="AL9" s="12">
         <f>MAX(0, (dc!AL5-dc!AK5))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM9" s="12">
         <f>MAX(0, (dc!AM5-dc!AL5))</f>
@@ -24701,7 +25298,7 @@
       </c>
       <c r="AL11" s="10">
         <f>MAX(0,(dc!AL7-dc!AK7))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AM11" s="10">
         <f>MAX(0,(dc!AM7-dc!AL7))</f>
@@ -25008,7 +25605,7 @@
       </c>
       <c r="AL12" s="10">
         <f>MAX(0,(dc!AL8-dc!AK8))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM12" s="10">
         <f>MAX(0,(dc!AM8-dc!AL8))</f>
@@ -25315,7 +25912,7 @@
       </c>
       <c r="AL13" s="10">
         <f>MAX(0,(dc!AL9-dc!AK9))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM13" s="10">
         <f>MAX(0,(dc!AM9-dc!AL9))</f>
@@ -25622,7 +26219,7 @@
       </c>
       <c r="AL14" s="10">
         <f>MAX(0,(dc!AL10-dc!AK10))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AM14" s="10">
         <f>MAX(0,(dc!AM10-dc!AL10))</f>
@@ -25929,7 +26526,7 @@
       </c>
       <c r="AL15" s="10">
         <f>MAX(0,(dc!AL11-dc!AK11))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AM15" s="10">
         <f>MAX(0,(dc!AM11-dc!AL11))</f>
@@ -26236,7 +26833,7 @@
       </c>
       <c r="AL16" s="10">
         <f>MAX(0,(dc!AL12-dc!AK12))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM16" s="10">
         <f>MAX(0,(dc!AM12-dc!AL12))</f>
@@ -26543,7 +27140,7 @@
       </c>
       <c r="AL17" s="10">
         <f>MAX(0,(dc!AL13-dc!AK13))</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AM17" s="10">
         <f>MAX(0,(dc!AM13-dc!AL13))</f>
@@ -26850,7 +27447,7 @@
       </c>
       <c r="AL18" s="10">
         <f>MAX(0,(dc!AL14-dc!AK14))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AM18" s="10">
         <f>MAX(0,(dc!AM14-dc!AL14))</f>
@@ -27157,7 +27754,7 @@
       </c>
       <c r="AL19" s="10">
         <f>MAX(0,(dc!AL15-dc!AK15))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AM19" s="10">
         <f>MAX(0,(dc!AM15-dc!AL15))</f>
@@ -27551,7 +28148,7 @@
       </c>
       <c r="AA2" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20.706069020230068</v>
       </c>
       <c r="AB2" s="21">
         <f t="shared" si="0"/>
@@ -27824,7 +28421,7 @@
       </c>
       <c r="AA3" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>24.712643678160919</v>
       </c>
       <c r="AB3" s="21">
         <f t="shared" si="2"/>
@@ -28097,7 +28694,7 @@
       </c>
       <c r="AA4" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.4061302681992336</v>
       </c>
       <c r="AB4" s="21">
         <f t="shared" si="4"/>
@@ -28433,7 +29030,7 @@
       </c>
       <c r="AA6" s="14">
         <f>MAX(0,(md!AA2-md!Z2)+(md!AA3-md!Z3))</f>
-        <v>0</v>
+        <v>2521</v>
       </c>
       <c r="AB6" s="14">
         <f>MAX(0,(md!AB2-md!AA2)+(md!AB3-md!AA3))</f>
@@ -28705,7 +29302,7 @@
       </c>
       <c r="AA7" s="14">
         <f>MAX(0,(md!AA3-md!Z3))</f>
-        <v>0</v>
+        <v>522</v>
       </c>
       <c r="AB7" s="14">
         <f>MAX(0,(md!AB3-md!AA3))</f>
@@ -28977,7 +29574,7 @@
       </c>
       <c r="AA8" s="14">
         <f>MAX(0,(md!AA4-md!Z4))</f>
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="AB8" s="14">
         <f>MAX(0,(md!AB4-md!AA4))</f>
@@ -29249,7 +29846,7 @@
       </c>
       <c r="AA9" s="14">
         <f>MAX(0,(md!AA5-md!Z5))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AB9" s="14">
         <f>MAX(0,(md!AB5-md!AA5))</f>
@@ -30012,7 +30609,7 @@
       </c>
       <c r="AA12" s="14">
         <f>MAX(0,(md!AA9-md!Z9))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AB12" s="14">
         <f>MAX(0,(md!AB9-md!AA9))</f>
@@ -30289,7 +30886,7 @@
       </c>
       <c r="AA13" s="14">
         <f>MAX(0,(md!AA9-md!Z9))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AB13" s="14">
         <f>MAX(0,(md!AB9-md!AA9))</f>
@@ -30566,7 +31163,7 @@
       </c>
       <c r="AA14" s="14">
         <f>MAX(0,(md!AA10-md!Z10))</f>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="AB14" s="14">
         <f>MAX(0,(md!AB10-md!AA10))</f>
@@ -30843,7 +31440,7 @@
       </c>
       <c r="AA15" s="14">
         <f>MAX(0,(md!AA11-md!Z11))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB15" s="14">
         <f>MAX(0,(md!AB11-md!AA11))</f>
@@ -31397,7 +31994,7 @@
       </c>
       <c r="AA17" s="14">
         <f>MAX(0,(md!AA13-md!Z13))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB17" s="14">
         <f>MAX(0,(md!AB13-md!AA13))</f>
@@ -31951,7 +32548,7 @@
       </c>
       <c r="AA19" s="14">
         <f>MAX(0,(md!AA15-md!Z15))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AB19" s="14">
         <f>MAX(0,(md!AB15-md!AA15))</f>
@@ -32228,7 +32825,7 @@
       </c>
       <c r="AA20" s="14">
         <f>MAX(0,(md!AA16-md!Z16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB20" s="14">
         <f>MAX(0,(md!AB16-md!AA16))</f>
@@ -32505,7 +33102,7 @@
       </c>
       <c r="AA21" s="14">
         <f>MAX(0,(md!AA17-md!Z17))</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AB21" s="14">
         <f>MAX(0,(md!AB17-md!AA17))</f>
@@ -33059,7 +33656,7 @@
       </c>
       <c r="AA23" s="14">
         <f>MAX(0,(md!AA19-md!Z19))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB23" s="14">
         <f>MAX(0,(md!AB19-md!AA19))</f>
@@ -33336,7 +33933,7 @@
       </c>
       <c r="AA24" s="14">
         <f>MAX(0,(md!AA20-md!Z20))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB24" s="14">
         <f>MAX(0,(md!AB20-md!AA20))</f>
@@ -33613,7 +34210,7 @@
       </c>
       <c r="AA25" s="14">
         <f>MAX(0,(md!AA21-md!Z21))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB25" s="14">
         <f>MAX(0,(md!AB21-md!AA21))</f>
@@ -33890,7 +34487,7 @@
       </c>
       <c r="AA26" s="14">
         <f>MAX(0,(md!AA22-md!Z22))</f>
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="AB26" s="14">
         <f>MAX(0,(md!AB22-md!AA22))</f>
@@ -34167,7 +34764,7 @@
       </c>
       <c r="AA27" s="14">
         <f>MAX(0,(md!AA23-md!Z23))</f>
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="AB27" s="14">
         <f>MAX(0,(md!AB23-md!AA23))</f>
@@ -34444,7 +35041,7 @@
       </c>
       <c r="AA28" s="14">
         <f>MAX(0,(md!AA24-md!Z24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB28" s="14">
         <f>MAX(0,(md!AB24-md!AA24))</f>
@@ -34721,7 +35318,7 @@
       </c>
       <c r="AA29" s="14">
         <f>MAX(0,(md!AA25-md!Z25))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB29" s="14">
         <f>MAX(0,(md!AB25-md!AA25))</f>
@@ -35275,7 +35872,7 @@
       </c>
       <c r="AA31" s="14">
         <f>MAX(0,(md!AA27-md!Z27))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB31" s="14">
         <f>MAX(0,(md!AB27-md!AA27))</f>
@@ -35552,7 +36149,7 @@
       </c>
       <c r="AA32" s="14">
         <f>MAX(0,(md!AA28-md!Z28))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB32" s="14">
         <f>MAX(0,(md!AB28-md!AA28))</f>
@@ -35829,7 +36426,7 @@
       </c>
       <c r="AA33" s="14">
         <f>MAX(0,(md!AA29-md!Z29))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB33" s="14">
         <f>MAX(0,(md!AB29-md!AA29))</f>
@@ -36106,7 +36703,7 @@
       </c>
       <c r="AA34" s="14">
         <f>MAX(0,(md!AA30-md!Z30))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB34" s="14">
         <f>MAX(0,(md!AB30-md!AA30))</f>
@@ -36458,8 +37055,8 @@
   </sheetPr>
   <dimension ref="A1:BS143"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36585,7 +37182,7 @@
       </c>
       <c r="AC2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.273376159885796</v>
       </c>
       <c r="AD2" s="20">
         <f t="shared" si="0"/>
@@ -36862,7 +37459,7 @@
       </c>
       <c r="AC3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>26.033057851239672</v>
       </c>
       <c r="AD3" s="20">
         <f t="shared" si="2"/>
@@ -37139,7 +37736,7 @@
       </c>
       <c r="AC4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.9256198347107438</v>
       </c>
       <c r="AD4" s="20">
         <f t="shared" si="4"/>
@@ -37416,7 +38013,7 @@
       </c>
       <c r="AC6" s="14">
         <f>MAX(0,(va!AD5-va!AC5))</f>
-        <v>0</v>
+        <v>2802</v>
       </c>
       <c r="AD6" s="14">
         <f>MAX(0,(va!AE5-va!AD5))</f>
@@ -37693,7 +38290,7 @@
       </c>
       <c r="AC7" s="14">
         <f>MAX(0,(va!AD2-va!AC2))</f>
-        <v>0</v>
+        <v>484</v>
       </c>
       <c r="AD7" s="14">
         <f>MAX(0,(va!AE2-va!AD2))</f>
@@ -37970,7 +38567,7 @@
       </c>
       <c r="AC8" s="14">
         <f>MAX(0,(va!AD3-va!AC3))</f>
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="AD8" s="14">
         <f>MAX(0,(va!AE3-va!AD3))</f>
@@ -38247,7 +38844,7 @@
       </c>
       <c r="AC9" s="14">
         <f>MAX(0,(va!AD4-va!AC4))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AD9" s="14">
         <f>MAX(0,(va!AE4-va!AD4))</f>
@@ -38744,7 +39341,7 @@
       </c>
       <c r="AC11" s="16">
         <f>MAX(0,(va!AD7-va!AC7))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AD11" s="16">
         <f>MAX(0,(va!AE7-va!AD7))</f>
@@ -39026,7 +39623,7 @@
       </c>
       <c r="AC12" s="16">
         <f>MAX(0,(va!AD8-va!AC8))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="16">
         <f>MAX(0,(va!AE8-va!AD8))</f>
@@ -39308,7 +39905,7 @@
       </c>
       <c r="AC13" s="16">
         <f>MAX(0,(va!AD9-va!AC9))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD13" s="16">
         <f>MAX(0,(va!AE9-va!AD9))</f>
@@ -39872,7 +40469,7 @@
       </c>
       <c r="AC15" s="16">
         <f>MAX(0,(va!AD11-va!AC11))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD15" s="16">
         <f>MAX(0,(va!AE11-va!AD11))</f>
@@ -40718,7 +41315,7 @@
       </c>
       <c r="AC18" s="16">
         <f>MAX(0,(va!AD14-va!AC14))</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="AD18" s="16">
         <f>MAX(0,(va!AE14-va!AD14))</f>
@@ -42692,7 +43289,7 @@
       </c>
       <c r="AC25" s="16">
         <f>MAX(0,(va!AD21-va!AC21))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD25" s="16">
         <f>MAX(0,(va!AE21-va!AD21))</f>
@@ -44384,7 +44981,7 @@
       </c>
       <c r="AC31" s="16">
         <f>MAX(0,(va!AD27-va!AC27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD31" s="16">
         <f>MAX(0,(va!AE27-va!AD27))</f>
@@ -45230,7 +45827,7 @@
       </c>
       <c r="AC34" s="16">
         <f>MAX(0,(va!AD30-va!AC30))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD34" s="16">
         <f>MAX(0,(va!AE30-va!AD30))</f>
@@ -45512,7 +46109,7 @@
       </c>
       <c r="AC35" s="16">
         <f>MAX(0,(va!AD31-va!AC31))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD35" s="16">
         <f>MAX(0,(va!AE31-va!AD31))</f>
@@ -46922,7 +47519,7 @@
       </c>
       <c r="AC40" s="16">
         <f>MAX(0,(va!AD36-va!AC36))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD40" s="16">
         <f>MAX(0,(va!AE36-va!AD36))</f>
@@ -50870,7 +51467,7 @@
       </c>
       <c r="AC54" s="16">
         <f>MAX(0,(va!AD50-va!AC50))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AD54" s="16">
         <f>MAX(0,(va!AE50-va!AD50))</f>
@@ -51152,7 +51749,7 @@
       </c>
       <c r="AC55" s="16">
         <f>MAX(0,(va!AD51-va!AC51))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD55" s="16">
         <f>MAX(0,(va!AE51-va!AD51))</f>
@@ -51434,7 +52031,7 @@
       </c>
       <c r="AC56" s="16">
         <f>MAX(0,(va!AD52-va!AC52))</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AD56" s="16">
         <f>MAX(0,(va!AE52-va!AD52))</f>
@@ -51716,7 +52313,7 @@
       </c>
       <c r="AC57" s="16">
         <f>MAX(0,(va!AD53-va!AC53))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD57" s="16">
         <f>MAX(0,(va!AE53-va!AD53))</f>
@@ -52280,7 +52877,7 @@
       </c>
       <c r="AC59" s="16">
         <f>MAX(0,(va!AD55-va!AC55))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD59" s="16">
         <f>MAX(0,(va!AE55-va!AD55))</f>
@@ -52562,7 +53159,7 @@
       </c>
       <c r="AC60" s="16">
         <f>MAX(0,(va!AD56-va!AC56))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AD60" s="16">
         <f>MAX(0,(va!AE56-va!AD56))</f>
@@ -53690,7 +54287,7 @@
       </c>
       <c r="AC64" s="16">
         <f>MAX(0,(va!AD60-va!AC60))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD64" s="16">
         <f>MAX(0,(va!AE60-va!AD60))</f>
@@ -55664,7 +56261,7 @@
       </c>
       <c r="AC71" s="16">
         <f>MAX(0,(va!AD67-va!AC67))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AD71" s="16">
         <f>MAX(0,(va!AE67-va!AD67))</f>
@@ -57074,7 +57671,7 @@
       </c>
       <c r="AC76" s="16">
         <f>MAX(0,(va!AD72-va!AC72))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD76" s="16">
         <f>MAX(0,(va!AE72-va!AD72))</f>
@@ -57356,7 +57953,7 @@
       </c>
       <c r="AC77" s="16">
         <f>MAX(0,(va!AD73-va!AC73))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD77" s="16">
         <f>MAX(0,(va!AE73-va!AD73))</f>
@@ -59612,7 +60209,7 @@
       </c>
       <c r="AC85" s="16">
         <f>MAX(0,(va!AD81-va!AC81))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD85" s="16">
         <f>MAX(0,(va!AE81-va!AD81))</f>
@@ -59894,7 +60491,7 @@
       </c>
       <c r="AC86" s="16">
         <f>MAX(0,(va!AD82-va!AC82))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD86" s="16">
         <f>MAX(0,(va!AE82-va!AD82))</f>
@@ -60176,7 +60773,7 @@
       </c>
       <c r="AC87" s="16">
         <f>MAX(0,(va!AD83-va!AC83))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD87" s="16">
         <f>MAX(0,(va!AE83-va!AD83))</f>
@@ -61304,7 +61901,7 @@
       </c>
       <c r="AC91" s="16">
         <f>MAX(0,(va!AD87-va!AC87))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD91" s="16">
         <f>MAX(0,(va!AE87-va!AD87))</f>
@@ -61586,7 +62183,7 @@
       </c>
       <c r="AC92" s="16">
         <f>MAX(0,(va!AD88-va!AC88))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD92" s="16">
         <f>MAX(0,(va!AE88-va!AD88))</f>
@@ -62714,7 +63311,7 @@
       </c>
       <c r="AC96" s="16">
         <f>MAX(0,(va!AD92-va!AC92))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD96" s="16">
         <f>MAX(0,(va!AE92-va!AD92))</f>
@@ -63560,7 +64157,7 @@
       </c>
       <c r="AC99" s="16">
         <f>MAX(0,(va!AD95-va!AC95))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD99" s="16">
         <f>MAX(0,(va!AE95-va!AD95))</f>
@@ -64124,7 +64721,7 @@
       </c>
       <c r="AC101" s="16">
         <f>MAX(0,(va!AD97-va!AC97))</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="AD101" s="16">
         <f>MAX(0,(va!AE97-va!AD97))</f>
@@ -64406,7 +65003,7 @@
       </c>
       <c r="AC102" s="16">
         <f>MAX(0,(va!AD98-va!AC98))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AD102" s="16">
         <f>MAX(0,(va!AE98-va!AD98))</f>
@@ -64688,7 +65285,7 @@
       </c>
       <c r="AC103" s="16">
         <f>MAX(0,(va!AD99-va!AC99))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD103" s="16">
         <f>MAX(0,(va!AE99-va!AD99))</f>
@@ -65534,7 +66131,7 @@
       </c>
       <c r="AC106" s="16">
         <f>MAX(0,(va!AD102-va!AC102))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD106" s="16">
         <f>MAX(0,(va!AE102-va!AD102))</f>
@@ -65816,7 +66413,7 @@
       </c>
       <c r="AC107" s="16">
         <f>MAX(0,(va!AD103-va!AC103))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AD107" s="16">
         <f>MAX(0,(va!AE103-va!AD103))</f>
@@ -66098,7 +66695,7 @@
       </c>
       <c r="AC108" s="16">
         <f>MAX(0,(va!AD104-va!AC104))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD108" s="16">
         <f>MAX(0,(va!AE104-va!AD104))</f>
@@ -66380,7 +66977,7 @@
       </c>
       <c r="AC109" s="16">
         <f>MAX(0,(va!AD105-va!AC105))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD109" s="16">
         <f>MAX(0,(va!AE105-va!AD105))</f>
@@ -66662,7 +67259,7 @@
       </c>
       <c r="AC110" s="16">
         <f>MAX(0,(va!AD106-va!AC106))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD110" s="16">
         <f>MAX(0,(va!AE106-va!AD106))</f>
@@ -67790,7 +68387,7 @@
       </c>
       <c r="AC114" s="16">
         <f>MAX(0,(va!AD110-va!AC110))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD114" s="16">
         <f>MAX(0,(va!AE110-va!AD110))</f>
@@ -68918,7 +69515,7 @@
       </c>
       <c r="AC118" s="16">
         <f>MAX(0,(va!AD114-va!AC114))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD118" s="16">
         <f>MAX(0,(va!AE114-va!AD114))</f>
@@ -69200,7 +69797,7 @@
       </c>
       <c r="AC119" s="16">
         <f>MAX(0,(va!AD115-va!AC115))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD119" s="16">
         <f>MAX(0,(va!AE115-va!AD115))</f>
@@ -73148,7 +73745,7 @@
       </c>
       <c r="AC133" s="16">
         <f>MAX(0,(va!AD129-va!AC129))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD133" s="16">
         <f>MAX(0,(va!AE129-va!AD129))</f>
@@ -73712,7 +74309,7 @@
       </c>
       <c r="AC135" s="16">
         <f>MAX(0,(va!AD131-va!AC131))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD135" s="16">
         <f>MAX(0,(va!AE131-va!AD131))</f>
@@ -75122,7 +75719,7 @@
       </c>
       <c r="AC140" s="16">
         <f>MAX(0,(va!AD136-va!AC136))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD140" s="16">
         <f>MAX(0,(va!AE136-va!AD136))</f>
@@ -75404,7 +76001,7 @@
       </c>
       <c r="AC141" s="16">
         <f>MAX(0,(va!AD137-va!AC137))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AD141" s="16">
         <f>MAX(0,(va!AE137-va!AD137))</f>
@@ -75968,7 +76565,7 @@
       </c>
       <c r="AC143" s="16">
         <f>MAX(0,(va!AD139-va!AC139))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD143" s="16">
         <f>MAX(0,(va!AE139-va!AD139))</f>

</xml_diff>

<commit_message>
24 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BA3791-10FF-4A49-8CF5-3EF5C5779C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB1B1C6-D996-4575-BD5B-D7CA0B8255CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4015,7 +4015,7 @@
   <dimension ref="A1:CC46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
@@ -4161,6 +4161,9 @@
       <c r="AP2" s="12">
         <v>15930</v>
       </c>
+      <c r="AQ2" s="12">
+        <v>16533</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4317,7 +4320,7 @@
       </c>
       <c r="AQ3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3528</v>
       </c>
       <c r="AR3" s="10">
         <f t="shared" si="0"/>
@@ -4604,6 +4607,9 @@
       <c r="AP5" s="10">
         <v>139</v>
       </c>
+      <c r="AQ5" s="10">
+        <v>153</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -4977,6 +4983,9 @@
       <c r="AP7" s="10">
         <v>376</v>
       </c>
+      <c r="AQ7" s="10">
+        <v>403</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5105,6 +5114,9 @@
       <c r="AP8" s="10">
         <v>252</v>
       </c>
+      <c r="AQ8" s="10">
+        <v>251</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5233,6 +5245,9 @@
       <c r="AP9" s="10">
         <v>227</v>
       </c>
+      <c r="AQ9" s="10">
+        <v>252</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5361,6 +5376,9 @@
       <c r="AP10" s="10">
         <v>562</v>
       </c>
+      <c r="AQ10" s="10">
+        <v>595</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5489,6 +5507,9 @@
       <c r="AP11" s="10">
         <v>456</v>
       </c>
+      <c r="AQ11" s="10">
+        <v>488</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5617,6 +5638,9 @@
       <c r="AP12" s="10">
         <v>406</v>
       </c>
+      <c r="AQ12" s="10">
+        <v>409</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5745,6 +5769,9 @@
       <c r="AP13" s="10">
         <v>508</v>
       </c>
+      <c r="AQ13" s="10">
+        <v>522</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -5873,6 +5900,9 @@
       <c r="AP14" s="10">
         <v>477</v>
       </c>
+      <c r="AQ14" s="10">
+        <v>498</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6000,6 +6030,9 @@
       </c>
       <c r="AP15" s="10">
         <v>97</v>
+      </c>
+      <c r="AQ15" s="10">
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6251,10 +6284,10 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomRight" activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6365,7 +6398,7 @@
         <v>64363</v>
       </c>
       <c r="AF2" s="10">
-        <v>0</v>
+        <v>68100</v>
       </c>
       <c r="AG2" s="10">
         <v>0</v>
@@ -6600,7 +6633,7 @@
       </c>
       <c r="AF3" s="10">
         <f>SUM(md[24-Apr])</f>
-        <v>0</v>
+        <v>16616</v>
       </c>
       <c r="AG3" s="10">
         <f>SUM(md[25-Apr])</f>
@@ -6843,7 +6876,7 @@
         <v>3477</v>
       </c>
       <c r="AF4" s="10">
-        <v>0</v>
+        <v>3618</v>
       </c>
       <c r="AG4" s="10">
         <v>0</v>
@@ -7049,7 +7082,7 @@
         <v>680</v>
       </c>
       <c r="AF5" s="10">
-        <v>0</v>
+        <v>723</v>
       </c>
       <c r="AG5" s="10">
         <v>0</v>
@@ -7466,6 +7499,9 @@
       <c r="AE7">
         <v>77</v>
       </c>
+      <c r="AF7">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7561,6 +7597,9 @@
       <c r="AE8" s="10">
         <v>1294</v>
       </c>
+      <c r="AF8" s="10">
+        <v>1373</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7656,6 +7695,9 @@
       <c r="AE9">
         <v>1672</v>
       </c>
+      <c r="AF9">
+        <v>1728</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7751,6 +7793,9 @@
       <c r="AE10">
         <v>2132</v>
       </c>
+      <c r="AF10">
+        <v>2234</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -7846,6 +7891,9 @@
       <c r="AE11">
         <v>121</v>
       </c>
+      <c r="AF11">
+        <v>125</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -7941,6 +7989,9 @@
       <c r="AE12">
         <v>50</v>
       </c>
+      <c r="AF12">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8036,6 +8087,9 @@
       <c r="AE13">
         <v>355</v>
       </c>
+      <c r="AF13">
+        <v>372</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8131,6 +8185,9 @@
       <c r="AE14">
         <v>140</v>
       </c>
+      <c r="AF14">
+        <v>144</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8226,6 +8283,9 @@
       <c r="AE15">
         <v>442</v>
       </c>
+      <c r="AF15">
+        <v>459</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8321,8 +8381,11 @@
       <c r="AE16" s="10">
         <v>31</v>
       </c>
+      <c r="AF16" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8416,8 +8479,11 @@
       <c r="AE17">
         <v>690</v>
       </c>
+      <c r="AF17">
+        <v>765</v>
+      </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8511,8 +8577,11 @@
       <c r="AE18">
         <v>4</v>
       </c>
+      <c r="AF18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8606,8 +8675,11 @@
       <c r="AE19">
         <v>280</v>
       </c>
+      <c r="AF19">
+        <v>289</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -8701,8 +8773,11 @@
       <c r="AE20">
         <v>618</v>
       </c>
+      <c r="AF20">
+        <v>642</v>
+      </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -8796,8 +8871,11 @@
       <c r="AE21">
         <v>64</v>
       </c>
+      <c r="AF21">
+        <v>67</v>
+      </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -8891,8 +8969,11 @@
       <c r="AE22">
         <v>3060</v>
       </c>
+      <c r="AF22">
+        <v>3227</v>
+      </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -8986,8 +9067,11 @@
       <c r="AE23">
         <v>4141</v>
       </c>
+      <c r="AF23">
+        <v>4403</v>
+      </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9081,8 +9165,11 @@
       <c r="AE24">
         <v>33</v>
       </c>
+      <c r="AF24">
+        <v>43</v>
+      </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9176,8 +9263,11 @@
       <c r="AE25">
         <v>115</v>
       </c>
+      <c r="AF25">
+        <v>119</v>
+      </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9271,8 +9361,11 @@
       <c r="AE26">
         <v>12</v>
       </c>
+      <c r="AF26">
+        <v>13</v>
+      </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -9366,8 +9459,11 @@
       <c r="AE27">
         <v>25</v>
       </c>
+      <c r="AF27">
+        <v>23</v>
+      </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -9461,8 +9557,11 @@
       <c r="AE28">
         <v>139</v>
       </c>
+      <c r="AF28">
+        <v>143</v>
+      </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -9556,8 +9655,11 @@
       <c r="AE29">
         <v>203</v>
       </c>
+      <c r="AF29">
+        <v>222</v>
+      </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -9651,8 +9753,11 @@
       <c r="AE30">
         <v>39</v>
       </c>
+      <c r="AF30">
+        <v>44</v>
+      </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -9746,10 +9851,10 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="Q6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9899,7 +10004,7 @@
       </c>
       <c r="AI2" s="10">
         <f>SUM(va[24-Apr])</f>
-        <v>0</v>
+        <v>11594</v>
       </c>
       <c r="AJ2" s="10">
         <f>SUM(va[25-Apr])</f>
@@ -10145,7 +10250,7 @@
         <v>1753</v>
       </c>
       <c r="AI3" s="10">
-        <v>0</v>
+        <v>1837</v>
       </c>
       <c r="AJ3" s="10">
         <v>0</v>
@@ -10354,7 +10459,7 @@
         <v>372</v>
       </c>
       <c r="AI4" s="10">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="AJ4" s="10">
         <v>0</v>
@@ -10563,7 +10668,7 @@
         <v>64518</v>
       </c>
       <c r="AI5" s="10">
-        <v>0</v>
+        <v>69015</v>
       </c>
       <c r="AJ5" s="10">
         <v>0</v>
@@ -10998,9 +11103,12 @@
       <c r="AH7" s="10">
         <v>512</v>
       </c>
+      <c r="AI7" s="10">
+        <v>547</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11102,9 +11210,12 @@
       <c r="AH8" s="10">
         <v>5</v>
       </c>
+      <c r="AI8" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11204,9 +11315,12 @@
       <c r="AH9" s="10">
         <v>26</v>
       </c>
+      <c r="AI9" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -11306,9 +11420,12 @@
       <c r="AH10" s="10">
         <v>2</v>
       </c>
+      <c r="AI10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -11408,9 +11525,12 @@
       <c r="AH11" s="10">
         <v>34</v>
       </c>
+      <c r="AI11" s="10">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -11510,9 +11630,12 @@
       <c r="AH12" s="10">
         <v>1</v>
       </c>
+      <c r="AI12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -11610,6 +11733,9 @@
         <v>8</v>
       </c>
       <c r="AH13" s="10">
+        <v>8</v>
+      </c>
+      <c r="AI13" s="10">
         <v>8</v>
       </c>
     </row>
@@ -11716,9 +11842,12 @@
       <c r="AH14" s="10">
         <v>686</v>
       </c>
+      <c r="AI14" s="10">
+        <v>722</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -11820,9 +11949,12 @@
       <c r="AH15" s="10">
         <v>33</v>
       </c>
+      <c r="AI15" s="10">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -11922,9 +12054,12 @@
       <c r="AH16" s="10">
         <v>0</v>
       </c>
+      <c r="AI16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12024,9 +12159,12 @@
       <c r="AH17" s="10">
         <v>1</v>
       </c>
+      <c r="AI17" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -12126,9 +12264,12 @@
       <c r="AH18" s="10">
         <v>5</v>
       </c>
+      <c r="AI18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -12228,9 +12369,12 @@
       <c r="AH19" s="10">
         <v>163</v>
       </c>
+      <c r="AI19" s="10">
+        <v>176</v>
+      </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -12330,9 +12474,12 @@
       <c r="AH20" s="10">
         <v>5</v>
       </c>
+      <c r="AI20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -12432,9 +12579,12 @@
       <c r="AH21" s="10">
         <v>346</v>
       </c>
+      <c r="AI21" s="10">
+        <v>355</v>
+      </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -12534,9 +12684,12 @@
       <c r="AH22" s="10">
         <v>3</v>
       </c>
+      <c r="AI22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -12636,9 +12789,12 @@
       <c r="AH23" s="10">
         <v>10</v>
       </c>
+      <c r="AI23" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -12738,9 +12894,12 @@
       <c r="AH24" s="10">
         <v>9</v>
       </c>
+      <c r="AI24" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -12842,9 +13001,12 @@
       <c r="AH25" s="10">
         <v>9</v>
       </c>
+      <c r="AI25" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -12944,9 +13106,12 @@
       <c r="AH26" s="10">
         <v>12</v>
       </c>
+      <c r="AI26" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -13046,9 +13211,12 @@
       <c r="AH27" s="10">
         <v>21</v>
       </c>
+      <c r="AI27" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -13148,9 +13316,12 @@
       <c r="AH28" s="10">
         <v>10</v>
       </c>
+      <c r="AI28" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -13250,8 +13421,11 @@
       <c r="AH29" s="10">
         <v>47</v>
       </c>
+      <c r="AI29" s="10">
+        <v>48</v>
+      </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -13354,9 +13528,12 @@
       <c r="AH30" s="10">
         <v>186</v>
       </c>
+      <c r="AI30" s="10">
+        <v>197</v>
+      </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -13458,9 +13635,12 @@
       <c r="AH31" s="10">
         <v>402</v>
       </c>
+      <c r="AI31" s="10">
+        <v>423</v>
+      </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -13560,9 +13740,12 @@
       <c r="AH32" s="10">
         <v>9</v>
       </c>
+      <c r="AI32" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -13662,9 +13845,12 @@
       <c r="AH33" s="10">
         <v>41</v>
       </c>
+      <c r="AI33" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -13766,9 +13952,12 @@
       <c r="AH34" s="10">
         <v>12</v>
       </c>
+      <c r="AI34" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -13868,9 +14057,12 @@
       <c r="AH35" s="10">
         <v>63</v>
       </c>
+      <c r="AI35" s="10">
+        <v>69</v>
+      </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -13970,9 +14162,12 @@
       <c r="AH36" s="10">
         <v>99</v>
       </c>
+      <c r="AI36" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -14072,9 +14267,12 @@
       <c r="AH37" s="10">
         <v>20</v>
       </c>
+      <c r="AI37" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -14176,9 +14374,12 @@
       <c r="AH38" s="10">
         <v>12</v>
       </c>
+      <c r="AI38" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -14278,9 +14479,12 @@
       <c r="AH39" s="10">
         <v>30</v>
       </c>
+      <c r="AI39" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -14380,9 +14584,12 @@
       <c r="AH40" s="10">
         <v>29</v>
       </c>
+      <c r="AI40" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -14482,9 +14689,12 @@
       <c r="AH41" s="10">
         <v>4</v>
       </c>
+      <c r="AI41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -14584,9 +14794,12 @@
       <c r="AH42" s="10">
         <v>25</v>
       </c>
+      <c r="AI42" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -14686,9 +14899,12 @@
       <c r="AH43" s="10">
         <v>18</v>
       </c>
+      <c r="AI43" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -14788,9 +15004,12 @@
       <c r="AH44" s="10">
         <v>19</v>
       </c>
+      <c r="AI44" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -14890,9 +15109,12 @@
       <c r="AH45" s="10">
         <v>27</v>
       </c>
+      <c r="AI45" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -14994,9 +15216,12 @@
       <c r="AH46" s="10">
         <v>12</v>
       </c>
+      <c r="AI46" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -15096,9 +15321,12 @@
       <c r="AH47" s="10">
         <v>0</v>
       </c>
+      <c r="AI47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -15198,9 +15426,12 @@
       <c r="AH48" s="10">
         <v>2</v>
       </c>
+      <c r="AI48" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -15300,9 +15531,12 @@
       <c r="AH49" s="10">
         <v>4</v>
       </c>
+      <c r="AI49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -15404,9 +15638,12 @@
       <c r="AH50" s="10">
         <v>76</v>
       </c>
+      <c r="AI50" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -15506,9 +15743,12 @@
       <c r="AH51" s="10">
         <v>12</v>
       </c>
+      <c r="AI51" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -15610,9 +15850,12 @@
       <c r="AH52" s="10">
         <v>2362</v>
       </c>
+      <c r="AI52" s="10">
+        <v>2534</v>
+      </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -15712,9 +15955,12 @@
       <c r="AH53" s="10">
         <v>26</v>
       </c>
+      <c r="AI53" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -15814,8 +16060,11 @@
       <c r="AH54" s="10">
         <v>25</v>
       </c>
+      <c r="AI54" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -15918,8 +16167,11 @@
       <c r="AH55" s="10">
         <v>99</v>
       </c>
+      <c r="AI55" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -16022,9 +16274,12 @@
       <c r="AH56" s="10">
         <v>718</v>
       </c>
+      <c r="AI56" s="10">
+        <v>729</v>
+      </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -16126,9 +16381,12 @@
       <c r="AH57" s="10">
         <v>7</v>
       </c>
+      <c r="AI57" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -16228,9 +16486,12 @@
       <c r="AH58" s="10">
         <v>5</v>
       </c>
+      <c r="AI58" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -16330,9 +16591,12 @@
       <c r="AH59" s="10">
         <v>20</v>
       </c>
+      <c r="AI59" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -16432,9 +16696,12 @@
       <c r="AH60" s="10">
         <v>2</v>
       </c>
+      <c r="AI60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -16536,9 +16803,12 @@
       <c r="AH61" s="10">
         <v>7</v>
       </c>
+      <c r="AI61" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -16638,9 +16908,12 @@
       <c r="AH62" s="10">
         <v>87</v>
       </c>
+      <c r="AI62" s="10">
+        <v>87</v>
+      </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -16740,9 +17013,12 @@
       <c r="AH63" s="10">
         <v>22</v>
       </c>
+      <c r="AI63" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -16842,9 +17118,12 @@
       <c r="AH64" s="10">
         <v>58</v>
       </c>
+      <c r="AI64" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -16944,9 +17223,12 @@
       <c r="AH65" s="10">
         <v>30</v>
       </c>
+      <c r="AI65" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -17046,8 +17328,11 @@
       <c r="AH66" s="10">
         <v>30</v>
       </c>
+      <c r="AI66" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -17150,9 +17435,12 @@
       <c r="AH67" s="10">
         <v>498</v>
       </c>
+      <c r="AI67" s="10">
+        <v>529</v>
+      </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -17254,9 +17542,12 @@
       <c r="AH68" s="10">
         <v>0</v>
       </c>
+      <c r="AI68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -17356,9 +17647,12 @@
       <c r="AH69" s="10">
         <v>3</v>
       </c>
+      <c r="AI69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -17458,9 +17752,12 @@
       <c r="AH70" s="10">
         <v>0</v>
       </c>
+      <c r="AI70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -17560,9 +17857,12 @@
       <c r="AH71" s="10">
         <v>13</v>
       </c>
+      <c r="AI71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -17662,9 +17962,12 @@
       <c r="AH72" s="10">
         <v>30</v>
       </c>
+      <c r="AI72" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -17764,9 +18067,12 @@
       <c r="AH73" s="10">
         <v>11</v>
       </c>
+      <c r="AI73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -17866,9 +18172,12 @@
       <c r="AH74" s="10">
         <v>1</v>
       </c>
+      <c r="AI74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -17968,9 +18277,12 @@
       <c r="AH75" s="10">
         <v>1</v>
       </c>
+      <c r="AI75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -18072,9 +18384,12 @@
       <c r="AH76" s="10">
         <v>1</v>
       </c>
+      <c r="AI76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -18174,9 +18489,12 @@
       <c r="AH77" s="10">
         <v>4</v>
       </c>
+      <c r="AI77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -18276,9 +18594,12 @@
       <c r="AH78" s="10">
         <v>50</v>
       </c>
+      <c r="AI78" s="10">
+        <v>50</v>
+      </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -18378,9 +18699,12 @@
       <c r="AH79" s="10">
         <v>9</v>
       </c>
+      <c r="AI79" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -18480,8 +18804,11 @@
       <c r="AH80" s="10">
         <v>2</v>
       </c>
+      <c r="AI80" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -18584,9 +18911,12 @@
       <c r="AH81" s="10">
         <v>136</v>
       </c>
+      <c r="AI81" s="10">
+        <v>141</v>
+      </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -18688,9 +19018,12 @@
       <c r="AH82" s="10">
         <v>149</v>
       </c>
+      <c r="AI82" s="10">
+        <v>150</v>
+      </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -18790,9 +19123,12 @@
       <c r="AH83" s="10">
         <v>43</v>
       </c>
+      <c r="AI83" s="10">
+        <v>43</v>
+      </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -18892,9 +19228,12 @@
       <c r="AH84" s="10">
         <v>105</v>
       </c>
+      <c r="AI84" s="10">
+        <v>107</v>
+      </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -18994,9 +19333,12 @@
       <c r="AH85" s="10">
         <v>6</v>
       </c>
+      <c r="AI85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -19096,9 +19438,12 @@
       <c r="AH86" s="10">
         <v>14</v>
       </c>
+      <c r="AI86" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A87" s="30" t="s">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -19200,9 +19545,12 @@
       <c r="AH87" s="10">
         <v>15</v>
       </c>
+      <c r="AI87" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -19302,9 +19650,12 @@
       <c r="AH88" s="10">
         <v>31</v>
       </c>
+      <c r="AI88" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -19404,9 +19755,12 @@
       <c r="AH89" s="10">
         <v>8</v>
       </c>
+      <c r="AI89" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -19506,9 +19860,12 @@
       <c r="AH90" s="10">
         <v>10</v>
       </c>
+      <c r="AI90" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -19608,9 +19965,12 @@
       <c r="AH91" s="10">
         <v>3</v>
       </c>
+      <c r="AI91" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A92" s="31"/>
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -19710,9 +20070,12 @@
       <c r="AH92" s="10">
         <v>8</v>
       </c>
+      <c r="AI92" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -19812,9 +20175,12 @@
       <c r="AH93" s="10">
         <v>29</v>
       </c>
+      <c r="AI93" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -19916,9 +20282,12 @@
       <c r="AH94" s="10">
         <v>11</v>
       </c>
+      <c r="AI94" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -20018,8 +20387,11 @@
       <c r="AH95" s="10">
         <v>31</v>
       </c>
+      <c r="AI95" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -20122,9 +20494,12 @@
       <c r="AH96" s="10">
         <v>98</v>
       </c>
+      <c r="AI96" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A97" s="33" t="s">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -20226,9 +20601,12 @@
       <c r="AH97" s="10">
         <v>1027</v>
       </c>
+      <c r="AI97" s="10">
+        <v>1110</v>
+      </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -20328,9 +20706,12 @@
       <c r="AH98" s="10">
         <v>127</v>
       </c>
+      <c r="AI98" s="10">
+        <v>137</v>
+      </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A99" s="35"/>
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -20430,9 +20811,12 @@
       <c r="AH99" s="10">
         <v>38</v>
       </c>
+      <c r="AI99" s="10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -20534,9 +20918,12 @@
       <c r="AH100" s="10">
         <v>21</v>
       </c>
+      <c r="AI100" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -20636,9 +21023,12 @@
       <c r="AH101" s="10">
         <v>21</v>
       </c>
+      <c r="AI101" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -20738,9 +21128,12 @@
       <c r="AH102" s="10">
         <v>94</v>
       </c>
+      <c r="AI102" s="10">
+        <v>97</v>
+      </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -20840,9 +21233,12 @@
       <c r="AH103" s="10">
         <v>180</v>
       </c>
+      <c r="AI103" s="10">
+        <v>193</v>
+      </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
+    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -20942,9 +21338,12 @@
       <c r="AH104" s="10">
         <v>20</v>
       </c>
+      <c r="AI104" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
+    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -21046,9 +21445,12 @@
       <c r="AH105" s="10">
         <v>84</v>
       </c>
+      <c r="AI105" s="10">
+        <v>90</v>
+      </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
+    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -21148,9 +21550,12 @@
       <c r="AH106" s="10">
         <v>64</v>
       </c>
+      <c r="AI106" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
+    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -21250,9 +21655,12 @@
       <c r="AH107" s="10">
         <v>14</v>
       </c>
+      <c r="AI107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
+    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -21352,9 +21760,12 @@
       <c r="AH108" s="10">
         <v>22</v>
       </c>
+      <c r="AI108" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -21454,8 +21865,11 @@
       <c r="AH109" s="10">
         <v>1</v>
       </c>
+      <c r="AI109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -21558,8 +21972,11 @@
       <c r="AH110" s="10">
         <v>259</v>
       </c>
+      <c r="AI110" s="10">
+        <v>267</v>
+      </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -21662,9 +22079,12 @@
       <c r="AH111" s="10">
         <v>28</v>
       </c>
+      <c r="AI111" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
+    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -21766,9 +22186,12 @@
       <c r="AH112" s="10">
         <v>13</v>
       </c>
+      <c r="AI112" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+    <row r="113" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -21868,9 +22291,12 @@
       <c r="AH113" s="10">
         <v>13</v>
       </c>
+      <c r="AI113" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A114" s="32"/>
+    <row r="114" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -21970,9 +22396,12 @@
       <c r="AH114" s="10">
         <v>71</v>
       </c>
+      <c r="AI114" s="10">
+        <v>74</v>
+      </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A115" s="33" t="s">
+    <row r="115" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -22074,9 +22503,12 @@
       <c r="AH115" s="10">
         <v>71</v>
       </c>
+      <c r="AI115" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
+    <row r="116" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -22176,9 +22608,12 @@
       <c r="AH116" s="10">
         <v>72</v>
       </c>
+      <c r="AI116" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+    <row r="117" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -22278,9 +22713,12 @@
       <c r="AH117" s="10">
         <v>10</v>
       </c>
+      <c r="AI117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
+    <row r="118" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -22380,9 +22818,12 @@
       <c r="AH118" s="10">
         <v>38</v>
       </c>
+      <c r="AI118" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+    <row r="119" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -22482,9 +22923,12 @@
       <c r="AH119" s="10">
         <v>7</v>
       </c>
+      <c r="AI119" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+    <row r="120" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -22584,9 +23028,12 @@
       <c r="AH120" s="10">
         <v>44</v>
       </c>
+      <c r="AI120" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="s">
+    <row r="121" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -22688,9 +23135,12 @@
       <c r="AH121" s="10">
         <v>3</v>
       </c>
+      <c r="AI121" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
+    <row r="122" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -22790,9 +23240,12 @@
       <c r="AH122" s="10">
         <v>21</v>
       </c>
+      <c r="AI122" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A123" s="31"/>
+    <row r="123" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -22892,9 +23345,12 @@
       <c r="AH123" s="10">
         <v>2</v>
       </c>
+      <c r="AI123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A124" s="31"/>
+    <row r="124" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -22994,9 +23450,12 @@
       <c r="AH124" s="10">
         <v>3</v>
       </c>
+      <c r="AI124" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A125" s="31"/>
+    <row r="125" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -23096,9 +23555,12 @@
       <c r="AH125" s="10">
         <v>1</v>
       </c>
+      <c r="AI125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A126" s="31"/>
+    <row r="126" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -23198,9 +23660,12 @@
       <c r="AH126" s="10">
         <v>3</v>
       </c>
+      <c r="AI126" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A127" s="31"/>
+    <row r="127" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -23300,9 +23765,12 @@
       <c r="AH127" s="10">
         <v>3</v>
       </c>
+      <c r="AI127" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A128" s="31"/>
+    <row r="128" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -23402,9 +23870,12 @@
       <c r="AH128" s="10">
         <v>6</v>
       </c>
+      <c r="AI128" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A129" s="31"/>
+    <row r="129" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -23504,9 +23975,12 @@
       <c r="AH129" s="10">
         <v>66</v>
       </c>
+      <c r="AI129" s="10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+    <row r="130" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -23606,8 +24080,11 @@
       <c r="AH130" s="10">
         <v>14</v>
       </c>
+      <c r="AI130" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="131" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -23710,9 +24187,12 @@
       <c r="AH131" s="10">
         <v>328</v>
       </c>
+      <c r="AI131" s="10">
+        <v>331</v>
+      </c>
     </row>
-    <row r="132" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="s">
+    <row r="132" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -23814,9 +24294,12 @@
       <c r="AH132" s="10">
         <v>17</v>
       </c>
+      <c r="AI132" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="133" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A133" s="31"/>
+    <row r="133" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -23916,9 +24399,12 @@
       <c r="AH133" s="10">
         <v>10</v>
       </c>
+      <c r="AI133" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A134" s="31"/>
+    <row r="134" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -24018,9 +24504,12 @@
       <c r="AH134" s="10">
         <v>1</v>
       </c>
+      <c r="AI134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A135" s="32"/>
+    <row r="135" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -24120,9 +24609,12 @@
       <c r="AH135" s="10">
         <v>0</v>
       </c>
+      <c r="AI135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="s">
+    <row r="136" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -24224,9 +24716,12 @@
       <c r="AH136" s="10">
         <v>91</v>
       </c>
+      <c r="AI136" s="10">
+        <v>91</v>
+      </c>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
+    <row r="137" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -24326,9 +24821,12 @@
       <c r="AH137" s="10">
         <v>71</v>
       </c>
+      <c r="AI137" s="10">
+        <v>75</v>
+      </c>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+    <row r="138" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -24428,9 +24926,12 @@
       <c r="AH138" s="10">
         <v>15</v>
       </c>
+      <c r="AI138" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A139" s="35"/>
+    <row r="139" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -24529,10 +25030,25 @@
       </c>
       <c r="AH139" s="10">
         <v>136</v>
+      </c>
+      <c r="AI139" s="10">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -24545,18 +25061,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -24848,7 +25352,7 @@
       </c>
       <c r="AQ2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>27.694859038142621</v>
       </c>
       <c r="AR2" s="18">
         <f t="shared" si="1"/>
@@ -25498,7 +26002,7 @@
       </c>
       <c r="AQ4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3832335329341312</v>
       </c>
       <c r="AR4" s="10">
         <f t="shared" si="7"/>
@@ -25823,7 +26327,7 @@
       </c>
       <c r="AQ6" s="12">
         <f>MAX(0, (dc!AQ2-dc!AP2))</f>
-        <v>0</v>
+        <v>603</v>
       </c>
       <c r="AR6" s="12">
         <f>MAX(0, (dc!AR2-dc!AQ2))</f>
@@ -26147,7 +26651,7 @@
       </c>
       <c r="AQ7" s="12">
         <f>MAX(0, (dc!AQ3-dc!AP3))</f>
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="AR7" s="12">
         <f>MAX(0, (dc!AR3-dc!AQ3))</f>
@@ -26795,7 +27299,7 @@
       </c>
       <c r="AQ9" s="12">
         <f>MAX(0, (dc!AQ5-dc!AP5))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AR9" s="12">
         <f>MAX(0, (dc!AR5-dc!AQ5))</f>
@@ -27347,7 +27851,7 @@
       </c>
       <c r="AQ11" s="10">
         <f>MAX(0,(dc!AQ7-dc!AP7))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AR11" s="10">
         <f>MAX(0,(dc!AR7-dc!AQ7))</f>
@@ -27961,7 +28465,7 @@
       </c>
       <c r="AQ13" s="10">
         <f>MAX(0,(dc!AQ9-dc!AP9))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AR13" s="10">
         <f>MAX(0,(dc!AR9-dc!AQ9))</f>
@@ -28268,7 +28772,7 @@
       </c>
       <c r="AQ14" s="10">
         <f>MAX(0,(dc!AQ10-dc!AP10))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AR14" s="10">
         <f>MAX(0,(dc!AR10-dc!AQ10))</f>
@@ -28575,7 +29079,7 @@
       </c>
       <c r="AQ15" s="10">
         <f>MAX(0,(dc!AQ11-dc!AP11))</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AR15" s="10">
         <f>MAX(0,(dc!AR11-dc!AQ11))</f>
@@ -28882,7 +29386,7 @@
       </c>
       <c r="AQ16" s="10">
         <f>MAX(0,(dc!AQ12-dc!AP12))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR16" s="10">
         <f>MAX(0,(dc!AR12-dc!AQ12))</f>
@@ -29189,7 +29693,7 @@
       </c>
       <c r="AQ17" s="10">
         <f>MAX(0,(dc!AQ13-dc!AP13))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AR17" s="10">
         <f>MAX(0,(dc!AR13-dc!AQ13))</f>
@@ -29496,7 +30000,7 @@
       </c>
       <c r="AQ18" s="10">
         <f>MAX(0,(dc!AQ14-dc!AP14))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AR18" s="10">
         <f>MAX(0,(dc!AR14-dc!AQ14))</f>
@@ -29803,7 +30307,7 @@
       </c>
       <c r="AQ19" s="10">
         <f>MAX(0,(dc!AQ15-dc!AP15))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AR19" s="10">
         <f>MAX(0,(dc!AR15-dc!AQ15))</f>
@@ -30197,7 +30701,7 @@
       </c>
       <c r="AF2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19.042461005199307</v>
       </c>
       <c r="AG2" s="20">
         <f t="shared" si="0"/>
@@ -30470,7 +30974,7 @@
       </c>
       <c r="AF3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16.040955631399317</v>
       </c>
       <c r="AG3" s="20">
         <f t="shared" si="2"/>
@@ -30743,7 +31247,7 @@
       </c>
       <c r="AF4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.8919226393629129</v>
       </c>
       <c r="AG4" s="20">
         <f t="shared" si="4"/>
@@ -31079,7 +31583,7 @@
       </c>
       <c r="AF6" s="14">
         <f>MAX(0,(md!AF2-md!AE2)+(md!AF3-md!AE3))</f>
-        <v>0</v>
+        <v>4616</v>
       </c>
       <c r="AG6" s="14">
         <f>MAX(0,(md!AG2-md!AF2)+(md!AG3-md!AF3))</f>
@@ -31351,7 +31855,7 @@
       </c>
       <c r="AF7" s="14">
         <f>MAX(0,(md!AF3-md!AE3))</f>
-        <v>0</v>
+        <v>879</v>
       </c>
       <c r="AG7" s="14">
         <f>MAX(0,(md!AG3-md!AF3))</f>
@@ -31623,7 +32127,7 @@
       </c>
       <c r="AF8" s="14">
         <f>MAX(0,(md!AF4-md!AE4))</f>
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="AG8" s="14">
         <f>MAX(0,(md!AG4-md!AF4))</f>
@@ -31895,7 +32399,7 @@
       </c>
       <c r="AF9" s="14">
         <f>MAX(0,(md!AF5-md!AE5))</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AG9" s="14">
         <f>MAX(0,(md!AG5-md!AF5))</f>
@@ -32381,7 +32885,7 @@
       </c>
       <c r="AF11" s="14">
         <f>MAX(0,(md!AF7-md!AE7))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AG11" s="14">
         <f>MAX(0,(md!AG7-md!AF7))</f>
@@ -32658,7 +33162,7 @@
       </c>
       <c r="AF12" s="14">
         <f>MAX(0,(md!AF9-md!AE9))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AG12" s="14">
         <f>MAX(0,(md!AG9-md!AF9))</f>
@@ -32935,7 +33439,7 @@
       </c>
       <c r="AF13" s="14">
         <f>MAX(0,(md!AF9-md!AE9))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AG13" s="14">
         <f>MAX(0,(md!AG9-md!AF9))</f>
@@ -33212,7 +33716,7 @@
       </c>
       <c r="AF14" s="14">
         <f>MAX(0,(md!AF10-md!AE10))</f>
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="AG14" s="14">
         <f>MAX(0,(md!AG10-md!AF10))</f>
@@ -33489,7 +33993,7 @@
       </c>
       <c r="AF15" s="14">
         <f>MAX(0,(md!AF11-md!AE11))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG15" s="14">
         <f>MAX(0,(md!AG11-md!AF11))</f>
@@ -33766,7 +34270,7 @@
       </c>
       <c r="AF16" s="14">
         <f>MAX(0,(md!AF12-md!AE12))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG16" s="14">
         <f>MAX(0,(md!AG12-md!AF12))</f>
@@ -34043,7 +34547,7 @@
       </c>
       <c r="AF17" s="14">
         <f>MAX(0,(md!AF13-md!AE13))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AG17" s="14">
         <f>MAX(0,(md!AG13-md!AF13))</f>
@@ -34320,7 +34824,7 @@
       </c>
       <c r="AF18" s="14">
         <f>MAX(0,(md!AF14-md!AE14))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG18" s="14">
         <f>MAX(0,(md!AG14-md!AF14))</f>
@@ -34597,7 +35101,7 @@
       </c>
       <c r="AF19" s="14">
         <f>MAX(0,(md!AF15-md!AE15))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AG19" s="14">
         <f>MAX(0,(md!AG15-md!AF15))</f>
@@ -34874,7 +35378,7 @@
       </c>
       <c r="AF20" s="14">
         <f>MAX(0,(md!AF16-md!AE16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG20" s="14">
         <f>MAX(0,(md!AG16-md!AF16))</f>
@@ -35151,7 +35655,7 @@
       </c>
       <c r="AF21" s="14">
         <f>MAX(0,(md!AF17-md!AE17))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AG21" s="14">
         <f>MAX(0,(md!AG17-md!AF17))</f>
@@ -35705,7 +36209,7 @@
       </c>
       <c r="AF23" s="14">
         <f>MAX(0,(md!AF19-md!AE19))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AG23" s="14">
         <f>MAX(0,(md!AG19-md!AF19))</f>
@@ -35982,7 +36486,7 @@
       </c>
       <c r="AF24" s="14">
         <f>MAX(0,(md!AF20-md!AE20))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AG24" s="14">
         <f>MAX(0,(md!AG20-md!AF20))</f>
@@ -36259,7 +36763,7 @@
       </c>
       <c r="AF25" s="14">
         <f>MAX(0,(md!AF21-md!AE21))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG25" s="14">
         <f>MAX(0,(md!AG21-md!AF21))</f>
@@ -36536,7 +37040,7 @@
       </c>
       <c r="AF26" s="14">
         <f>MAX(0,(md!AF22-md!AE22))</f>
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="AG26" s="14">
         <f>MAX(0,(md!AG22-md!AF22))</f>
@@ -36813,7 +37317,7 @@
       </c>
       <c r="AF27" s="14">
         <f>MAX(0,(md!AF23-md!AE23))</f>
-        <v>0</v>
+        <v>262</v>
       </c>
       <c r="AG27" s="14">
         <f>MAX(0,(md!AG23-md!AF23))</f>
@@ -37090,7 +37594,7 @@
       </c>
       <c r="AF28" s="14">
         <f>MAX(0,(md!AF24-md!AE24))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG28" s="14">
         <f>MAX(0,(md!AG24-md!AF24))</f>
@@ -37367,7 +37871,7 @@
       </c>
       <c r="AF29" s="14">
         <f>MAX(0,(md!AF25-md!AE25))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG29" s="14">
         <f>MAX(0,(md!AG25-md!AF25))</f>
@@ -37644,7 +38148,7 @@
       </c>
       <c r="AF30" s="14">
         <f>MAX(0,(md!AF26-md!AE26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG30" s="14">
         <f>MAX(0,(md!AG26-md!AF26))</f>
@@ -38198,7 +38702,7 @@
       </c>
       <c r="AF32" s="14">
         <f>MAX(0,(md!AF28-md!AE28))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG32" s="14">
         <f>MAX(0,(md!AG28-md!AF28))</f>
@@ -38475,7 +38979,7 @@
       </c>
       <c r="AF33" s="14">
         <f>MAX(0,(md!AF29-md!AE29))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AG33" s="14">
         <f>MAX(0,(md!AG29-md!AF29))</f>
@@ -38752,7 +39256,7 @@
       </c>
       <c r="AF34" s="14">
         <f>MAX(0,(md!AF30-md!AE30))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG34" s="14">
         <f>MAX(0,(md!AG30-md!AF30))</f>
@@ -39231,7 +39735,7 @@
       </c>
       <c r="AH2" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.253279964420726</v>
       </c>
       <c r="AI2" s="19">
         <f t="shared" si="0"/>
@@ -39508,7 +40012,7 @@
       </c>
       <c r="AH3" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14.093959731543624</v>
       </c>
       <c r="AI3" s="19">
         <f t="shared" si="2"/>
@@ -39785,7 +40289,7 @@
       </c>
       <c r="AH4" s="19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.375838926174497</v>
       </c>
       <c r="AI4" s="19">
         <f t="shared" si="4"/>
@@ -40062,7 +40566,7 @@
       </c>
       <c r="AH6" s="14">
         <f>MAX(0,(va!AI5-va!AH5))</f>
-        <v>0</v>
+        <v>4497</v>
       </c>
       <c r="AI6" s="14">
         <f>MAX(0,(va!AJ5-va!AI5))</f>
@@ -40339,7 +40843,7 @@
       </c>
       <c r="AH7" s="14">
         <f>MAX(0,(va!AI2-va!AH2))</f>
-        <v>0</v>
+        <v>596</v>
       </c>
       <c r="AI7" s="14">
         <f>MAX(0,(va!AJ2-va!AI2))</f>
@@ -40616,7 +41120,7 @@
       </c>
       <c r="AH8" s="14">
         <f>MAX(0,(va!AI3-va!AH3))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="AI8" s="14">
         <f>MAX(0,(va!AJ3-va!AI3))</f>
@@ -40893,7 +41397,7 @@
       </c>
       <c r="AH9" s="14">
         <f>MAX(0,(va!AI4-va!AH4))</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AI9" s="14">
         <f>MAX(0,(va!AJ4-va!AI4))</f>
@@ -41390,7 +41894,7 @@
       </c>
       <c r="AH11" s="16">
         <f>MAX(0,(va!AI7-va!AH7))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AI11" s="16">
         <f>MAX(0,(va!AJ7-va!AI7))</f>
@@ -41954,7 +42458,7 @@
       </c>
       <c r="AH13" s="16">
         <f>MAX(0,(va!AI9-va!AH9))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" s="16">
         <f>MAX(0,(va!AJ9-va!AI9))</f>
@@ -42518,7 +43022,7 @@
       </c>
       <c r="AH15" s="16">
         <f>MAX(0,(va!AI11-va!AH11))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI15" s="16">
         <f>MAX(0,(va!AJ11-va!AI11))</f>
@@ -43364,7 +43868,7 @@
       </c>
       <c r="AH18" s="16">
         <f>MAX(0,(va!AI14-va!AH14))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AI18" s="16">
         <f>MAX(0,(va!AJ14-va!AI14))</f>
@@ -43646,7 +44150,7 @@
       </c>
       <c r="AH19" s="16">
         <f>MAX(0,(va!AI15-va!AH15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI19" s="16">
         <f>MAX(0,(va!AJ15-va!AI15))</f>
@@ -44774,7 +45278,7 @@
       </c>
       <c r="AH23" s="16">
         <f>MAX(0,(va!AI19-va!AH19))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AI23" s="16">
         <f>MAX(0,(va!AJ19-va!AI19))</f>
@@ -45338,7 +45842,7 @@
       </c>
       <c r="AH25" s="16">
         <f>MAX(0,(va!AI21-va!AH21))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AI25" s="16">
         <f>MAX(0,(va!AJ21-va!AI21))</f>
@@ -46184,7 +46688,7 @@
       </c>
       <c r="AH28" s="16">
         <f>MAX(0,(va!AI24-va!AH24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI28" s="16">
         <f>MAX(0,(va!AJ24-va!AI24))</f>
@@ -47030,7 +47534,7 @@
       </c>
       <c r="AH31" s="16">
         <f>MAX(0,(va!AI27-va!AH27))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI31" s="16">
         <f>MAX(0,(va!AJ27-va!AI27))</f>
@@ -47594,7 +48098,7 @@
       </c>
       <c r="AH33" s="16">
         <f>MAX(0,(va!AI29-va!AH29))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI33" s="16">
         <f>MAX(0,(va!AJ29-va!AI29))</f>
@@ -47876,7 +48380,7 @@
       </c>
       <c r="AH34" s="16">
         <f>MAX(0,(va!AI30-va!AH30))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AI34" s="16">
         <f>MAX(0,(va!AJ30-va!AI30))</f>
@@ -48158,7 +48662,7 @@
       </c>
       <c r="AH35" s="16">
         <f>MAX(0,(va!AI31-va!AH31))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AI35" s="16">
         <f>MAX(0,(va!AJ31-va!AI31))</f>
@@ -49286,7 +49790,7 @@
       </c>
       <c r="AH39" s="16">
         <f>MAX(0,(va!AI35-va!AH35))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AI39" s="16">
         <f>MAX(0,(va!AJ35-va!AI35))</f>
@@ -49568,7 +50072,7 @@
       </c>
       <c r="AH40" s="16">
         <f>MAX(0,(va!AI36-va!AH36))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI40" s="16">
         <f>MAX(0,(va!AJ36-va!AI36))</f>
@@ -51260,7 +51764,7 @@
       </c>
       <c r="AH46" s="16">
         <f>MAX(0,(va!AI42-va!AH42))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI46" s="16">
         <f>MAX(0,(va!AJ42-va!AI42))</f>
@@ -53516,7 +54020,7 @@
       </c>
       <c r="AH54" s="16">
         <f>MAX(0,(va!AI50-va!AH50))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AI54" s="16">
         <f>MAX(0,(va!AJ50-va!AI50))</f>
@@ -53798,7 +54302,7 @@
       </c>
       <c r="AH55" s="16">
         <f>MAX(0,(va!AI51-va!AH51))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI55" s="16">
         <f>MAX(0,(va!AJ51-va!AI51))</f>
@@ -54080,7 +54584,7 @@
       </c>
       <c r="AH56" s="16">
         <f>MAX(0,(va!AI52-va!AH52))</f>
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="AI56" s="16">
         <f>MAX(0,(va!AJ52-va!AI52))</f>
@@ -55208,7 +55712,7 @@
       </c>
       <c r="AH60" s="16">
         <f>MAX(0,(va!AI56-va!AH56))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AI60" s="16">
         <f>MAX(0,(va!AJ56-va!AI56))</f>
@@ -55490,7 +55994,7 @@
       </c>
       <c r="AH61" s="16">
         <f>MAX(0,(va!AI57-va!AH57))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI61" s="16">
         <f>MAX(0,(va!AJ57-va!AI57))</f>
@@ -57182,7 +57686,7 @@
       </c>
       <c r="AH67" s="16">
         <f>MAX(0,(va!AI63-va!AH63))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI67" s="16">
         <f>MAX(0,(va!AJ63-va!AI63))</f>
@@ -57464,7 +57968,7 @@
       </c>
       <c r="AH68" s="16">
         <f>MAX(0,(va!AI64-va!AH64))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI68" s="16">
         <f>MAX(0,(va!AJ64-va!AI64))</f>
@@ -57746,7 +58250,7 @@
       </c>
       <c r="AH69" s="16">
         <f>MAX(0,(va!AI65-va!AH65))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AI69" s="16">
         <f>MAX(0,(va!AJ65-va!AI65))</f>
@@ -58028,7 +58532,7 @@
       </c>
       <c r="AH70" s="16">
         <f>MAX(0,(va!AI66-va!AH66))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI70" s="16">
         <f>MAX(0,(va!AJ66-va!AI66))</f>
@@ -58310,7 +58814,7 @@
       </c>
       <c r="AH71" s="16">
         <f>MAX(0,(va!AI67-va!AH67))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AI71" s="16">
         <f>MAX(0,(va!AJ67-va!AI67))</f>
@@ -61694,7 +62198,7 @@
       </c>
       <c r="AH83" s="16">
         <f>MAX(0,(va!AI79-va!AH79))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI83" s="16">
         <f>MAX(0,(va!AJ79-va!AI79))</f>
@@ -62258,7 +62762,7 @@
       </c>
       <c r="AH85" s="16">
         <f>MAX(0,(va!AI81-va!AH81))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI85" s="16">
         <f>MAX(0,(va!AJ81-va!AI81))</f>
@@ -62540,7 +63044,7 @@
       </c>
       <c r="AH86" s="16">
         <f>MAX(0,(va!AI82-va!AH82))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI86" s="16">
         <f>MAX(0,(va!AJ82-va!AI82))</f>
@@ -63104,7 +63608,7 @@
       </c>
       <c r="AH88" s="16">
         <f>MAX(0,(va!AI84-va!AH84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI88" s="16">
         <f>MAX(0,(va!AJ84-va!AI84))</f>
@@ -65360,7 +65864,7 @@
       </c>
       <c r="AH96" s="16">
         <f>MAX(0,(va!AI92-va!AH92))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI96" s="16">
         <f>MAX(0,(va!AJ92-va!AI92))</f>
@@ -65642,7 +66146,7 @@
       </c>
       <c r="AH97" s="16">
         <f>MAX(0,(va!AI93-va!AH93))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI97" s="16">
         <f>MAX(0,(va!AJ93-va!AI93))</f>
@@ -66488,7 +66992,7 @@
       </c>
       <c r="AH100" s="16">
         <f>MAX(0,(va!AI96-va!AH96))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI100" s="16">
         <f>MAX(0,(va!AJ96-va!AI96))</f>
@@ -66770,7 +67274,7 @@
       </c>
       <c r="AH101" s="16">
         <f>MAX(0,(va!AI97-va!AH97))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="AI101" s="16">
         <f>MAX(0,(va!AJ97-va!AI97))</f>
@@ -67052,7 +67556,7 @@
       </c>
       <c r="AH102" s="16">
         <f>MAX(0,(va!AI98-va!AH98))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AI102" s="16">
         <f>MAX(0,(va!AJ98-va!AI98))</f>
@@ -67334,7 +67838,7 @@
       </c>
       <c r="AH103" s="16">
         <f>MAX(0,(va!AI99-va!AH99))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AI103" s="16">
         <f>MAX(0,(va!AJ99-va!AI99))</f>
@@ -67898,7 +68402,7 @@
       </c>
       <c r="AH105" s="16">
         <f>MAX(0,(va!AI101-va!AH101))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI105" s="16">
         <f>MAX(0,(va!AJ101-va!AI101))</f>
@@ -68180,7 +68684,7 @@
       </c>
       <c r="AH106" s="16">
         <f>MAX(0,(va!AI102-va!AH102))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI106" s="16">
         <f>MAX(0,(va!AJ102-va!AI102))</f>
@@ -68462,7 +68966,7 @@
       </c>
       <c r="AH107" s="16">
         <f>MAX(0,(va!AI103-va!AH103))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AI107" s="16">
         <f>MAX(0,(va!AJ103-va!AI103))</f>
@@ -68744,7 +69248,7 @@
       </c>
       <c r="AH108" s="16">
         <f>MAX(0,(va!AI104-va!AH104))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI108" s="16">
         <f>MAX(0,(va!AJ104-va!AI104))</f>
@@ -69026,7 +69530,7 @@
       </c>
       <c r="AH109" s="16">
         <f>MAX(0,(va!AI105-va!AH105))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AI109" s="16">
         <f>MAX(0,(va!AJ105-va!AI105))</f>
@@ -69308,7 +69812,7 @@
       </c>
       <c r="AH110" s="16">
         <f>MAX(0,(va!AI106-va!AH106))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AI110" s="16">
         <f>MAX(0,(va!AJ106-va!AI106))</f>
@@ -70436,7 +70940,7 @@
       </c>
       <c r="AH114" s="16">
         <f>MAX(0,(va!AI110-va!AH110))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI114" s="16">
         <f>MAX(0,(va!AJ110-va!AI110))</f>
@@ -70718,7 +71222,7 @@
       </c>
       <c r="AH115" s="16">
         <f>MAX(0,(va!AI111-va!AH111))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI115" s="16">
         <f>MAX(0,(va!AJ111-va!AI111))</f>
@@ -71000,7 +71504,7 @@
       </c>
       <c r="AH116" s="16">
         <f>MAX(0,(va!AI112-va!AH112))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI116" s="16">
         <f>MAX(0,(va!AJ112-va!AI112))</f>
@@ -71282,7 +71786,7 @@
       </c>
       <c r="AH117" s="16">
         <f>MAX(0,(va!AI113-va!AH113))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI117" s="16">
         <f>MAX(0,(va!AJ113-va!AI113))</f>
@@ -71564,7 +72068,7 @@
       </c>
       <c r="AH118" s="16">
         <f>MAX(0,(va!AI114-va!AH114))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI118" s="16">
         <f>MAX(0,(va!AJ114-va!AI114))</f>
@@ -71846,7 +72350,7 @@
       </c>
       <c r="AH119" s="16">
         <f>MAX(0,(va!AI115-va!AH115))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI119" s="16">
         <f>MAX(0,(va!AJ115-va!AI115))</f>
@@ -73256,7 +73760,7 @@
       </c>
       <c r="AH124" s="16">
         <f>MAX(0,(va!AI120-va!AH120))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI124" s="16">
         <f>MAX(0,(va!AJ120-va!AI120))</f>
@@ -76358,7 +76862,7 @@
       </c>
       <c r="AH135" s="16">
         <f>MAX(0,(va!AI131-va!AH131))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI135" s="16">
         <f>MAX(0,(va!AJ131-va!AI131))</f>
@@ -76640,7 +77144,7 @@
       </c>
       <c r="AH136" s="16">
         <f>MAX(0,(va!AI132-va!AH132))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI136" s="16">
         <f>MAX(0,(va!AJ132-va!AI132))</f>
@@ -76922,7 +77426,7 @@
       </c>
       <c r="AH137" s="16">
         <f>MAX(0,(va!AI133-va!AH133))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI137" s="16">
         <f>MAX(0,(va!AJ133-va!AI133))</f>
@@ -77204,7 +77708,7 @@
       </c>
       <c r="AH138" s="16">
         <f>MAX(0,(va!AI134-va!AH134))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI138" s="16">
         <f>MAX(0,(va!AJ134-va!AI134))</f>
@@ -78050,7 +78554,7 @@
       </c>
       <c r="AH141" s="16">
         <f>MAX(0,(va!AI137-va!AH137))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI141" s="16">
         <f>MAX(0,(va!AJ137-va!AI137))</f>
@@ -78614,7 +79118,7 @@
       </c>
       <c r="AH143" s="16">
         <f>MAX(0,(va!AI139-va!AH139))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI143" s="16">
         <f>MAX(0,(va!AJ139-va!AI139))</f>

</xml_diff>

<commit_message>
25 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB1B1C6-D996-4575-BD5B-D7CA0B8255CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1831BD83-602B-4498-B9E7-90E418366668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2999,6 +2999,10 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6A2AD35F-60C9-437C-AA7B-C217E8DC7927}" name="va" displayName="va" ref="B6:BT140" totalsRowShown="0">
+  <autoFilter ref="B6:BT140" xr:uid="{CC6A9FB3-0DF8-4FF3-B6B0-EFF5822E8885}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:BT140">
+    <sortCondition ref="C6:C140"/>
+  </sortState>
   <tableColumns count="71">
     <tableColumn id="54" xr3:uid="{F1106E80-B529-4637-9194-7C9771A7B601}" name="Locality" dataDxfId="157"/>
     <tableColumn id="1" xr3:uid="{179FB13D-5548-4710-AF18-46935F888BFD}" name="idx" dataDxfId="156"/>
@@ -4018,7 +4022,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
+      <selection pane="bottomRight" activeCell="AR2" sqref="AR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4164,6 +4168,9 @@
       <c r="AQ2" s="12">
         <v>16533</v>
       </c>
+      <c r="AR2" s="12">
+        <v>17302</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4324,7 +4331,7 @@
       </c>
       <c r="AR3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3699</v>
       </c>
       <c r="AS3" s="10">
         <f t="shared" si="0"/>
@@ -4610,6 +4617,9 @@
       <c r="AQ5" s="10">
         <v>153</v>
       </c>
+      <c r="AR5" s="10">
+        <v>165</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -4986,6 +4996,9 @@
       <c r="AQ7" s="10">
         <v>403</v>
       </c>
+      <c r="AR7" s="10">
+        <v>427</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5117,6 +5130,9 @@
       <c r="AQ8" s="10">
         <v>251</v>
       </c>
+      <c r="AR8" s="10">
+        <v>256</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5248,6 +5264,9 @@
       <c r="AQ9" s="10">
         <v>252</v>
       </c>
+      <c r="AR9" s="10">
+        <v>258</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5379,6 +5398,9 @@
       <c r="AQ10" s="10">
         <v>595</v>
       </c>
+      <c r="AR10" s="10">
+        <v>636</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5510,6 +5532,9 @@
       <c r="AQ11" s="10">
         <v>488</v>
       </c>
+      <c r="AR11" s="10">
+        <v>513</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5641,6 +5666,9 @@
       <c r="AQ12" s="10">
         <v>409</v>
       </c>
+      <c r="AR12" s="10">
+        <v>414</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5772,6 +5800,9 @@
       <c r="AQ13" s="10">
         <v>522</v>
       </c>
+      <c r="AR13" s="10">
+        <v>543</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -5903,6 +5934,9 @@
       <c r="AQ14" s="10">
         <v>498</v>
       </c>
+      <c r="AR14" s="10">
+        <v>518</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6033,6 +6067,9 @@
       </c>
       <c r="AQ15" s="10">
         <v>110</v>
+      </c>
+      <c r="AR15" s="10">
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6287,7 +6324,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AF2" sqref="AF2"/>
+      <selection pane="bottomRight" activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6401,7 +6438,7 @@
         <v>68100</v>
       </c>
       <c r="AG2" s="10">
-        <v>0</v>
+        <v>71357</v>
       </c>
       <c r="AH2" s="10">
         <v>0</v>
@@ -6637,7 +6674,7 @@
       </c>
       <c r="AG3" s="10">
         <f>SUM(md[25-Apr])</f>
-        <v>0</v>
+        <v>17766</v>
       </c>
       <c r="AH3" s="10">
         <f>SUM(md[26-Apr])</f>
@@ -6879,7 +6916,7 @@
         <v>3618</v>
       </c>
       <c r="AG4" s="10">
-        <v>0</v>
+        <v>3760</v>
       </c>
       <c r="AH4" s="10">
         <v>0</v>
@@ -7085,7 +7122,7 @@
         <v>723</v>
       </c>
       <c r="AG5" s="10">
-        <v>0</v>
+        <v>797</v>
       </c>
       <c r="AH5" s="10">
         <v>0</v>
@@ -7502,6 +7539,9 @@
       <c r="AF7">
         <v>90</v>
       </c>
+      <c r="AG7">
+        <v>105</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7600,6 +7640,9 @@
       <c r="AF8" s="10">
         <v>1373</v>
       </c>
+      <c r="AG8" s="10">
+        <v>1430</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7698,6 +7741,9 @@
       <c r="AF9">
         <v>1728</v>
       </c>
+      <c r="AG9">
+        <v>1791</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7796,6 +7842,9 @@
       <c r="AF10">
         <v>2234</v>
       </c>
+      <c r="AG10">
+        <v>2387</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -7894,6 +7943,9 @@
       <c r="AF11">
         <v>125</v>
       </c>
+      <c r="AG11">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -7992,6 +8044,9 @@
       <c r="AF12">
         <v>55</v>
       </c>
+      <c r="AG12">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8090,6 +8145,9 @@
       <c r="AF13">
         <v>372</v>
       </c>
+      <c r="AG13">
+        <v>384</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8188,6 +8246,9 @@
       <c r="AF14">
         <v>144</v>
       </c>
+      <c r="AG14">
+        <v>146</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8286,6 +8347,9 @@
       <c r="AF15">
         <v>459</v>
       </c>
+      <c r="AG15">
+        <v>483</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8384,8 +8448,11 @@
       <c r="AF16" s="10">
         <v>32</v>
       </c>
+      <c r="AG16" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8482,8 +8549,11 @@
       <c r="AF17">
         <v>765</v>
       </c>
+      <c r="AG17">
+        <v>814</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8580,8 +8650,11 @@
       <c r="AF18">
         <v>4</v>
       </c>
+      <c r="AG18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8678,8 +8751,11 @@
       <c r="AF19">
         <v>289</v>
       </c>
+      <c r="AG19">
+        <v>302</v>
+      </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -8776,8 +8852,11 @@
       <c r="AF20">
         <v>642</v>
       </c>
+      <c r="AG20">
+        <v>686</v>
+      </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -8874,8 +8953,11 @@
       <c r="AF21">
         <v>67</v>
       </c>
+      <c r="AG21">
+        <v>67</v>
+      </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -8972,8 +9054,11 @@
       <c r="AF22">
         <v>3227</v>
       </c>
+      <c r="AG22">
+        <v>3483</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9070,8 +9155,11 @@
       <c r="AF23">
         <v>4403</v>
       </c>
+      <c r="AG23">
+        <v>4795</v>
+      </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9168,8 +9256,11 @@
       <c r="AF24">
         <v>43</v>
       </c>
+      <c r="AG24">
+        <v>52</v>
+      </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9266,8 +9357,11 @@
       <c r="AF25">
         <v>119</v>
       </c>
+      <c r="AG25">
+        <v>124</v>
+      </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9364,8 +9458,11 @@
       <c r="AF26">
         <v>13</v>
       </c>
+      <c r="AG26">
+        <v>14</v>
+      </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -9462,8 +9559,11 @@
       <c r="AF27">
         <v>23</v>
       </c>
+      <c r="AG27">
+        <v>28</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -9560,8 +9660,11 @@
       <c r="AF28">
         <v>143</v>
       </c>
+      <c r="AG28">
+        <v>154</v>
+      </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -9658,8 +9761,11 @@
       <c r="AF29">
         <v>222</v>
       </c>
+      <c r="AG29">
+        <v>242</v>
+      </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -9756,8 +9862,11 @@
       <c r="AF30">
         <v>44</v>
       </c>
+      <c r="AG30">
+        <v>46</v>
+      </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -9854,7 +9963,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="Q6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ3" sqref="AJ3"/>
+      <selection pane="bottomRight" activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10008,7 +10117,7 @@
       </c>
       <c r="AJ2" s="10">
         <f>SUM(va[25-Apr])</f>
-        <v>0</v>
+        <v>12366</v>
       </c>
       <c r="AK2" s="10">
         <f>SUM(va[26-Apr])</f>
@@ -10253,7 +10362,7 @@
         <v>1837</v>
       </c>
       <c r="AJ3" s="10">
-        <v>0</v>
+        <v>1942</v>
       </c>
       <c r="AK3" s="10">
         <v>0</v>
@@ -10462,7 +10571,7 @@
         <v>410</v>
       </c>
       <c r="AJ4" s="10">
-        <v>0</v>
+        <v>436</v>
       </c>
       <c r="AK4" s="10">
         <v>0</v>
@@ -10671,7 +10780,7 @@
         <v>69015</v>
       </c>
       <c r="AJ5" s="10">
-        <v>0</v>
+        <v>72178</v>
       </c>
       <c r="AK5" s="10">
         <v>0</v>
@@ -11106,9 +11215,12 @@
       <c r="AI7" s="10">
         <v>547</v>
       </c>
+      <c r="AJ7" s="10">
+        <v>575</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11213,9 +11325,12 @@
       <c r="AI8" s="10">
         <v>5</v>
       </c>
+      <c r="AJ8" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11318,9 +11433,12 @@
       <c r="AI9" s="10">
         <v>27</v>
       </c>
+      <c r="AJ9" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -11423,9 +11541,12 @@
       <c r="AI10" s="10">
         <v>2</v>
       </c>
+      <c r="AJ10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -11528,9 +11649,12 @@
       <c r="AI11" s="10">
         <v>39</v>
       </c>
+      <c r="AJ11" s="10">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -11633,9 +11757,12 @@
       <c r="AI12" s="10">
         <v>1</v>
       </c>
+      <c r="AJ12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -11736,6 +11863,9 @@
         <v>8</v>
       </c>
       <c r="AI13" s="10">
+        <v>8</v>
+      </c>
+      <c r="AJ13" s="10">
         <v>8</v>
       </c>
     </row>
@@ -11845,9 +11975,12 @@
       <c r="AI14" s="10">
         <v>722</v>
       </c>
+      <c r="AJ14" s="10">
+        <v>764</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -11952,9 +12085,12 @@
       <c r="AI15" s="10">
         <v>34</v>
       </c>
+      <c r="AJ15" s="10">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -12057,9 +12193,12 @@
       <c r="AI16" s="10">
         <v>0</v>
       </c>
+      <c r="AJ16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12162,9 +12301,12 @@
       <c r="AI17" s="10">
         <v>1</v>
       </c>
+      <c r="AJ17" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -12267,9 +12409,12 @@
       <c r="AI18" s="10">
         <v>5</v>
       </c>
+      <c r="AJ18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -12372,9 +12517,12 @@
       <c r="AI19" s="10">
         <v>176</v>
       </c>
+      <c r="AJ19" s="10">
+        <v>184</v>
+      </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -12477,9 +12625,12 @@
       <c r="AI20" s="10">
         <v>5</v>
       </c>
+      <c r="AJ20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -12582,9 +12733,12 @@
       <c r="AI21" s="10">
         <v>355</v>
       </c>
+      <c r="AJ21" s="10">
+        <v>370</v>
+      </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -12687,9 +12841,12 @@
       <c r="AI22" s="10">
         <v>3</v>
       </c>
+      <c r="AJ22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -12792,9 +12949,12 @@
       <c r="AI23" s="10">
         <v>10</v>
       </c>
+      <c r="AJ23" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -12897,9 +13057,12 @@
       <c r="AI24" s="10">
         <v>10</v>
       </c>
+      <c r="AJ24" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -13004,9 +13167,12 @@
       <c r="AI25" s="10">
         <v>9</v>
       </c>
+      <c r="AJ25" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -13109,9 +13275,12 @@
       <c r="AI26" s="10">
         <v>12</v>
       </c>
+      <c r="AJ26" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -13214,9 +13383,12 @@
       <c r="AI27" s="10">
         <v>23</v>
       </c>
+      <c r="AJ27" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -13319,9 +13491,12 @@
       <c r="AI28" s="10">
         <v>10</v>
       </c>
+      <c r="AJ28" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -13424,8 +13599,11 @@
       <c r="AI29" s="10">
         <v>48</v>
       </c>
+      <c r="AJ29" s="10">
+        <v>48</v>
+      </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -13531,9 +13709,12 @@
       <c r="AI30" s="10">
         <v>197</v>
       </c>
+      <c r="AJ30" s="10">
+        <v>200</v>
+      </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -13638,9 +13819,12 @@
       <c r="AI31" s="10">
         <v>423</v>
       </c>
+      <c r="AJ31" s="10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -13743,9 +13927,12 @@
       <c r="AI32" s="10">
         <v>9</v>
       </c>
+      <c r="AJ32" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -13848,9 +14035,12 @@
       <c r="AI33" s="10">
         <v>41</v>
       </c>
+      <c r="AJ33" s="10">
+        <v>43</v>
+      </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -13955,9 +14145,12 @@
       <c r="AI34" s="10">
         <v>12</v>
       </c>
+      <c r="AJ34" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -14060,9 +14253,12 @@
       <c r="AI35" s="10">
         <v>69</v>
       </c>
+      <c r="AJ35" s="10">
+        <v>69</v>
+      </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -14165,9 +14361,12 @@
       <c r="AI36" s="10">
         <v>100</v>
       </c>
+      <c r="AJ36" s="10">
+        <v>103</v>
+      </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -14270,9 +14469,12 @@
       <c r="AI37" s="10">
         <v>20</v>
       </c>
+      <c r="AJ37" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -14377,9 +14579,12 @@
       <c r="AI38" s="10">
         <v>12</v>
       </c>
+      <c r="AJ38" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -14482,9 +14687,12 @@
       <c r="AI39" s="10">
         <v>30</v>
       </c>
+      <c r="AJ39" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -14587,9 +14795,12 @@
       <c r="AI40" s="10">
         <v>29</v>
       </c>
+      <c r="AJ40" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -14692,9 +14903,12 @@
       <c r="AI41" s="10">
         <v>4</v>
       </c>
+      <c r="AJ41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -14797,9 +15011,12 @@
       <c r="AI42" s="10">
         <v>28</v>
       </c>
+      <c r="AJ42" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -14902,9 +15119,12 @@
       <c r="AI43" s="10">
         <v>18</v>
       </c>
+      <c r="AJ43" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -15007,9 +15227,12 @@
       <c r="AI44" s="10">
         <v>19</v>
       </c>
+      <c r="AJ44" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -15112,9 +15335,12 @@
       <c r="AI45" s="10">
         <v>27</v>
       </c>
+      <c r="AJ45" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -15219,9 +15445,12 @@
       <c r="AI46" s="10">
         <v>12</v>
       </c>
+      <c r="AJ46" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -15324,9 +15553,12 @@
       <c r="AI47" s="10">
         <v>0</v>
       </c>
+      <c r="AJ47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -15429,9 +15661,12 @@
       <c r="AI48" s="10">
         <v>2</v>
       </c>
+      <c r="AJ48" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -15534,9 +15769,12 @@
       <c r="AI49" s="10">
         <v>4</v>
       </c>
+      <c r="AJ49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -15641,9 +15879,12 @@
       <c r="AI50" s="10">
         <v>100</v>
       </c>
+      <c r="AJ50" s="10">
+        <v>146</v>
+      </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -15746,9 +15987,12 @@
       <c r="AI51" s="10">
         <v>15</v>
       </c>
+      <c r="AJ51" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -15853,9 +16097,12 @@
       <c r="AI52" s="10">
         <v>2534</v>
       </c>
+      <c r="AJ52" s="10">
+        <v>2745</v>
+      </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -15958,9 +16205,12 @@
       <c r="AI53" s="10">
         <v>26</v>
       </c>
+      <c r="AJ53" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A54" s="32"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -16063,8 +16313,11 @@
       <c r="AI54" s="10">
         <v>24</v>
       </c>
+      <c r="AJ54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -16170,8 +16423,11 @@
       <c r="AI55" s="10">
         <v>99</v>
       </c>
+      <c r="AJ55" s="10">
+        <v>101</v>
+      </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -16277,9 +16533,12 @@
       <c r="AI56" s="10">
         <v>729</v>
       </c>
+      <c r="AJ56" s="10">
+        <v>764</v>
+      </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -16384,9 +16643,12 @@
       <c r="AI57" s="10">
         <v>8</v>
       </c>
+      <c r="AJ57" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -16489,9 +16751,12 @@
       <c r="AI58" s="10">
         <v>5</v>
       </c>
+      <c r="AJ58" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -16594,9 +16859,12 @@
       <c r="AI59" s="10">
         <v>20</v>
       </c>
+      <c r="AJ59" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -16699,9 +16967,12 @@
       <c r="AI60" s="10">
         <v>2</v>
       </c>
+      <c r="AJ60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -16806,9 +17077,12 @@
       <c r="AI61" s="10">
         <v>7</v>
       </c>
+      <c r="AJ61" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -16911,9 +17185,12 @@
       <c r="AI62" s="10">
         <v>87</v>
       </c>
+      <c r="AJ62" s="10">
+        <v>93</v>
+      </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -17016,9 +17293,12 @@
       <c r="AI63" s="10">
         <v>30</v>
       </c>
+      <c r="AJ63" s="10">
+        <v>82</v>
+      </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -17121,9 +17401,12 @@
       <c r="AI64" s="10">
         <v>65</v>
       </c>
+      <c r="AJ64" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -17226,9 +17509,12 @@
       <c r="AI65" s="10">
         <v>36</v>
       </c>
+      <c r="AJ65" s="10">
+        <v>42</v>
+      </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A66" s="32"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -17331,8 +17617,11 @@
       <c r="AI66" s="10">
         <v>31</v>
       </c>
+      <c r="AJ66" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -17438,9 +17727,12 @@
       <c r="AI67" s="10">
         <v>529</v>
       </c>
+      <c r="AJ67" s="10">
+        <v>564</v>
+      </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -17545,9 +17837,12 @@
       <c r="AI68" s="10">
         <v>0</v>
       </c>
+      <c r="AJ68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -17650,9 +17945,12 @@
       <c r="AI69" s="10">
         <v>3</v>
       </c>
+      <c r="AJ69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -17755,9 +18053,12 @@
       <c r="AI70" s="10">
         <v>0</v>
       </c>
+      <c r="AJ70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A71" s="31"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -17860,9 +18161,12 @@
       <c r="AI71" s="10">
         <v>13</v>
       </c>
+      <c r="AJ71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A72" s="31"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -17965,9 +18269,12 @@
       <c r="AI72" s="10">
         <v>30</v>
       </c>
+      <c r="AJ72" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A73" s="31"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -18070,9 +18377,12 @@
       <c r="AI73" s="10">
         <v>11</v>
       </c>
+      <c r="AJ73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A74" s="31"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -18175,9 +18485,12 @@
       <c r="AI74" s="10">
         <v>1</v>
       </c>
+      <c r="AJ74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A75" s="32"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -18280,9 +18593,12 @@
       <c r="AI75" s="10">
         <v>1</v>
       </c>
+      <c r="AJ75" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A76" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -18387,9 +18703,12 @@
       <c r="AI76" s="10">
         <v>1</v>
       </c>
+      <c r="AJ76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A77" s="34"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -18492,9 +18811,12 @@
       <c r="AI77" s="10">
         <v>4</v>
       </c>
+      <c r="AJ77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A78" s="34"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -18597,9 +18919,12 @@
       <c r="AI78" s="10">
         <v>50</v>
       </c>
+      <c r="AJ78" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A79" s="34"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -18702,9 +19027,12 @@
       <c r="AI79" s="10">
         <v>10</v>
       </c>
+      <c r="AJ79" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -18807,8 +19135,11 @@
       <c r="AI80" s="10">
         <v>2</v>
       </c>
+      <c r="AJ80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -18914,9 +19245,12 @@
       <c r="AI81" s="10">
         <v>141</v>
       </c>
+      <c r="AJ81" s="10">
+        <v>169</v>
+      </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A82" s="30" t="s">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -19021,9 +19355,12 @@
       <c r="AI82" s="10">
         <v>150</v>
       </c>
+      <c r="AJ82" s="10">
+        <v>151</v>
+      </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A83" s="34"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -19126,9 +19463,12 @@
       <c r="AI83" s="10">
         <v>43</v>
       </c>
+      <c r="AJ83" s="10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A84" s="34"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -19231,9 +19571,12 @@
       <c r="AI84" s="10">
         <v>107</v>
       </c>
+      <c r="AJ84" s="10">
+        <v>109</v>
+      </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A85" s="34"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -19336,9 +19679,12 @@
       <c r="AI85" s="10">
         <v>6</v>
       </c>
+      <c r="AJ85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A86" s="35"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -19441,9 +19787,12 @@
       <c r="AI86" s="10">
         <v>14</v>
       </c>
+      <c r="AJ86" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A87" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -19548,9 +19897,12 @@
       <c r="AI87" s="10">
         <v>15</v>
       </c>
+      <c r="AJ87" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -19653,9 +20005,12 @@
       <c r="AI88" s="10">
         <v>31</v>
       </c>
+      <c r="AJ88" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -19758,9 +20113,12 @@
       <c r="AI89" s="10">
         <v>8</v>
       </c>
+      <c r="AJ89" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
+    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -19863,9 +20221,12 @@
       <c r="AI90" s="10">
         <v>10</v>
       </c>
+      <c r="AJ90" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
+    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -19968,9 +20329,12 @@
       <c r="AI91" s="10">
         <v>3</v>
       </c>
+      <c r="AJ91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
+    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -20073,9 +20437,12 @@
       <c r="AI92" s="10">
         <v>10</v>
       </c>
+      <c r="AJ92" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A93" s="32"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -20178,9 +20545,12 @@
       <c r="AI93" s="10">
         <v>34</v>
       </c>
+      <c r="AJ93" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -20285,9 +20655,12 @@
       <c r="AI94" s="10">
         <v>11</v>
       </c>
+      <c r="AJ94" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A95" s="35"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -20390,8 +20763,11 @@
       <c r="AI95" s="10">
         <v>31</v>
       </c>
+      <c r="AJ95" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -20497,9 +20873,12 @@
       <c r="AI96" s="10">
         <v>100</v>
       </c>
+      <c r="AJ96" s="10">
+        <v>103</v>
+      </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A97" s="33" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -20604,9 +20983,12 @@
       <c r="AI97" s="10">
         <v>1110</v>
       </c>
+      <c r="AJ97" s="10">
+        <v>1184</v>
+      </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A98" s="34"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -20709,9 +21091,12 @@
       <c r="AI98" s="10">
         <v>137</v>
       </c>
+      <c r="AJ98" s="10">
+        <v>154</v>
+      </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
+    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A99" s="35"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -20814,9 +21199,12 @@
       <c r="AI99" s="10">
         <v>44</v>
       </c>
+      <c r="AJ99" s="10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A100" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -20921,9 +21309,12 @@
       <c r="AI100" s="10">
         <v>21</v>
       </c>
+      <c r="AJ100" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -21026,9 +21417,12 @@
       <c r="AI101" s="10">
         <v>23</v>
       </c>
+      <c r="AJ101" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
+    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -21131,9 +21525,12 @@
       <c r="AI102" s="10">
         <v>97</v>
       </c>
+      <c r="AJ102" s="10">
+        <v>101</v>
+      </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
+    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -21236,9 +21633,12 @@
       <c r="AI103" s="10">
         <v>193</v>
       </c>
+      <c r="AJ103" s="10">
+        <v>198</v>
+      </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
+    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A104" s="32"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -21341,9 +21741,12 @@
       <c r="AI104" s="10">
         <v>21</v>
       </c>
+      <c r="AJ104" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A105" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -21448,9 +21851,12 @@
       <c r="AI105" s="10">
         <v>90</v>
       </c>
+      <c r="AJ105" s="10">
+        <v>95</v>
+      </c>
     </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A106" s="34"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -21553,9 +21959,12 @@
       <c r="AI106" s="10">
         <v>73</v>
       </c>
+      <c r="AJ106" s="10">
+        <v>80</v>
+      </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A107" s="34"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -21658,9 +22067,12 @@
       <c r="AI107" s="10">
         <v>14</v>
       </c>
+      <c r="AJ107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A108" s="34"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -21763,9 +22175,12 @@
       <c r="AI108" s="10">
         <v>22</v>
       </c>
+      <c r="AJ108" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A109" s="32"/>
+    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A109" s="35"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -21868,8 +22283,11 @@
       <c r="AI109" s="10">
         <v>1</v>
       </c>
+      <c r="AJ109" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -21975,8 +22393,11 @@
       <c r="AI110" s="10">
         <v>267</v>
       </c>
+      <c r="AJ110" s="10">
+        <v>287</v>
+      </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -22082,9 +22503,12 @@
       <c r="AI111" s="10">
         <v>33</v>
       </c>
+      <c r="AJ111" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A112" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -22189,9 +22613,12 @@
       <c r="AI112" s="10">
         <v>14</v>
       </c>
+      <c r="AJ112" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -22294,9 +22721,12 @@
       <c r="AI113" s="10">
         <v>16</v>
       </c>
+      <c r="AJ113" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A114" s="32"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -22399,9 +22829,12 @@
       <c r="AI114" s="10">
         <v>74</v>
       </c>
+      <c r="AJ114" s="10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A115" s="30" t="s">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A115" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -22506,9 +22939,12 @@
       <c r="AI115" s="10">
         <v>72</v>
       </c>
+      <c r="AJ115" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A116" s="31"/>
+    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A116" s="34"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -22611,9 +23047,12 @@
       <c r="AI116" s="10">
         <v>72</v>
       </c>
+      <c r="AJ116" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="117" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
+    <row r="117" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A117" s="34"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -22716,9 +23155,12 @@
       <c r="AI117" s="10">
         <v>10</v>
       </c>
+      <c r="AJ117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
+    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A118" s="34"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -22821,9 +23263,12 @@
       <c r="AI118" s="10">
         <v>38</v>
       </c>
+      <c r="AJ118" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="119" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
+    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A119" s="34"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -22926,9 +23371,12 @@
       <c r="AI119" s="10">
         <v>7</v>
       </c>
+      <c r="AJ119" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="120" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+    <row r="120" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A120" s="35"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -23031,9 +23479,12 @@
       <c r="AI120" s="10">
         <v>45</v>
       </c>
+      <c r="AJ120" s="10">
+        <v>48</v>
+      </c>
     </row>
-    <row r="121" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A121" s="33" t="s">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A121" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -23138,9 +23589,12 @@
       <c r="AI121" s="10">
         <v>3</v>
       </c>
+      <c r="AJ121" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="122" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
+    <row r="122" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -23243,9 +23697,12 @@
       <c r="AI122" s="10">
         <v>21</v>
       </c>
+      <c r="AJ122" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="123" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+    <row r="123" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -23348,9 +23805,12 @@
       <c r="AI123" s="10">
         <v>2</v>
       </c>
+      <c r="AJ123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -23453,9 +23913,12 @@
       <c r="AI124" s="10">
         <v>3</v>
       </c>
+      <c r="AJ124" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="125" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
+    <row r="125" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -23558,9 +24021,12 @@
       <c r="AI125" s="10">
         <v>1</v>
       </c>
+      <c r="AJ125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+    <row r="126" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -23663,9 +24129,12 @@
       <c r="AI126" s="10">
         <v>3</v>
       </c>
+      <c r="AJ126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+    <row r="127" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -23768,9 +24237,12 @@
       <c r="AI127" s="10">
         <v>3</v>
       </c>
+      <c r="AJ127" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="128" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
+    <row r="128" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -23873,9 +24345,12 @@
       <c r="AI128" s="10">
         <v>6</v>
       </c>
+      <c r="AJ128" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="129" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+    <row r="129" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A129" s="31"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -23978,9 +24453,12 @@
       <c r="AI129" s="10">
         <v>66</v>
       </c>
+      <c r="AJ129" s="10">
+        <v>79</v>
+      </c>
     </row>
-    <row r="130" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+    <row r="130" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A130" s="32"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -24083,8 +24561,11 @@
       <c r="AI130" s="10">
         <v>14</v>
       </c>
+      <c r="AJ130" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="131" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -24190,9 +24671,12 @@
       <c r="AI131" s="10">
         <v>331</v>
       </c>
+      <c r="AJ131" s="10">
+        <v>335</v>
+      </c>
     </row>
-    <row r="132" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A132" s="33" t="s">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A132" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -24297,9 +24781,12 @@
       <c r="AI132" s="10">
         <v>19</v>
       </c>
+      <c r="AJ132" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="133" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+    <row r="133" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A133" s="31"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -24402,9 +24889,12 @@
       <c r="AI133" s="10">
         <v>12</v>
       </c>
+      <c r="AJ133" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="134" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+    <row r="134" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A134" s="31"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -24507,9 +24997,12 @@
       <c r="AI134" s="10">
         <v>2</v>
       </c>
+      <c r="AJ134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A135" s="35"/>
+    <row r="135" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A135" s="32"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -24612,9 +25105,12 @@
       <c r="AI135" s="10">
         <v>0</v>
       </c>
+      <c r="AJ135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A136" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -24719,9 +25215,12 @@
       <c r="AI136" s="10">
         <v>91</v>
       </c>
+      <c r="AJ136" s="10">
+        <v>91</v>
+      </c>
     </row>
-    <row r="137" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
+    <row r="137" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A137" s="34"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -24824,9 +25323,12 @@
       <c r="AI137" s="10">
         <v>75</v>
       </c>
+      <c r="AJ137" s="10">
+        <v>75</v>
+      </c>
     </row>
-    <row r="138" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
+    <row r="138" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A138" s="34"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -24929,9 +25431,12 @@
       <c r="AI138" s="10">
         <v>15</v>
       </c>
+      <c r="AJ138" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="139" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A139" s="32"/>
+    <row r="139" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A139" s="35"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -25033,10 +25538,25 @@
       </c>
       <c r="AI139" s="10">
         <v>138</v>
+      </c>
+      <c r="AJ139" s="10">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -25049,18 +25569,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -25165,7 +25673,10 @@
   <dimension ref="A1:CC19"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25356,7 +25867,7 @@
       </c>
       <c r="AR2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>22.23667100130039</v>
       </c>
       <c r="AS2" s="18">
         <f t="shared" si="1"/>
@@ -26006,7 +26517,7 @@
       </c>
       <c r="AR4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7.0175438596491224</v>
       </c>
       <c r="AS4" s="10">
         <f t="shared" si="7"/>
@@ -26331,7 +26842,7 @@
       </c>
       <c r="AR6" s="12">
         <f>MAX(0, (dc!AR2-dc!AQ2))</f>
-        <v>0</v>
+        <v>769</v>
       </c>
       <c r="AS6" s="12">
         <f>MAX(0, (dc!AS2-dc!AR2))</f>
@@ -26655,7 +27166,7 @@
       </c>
       <c r="AR7" s="12">
         <f>MAX(0, (dc!AR3-dc!AQ3))</f>
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="AS7" s="12">
         <f>MAX(0, (dc!AS3-dc!AR3))</f>
@@ -27303,7 +27814,7 @@
       </c>
       <c r="AR9" s="12">
         <f>MAX(0, (dc!AR5-dc!AQ5))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AS9" s="12">
         <f>MAX(0, (dc!AS5-dc!AR5))</f>
@@ -27855,7 +28366,7 @@
       </c>
       <c r="AR11" s="10">
         <f>MAX(0,(dc!AR7-dc!AQ7))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AS11" s="10">
         <f>MAX(0,(dc!AS7-dc!AR7))</f>
@@ -28162,7 +28673,7 @@
       </c>
       <c r="AR12" s="10">
         <f>MAX(0,(dc!AR8-dc!AQ8))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS12" s="10">
         <f>MAX(0,(dc!AS8-dc!AR8))</f>
@@ -28469,7 +28980,7 @@
       </c>
       <c r="AR13" s="10">
         <f>MAX(0,(dc!AR9-dc!AQ9))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AS13" s="10">
         <f>MAX(0,(dc!AS9-dc!AR9))</f>
@@ -28776,7 +29287,7 @@
       </c>
       <c r="AR14" s="10">
         <f>MAX(0,(dc!AR10-dc!AQ10))</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="AS14" s="10">
         <f>MAX(0,(dc!AS10-dc!AR10))</f>
@@ -29083,7 +29594,7 @@
       </c>
       <c r="AR15" s="10">
         <f>MAX(0,(dc!AR11-dc!AQ11))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AS15" s="10">
         <f>MAX(0,(dc!AS11-dc!AR11))</f>
@@ -29390,7 +29901,7 @@
       </c>
       <c r="AR16" s="10">
         <f>MAX(0,(dc!AR12-dc!AQ12))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS16" s="10">
         <f>MAX(0,(dc!AS12-dc!AR12))</f>
@@ -29697,7 +30208,7 @@
       </c>
       <c r="AR17" s="10">
         <f>MAX(0,(dc!AR13-dc!AQ13))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AS17" s="10">
         <f>MAX(0,(dc!AS13-dc!AR13))</f>
@@ -30004,7 +30515,7 @@
       </c>
       <c r="AR18" s="10">
         <f>MAX(0,(dc!AR14-dc!AQ14))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AS18" s="10">
         <f>MAX(0,(dc!AS14-dc!AR14))</f>
@@ -30311,7 +30822,7 @@
       </c>
       <c r="AR19" s="10">
         <f>MAX(0,(dc!AR15-dc!AQ15))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AS19" s="10">
         <f>MAX(0,(dc!AS15-dc!AR15))</f>
@@ -30566,7 +31077,10 @@
   <dimension ref="A1:BQ70"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30705,7 +31219,7 @@
       </c>
       <c r="AG2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.094849103698657</v>
       </c>
       <c r="AH2" s="20">
         <f t="shared" si="0"/>
@@ -30978,7 +31492,7 @@
       </c>
       <c r="AG3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.347826086956522</v>
       </c>
       <c r="AH3" s="20">
         <f t="shared" si="2"/>
@@ -31251,7 +31765,7 @@
       </c>
       <c r="AG4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.4347826086956523</v>
       </c>
       <c r="AH4" s="20">
         <f t="shared" si="4"/>
@@ -31587,7 +32101,7 @@
       </c>
       <c r="AG6" s="14">
         <f>MAX(0,(md!AG2-md!AF2)+(md!AG3-md!AF3))</f>
-        <v>0</v>
+        <v>4407</v>
       </c>
       <c r="AH6" s="14">
         <f>MAX(0,(md!AH2-md!AG2)+(md!AH3-md!AG3))</f>
@@ -31859,7 +32373,7 @@
       </c>
       <c r="AG7" s="14">
         <f>MAX(0,(md!AG3-md!AF3))</f>
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="AH7" s="14">
         <f>MAX(0,(md!AH3-md!AG3))</f>
@@ -32131,7 +32645,7 @@
       </c>
       <c r="AG8" s="14">
         <f>MAX(0,(md!AG4-md!AF4))</f>
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="AH8" s="14">
         <f>MAX(0,(md!AH4-md!AG4))</f>
@@ -32403,7 +32917,7 @@
       </c>
       <c r="AG9" s="14">
         <f>MAX(0,(md!AG5-md!AF5))</f>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="AH9" s="14">
         <f>MAX(0,(md!AH5-md!AG5))</f>
@@ -32889,7 +33403,7 @@
       </c>
       <c r="AG11" s="14">
         <f>MAX(0,(md!AG7-md!AF7))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AH11" s="14">
         <f>MAX(0,(md!AH7-md!AG7))</f>
@@ -33049,267 +33563,267 @@
         <v>0</v>
       </c>
       <c r="D12" s="14">
-        <f>MAX(0,(md!D9-md!C9))</f>
-        <v>16</v>
+        <f>MAX(0,(md!D8-md!C8))</f>
+        <v>22</v>
       </c>
       <c r="E12" s="14">
-        <f>MAX(0,(md!E9-md!D9))</f>
+        <f>MAX(0,(md!E8-md!D8))</f>
+        <v>25</v>
+      </c>
+      <c r="F12" s="14">
+        <f>MAX(0,(md!F8-md!E8))</f>
+        <v>11</v>
+      </c>
+      <c r="G12" s="14">
+        <f>MAX(0,(md!G8-md!F8))</f>
+        <v>11</v>
+      </c>
+      <c r="H12" s="14">
+        <f>MAX(0,(md!H8-md!G8))</f>
+        <v>17</v>
+      </c>
+      <c r="I12" s="14">
+        <f>MAX(0,(md!I8-md!H8))</f>
+        <v>31</v>
+      </c>
+      <c r="J12" s="14">
+        <f>MAX(0,(md!J8-md!I8))</f>
+        <v>48</v>
+      </c>
+      <c r="K12" s="14">
+        <f>MAX(0,(md!K8-md!J8))</f>
+        <v>43</v>
+      </c>
+      <c r="L12" s="14">
+        <f>MAX(0,(md!L8-md!K8))</f>
+        <v>40</v>
+      </c>
+      <c r="M12" s="14">
+        <f>MAX(0,(md!M8-md!L8))</f>
+        <v>30</v>
+      </c>
+      <c r="N12" s="14">
+        <f>MAX(0,(md!N8-md!M8))</f>
         <v>24</v>
       </c>
-      <c r="F12" s="14">
-        <f>MAX(0,(md!F9-md!E9))</f>
-        <v>17</v>
-      </c>
-      <c r="G12" s="14">
-        <f>MAX(0,(md!G9-md!F9))</f>
-        <v>23</v>
-      </c>
-      <c r="H12" s="14">
-        <f>MAX(0,(md!H9-md!G9))</f>
-        <v>35</v>
-      </c>
-      <c r="I12" s="14">
-        <f>MAX(0,(md!I9-md!H9))</f>
-        <v>34</v>
-      </c>
-      <c r="J12" s="14">
-        <f>MAX(0,(md!J9-md!I9))</f>
+      <c r="O12" s="14">
+        <f>MAX(0,(md!O8-md!N8))</f>
+        <v>27</v>
+      </c>
+      <c r="P12" s="14">
+        <f>MAX(0,(md!P8-md!O8))</f>
+        <v>96</v>
+      </c>
+      <c r="Q12" s="14">
+        <f>MAX(0,(md!Q8-md!P8))</f>
+        <v>39</v>
+      </c>
+      <c r="R12" s="14">
+        <f>MAX(0,(md!R8-md!Q8))</f>
+        <v>49</v>
+      </c>
+      <c r="S12" s="14">
+        <f>MAX(0,(md!S8-md!R8))</f>
+        <v>61</v>
+      </c>
+      <c r="T12" s="14">
+        <f>MAX(0,(md!T8-md!S8))</f>
         <v>44</v>
       </c>
-      <c r="K12" s="14">
-        <f>MAX(0,(md!K9-md!J9))</f>
-        <v>48</v>
-      </c>
-      <c r="L12" s="14">
-        <f>MAX(0,(md!L9-md!K9))</f>
-        <v>30</v>
-      </c>
-      <c r="M12" s="14">
-        <f>MAX(0,(md!M9-md!L9))</f>
+      <c r="U12" s="14">
+        <f>MAX(0,(md!U8-md!T8))</f>
+        <v>65</v>
+      </c>
+      <c r="V12" s="14">
+        <f>MAX(0,(md!V8-md!U8))</f>
+        <v>59</v>
+      </c>
+      <c r="W12" s="14">
+        <f>MAX(0,(md!W8-md!V8))</f>
+        <v>62</v>
+      </c>
+      <c r="X12" s="14">
+        <f>MAX(0,(md!X8-md!W8))</f>
         <v>51</v>
       </c>
-      <c r="N12" s="14">
-        <f>MAX(0,(md!N9-md!M9))</f>
-        <v>41</v>
-      </c>
-      <c r="O12" s="14">
-        <f>MAX(0,(md!O9-md!N9))</f>
-        <v>24</v>
-      </c>
-      <c r="P12" s="14">
-        <f>MAX(0,(md!P9-md!O9))</f>
-        <v>112</v>
-      </c>
-      <c r="Q12" s="14">
-        <f>MAX(0,(md!Q9-md!P9))</f>
-        <v>67</v>
-      </c>
-      <c r="R12" s="14">
-        <f>MAX(0,(md!R9-md!Q9))</f>
+      <c r="Y12" s="14">
+        <f>MAX(0,(md!Y8-md!X8))</f>
+        <v>70</v>
+      </c>
+      <c r="Z12" s="14">
+        <f>MAX(0,(md!Z8-md!Y8))</f>
+        <v>39</v>
+      </c>
+      <c r="AA12" s="14">
+        <f>MAX(0,(md!AA8-md!Z8))</f>
+        <v>42</v>
+      </c>
+      <c r="AB12" s="14">
+        <f>MAX(0,(md!AB8-md!AA8))</f>
         <v>51</v>
       </c>
-      <c r="S12" s="14">
-        <f>MAX(0,(md!S9-md!R9))</f>
-        <v>67</v>
-      </c>
-      <c r="T12" s="14">
-        <f>MAX(0,(md!T9-md!S9))</f>
-        <v>56</v>
-      </c>
-      <c r="U12" s="14">
-        <f>MAX(0,(md!U9-md!T9))</f>
-        <v>61</v>
-      </c>
-      <c r="V12" s="14">
-        <f>MAX(0,(md!V9-md!U9))</f>
-        <v>89</v>
-      </c>
-      <c r="W12" s="14">
-        <f>MAX(0,(md!W9-md!V9))</f>
-        <v>98</v>
-      </c>
-      <c r="X12" s="14">
-        <f>MAX(0,(md!X9-md!W9))</f>
-        <v>100</v>
-      </c>
-      <c r="Y12" s="14">
-        <f>MAX(0,(md!Y9-md!X9))</f>
-        <v>113</v>
-      </c>
-      <c r="Z12" s="14">
-        <f>MAX(0,(md!Z9-md!Y9))</f>
-        <v>105</v>
-      </c>
-      <c r="AA12" s="14">
-        <f>MAX(0,(md!AA9-md!Z9))</f>
-        <v>14</v>
-      </c>
-      <c r="AB12" s="14">
-        <f>MAX(0,(md!AB9-md!AA9))</f>
-        <v>119</v>
-      </c>
       <c r="AC12" s="14">
-        <f>MAX(0,(md!AC9-md!AB9))</f>
-        <v>31</v>
+        <f>MAX(0,(md!AC8-md!AB8))</f>
+        <v>59</v>
       </c>
       <c r="AD12" s="14">
-        <f>MAX(0,(md!AD9-md!AC9))</f>
-        <v>60</v>
+        <f>MAX(0,(md!AD8-md!AC8))</f>
+        <v>33</v>
       </c>
       <c r="AE12" s="14">
-        <f>MAX(0,(md!AE9-md!AD9))</f>
-        <v>70</v>
+        <f>MAX(0,(md!AE8-md!AD8))</f>
+        <v>104</v>
       </c>
       <c r="AF12" s="14">
-        <f>MAX(0,(md!AF9-md!AE9))</f>
-        <v>56</v>
+        <f>MAX(0,(md!AF8-md!AE8))</f>
+        <v>79</v>
       </c>
       <c r="AG12" s="14">
-        <f>MAX(0,(md!AG9-md!AF9))</f>
-        <v>0</v>
+        <f>MAX(0,(md!AG8-md!AF8))</f>
+        <v>57</v>
       </c>
       <c r="AH12" s="14">
-        <f>MAX(0,(md!AH9-md!AG9))</f>
+        <f>MAX(0,(md!AH8-md!AG8))</f>
         <v>0</v>
       </c>
       <c r="AI12" s="14">
-        <f>MAX(0,(md!AI9-md!AH9))</f>
+        <f>MAX(0,(md!AI8-md!AH8))</f>
         <v>0</v>
       </c>
       <c r="AJ12" s="14">
-        <f>MAX(0,(md!AJ9-md!AI9))</f>
+        <f>MAX(0,(md!AJ8-md!AI8))</f>
         <v>0</v>
       </c>
       <c r="AK12" s="14">
-        <f>MAX(0,(md!AK9-md!AJ9))</f>
+        <f>MAX(0,(md!AK8-md!AJ8))</f>
         <v>0</v>
       </c>
       <c r="AL12" s="14">
-        <f>MAX(0,(md!AL9-md!AK9))</f>
+        <f>MAX(0,(md!AL8-md!AK8))</f>
         <v>0</v>
       </c>
       <c r="AM12" s="14">
-        <f>MAX(0,(md!AM9-md!AL9))</f>
+        <f>MAX(0,(md!AM8-md!AL8))</f>
         <v>0</v>
       </c>
       <c r="AN12" s="14">
-        <f>MAX(0,(md!AN9-md!AM9))</f>
+        <f>MAX(0,(md!AN8-md!AM8))</f>
         <v>0</v>
       </c>
       <c r="AO12" s="14">
-        <f>MAX(0,(md!AO9-md!AN9))</f>
+        <f>MAX(0,(md!AO8-md!AN8))</f>
         <v>0</v>
       </c>
       <c r="AP12" s="14">
-        <f>MAX(0,(md!AP9-md!AO9))</f>
+        <f>MAX(0,(md!AP8-md!AO8))</f>
         <v>0</v>
       </c>
       <c r="AQ12" s="14">
-        <f>MAX(0,(md!AQ9-md!AP9))</f>
+        <f>MAX(0,(md!AQ8-md!AP8))</f>
         <v>0</v>
       </c>
       <c r="AR12" s="14">
-        <f>MAX(0,(md!AR9-md!AQ9))</f>
+        <f>MAX(0,(md!AR8-md!AQ8))</f>
         <v>0</v>
       </c>
       <c r="AS12" s="14">
-        <f>MAX(0,(md!AS9-md!AR9))</f>
+        <f>MAX(0,(md!AS8-md!AR8))</f>
         <v>0</v>
       </c>
       <c r="AT12" s="14">
-        <f>MAX(0,(md!AT9-md!AS9))</f>
+        <f>MAX(0,(md!AT8-md!AS8))</f>
         <v>0</v>
       </c>
       <c r="AU12" s="14">
-        <f>MAX(0,(md!AU9-md!AT9))</f>
+        <f>MAX(0,(md!AU8-md!AT8))</f>
         <v>0</v>
       </c>
       <c r="AV12" s="14">
-        <f>MAX(0,(md!AV9-md!AU9))</f>
+        <f>MAX(0,(md!AV8-md!AU8))</f>
         <v>0</v>
       </c>
       <c r="AW12" s="14">
-        <f>MAX(0,(md!AW9-md!AV9))</f>
+        <f>MAX(0,(md!AW8-md!AV8))</f>
         <v>0</v>
       </c>
       <c r="AX12" s="14">
-        <f>MAX(0,(md!AX9-md!AW9))</f>
+        <f>MAX(0,(md!AX8-md!AW8))</f>
         <v>0</v>
       </c>
       <c r="AY12" s="14">
-        <f>MAX(0,(md!AY9-md!AX9))</f>
+        <f>MAX(0,(md!AY8-md!AX8))</f>
         <v>0</v>
       </c>
       <c r="AZ12" s="14">
-        <f>MAX(0,(md!AZ9-md!AY9))</f>
+        <f>MAX(0,(md!AZ8-md!AY8))</f>
         <v>0</v>
       </c>
       <c r="BA12" s="14">
-        <f>MAX(0,(md!BA9-md!AZ9))</f>
+        <f>MAX(0,(md!BA8-md!AZ8))</f>
         <v>0</v>
       </c>
       <c r="BB12" s="14">
-        <f>MAX(0,(md!BB9-md!BA9))</f>
+        <f>MAX(0,(md!BB8-md!BA8))</f>
         <v>0</v>
       </c>
       <c r="BC12" s="14">
-        <f>MAX(0,(md!BC9-md!BB9))</f>
+        <f>MAX(0,(md!BC8-md!BB8))</f>
         <v>0</v>
       </c>
       <c r="BD12" s="14">
-        <f>MAX(0,(md!BD9-md!BC9))</f>
+        <f>MAX(0,(md!BD8-md!BC8))</f>
         <v>0</v>
       </c>
       <c r="BE12" s="14">
-        <f>MAX(0,(md!BE9-md!BD9))</f>
+        <f>MAX(0,(md!BE8-md!BD8))</f>
         <v>0</v>
       </c>
       <c r="BF12" s="14">
-        <f>MAX(0,(md!BF9-md!BE9))</f>
+        <f>MAX(0,(md!BF8-md!BE8))</f>
         <v>0</v>
       </c>
       <c r="BG12" s="14">
-        <f>MAX(0,(md!BG9-md!BF9))</f>
+        <f>MAX(0,(md!BG8-md!BF8))</f>
         <v>0</v>
       </c>
       <c r="BH12" s="14">
-        <f>MAX(0,(md!BH9-md!BG9))</f>
+        <f>MAX(0,(md!BH8-md!BG8))</f>
         <v>0</v>
       </c>
       <c r="BI12" s="14">
-        <f>MAX(0,(md!BI9-md!BH9))</f>
+        <f>MAX(0,(md!BI8-md!BH8))</f>
         <v>0</v>
       </c>
       <c r="BJ12" s="14">
-        <f>MAX(0,(md!BJ9-md!BI9))</f>
+        <f>MAX(0,(md!BJ8-md!BI8))</f>
         <v>0</v>
       </c>
       <c r="BK12" s="14">
-        <f>MAX(0,(md!BK9-md!BJ9))</f>
+        <f>MAX(0,(md!BK8-md!BJ8))</f>
         <v>0</v>
       </c>
       <c r="BL12" s="14">
-        <f>MAX(0,(md!BL9-md!BK9))</f>
+        <f>MAX(0,(md!BL8-md!BK8))</f>
         <v>0</v>
       </c>
       <c r="BM12" s="14">
-        <f>MAX(0,(md!BM9-md!BL9))</f>
+        <f>MAX(0,(md!BM8-md!BL8))</f>
         <v>0</v>
       </c>
       <c r="BN12" s="14">
-        <f>MAX(0,(md!BN9-md!BM9))</f>
+        <f>MAX(0,(md!BN8-md!BM8))</f>
         <v>0</v>
       </c>
       <c r="BO12" s="14">
-        <f>MAX(0,(md!BO9-md!BN9))</f>
+        <f>MAX(0,(md!BO8-md!BN8))</f>
         <v>0</v>
       </c>
       <c r="BP12" s="14">
-        <f>MAX(0,(md!BP9-md!BO9))</f>
+        <f>MAX(0,(md!BP8-md!BO8))</f>
         <v>0</v>
       </c>
       <c r="BQ12" s="14">
-        <f>MAX(0,(md!BQ9-md!BP9))</f>
+        <f>MAX(0,(md!BQ8-md!BP8))</f>
         <v>0</v>
       </c>
     </row>
@@ -33443,7 +33957,7 @@
       </c>
       <c r="AG13" s="14">
         <f>MAX(0,(md!AG9-md!AF9))</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="AH13" s="14">
         <f>MAX(0,(md!AH9-md!AG9))</f>
@@ -33720,7 +34234,7 @@
       </c>
       <c r="AG14" s="14">
         <f>MAX(0,(md!AG10-md!AF10))</f>
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="AH14" s="14">
         <f>MAX(0,(md!AH10-md!AG10))</f>
@@ -33997,7 +34511,7 @@
       </c>
       <c r="AG15" s="14">
         <f>MAX(0,(md!AG11-md!AF11))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH15" s="14">
         <f>MAX(0,(md!AH11-md!AG11))</f>
@@ -34274,7 +34788,7 @@
       </c>
       <c r="AG16" s="14">
         <f>MAX(0,(md!AG12-md!AF12))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AH16" s="14">
         <f>MAX(0,(md!AH12-md!AG12))</f>
@@ -34551,7 +35065,7 @@
       </c>
       <c r="AG17" s="14">
         <f>MAX(0,(md!AG13-md!AF13))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AH17" s="14">
         <f>MAX(0,(md!AH13-md!AG13))</f>
@@ -34828,7 +35342,7 @@
       </c>
       <c r="AG18" s="14">
         <f>MAX(0,(md!AG14-md!AF14))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH18" s="14">
         <f>MAX(0,(md!AH14-md!AG14))</f>
@@ -35105,7 +35619,7 @@
       </c>
       <c r="AG19" s="14">
         <f>MAX(0,(md!AG15-md!AF15))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AH19" s="14">
         <f>MAX(0,(md!AH15-md!AG15))</f>
@@ -35382,7 +35896,7 @@
       </c>
       <c r="AG20" s="14">
         <f>MAX(0,(md!AG16-md!AF16))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AH20" s="14">
         <f>MAX(0,(md!AH16-md!AG16))</f>
@@ -35659,7 +36173,7 @@
       </c>
       <c r="AG21" s="14">
         <f>MAX(0,(md!AG17-md!AF17))</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="AH21" s="14">
         <f>MAX(0,(md!AH17-md!AG17))</f>
@@ -36213,7 +36727,7 @@
       </c>
       <c r="AG23" s="14">
         <f>MAX(0,(md!AG19-md!AF19))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AH23" s="14">
         <f>MAX(0,(md!AH19-md!AG19))</f>
@@ -36490,7 +37004,7 @@
       </c>
       <c r="AG24" s="14">
         <f>MAX(0,(md!AG20-md!AF20))</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="AH24" s="14">
         <f>MAX(0,(md!AH20-md!AG20))</f>
@@ -37044,7 +37558,7 @@
       </c>
       <c r="AG26" s="14">
         <f>MAX(0,(md!AG22-md!AF22))</f>
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="AH26" s="14">
         <f>MAX(0,(md!AH22-md!AG22))</f>
@@ -37321,7 +37835,7 @@
       </c>
       <c r="AG27" s="14">
         <f>MAX(0,(md!AG23-md!AF23))</f>
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="AH27" s="14">
         <f>MAX(0,(md!AH23-md!AG23))</f>
@@ -37598,7 +38112,7 @@
       </c>
       <c r="AG28" s="14">
         <f>MAX(0,(md!AG24-md!AF24))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AH28" s="14">
         <f>MAX(0,(md!AH24-md!AG24))</f>
@@ -37875,7 +38389,7 @@
       </c>
       <c r="AG29" s="14">
         <f>MAX(0,(md!AG25-md!AF25))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH29" s="14">
         <f>MAX(0,(md!AH25-md!AG25))</f>
@@ -38152,7 +38666,7 @@
       </c>
       <c r="AG30" s="14">
         <f>MAX(0,(md!AG26-md!AF26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH30" s="14">
         <f>MAX(0,(md!AH26-md!AG26))</f>
@@ -38429,7 +38943,7 @@
       </c>
       <c r="AG31" s="14">
         <f>MAX(0,(md!AG27-md!AF27))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH31" s="14">
         <f>MAX(0,(md!AH27-md!AG27))</f>
@@ -38706,7 +39220,7 @@
       </c>
       <c r="AG32" s="14">
         <f>MAX(0,(md!AG28-md!AF28))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AH32" s="14">
         <f>MAX(0,(md!AH28-md!AG28))</f>
@@ -38983,7 +39497,7 @@
       </c>
       <c r="AG33" s="14">
         <f>MAX(0,(md!AG29-md!AF29))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AH33" s="14">
         <f>MAX(0,(md!AH29-md!AG29))</f>
@@ -39260,7 +39774,7 @@
       </c>
       <c r="AG34" s="14">
         <f>MAX(0,(md!AG30-md!AF30))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH34" s="14">
         <f>MAX(0,(md!AH30-md!AG30))</f>
@@ -39739,7 +40253,7 @@
       </c>
       <c r="AI2" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24.407208346506483</v>
       </c>
       <c r="AJ2" s="19">
         <f t="shared" ref="AJ2:BS2" si="1">(AJ7/(MAX(AJ6,1))*100)</f>
@@ -40016,7 +40530,7 @@
       </c>
       <c r="AI3" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.601036269430052</v>
       </c>
       <c r="AJ3" s="19">
         <f t="shared" ref="AJ3:BS3" si="3">(AJ8/MAX(1,AJ7))*100</f>
@@ -40293,7 +40807,7 @@
       </c>
       <c r="AI4" s="19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.3678756476683938</v>
       </c>
       <c r="AJ4" s="19">
         <f t="shared" ref="AJ4:BS4" si="5">(AJ9/MAX(1,AJ7))*100</f>
@@ -40570,7 +41084,7 @@
       </c>
       <c r="AI6" s="14">
         <f>MAX(0,(va!AJ5-va!AI5))</f>
-        <v>0</v>
+        <v>3163</v>
       </c>
       <c r="AJ6" s="14">
         <f>MAX(0,(va!AK5-va!AJ5))</f>
@@ -40847,7 +41361,7 @@
       </c>
       <c r="AI7" s="14">
         <f>MAX(0,(va!AJ2-va!AI2))</f>
-        <v>0</v>
+        <v>772</v>
       </c>
       <c r="AJ7" s="14">
         <f>MAX(0,(va!AK2-va!AJ2))</f>
@@ -41124,7 +41638,7 @@
       </c>
       <c r="AI8" s="14">
         <f>MAX(0,(va!AJ3-va!AI3))</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="AJ8" s="14">
         <f>MAX(0,(va!AK3-va!AJ3))</f>
@@ -41401,7 +41915,7 @@
       </c>
       <c r="AI9" s="14">
         <f>MAX(0,(va!AJ4-va!AI4))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AJ9" s="14">
         <f>MAX(0,(va!AK4-va!AJ4))</f>
@@ -41898,7 +42412,7 @@
       </c>
       <c r="AI11" s="16">
         <f>MAX(0,(va!AJ7-va!AI7))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AJ11" s="16">
         <f>MAX(0,(va!AK7-va!AJ7))</f>
@@ -43872,7 +44386,7 @@
       </c>
       <c r="AI18" s="16">
         <f>MAX(0,(va!AJ14-va!AI14))</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="AJ18" s="16">
         <f>MAX(0,(va!AK14-va!AJ14))</f>
@@ -44154,7 +44668,7 @@
       </c>
       <c r="AI19" s="16">
         <f>MAX(0,(va!AJ15-va!AI15))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ19" s="16">
         <f>MAX(0,(va!AK15-va!AJ15))</f>
@@ -45282,7 +45796,7 @@
       </c>
       <c r="AI23" s="16">
         <f>MAX(0,(va!AJ19-va!AI19))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AJ23" s="16">
         <f>MAX(0,(va!AK19-va!AJ19))</f>
@@ -45846,7 +46360,7 @@
       </c>
       <c r="AI25" s="16">
         <f>MAX(0,(va!AJ21-va!AI21))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AJ25" s="16">
         <f>MAX(0,(va!AK21-va!AJ21))</f>
@@ -47538,7 +48052,7 @@
       </c>
       <c r="AI31" s="16">
         <f>MAX(0,(va!AJ27-va!AI27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ31" s="16">
         <f>MAX(0,(va!AK27-va!AJ27))</f>
@@ -48384,7 +48898,7 @@
       </c>
       <c r="AI34" s="16">
         <f>MAX(0,(va!AJ30-va!AI30))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ34" s="16">
         <f>MAX(0,(va!AK30-va!AJ30))</f>
@@ -48666,7 +49180,7 @@
       </c>
       <c r="AI35" s="16">
         <f>MAX(0,(va!AJ31-va!AI31))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AJ35" s="16">
         <f>MAX(0,(va!AK31-va!AJ31))</f>
@@ -48948,7 +49462,7 @@
       </c>
       <c r="AI36" s="16">
         <f>MAX(0,(va!AJ32-va!AI32))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ36" s="16">
         <f>MAX(0,(va!AK32-va!AJ32))</f>
@@ -49230,7 +49744,7 @@
       </c>
       <c r="AI37" s="16">
         <f>MAX(0,(va!AJ33-va!AI33))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ37" s="16">
         <f>MAX(0,(va!AK33-va!AJ33))</f>
@@ -50076,7 +50590,7 @@
       </c>
       <c r="AI40" s="16">
         <f>MAX(0,(va!AJ36-va!AI36))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ40" s="16">
         <f>MAX(0,(va!AK36-va!AJ36))</f>
@@ -51204,7 +51718,7 @@
       </c>
       <c r="AI44" s="16">
         <f>MAX(0,(va!AJ40-va!AI40))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ44" s="16">
         <f>MAX(0,(va!AK40-va!AJ40))</f>
@@ -52332,7 +52846,7 @@
       </c>
       <c r="AI48" s="16">
         <f>MAX(0,(va!AJ44-va!AI44))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ48" s="16">
         <f>MAX(0,(va!AK44-va!AJ44))</f>
@@ -52896,7 +53410,7 @@
       </c>
       <c r="AI50" s="16">
         <f>MAX(0,(va!AJ46-va!AI46))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ50" s="16">
         <f>MAX(0,(va!AK46-va!AJ46))</f>
@@ -53460,7 +53974,7 @@
       </c>
       <c r="AI52" s="16">
         <f>MAX(0,(va!AJ48-va!AI48))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ52" s="16">
         <f>MAX(0,(va!AK48-va!AJ48))</f>
@@ -54024,7 +54538,7 @@
       </c>
       <c r="AI54" s="16">
         <f>MAX(0,(va!AJ50-va!AI50))</f>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AJ54" s="16">
         <f>MAX(0,(va!AK50-va!AJ50))</f>
@@ -54306,7 +54820,7 @@
       </c>
       <c r="AI55" s="16">
         <f>MAX(0,(va!AJ51-va!AI51))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ55" s="16">
         <f>MAX(0,(va!AK51-va!AJ51))</f>
@@ -54588,7 +55102,7 @@
       </c>
       <c r="AI56" s="16">
         <f>MAX(0,(va!AJ52-va!AI52))</f>
-        <v>0</v>
+        <v>211</v>
       </c>
       <c r="AJ56" s="16">
         <f>MAX(0,(va!AK52-va!AJ52))</f>
@@ -55152,7 +55666,7 @@
       </c>
       <c r="AI58" s="16">
         <f>MAX(0,(va!AJ54-va!AI54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ58" s="16">
         <f>MAX(0,(va!AK54-va!AJ54))</f>
@@ -55434,7 +55948,7 @@
       </c>
       <c r="AI59" s="16">
         <f>MAX(0,(va!AJ55-va!AI55))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ59" s="16">
         <f>MAX(0,(va!AK55-va!AJ55))</f>
@@ -55716,7 +56230,7 @@
       </c>
       <c r="AI60" s="16">
         <f>MAX(0,(va!AJ56-va!AI56))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AJ60" s="16">
         <f>MAX(0,(va!AK56-va!AJ56))</f>
@@ -57408,7 +57922,7 @@
       </c>
       <c r="AI66" s="16">
         <f>MAX(0,(va!AJ62-va!AI62))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AJ66" s="16">
         <f>MAX(0,(va!AK62-va!AJ62))</f>
@@ -57690,7 +58204,7 @@
       </c>
       <c r="AI67" s="16">
         <f>MAX(0,(va!AJ63-va!AI63))</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AJ67" s="16">
         <f>MAX(0,(va!AK63-va!AJ63))</f>
@@ -57972,7 +58486,7 @@
       </c>
       <c r="AI68" s="16">
         <f>MAX(0,(va!AJ64-va!AI64))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AJ68" s="16">
         <f>MAX(0,(va!AK64-va!AJ64))</f>
@@ -58254,7 +58768,7 @@
       </c>
       <c r="AI69" s="16">
         <f>MAX(0,(va!AJ65-va!AI65))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AJ69" s="16">
         <f>MAX(0,(va!AK65-va!AJ65))</f>
@@ -58536,7 +59050,7 @@
       </c>
       <c r="AI70" s="16">
         <f>MAX(0,(va!AJ66-va!AI66))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ70" s="16">
         <f>MAX(0,(va!AK66-va!AJ66))</f>
@@ -58818,7 +59332,7 @@
       </c>
       <c r="AI71" s="16">
         <f>MAX(0,(va!AJ67-va!AI67))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AJ71" s="16">
         <f>MAX(0,(va!AK67-va!AJ67))</f>
@@ -61920,7 +62434,7 @@
       </c>
       <c r="AI82" s="16">
         <f>MAX(0,(va!AJ78-va!AI78))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ82" s="16">
         <f>MAX(0,(va!AK78-va!AJ78))</f>
@@ -62484,7 +62998,7 @@
       </c>
       <c r="AI84" s="16">
         <f>MAX(0,(va!AJ80-va!AI80))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ84" s="16">
         <f>MAX(0,(va!AK80-va!AJ80))</f>
@@ -62766,7 +63280,7 @@
       </c>
       <c r="AI85" s="16">
         <f>MAX(0,(va!AJ81-va!AI81))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AJ85" s="16">
         <f>MAX(0,(va!AK81-va!AJ81))</f>
@@ -63048,7 +63562,7 @@
       </c>
       <c r="AI86" s="16">
         <f>MAX(0,(va!AJ82-va!AI82))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ86" s="16">
         <f>MAX(0,(va!AK82-va!AJ82))</f>
@@ -63330,7 +63844,7 @@
       </c>
       <c r="AI87" s="16">
         <f>MAX(0,(va!AJ83-va!AI83))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ87" s="16">
         <f>MAX(0,(va!AK83-va!AJ83))</f>
@@ -63612,7 +64126,7 @@
       </c>
       <c r="AI88" s="16">
         <f>MAX(0,(va!AJ84-va!AI84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ88" s="16">
         <f>MAX(0,(va!AK84-va!AJ84))</f>
@@ -64176,7 +64690,7 @@
       </c>
       <c r="AI90" s="16">
         <f>MAX(0,(va!AJ86-va!AI86))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ90" s="16">
         <f>MAX(0,(va!AK86-va!AJ86))</f>
@@ -64740,7 +65254,7 @@
       </c>
       <c r="AI92" s="16">
         <f>MAX(0,(va!AJ88-va!AI88))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ92" s="16">
         <f>MAX(0,(va!AK88-va!AJ88))</f>
@@ -65586,7 +66100,7 @@
       </c>
       <c r="AI95" s="16">
         <f>MAX(0,(va!AJ91-va!AI91))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ95" s="16">
         <f>MAX(0,(va!AK91-va!AJ91))</f>
@@ -65868,7 +66382,7 @@
       </c>
       <c r="AI96" s="16">
         <f>MAX(0,(va!AJ92-va!AI92))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ96" s="16">
         <f>MAX(0,(va!AK92-va!AJ92))</f>
@@ -66150,7 +66664,7 @@
       </c>
       <c r="AI97" s="16">
         <f>MAX(0,(va!AJ93-va!AI93))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ97" s="16">
         <f>MAX(0,(va!AK93-va!AJ93))</f>
@@ -66714,7 +67228,7 @@
       </c>
       <c r="AI99" s="16">
         <f>MAX(0,(va!AJ95-va!AI95))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ99" s="16">
         <f>MAX(0,(va!AK95-va!AJ95))</f>
@@ -66996,7 +67510,7 @@
       </c>
       <c r="AI100" s="16">
         <f>MAX(0,(va!AJ96-va!AI96))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ100" s="16">
         <f>MAX(0,(va!AK96-va!AJ96))</f>
@@ -67278,7 +67792,7 @@
       </c>
       <c r="AI101" s="16">
         <f>MAX(0,(va!AJ97-va!AI97))</f>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="AJ101" s="16">
         <f>MAX(0,(va!AK97-va!AJ97))</f>
@@ -67560,7 +68074,7 @@
       </c>
       <c r="AI102" s="16">
         <f>MAX(0,(va!AJ98-va!AI98))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AJ102" s="16">
         <f>MAX(0,(va!AK98-va!AJ98))</f>
@@ -68406,7 +68920,7 @@
       </c>
       <c r="AI105" s="16">
         <f>MAX(0,(va!AJ101-va!AI101))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ105" s="16">
         <f>MAX(0,(va!AK101-va!AJ101))</f>
@@ -68688,7 +69202,7 @@
       </c>
       <c r="AI106" s="16">
         <f>MAX(0,(va!AJ102-va!AI102))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ106" s="16">
         <f>MAX(0,(va!AK102-va!AJ102))</f>
@@ -68970,7 +69484,7 @@
       </c>
       <c r="AI107" s="16">
         <f>MAX(0,(va!AJ103-va!AI103))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ107" s="16">
         <f>MAX(0,(va!AK103-va!AJ103))</f>
@@ -69252,7 +69766,7 @@
       </c>
       <c r="AI108" s="16">
         <f>MAX(0,(va!AJ104-va!AI104))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ108" s="16">
         <f>MAX(0,(va!AK104-va!AJ104))</f>
@@ -69534,7 +70048,7 @@
       </c>
       <c r="AI109" s="16">
         <f>MAX(0,(va!AJ105-va!AI105))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ109" s="16">
         <f>MAX(0,(va!AK105-va!AJ105))</f>
@@ -69816,7 +70330,7 @@
       </c>
       <c r="AI110" s="16">
         <f>MAX(0,(va!AJ106-va!AI106))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AJ110" s="16">
         <f>MAX(0,(va!AK106-va!AJ106))</f>
@@ -70380,7 +70894,7 @@
       </c>
       <c r="AI112" s="16">
         <f>MAX(0,(va!AJ108-va!AI108))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ112" s="16">
         <f>MAX(0,(va!AK108-va!AJ108))</f>
@@ -70662,7 +71176,7 @@
       </c>
       <c r="AI113" s="16">
         <f>MAX(0,(va!AJ109-va!AI109))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ113" s="16">
         <f>MAX(0,(va!AK109-va!AJ109))</f>
@@ -70944,7 +71458,7 @@
       </c>
       <c r="AI114" s="16">
         <f>MAX(0,(va!AJ110-va!AI110))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AJ114" s="16">
         <f>MAX(0,(va!AK110-va!AJ110))</f>
@@ -72072,7 +72586,7 @@
       </c>
       <c r="AI118" s="16">
         <f>MAX(0,(va!AJ114-va!AI114))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AJ118" s="16">
         <f>MAX(0,(va!AK114-va!AJ114))</f>
@@ -72354,7 +72868,7 @@
       </c>
       <c r="AI119" s="16">
         <f>MAX(0,(va!AJ115-va!AI115))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ119" s="16">
         <f>MAX(0,(va!AK115-va!AJ115))</f>
@@ -73200,7 +73714,7 @@
       </c>
       <c r="AI122" s="16">
         <f>MAX(0,(va!AJ118-va!AI118))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ122" s="16">
         <f>MAX(0,(va!AK118-va!AJ118))</f>
@@ -73764,7 +74278,7 @@
       </c>
       <c r="AI124" s="16">
         <f>MAX(0,(va!AJ120-va!AI120))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ124" s="16">
         <f>MAX(0,(va!AK120-va!AJ120))</f>
@@ -74046,7 +74560,7 @@
       </c>
       <c r="AI125" s="16">
         <f>MAX(0,(va!AJ121-va!AI121))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ125" s="16">
         <f>MAX(0,(va!AK121-va!AJ121))</f>
@@ -74328,7 +74842,7 @@
       </c>
       <c r="AI126" s="16">
         <f>MAX(0,(va!AJ122-va!AI122))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ126" s="16">
         <f>MAX(0,(va!AK122-va!AJ122))</f>
@@ -74892,7 +75406,7 @@
       </c>
       <c r="AI128" s="16">
         <f>MAX(0,(va!AJ124-va!AI124))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ128" s="16">
         <f>MAX(0,(va!AK124-va!AJ124))</f>
@@ -75456,7 +75970,7 @@
       </c>
       <c r="AI130" s="16">
         <f>MAX(0,(va!AJ126-va!AI126))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ130" s="16">
         <f>MAX(0,(va!AK126-va!AJ126))</f>
@@ -75738,7 +76252,7 @@
       </c>
       <c r="AI131" s="16">
         <f>MAX(0,(va!AJ127-va!AI127))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ131" s="16">
         <f>MAX(0,(va!AK127-va!AJ127))</f>
@@ -76020,7 +76534,7 @@
       </c>
       <c r="AI132" s="16">
         <f>MAX(0,(va!AJ128-va!AI128))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ132" s="16">
         <f>MAX(0,(va!AK128-va!AJ128))</f>
@@ -76302,7 +76816,7 @@
       </c>
       <c r="AI133" s="16">
         <f>MAX(0,(va!AJ129-va!AI129))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AJ133" s="16">
         <f>MAX(0,(va!AK129-va!AJ129))</f>
@@ -76584,7 +77098,7 @@
       </c>
       <c r="AI134" s="16">
         <f>MAX(0,(va!AJ130-va!AI130))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ134" s="16">
         <f>MAX(0,(va!AK130-va!AJ130))</f>
@@ -76866,7 +77380,7 @@
       </c>
       <c r="AI135" s="16">
         <f>MAX(0,(va!AJ131-va!AI131))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ135" s="16">
         <f>MAX(0,(va!AK131-va!AJ131))</f>
@@ -77430,7 +77944,7 @@
       </c>
       <c r="AI137" s="16">
         <f>MAX(0,(va!AJ133-va!AI133))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ137" s="16">
         <f>MAX(0,(va!AK133-va!AJ133))</f>
@@ -78840,7 +79354,7 @@
       </c>
       <c r="AI142" s="16">
         <f>MAX(0,(va!AJ138-va!AI138))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ142" s="16">
         <f>MAX(0,(va!AK138-va!AJ138))</f>
@@ -79122,7 +79636,7 @@
       </c>
       <c r="AI143" s="16">
         <f>MAX(0,(va!AJ139-va!AI139))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ143" s="16">
         <f>MAX(0,(va!AK139-va!AJ139))</f>

</xml_diff>

<commit_message>
26 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1831BD83-602B-4498-B9E7-90E418366668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C194E-021B-4465-BE29-94CE3D458442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2999,10 +2999,6 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6A2AD35F-60C9-437C-AA7B-C217E8DC7927}" name="va" displayName="va" ref="B6:BT140" totalsRowShown="0">
-  <autoFilter ref="B6:BT140" xr:uid="{CC6A9FB3-0DF8-4FF3-B6B0-EFF5822E8885}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:BT140">
-    <sortCondition ref="C6:C140"/>
-  </sortState>
   <tableColumns count="71">
     <tableColumn id="54" xr3:uid="{F1106E80-B529-4637-9194-7C9771A7B601}" name="Locality" dataDxfId="157"/>
     <tableColumn id="1" xr3:uid="{179FB13D-5548-4710-AF18-46935F888BFD}" name="idx" dataDxfId="156"/>
@@ -4022,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AR2" sqref="AR2"/>
+      <selection pane="bottomRight" activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4171,6 +4167,9 @@
       <c r="AR2" s="12">
         <v>17302</v>
       </c>
+      <c r="AS2" s="12">
+        <v>18068</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4335,7 +4334,7 @@
       </c>
       <c r="AS3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3841</v>
       </c>
       <c r="AT3" s="10">
         <f t="shared" si="0"/>
@@ -4620,6 +4619,9 @@
       <c r="AR5" s="10">
         <v>165</v>
       </c>
+      <c r="AS5" s="10">
+        <v>178</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -4999,6 +5001,9 @@
       <c r="AR7" s="10">
         <v>427</v>
       </c>
+      <c r="AS7" s="10">
+        <v>444</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5133,6 +5138,9 @@
       <c r="AR8" s="10">
         <v>256</v>
       </c>
+      <c r="AS8" s="10">
+        <v>261</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5267,6 +5275,9 @@
       <c r="AR9" s="10">
         <v>258</v>
       </c>
+      <c r="AS9" s="10">
+        <v>268</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5401,6 +5412,9 @@
       <c r="AR10" s="10">
         <v>636</v>
       </c>
+      <c r="AS10" s="10">
+        <v>663</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5535,6 +5549,9 @@
       <c r="AR11" s="10">
         <v>513</v>
       </c>
+      <c r="AS11" s="10">
+        <v>552</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5669,6 +5686,9 @@
       <c r="AR12" s="10">
         <v>414</v>
       </c>
+      <c r="AS12" s="10">
+        <v>419</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5803,6 +5823,9 @@
       <c r="AR13" s="10">
         <v>543</v>
       </c>
+      <c r="AS13" s="10">
+        <v>570</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -5937,6 +5960,9 @@
       <c r="AR14" s="10">
         <v>518</v>
       </c>
+      <c r="AS14" s="10">
+        <v>530</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6069,6 +6095,9 @@
         <v>110</v>
       </c>
       <c r="AR15" s="10">
+        <v>134</v>
+      </c>
+      <c r="AS15" s="10">
         <v>134</v>
       </c>
     </row>
@@ -6324,7 +6353,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AG2" sqref="AG2"/>
+      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6441,7 +6470,7 @@
         <v>71357</v>
       </c>
       <c r="AH2" s="10">
-        <v>0</v>
+        <v>78084</v>
       </c>
       <c r="AI2" s="10">
         <v>0</v>
@@ -6678,7 +6707,7 @@
       </c>
       <c r="AH3" s="10">
         <f>SUM(md[26-Apr])</f>
-        <v>0</v>
+        <v>18581</v>
       </c>
       <c r="AI3" s="10">
         <f>SUM(md[27-Apr])</f>
@@ -6919,7 +6948,7 @@
         <v>3760</v>
       </c>
       <c r="AH4" s="10">
-        <v>0</v>
+        <v>3962</v>
       </c>
       <c r="AI4" s="10">
         <v>0</v>
@@ -7125,7 +7154,7 @@
         <v>797</v>
       </c>
       <c r="AH5" s="10">
-        <v>0</v>
+        <v>827</v>
       </c>
       <c r="AI5" s="10">
         <v>0</v>
@@ -7542,6 +7571,9 @@
       <c r="AG7">
         <v>105</v>
       </c>
+      <c r="AH7">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7643,6 +7675,9 @@
       <c r="AG8" s="10">
         <v>1430</v>
       </c>
+      <c r="AH8" s="10">
+        <v>1510</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7744,6 +7779,9 @@
       <c r="AG9">
         <v>1791</v>
       </c>
+      <c r="AH9">
+        <v>1866</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7845,6 +7883,9 @@
       <c r="AG10">
         <v>2387</v>
       </c>
+      <c r="AH10">
+        <v>2509</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -7946,6 +7987,9 @@
       <c r="AG11">
         <v>130</v>
       </c>
+      <c r="AH11">
+        <v>134</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8047,6 +8091,9 @@
       <c r="AG12">
         <v>61</v>
       </c>
+      <c r="AH12">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8148,6 +8195,9 @@
       <c r="AG13">
         <v>384</v>
       </c>
+      <c r="AH13">
+        <v>391</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8249,6 +8299,9 @@
       <c r="AG14">
         <v>146</v>
       </c>
+      <c r="AH14">
+        <v>154</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8350,6 +8403,9 @@
       <c r="AG15">
         <v>483</v>
       </c>
+      <c r="AH15">
+        <v>504</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8451,8 +8507,11 @@
       <c r="AG16" s="10">
         <v>38</v>
       </c>
+      <c r="AH16" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8552,8 +8611,11 @@
       <c r="AG17">
         <v>814</v>
       </c>
+      <c r="AH17">
+        <v>834</v>
+      </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8653,8 +8715,11 @@
       <c r="AG18">
         <v>4</v>
       </c>
+      <c r="AH18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8754,8 +8819,11 @@
       <c r="AG19">
         <v>302</v>
       </c>
+      <c r="AH19">
+        <v>319</v>
+      </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -8855,8 +8923,11 @@
       <c r="AG20">
         <v>686</v>
       </c>
+      <c r="AH20">
+        <v>707</v>
+      </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -8956,8 +9027,11 @@
       <c r="AG21">
         <v>67</v>
       </c>
+      <c r="AH21">
+        <v>68</v>
+      </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9057,8 +9131,11 @@
       <c r="AG22">
         <v>3483</v>
       </c>
+      <c r="AH22">
+        <v>3645</v>
+      </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9158,8 +9235,11 @@
       <c r="AG23">
         <v>4795</v>
       </c>
+      <c r="AH23">
+        <v>4987</v>
+      </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9259,8 +9339,11 @@
       <c r="AG24">
         <v>52</v>
       </c>
+      <c r="AH24">
+        <v>53</v>
+      </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9360,8 +9443,11 @@
       <c r="AG25">
         <v>124</v>
       </c>
+      <c r="AH25">
+        <v>133</v>
+      </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9461,8 +9547,11 @@
       <c r="AG26">
         <v>14</v>
       </c>
+      <c r="AH26">
+        <v>16</v>
+      </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -9562,8 +9651,11 @@
       <c r="AG27">
         <v>28</v>
       </c>
+      <c r="AH27">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -9663,8 +9755,11 @@
       <c r="AG28">
         <v>154</v>
       </c>
+      <c r="AH28">
+        <v>173</v>
+      </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -9764,8 +9859,11 @@
       <c r="AG29">
         <v>242</v>
       </c>
+      <c r="AH29">
+        <v>270</v>
+      </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -9865,8 +9963,11 @@
       <c r="AG30">
         <v>46</v>
       </c>
+      <c r="AH30">
+        <v>48</v>
+      </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -9963,7 +10064,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="Q6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ2" sqref="AJ2"/>
+      <selection pane="bottomRight" activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10121,7 +10222,7 @@
       </c>
       <c r="AK2" s="10">
         <f>SUM(va[26-Apr])</f>
-        <v>0</v>
+        <v>12970</v>
       </c>
       <c r="AL2" s="10">
         <f>SUM(va[27-Apr])</f>
@@ -10365,7 +10466,7 @@
         <v>1942</v>
       </c>
       <c r="AK3" s="10">
-        <v>0</v>
+        <v>2014</v>
       </c>
       <c r="AL3" s="10">
         <v>0</v>
@@ -10574,7 +10675,7 @@
         <v>436</v>
       </c>
       <c r="AK4" s="10">
-        <v>0</v>
+        <v>448</v>
       </c>
       <c r="AL4" s="10">
         <v>0</v>
@@ -10783,7 +10884,7 @@
         <v>72178</v>
       </c>
       <c r="AK5" s="10">
-        <v>0</v>
+        <v>76118</v>
       </c>
       <c r="AL5" s="10">
         <v>0</v>
@@ -11218,9 +11319,12 @@
       <c r="AJ7" s="10">
         <v>575</v>
       </c>
+      <c r="AK7" s="10">
+        <v>591</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11328,9 +11432,12 @@
       <c r="AJ8" s="10">
         <v>5</v>
       </c>
+      <c r="AK8" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11436,9 +11543,12 @@
       <c r="AJ9" s="10">
         <v>27</v>
       </c>
+      <c r="AK9" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -11544,9 +11654,12 @@
       <c r="AJ10" s="10">
         <v>2</v>
       </c>
+      <c r="AK10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -11652,9 +11765,12 @@
       <c r="AJ11" s="10">
         <v>39</v>
       </c>
+      <c r="AK11" s="10">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -11760,9 +11876,12 @@
       <c r="AJ12" s="10">
         <v>1</v>
       </c>
+      <c r="AK12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -11867,6 +11986,9 @@
       </c>
       <c r="AJ13" s="10">
         <v>8</v>
+      </c>
+      <c r="AK13" s="10">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
@@ -11978,9 +12100,12 @@
       <c r="AJ14" s="10">
         <v>764</v>
       </c>
+      <c r="AK14" s="10">
+        <v>790</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12088,9 +12213,12 @@
       <c r="AJ15" s="10">
         <v>36</v>
       </c>
+      <c r="AK15" s="10">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -12196,9 +12324,12 @@
       <c r="AJ16" s="10">
         <v>0</v>
       </c>
+      <c r="AK16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12304,9 +12435,12 @@
       <c r="AJ17" s="10">
         <v>1</v>
       </c>
+      <c r="AK17" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -12412,9 +12546,12 @@
       <c r="AJ18" s="10">
         <v>5</v>
       </c>
+      <c r="AK18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -12520,9 +12657,12 @@
       <c r="AJ19" s="10">
         <v>184</v>
       </c>
+      <c r="AK19" s="10">
+        <v>184</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -12628,9 +12768,12 @@
       <c r="AJ20" s="10">
         <v>5</v>
       </c>
+      <c r="AK20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -12736,9 +12879,12 @@
       <c r="AJ21" s="10">
         <v>370</v>
       </c>
+      <c r="AK21" s="10">
+        <v>371</v>
+      </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -12844,9 +12990,12 @@
       <c r="AJ22" s="10">
         <v>3</v>
       </c>
+      <c r="AK22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -12952,9 +13101,12 @@
       <c r="AJ23" s="10">
         <v>10</v>
       </c>
+      <c r="AK23" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -13060,9 +13212,12 @@
       <c r="AJ24" s="10">
         <v>10</v>
       </c>
+      <c r="AK24" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -13170,9 +13325,12 @@
       <c r="AJ25" s="10">
         <v>9</v>
       </c>
+      <c r="AK25" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -13278,9 +13436,12 @@
       <c r="AJ26" s="10">
         <v>12</v>
       </c>
+      <c r="AK26" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -13386,9 +13547,12 @@
       <c r="AJ27" s="10">
         <v>24</v>
       </c>
+      <c r="AK27" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -13494,9 +13658,12 @@
       <c r="AJ28" s="10">
         <v>10</v>
       </c>
+      <c r="AK28" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -13602,8 +13769,11 @@
       <c r="AJ29" s="10">
         <v>48</v>
       </c>
+      <c r="AK29" s="10">
+        <v>50</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -13712,9 +13882,12 @@
       <c r="AJ30" s="10">
         <v>200</v>
       </c>
+      <c r="AK30" s="10">
+        <v>208</v>
+      </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -13822,9 +13995,12 @@
       <c r="AJ31" s="10">
         <v>440</v>
       </c>
+      <c r="AK31" s="10">
+        <v>457</v>
+      </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -13930,9 +14106,12 @@
       <c r="AJ32" s="10">
         <v>11</v>
       </c>
+      <c r="AK32" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -14038,9 +14217,12 @@
       <c r="AJ33" s="10">
         <v>43</v>
       </c>
+      <c r="AK33" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -14148,9 +14330,12 @@
       <c r="AJ34" s="10">
         <v>12</v>
       </c>
+      <c r="AK34" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -14256,9 +14441,12 @@
       <c r="AJ35" s="10">
         <v>69</v>
       </c>
+      <c r="AK35" s="10">
+        <v>70</v>
+      </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -14364,9 +14552,12 @@
       <c r="AJ36" s="10">
         <v>103</v>
       </c>
+      <c r="AK36" s="10">
+        <v>105</v>
+      </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -14472,9 +14663,12 @@
       <c r="AJ37" s="10">
         <v>20</v>
       </c>
+      <c r="AK37" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -14582,9 +14776,12 @@
       <c r="AJ38" s="10">
         <v>12</v>
       </c>
+      <c r="AK38" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -14690,9 +14887,12 @@
       <c r="AJ39" s="10">
         <v>30</v>
       </c>
+      <c r="AK39" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -14798,9 +14998,12 @@
       <c r="AJ40" s="10">
         <v>30</v>
       </c>
+      <c r="AK40" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -14906,9 +15109,12 @@
       <c r="AJ41" s="10">
         <v>4</v>
       </c>
+      <c r="AK41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -15014,9 +15220,12 @@
       <c r="AJ42" s="10">
         <v>28</v>
       </c>
+      <c r="AK42" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -15122,9 +15331,12 @@
       <c r="AJ43" s="10">
         <v>18</v>
       </c>
+      <c r="AK43" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -15230,9 +15442,12 @@
       <c r="AJ44" s="10">
         <v>21</v>
       </c>
+      <c r="AK44" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -15338,9 +15553,12 @@
       <c r="AJ45" s="10">
         <v>27</v>
       </c>
+      <c r="AK45" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -15448,9 +15666,12 @@
       <c r="AJ46" s="10">
         <v>13</v>
       </c>
+      <c r="AK46" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -15556,9 +15777,12 @@
       <c r="AJ47" s="10">
         <v>0</v>
       </c>
+      <c r="AK47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -15664,9 +15888,12 @@
       <c r="AJ48" s="10">
         <v>3</v>
       </c>
+      <c r="AK48" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -15772,9 +15999,12 @@
       <c r="AJ49" s="10">
         <v>4</v>
       </c>
+      <c r="AK49" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -15882,9 +16112,12 @@
       <c r="AJ50" s="10">
         <v>146</v>
       </c>
+      <c r="AK50" s="10">
+        <v>187</v>
+      </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -15990,9 +16223,12 @@
       <c r="AJ51" s="10">
         <v>20</v>
       </c>
+      <c r="AK51" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -16100,9 +16336,12 @@
       <c r="AJ52" s="10">
         <v>2745</v>
       </c>
+      <c r="AK52" s="10">
+        <v>2889</v>
+      </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -16208,9 +16447,12 @@
       <c r="AJ53" s="10">
         <v>26</v>
       </c>
+      <c r="AK53" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -16316,8 +16558,11 @@
       <c r="AJ54" s="10">
         <v>26</v>
       </c>
+      <c r="AK54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -16426,8 +16671,11 @@
       <c r="AJ55" s="10">
         <v>101</v>
       </c>
+      <c r="AK55" s="10">
+        <v>104</v>
+      </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -16536,9 +16784,12 @@
       <c r="AJ56" s="10">
         <v>764</v>
       </c>
+      <c r="AK56" s="10">
+        <v>792</v>
+      </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -16646,9 +16897,12 @@
       <c r="AJ57" s="10">
         <v>8</v>
       </c>
+      <c r="AK57" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -16754,9 +17008,12 @@
       <c r="AJ58" s="10">
         <v>5</v>
       </c>
+      <c r="AK58" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -16862,9 +17119,12 @@
       <c r="AJ59" s="10">
         <v>20</v>
       </c>
+      <c r="AK59" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -16970,9 +17230,12 @@
       <c r="AJ60" s="10">
         <v>2</v>
       </c>
+      <c r="AK60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -17080,9 +17343,12 @@
       <c r="AJ61" s="10">
         <v>7</v>
       </c>
+      <c r="AK61" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -17188,9 +17454,12 @@
       <c r="AJ62" s="10">
         <v>93</v>
       </c>
+      <c r="AK62" s="10">
+        <v>93</v>
+      </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -17296,9 +17565,12 @@
       <c r="AJ63" s="10">
         <v>82</v>
       </c>
+      <c r="AK63" s="10">
+        <v>84</v>
+      </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -17404,9 +17676,12 @@
       <c r="AJ64" s="10">
         <v>72</v>
       </c>
+      <c r="AK64" s="10">
+        <v>74</v>
+      </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -17512,9 +17787,12 @@
       <c r="AJ65" s="10">
         <v>42</v>
       </c>
+      <c r="AK65" s="10">
+        <v>43</v>
+      </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -17620,8 +17898,11 @@
       <c r="AJ66" s="10">
         <v>33</v>
       </c>
+      <c r="AK66" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -17730,9 +18011,12 @@
       <c r="AJ67" s="10">
         <v>564</v>
       </c>
+      <c r="AK67" s="10">
+        <v>596</v>
+      </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -17840,9 +18124,12 @@
       <c r="AJ68" s="10">
         <v>0</v>
       </c>
+      <c r="AK68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -17948,9 +18235,12 @@
       <c r="AJ69" s="10">
         <v>3</v>
       </c>
+      <c r="AK69" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -18056,9 +18346,12 @@
       <c r="AJ70" s="10">
         <v>0</v>
       </c>
+      <c r="AK70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -18164,9 +18457,12 @@
       <c r="AJ71" s="10">
         <v>13</v>
       </c>
+      <c r="AK71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -18272,9 +18568,12 @@
       <c r="AJ72" s="10">
         <v>30</v>
       </c>
+      <c r="AK72" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -18380,9 +18679,12 @@
       <c r="AJ73" s="10">
         <v>11</v>
       </c>
+      <c r="AK73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -18488,9 +18790,12 @@
       <c r="AJ74" s="10">
         <v>1</v>
       </c>
+      <c r="AK74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -18596,9 +18901,12 @@
       <c r="AJ75" s="10">
         <v>1</v>
       </c>
+      <c r="AK75" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -18706,9 +19014,12 @@
       <c r="AJ76" s="10">
         <v>1</v>
       </c>
+      <c r="AK76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -18814,9 +19125,12 @@
       <c r="AJ77" s="10">
         <v>4</v>
       </c>
+      <c r="AK77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -18922,9 +19236,12 @@
       <c r="AJ78" s="10">
         <v>51</v>
       </c>
+      <c r="AK78" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -19030,9 +19347,12 @@
       <c r="AJ79" s="10">
         <v>10</v>
       </c>
+      <c r="AK79" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
+    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -19138,8 +19458,11 @@
       <c r="AJ80" s="10">
         <v>3</v>
       </c>
+      <c r="AK80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -19248,9 +19571,12 @@
       <c r="AJ81" s="10">
         <v>169</v>
       </c>
+      <c r="AK81" s="10">
+        <v>179</v>
+      </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -19358,9 +19684,12 @@
       <c r="AJ82" s="10">
         <v>151</v>
       </c>
+      <c r="AK82" s="10">
+        <v>153</v>
+      </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
+    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -19466,9 +19795,12 @@
       <c r="AJ83" s="10">
         <v>44</v>
       </c>
+      <c r="AK83" s="10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
+    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -19574,9 +19906,12 @@
       <c r="AJ84" s="10">
         <v>109</v>
       </c>
+      <c r="AK84" s="10">
+        <v>111</v>
+      </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
+    <row r="85" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -19682,9 +20017,12 @@
       <c r="AJ85" s="10">
         <v>6</v>
       </c>
+      <c r="AK85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
+    <row r="86" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -19790,9 +20128,12 @@
       <c r="AJ86" s="10">
         <v>15</v>
       </c>
+      <c r="AK86" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A87" s="30" t="s">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -19900,9 +20241,12 @@
       <c r="AJ87" s="10">
         <v>15</v>
       </c>
+      <c r="AK87" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+    <row r="88" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -20008,9 +20352,12 @@
       <c r="AJ88" s="10">
         <v>34</v>
       </c>
+      <c r="AK88" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+    <row r="89" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -20116,9 +20463,12 @@
       <c r="AJ89" s="10">
         <v>7</v>
       </c>
+      <c r="AK89" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+    <row r="90" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -20224,9 +20574,12 @@
       <c r="AJ90" s="10">
         <v>10</v>
       </c>
+      <c r="AK90" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+    <row r="91" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -20332,9 +20685,12 @@
       <c r="AJ91" s="10">
         <v>4</v>
       </c>
+      <c r="AK91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A92" s="31"/>
+    <row r="92" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -20440,9 +20796,12 @@
       <c r="AJ92" s="10">
         <v>11</v>
       </c>
+      <c r="AK92" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
+    <row r="93" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -20548,9 +20907,12 @@
       <c r="AJ93" s="10">
         <v>37</v>
       </c>
+      <c r="AK93" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -20658,9 +21020,12 @@
       <c r="AJ94" s="10">
         <v>11</v>
       </c>
+      <c r="AK94" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+    <row r="95" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -20766,8 +21131,11 @@
       <c r="AJ95" s="10">
         <v>32</v>
       </c>
+      <c r="AK95" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -20876,9 +21244,12 @@
       <c r="AJ96" s="10">
         <v>103</v>
       </c>
+      <c r="AK96" s="10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A97" s="33" t="s">
+    <row r="97" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -20986,9 +21357,12 @@
       <c r="AJ97" s="10">
         <v>1184</v>
       </c>
+      <c r="AK97" s="10">
+        <v>1265</v>
+      </c>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
+    <row r="98" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -21094,9 +21468,12 @@
       <c r="AJ98" s="10">
         <v>154</v>
       </c>
+      <c r="AK98" s="10">
+        <v>158</v>
+      </c>
     </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A99" s="35"/>
+    <row r="99" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -21202,9 +21579,12 @@
       <c r="AJ99" s="10">
         <v>44</v>
       </c>
+      <c r="AK99" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="100" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -21312,9 +21692,12 @@
       <c r="AJ100" s="10">
         <v>21</v>
       </c>
+      <c r="AK100" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+    <row r="101" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -21420,9 +21803,12 @@
       <c r="AJ101" s="10">
         <v>25</v>
       </c>
+      <c r="AK101" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+    <row r="102" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -21528,9 +21914,12 @@
       <c r="AJ102" s="10">
         <v>101</v>
       </c>
+      <c r="AK102" s="10">
+        <v>107</v>
+      </c>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+    <row r="103" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -21636,9 +22025,12 @@
       <c r="AJ103" s="10">
         <v>198</v>
       </c>
+      <c r="AK103" s="10">
+        <v>213</v>
+      </c>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
+    <row r="104" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -21744,9 +22136,12 @@
       <c r="AJ104" s="10">
         <v>23</v>
       </c>
+      <c r="AK104" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -21854,9 +22249,12 @@
       <c r="AJ105" s="10">
         <v>95</v>
       </c>
+      <c r="AK105" s="10">
+        <v>103</v>
+      </c>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
+    <row r="106" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -21962,9 +22360,12 @@
       <c r="AJ106" s="10">
         <v>80</v>
       </c>
+      <c r="AK106" s="10">
+        <v>87</v>
+      </c>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
+    <row r="107" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -22070,9 +22471,12 @@
       <c r="AJ107" s="10">
         <v>14</v>
       </c>
+      <c r="AK107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
+    <row r="108" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -22178,9 +22582,12 @@
       <c r="AJ108" s="10">
         <v>25</v>
       </c>
+      <c r="AK108" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+    <row r="109" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -22286,8 +22693,11 @@
       <c r="AJ109" s="10">
         <v>2</v>
       </c>
+      <c r="AK109" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -22396,8 +22806,11 @@
       <c r="AJ110" s="10">
         <v>287</v>
       </c>
+      <c r="AK110" s="10">
+        <v>301</v>
+      </c>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -22506,9 +22919,12 @@
       <c r="AJ111" s="10">
         <v>33</v>
       </c>
+      <c r="AK111" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
+    <row r="112" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -22616,9 +23032,12 @@
       <c r="AJ112" s="10">
         <v>14</v>
       </c>
+      <c r="AK112" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -22724,9 +23143,12 @@
       <c r="AJ113" s="10">
         <v>16</v>
       </c>
+      <c r="AK113" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A114" s="32"/>
+    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -22832,9 +23254,12 @@
       <c r="AJ114" s="10">
         <v>85</v>
       </c>
+      <c r="AK114" s="10">
+        <v>94</v>
+      </c>
     </row>
-    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A115" s="33" t="s">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -22942,9 +23367,12 @@
       <c r="AJ115" s="10">
         <v>73</v>
       </c>
+      <c r="AK115" s="10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
+    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -23050,9 +23478,12 @@
       <c r="AJ116" s="10">
         <v>72</v>
       </c>
+      <c r="AK116" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="117" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+    <row r="117" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -23158,9 +23589,12 @@
       <c r="AJ117" s="10">
         <v>10</v>
       </c>
+      <c r="AK117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
+    <row r="118" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -23266,9 +23700,12 @@
       <c r="AJ118" s="10">
         <v>39</v>
       </c>
+      <c r="AK118" s="10">
+        <v>40</v>
+      </c>
     </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -23374,9 +23811,12 @@
       <c r="AJ119" s="10">
         <v>7</v>
       </c>
+      <c r="AK119" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="120" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+    <row r="120" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -23482,9 +23922,12 @@
       <c r="AJ120" s="10">
         <v>48</v>
       </c>
+      <c r="AK120" s="10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="121" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="s">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -23592,9 +24035,12 @@
       <c r="AJ121" s="10">
         <v>4</v>
       </c>
+      <c r="AK121" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="122" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
+    <row r="122" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -23700,9 +24146,12 @@
       <c r="AJ122" s="10">
         <v>22</v>
       </c>
+      <c r="AK122" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="123" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A123" s="31"/>
+    <row r="123" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -23808,9 +24257,12 @@
       <c r="AJ123" s="10">
         <v>2</v>
       </c>
+      <c r="AK123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A124" s="31"/>
+    <row r="124" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -23916,9 +24368,12 @@
       <c r="AJ124" s="10">
         <v>5</v>
       </c>
+      <c r="AK124" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="125" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A125" s="31"/>
+    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -24024,9 +24479,12 @@
       <c r="AJ125" s="10">
         <v>1</v>
       </c>
+      <c r="AK125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A126" s="31"/>
+    <row r="126" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -24132,9 +24590,12 @@
       <c r="AJ126" s="10">
         <v>4</v>
       </c>
+      <c r="AK126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A127" s="31"/>
+    <row r="127" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -24240,9 +24701,12 @@
       <c r="AJ127" s="10">
         <v>4</v>
       </c>
+      <c r="AK127" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="128" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A128" s="31"/>
+    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -24348,9 +24812,12 @@
       <c r="AJ128" s="10">
         <v>8</v>
       </c>
+      <c r="AK128" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="129" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A129" s="31"/>
+    <row r="129" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -24456,9 +24923,12 @@
       <c r="AJ129" s="10">
         <v>79</v>
       </c>
+      <c r="AK129" s="10">
+        <v>89</v>
+      </c>
     </row>
-    <row r="130" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+    <row r="130" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -24564,8 +25034,11 @@
       <c r="AJ130" s="10">
         <v>17</v>
       </c>
+      <c r="AK130" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="131" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -24674,9 +25147,12 @@
       <c r="AJ131" s="10">
         <v>335</v>
       </c>
+      <c r="AK131" s="10">
+        <v>345</v>
+      </c>
     </row>
-    <row r="132" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="s">
+    <row r="132" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -24784,9 +25260,12 @@
       <c r="AJ132" s="10">
         <v>19</v>
       </c>
+      <c r="AK132" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="133" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A133" s="31"/>
+    <row r="133" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -24892,9 +25371,12 @@
       <c r="AJ133" s="10">
         <v>13</v>
       </c>
+      <c r="AK133" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="134" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A134" s="31"/>
+    <row r="134" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -25000,9 +25482,12 @@
       <c r="AJ134" s="10">
         <v>2</v>
       </c>
+      <c r="AK134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A135" s="32"/>
+    <row r="135" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -25108,9 +25593,12 @@
       <c r="AJ135" s="10">
         <v>0</v>
       </c>
+      <c r="AK135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="s">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -25218,9 +25706,12 @@
       <c r="AJ136" s="10">
         <v>91</v>
       </c>
+      <c r="AK136" s="10">
+        <v>93</v>
+      </c>
     </row>
-    <row r="137" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
+    <row r="137" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -25326,9 +25817,12 @@
       <c r="AJ137" s="10">
         <v>75</v>
       </c>
+      <c r="AK137" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="138" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+    <row r="138" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -25434,9 +25928,12 @@
       <c r="AJ138" s="10">
         <v>16</v>
       </c>
+      <c r="AK138" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="139" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A139" s="35"/>
+    <row r="139" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -25541,10 +26038,25 @@
       </c>
       <c r="AJ139" s="10">
         <v>141</v>
+      </c>
+      <c r="AK139" s="10">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -25557,18 +26069,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -25871,7 +26371,7 @@
       </c>
       <c r="AS2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.5378590078329</v>
       </c>
       <c r="AT2" s="18">
         <f t="shared" si="1"/>
@@ -26521,7 +27021,7 @@
       </c>
       <c r="AS4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.1549295774647899</v>
       </c>
       <c r="AT4" s="10">
         <f t="shared" si="7"/>
@@ -26846,7 +27346,7 @@
       </c>
       <c r="AS6" s="12">
         <f>MAX(0, (dc!AS2-dc!AR2))</f>
-        <v>0</v>
+        <v>766</v>
       </c>
       <c r="AT6" s="12">
         <f>MAX(0, (dc!AT2-dc!AS2))</f>
@@ -27170,7 +27670,7 @@
       </c>
       <c r="AS7" s="12">
         <f>MAX(0, (dc!AS3-dc!AR3))</f>
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="AT7" s="12">
         <f>MAX(0, (dc!AT3-dc!AS3))</f>
@@ -27818,7 +28318,7 @@
       </c>
       <c r="AS9" s="12">
         <f>MAX(0, (dc!AS5-dc!AR5))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AT9" s="12">
         <f>MAX(0, (dc!AT5-dc!AS5))</f>
@@ -28370,7 +28870,7 @@
       </c>
       <c r="AS11" s="10">
         <f>MAX(0,(dc!AS7-dc!AR7))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AT11" s="10">
         <f>MAX(0,(dc!AT7-dc!AS7))</f>
@@ -28677,7 +29177,7 @@
       </c>
       <c r="AS12" s="10">
         <f>MAX(0,(dc!AS8-dc!AR8))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AT12" s="10">
         <f>MAX(0,(dc!AT8-dc!AS8))</f>
@@ -28984,7 +29484,7 @@
       </c>
       <c r="AS13" s="10">
         <f>MAX(0,(dc!AS9-dc!AR9))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AT13" s="10">
         <f>MAX(0,(dc!AT9-dc!AS9))</f>
@@ -29291,7 +29791,7 @@
       </c>
       <c r="AS14" s="10">
         <f>MAX(0,(dc!AS10-dc!AR10))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AT14" s="10">
         <f>MAX(0,(dc!AT10-dc!AS10))</f>
@@ -29598,7 +30098,7 @@
       </c>
       <c r="AS15" s="10">
         <f>MAX(0,(dc!AS11-dc!AR11))</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AT15" s="10">
         <f>MAX(0,(dc!AT11-dc!AS11))</f>
@@ -29905,7 +30405,7 @@
       </c>
       <c r="AS16" s="10">
         <f>MAX(0,(dc!AS12-dc!AR12))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AT16" s="10">
         <f>MAX(0,(dc!AT12-dc!AS12))</f>
@@ -30212,7 +30712,7 @@
       </c>
       <c r="AS17" s="10">
         <f>MAX(0,(dc!AS13-dc!AR13))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AT17" s="10">
         <f>MAX(0,(dc!AT13-dc!AS13))</f>
@@ -30519,7 +31019,7 @@
       </c>
       <c r="AS18" s="10">
         <f>MAX(0,(dc!AS14-dc!AR14))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AT18" s="10">
         <f>MAX(0,(dc!AT14-dc!AS14))</f>
@@ -31223,7 +31723,7 @@
       </c>
       <c r="AH2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.806152214266774</v>
       </c>
       <c r="AI2" s="20">
         <f t="shared" si="0"/>
@@ -31496,7 +31996,7 @@
       </c>
       <c r="AH3" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>24.785276073619634</v>
       </c>
       <c r="AI3" s="20">
         <f t="shared" ref="AI3:BQ3" si="3">(AI8/MAX(1,AI7))*100</f>
@@ -31769,7 +32269,7 @@
       </c>
       <c r="AH4" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.6809815950920246</v>
       </c>
       <c r="AI4" s="20">
         <f t="shared" ref="AI4:BQ4" si="5">(AI9/MAX(1,AI7))*100</f>
@@ -32105,7 +32605,7 @@
       </c>
       <c r="AH6" s="14">
         <f>MAX(0,(md!AH2-md!AG2)+(md!AH3-md!AG3))</f>
-        <v>0</v>
+        <v>7542</v>
       </c>
       <c r="AI6" s="14">
         <f>MAX(0,(md!AI2-md!AH2)+(md!AI3-md!AH3))</f>
@@ -32377,7 +32877,7 @@
       </c>
       <c r="AH7" s="14">
         <f>MAX(0,(md!AH3-md!AG3))</f>
-        <v>0</v>
+        <v>815</v>
       </c>
       <c r="AI7" s="14">
         <f>MAX(0,(md!AI3-md!AH3))</f>
@@ -32649,7 +33149,7 @@
       </c>
       <c r="AH8" s="14">
         <f>MAX(0,(md!AH4-md!AG4))</f>
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="AI8" s="14">
         <f>MAX(0,(md!AI4-md!AH4))</f>
@@ -32921,7 +33421,7 @@
       </c>
       <c r="AH9" s="14">
         <f>MAX(0,(md!AH5-md!AG5))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AI9" s="14">
         <f>MAX(0,(md!AI5-md!AH5))</f>
@@ -33407,7 +33907,7 @@
       </c>
       <c r="AH11" s="14">
         <f>MAX(0,(md!AH7-md!AG7))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI11" s="14">
         <f>MAX(0,(md!AI7-md!AH7))</f>
@@ -33684,7 +34184,7 @@
       </c>
       <c r="AH12" s="14">
         <f>MAX(0,(md!AH8-md!AG8))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="AI12" s="14">
         <f>MAX(0,(md!AI8-md!AH8))</f>
@@ -33961,7 +34461,7 @@
       </c>
       <c r="AH13" s="14">
         <f>MAX(0,(md!AH9-md!AG9))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AI13" s="14">
         <f>MAX(0,(md!AI9-md!AH9))</f>
@@ -34238,7 +34738,7 @@
       </c>
       <c r="AH14" s="14">
         <f>MAX(0,(md!AH10-md!AG10))</f>
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="AI14" s="14">
         <f>MAX(0,(md!AI10-md!AH10))</f>
@@ -34515,7 +35015,7 @@
       </c>
       <c r="AH15" s="14">
         <f>MAX(0,(md!AH11-md!AG11))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI15" s="14">
         <f>MAX(0,(md!AI11-md!AH11))</f>
@@ -34792,7 +35292,7 @@
       </c>
       <c r="AH16" s="14">
         <f>MAX(0,(md!AH12-md!AG12))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI16" s="14">
         <f>MAX(0,(md!AI12-md!AH12))</f>
@@ -35069,7 +35569,7 @@
       </c>
       <c r="AH17" s="14">
         <f>MAX(0,(md!AH13-md!AG13))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI17" s="14">
         <f>MAX(0,(md!AI13-md!AH13))</f>
@@ -35346,7 +35846,7 @@
       </c>
       <c r="AH18" s="14">
         <f>MAX(0,(md!AH14-md!AG14))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI18" s="14">
         <f>MAX(0,(md!AI14-md!AH14))</f>
@@ -35623,7 +36123,7 @@
       </c>
       <c r="AH19" s="14">
         <f>MAX(0,(md!AH15-md!AG15))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AI19" s="14">
         <f>MAX(0,(md!AI15-md!AH15))</f>
@@ -35900,7 +36400,7 @@
       </c>
       <c r="AH20" s="14">
         <f>MAX(0,(md!AH16-md!AG16))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI20" s="14">
         <f>MAX(0,(md!AI16-md!AH16))</f>
@@ -36177,7 +36677,7 @@
       </c>
       <c r="AH21" s="14">
         <f>MAX(0,(md!AH17-md!AG17))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AI21" s="14">
         <f>MAX(0,(md!AI17-md!AH17))</f>
@@ -36731,7 +37231,7 @@
       </c>
       <c r="AH23" s="14">
         <f>MAX(0,(md!AH19-md!AG19))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AI23" s="14">
         <f>MAX(0,(md!AI19-md!AH19))</f>
@@ -37008,7 +37508,7 @@
       </c>
       <c r="AH24" s="14">
         <f>MAX(0,(md!AH20-md!AG20))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AI24" s="14">
         <f>MAX(0,(md!AI20-md!AH20))</f>
@@ -37285,7 +37785,7 @@
       </c>
       <c r="AH25" s="14">
         <f>MAX(0,(md!AH21-md!AG21))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI25" s="14">
         <f>MAX(0,(md!AI21-md!AH21))</f>
@@ -37562,7 +38062,7 @@
       </c>
       <c r="AH26" s="14">
         <f>MAX(0,(md!AH22-md!AG22))</f>
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="AI26" s="14">
         <f>MAX(0,(md!AI22-md!AH22))</f>
@@ -37839,7 +38339,7 @@
       </c>
       <c r="AH27" s="14">
         <f>MAX(0,(md!AH23-md!AG23))</f>
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="AI27" s="14">
         <f>MAX(0,(md!AI23-md!AH23))</f>
@@ -38116,7 +38616,7 @@
       </c>
       <c r="AH28" s="14">
         <f>MAX(0,(md!AH24-md!AG24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI28" s="14">
         <f>MAX(0,(md!AI24-md!AH24))</f>
@@ -38393,7 +38893,7 @@
       </c>
       <c r="AH29" s="14">
         <f>MAX(0,(md!AH25-md!AG25))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AI29" s="14">
         <f>MAX(0,(md!AI25-md!AH25))</f>
@@ -38670,7 +39170,7 @@
       </c>
       <c r="AH30" s="14">
         <f>MAX(0,(md!AH26-md!AG26))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI30" s="14">
         <f>MAX(0,(md!AI26-md!AH26))</f>
@@ -38947,7 +39447,7 @@
       </c>
       <c r="AH31" s="14">
         <f>MAX(0,(md!AH27-md!AG27))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AI31" s="14">
         <f>MAX(0,(md!AI27-md!AH27))</f>
@@ -39224,7 +39724,7 @@
       </c>
       <c r="AH32" s="14">
         <f>MAX(0,(md!AH28-md!AG28))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AI32" s="14">
         <f>MAX(0,(md!AI28-md!AH28))</f>
@@ -39501,7 +40001,7 @@
       </c>
       <c r="AH33" s="14">
         <f>MAX(0,(md!AH29-md!AG29))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AI33" s="14">
         <f>MAX(0,(md!AI29-md!AH29))</f>
@@ -39778,7 +40278,7 @@
       </c>
       <c r="AH34" s="14">
         <f>MAX(0,(md!AH30-md!AG30))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI34" s="14">
         <f>MAX(0,(md!AI30-md!AH30))</f>
@@ -40257,7 +40757,7 @@
       </c>
       <c r="AJ2" s="19">
         <f t="shared" ref="AJ2:BS2" si="1">(AJ7/(MAX(AJ6,1))*100)</f>
-        <v>0</v>
+        <v>15.32994923857868</v>
       </c>
       <c r="AK2" s="19">
         <f t="shared" si="1"/>
@@ -40534,7 +41034,7 @@
       </c>
       <c r="AJ3" s="19">
         <f t="shared" ref="AJ3:BS3" si="3">(AJ8/MAX(1,AJ7))*100</f>
-        <v>0</v>
+        <v>11.920529801324504</v>
       </c>
       <c r="AK3" s="19">
         <f t="shared" si="3"/>
@@ -40811,7 +41311,7 @@
       </c>
       <c r="AJ4" s="19">
         <f t="shared" ref="AJ4:BS4" si="5">(AJ9/MAX(1,AJ7))*100</f>
-        <v>0</v>
+        <v>1.9867549668874174</v>
       </c>
       <c r="AK4" s="19">
         <f t="shared" si="5"/>
@@ -41088,7 +41588,7 @@
       </c>
       <c r="AJ6" s="14">
         <f>MAX(0,(va!AK5-va!AJ5))</f>
-        <v>0</v>
+        <v>3940</v>
       </c>
       <c r="AK6" s="14">
         <f>MAX(0,(va!AL5-va!AK5))</f>
@@ -41365,7 +41865,7 @@
       </c>
       <c r="AJ7" s="14">
         <f>MAX(0,(va!AK2-va!AJ2))</f>
-        <v>0</v>
+        <v>604</v>
       </c>
       <c r="AK7" s="14">
         <f>MAX(0,(va!AL2-va!AK2))</f>
@@ -41642,7 +42142,7 @@
       </c>
       <c r="AJ8" s="14">
         <f>MAX(0,(va!AK3-va!AJ3))</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="AK8" s="14">
         <f>MAX(0,(va!AL3-va!AK3))</f>
@@ -41919,7 +42419,7 @@
       </c>
       <c r="AJ9" s="14">
         <f>MAX(0,(va!AK4-va!AJ4))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AK9" s="14">
         <f>MAX(0,(va!AL4-va!AK4))</f>
@@ -42416,7 +42916,7 @@
       </c>
       <c r="AJ11" s="16">
         <f>MAX(0,(va!AK7-va!AJ7))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AK11" s="16">
         <f>MAX(0,(va!AL7-va!AK7))</f>
@@ -44108,7 +44608,7 @@
       </c>
       <c r="AJ17" s="16">
         <f>MAX(0,(va!AK13-va!AJ13))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK17" s="16">
         <f>MAX(0,(va!AL13-va!AK13))</f>
@@ -44390,7 +44890,7 @@
       </c>
       <c r="AJ18" s="16">
         <f>MAX(0,(va!AK14-va!AJ14))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AK18" s="16">
         <f>MAX(0,(va!AL14-va!AK14))</f>
@@ -46364,7 +46864,7 @@
       </c>
       <c r="AJ25" s="16">
         <f>MAX(0,(va!AK21-va!AJ21))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK25" s="16">
         <f>MAX(0,(va!AL21-va!AK21))</f>
@@ -47774,7 +48274,7 @@
       </c>
       <c r="AJ30" s="16">
         <f>MAX(0,(va!AK26-va!AJ26))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK30" s="16">
         <f>MAX(0,(va!AL26-va!AK26))</f>
@@ -48338,7 +48838,7 @@
       </c>
       <c r="AJ32" s="16">
         <f>MAX(0,(va!AK28-va!AJ28))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK32" s="16">
         <f>MAX(0,(va!AL28-va!AK28))</f>
@@ -48620,7 +49120,7 @@
       </c>
       <c r="AJ33" s="16">
         <f>MAX(0,(va!AK29-va!AJ29))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK33" s="16">
         <f>MAX(0,(va!AL29-va!AK29))</f>
@@ -48902,7 +49402,7 @@
       </c>
       <c r="AJ34" s="16">
         <f>MAX(0,(va!AK30-va!AJ30))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK34" s="16">
         <f>MAX(0,(va!AL30-va!AK30))</f>
@@ -49184,7 +49684,7 @@
       </c>
       <c r="AJ35" s="16">
         <f>MAX(0,(va!AK31-va!AJ31))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AK35" s="16">
         <f>MAX(0,(va!AL31-va!AK31))</f>
@@ -49748,7 +50248,7 @@
       </c>
       <c r="AJ37" s="16">
         <f>MAX(0,(va!AK33-va!AJ33))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK37" s="16">
         <f>MAX(0,(va!AL33-va!AK33))</f>
@@ -50030,7 +50530,7 @@
       </c>
       <c r="AJ38" s="16">
         <f>MAX(0,(va!AK34-va!AJ34))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK38" s="16">
         <f>MAX(0,(va!AL34-va!AK34))</f>
@@ -50312,7 +50812,7 @@
       </c>
       <c r="AJ39" s="16">
         <f>MAX(0,(va!AK35-va!AJ35))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK39" s="16">
         <f>MAX(0,(va!AL35-va!AK35))</f>
@@ -50594,7 +51094,7 @@
       </c>
       <c r="AJ40" s="16">
         <f>MAX(0,(va!AK36-va!AJ36))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK40" s="16">
         <f>MAX(0,(va!AL36-va!AK36))</f>
@@ -51158,7 +51658,7 @@
       </c>
       <c r="AJ42" s="16">
         <f>MAX(0,(va!AK38-va!AJ38))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK42" s="16">
         <f>MAX(0,(va!AL38-va!AK38))</f>
@@ -52850,7 +53350,7 @@
       </c>
       <c r="AJ48" s="16">
         <f>MAX(0,(va!AK44-va!AJ44))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK48" s="16">
         <f>MAX(0,(va!AL44-va!AK44))</f>
@@ -54542,7 +55042,7 @@
       </c>
       <c r="AJ54" s="16">
         <f>MAX(0,(va!AK50-va!AJ50))</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="AK54" s="16">
         <f>MAX(0,(va!AL50-va!AK50))</f>
@@ -54824,7 +55324,7 @@
       </c>
       <c r="AJ55" s="16">
         <f>MAX(0,(va!AK51-va!AJ51))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK55" s="16">
         <f>MAX(0,(va!AL51-va!AK51))</f>
@@ -55106,7 +55606,7 @@
       </c>
       <c r="AJ56" s="16">
         <f>MAX(0,(va!AK52-va!AJ52))</f>
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="AK56" s="16">
         <f>MAX(0,(va!AL52-va!AK52))</f>
@@ -55952,7 +56452,7 @@
       </c>
       <c r="AJ59" s="16">
         <f>MAX(0,(va!AK55-va!AJ55))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK59" s="16">
         <f>MAX(0,(va!AL55-va!AK55))</f>
@@ -56234,7 +56734,7 @@
       </c>
       <c r="AJ60" s="16">
         <f>MAX(0,(va!AK56-va!AJ56))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AK60" s="16">
         <f>MAX(0,(va!AL56-va!AK56))</f>
@@ -56798,7 +57298,7 @@
       </c>
       <c r="AJ62" s="16">
         <f>MAX(0,(va!AK58-va!AJ58))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK62" s="16">
         <f>MAX(0,(va!AL58-va!AK58))</f>
@@ -58208,7 +58708,7 @@
       </c>
       <c r="AJ67" s="16">
         <f>MAX(0,(va!AK63-va!AJ63))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK67" s="16">
         <f>MAX(0,(va!AL63-va!AK63))</f>
@@ -58490,7 +58990,7 @@
       </c>
       <c r="AJ68" s="16">
         <f>MAX(0,(va!AK64-va!AJ64))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK68" s="16">
         <f>MAX(0,(va!AL64-va!AK64))</f>
@@ -58772,7 +59272,7 @@
       </c>
       <c r="AJ69" s="16">
         <f>MAX(0,(va!AK65-va!AJ65))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK69" s="16">
         <f>MAX(0,(va!AL65-va!AK65))</f>
@@ -59336,7 +59836,7 @@
       </c>
       <c r="AJ71" s="16">
         <f>MAX(0,(va!AK67-va!AJ67))</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AK71" s="16">
         <f>MAX(0,(va!AL67-va!AK67))</f>
@@ -60746,7 +61246,7 @@
       </c>
       <c r="AJ76" s="16">
         <f>MAX(0,(va!AK72-va!AJ72))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK76" s="16">
         <f>MAX(0,(va!AL72-va!AK72))</f>
@@ -61592,7 +62092,7 @@
       </c>
       <c r="AJ79" s="16">
         <f>MAX(0,(va!AK75-va!AJ75))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK79" s="16">
         <f>MAX(0,(va!AL75-va!AK75))</f>
@@ -63284,7 +63784,7 @@
       </c>
       <c r="AJ85" s="16">
         <f>MAX(0,(va!AK81-va!AJ81))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK85" s="16">
         <f>MAX(0,(va!AL81-va!AK81))</f>
@@ -63566,7 +64066,7 @@
       </c>
       <c r="AJ86" s="16">
         <f>MAX(0,(va!AK82-va!AJ82))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK86" s="16">
         <f>MAX(0,(va!AL82-va!AK82))</f>
@@ -64130,7 +64630,7 @@
       </c>
       <c r="AJ88" s="16">
         <f>MAX(0,(va!AK84-va!AJ84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK88" s="16">
         <f>MAX(0,(va!AL84-va!AK84))</f>
@@ -65258,7 +65758,7 @@
       </c>
       <c r="AJ92" s="16">
         <f>MAX(0,(va!AK88-va!AJ88))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK92" s="16">
         <f>MAX(0,(va!AL88-va!AK88))</f>
@@ -66668,7 +67168,7 @@
       </c>
       <c r="AJ97" s="16">
         <f>MAX(0,(va!AK93-va!AJ93))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK97" s="16">
         <f>MAX(0,(va!AL93-va!AK93))</f>
@@ -67232,7 +67732,7 @@
       </c>
       <c r="AJ99" s="16">
         <f>MAX(0,(va!AK95-va!AJ95))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK99" s="16">
         <f>MAX(0,(va!AL95-va!AK95))</f>
@@ -67514,7 +68014,7 @@
       </c>
       <c r="AJ100" s="16">
         <f>MAX(0,(va!AK96-va!AJ96))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK100" s="16">
         <f>MAX(0,(va!AL96-va!AK96))</f>
@@ -67796,7 +68296,7 @@
       </c>
       <c r="AJ101" s="16">
         <f>MAX(0,(va!AK97-va!AJ97))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="AK101" s="16">
         <f>MAX(0,(va!AL97-va!AK97))</f>
@@ -68078,7 +68578,7 @@
       </c>
       <c r="AJ102" s="16">
         <f>MAX(0,(va!AK98-va!AJ98))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK102" s="16">
         <f>MAX(0,(va!AL98-va!AK98))</f>
@@ -68360,7 +68860,7 @@
       </c>
       <c r="AJ103" s="16">
         <f>MAX(0,(va!AK99-va!AJ99))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK103" s="16">
         <f>MAX(0,(va!AL99-va!AK99))</f>
@@ -68924,7 +69424,7 @@
       </c>
       <c r="AJ105" s="16">
         <f>MAX(0,(va!AK101-va!AJ101))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK105" s="16">
         <f>MAX(0,(va!AL101-va!AK101))</f>
@@ -69206,7 +69706,7 @@
       </c>
       <c r="AJ106" s="16">
         <f>MAX(0,(va!AK102-va!AJ102))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK106" s="16">
         <f>MAX(0,(va!AL102-va!AK102))</f>
@@ -69488,7 +69988,7 @@
       </c>
       <c r="AJ107" s="16">
         <f>MAX(0,(va!AK103-va!AJ103))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AK107" s="16">
         <f>MAX(0,(va!AL103-va!AK103))</f>
@@ -70052,7 +70552,7 @@
       </c>
       <c r="AJ109" s="16">
         <f>MAX(0,(va!AK105-va!AJ105))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK109" s="16">
         <f>MAX(0,(va!AL105-va!AK105))</f>
@@ -70334,7 +70834,7 @@
       </c>
       <c r="AJ110" s="16">
         <f>MAX(0,(va!AK106-va!AJ106))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK110" s="16">
         <f>MAX(0,(va!AL106-va!AK106))</f>
@@ -70898,7 +71398,7 @@
       </c>
       <c r="AJ112" s="16">
         <f>MAX(0,(va!AK108-va!AJ108))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK112" s="16">
         <f>MAX(0,(va!AL108-va!AK108))</f>
@@ -71462,7 +71962,7 @@
       </c>
       <c r="AJ114" s="16">
         <f>MAX(0,(va!AK110-va!AJ110))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AK114" s="16">
         <f>MAX(0,(va!AL110-va!AK110))</f>
@@ -72308,7 +72808,7 @@
       </c>
       <c r="AJ117" s="16">
         <f>MAX(0,(va!AK113-va!AJ113))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK117" s="16">
         <f>MAX(0,(va!AL113-va!AK113))</f>
@@ -72590,7 +73090,7 @@
       </c>
       <c r="AJ118" s="16">
         <f>MAX(0,(va!AK114-va!AJ114))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK118" s="16">
         <f>MAX(0,(va!AL114-va!AK114))</f>
@@ -72872,7 +73372,7 @@
       </c>
       <c r="AJ119" s="16">
         <f>MAX(0,(va!AK115-va!AJ115))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK119" s="16">
         <f>MAX(0,(va!AL115-va!AK115))</f>
@@ -73718,7 +74218,7 @@
       </c>
       <c r="AJ122" s="16">
         <f>MAX(0,(va!AK118-va!AJ118))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK122" s="16">
         <f>MAX(0,(va!AL118-va!AK118))</f>
@@ -74282,7 +74782,7 @@
       </c>
       <c r="AJ124" s="16">
         <f>MAX(0,(va!AK120-va!AJ120))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK124" s="16">
         <f>MAX(0,(va!AL120-va!AK120))</f>
@@ -74564,7 +75064,7 @@
       </c>
       <c r="AJ125" s="16">
         <f>MAX(0,(va!AK121-va!AJ121))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK125" s="16">
         <f>MAX(0,(va!AL121-va!AK121))</f>
@@ -76820,7 +77320,7 @@
       </c>
       <c r="AJ133" s="16">
         <f>MAX(0,(va!AK129-va!AJ129))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK133" s="16">
         <f>MAX(0,(va!AL129-va!AK129))</f>
@@ -77102,7 +77602,7 @@
       </c>
       <c r="AJ134" s="16">
         <f>MAX(0,(va!AK130-va!AJ130))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK134" s="16">
         <f>MAX(0,(va!AL130-va!AK130))</f>
@@ -77384,7 +77884,7 @@
       </c>
       <c r="AJ135" s="16">
         <f>MAX(0,(va!AK131-va!AJ131))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK135" s="16">
         <f>MAX(0,(va!AL131-va!AK131))</f>
@@ -77948,7 +78448,7 @@
       </c>
       <c r="AJ137" s="16">
         <f>MAX(0,(va!AK133-va!AJ133))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK137" s="16">
         <f>MAX(0,(va!AL133-va!AK133))</f>
@@ -78794,7 +79294,7 @@
       </c>
       <c r="AJ140" s="16">
         <f>MAX(0,(va!AK136-va!AJ136))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK140" s="16">
         <f>MAX(0,(va!AL136-va!AK136))</f>
@@ -79076,7 +79576,7 @@
       </c>
       <c r="AJ141" s="16">
         <f>MAX(0,(va!AK137-va!AJ137))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AK141" s="16">
         <f>MAX(0,(va!AL137-va!AK137))</f>
@@ -79640,7 +80140,7 @@
       </c>
       <c r="AJ143" s="16">
         <f>MAX(0,(va!AK139-va!AJ139))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK143" s="16">
         <f>MAX(0,(va!AL139-va!AK139))</f>

</xml_diff>

<commit_message>
27 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C194E-021B-4465-BE29-94CE3D458442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DF7625-0695-4C6D-89B7-C03D9EF17B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="5400" yWindow="4005" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4018,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AS2" sqref="AS2"/>
+      <selection pane="bottomRight" activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4170,6 +4170,9 @@
       <c r="AS2" s="12">
         <v>18068</v>
       </c>
+      <c r="AT2" s="12">
+        <v>18416</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4338,7 +4341,7 @@
       </c>
       <c r="AT3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3892</v>
       </c>
       <c r="AU3" s="10">
         <f t="shared" si="0"/>
@@ -4622,6 +4625,9 @@
       <c r="AS5" s="10">
         <v>178</v>
       </c>
+      <c r="AT5" s="10">
+        <v>185</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5004,6 +5010,9 @@
       <c r="AS7" s="10">
         <v>444</v>
       </c>
+      <c r="AT7" s="10">
+        <v>450</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5141,6 +5150,9 @@
       <c r="AS8" s="10">
         <v>261</v>
       </c>
+      <c r="AT8" s="10">
+        <v>261</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5278,6 +5290,9 @@
       <c r="AS9" s="10">
         <v>268</v>
       </c>
+      <c r="AT9" s="10">
+        <v>261</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5415,6 +5430,9 @@
       <c r="AS10" s="10">
         <v>663</v>
       </c>
+      <c r="AT10" s="10">
+        <v>681</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5552,6 +5570,9 @@
       <c r="AS11" s="10">
         <v>552</v>
       </c>
+      <c r="AT11" s="10">
+        <v>571</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5689,6 +5710,9 @@
       <c r="AS12" s="10">
         <v>419</v>
       </c>
+      <c r="AT12" s="10">
+        <v>405</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5826,6 +5850,9 @@
       <c r="AS13" s="10">
         <v>570</v>
       </c>
+      <c r="AT13" s="10">
+        <v>578</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -5963,6 +5990,9 @@
       <c r="AS14" s="10">
         <v>530</v>
       </c>
+      <c r="AT14" s="10">
+        <v>535</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6099,6 +6129,9 @@
       </c>
       <c r="AS15" s="10">
         <v>134</v>
+      </c>
+      <c r="AT15" s="10">
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6473,7 +6506,7 @@
         <v>78084</v>
       </c>
       <c r="AI2" s="10">
-        <v>0</v>
+        <v>85489</v>
       </c>
       <c r="AJ2" s="10">
         <v>0</v>
@@ -6711,7 +6744,7 @@
       </c>
       <c r="AI3" s="10">
         <f>SUM(md[27-Apr])</f>
-        <v>0</v>
+        <v>19487</v>
       </c>
       <c r="AJ3" s="10">
         <f>SUM(md[28-Apr])</f>
@@ -6951,7 +6984,7 @@
         <v>3962</v>
       </c>
       <c r="AI4" s="10">
-        <v>0</v>
+        <v>4101</v>
       </c>
       <c r="AJ4" s="10">
         <v>0</v>
@@ -7157,7 +7190,7 @@
         <v>827</v>
       </c>
       <c r="AI5" s="10">
-        <v>0</v>
+        <v>858</v>
       </c>
       <c r="AJ5" s="10">
         <v>0</v>
@@ -7574,6 +7607,9 @@
       <c r="AH7">
         <v>113</v>
       </c>
+      <c r="AI7">
+        <v>114</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7678,6 +7714,9 @@
       <c r="AH8" s="10">
         <v>1510</v>
       </c>
+      <c r="AI8" s="10">
+        <v>1544</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7782,6 +7821,9 @@
       <c r="AH9">
         <v>1866</v>
       </c>
+      <c r="AI9">
+        <v>1933</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7886,6 +7928,9 @@
       <c r="AH10">
         <v>2509</v>
       </c>
+      <c r="AI10">
+        <v>2548</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -7990,6 +8035,9 @@
       <c r="AH11">
         <v>134</v>
       </c>
+      <c r="AI11">
+        <v>138</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8094,6 +8142,9 @@
       <c r="AH12">
         <v>63</v>
       </c>
+      <c r="AI12">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8198,6 +8249,9 @@
       <c r="AH13">
         <v>391</v>
       </c>
+      <c r="AI13">
+        <v>403</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8302,6 +8356,9 @@
       <c r="AH14">
         <v>154</v>
       </c>
+      <c r="AI14">
+        <v>163</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8406,6 +8463,9 @@
       <c r="AH15">
         <v>504</v>
       </c>
+      <c r="AI15">
+        <v>529</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8510,8 +8570,11 @@
       <c r="AH16" s="10">
         <v>46</v>
       </c>
+      <c r="AI16" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8614,8 +8677,11 @@
       <c r="AH17">
         <v>834</v>
       </c>
+      <c r="AI17">
+        <v>865</v>
+      </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8718,8 +8784,11 @@
       <c r="AH18">
         <v>4</v>
       </c>
+      <c r="AI18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8822,8 +8891,11 @@
       <c r="AH19">
         <v>319</v>
       </c>
+      <c r="AI19">
+        <v>352</v>
+      </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -8926,8 +8998,11 @@
       <c r="AH20">
         <v>707</v>
       </c>
+      <c r="AI20">
+        <v>778</v>
+      </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9030,8 +9105,11 @@
       <c r="AH21">
         <v>68</v>
       </c>
+      <c r="AI21">
+        <v>70</v>
+      </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9134,8 +9212,11 @@
       <c r="AH22">
         <v>3645</v>
       </c>
+      <c r="AI22">
+        <v>3843</v>
+      </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9238,8 +9319,11 @@
       <c r="AH23">
         <v>4987</v>
       </c>
+      <c r="AI23">
+        <v>5263</v>
+      </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9342,8 +9426,11 @@
       <c r="AH24">
         <v>53</v>
       </c>
+      <c r="AI24">
+        <v>54</v>
+      </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9446,8 +9533,11 @@
       <c r="AH25">
         <v>133</v>
       </c>
+      <c r="AI25">
+        <v>144</v>
+      </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9550,8 +9640,11 @@
       <c r="AH26">
         <v>16</v>
       </c>
+      <c r="AI26">
+        <v>19</v>
+      </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -9654,8 +9747,11 @@
       <c r="AH27">
         <v>34</v>
       </c>
+      <c r="AI27">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -9758,8 +9854,11 @@
       <c r="AH28">
         <v>173</v>
       </c>
+      <c r="AI28">
+        <v>181</v>
+      </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -9862,8 +9961,11 @@
       <c r="AH29">
         <v>270</v>
       </c>
+      <c r="AI29">
+        <v>336</v>
+      </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -9966,8 +10068,11 @@
       <c r="AH30">
         <v>48</v>
       </c>
+      <c r="AI30">
+        <v>53</v>
+      </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10061,10 +10166,10 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="Q6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="U35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AK3" sqref="AK3"/>
+      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10226,7 +10331,7 @@
       </c>
       <c r="AL2" s="10">
         <f>SUM(va[27-Apr])</f>
-        <v>0</v>
+        <v>13535</v>
       </c>
       <c r="AM2" s="10">
         <f>SUM(va[28-Apr])</f>
@@ -10469,7 +10574,7 @@
         <v>2014</v>
       </c>
       <c r="AL3" s="10">
-        <v>0</v>
+        <v>2066</v>
       </c>
       <c r="AM3" s="10">
         <v>0</v>
@@ -10678,7 +10783,7 @@
         <v>448</v>
       </c>
       <c r="AL4" s="10">
-        <v>0</v>
+        <v>458</v>
       </c>
       <c r="AM4" s="10">
         <v>0</v>
@@ -10887,7 +10992,7 @@
         <v>76118</v>
       </c>
       <c r="AL5" s="10">
-        <v>0</v>
+        <v>80180</v>
       </c>
       <c r="AM5" s="10">
         <v>0</v>
@@ -11322,9 +11427,12 @@
       <c r="AK7" s="10">
         <v>591</v>
       </c>
+      <c r="AL7" s="10">
+        <v>627</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11435,9 +11543,12 @@
       <c r="AK8" s="10">
         <v>5</v>
       </c>
+      <c r="AL8" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11546,9 +11657,12 @@
       <c r="AK9" s="10">
         <v>27</v>
       </c>
+      <c r="AL9" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -11657,9 +11771,12 @@
       <c r="AK10" s="10">
         <v>2</v>
       </c>
+      <c r="AL10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -11768,9 +11885,12 @@
       <c r="AK11" s="10">
         <v>39</v>
       </c>
+      <c r="AL11" s="10">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -11879,9 +11999,12 @@
       <c r="AK12" s="10">
         <v>1</v>
       </c>
+      <c r="AL12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -11989,6 +12112,9 @@
       </c>
       <c r="AK13" s="10">
         <v>9</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
@@ -12103,9 +12229,12 @@
       <c r="AK14" s="10">
         <v>790</v>
       </c>
+      <c r="AL14" s="10">
+        <v>836</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12216,9 +12345,12 @@
       <c r="AK15" s="10">
         <v>36</v>
       </c>
+      <c r="AL15" s="10">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -12327,9 +12459,12 @@
       <c r="AK16" s="10">
         <v>0</v>
       </c>
+      <c r="AL16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12438,9 +12573,12 @@
       <c r="AK17" s="10">
         <v>1</v>
       </c>
+      <c r="AL17" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -12549,9 +12687,12 @@
       <c r="AK18" s="10">
         <v>5</v>
       </c>
+      <c r="AL18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -12660,9 +12801,12 @@
       <c r="AK19" s="10">
         <v>184</v>
       </c>
+      <c r="AL19" s="10">
+        <v>193</v>
+      </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -12771,9 +12915,12 @@
       <c r="AK20" s="10">
         <v>5</v>
       </c>
+      <c r="AL20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -12882,9 +13029,12 @@
       <c r="AK21" s="10">
         <v>371</v>
       </c>
+      <c r="AL21" s="10">
+        <v>383</v>
+      </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -12993,9 +13143,12 @@
       <c r="AK22" s="10">
         <v>3</v>
       </c>
+      <c r="AL22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -13104,9 +13257,12 @@
       <c r="AK23" s="10">
         <v>10</v>
       </c>
+      <c r="AL23" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -13215,9 +13371,12 @@
       <c r="AK24" s="10">
         <v>10</v>
       </c>
+      <c r="AL24" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -13328,9 +13487,12 @@
       <c r="AK25" s="10">
         <v>9</v>
       </c>
+      <c r="AL25" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -13439,9 +13601,12 @@
       <c r="AK26" s="10">
         <v>17</v>
       </c>
+      <c r="AL26" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -13550,9 +13715,12 @@
       <c r="AK27" s="10">
         <v>24</v>
       </c>
+      <c r="AL27" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -13661,9 +13829,12 @@
       <c r="AK28" s="10">
         <v>11</v>
       </c>
+      <c r="AL28" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -13772,8 +13943,11 @@
       <c r="AK29" s="10">
         <v>50</v>
       </c>
+      <c r="AL29" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -13885,9 +14059,12 @@
       <c r="AK30" s="10">
         <v>208</v>
       </c>
+      <c r="AL30" s="10">
+        <v>214</v>
+      </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -13998,9 +14175,12 @@
       <c r="AK31" s="10">
         <v>457</v>
       </c>
+      <c r="AL31" s="10">
+        <v>457</v>
+      </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -14109,9 +14289,12 @@
       <c r="AK32" s="10">
         <v>11</v>
       </c>
+      <c r="AL32" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -14220,9 +14403,12 @@
       <c r="AK33" s="10">
         <v>45</v>
       </c>
+      <c r="AL33" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -14333,9 +14519,12 @@
       <c r="AK34" s="10">
         <v>13</v>
       </c>
+      <c r="AL34" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -14444,9 +14633,12 @@
       <c r="AK35" s="10">
         <v>70</v>
       </c>
+      <c r="AL35" s="10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -14555,9 +14747,12 @@
       <c r="AK36" s="10">
         <v>105</v>
       </c>
+      <c r="AL36" s="10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -14666,9 +14861,12 @@
       <c r="AK37" s="10">
         <v>20</v>
       </c>
+      <c r="AL37" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -14779,9 +14977,12 @@
       <c r="AK38" s="10">
         <v>14</v>
       </c>
+      <c r="AL38" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -14890,9 +15091,12 @@
       <c r="AK39" s="10">
         <v>30</v>
       </c>
+      <c r="AL39" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -15001,9 +15205,12 @@
       <c r="AK40" s="10">
         <v>30</v>
       </c>
+      <c r="AL40" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -15112,9 +15319,12 @@
       <c r="AK41" s="10">
         <v>4</v>
       </c>
+      <c r="AL41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -15223,9 +15433,12 @@
       <c r="AK42" s="10">
         <v>28</v>
       </c>
+      <c r="AL42" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -15334,9 +15547,12 @@
       <c r="AK43" s="10">
         <v>18</v>
       </c>
+      <c r="AL43" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -15445,9 +15661,12 @@
       <c r="AK44" s="10">
         <v>22</v>
       </c>
+      <c r="AL44" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -15556,9 +15775,12 @@
       <c r="AK45" s="10">
         <v>27</v>
       </c>
+      <c r="AL45" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -15669,9 +15891,12 @@
       <c r="AK46" s="10">
         <v>13</v>
       </c>
+      <c r="AL46" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -15780,9 +16005,12 @@
       <c r="AK47" s="10">
         <v>0</v>
       </c>
+      <c r="AL47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -15891,9 +16119,12 @@
       <c r="AK48" s="10">
         <v>3</v>
       </c>
+      <c r="AL48" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -16002,9 +16233,12 @@
       <c r="AK49" s="10">
         <v>4</v>
       </c>
+      <c r="AL49" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -16115,9 +16349,12 @@
       <c r="AK50" s="10">
         <v>187</v>
       </c>
+      <c r="AL50" s="10">
+        <v>195</v>
+      </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -16226,9 +16463,12 @@
       <c r="AK51" s="10">
         <v>24</v>
       </c>
+      <c r="AL51" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -16339,9 +16579,12 @@
       <c r="AK52" s="10">
         <v>2889</v>
       </c>
+      <c r="AL52" s="10">
+        <v>3002</v>
+      </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -16450,9 +16693,12 @@
       <c r="AK53" s="10">
         <v>26</v>
       </c>
+      <c r="AL53" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A54" s="32"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -16561,8 +16807,11 @@
       <c r="AK54" s="10">
         <v>26</v>
       </c>
+      <c r="AL54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -16674,8 +16923,11 @@
       <c r="AK55" s="10">
         <v>104</v>
       </c>
+      <c r="AL55" s="10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -16787,9 +17039,12 @@
       <c r="AK56" s="10">
         <v>792</v>
       </c>
+      <c r="AL56" s="10">
+        <v>817</v>
+      </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -16900,9 +17155,12 @@
       <c r="AK57" s="10">
         <v>8</v>
       </c>
+      <c r="AL57" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -17011,9 +17269,12 @@
       <c r="AK58" s="10">
         <v>6</v>
       </c>
+      <c r="AL58" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -17122,9 +17383,12 @@
       <c r="AK59" s="10">
         <v>20</v>
       </c>
+      <c r="AL59" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -17233,9 +17497,12 @@
       <c r="AK60" s="10">
         <v>2</v>
       </c>
+      <c r="AL60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -17346,9 +17613,12 @@
       <c r="AK61" s="10">
         <v>7</v>
       </c>
+      <c r="AL61" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -17457,9 +17727,12 @@
       <c r="AK62" s="10">
         <v>93</v>
       </c>
+      <c r="AL62" s="10">
+        <v>95</v>
+      </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -17568,9 +17841,12 @@
       <c r="AK63" s="10">
         <v>84</v>
       </c>
+      <c r="AL63" s="10">
+        <v>87</v>
+      </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -17679,9 +17955,12 @@
       <c r="AK64" s="10">
         <v>74</v>
       </c>
+      <c r="AL64" s="10">
+        <v>78</v>
+      </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -17790,9 +18069,12 @@
       <c r="AK65" s="10">
         <v>43</v>
       </c>
+      <c r="AL65" s="10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A66" s="32"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -17901,8 +18183,11 @@
       <c r="AK66" s="10">
         <v>33</v>
       </c>
+      <c r="AL66" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -18014,9 +18299,12 @@
       <c r="AK67" s="10">
         <v>596</v>
       </c>
+      <c r="AL67" s="10">
+        <v>628</v>
+      </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -18127,9 +18415,12 @@
       <c r="AK68" s="10">
         <v>0</v>
       </c>
+      <c r="AL68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -18238,9 +18529,12 @@
       <c r="AK69" s="10">
         <v>3</v>
       </c>
+      <c r="AL69" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -18349,9 +18643,12 @@
       <c r="AK70" s="10">
         <v>0</v>
       </c>
+      <c r="AL70" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A71" s="31"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -18460,9 +18757,12 @@
       <c r="AK71" s="10">
         <v>13</v>
       </c>
+      <c r="AL71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A72" s="31"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -18571,9 +18871,12 @@
       <c r="AK72" s="10">
         <v>34</v>
       </c>
+      <c r="AL72" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A73" s="31"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -18682,9 +18985,12 @@
       <c r="AK73" s="10">
         <v>11</v>
       </c>
+      <c r="AL73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
+    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A74" s="31"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -18793,9 +19099,12 @@
       <c r="AK74" s="10">
         <v>1</v>
       </c>
+      <c r="AL74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A75" s="32"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -18904,9 +19213,12 @@
       <c r="AK75" s="10">
         <v>4</v>
       </c>
+      <c r="AL75" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A76" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -19017,9 +19329,12 @@
       <c r="AK76" s="10">
         <v>1</v>
       </c>
+      <c r="AL76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A77" s="34"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -19128,9 +19443,12 @@
       <c r="AK77" s="10">
         <v>4</v>
       </c>
+      <c r="AL77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
+    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A78" s="34"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -19239,9 +19557,12 @@
       <c r="AK78" s="10">
         <v>51</v>
       </c>
+      <c r="AL78" s="10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
+    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A79" s="34"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -19350,9 +19671,12 @@
       <c r="AK79" s="10">
         <v>10</v>
       </c>
+      <c r="AL79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -19461,8 +19785,11 @@
       <c r="AK80" s="10">
         <v>3</v>
       </c>
+      <c r="AL80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -19574,9 +19901,12 @@
       <c r="AK81" s="10">
         <v>179</v>
       </c>
+      <c r="AL81" s="10">
+        <v>184</v>
+      </c>
     </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A82" s="30" t="s">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -19687,9 +20017,12 @@
       <c r="AK82" s="10">
         <v>153</v>
       </c>
+      <c r="AL82" s="10">
+        <v>154</v>
+      </c>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
+    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A83" s="34"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -19798,9 +20131,12 @@
       <c r="AK83" s="10">
         <v>44</v>
       </c>
+      <c r="AL83" s="10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A84" s="34"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -19909,9 +20245,12 @@
       <c r="AK84" s="10">
         <v>111</v>
       </c>
+      <c r="AL84" s="10">
+        <v>112</v>
+      </c>
     </row>
-    <row r="85" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A85" s="34"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -20020,9 +20359,12 @@
       <c r="AK85" s="10">
         <v>6</v>
       </c>
+      <c r="AL85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
+    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A86" s="35"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -20131,9 +20473,12 @@
       <c r="AK86" s="10">
         <v>15</v>
       </c>
+      <c r="AL86" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="87" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A87" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -20244,9 +20589,12 @@
       <c r="AK87" s="10">
         <v>15</v>
       </c>
+      <c r="AL87" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="88" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -20355,9 +20703,12 @@
       <c r="AK88" s="10">
         <v>35</v>
       </c>
+      <c r="AL88" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="89" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
+    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -20466,9 +20817,12 @@
       <c r="AK89" s="10">
         <v>7</v>
       </c>
+      <c r="AL89" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="90" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
+    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -20577,9 +20931,12 @@
       <c r="AK90" s="10">
         <v>10</v>
       </c>
+      <c r="AL90" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="91" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
+    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -20688,9 +21045,12 @@
       <c r="AK91" s="10">
         <v>4</v>
       </c>
+      <c r="AL91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
+    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -20799,9 +21159,12 @@
       <c r="AK92" s="10">
         <v>11</v>
       </c>
+      <c r="AL92" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="93" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A93" s="32"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -20910,9 +21273,12 @@
       <c r="AK93" s="10">
         <v>41</v>
       </c>
+      <c r="AL93" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="94" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -21023,9 +21389,12 @@
       <c r="AK94" s="10">
         <v>11</v>
       </c>
+      <c r="AL94" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="95" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
+    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A95" s="35"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -21134,8 +21503,11 @@
       <c r="AK95" s="10">
         <v>33</v>
       </c>
+      <c r="AL95" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="96" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -21247,9 +21619,12 @@
       <c r="AK96" s="10">
         <v>108</v>
       </c>
+      <c r="AL96" s="10">
+        <v>114</v>
+      </c>
     </row>
-    <row r="97" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A97" s="33" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -21360,9 +21735,12 @@
       <c r="AK97" s="10">
         <v>1265</v>
       </c>
+      <c r="AL97" s="10">
+        <v>1353</v>
+      </c>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A98" s="34"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -21471,9 +21849,12 @@
       <c r="AK98" s="10">
         <v>158</v>
       </c>
+      <c r="AL98" s="10">
+        <v>165</v>
+      </c>
     </row>
-    <row r="99" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
+    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A99" s="35"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -21582,9 +21963,12 @@
       <c r="AK99" s="10">
         <v>45</v>
       </c>
+      <c r="AL99" s="10">
+        <v>50</v>
+      </c>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A100" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -21695,9 +22079,12 @@
       <c r="AK100" s="10">
         <v>21</v>
       </c>
+      <c r="AL100" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="101" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
+    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -21806,9 +22193,12 @@
       <c r="AK101" s="10">
         <v>27</v>
       </c>
+      <c r="AL101" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="102" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
+    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -21917,9 +22307,12 @@
       <c r="AK102" s="10">
         <v>107</v>
       </c>
+      <c r="AL102" s="10">
+        <v>119</v>
+      </c>
     </row>
-    <row r="103" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
+    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -22028,9 +22421,12 @@
       <c r="AK103" s="10">
         <v>213</v>
       </c>
+      <c r="AL103" s="10">
+        <v>218</v>
+      </c>
     </row>
-    <row r="104" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
+    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A104" s="32"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -22139,9 +22535,12 @@
       <c r="AK104" s="10">
         <v>23</v>
       </c>
+      <c r="AL104" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A105" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -22252,9 +22651,12 @@
       <c r="AK105" s="10">
         <v>103</v>
       </c>
+      <c r="AL105" s="10">
+        <v>113</v>
+      </c>
     </row>
-    <row r="106" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A106" s="34"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -22363,9 +22765,12 @@
       <c r="AK106" s="10">
         <v>87</v>
       </c>
+      <c r="AL106" s="10">
+        <v>96</v>
+      </c>
     </row>
-    <row r="107" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A107" s="34"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -22474,9 +22879,12 @@
       <c r="AK107" s="10">
         <v>14</v>
       </c>
+      <c r="AL107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A108" s="34"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -22585,9 +22993,12 @@
       <c r="AK108" s="10">
         <v>26</v>
       </c>
+      <c r="AL108" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="109" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A109" s="32"/>
+    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A109" s="35"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -22696,8 +23107,11 @@
       <c r="AK109" s="10">
         <v>2</v>
       </c>
+      <c r="AL109" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -22809,8 +23223,11 @@
       <c r="AK110" s="10">
         <v>301</v>
       </c>
+      <c r="AL110" s="10">
+        <v>304</v>
+      </c>
     </row>
-    <row r="111" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -22922,9 +23339,12 @@
       <c r="AK111" s="10">
         <v>33</v>
       </c>
+      <c r="AL111" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="112" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A112" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -23035,9 +23455,12 @@
       <c r="AK112" s="10">
         <v>14</v>
       </c>
+      <c r="AL112" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -23146,9 +23569,12 @@
       <c r="AK113" s="10">
         <v>17</v>
       </c>
+      <c r="AL113" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A114" s="32"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -23257,9 +23683,12 @@
       <c r="AK114" s="10">
         <v>94</v>
       </c>
+      <c r="AL114" s="10">
+        <v>98</v>
+      </c>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A115" s="30" t="s">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A115" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -23370,9 +23799,12 @@
       <c r="AK115" s="10">
         <v>76</v>
       </c>
+      <c r="AL115" s="10">
+        <v>77</v>
+      </c>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A116" s="31"/>
+    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A116" s="34"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -23481,9 +23913,12 @@
       <c r="AK116" s="10">
         <v>72</v>
       </c>
+      <c r="AL116" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="117" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
+    <row r="117" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A117" s="34"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -23592,9 +24027,12 @@
       <c r="AK117" s="10">
         <v>10</v>
       </c>
+      <c r="AL117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
+    <row r="118" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A118" s="34"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -23703,9 +24141,12 @@
       <c r="AK118" s="10">
         <v>40</v>
       </c>
+      <c r="AL118" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
+    <row r="119" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A119" s="34"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -23814,9 +24255,12 @@
       <c r="AK119" s="10">
         <v>7</v>
       </c>
+      <c r="AL119" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="120" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A120" s="35"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -23925,9 +24369,12 @@
       <c r="AK120" s="10">
         <v>49</v>
       </c>
+      <c r="AL120" s="10">
+        <v>50</v>
+      </c>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A121" s="33" t="s">
+    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A121" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -24038,9 +24485,12 @@
       <c r="AK121" s="10">
         <v>6</v>
       </c>
+      <c r="AL121" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
+    <row r="122" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -24149,9 +24599,12 @@
       <c r="AK122" s="10">
         <v>22</v>
       </c>
+      <c r="AL122" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="123" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+    <row r="123" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -24260,9 +24713,12 @@
       <c r="AK123" s="10">
         <v>2</v>
       </c>
+      <c r="AL123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+    <row r="124" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -24371,9 +24827,12 @@
       <c r="AK124" s="10">
         <v>5</v>
       </c>
+      <c r="AL124" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
+    <row r="125" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -24482,9 +24941,12 @@
       <c r="AK125" s="10">
         <v>1</v>
       </c>
+      <c r="AL125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+    <row r="126" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -24593,9 +25055,12 @@
       <c r="AK126" s="10">
         <v>4</v>
       </c>
+      <c r="AL126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+    <row r="127" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -24704,9 +25169,12 @@
       <c r="AK127" s="10">
         <v>4</v>
       </c>
+      <c r="AL127" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
+    <row r="128" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -24815,9 +25283,12 @@
       <c r="AK128" s="10">
         <v>8</v>
       </c>
+      <c r="AL128" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="129" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+    <row r="129" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A129" s="31"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -24926,9 +25397,12 @@
       <c r="AK129" s="10">
         <v>89</v>
       </c>
+      <c r="AL129" s="10">
+        <v>132</v>
+      </c>
     </row>
-    <row r="130" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+    <row r="130" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A130" s="32"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -25037,8 +25511,11 @@
       <c r="AK130" s="10">
         <v>20</v>
       </c>
+      <c r="AL130" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="131" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -25150,9 +25627,12 @@
       <c r="AK131" s="10">
         <v>345</v>
       </c>
+      <c r="AL131" s="10">
+        <v>355</v>
+      </c>
     </row>
-    <row r="132" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A132" s="33" t="s">
+    <row r="132" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A132" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -25263,9 +25743,12 @@
       <c r="AK132" s="10">
         <v>19</v>
       </c>
+      <c r="AL132" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="133" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+    <row r="133" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A133" s="31"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -25374,9 +25857,12 @@
       <c r="AK133" s="10">
         <v>14</v>
       </c>
+      <c r="AL133" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="134" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+    <row r="134" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A134" s="31"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -25485,9 +25971,12 @@
       <c r="AK134" s="10">
         <v>2</v>
       </c>
+      <c r="AL134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A135" s="35"/>
+    <row r="135" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A135" s="32"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -25596,9 +26085,12 @@
       <c r="AK135" s="10">
         <v>0</v>
       </c>
+      <c r="AL135" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+    <row r="136" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A136" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -25709,9 +26201,12 @@
       <c r="AK136" s="10">
         <v>93</v>
       </c>
+      <c r="AL136" s="10">
+        <v>93</v>
+      </c>
     </row>
-    <row r="137" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
+    <row r="137" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A137" s="34"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -25820,9 +26315,12 @@
       <c r="AK137" s="10">
         <v>115</v>
       </c>
+      <c r="AL137" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="138" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
+    <row r="138" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A138" s="34"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -25931,9 +26429,12 @@
       <c r="AK138" s="10">
         <v>16</v>
       </c>
+      <c r="AL138" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="139" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A139" s="32"/>
+    <row r="139" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A139" s="35"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -26040,11 +26541,26 @@
         <v>141</v>
       </c>
       <c r="AK139" s="10">
+        <v>147</v>
+      </c>
+      <c r="AL139" s="10">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -26057,18 +26573,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -26173,7 +26677,7 @@
   <dimension ref="A1:CC19"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="R11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
       <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
@@ -26375,7 +26879,7 @@
       </c>
       <c r="AT2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14.655172413793101</v>
       </c>
       <c r="AU2" s="18">
         <f t="shared" si="1"/>
@@ -27025,7 +27529,7 @@
       </c>
       <c r="AT4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>13.725490196078432</v>
       </c>
       <c r="AU4" s="10">
         <f t="shared" si="7"/>
@@ -27350,7 +27854,7 @@
       </c>
       <c r="AT6" s="12">
         <f>MAX(0, (dc!AT2-dc!AS2))</f>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AU6" s="12">
         <f>MAX(0, (dc!AU2-dc!AT2))</f>
@@ -27674,7 +28178,7 @@
       </c>
       <c r="AT7" s="12">
         <f>MAX(0, (dc!AT3-dc!AS3))</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="AU7" s="12">
         <f>MAX(0, (dc!AU3-dc!AT3))</f>
@@ -28322,7 +28826,7 @@
       </c>
       <c r="AT9" s="12">
         <f>MAX(0, (dc!AT5-dc!AS5))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AU9" s="12">
         <f>MAX(0, (dc!AU5-dc!AT5))</f>
@@ -28874,7 +29378,7 @@
       </c>
       <c r="AT11" s="10">
         <f>MAX(0,(dc!AT7-dc!AS7))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AU11" s="10">
         <f>MAX(0,(dc!AU7-dc!AT7))</f>
@@ -29795,7 +30299,7 @@
       </c>
       <c r="AT14" s="10">
         <f>MAX(0,(dc!AT10-dc!AS10))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AU14" s="10">
         <f>MAX(0,(dc!AU10-dc!AT10))</f>
@@ -30102,7 +30606,7 @@
       </c>
       <c r="AT15" s="10">
         <f>MAX(0,(dc!AT11-dc!AS11))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AU15" s="10">
         <f>MAX(0,(dc!AU11-dc!AT11))</f>
@@ -30716,7 +31220,7 @@
       </c>
       <c r="AT17" s="10">
         <f>MAX(0,(dc!AT13-dc!AS13))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AU17" s="10">
         <f>MAX(0,(dc!AU13-dc!AT13))</f>
@@ -31023,7 +31527,7 @@
       </c>
       <c r="AT18" s="10">
         <f>MAX(0,(dc!AT14-dc!AS14))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU18" s="10">
         <f>MAX(0,(dc!AU14-dc!AT14))</f>
@@ -31330,7 +31834,7 @@
       </c>
       <c r="AT19" s="10">
         <f>MAX(0,(dc!AT15-dc!AS15))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AU19" s="10">
         <f>MAX(0,(dc!AU15-dc!AT15))</f>
@@ -31727,7 +32231,7 @@
       </c>
       <c r="AI2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.901215256888461</v>
       </c>
       <c r="AJ2" s="20">
         <f t="shared" si="0"/>
@@ -32000,7 +32504,7 @@
       </c>
       <c r="AI3" s="20">
         <f t="shared" ref="AI3:BQ3" si="3">(AI8/MAX(1,AI7))*100</f>
-        <v>0</v>
+        <v>15.342163355408388</v>
       </c>
       <c r="AJ3" s="20">
         <f t="shared" si="3"/>
@@ -32273,7 +32777,7 @@
       </c>
       <c r="AI4" s="20">
         <f t="shared" ref="AI4:BQ4" si="5">(AI9/MAX(1,AI7))*100</f>
-        <v>0</v>
+        <v>3.4216335540838854</v>
       </c>
       <c r="AJ4" s="20">
         <f t="shared" si="5"/>
@@ -32609,7 +33113,7 @@
       </c>
       <c r="AI6" s="14">
         <f>MAX(0,(md!AI2-md!AH2)+(md!AI3-md!AH3))</f>
-        <v>0</v>
+        <v>8311</v>
       </c>
       <c r="AJ6" s="14">
         <f>MAX(0,(md!AJ2-md!AI2)+(md!AJ3-md!AI3))</f>
@@ -32881,7 +33385,7 @@
       </c>
       <c r="AI7" s="14">
         <f>MAX(0,(md!AI3-md!AH3))</f>
-        <v>0</v>
+        <v>906</v>
       </c>
       <c r="AJ7" s="14">
         <f>MAX(0,(md!AJ3-md!AI3))</f>
@@ -33153,7 +33657,7 @@
       </c>
       <c r="AI8" s="14">
         <f>MAX(0,(md!AI4-md!AH4))</f>
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="AJ8" s="14">
         <f>MAX(0,(md!AJ4-md!AI4))</f>
@@ -33425,7 +33929,7 @@
       </c>
       <c r="AI9" s="14">
         <f>MAX(0,(md!AI5-md!AH5))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AJ9" s="14">
         <f>MAX(0,(md!AJ5-md!AI5))</f>
@@ -33911,7 +34415,7 @@
       </c>
       <c r="AI11" s="14">
         <f>MAX(0,(md!AI7-md!AH7))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11" s="14">
         <f>MAX(0,(md!AJ7-md!AI7))</f>
@@ -34188,7 +34692,7 @@
       </c>
       <c r="AI12" s="14">
         <f>MAX(0,(md!AI8-md!AH8))</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AJ12" s="14">
         <f>MAX(0,(md!AJ8-md!AI8))</f>
@@ -34465,7 +34969,7 @@
       </c>
       <c r="AI13" s="14">
         <f>MAX(0,(md!AI9-md!AH9))</f>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="AJ13" s="14">
         <f>MAX(0,(md!AJ9-md!AI9))</f>
@@ -34742,7 +35246,7 @@
       </c>
       <c r="AI14" s="14">
         <f>MAX(0,(md!AI10-md!AH10))</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AJ14" s="14">
         <f>MAX(0,(md!AJ10-md!AI10))</f>
@@ -35019,7 +35523,7 @@
       </c>
       <c r="AI15" s="14">
         <f>MAX(0,(md!AI11-md!AH11))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ15" s="14">
         <f>MAX(0,(md!AJ11-md!AI11))</f>
@@ -35296,7 +35800,7 @@
       </c>
       <c r="AI16" s="14">
         <f>MAX(0,(md!AI12-md!AH12))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ16" s="14">
         <f>MAX(0,(md!AJ12-md!AI12))</f>
@@ -35573,7 +36077,7 @@
       </c>
       <c r="AI17" s="14">
         <f>MAX(0,(md!AI13-md!AH13))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AJ17" s="14">
         <f>MAX(0,(md!AJ13-md!AI13))</f>
@@ -35850,7 +36354,7 @@
       </c>
       <c r="AI18" s="14">
         <f>MAX(0,(md!AI14-md!AH14))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AJ18" s="14">
         <f>MAX(0,(md!AJ14-md!AI14))</f>
@@ -36127,7 +36631,7 @@
       </c>
       <c r="AI19" s="14">
         <f>MAX(0,(md!AI15-md!AH15))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AJ19" s="14">
         <f>MAX(0,(md!AJ15-md!AI15))</f>
@@ -36404,7 +36908,7 @@
       </c>
       <c r="AI20" s="14">
         <f>MAX(0,(md!AI16-md!AH16))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ20" s="14">
         <f>MAX(0,(md!AJ16-md!AI16))</f>
@@ -36681,7 +37185,7 @@
       </c>
       <c r="AI21" s="14">
         <f>MAX(0,(md!AI17-md!AH17))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AJ21" s="14">
         <f>MAX(0,(md!AJ17-md!AI17))</f>
@@ -37235,7 +37739,7 @@
       </c>
       <c r="AI23" s="14">
         <f>MAX(0,(md!AI19-md!AH19))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AJ23" s="14">
         <f>MAX(0,(md!AJ19-md!AI19))</f>
@@ -37512,7 +38016,7 @@
       </c>
       <c r="AI24" s="14">
         <f>MAX(0,(md!AI20-md!AH20))</f>
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="AJ24" s="14">
         <f>MAX(0,(md!AJ20-md!AI20))</f>
@@ -37789,7 +38293,7 @@
       </c>
       <c r="AI25" s="14">
         <f>MAX(0,(md!AI21-md!AH21))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ25" s="14">
         <f>MAX(0,(md!AJ21-md!AI21))</f>
@@ -38066,7 +38570,7 @@
       </c>
       <c r="AI26" s="14">
         <f>MAX(0,(md!AI22-md!AH22))</f>
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="AJ26" s="14">
         <f>MAX(0,(md!AJ22-md!AI22))</f>
@@ -38343,7 +38847,7 @@
       </c>
       <c r="AI27" s="14">
         <f>MAX(0,(md!AI23-md!AH23))</f>
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="AJ27" s="14">
         <f>MAX(0,(md!AJ23-md!AI23))</f>
@@ -38620,7 +39124,7 @@
       </c>
       <c r="AI28" s="14">
         <f>MAX(0,(md!AI24-md!AH24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ28" s="14">
         <f>MAX(0,(md!AJ24-md!AI24))</f>
@@ -38897,7 +39401,7 @@
       </c>
       <c r="AI29" s="14">
         <f>MAX(0,(md!AI25-md!AH25))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AJ29" s="14">
         <f>MAX(0,(md!AJ25-md!AI25))</f>
@@ -39174,7 +39678,7 @@
       </c>
       <c r="AI30" s="14">
         <f>MAX(0,(md!AI26-md!AH26))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ30" s="14">
         <f>MAX(0,(md!AJ26-md!AI26))</f>
@@ -39728,7 +40232,7 @@
       </c>
       <c r="AI32" s="14">
         <f>MAX(0,(md!AI28-md!AH28))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AJ32" s="14">
         <f>MAX(0,(md!AJ28-md!AI28))</f>
@@ -40005,7 +40509,7 @@
       </c>
       <c r="AI33" s="14">
         <f>MAX(0,(md!AI29-md!AH29))</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AJ33" s="14">
         <f>MAX(0,(md!AJ29-md!AI29))</f>
@@ -40282,7 +40786,7 @@
       </c>
       <c r="AI34" s="14">
         <f>MAX(0,(md!AI30-md!AH30))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ34" s="14">
         <f>MAX(0,(md!AJ30-md!AI30))</f>
@@ -40603,7 +41107,7 @@
   <dimension ref="A1:BS143"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="AK6" sqref="AK6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40761,7 +41265,7 @@
       </c>
       <c r="AK2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.909404234367306</v>
       </c>
       <c r="AL2" s="19">
         <f t="shared" si="1"/>
@@ -41038,7 +41542,7 @@
       </c>
       <c r="AK3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.2035398230088497</v>
       </c>
       <c r="AL3" s="19">
         <f t="shared" si="3"/>
@@ -41315,7 +41819,7 @@
       </c>
       <c r="AK4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.7699115044247788</v>
       </c>
       <c r="AL4" s="19">
         <f t="shared" si="5"/>
@@ -41592,7 +42096,7 @@
       </c>
       <c r="AK6" s="14">
         <f>MAX(0,(va!AL5-va!AK5))</f>
-        <v>0</v>
+        <v>4062</v>
       </c>
       <c r="AL6" s="14">
         <f>MAX(0,(va!AM5-va!AL5))</f>
@@ -41869,7 +42373,7 @@
       </c>
       <c r="AK7" s="14">
         <f>MAX(0,(va!AL2-va!AK2))</f>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="AL7" s="14">
         <f>MAX(0,(va!AM2-va!AL2))</f>
@@ -42146,7 +42650,7 @@
       </c>
       <c r="AK8" s="14">
         <f>MAX(0,(va!AL3-va!AK3))</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AL8" s="14">
         <f>MAX(0,(va!AM3-va!AL3))</f>
@@ -42423,7 +42927,7 @@
       </c>
       <c r="AK9" s="14">
         <f>MAX(0,(va!AL4-va!AK4))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL9" s="14">
         <f>MAX(0,(va!AM4-va!AL4))</f>
@@ -42920,7 +43424,7 @@
       </c>
       <c r="AK11" s="16">
         <f>MAX(0,(va!AL7-va!AK7))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AL11" s="16">
         <f>MAX(0,(va!AM7-va!AL7))</f>
@@ -44048,7 +44552,7 @@
       </c>
       <c r="AK15" s="16">
         <f>MAX(0,(va!AL11-va!AK11))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL15" s="16">
         <f>MAX(0,(va!AM11-va!AL11))</f>
@@ -44612,7 +45116,7 @@
       </c>
       <c r="AK17" s="16">
         <f>MAX(0,(va!AL13-va!AK13))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL17" s="16">
         <f>MAX(0,(va!AM13-va!AL13))</f>
@@ -44894,7 +45398,7 @@
       </c>
       <c r="AK18" s="16">
         <f>MAX(0,(va!AL14-va!AK14))</f>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AL18" s="16">
         <f>MAX(0,(va!AM14-va!AL14))</f>
@@ -46304,7 +46808,7 @@
       </c>
       <c r="AK23" s="16">
         <f>MAX(0,(va!AL19-va!AK19))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL23" s="16">
         <f>MAX(0,(va!AM19-va!AL19))</f>
@@ -46868,7 +47372,7 @@
       </c>
       <c r="AK25" s="16">
         <f>MAX(0,(va!AL21-va!AK21))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AL25" s="16">
         <f>MAX(0,(va!AM21-va!AL21))</f>
@@ -47714,7 +48218,7 @@
       </c>
       <c r="AK28" s="16">
         <f>MAX(0,(va!AL24-va!AK24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL28" s="16">
         <f>MAX(0,(va!AM24-va!AL24))</f>
@@ -48560,7 +49064,7 @@
       </c>
       <c r="AK31" s="16">
         <f>MAX(0,(va!AL27-va!AK27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL31" s="16">
         <f>MAX(0,(va!AM27-va!AL27))</f>
@@ -49124,7 +49628,7 @@
       </c>
       <c r="AK33" s="16">
         <f>MAX(0,(va!AL29-va!AK29))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL33" s="16">
         <f>MAX(0,(va!AM29-va!AL29))</f>
@@ -49406,7 +49910,7 @@
       </c>
       <c r="AK34" s="16">
         <f>MAX(0,(va!AL30-va!AK30))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AL34" s="16">
         <f>MAX(0,(va!AM30-va!AL30))</f>
@@ -50816,7 +51320,7 @@
       </c>
       <c r="AK39" s="16">
         <f>MAX(0,(va!AL35-va!AK35))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL39" s="16">
         <f>MAX(0,(va!AM35-va!AL35))</f>
@@ -51098,7 +51602,7 @@
       </c>
       <c r="AK40" s="16">
         <f>MAX(0,(va!AL36-va!AK36))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL40" s="16">
         <f>MAX(0,(va!AM36-va!AL36))</f>
@@ -51662,7 +52166,7 @@
       </c>
       <c r="AK42" s="16">
         <f>MAX(0,(va!AL38-va!AK38))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL42" s="16">
         <f>MAX(0,(va!AM38-va!AL38))</f>
@@ -51944,7 +52448,7 @@
       </c>
       <c r="AK43" s="16">
         <f>MAX(0,(va!AL39-va!AK39))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AL43" s="16">
         <f>MAX(0,(va!AM39-va!AL39))</f>
@@ -52226,7 +52730,7 @@
       </c>
       <c r="AK44" s="16">
         <f>MAX(0,(va!AL40-va!AK40))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL44" s="16">
         <f>MAX(0,(va!AM40-va!AL40))</f>
@@ -52790,7 +53294,7 @@
       </c>
       <c r="AK46" s="16">
         <f>MAX(0,(va!AL42-va!AK42))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL46" s="16">
         <f>MAX(0,(va!AM42-va!AL42))</f>
@@ -53072,7 +53576,7 @@
       </c>
       <c r="AK47" s="16">
         <f>MAX(0,(va!AL43-va!AK43))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL47" s="16">
         <f>MAX(0,(va!AM43-va!AL43))</f>
@@ -53354,7 +53858,7 @@
       </c>
       <c r="AK48" s="16">
         <f>MAX(0,(va!AL44-va!AK44))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL48" s="16">
         <f>MAX(0,(va!AM44-va!AL44))</f>
@@ -53636,7 +54140,7 @@
       </c>
       <c r="AK49" s="16">
         <f>MAX(0,(va!AL45-va!AK45))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL49" s="16">
         <f>MAX(0,(va!AM45-va!AL45))</f>
@@ -53918,7 +54422,7 @@
       </c>
       <c r="AK50" s="16">
         <f>MAX(0,(va!AL46-va!AK46))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL50" s="16">
         <f>MAX(0,(va!AM46-va!AL46))</f>
@@ -54764,7 +55268,7 @@
       </c>
       <c r="AK53" s="16">
         <f>MAX(0,(va!AL49-va!AK49))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL53" s="16">
         <f>MAX(0,(va!AM49-va!AL49))</f>
@@ -55046,7 +55550,7 @@
       </c>
       <c r="AK54" s="16">
         <f>MAX(0,(va!AL50-va!AK50))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AL54" s="16">
         <f>MAX(0,(va!AM50-va!AL50))</f>
@@ -55328,7 +55832,7 @@
       </c>
       <c r="AK55" s="16">
         <f>MAX(0,(va!AL51-va!AK51))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL55" s="16">
         <f>MAX(0,(va!AM51-va!AL51))</f>
@@ -55610,7 +56114,7 @@
       </c>
       <c r="AK56" s="16">
         <f>MAX(0,(va!AL52-va!AK52))</f>
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="AL56" s="16">
         <f>MAX(0,(va!AM52-va!AL52))</f>
@@ -55892,7 +56396,7 @@
       </c>
       <c r="AK57" s="16">
         <f>MAX(0,(va!AL53-va!AK53))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL57" s="16">
         <f>MAX(0,(va!AM53-va!AL53))</f>
@@ -56456,7 +56960,7 @@
       </c>
       <c r="AK59" s="16">
         <f>MAX(0,(va!AL55-va!AK55))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL59" s="16">
         <f>MAX(0,(va!AM55-va!AL55))</f>
@@ -56738,7 +57242,7 @@
       </c>
       <c r="AK60" s="16">
         <f>MAX(0,(va!AL56-va!AK56))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AL60" s="16">
         <f>MAX(0,(va!AM56-va!AL56))</f>
@@ -57584,7 +58088,7 @@
       </c>
       <c r="AK63" s="16">
         <f>MAX(0,(va!AL59-va!AK59))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL63" s="16">
         <f>MAX(0,(va!AM59-va!AL59))</f>
@@ -58430,7 +58934,7 @@
       </c>
       <c r="AK66" s="16">
         <f>MAX(0,(va!AL62-va!AK62))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL66" s="16">
         <f>MAX(0,(va!AM62-va!AL62))</f>
@@ -58712,7 +59216,7 @@
       </c>
       <c r="AK67" s="16">
         <f>MAX(0,(va!AL63-va!AK63))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL67" s="16">
         <f>MAX(0,(va!AM63-va!AL63))</f>
@@ -58994,7 +59498,7 @@
       </c>
       <c r="AK68" s="16">
         <f>MAX(0,(va!AL64-va!AK64))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL68" s="16">
         <f>MAX(0,(va!AM64-va!AL64))</f>
@@ -59276,7 +59780,7 @@
       </c>
       <c r="AK69" s="16">
         <f>MAX(0,(va!AL65-va!AK65))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL69" s="16">
         <f>MAX(0,(va!AM65-va!AL65))</f>
@@ -59840,7 +60344,7 @@
       </c>
       <c r="AK71" s="16">
         <f>MAX(0,(va!AL67-va!AK67))</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AL71" s="16">
         <f>MAX(0,(va!AM67-va!AL67))</f>
@@ -60404,7 +60908,7 @@
       </c>
       <c r="AK73" s="16">
         <f>MAX(0,(va!AL69-va!AK69))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL73" s="16">
         <f>MAX(0,(va!AM69-va!AL69))</f>
@@ -62942,7 +63446,7 @@
       </c>
       <c r="AK82" s="16">
         <f>MAX(0,(va!AL78-va!AK78))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL82" s="16">
         <f>MAX(0,(va!AM78-va!AL78))</f>
@@ -63788,7 +64292,7 @@
       </c>
       <c r="AK85" s="16">
         <f>MAX(0,(va!AL81-va!AK81))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL85" s="16">
         <f>MAX(0,(va!AM81-va!AL81))</f>
@@ -64070,7 +64574,7 @@
       </c>
       <c r="AK86" s="16">
         <f>MAX(0,(va!AL82-va!AK82))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL86" s="16">
         <f>MAX(0,(va!AM82-va!AL82))</f>
@@ -64634,7 +65138,7 @@
       </c>
       <c r="AK88" s="16">
         <f>MAX(0,(va!AL84-va!AK84))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL88" s="16">
         <f>MAX(0,(va!AM84-va!AL84))</f>
@@ -65762,7 +66266,7 @@
       </c>
       <c r="AK92" s="16">
         <f>MAX(0,(va!AL88-va!AK88))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL92" s="16">
         <f>MAX(0,(va!AM88-va!AL88))</f>
@@ -68018,7 +68522,7 @@
       </c>
       <c r="AK100" s="16">
         <f>MAX(0,(va!AL96-va!AK96))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AL100" s="16">
         <f>MAX(0,(va!AM96-va!AL96))</f>
@@ -68300,7 +68804,7 @@
       </c>
       <c r="AK101" s="16">
         <f>MAX(0,(va!AL97-va!AK97))</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AL101" s="16">
         <f>MAX(0,(va!AM97-va!AL97))</f>
@@ -68582,7 +69086,7 @@
       </c>
       <c r="AK102" s="16">
         <f>MAX(0,(va!AL98-va!AK98))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AL102" s="16">
         <f>MAX(0,(va!AM98-va!AL98))</f>
@@ -68864,7 +69368,7 @@
       </c>
       <c r="AK103" s="16">
         <f>MAX(0,(va!AL99-va!AK99))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL103" s="16">
         <f>MAX(0,(va!AM99-va!AL99))</f>
@@ -69428,7 +69932,7 @@
       </c>
       <c r="AK105" s="16">
         <f>MAX(0,(va!AL101-va!AK101))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL105" s="16">
         <f>MAX(0,(va!AM101-va!AL101))</f>
@@ -69710,7 +70214,7 @@
       </c>
       <c r="AK106" s="16">
         <f>MAX(0,(va!AL102-va!AK102))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AL106" s="16">
         <f>MAX(0,(va!AM102-va!AL102))</f>
@@ -69992,7 +70496,7 @@
       </c>
       <c r="AK107" s="16">
         <f>MAX(0,(va!AL103-va!AK103))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL107" s="16">
         <f>MAX(0,(va!AM103-va!AL103))</f>
@@ -70274,7 +70778,7 @@
       </c>
       <c r="AK108" s="16">
         <f>MAX(0,(va!AL104-va!AK104))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL108" s="16">
         <f>MAX(0,(va!AM104-va!AL104))</f>
@@ -70556,7 +71060,7 @@
       </c>
       <c r="AK109" s="16">
         <f>MAX(0,(va!AL105-va!AK105))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL109" s="16">
         <f>MAX(0,(va!AM105-va!AL105))</f>
@@ -70838,7 +71342,7 @@
       </c>
       <c r="AK110" s="16">
         <f>MAX(0,(va!AL106-va!AK106))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL110" s="16">
         <f>MAX(0,(va!AM106-va!AL106))</f>
@@ -71966,7 +72470,7 @@
       </c>
       <c r="AK114" s="16">
         <f>MAX(0,(va!AL110-va!AK110))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL114" s="16">
         <f>MAX(0,(va!AM110-va!AL110))</f>
@@ -73094,7 +73598,7 @@
       </c>
       <c r="AK118" s="16">
         <f>MAX(0,(va!AL114-va!AK114))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL118" s="16">
         <f>MAX(0,(va!AM114-va!AL114))</f>
@@ -73376,7 +73880,7 @@
       </c>
       <c r="AK119" s="16">
         <f>MAX(0,(va!AL115-va!AK115))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL119" s="16">
         <f>MAX(0,(va!AM115-va!AL115))</f>
@@ -73658,7 +74162,7 @@
       </c>
       <c r="AK120" s="16">
         <f>MAX(0,(va!AL116-va!AK116))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL120" s="16">
         <f>MAX(0,(va!AM116-va!AL116))</f>
@@ -74222,7 +74726,7 @@
       </c>
       <c r="AK122" s="16">
         <f>MAX(0,(va!AL118-va!AK118))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL122" s="16">
         <f>MAX(0,(va!AM118-va!AL118))</f>
@@ -74786,7 +75290,7 @@
       </c>
       <c r="AK124" s="16">
         <f>MAX(0,(va!AL120-va!AK120))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL124" s="16">
         <f>MAX(0,(va!AM120-va!AL120))</f>
@@ -77324,7 +77828,7 @@
       </c>
       <c r="AK133" s="16">
         <f>MAX(0,(va!AL129-va!AK129))</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AL133" s="16">
         <f>MAX(0,(va!AM129-va!AL129))</f>
@@ -77888,7 +78392,7 @@
       </c>
       <c r="AK135" s="16">
         <f>MAX(0,(va!AL131-va!AK131))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL135" s="16">
         <f>MAX(0,(va!AM131-va!AL131))</f>
@@ -78452,7 +78956,7 @@
       </c>
       <c r="AK137" s="16">
         <f>MAX(0,(va!AL133-va!AK133))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL137" s="16">
         <f>MAX(0,(va!AM133-va!AL133))</f>

</xml_diff>

<commit_message>
28 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DF7625-0695-4C6D-89B7-C03D9EF17B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803C940-261A-42A9-A4C1-0B2446A42A1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="4005" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4018,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AT2" sqref="AT2"/>
+      <selection pane="bottomRight" activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4173,6 +4173,9 @@
       <c r="AT2" s="12">
         <v>18416</v>
       </c>
+      <c r="AU2" s="12">
+        <v>18885</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4345,7 +4348,7 @@
       </c>
       <c r="AU3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3994</v>
       </c>
       <c r="AV3" s="10">
         <f t="shared" si="0"/>
@@ -4628,6 +4631,9 @@
       <c r="AT5" s="10">
         <v>185</v>
       </c>
+      <c r="AU5" s="10">
+        <v>190</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5013,6 +5019,9 @@
       <c r="AT7" s="10">
         <v>450</v>
       </c>
+      <c r="AU7" s="10">
+        <v>475</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5153,6 +5162,9 @@
       <c r="AT8" s="10">
         <v>261</v>
       </c>
+      <c r="AU8" s="10">
+        <v>266</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5293,6 +5305,9 @@
       <c r="AT9" s="10">
         <v>261</v>
       </c>
+      <c r="AU9" s="10">
+        <v>264</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5433,6 +5448,9 @@
       <c r="AT10" s="10">
         <v>681</v>
       </c>
+      <c r="AU10" s="10">
+        <v>702</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5573,6 +5591,9 @@
       <c r="AT11" s="10">
         <v>571</v>
       </c>
+      <c r="AU11" s="10">
+        <v>587</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5713,6 +5734,9 @@
       <c r="AT12" s="10">
         <v>405</v>
       </c>
+      <c r="AU12" s="10">
+        <v>414</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5853,6 +5877,9 @@
       <c r="AT13" s="10">
         <v>578</v>
       </c>
+      <c r="AU13" s="10">
+        <v>594</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -5993,6 +6020,9 @@
       <c r="AT14" s="10">
         <v>535</v>
       </c>
+      <c r="AU14" s="10">
+        <v>560</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6132,6 +6162,9 @@
       </c>
       <c r="AT15" s="10">
         <v>150</v>
+      </c>
+      <c r="AU15" s="10">
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6386,7 +6419,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
+      <selection pane="bottomRight" activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6509,7 +6542,7 @@
         <v>85489</v>
       </c>
       <c r="AJ2" s="10">
-        <v>0</v>
+        <v>87672</v>
       </c>
       <c r="AK2" s="10">
         <v>0</v>
@@ -6748,7 +6781,7 @@
       </c>
       <c r="AJ3" s="10">
         <f>SUM(md[28-Apr])</f>
-        <v>0</v>
+        <v>20113</v>
       </c>
       <c r="AK3" s="10">
         <f>SUM(md[29-Apr])</f>
@@ -6987,7 +7020,7 @@
         <v>4101</v>
       </c>
       <c r="AJ4" s="10">
-        <v>0</v>
+        <v>4268</v>
       </c>
       <c r="AK4" s="10">
         <v>0</v>
@@ -7193,7 +7226,7 @@
         <v>858</v>
       </c>
       <c r="AJ5" s="10">
-        <v>0</v>
+        <v>929</v>
       </c>
       <c r="AK5" s="10">
         <v>0</v>
@@ -7610,6 +7643,9 @@
       <c r="AI7">
         <v>114</v>
       </c>
+      <c r="AJ7">
+        <v>115</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7717,6 +7753,9 @@
       <c r="AI8" s="10">
         <v>1544</v>
       </c>
+      <c r="AJ8" s="10">
+        <v>1571</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7824,6 +7863,9 @@
       <c r="AI9">
         <v>1933</v>
       </c>
+      <c r="AJ9">
+        <v>1977</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7931,6 +7973,9 @@
       <c r="AI10">
         <v>2548</v>
       </c>
+      <c r="AJ10">
+        <v>2631</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8038,6 +8083,9 @@
       <c r="AI11">
         <v>138</v>
       </c>
+      <c r="AJ11">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8145,6 +8193,9 @@
       <c r="AI12">
         <v>68</v>
       </c>
+      <c r="AJ12">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8252,6 +8303,9 @@
       <c r="AI13">
         <v>403</v>
       </c>
+      <c r="AJ13">
+        <v>416</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8359,6 +8413,9 @@
       <c r="AI14">
         <v>163</v>
       </c>
+      <c r="AJ14">
+        <v>163</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8466,6 +8523,9 @@
       <c r="AI15">
         <v>529</v>
       </c>
+      <c r="AJ15">
+        <v>539</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8573,8 +8633,11 @@
       <c r="AI16" s="10">
         <v>51</v>
       </c>
+      <c r="AJ16" s="10">
+        <v>52</v>
+      </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8680,8 +8743,11 @@
       <c r="AI17">
         <v>865</v>
       </c>
+      <c r="AJ17">
+        <v>870</v>
+      </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8787,8 +8853,11 @@
       <c r="AI18">
         <v>4</v>
       </c>
+      <c r="AJ18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8894,8 +8963,11 @@
       <c r="AI19">
         <v>352</v>
       </c>
+      <c r="AJ19">
+        <v>358</v>
+      </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9001,8 +9073,11 @@
       <c r="AI20">
         <v>778</v>
       </c>
+      <c r="AJ20">
+        <v>802</v>
+      </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9108,8 +9183,11 @@
       <c r="AI21">
         <v>70</v>
       </c>
+      <c r="AJ21">
+        <v>73</v>
+      </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9215,8 +9293,11 @@
       <c r="AI22">
         <v>3843</v>
       </c>
+      <c r="AJ22">
+        <v>4003</v>
+      </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9322,8 +9403,11 @@
       <c r="AI23">
         <v>5263</v>
       </c>
+      <c r="AJ23">
+        <v>5496</v>
+      </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9429,8 +9513,11 @@
       <c r="AI24">
         <v>54</v>
       </c>
+      <c r="AJ24">
+        <v>55</v>
+      </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9536,8 +9623,11 @@
       <c r="AI25">
         <v>144</v>
       </c>
+      <c r="AJ25">
+        <v>145</v>
+      </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9643,8 +9733,11 @@
       <c r="AI26">
         <v>19</v>
       </c>
+      <c r="AJ26">
+        <v>20</v>
+      </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -9750,8 +9843,11 @@
       <c r="AI27">
         <v>34</v>
       </c>
+      <c r="AJ27">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -9857,8 +9953,11 @@
       <c r="AI28">
         <v>181</v>
       </c>
+      <c r="AJ28">
+        <v>187</v>
+      </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -9964,8 +10063,11 @@
       <c r="AI29">
         <v>336</v>
       </c>
+      <c r="AJ29">
+        <v>340</v>
+      </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10071,8 +10173,11 @@
       <c r="AI30">
         <v>53</v>
       </c>
+      <c r="AJ30">
+        <v>54</v>
+      </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10166,10 +10271,10 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="U35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="U15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
+      <selection pane="bottomRight" activeCell="AM3" sqref="AM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10335,7 +10440,7 @@
       </c>
       <c r="AM2" s="10">
         <f>SUM(va[28-Apr])</f>
-        <v>0</v>
+        <v>14339</v>
       </c>
       <c r="AN2" s="10">
         <f>SUM(va[29-Apr])</f>
@@ -10577,7 +10682,7 @@
         <v>2066</v>
       </c>
       <c r="AM3" s="10">
-        <v>0</v>
+        <v>2165</v>
       </c>
       <c r="AN3" s="10">
         <v>0</v>
@@ -10786,7 +10891,7 @@
         <v>458</v>
       </c>
       <c r="AM4" s="10">
-        <v>0</v>
+        <v>492</v>
       </c>
       <c r="AN4" s="10">
         <v>0</v>
@@ -10995,7 +11100,7 @@
         <v>80180</v>
       </c>
       <c r="AM5" s="10">
-        <v>0</v>
+        <v>82753</v>
       </c>
       <c r="AN5" s="10">
         <v>0</v>
@@ -11430,9 +11535,12 @@
       <c r="AL7" s="10">
         <v>627</v>
       </c>
+      <c r="AM7" s="10">
+        <v>653</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11546,9 +11654,12 @@
       <c r="AL8" s="10">
         <v>5</v>
       </c>
+      <c r="AM8" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11660,9 +11771,12 @@
       <c r="AL9" s="10">
         <v>27</v>
       </c>
+      <c r="AM9" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -11774,9 +11888,12 @@
       <c r="AL10" s="10">
         <v>2</v>
       </c>
+      <c r="AM10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -11888,9 +12005,12 @@
       <c r="AL11" s="10">
         <v>41</v>
       </c>
+      <c r="AM11" s="10">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -12002,9 +12122,12 @@
       <c r="AL12" s="10">
         <v>1</v>
       </c>
+      <c r="AM12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -12115,6 +12238,9 @@
       </c>
       <c r="AL13" s="10">
         <v>11</v>
+      </c>
+      <c r="AM13" s="10">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
@@ -12232,9 +12358,12 @@
       <c r="AL14" s="10">
         <v>836</v>
       </c>
+      <c r="AM14" s="10">
+        <v>865</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12348,9 +12477,12 @@
       <c r="AL15" s="10">
         <v>36</v>
       </c>
+      <c r="AM15" s="10">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -12462,9 +12594,12 @@
       <c r="AL16" s="10">
         <v>0</v>
       </c>
+      <c r="AM16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12576,9 +12711,12 @@
       <c r="AL17" s="10">
         <v>1</v>
       </c>
+      <c r="AM17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -12690,9 +12828,12 @@
       <c r="AL18" s="10">
         <v>5</v>
       </c>
+      <c r="AM18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -12804,9 +12945,12 @@
       <c r="AL19" s="10">
         <v>193</v>
       </c>
+      <c r="AM19" s="10">
+        <v>216</v>
+      </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -12918,9 +13062,12 @@
       <c r="AL20" s="10">
         <v>5</v>
       </c>
+      <c r="AM20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -13032,9 +13179,12 @@
       <c r="AL21" s="10">
         <v>383</v>
       </c>
+      <c r="AM21" s="10">
+        <v>406</v>
+      </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -13146,9 +13296,12 @@
       <c r="AL22" s="10">
         <v>3</v>
       </c>
+      <c r="AM22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -13260,9 +13413,12 @@
       <c r="AL23" s="10">
         <v>10</v>
       </c>
+      <c r="AM23" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -13374,9 +13530,12 @@
       <c r="AL24" s="10">
         <v>11</v>
       </c>
+      <c r="AM24" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -13490,9 +13649,12 @@
       <c r="AL25" s="10">
         <v>9</v>
       </c>
+      <c r="AM25" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -13604,9 +13766,12 @@
       <c r="AL26" s="10">
         <v>17</v>
       </c>
+      <c r="AM26" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -13718,9 +13883,12 @@
       <c r="AL27" s="10">
         <v>25</v>
       </c>
+      <c r="AM27" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -13832,9 +14000,12 @@
       <c r="AL28" s="10">
         <v>11</v>
       </c>
+      <c r="AM28" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -13946,8 +14117,11 @@
       <c r="AL29" s="10">
         <v>51</v>
       </c>
+      <c r="AM29" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -14062,9 +14236,12 @@
       <c r="AL30" s="10">
         <v>214</v>
       </c>
+      <c r="AM30" s="10">
+        <v>220</v>
+      </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -14178,9 +14355,12 @@
       <c r="AL31" s="10">
         <v>457</v>
       </c>
+      <c r="AM31" s="10">
+        <v>488</v>
+      </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -14292,9 +14472,12 @@
       <c r="AL32" s="10">
         <v>11</v>
       </c>
+      <c r="AM32" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -14406,9 +14589,12 @@
       <c r="AL33" s="10">
         <v>45</v>
       </c>
+      <c r="AM33" s="10">
+        <v>47</v>
+      </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -14522,9 +14708,12 @@
       <c r="AL34" s="10">
         <v>13</v>
       </c>
+      <c r="AM34" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -14636,9 +14825,12 @@
       <c r="AL35" s="10">
         <v>72</v>
       </c>
+      <c r="AM35" s="10">
+        <v>74</v>
+      </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -14750,9 +14942,12 @@
       <c r="AL36" s="10">
         <v>108</v>
       </c>
+      <c r="AM36" s="10">
+        <v>109</v>
+      </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -14864,9 +15059,12 @@
       <c r="AL37" s="10">
         <v>20</v>
       </c>
+      <c r="AM37" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -14980,9 +15178,12 @@
       <c r="AL38" s="10">
         <v>15</v>
       </c>
+      <c r="AM38" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -15094,9 +15295,12 @@
       <c r="AL39" s="10">
         <v>36</v>
       </c>
+      <c r="AM39" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -15208,9 +15412,12 @@
       <c r="AL40" s="10">
         <v>31</v>
       </c>
+      <c r="AM40" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -15322,9 +15529,12 @@
       <c r="AL41" s="10">
         <v>4</v>
       </c>
+      <c r="AM41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -15436,9 +15646,12 @@
       <c r="AL42" s="10">
         <v>30</v>
       </c>
+      <c r="AM42" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -15550,9 +15763,12 @@
       <c r="AL43" s="10">
         <v>20</v>
       </c>
+      <c r="AM43" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -15664,9 +15880,12 @@
       <c r="AL44" s="10">
         <v>24</v>
       </c>
+      <c r="AM44" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -15778,9 +15997,12 @@
       <c r="AL45" s="10">
         <v>30</v>
       </c>
+      <c r="AM45" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -15894,9 +16116,12 @@
       <c r="AL46" s="10">
         <v>14</v>
       </c>
+      <c r="AM46" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -16008,9 +16233,12 @@
       <c r="AL47" s="10">
         <v>0</v>
       </c>
+      <c r="AM47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -16122,9 +16350,12 @@
       <c r="AL48" s="10">
         <v>3</v>
       </c>
+      <c r="AM48" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -16236,9 +16467,12 @@
       <c r="AL49" s="10">
         <v>5</v>
       </c>
+      <c r="AM49" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -16352,9 +16586,12 @@
       <c r="AL50" s="10">
         <v>195</v>
       </c>
+      <c r="AM50" s="10">
+        <v>223</v>
+      </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -16466,9 +16703,12 @@
       <c r="AL51" s="10">
         <v>28</v>
       </c>
+      <c r="AM51" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -16582,9 +16822,12 @@
       <c r="AL52" s="10">
         <v>3002</v>
       </c>
+      <c r="AM52" s="10">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -16696,9 +16939,12 @@
       <c r="AL53" s="10">
         <v>27</v>
       </c>
+      <c r="AM53" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -16810,8 +17056,11 @@
       <c r="AL54" s="10">
         <v>26</v>
       </c>
+      <c r="AM54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -16926,8 +17175,11 @@
       <c r="AL55" s="10">
         <v>108</v>
       </c>
+      <c r="AM55" s="10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -17042,9 +17294,12 @@
       <c r="AL56" s="10">
         <v>817</v>
       </c>
+      <c r="AM56" s="10">
+        <v>835</v>
+      </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -17158,9 +17413,12 @@
       <c r="AL57" s="10">
         <v>8</v>
       </c>
+      <c r="AM57" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -17272,9 +17530,12 @@
       <c r="AL58" s="10">
         <v>6</v>
       </c>
+      <c r="AM58" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -17386,9 +17647,12 @@
       <c r="AL59" s="10">
         <v>21</v>
       </c>
+      <c r="AM59" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -17500,9 +17764,12 @@
       <c r="AL60" s="10">
         <v>2</v>
       </c>
+      <c r="AM60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -17616,9 +17883,12 @@
       <c r="AL61" s="10">
         <v>7</v>
       </c>
+      <c r="AM61" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -17730,9 +18000,12 @@
       <c r="AL62" s="10">
         <v>95</v>
       </c>
+      <c r="AM62" s="10">
+        <v>97</v>
+      </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -17844,9 +18117,12 @@
       <c r="AL63" s="10">
         <v>87</v>
       </c>
+      <c r="AM63" s="10">
+        <v>89</v>
+      </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -17958,9 +18234,12 @@
       <c r="AL64" s="10">
         <v>78</v>
       </c>
+      <c r="AM64" s="10">
+        <v>79</v>
+      </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
+    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -18072,9 +18351,12 @@
       <c r="AL65" s="10">
         <v>44</v>
       </c>
+      <c r="AM65" s="10">
+        <v>47</v>
+      </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -18186,8 +18468,11 @@
       <c r="AL66" s="10">
         <v>33</v>
       </c>
+      <c r="AM66" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -18302,9 +18587,12 @@
       <c r="AL67" s="10">
         <v>628</v>
       </c>
+      <c r="AM67" s="10">
+        <v>688</v>
+      </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -18418,9 +18706,12 @@
       <c r="AL68" s="10">
         <v>0</v>
       </c>
+      <c r="AM68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -18532,9 +18823,12 @@
       <c r="AL69" s="10">
         <v>4</v>
       </c>
+      <c r="AM69" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -18646,9 +18940,12 @@
       <c r="AL70" s="10">
         <v>0</v>
       </c>
+      <c r="AM70" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -18760,9 +19057,12 @@
       <c r="AL71" s="10">
         <v>13</v>
       </c>
+      <c r="AM71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -18874,9 +19174,12 @@
       <c r="AL72" s="10">
         <v>34</v>
       </c>
+      <c r="AM72" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
+    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -18988,9 +19291,12 @@
       <c r="AL73" s="10">
         <v>11</v>
       </c>
+      <c r="AM73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -19102,9 +19408,12 @@
       <c r="AL74" s="10">
         <v>1</v>
       </c>
+      <c r="AM74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
+    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -19216,9 +19525,12 @@
       <c r="AL75" s="10">
         <v>3</v>
       </c>
+      <c r="AM75" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -19332,9 +19644,12 @@
       <c r="AL76" s="10">
         <v>1</v>
       </c>
+      <c r="AM76" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -19446,9 +19761,12 @@
       <c r="AL77" s="10">
         <v>4</v>
       </c>
+      <c r="AM77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
+    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -19560,9 +19878,12 @@
       <c r="AL78" s="10">
         <v>54</v>
       </c>
+      <c r="AM78" s="10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
+    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -19674,9 +19995,12 @@
       <c r="AL79" s="10">
         <v>9</v>
       </c>
+      <c r="AM79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
+    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -19788,8 +20112,11 @@
       <c r="AL80" s="10">
         <v>3</v>
       </c>
+      <c r="AM80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -19904,9 +20231,12 @@
       <c r="AL81" s="10">
         <v>184</v>
       </c>
+      <c r="AM81" s="10">
+        <v>188</v>
+      </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -20020,9 +20350,12 @@
       <c r="AL82" s="10">
         <v>154</v>
       </c>
+      <c r="AM82" s="10">
+        <v>155</v>
+      </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
+    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -20134,9 +20467,12 @@
       <c r="AL83" s="10">
         <v>44</v>
       </c>
+      <c r="AM83" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
+    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -20248,9 +20584,12 @@
       <c r="AL84" s="10">
         <v>112</v>
       </c>
+      <c r="AM84" s="10">
+        <v>112</v>
+      </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
+    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -20362,9 +20701,12 @@
       <c r="AL85" s="10">
         <v>6</v>
       </c>
+      <c r="AM85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
+    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -20476,9 +20818,12 @@
       <c r="AL86" s="10">
         <v>15</v>
       </c>
+      <c r="AM86" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A87" s="30" t="s">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -20592,9 +20937,12 @@
       <c r="AL87" s="10">
         <v>15</v>
       </c>
+      <c r="AM87" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -20706,9 +21054,12 @@
       <c r="AL88" s="10">
         <v>45</v>
       </c>
+      <c r="AM88" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -20820,9 +21171,12 @@
       <c r="AL89" s="10">
         <v>7</v>
       </c>
+      <c r="AM89" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -20934,9 +21288,12 @@
       <c r="AL90" s="10">
         <v>10</v>
       </c>
+      <c r="AM90" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -21048,9 +21405,12 @@
       <c r="AL91" s="10">
         <v>4</v>
       </c>
+      <c r="AM91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A92" s="31"/>
+    <row r="92" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -21162,9 +21522,12 @@
       <c r="AL92" s="10">
         <v>11</v>
       </c>
+      <c r="AM92" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
+    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -21276,9 +21639,12 @@
       <c r="AL93" s="10">
         <v>41</v>
       </c>
+      <c r="AM93" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -21392,9 +21758,12 @@
       <c r="AL94" s="10">
         <v>11</v>
       </c>
+      <c r="AM94" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -21506,8 +21875,11 @@
       <c r="AL95" s="10">
         <v>33</v>
       </c>
+      <c r="AM95" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -21622,9 +21994,12 @@
       <c r="AL96" s="10">
         <v>114</v>
       </c>
+      <c r="AM96" s="10">
+        <v>149</v>
+      </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A97" s="33" t="s">
+    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -21738,9 +22113,12 @@
       <c r="AL97" s="10">
         <v>1353</v>
       </c>
+      <c r="AM97" s="10">
+        <v>1449</v>
+      </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
+    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -21852,9 +22230,12 @@
       <c r="AL98" s="10">
         <v>165</v>
       </c>
+      <c r="AM98" s="10">
+        <v>175</v>
+      </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A99" s="35"/>
+    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -21966,9 +22347,12 @@
       <c r="AL99" s="10">
         <v>50</v>
       </c>
+      <c r="AM99" s="10">
+        <v>53</v>
+      </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -22082,9 +22466,12 @@
       <c r="AL100" s="10">
         <v>21</v>
       </c>
+      <c r="AM100" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -22196,9 +22583,12 @@
       <c r="AL101" s="10">
         <v>28</v>
       </c>
+      <c r="AM101" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -22310,9 +22700,12 @@
       <c r="AL102" s="10">
         <v>119</v>
       </c>
+      <c r="AM102" s="10">
+        <v>126</v>
+      </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -22424,9 +22817,12 @@
       <c r="AL103" s="10">
         <v>218</v>
       </c>
+      <c r="AM103" s="10">
+        <v>221</v>
+      </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
+    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -22538,9 +22934,12 @@
       <c r="AL104" s="10">
         <v>24</v>
       </c>
+      <c r="AM104" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -22654,9 +23053,12 @@
       <c r="AL105" s="10">
         <v>113</v>
       </c>
+      <c r="AM105" s="10">
+        <v>126</v>
+      </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
+    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -22768,9 +23170,12 @@
       <c r="AL106" s="10">
         <v>96</v>
       </c>
+      <c r="AM106" s="10">
+        <v>105</v>
+      </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
+    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -22882,9 +23287,12 @@
       <c r="AL107" s="10">
         <v>14</v>
       </c>
+      <c r="AM107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
+    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -22996,9 +23404,12 @@
       <c r="AL108" s="10">
         <v>26</v>
       </c>
+      <c r="AM108" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -23110,8 +23521,11 @@
       <c r="AL109" s="10">
         <v>1</v>
       </c>
+      <c r="AM109" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -23226,8 +23640,11 @@
       <c r="AL110" s="10">
         <v>304</v>
       </c>
+      <c r="AM110" s="10">
+        <v>312</v>
+      </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -23342,9 +23759,12 @@
       <c r="AL111" s="10">
         <v>33</v>
       </c>
+      <c r="AM111" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -23458,9 +23878,12 @@
       <c r="AL112" s="10">
         <v>14</v>
       </c>
+      <c r="AM112" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -23572,9 +23995,12 @@
       <c r="AL113" s="10">
         <v>17</v>
       </c>
+      <c r="AM113" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A114" s="32"/>
+    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -23686,9 +24112,12 @@
       <c r="AL114" s="10">
         <v>98</v>
       </c>
+      <c r="AM114" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A115" s="33" t="s">
+    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -23802,9 +24231,12 @@
       <c r="AL115" s="10">
         <v>77</v>
       </c>
+      <c r="AM115" s="10">
+        <v>80</v>
+      </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
+    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -23916,9 +24348,12 @@
       <c r="AL116" s="10">
         <v>73</v>
       </c>
+      <c r="AM116" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+    <row r="117" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -24030,9 +24465,12 @@
       <c r="AL117" s="10">
         <v>10</v>
       </c>
+      <c r="AM117" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
+    <row r="118" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -24144,9 +24582,12 @@
       <c r="AL118" s="10">
         <v>41</v>
       </c>
+      <c r="AM118" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+    <row r="119" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -24258,9 +24699,12 @@
       <c r="AL119" s="10">
         <v>7</v>
       </c>
+      <c r="AM119" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+    <row r="120" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -24372,9 +24816,12 @@
       <c r="AL120" s="10">
         <v>50</v>
       </c>
+      <c r="AM120" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="s">
+    <row r="121" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -24488,9 +24935,12 @@
       <c r="AL121" s="10">
         <v>6</v>
       </c>
+      <c r="AM121" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
+    <row r="122" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -24602,9 +25052,12 @@
       <c r="AL122" s="10">
         <v>22</v>
       </c>
+      <c r="AM122" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A123" s="31"/>
+    <row r="123" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -24716,9 +25169,12 @@
       <c r="AL123" s="10">
         <v>2</v>
       </c>
+      <c r="AM123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A124" s="31"/>
+    <row r="124" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -24830,9 +25286,12 @@
       <c r="AL124" s="10">
         <v>5</v>
       </c>
+      <c r="AM124" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A125" s="31"/>
+    <row r="125" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -24944,9 +25403,12 @@
       <c r="AL125" s="10">
         <v>1</v>
       </c>
+      <c r="AM125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A126" s="31"/>
+    <row r="126" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -25058,9 +25520,12 @@
       <c r="AL126" s="10">
         <v>4</v>
       </c>
+      <c r="AM126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A127" s="31"/>
+    <row r="127" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -25172,9 +25637,12 @@
       <c r="AL127" s="10">
         <v>4</v>
       </c>
+      <c r="AM127" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A128" s="31"/>
+    <row r="128" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -25286,9 +25754,12 @@
       <c r="AL128" s="10">
         <v>8</v>
       </c>
+      <c r="AM128" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A129" s="31"/>
+    <row r="129" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -25400,9 +25871,12 @@
       <c r="AL129" s="10">
         <v>132</v>
       </c>
+      <c r="AM129" s="10">
+        <v>141</v>
+      </c>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+    <row r="130" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -25514,8 +25988,11 @@
       <c r="AL130" s="10">
         <v>20</v>
       </c>
+      <c r="AM130" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -25630,9 +26107,12 @@
       <c r="AL131" s="10">
         <v>355</v>
       </c>
+      <c r="AM131" s="10">
+        <v>359</v>
+      </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="s">
+    <row r="132" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -25746,9 +26226,12 @@
       <c r="AL132" s="10">
         <v>19</v>
       </c>
+      <c r="AM132" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A133" s="31"/>
+    <row r="133" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -25860,9 +26343,12 @@
       <c r="AL133" s="10">
         <v>15</v>
       </c>
+      <c r="AM133" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A134" s="31"/>
+    <row r="134" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -25974,9 +26460,12 @@
       <c r="AL134" s="10">
         <v>2</v>
       </c>
+      <c r="AM134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A135" s="32"/>
+    <row r="135" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -26088,9 +26577,12 @@
       <c r="AL135" s="10">
         <v>0</v>
       </c>
+      <c r="AM135" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="s">
+    <row r="136" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -26204,9 +26696,12 @@
       <c r="AL136" s="10">
         <v>93</v>
       </c>
+      <c r="AM136" s="10">
+        <v>96</v>
+      </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
+    <row r="137" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -26318,9 +26813,12 @@
       <c r="AL137" s="10">
         <v>115</v>
       </c>
+      <c r="AM137" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+    <row r="138" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -26432,9 +26930,12 @@
       <c r="AL138" s="10">
         <v>16</v>
       </c>
+      <c r="AM138" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A139" s="35"/>
+    <row r="139" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -26545,10 +27046,25 @@
       </c>
       <c r="AL139" s="10">
         <v>147</v>
+      </c>
+      <c r="AM139" s="10">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -26561,18 +27077,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -26883,7 +27387,7 @@
       </c>
       <c r="AU2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>21.748400852878465</v>
       </c>
       <c r="AV2" s="18">
         <f t="shared" si="1"/>
@@ -27533,7 +28037,7 @@
       </c>
       <c r="AU4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.9019607843137258</v>
       </c>
       <c r="AV4" s="10">
         <f t="shared" si="7"/>
@@ -27858,7 +28362,7 @@
       </c>
       <c r="AU6" s="12">
         <f>MAX(0, (dc!AU2-dc!AT2))</f>
-        <v>0</v>
+        <v>469</v>
       </c>
       <c r="AV6" s="12">
         <f>MAX(0, (dc!AV2-dc!AU2))</f>
@@ -28182,7 +28686,7 @@
       </c>
       <c r="AU7" s="12">
         <f>MAX(0, (dc!AU3-dc!AT3))</f>
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="AV7" s="12">
         <f>MAX(0, (dc!AV3-dc!AU3))</f>
@@ -28830,7 +29334,7 @@
       </c>
       <c r="AU9" s="12">
         <f>MAX(0, (dc!AU5-dc!AT5))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV9" s="12">
         <f>MAX(0, (dc!AV5-dc!AU5))</f>
@@ -29382,7 +29886,7 @@
       </c>
       <c r="AU11" s="10">
         <f>MAX(0,(dc!AU7-dc!AT7))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AV11" s="10">
         <f>MAX(0,(dc!AV7-dc!AU7))</f>
@@ -29689,7 +30193,7 @@
       </c>
       <c r="AU12" s="10">
         <f>MAX(0,(dc!AU8-dc!AT8))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV12" s="10">
         <f>MAX(0,(dc!AV8-dc!AU8))</f>
@@ -29996,7 +30500,7 @@
       </c>
       <c r="AU13" s="10">
         <f>MAX(0,(dc!AU9-dc!AT9))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AV13" s="10">
         <f>MAX(0,(dc!AV9-dc!AU9))</f>
@@ -30303,7 +30807,7 @@
       </c>
       <c r="AU14" s="10">
         <f>MAX(0,(dc!AU10-dc!AT10))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AV14" s="10">
         <f>MAX(0,(dc!AV10-dc!AU10))</f>
@@ -30610,7 +31114,7 @@
       </c>
       <c r="AU15" s="10">
         <f>MAX(0,(dc!AU11-dc!AT11))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AV15" s="10">
         <f>MAX(0,(dc!AV11-dc!AU11))</f>
@@ -30917,7 +31421,7 @@
       </c>
       <c r="AU16" s="10">
         <f>MAX(0,(dc!AU12-dc!AT12))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AV16" s="10">
         <f>MAX(0,(dc!AV12-dc!AU12))</f>
@@ -31224,7 +31728,7 @@
       </c>
       <c r="AU17" s="10">
         <f>MAX(0,(dc!AU13-dc!AT13))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AV17" s="10">
         <f>MAX(0,(dc!AV13-dc!AU13))</f>
@@ -31531,7 +32035,7 @@
       </c>
       <c r="AU18" s="10">
         <f>MAX(0,(dc!AU14-dc!AT14))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AV18" s="10">
         <f>MAX(0,(dc!AV14-dc!AU14))</f>
@@ -32081,10 +32585,10 @@
   <dimension ref="A1:BQ70"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="10" topLeftCell="G11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="AJ20" sqref="AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32235,7 +32739,7 @@
       </c>
       <c r="AJ2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.285510857956567</v>
       </c>
       <c r="AK2" s="20">
         <f t="shared" si="0"/>
@@ -32508,7 +33012,7 @@
       </c>
       <c r="AJ3" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>26.677316293929714</v>
       </c>
       <c r="AK3" s="20">
         <f t="shared" si="3"/>
@@ -32781,7 +33285,7 @@
       </c>
       <c r="AJ4" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.341853035143771</v>
       </c>
       <c r="AK4" s="20">
         <f t="shared" si="5"/>
@@ -33117,7 +33621,7 @@
       </c>
       <c r="AJ6" s="14">
         <f>MAX(0,(md!AJ2-md!AI2)+(md!AJ3-md!AI3))</f>
-        <v>0</v>
+        <v>2809</v>
       </c>
       <c r="AK6" s="14">
         <f>MAX(0,(md!AK2-md!AJ2)+(md!AK3-md!AJ3))</f>
@@ -33389,7 +33893,7 @@
       </c>
       <c r="AJ7" s="14">
         <f>MAX(0,(md!AJ3-md!AI3))</f>
-        <v>0</v>
+        <v>626</v>
       </c>
       <c r="AK7" s="14">
         <f>MAX(0,(md!AK3-md!AJ3))</f>
@@ -33661,7 +34165,7 @@
       </c>
       <c r="AJ8" s="14">
         <f>MAX(0,(md!AJ4-md!AI4))</f>
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="AK8" s="14">
         <f>MAX(0,(md!AK4-md!AJ4))</f>
@@ -33933,7 +34437,7 @@
       </c>
       <c r="AJ9" s="14">
         <f>MAX(0,(md!AJ5-md!AI5))</f>
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="AK9" s="14">
         <f>MAX(0,(md!AK5-md!AJ5))</f>
@@ -34419,7 +34923,7 @@
       </c>
       <c r="AJ11" s="14">
         <f>MAX(0,(md!AJ7-md!AI7))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK11" s="14">
         <f>MAX(0,(md!AK7-md!AJ7))</f>
@@ -34696,7 +35200,7 @@
       </c>
       <c r="AJ12" s="14">
         <f>MAX(0,(md!AJ8-md!AI8))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AK12" s="14">
         <f>MAX(0,(md!AK8-md!AJ8))</f>
@@ -34973,7 +35477,7 @@
       </c>
       <c r="AJ13" s="14">
         <f>MAX(0,(md!AJ9-md!AI9))</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="AK13" s="14">
         <f>MAX(0,(md!AK9-md!AJ9))</f>
@@ -35250,7 +35754,7 @@
       </c>
       <c r="AJ14" s="14">
         <f>MAX(0,(md!AJ10-md!AI10))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="AK14" s="14">
         <f>MAX(0,(md!AK10-md!AJ10))</f>
@@ -35527,7 +36031,7 @@
       </c>
       <c r="AJ15" s="14">
         <f>MAX(0,(md!AJ11-md!AI11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15" s="14">
         <f>MAX(0,(md!AK11-md!AJ11))</f>
@@ -35804,7 +36308,7 @@
       </c>
       <c r="AJ16" s="14">
         <f>MAX(0,(md!AJ12-md!AI12))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK16" s="14">
         <f>MAX(0,(md!AK12-md!AJ12))</f>
@@ -36081,7 +36585,7 @@
       </c>
       <c r="AJ17" s="14">
         <f>MAX(0,(md!AJ13-md!AI13))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AK17" s="14">
         <f>MAX(0,(md!AK13-md!AJ13))</f>
@@ -36635,7 +37139,7 @@
       </c>
       <c r="AJ19" s="14">
         <f>MAX(0,(md!AJ15-md!AI15))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK19" s="14">
         <f>MAX(0,(md!AK15-md!AJ15))</f>
@@ -36912,7 +37416,7 @@
       </c>
       <c r="AJ20" s="14">
         <f>MAX(0,(md!AJ16-md!AI16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK20" s="14">
         <f>MAX(0,(md!AK16-md!AJ16))</f>
@@ -37189,7 +37693,7 @@
       </c>
       <c r="AJ21" s="14">
         <f>MAX(0,(md!AJ17-md!AI17))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK21" s="14">
         <f>MAX(0,(md!AK17-md!AJ17))</f>
@@ -37743,7 +38247,7 @@
       </c>
       <c r="AJ23" s="14">
         <f>MAX(0,(md!AJ19-md!AI19))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK23" s="14">
         <f>MAX(0,(md!AK19-md!AJ19))</f>
@@ -38020,7 +38524,7 @@
       </c>
       <c r="AJ24" s="14">
         <f>MAX(0,(md!AJ20-md!AI20))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AK24" s="14">
         <f>MAX(0,(md!AK20-md!AJ20))</f>
@@ -38297,7 +38801,7 @@
       </c>
       <c r="AJ25" s="14">
         <f>MAX(0,(md!AJ21-md!AI21))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK25" s="14">
         <f>MAX(0,(md!AK21-md!AJ21))</f>
@@ -38574,7 +39078,7 @@
       </c>
       <c r="AJ26" s="14">
         <f>MAX(0,(md!AJ22-md!AI22))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="AK26" s="14">
         <f>MAX(0,(md!AK22-md!AJ22))</f>
@@ -38851,7 +39355,7 @@
       </c>
       <c r="AJ27" s="14">
         <f>MAX(0,(md!AJ23-md!AI23))</f>
-        <v>0</v>
+        <v>233</v>
       </c>
       <c r="AK27" s="14">
         <f>MAX(0,(md!AK23-md!AJ23))</f>
@@ -39128,7 +39632,7 @@
       </c>
       <c r="AJ28" s="14">
         <f>MAX(0,(md!AJ24-md!AI24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK28" s="14">
         <f>MAX(0,(md!AK24-md!AJ24))</f>
@@ -39405,7 +39909,7 @@
       </c>
       <c r="AJ29" s="14">
         <f>MAX(0,(md!AJ25-md!AI25))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK29" s="14">
         <f>MAX(0,(md!AK25-md!AJ25))</f>
@@ -39682,7 +40186,7 @@
       </c>
       <c r="AJ30" s="14">
         <f>MAX(0,(md!AJ26-md!AI26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK30" s="14">
         <f>MAX(0,(md!AK26-md!AJ26))</f>
@@ -40236,7 +40740,7 @@
       </c>
       <c r="AJ32" s="14">
         <f>MAX(0,(md!AJ28-md!AI28))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK32" s="14">
         <f>MAX(0,(md!AK28-md!AJ28))</f>
@@ -40513,7 +41017,7 @@
       </c>
       <c r="AJ33" s="14">
         <f>MAX(0,(md!AJ29-md!AI29))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK33" s="14">
         <f>MAX(0,(md!AK29-md!AJ29))</f>
@@ -40790,7 +41294,7 @@
       </c>
       <c r="AJ34" s="14">
         <f>MAX(0,(md!AJ30-md!AI30))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK34" s="14">
         <f>MAX(0,(md!AK30-md!AJ30))</f>
@@ -41107,7 +41611,7 @@
   <dimension ref="A1:BS143"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AK6" sqref="AK6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41269,7 +41773,7 @@
       </c>
       <c r="AL2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31.247570928876801</v>
       </c>
       <c r="AM2" s="19">
         <f t="shared" si="1"/>
@@ -41546,7 +42050,7 @@
       </c>
       <c r="AL3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12.313432835820896</v>
       </c>
       <c r="AM3" s="19">
         <f t="shared" si="3"/>
@@ -41823,7 +42327,7 @@
       </c>
       <c r="AL4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.2288557213930353</v>
       </c>
       <c r="AM4" s="19">
         <f t="shared" si="5"/>
@@ -42100,7 +42604,7 @@
       </c>
       <c r="AL6" s="14">
         <f>MAX(0,(va!AM5-va!AL5))</f>
-        <v>0</v>
+        <v>2573</v>
       </c>
       <c r="AM6" s="14">
         <f>MAX(0,(va!AN5-va!AM5))</f>
@@ -42377,7 +42881,7 @@
       </c>
       <c r="AL7" s="14">
         <f>MAX(0,(va!AM2-va!AL2))</f>
-        <v>0</v>
+        <v>804</v>
       </c>
       <c r="AM7" s="14">
         <f>MAX(0,(va!AN2-va!AM2))</f>
@@ -42654,7 +43158,7 @@
       </c>
       <c r="AL8" s="14">
         <f>MAX(0,(va!AM3-va!AL3))</f>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AM8" s="14">
         <f>MAX(0,(va!AN3-va!AM3))</f>
@@ -42931,7 +43435,7 @@
       </c>
       <c r="AL9" s="14">
         <f>MAX(0,(va!AM4-va!AL4))</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AM9" s="14">
         <f>MAX(0,(va!AN4-va!AM4))</f>
@@ -43428,7 +43932,7 @@
       </c>
       <c r="AL11" s="16">
         <f>MAX(0,(va!AM7-va!AL7))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AM11" s="16">
         <f>MAX(0,(va!AN7-va!AM7))</f>
@@ -45120,7 +45624,7 @@
       </c>
       <c r="AL17" s="16">
         <f>MAX(0,(va!AM13-va!AL13))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM17" s="16">
         <f>MAX(0,(va!AN13-va!AM13))</f>
@@ -45402,7 +45906,7 @@
       </c>
       <c r="AL18" s="16">
         <f>MAX(0,(va!AM14-va!AL14))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AM18" s="16">
         <f>MAX(0,(va!AN14-va!AM14))</f>
@@ -45684,7 +46188,7 @@
       </c>
       <c r="AL19" s="16">
         <f>MAX(0,(va!AM15-va!AL15))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM19" s="16">
         <f>MAX(0,(va!AN15-va!AM15))</f>
@@ -46248,7 +46752,7 @@
       </c>
       <c r="AL21" s="16">
         <f>MAX(0,(va!AM17-va!AL17))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM21" s="16">
         <f>MAX(0,(va!AN17-va!AM17))</f>
@@ -46812,7 +47316,7 @@
       </c>
       <c r="AL23" s="16">
         <f>MAX(0,(va!AM19-va!AL19))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AM23" s="16">
         <f>MAX(0,(va!AN19-va!AM19))</f>
@@ -47376,7 +47880,7 @@
       </c>
       <c r="AL25" s="16">
         <f>MAX(0,(va!AM21-va!AL21))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AM25" s="16">
         <f>MAX(0,(va!AN21-va!AM21))</f>
@@ -47940,7 +48444,7 @@
       </c>
       <c r="AL27" s="16">
         <f>MAX(0,(va!AM23-va!AL23))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM27" s="16">
         <f>MAX(0,(va!AN23-va!AM23))</f>
@@ -49914,7 +50418,7 @@
       </c>
       <c r="AL34" s="16">
         <f>MAX(0,(va!AM30-va!AL30))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM34" s="16">
         <f>MAX(0,(va!AN30-va!AM30))</f>
@@ -50196,7 +50700,7 @@
       </c>
       <c r="AL35" s="16">
         <f>MAX(0,(va!AM31-va!AL31))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AM35" s="16">
         <f>MAX(0,(va!AN31-va!AM31))</f>
@@ -50760,7 +51264,7 @@
       </c>
       <c r="AL37" s="16">
         <f>MAX(0,(va!AM33-va!AL33))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM37" s="16">
         <f>MAX(0,(va!AN33-va!AM33))</f>
@@ -51324,7 +51828,7 @@
       </c>
       <c r="AL39" s="16">
         <f>MAX(0,(va!AM35-va!AL35))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM39" s="16">
         <f>MAX(0,(va!AN35-va!AM35))</f>
@@ -51606,7 +52110,7 @@
       </c>
       <c r="AL40" s="16">
         <f>MAX(0,(va!AM36-va!AL36))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM40" s="16">
         <f>MAX(0,(va!AN36-va!AM36))</f>
@@ -51888,7 +52392,7 @@
       </c>
       <c r="AL41" s="16">
         <f>MAX(0,(va!AM37-va!AL37))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM41" s="16">
         <f>MAX(0,(va!AN37-va!AM37))</f>
@@ -54426,7 +54930,7 @@
       </c>
       <c r="AL50" s="16">
         <f>MAX(0,(va!AM46-va!AL46))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM50" s="16">
         <f>MAX(0,(va!AN46-va!AM46))</f>
@@ -55554,7 +56058,7 @@
       </c>
       <c r="AL54" s="16">
         <f>MAX(0,(va!AM50-va!AL50))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AM54" s="16">
         <f>MAX(0,(va!AN50-va!AM50))</f>
@@ -55836,7 +56340,7 @@
       </c>
       <c r="AL55" s="16">
         <f>MAX(0,(va!AM51-va!AL51))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AM55" s="16">
         <f>MAX(0,(va!AN51-va!AM51))</f>
@@ -56118,7 +56622,7 @@
       </c>
       <c r="AL56" s="16">
         <f>MAX(0,(va!AM52-va!AL52))</f>
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="AM56" s="16">
         <f>MAX(0,(va!AN52-va!AM52))</f>
@@ -57246,7 +57750,7 @@
       </c>
       <c r="AL60" s="16">
         <f>MAX(0,(va!AM56-va!AL56))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AM60" s="16">
         <f>MAX(0,(va!AN56-va!AM56))</f>
@@ -57528,7 +58032,7 @@
       </c>
       <c r="AL61" s="16">
         <f>MAX(0,(va!AM57-va!AL57))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM61" s="16">
         <f>MAX(0,(va!AN57-va!AM57))</f>
@@ -57810,7 +58314,7 @@
       </c>
       <c r="AL62" s="16">
         <f>MAX(0,(va!AM58-va!AL58))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM62" s="16">
         <f>MAX(0,(va!AN58-va!AM58))</f>
@@ -58092,7 +58596,7 @@
       </c>
       <c r="AL63" s="16">
         <f>MAX(0,(va!AM59-va!AL59))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM63" s="16">
         <f>MAX(0,(va!AN59-va!AM59))</f>
@@ -58938,7 +59442,7 @@
       </c>
       <c r="AL66" s="16">
         <f>MAX(0,(va!AM62-va!AL62))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM66" s="16">
         <f>MAX(0,(va!AN62-va!AM62))</f>
@@ -59220,7 +59724,7 @@
       </c>
       <c r="AL67" s="16">
         <f>MAX(0,(va!AM63-va!AL63))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM67" s="16">
         <f>MAX(0,(va!AN63-va!AM63))</f>
@@ -59502,7 +60006,7 @@
       </c>
       <c r="AL68" s="16">
         <f>MAX(0,(va!AM64-va!AL64))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM68" s="16">
         <f>MAX(0,(va!AN64-va!AM64))</f>
@@ -59784,7 +60288,7 @@
       </c>
       <c r="AL69" s="16">
         <f>MAX(0,(va!AM65-va!AL65))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM69" s="16">
         <f>MAX(0,(va!AN65-va!AM65))</f>
@@ -60066,7 +60570,7 @@
       </c>
       <c r="AL70" s="16">
         <f>MAX(0,(va!AM66-va!AL66))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM70" s="16">
         <f>MAX(0,(va!AN66-va!AM66))</f>
@@ -60348,7 +60852,7 @@
       </c>
       <c r="AL71" s="16">
         <f>MAX(0,(va!AM67-va!AL67))</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AM71" s="16">
         <f>MAX(0,(va!AN67-va!AM67))</f>
@@ -61194,7 +61698,7 @@
       </c>
       <c r="AL74" s="16">
         <f>MAX(0,(va!AM70-va!AL70))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM74" s="16">
         <f>MAX(0,(va!AN70-va!AM70))</f>
@@ -62604,7 +63108,7 @@
       </c>
       <c r="AL79" s="16">
         <f>MAX(0,(va!AM75-va!AL75))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM79" s="16">
         <f>MAX(0,(va!AN75-va!AM75))</f>
@@ -64296,7 +64800,7 @@
       </c>
       <c r="AL85" s="16">
         <f>MAX(0,(va!AM81-va!AL81))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM85" s="16">
         <f>MAX(0,(va!AN81-va!AM81))</f>
@@ -64578,7 +65082,7 @@
       </c>
       <c r="AL86" s="16">
         <f>MAX(0,(va!AM82-va!AL82))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM86" s="16">
         <f>MAX(0,(va!AN82-va!AM82))</f>
@@ -64860,7 +65364,7 @@
       </c>
       <c r="AL87" s="16">
         <f>MAX(0,(va!AM83-va!AL83))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM87" s="16">
         <f>MAX(0,(va!AN83-va!AM83))</f>
@@ -65706,7 +66210,7 @@
       </c>
       <c r="AL90" s="16">
         <f>MAX(0,(va!AM86-va!AL86))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM90" s="16">
         <f>MAX(0,(va!AN86-va!AM86))</f>
@@ -66270,7 +66774,7 @@
       </c>
       <c r="AL92" s="16">
         <f>MAX(0,(va!AM88-va!AL88))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AM92" s="16">
         <f>MAX(0,(va!AN88-va!AM88))</f>
@@ -66834,7 +67338,7 @@
       </c>
       <c r="AL94" s="16">
         <f>MAX(0,(va!AM90-va!AL90))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM94" s="16">
         <f>MAX(0,(va!AN90-va!AM90))</f>
@@ -68526,7 +69030,7 @@
       </c>
       <c r="AL100" s="16">
         <f>MAX(0,(va!AM96-va!AL96))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AM100" s="16">
         <f>MAX(0,(va!AN96-va!AM96))</f>
@@ -68808,7 +69312,7 @@
       </c>
       <c r="AL101" s="16">
         <f>MAX(0,(va!AM97-va!AL97))</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="AM101" s="16">
         <f>MAX(0,(va!AN97-va!AM97))</f>
@@ -69090,7 +69594,7 @@
       </c>
       <c r="AL102" s="16">
         <f>MAX(0,(va!AM98-va!AL98))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AM102" s="16">
         <f>MAX(0,(va!AN98-va!AM98))</f>
@@ -69372,7 +69876,7 @@
       </c>
       <c r="AL103" s="16">
         <f>MAX(0,(va!AM99-va!AL99))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM103" s="16">
         <f>MAX(0,(va!AN99-va!AM99))</f>
@@ -69654,7 +70158,7 @@
       </c>
       <c r="AL104" s="16">
         <f>MAX(0,(va!AM100-va!AL100))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM104" s="16">
         <f>MAX(0,(va!AN100-va!AM100))</f>
@@ -69936,7 +70440,7 @@
       </c>
       <c r="AL105" s="16">
         <f>MAX(0,(va!AM101-va!AL101))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM105" s="16">
         <f>MAX(0,(va!AN101-va!AM101))</f>
@@ -70218,7 +70722,7 @@
       </c>
       <c r="AL106" s="16">
         <f>MAX(0,(va!AM102-va!AL102))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AM106" s="16">
         <f>MAX(0,(va!AN102-va!AM102))</f>
@@ -70500,7 +71004,7 @@
       </c>
       <c r="AL107" s="16">
         <f>MAX(0,(va!AM103-va!AL103))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM107" s="16">
         <f>MAX(0,(va!AN103-va!AM103))</f>
@@ -70782,7 +71286,7 @@
       </c>
       <c r="AL108" s="16">
         <f>MAX(0,(va!AM104-va!AL104))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM108" s="16">
         <f>MAX(0,(va!AN104-va!AM104))</f>
@@ -71064,7 +71568,7 @@
       </c>
       <c r="AL109" s="16">
         <f>MAX(0,(va!AM105-va!AL105))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AM109" s="16">
         <f>MAX(0,(va!AN105-va!AM105))</f>
@@ -71346,7 +71850,7 @@
       </c>
       <c r="AL110" s="16">
         <f>MAX(0,(va!AM106-va!AL106))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AM110" s="16">
         <f>MAX(0,(va!AN106-va!AM106))</f>
@@ -71910,7 +72414,7 @@
       </c>
       <c r="AL112" s="16">
         <f>MAX(0,(va!AM108-va!AL108))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM112" s="16">
         <f>MAX(0,(va!AN108-va!AM108))</f>
@@ -72192,7 +72696,7 @@
       </c>
       <c r="AL113" s="16">
         <f>MAX(0,(va!AM109-va!AL109))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM113" s="16">
         <f>MAX(0,(va!AN109-va!AM109))</f>
@@ -72474,7 +72978,7 @@
       </c>
       <c r="AL114" s="16">
         <f>MAX(0,(va!AM110-va!AL110))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM114" s="16">
         <f>MAX(0,(va!AN110-va!AM110))</f>
@@ -72756,7 +73260,7 @@
       </c>
       <c r="AL115" s="16">
         <f>MAX(0,(va!AM111-va!AL111))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM115" s="16">
         <f>MAX(0,(va!AN111-va!AM111))</f>
@@ -73602,7 +74106,7 @@
       </c>
       <c r="AL118" s="16">
         <f>MAX(0,(va!AM114-va!AL114))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM118" s="16">
         <f>MAX(0,(va!AN114-va!AM114))</f>
@@ -73884,7 +74388,7 @@
       </c>
       <c r="AL119" s="16">
         <f>MAX(0,(va!AM115-va!AL115))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM119" s="16">
         <f>MAX(0,(va!AN115-va!AM115))</f>
@@ -75294,7 +75798,7 @@
       </c>
       <c r="AL124" s="16">
         <f>MAX(0,(va!AM120-va!AL120))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM124" s="16">
         <f>MAX(0,(va!AN120-va!AM120))</f>
@@ -77832,7 +78336,7 @@
       </c>
       <c r="AL133" s="16">
         <f>MAX(0,(va!AM129-va!AL129))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AM133" s="16">
         <f>MAX(0,(va!AN129-va!AM129))</f>
@@ -78114,7 +78618,7 @@
       </c>
       <c r="AL134" s="16">
         <f>MAX(0,(va!AM130-va!AL130))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM134" s="16">
         <f>MAX(0,(va!AN130-va!AM130))</f>
@@ -78396,7 +78900,7 @@
       </c>
       <c r="AL135" s="16">
         <f>MAX(0,(va!AM131-va!AL131))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM135" s="16">
         <f>MAX(0,(va!AN131-va!AM131))</f>
@@ -78678,7 +79182,7 @@
       </c>
       <c r="AL136" s="16">
         <f>MAX(0,(va!AM132-va!AL132))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM136" s="16">
         <f>MAX(0,(va!AN132-va!AM132))</f>
@@ -78960,7 +79464,7 @@
       </c>
       <c r="AL137" s="16">
         <f>MAX(0,(va!AM133-va!AL133))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM137" s="16">
         <f>MAX(0,(va!AN133-va!AM133))</f>
@@ -79524,7 +80028,7 @@
       </c>
       <c r="AL139" s="16">
         <f>MAX(0,(va!AM135-va!AL135))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM139" s="16">
         <f>MAX(0,(va!AN135-va!AM135))</f>
@@ -79806,7 +80310,7 @@
       </c>
       <c r="AL140" s="16">
         <f>MAX(0,(va!AM136-va!AL136))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM140" s="16">
         <f>MAX(0,(va!AN136-va!AM136))</f>
@@ -80370,7 +80874,7 @@
       </c>
       <c r="AL142" s="16">
         <f>MAX(0,(va!AM138-va!AL138))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM142" s="16">
         <f>MAX(0,(va!AN138-va!AM138))</f>
@@ -80652,7 +81156,7 @@
       </c>
       <c r="AL143" s="16">
         <f>MAX(0,(va!AM139-va!AL139))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM143" s="16">
         <f>MAX(0,(va!AN139-va!AM139))</f>

</xml_diff>

<commit_message>
29 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803C940-261A-42A9-A4C1-0B2446A42A1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB04DD1-4059-4111-A6D7-C7FCFAE19FF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4018,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AU2" sqref="AU2"/>
+      <selection pane="bottomRight" activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4176,6 +4176,9 @@
       <c r="AU2" s="12">
         <v>18885</v>
       </c>
+      <c r="AV2" s="12">
+        <v>19229</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4352,7 +4355,7 @@
       </c>
       <c r="AV3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4106</v>
       </c>
       <c r="AW3" s="10">
         <f t="shared" si="0"/>
@@ -4634,6 +4637,9 @@
       <c r="AU5" s="10">
         <v>190</v>
       </c>
+      <c r="AV5" s="10">
+        <v>205</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5022,6 +5028,9 @@
       <c r="AU7" s="10">
         <v>475</v>
       </c>
+      <c r="AV7" s="10">
+        <v>503</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5165,6 +5174,9 @@
       <c r="AU8" s="10">
         <v>266</v>
       </c>
+      <c r="AV8" s="10">
+        <v>284</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5308,6 +5320,9 @@
       <c r="AU9" s="10">
         <v>264</v>
       </c>
+      <c r="AV9" s="10">
+        <v>270</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5451,6 +5466,9 @@
       <c r="AU10" s="10">
         <v>702</v>
       </c>
+      <c r="AV10" s="10">
+        <v>727</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5594,6 +5612,9 @@
       <c r="AU11" s="10">
         <v>587</v>
       </c>
+      <c r="AV11" s="10">
+        <v>622</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5737,6 +5758,9 @@
       <c r="AU12" s="10">
         <v>414</v>
       </c>
+      <c r="AV12" s="10">
+        <v>433</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5880,6 +5904,9 @@
       <c r="AU13" s="10">
         <v>594</v>
       </c>
+      <c r="AV13" s="10">
+        <v>630</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6023,6 +6050,9 @@
       <c r="AU14" s="10">
         <v>560</v>
       </c>
+      <c r="AV14" s="10">
+        <v>597</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6165,6 +6195,9 @@
       </c>
       <c r="AU15" s="10">
         <v>132</v>
+      </c>
+      <c r="AV15" s="10">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6419,7 +6452,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ2" sqref="AJ2"/>
+      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6545,7 +6578,7 @@
         <v>87672</v>
       </c>
       <c r="AK2" s="10">
-        <v>0</v>
+        <v>90080</v>
       </c>
       <c r="AL2" s="10">
         <v>0</v>
@@ -6785,7 +6818,7 @@
       </c>
       <c r="AK3" s="10">
         <f>SUM(md[29-Apr])</f>
-        <v>0</v>
+        <v>20849</v>
       </c>
       <c r="AL3" s="10">
         <f>SUM(md[30-Apr])</f>
@@ -7023,7 +7056,7 @@
         <v>4268</v>
       </c>
       <c r="AK4" s="10">
-        <v>0</v>
+        <v>4402</v>
       </c>
       <c r="AL4" s="10">
         <v>0</v>
@@ -7229,7 +7262,7 @@
         <v>929</v>
       </c>
       <c r="AK5" s="10">
-        <v>0</v>
+        <v>985</v>
       </c>
       <c r="AL5" s="10">
         <v>0</v>
@@ -7646,6 +7679,9 @@
       <c r="AJ7">
         <v>115</v>
       </c>
+      <c r="AK7">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7756,6 +7792,9 @@
       <c r="AJ8" s="10">
         <v>1571</v>
       </c>
+      <c r="AK8" s="10">
+        <v>1662</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7866,6 +7905,9 @@
       <c r="AJ9">
         <v>1977</v>
       </c>
+      <c r="AK9">
+        <v>2014</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -7976,6 +8018,9 @@
       <c r="AJ10">
         <v>2631</v>
       </c>
+      <c r="AK10">
+        <v>2740</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8086,6 +8131,9 @@
       <c r="AJ11">
         <v>139</v>
       </c>
+      <c r="AK11">
+        <v>142</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8196,6 +8244,9 @@
       <c r="AJ12">
         <v>69</v>
       </c>
+      <c r="AK12">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8306,6 +8357,9 @@
       <c r="AJ13">
         <v>416</v>
       </c>
+      <c r="AK13">
+        <v>421</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8416,6 +8470,9 @@
       <c r="AJ14">
         <v>163</v>
       </c>
+      <c r="AK14">
+        <v>164</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8526,6 +8583,9 @@
       <c r="AJ15">
         <v>539</v>
       </c>
+      <c r="AK15">
+        <v>551</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8636,8 +8696,11 @@
       <c r="AJ16" s="10">
         <v>52</v>
       </c>
+      <c r="AK16" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8746,8 +8809,11 @@
       <c r="AJ17">
         <v>870</v>
       </c>
+      <c r="AK17">
+        <v>893</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8856,8 +8922,11 @@
       <c r="AJ18">
         <v>4</v>
       </c>
+      <c r="AK18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -8966,8 +9035,11 @@
       <c r="AJ19">
         <v>358</v>
       </c>
+      <c r="AK19">
+        <v>371</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9076,8 +9148,11 @@
       <c r="AJ20">
         <v>802</v>
       </c>
+      <c r="AK20">
+        <v>831</v>
+      </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9186,8 +9261,11 @@
       <c r="AJ21">
         <v>73</v>
       </c>
+      <c r="AK21">
+        <v>73</v>
+      </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9296,8 +9374,11 @@
       <c r="AJ22">
         <v>4003</v>
       </c>
+      <c r="AK22">
+        <v>4152</v>
+      </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9406,8 +9487,11 @@
       <c r="AJ23">
         <v>5496</v>
       </c>
+      <c r="AK23">
+        <v>5738</v>
+      </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9516,8 +9600,11 @@
       <c r="AJ24">
         <v>55</v>
       </c>
+      <c r="AK24">
+        <v>55</v>
+      </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9626,8 +9713,11 @@
       <c r="AJ25">
         <v>145</v>
       </c>
+      <c r="AK25">
+        <v>145</v>
+      </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9736,8 +9826,11 @@
       <c r="AJ26">
         <v>20</v>
       </c>
+      <c r="AK26">
+        <v>21</v>
+      </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -9846,8 +9939,11 @@
       <c r="AJ27">
         <v>34</v>
       </c>
+      <c r="AK27">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -9956,8 +10052,11 @@
       <c r="AJ28">
         <v>187</v>
       </c>
+      <c r="AK28">
+        <v>197</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -10066,8 +10165,11 @@
       <c r="AJ29">
         <v>340</v>
       </c>
+      <c r="AK29">
+        <v>350</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10176,8 +10278,11 @@
       <c r="AJ30">
         <v>54</v>
       </c>
+      <c r="AK30">
+        <v>55</v>
+      </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10271,10 +10376,10 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="U15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AM3" sqref="AM3"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10444,7 +10549,7 @@
       </c>
       <c r="AN2" s="10">
         <f>SUM(va[29-Apr])</f>
-        <v>0</v>
+        <v>14961</v>
       </c>
       <c r="AO2" s="10">
         <f>SUM(va[30-Apr])</f>
@@ -10685,7 +10790,7 @@
         <v>2165</v>
       </c>
       <c r="AN3" s="10">
-        <v>0</v>
+        <v>2259</v>
       </c>
       <c r="AO3" s="10">
         <v>0</v>
@@ -10894,7 +10999,7 @@
         <v>492</v>
       </c>
       <c r="AN4" s="10">
-        <v>0</v>
+        <v>522</v>
       </c>
       <c r="AO4" s="10">
         <v>0</v>
@@ -11103,7 +11208,7 @@
         <v>82753</v>
       </c>
       <c r="AN5" s="10">
-        <v>0</v>
+        <v>85307</v>
       </c>
       <c r="AO5" s="10">
         <v>0</v>
@@ -11538,9 +11643,12 @@
       <c r="AM7" s="10">
         <v>653</v>
       </c>
+      <c r="AN7" s="10">
+        <v>700</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11657,9 +11765,12 @@
       <c r="AM8" s="10">
         <v>5</v>
       </c>
+      <c r="AN8" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11774,9 +11885,12 @@
       <c r="AM9" s="10">
         <v>27</v>
       </c>
+      <c r="AN9" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -11891,9 +12005,12 @@
       <c r="AM10" s="10">
         <v>2</v>
       </c>
+      <c r="AN10" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -12008,9 +12125,12 @@
       <c r="AM11" s="10">
         <v>41</v>
       </c>
+      <c r="AN11" s="10">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -12125,9 +12245,12 @@
       <c r="AM12" s="10">
         <v>1</v>
       </c>
+      <c r="AN12" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -12241,6 +12364,9 @@
       </c>
       <c r="AM13" s="10">
         <v>12</v>
+      </c>
+      <c r="AN13" s="10">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
@@ -12361,9 +12487,12 @@
       <c r="AM14" s="10">
         <v>865</v>
       </c>
+      <c r="AN14" s="10">
+        <v>912</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12480,9 +12609,12 @@
       <c r="AM15" s="10">
         <v>39</v>
       </c>
+      <c r="AN15" s="10">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -12597,9 +12729,12 @@
       <c r="AM16" s="10">
         <v>0</v>
       </c>
+      <c r="AN16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12714,9 +12849,12 @@
       <c r="AM17" s="10">
         <v>2</v>
       </c>
+      <c r="AN17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -12831,9 +12969,12 @@
       <c r="AM18" s="10">
         <v>5</v>
       </c>
+      <c r="AN18" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -12948,9 +13089,12 @@
       <c r="AM19" s="10">
         <v>216</v>
       </c>
+      <c r="AN19" s="10">
+        <v>220</v>
+      </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -13065,9 +13209,12 @@
       <c r="AM20" s="10">
         <v>5</v>
       </c>
+      <c r="AN20" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -13182,9 +13329,12 @@
       <c r="AM21" s="10">
         <v>406</v>
       </c>
+      <c r="AN21" s="10">
+        <v>411</v>
+      </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -13299,9 +13449,12 @@
       <c r="AM22" s="10">
         <v>3</v>
       </c>
+      <c r="AN22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -13416,9 +13569,12 @@
       <c r="AM23" s="10">
         <v>11</v>
       </c>
+      <c r="AN23" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -13533,9 +13689,12 @@
       <c r="AM24" s="10">
         <v>11</v>
       </c>
+      <c r="AN24" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -13652,9 +13811,12 @@
       <c r="AM25" s="10">
         <v>9</v>
       </c>
+      <c r="AN25" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -13769,9 +13931,12 @@
       <c r="AM26" s="10">
         <v>17</v>
       </c>
+      <c r="AN26" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -13886,9 +14051,12 @@
       <c r="AM27" s="10">
         <v>25</v>
       </c>
+      <c r="AN27" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -14003,9 +14171,12 @@
       <c r="AM28" s="10">
         <v>11</v>
       </c>
+      <c r="AN28" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -14120,8 +14291,11 @@
       <c r="AM29" s="10">
         <v>51</v>
       </c>
+      <c r="AN29" s="10">
+        <v>52</v>
+      </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -14239,9 +14413,12 @@
       <c r="AM30" s="10">
         <v>220</v>
       </c>
+      <c r="AN30" s="10">
+        <v>232</v>
+      </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -14358,9 +14535,12 @@
       <c r="AM31" s="10">
         <v>488</v>
       </c>
+      <c r="AN31" s="10">
+        <v>501</v>
+      </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -14475,9 +14655,12 @@
       <c r="AM32" s="10">
         <v>11</v>
       </c>
+      <c r="AN32" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -14592,9 +14775,12 @@
       <c r="AM33" s="10">
         <v>47</v>
       </c>
+      <c r="AN33" s="10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -14711,9 +14897,12 @@
       <c r="AM34" s="10">
         <v>13</v>
       </c>
+      <c r="AN34" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -14828,9 +15017,12 @@
       <c r="AM35" s="10">
         <v>74</v>
       </c>
+      <c r="AN35" s="10">
+        <v>74</v>
+      </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -14945,9 +15137,12 @@
       <c r="AM36" s="10">
         <v>109</v>
       </c>
+      <c r="AN36" s="10">
+        <v>113</v>
+      </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -15062,9 +15257,12 @@
       <c r="AM37" s="10">
         <v>21</v>
       </c>
+      <c r="AN37" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -15181,9 +15379,12 @@
       <c r="AM38" s="10">
         <v>15</v>
       </c>
+      <c r="AN38" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -15298,9 +15499,12 @@
       <c r="AM39" s="10">
         <v>36</v>
       </c>
+      <c r="AN39" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -15415,9 +15619,12 @@
       <c r="AM40" s="10">
         <v>31</v>
       </c>
+      <c r="AN40" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -15532,9 +15739,12 @@
       <c r="AM41" s="10">
         <v>4</v>
       </c>
+      <c r="AN41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -15649,9 +15859,12 @@
       <c r="AM42" s="10">
         <v>30</v>
       </c>
+      <c r="AN42" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -15766,9 +15979,12 @@
       <c r="AM43" s="10">
         <v>20</v>
       </c>
+      <c r="AN43" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -15883,9 +16099,12 @@
       <c r="AM44" s="10">
         <v>24</v>
       </c>
+      <c r="AN44" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -16000,9 +16219,12 @@
       <c r="AM45" s="10">
         <v>30</v>
       </c>
+      <c r="AN45" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -16119,9 +16341,12 @@
       <c r="AM46" s="10">
         <v>16</v>
       </c>
+      <c r="AN46" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -16236,9 +16461,12 @@
       <c r="AM47" s="10">
         <v>0</v>
       </c>
+      <c r="AN47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -16353,9 +16581,12 @@
       <c r="AM48" s="10">
         <v>3</v>
       </c>
+      <c r="AN48" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -16470,9 +16701,12 @@
       <c r="AM49" s="10">
         <v>5</v>
       </c>
+      <c r="AN49" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -16589,9 +16823,12 @@
       <c r="AM50" s="10">
         <v>223</v>
       </c>
+      <c r="AN50" s="10">
+        <v>229</v>
+      </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -16706,9 +16943,12 @@
       <c r="AM51" s="10">
         <v>35</v>
       </c>
+      <c r="AN51" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -16825,9 +17065,12 @@
       <c r="AM52" s="10">
         <v>3278</v>
       </c>
+      <c r="AN52" s="10">
+        <v>3448</v>
+      </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -16942,9 +17185,12 @@
       <c r="AM53" s="10">
         <v>27</v>
       </c>
+      <c r="AN53" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A54" s="32"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -17059,8 +17305,11 @@
       <c r="AM54" s="10">
         <v>26</v>
       </c>
+      <c r="AN54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -17178,8 +17427,11 @@
       <c r="AM55" s="10">
         <v>108</v>
       </c>
+      <c r="AN55" s="10">
+        <v>109</v>
+      </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -17297,9 +17549,12 @@
       <c r="AM56" s="10">
         <v>835</v>
       </c>
+      <c r="AN56" s="10">
+        <v>846</v>
+      </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -17416,9 +17671,12 @@
       <c r="AM57" s="10">
         <v>9</v>
       </c>
+      <c r="AN57" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -17533,9 +17791,12 @@
       <c r="AM58" s="10">
         <v>7</v>
       </c>
+      <c r="AN58" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
+    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -17650,9 +17911,12 @@
       <c r="AM59" s="10">
         <v>22</v>
       </c>
+      <c r="AN59" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -17767,9 +18031,12 @@
       <c r="AM60" s="10">
         <v>2</v>
       </c>
+      <c r="AN60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -17886,9 +18153,12 @@
       <c r="AM61" s="10">
         <v>7</v>
       </c>
+      <c r="AN61" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+    <row r="62" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -18003,9 +18273,12 @@
       <c r="AM62" s="10">
         <v>97</v>
       </c>
+      <c r="AN62" s="10">
+        <v>101</v>
+      </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
+    <row r="63" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -18120,9 +18393,12 @@
       <c r="AM63" s="10">
         <v>89</v>
       </c>
+      <c r="AN63" s="10">
+        <v>91</v>
+      </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+    <row r="64" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -18237,9 +18513,12 @@
       <c r="AM64" s="10">
         <v>79</v>
       </c>
+      <c r="AN64" s="10">
+        <v>95</v>
+      </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+    <row r="65" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -18354,9 +18633,12 @@
       <c r="AM65" s="10">
         <v>47</v>
       </c>
+      <c r="AN65" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+    <row r="66" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A66" s="32"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -18471,8 +18753,11 @@
       <c r="AM66" s="10">
         <v>36</v>
       </c>
+      <c r="AN66" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -18590,9 +18875,12 @@
       <c r="AM67" s="10">
         <v>688</v>
       </c>
+      <c r="AN67" s="10">
+        <v>727</v>
+      </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+    <row r="68" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -18709,9 +18997,12 @@
       <c r="AM68" s="10">
         <v>0</v>
       </c>
+      <c r="AN68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+    <row r="69" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -18826,9 +19117,12 @@
       <c r="AM69" s="10">
         <v>4</v>
       </c>
+      <c r="AN69" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+    <row r="70" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -18943,9 +19237,12 @@
       <c r="AM70" s="10">
         <v>1</v>
       </c>
+      <c r="AN70" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+    <row r="71" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A71" s="31"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -19060,9 +19357,12 @@
       <c r="AM71" s="10">
         <v>13</v>
       </c>
+      <c r="AN71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+    <row r="72" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A72" s="31"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -19177,9 +19477,12 @@
       <c r="AM72" s="10">
         <v>34</v>
       </c>
+      <c r="AN72" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+    <row r="73" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A73" s="31"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -19294,9 +19597,12 @@
       <c r="AM73" s="10">
         <v>11</v>
       </c>
+      <c r="AN73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
+    <row r="74" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A74" s="31"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -19411,9 +19717,12 @@
       <c r="AM74" s="10">
         <v>1</v>
       </c>
+      <c r="AN74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+    <row r="75" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A75" s="32"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -19528,9 +19837,12 @@
       <c r="AM75" s="10">
         <v>4</v>
       </c>
+      <c r="AN75" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+    <row r="76" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A76" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -19647,9 +19959,12 @@
       <c r="AM76" s="10">
         <v>1</v>
       </c>
+      <c r="AN76" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+    <row r="77" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A77" s="34"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -19764,9 +20079,12 @@
       <c r="AM77" s="10">
         <v>4</v>
       </c>
+      <c r="AN77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
+    <row r="78" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A78" s="34"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -19881,9 +20199,12 @@
       <c r="AM78" s="10">
         <v>54</v>
       </c>
+      <c r="AN78" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
+    <row r="79" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A79" s="34"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -19998,9 +20319,12 @@
       <c r="AM79" s="10">
         <v>9</v>
       </c>
+      <c r="AN79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+    <row r="80" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -20115,8 +20439,11 @@
       <c r="AM80" s="10">
         <v>3</v>
       </c>
+      <c r="AN80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -20234,9 +20561,12 @@
       <c r="AM81" s="10">
         <v>188</v>
       </c>
+      <c r="AN81" s="10">
+        <v>192</v>
+      </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A82" s="30" t="s">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -20353,9 +20683,12 @@
       <c r="AM82" s="10">
         <v>155</v>
       </c>
+      <c r="AN82" s="10">
+        <v>155</v>
+      </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
+    <row r="83" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A83" s="34"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -20470,9 +20803,12 @@
       <c r="AM83" s="10">
         <v>45</v>
       </c>
+      <c r="AN83" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+    <row r="84" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A84" s="34"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -20587,9 +20923,12 @@
       <c r="AM84" s="10">
         <v>112</v>
       </c>
+      <c r="AN84" s="10">
+        <v>114</v>
+      </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+    <row r="85" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A85" s="34"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -20704,9 +21043,12 @@
       <c r="AM85" s="10">
         <v>6</v>
       </c>
+      <c r="AN85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
+    <row r="86" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A86" s="35"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -20821,9 +21163,12 @@
       <c r="AM86" s="10">
         <v>18</v>
       </c>
+      <c r="AN86" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A87" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -20940,9 +21285,12 @@
       <c r="AM87" s="10">
         <v>15</v>
       </c>
+      <c r="AN87" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+    <row r="88" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -21057,9 +21405,12 @@
       <c r="AM88" s="10">
         <v>55</v>
       </c>
+      <c r="AN88" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
+    <row r="89" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -21174,9 +21525,12 @@
       <c r="AM89" s="10">
         <v>7</v>
       </c>
+      <c r="AN89" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
+    <row r="90" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -21291,9 +21645,12 @@
       <c r="AM90" s="10">
         <v>11</v>
       </c>
+      <c r="AN90" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
+    <row r="91" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -21408,9 +21765,12 @@
       <c r="AM91" s="10">
         <v>4</v>
       </c>
+      <c r="AN91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
+    <row r="92" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -21525,9 +21885,12 @@
       <c r="AM92" s="10">
         <v>11</v>
       </c>
+      <c r="AN92" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+    <row r="93" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A93" s="32"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -21642,9 +22005,12 @@
       <c r="AM93" s="10">
         <v>41</v>
       </c>
+      <c r="AN93" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -21761,9 +22127,12 @@
       <c r="AM94" s="10">
         <v>11</v>
       </c>
+      <c r="AN94" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
+    <row r="95" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A95" s="35"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -21878,8 +22247,11 @@
       <c r="AM95" s="10">
         <v>33</v>
       </c>
+      <c r="AN95" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -21997,9 +22369,12 @@
       <c r="AM96" s="10">
         <v>149</v>
       </c>
+      <c r="AN96" s="10">
+        <v>150</v>
+      </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A97" s="33" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -22116,9 +22491,12 @@
       <c r="AM97" s="10">
         <v>1449</v>
       </c>
+      <c r="AN97" s="10">
+        <v>1527</v>
+      </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+    <row r="98" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A98" s="34"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -22233,9 +22611,12 @@
       <c r="AM98" s="10">
         <v>175</v>
       </c>
+      <c r="AN98" s="10">
+        <v>196</v>
+      </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
+    <row r="99" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A99" s="35"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -22350,9 +22731,12 @@
       <c r="AM99" s="10">
         <v>53</v>
       </c>
+      <c r="AN99" s="10">
+        <v>60</v>
+      </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A100" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -22469,9 +22853,12 @@
       <c r="AM100" s="10">
         <v>22</v>
       </c>
+      <c r="AN100" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
+    <row r="101" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -22586,9 +22973,12 @@
       <c r="AM101" s="10">
         <v>30</v>
       </c>
+      <c r="AN101" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
+    <row r="102" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -22703,9 +23093,12 @@
       <c r="AM102" s="10">
         <v>126</v>
       </c>
+      <c r="AN102" s="10">
+        <v>131</v>
+      </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
+    <row r="103" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -22820,9 +23213,12 @@
       <c r="AM103" s="10">
         <v>221</v>
       </c>
+      <c r="AN103" s="10">
+        <v>225</v>
+      </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
+    <row r="104" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A104" s="32"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -22937,9 +23333,12 @@
       <c r="AM104" s="10">
         <v>27</v>
       </c>
+      <c r="AN104" s="10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A105" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -23056,9 +23455,12 @@
       <c r="AM105" s="10">
         <v>126</v>
       </c>
+      <c r="AN105" s="10">
+        <v>129</v>
+      </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+    <row r="106" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A106" s="34"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -23173,9 +23575,12 @@
       <c r="AM106" s="10">
         <v>105</v>
       </c>
+      <c r="AN106" s="10">
+        <v>109</v>
+      </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+    <row r="107" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A107" s="34"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -23290,9 +23695,12 @@
       <c r="AM107" s="10">
         <v>14</v>
       </c>
+      <c r="AN107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+    <row r="108" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A108" s="34"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -23407,9 +23815,12 @@
       <c r="AM108" s="10">
         <v>27</v>
       </c>
+      <c r="AN108" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A109" s="32"/>
+    <row r="109" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A109" s="35"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -23524,8 +23935,11 @@
       <c r="AM109" s="10">
         <v>3</v>
       </c>
+      <c r="AN109" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -23643,8 +24057,11 @@
       <c r="AM110" s="10">
         <v>312</v>
       </c>
+      <c r="AN110" s="10">
+        <v>323</v>
+      </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -23762,9 +24179,12 @@
       <c r="AM111" s="10">
         <v>35</v>
       </c>
+      <c r="AN111" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A112" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -23881,9 +24301,12 @@
       <c r="AM112" s="10">
         <v>13</v>
       </c>
+      <c r="AN112" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+    <row r="113" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -23998,9 +24421,12 @@
       <c r="AM113" s="10">
         <v>17</v>
       </c>
+      <c r="AN113" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+    <row r="114" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A114" s="32"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -24115,9 +24541,12 @@
       <c r="AM114" s="10">
         <v>100</v>
       </c>
+      <c r="AN114" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A115" s="30" t="s">
+    <row r="115" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A115" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -24234,9 +24663,12 @@
       <c r="AM115" s="10">
         <v>80</v>
       </c>
+      <c r="AN115" s="10">
+        <v>81</v>
+      </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A116" s="31"/>
+    <row r="116" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A116" s="34"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -24351,9 +24783,12 @@
       <c r="AM116" s="10">
         <v>73</v>
       </c>
+      <c r="AN116" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
+    <row r="117" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A117" s="34"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -24468,9 +24903,12 @@
       <c r="AM117" s="10">
         <v>9</v>
       </c>
+      <c r="AN117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
+    <row r="118" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A118" s="34"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -24585,9 +25023,12 @@
       <c r="AM118" s="10">
         <v>41</v>
       </c>
+      <c r="AN118" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
+    <row r="119" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A119" s="34"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -24702,9 +25143,12 @@
       <c r="AM119" s="10">
         <v>7</v>
       </c>
+      <c r="AN119" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="120" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+    <row r="120" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A120" s="35"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -24819,9 +25263,12 @@
       <c r="AM120" s="10">
         <v>51</v>
       </c>
+      <c r="AN120" s="10">
+        <v>52</v>
+      </c>
     </row>
-    <row r="121" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A121" s="33" t="s">
+    <row r="121" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A121" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -24938,9 +25385,12 @@
       <c r="AM121" s="10">
         <v>6</v>
       </c>
+      <c r="AN121" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="122" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
+    <row r="122" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -25055,9 +25505,12 @@
       <c r="AM122" s="10">
         <v>22</v>
       </c>
+      <c r="AN122" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="123" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+    <row r="123" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -25172,9 +25625,12 @@
       <c r="AM123" s="10">
         <v>2</v>
       </c>
+      <c r="AN123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+    <row r="124" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -25289,9 +25745,12 @@
       <c r="AM124" s="10">
         <v>5</v>
       </c>
+      <c r="AN124" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
+    <row r="125" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -25406,9 +25865,12 @@
       <c r="AM125" s="10">
         <v>1</v>
       </c>
+      <c r="AN125" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+    <row r="126" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -25523,9 +25985,12 @@
       <c r="AM126" s="10">
         <v>4</v>
       </c>
+      <c r="AN126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+    <row r="127" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -25640,9 +26105,12 @@
       <c r="AM127" s="10">
         <v>4</v>
       </c>
+      <c r="AN127" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
+    <row r="128" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -25757,9 +26225,12 @@
       <c r="AM128" s="10">
         <v>8</v>
       </c>
+      <c r="AN128" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="129" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+    <row r="129" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A129" s="31"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -25874,9 +26345,12 @@
       <c r="AM129" s="10">
         <v>141</v>
       </c>
+      <c r="AN129" s="10">
+        <v>143</v>
+      </c>
     </row>
-    <row r="130" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+    <row r="130" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A130" s="32"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -25991,8 +26465,11 @@
       <c r="AM130" s="10">
         <v>21</v>
       </c>
+      <c r="AN130" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="131" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -26110,9 +26587,12 @@
       <c r="AM131" s="10">
         <v>359</v>
       </c>
+      <c r="AN131" s="10">
+        <v>365</v>
+      </c>
     </row>
-    <row r="132" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A132" s="33" t="s">
+    <row r="132" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A132" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -26229,9 +26709,12 @@
       <c r="AM132" s="10">
         <v>20</v>
       </c>
+      <c r="AN132" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="133" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+    <row r="133" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A133" s="31"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -26346,9 +26829,12 @@
       <c r="AM133" s="10">
         <v>16</v>
       </c>
+      <c r="AN133" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="134" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+    <row r="134" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A134" s="31"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -26463,9 +26949,12 @@
       <c r="AM134" s="10">
         <v>2</v>
       </c>
+      <c r="AN134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A135" s="35"/>
+    <row r="135" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A135" s="32"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -26580,9 +27069,12 @@
       <c r="AM135" s="10">
         <v>2</v>
       </c>
+      <c r="AN135" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="136" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+    <row r="136" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A136" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -26699,9 +27191,12 @@
       <c r="AM136" s="10">
         <v>96</v>
       </c>
+      <c r="AN136" s="10">
+        <v>96</v>
+      </c>
     </row>
-    <row r="137" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
+    <row r="137" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A137" s="34"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -26816,9 +27311,12 @@
       <c r="AM137" s="10">
         <v>115</v>
       </c>
+      <c r="AN137" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="138" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
+    <row r="138" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A138" s="34"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -26933,9 +27431,12 @@
       <c r="AM138" s="10">
         <v>18</v>
       </c>
+      <c r="AN138" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="139" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A139" s="32"/>
+    <row r="139" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A139" s="35"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -27049,10 +27550,25 @@
       </c>
       <c r="AM139" s="10">
         <v>152</v>
+      </c>
+      <c r="AN139" s="10">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -27065,18 +27581,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -27391,7 +27895,7 @@
       </c>
       <c r="AV2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32.558139534883722</v>
       </c>
       <c r="AW2" s="18">
         <f t="shared" si="1"/>
@@ -28041,7 +28545,7 @@
       </c>
       <c r="AV4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>13.392857142857142</v>
       </c>
       <c r="AW4" s="10">
         <f t="shared" si="7"/>
@@ -28366,7 +28870,7 @@
       </c>
       <c r="AV6" s="12">
         <f>MAX(0, (dc!AV2-dc!AU2))</f>
-        <v>0</v>
+        <v>344</v>
       </c>
       <c r="AW6" s="12">
         <f>MAX(0, (dc!AW2-dc!AV2))</f>
@@ -28690,7 +29194,7 @@
       </c>
       <c r="AV7" s="12">
         <f>MAX(0, (dc!AV3-dc!AU3))</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="AW7" s="12">
         <f>MAX(0, (dc!AW3-dc!AV3))</f>
@@ -29338,7 +29842,7 @@
       </c>
       <c r="AV9" s="12">
         <f>MAX(0, (dc!AV5-dc!AU5))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AW9" s="12">
         <f>MAX(0, (dc!AW5-dc!AV5))</f>
@@ -29890,7 +30394,7 @@
       </c>
       <c r="AV11" s="10">
         <f>MAX(0,(dc!AV7-dc!AU7))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AW11" s="10">
         <f>MAX(0,(dc!AW7-dc!AV7))</f>
@@ -30197,7 +30701,7 @@
       </c>
       <c r="AV12" s="10">
         <f>MAX(0,(dc!AV8-dc!AU8))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AW12" s="10">
         <f>MAX(0,(dc!AW8-dc!AV8))</f>
@@ -30504,7 +31008,7 @@
       </c>
       <c r="AV13" s="10">
         <f>MAX(0,(dc!AV9-dc!AU9))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW13" s="10">
         <f>MAX(0,(dc!AW9-dc!AV9))</f>
@@ -30811,7 +31315,7 @@
       </c>
       <c r="AV14" s="10">
         <f>MAX(0,(dc!AV10-dc!AU10))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AW14" s="10">
         <f>MAX(0,(dc!AW10-dc!AV10))</f>
@@ -31118,7 +31622,7 @@
       </c>
       <c r="AV15" s="10">
         <f>MAX(0,(dc!AV11-dc!AU11))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AW15" s="10">
         <f>MAX(0,(dc!AW11-dc!AV11))</f>
@@ -31425,7 +31929,7 @@
       </c>
       <c r="AV16" s="10">
         <f>MAX(0,(dc!AV12-dc!AU12))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AW16" s="10">
         <f>MAX(0,(dc!AW12-dc!AV12))</f>
@@ -31732,7 +32236,7 @@
       </c>
       <c r="AV17" s="10">
         <f>MAX(0,(dc!AV13-dc!AU13))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AW17" s="10">
         <f>MAX(0,(dc!AW13-dc!AV13))</f>
@@ -32039,7 +32543,7 @@
       </c>
       <c r="AV18" s="10">
         <f>MAX(0,(dc!AV14-dc!AU14))</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AW18" s="10">
         <f>MAX(0,(dc!AW14-dc!AV14))</f>
@@ -32743,7 +33247,7 @@
       </c>
       <c r="AK2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23.409669211195929</v>
       </c>
       <c r="AL2" s="20">
         <f t="shared" si="0"/>
@@ -33016,7 +33520,7 @@
       </c>
       <c r="AK3" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>18.206521739130434</v>
       </c>
       <c r="AL3" s="20">
         <f t="shared" si="3"/>
@@ -33289,7 +33793,7 @@
       </c>
       <c r="AK4" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.608695652173914</v>
       </c>
       <c r="AL4" s="20">
         <f t="shared" si="5"/>
@@ -33625,7 +34129,7 @@
       </c>
       <c r="AK6" s="14">
         <f>MAX(0,(md!AK2-md!AJ2)+(md!AK3-md!AJ3))</f>
-        <v>0</v>
+        <v>3144</v>
       </c>
       <c r="AL6" s="14">
         <f>MAX(0,(md!AL2-md!AK2)+(md!AL3-md!AK3))</f>
@@ -33897,7 +34401,7 @@
       </c>
       <c r="AK7" s="14">
         <f>MAX(0,(md!AK3-md!AJ3))</f>
-        <v>0</v>
+        <v>736</v>
       </c>
       <c r="AL7" s="14">
         <f>MAX(0,(md!AL3-md!AK3))</f>
@@ -34169,7 +34673,7 @@
       </c>
       <c r="AK8" s="14">
         <f>MAX(0,(md!AK4-md!AJ4))</f>
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="AL8" s="14">
         <f>MAX(0,(md!AL4-md!AK4))</f>
@@ -34441,7 +34945,7 @@
       </c>
       <c r="AK9" s="14">
         <f>MAX(0,(md!AK5-md!AJ5))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AL9" s="14">
         <f>MAX(0,(md!AL5-md!AK5))</f>
@@ -34927,7 +35431,7 @@
       </c>
       <c r="AK11" s="14">
         <f>MAX(0,(md!AK7-md!AJ7))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL11" s="14">
         <f>MAX(0,(md!AL7-md!AK7))</f>
@@ -35204,7 +35708,7 @@
       </c>
       <c r="AK12" s="14">
         <f>MAX(0,(md!AK8-md!AJ8))</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="AL12" s="14">
         <f>MAX(0,(md!AL8-md!AK8))</f>
@@ -35481,7 +35985,7 @@
       </c>
       <c r="AK13" s="14">
         <f>MAX(0,(md!AK9-md!AJ9))</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AL13" s="14">
         <f>MAX(0,(md!AL9-md!AK9))</f>
@@ -35758,7 +36262,7 @@
       </c>
       <c r="AK14" s="14">
         <f>MAX(0,(md!AK10-md!AJ10))</f>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="AL14" s="14">
         <f>MAX(0,(md!AL10-md!AK10))</f>
@@ -36035,7 +36539,7 @@
       </c>
       <c r="AK15" s="14">
         <f>MAX(0,(md!AK11-md!AJ11))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL15" s="14">
         <f>MAX(0,(md!AL11-md!AK11))</f>
@@ -36589,7 +37093,7 @@
       </c>
       <c r="AK17" s="14">
         <f>MAX(0,(md!AK13-md!AJ13))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL17" s="14">
         <f>MAX(0,(md!AL13-md!AK13))</f>
@@ -36866,7 +37370,7 @@
       </c>
       <c r="AK18" s="14">
         <f>MAX(0,(md!AK14-md!AJ14))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL18" s="14">
         <f>MAX(0,(md!AL14-md!AK14))</f>
@@ -37143,7 +37647,7 @@
       </c>
       <c r="AK19" s="14">
         <f>MAX(0,(md!AK15-md!AJ15))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AL19" s="14">
         <f>MAX(0,(md!AL15-md!AK15))</f>
@@ -37697,7 +38201,7 @@
       </c>
       <c r="AK21" s="14">
         <f>MAX(0,(md!AK17-md!AJ17))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AL21" s="14">
         <f>MAX(0,(md!AL17-md!AK17))</f>
@@ -38251,7 +38755,7 @@
       </c>
       <c r="AK23" s="14">
         <f>MAX(0,(md!AK19-md!AJ19))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AL23" s="14">
         <f>MAX(0,(md!AL19-md!AK19))</f>
@@ -38528,7 +39032,7 @@
       </c>
       <c r="AK24" s="14">
         <f>MAX(0,(md!AK20-md!AJ20))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AL24" s="14">
         <f>MAX(0,(md!AL20-md!AK20))</f>
@@ -39082,7 +39586,7 @@
       </c>
       <c r="AK26" s="14">
         <f>MAX(0,(md!AK22-md!AJ22))</f>
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="AL26" s="14">
         <f>MAX(0,(md!AL22-md!AK22))</f>
@@ -39359,7 +39863,7 @@
       </c>
       <c r="AK27" s="14">
         <f>MAX(0,(md!AK23-md!AJ23))</f>
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="AL27" s="14">
         <f>MAX(0,(md!AL23-md!AK23))</f>
@@ -40190,7 +40694,7 @@
       </c>
       <c r="AK30" s="14">
         <f>MAX(0,(md!AK26-md!AJ26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL30" s="14">
         <f>MAX(0,(md!AL26-md!AK26))</f>
@@ -40744,7 +41248,7 @@
       </c>
       <c r="AK32" s="14">
         <f>MAX(0,(md!AK28-md!AJ28))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL32" s="14">
         <f>MAX(0,(md!AL28-md!AK28))</f>
@@ -41021,7 +41525,7 @@
       </c>
       <c r="AK33" s="14">
         <f>MAX(0,(md!AK29-md!AJ29))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL33" s="14">
         <f>MAX(0,(md!AL29-md!AK29))</f>
@@ -41298,7 +41802,7 @@
       </c>
       <c r="AK34" s="14">
         <f>MAX(0,(md!AK30-md!AJ30))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL34" s="14">
         <f>MAX(0,(md!AL30-md!AK30))</f>
@@ -41777,7 +42281,7 @@
       </c>
       <c r="AM2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24.353954581049333</v>
       </c>
       <c r="AN2" s="19">
         <f t="shared" si="1"/>
@@ -42054,7 +42558,7 @@
       </c>
       <c r="AM3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15.112540192926044</v>
       </c>
       <c r="AN3" s="19">
         <f t="shared" si="3"/>
@@ -42331,7 +42835,7 @@
       </c>
       <c r="AM4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.823151125401929</v>
       </c>
       <c r="AN4" s="19">
         <f t="shared" si="5"/>
@@ -42608,7 +43112,7 @@
       </c>
       <c r="AM6" s="14">
         <f>MAX(0,(va!AN5-va!AM5))</f>
-        <v>0</v>
+        <v>2554</v>
       </c>
       <c r="AN6" s="14">
         <f>MAX(0,(va!AO5-va!AN5))</f>
@@ -42885,7 +43389,7 @@
       </c>
       <c r="AM7" s="14">
         <f>MAX(0,(va!AN2-va!AM2))</f>
-        <v>0</v>
+        <v>622</v>
       </c>
       <c r="AN7" s="14">
         <f>MAX(0,(va!AO2-va!AN2))</f>
@@ -43162,7 +43666,7 @@
       </c>
       <c r="AM8" s="14">
         <f>MAX(0,(va!AN3-va!AM3))</f>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="AN8" s="14">
         <f>MAX(0,(va!AO3-va!AN3))</f>
@@ -43439,7 +43943,7 @@
       </c>
       <c r="AM9" s="14">
         <f>MAX(0,(va!AN4-va!AM4))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AN9" s="14">
         <f>MAX(0,(va!AO4-va!AN4))</f>
@@ -43936,7 +44440,7 @@
       </c>
       <c r="AM11" s="16">
         <f>MAX(0,(va!AN7-va!AM7))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AN11" s="16">
         <f>MAX(0,(va!AO7-va!AN7))</f>
@@ -44218,7 +44722,7 @@
       </c>
       <c r="AM12" s="16">
         <f>MAX(0,(va!AN8-va!AM8))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN12" s="16">
         <f>MAX(0,(va!AO8-va!AN8))</f>
@@ -44500,7 +45004,7 @@
       </c>
       <c r="AM13" s="16">
         <f>MAX(0,(va!AN9-va!AM9))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN13" s="16">
         <f>MAX(0,(va!AO9-va!AN9))</f>
@@ -45064,7 +45568,7 @@
       </c>
       <c r="AM15" s="16">
         <f>MAX(0,(va!AN11-va!AM11))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN15" s="16">
         <f>MAX(0,(va!AO11-va!AN11))</f>
@@ -45628,7 +46132,7 @@
       </c>
       <c r="AM17" s="16">
         <f>MAX(0,(va!AN13-va!AM13))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN17" s="16">
         <f>MAX(0,(va!AO13-va!AN13))</f>
@@ -45910,7 +46414,7 @@
       </c>
       <c r="AM18" s="16">
         <f>MAX(0,(va!AN14-va!AM14))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AN18" s="16">
         <f>MAX(0,(va!AO14-va!AN14))</f>
@@ -46192,7 +46696,7 @@
       </c>
       <c r="AM19" s="16">
         <f>MAX(0,(va!AN15-va!AM15))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN19" s="16">
         <f>MAX(0,(va!AO15-va!AN15))</f>
@@ -47320,7 +47824,7 @@
       </c>
       <c r="AM23" s="16">
         <f>MAX(0,(va!AN19-va!AM19))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN23" s="16">
         <f>MAX(0,(va!AO19-va!AN19))</f>
@@ -47884,7 +48388,7 @@
       </c>
       <c r="AM25" s="16">
         <f>MAX(0,(va!AN21-va!AM21))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN25" s="16">
         <f>MAX(0,(va!AO21-va!AN21))</f>
@@ -48448,7 +48952,7 @@
       </c>
       <c r="AM27" s="16">
         <f>MAX(0,(va!AN23-va!AM23))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN27" s="16">
         <f>MAX(0,(va!AO23-va!AN23))</f>
@@ -49012,7 +49516,7 @@
       </c>
       <c r="AM29" s="16">
         <f>MAX(0,(va!AN25-va!AM25))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN29" s="16">
         <f>MAX(0,(va!AO25-va!AN25))</f>
@@ -49294,7 +49798,7 @@
       </c>
       <c r="AM30" s="16">
         <f>MAX(0,(va!AN26-va!AM26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN30" s="16">
         <f>MAX(0,(va!AO26-va!AN26))</f>
@@ -49576,7 +50080,7 @@
       </c>
       <c r="AM31" s="16">
         <f>MAX(0,(va!AN27-va!AM27))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN31" s="16">
         <f>MAX(0,(va!AO27-va!AN27))</f>
@@ -49858,7 +50362,7 @@
       </c>
       <c r="AM32" s="16">
         <f>MAX(0,(va!AN28-va!AM28))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN32" s="16">
         <f>MAX(0,(va!AO28-va!AN28))</f>
@@ -50140,7 +50644,7 @@
       </c>
       <c r="AM33" s="16">
         <f>MAX(0,(va!AN29-va!AM29))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN33" s="16">
         <f>MAX(0,(va!AO29-va!AN29))</f>
@@ -50422,7 +50926,7 @@
       </c>
       <c r="AM34" s="16">
         <f>MAX(0,(va!AN30-va!AM30))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AN34" s="16">
         <f>MAX(0,(va!AO30-va!AN30))</f>
@@ -50704,7 +51208,7 @@
       </c>
       <c r="AM35" s="16">
         <f>MAX(0,(va!AN31-va!AM31))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AN35" s="16">
         <f>MAX(0,(va!AO31-va!AN31))</f>
@@ -50986,7 +51490,7 @@
       </c>
       <c r="AM36" s="16">
         <f>MAX(0,(va!AN32-va!AM32))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN36" s="16">
         <f>MAX(0,(va!AO32-va!AN32))</f>
@@ -51268,7 +51772,7 @@
       </c>
       <c r="AM37" s="16">
         <f>MAX(0,(va!AN33-va!AM33))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN37" s="16">
         <f>MAX(0,(va!AO33-va!AN33))</f>
@@ -52114,7 +52618,7 @@
       </c>
       <c r="AM40" s="16">
         <f>MAX(0,(va!AN36-va!AM36))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN40" s="16">
         <f>MAX(0,(va!AO36-va!AN36))</f>
@@ -52396,7 +52900,7 @@
       </c>
       <c r="AM41" s="16">
         <f>MAX(0,(va!AN37-va!AM37))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN41" s="16">
         <f>MAX(0,(va!AO37-va!AN37))</f>
@@ -52960,7 +53464,7 @@
       </c>
       <c r="AM43" s="16">
         <f>MAX(0,(va!AN39-va!AM39))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN43" s="16">
         <f>MAX(0,(va!AO39-va!AN39))</f>
@@ -53242,7 +53746,7 @@
       </c>
       <c r="AM44" s="16">
         <f>MAX(0,(va!AN40-va!AM40))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN44" s="16">
         <f>MAX(0,(va!AO40-va!AN40))</f>
@@ -54088,7 +54592,7 @@
       </c>
       <c r="AM47" s="16">
         <f>MAX(0,(va!AN43-va!AM43))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN47" s="16">
         <f>MAX(0,(va!AO43-va!AN43))</f>
@@ -54652,7 +55156,7 @@
       </c>
       <c r="AM49" s="16">
         <f>MAX(0,(va!AN45-va!AM45))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN49" s="16">
         <f>MAX(0,(va!AO45-va!AN45))</f>
@@ -55780,7 +56284,7 @@
       </c>
       <c r="AM53" s="16">
         <f>MAX(0,(va!AN49-va!AM49))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN53" s="16">
         <f>MAX(0,(va!AO49-va!AN49))</f>
@@ -56062,7 +56566,7 @@
       </c>
       <c r="AM54" s="16">
         <f>MAX(0,(va!AN50-va!AM50))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN54" s="16">
         <f>MAX(0,(va!AO50-va!AN50))</f>
@@ -56344,7 +56848,7 @@
       </c>
       <c r="AM55" s="16">
         <f>MAX(0,(va!AN51-va!AM51))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN55" s="16">
         <f>MAX(0,(va!AO51-va!AN51))</f>
@@ -56626,7 +57130,7 @@
       </c>
       <c r="AM56" s="16">
         <f>MAX(0,(va!AN52-va!AM52))</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="AN56" s="16">
         <f>MAX(0,(va!AO52-va!AN52))</f>
@@ -57472,7 +57976,7 @@
       </c>
       <c r="AM59" s="16">
         <f>MAX(0,(va!AN55-va!AM55))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN59" s="16">
         <f>MAX(0,(va!AO55-va!AN55))</f>
@@ -57754,7 +58258,7 @@
       </c>
       <c r="AM60" s="16">
         <f>MAX(0,(va!AN56-va!AM56))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AN60" s="16">
         <f>MAX(0,(va!AO56-va!AN56))</f>
@@ -59164,7 +59668,7 @@
       </c>
       <c r="AM65" s="16">
         <f>MAX(0,(va!AN61-va!AM61))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN65" s="16">
         <f>MAX(0,(va!AO61-va!AN61))</f>
@@ -59446,7 +59950,7 @@
       </c>
       <c r="AM66" s="16">
         <f>MAX(0,(va!AN62-va!AM62))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN66" s="16">
         <f>MAX(0,(va!AO62-va!AN62))</f>
@@ -59728,7 +60232,7 @@
       </c>
       <c r="AM67" s="16">
         <f>MAX(0,(va!AN63-va!AM63))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN67" s="16">
         <f>MAX(0,(va!AO63-va!AN63))</f>
@@ -60010,7 +60514,7 @@
       </c>
       <c r="AM68" s="16">
         <f>MAX(0,(va!AN64-va!AM64))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AN68" s="16">
         <f>MAX(0,(va!AO64-va!AN64))</f>
@@ -60292,7 +60796,7 @@
       </c>
       <c r="AM69" s="16">
         <f>MAX(0,(va!AN65-va!AM65))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN69" s="16">
         <f>MAX(0,(va!AO65-va!AN65))</f>
@@ -60856,7 +61360,7 @@
       </c>
       <c r="AM71" s="16">
         <f>MAX(0,(va!AN67-va!AM67))</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AN71" s="16">
         <f>MAX(0,(va!AO67-va!AN67))</f>
@@ -61420,7 +61924,7 @@
       </c>
       <c r="AM73" s="16">
         <f>MAX(0,(va!AN69-va!AM69))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN73" s="16">
         <f>MAX(0,(va!AO69-va!AN69))</f>
@@ -62266,7 +62770,7 @@
       </c>
       <c r="AM76" s="16">
         <f>MAX(0,(va!AN72-va!AM72))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN76" s="16">
         <f>MAX(0,(va!AO72-va!AN72))</f>
@@ -63394,7 +63898,7 @@
       </c>
       <c r="AM80" s="16">
         <f>MAX(0,(va!AN76-va!AM76))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN80" s="16">
         <f>MAX(0,(va!AO76-va!AN76))</f>
@@ -63958,7 +64462,7 @@
       </c>
       <c r="AM82" s="16">
         <f>MAX(0,(va!AN78-va!AM78))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN82" s="16">
         <f>MAX(0,(va!AO78-va!AN78))</f>
@@ -64804,7 +65308,7 @@
       </c>
       <c r="AM85" s="16">
         <f>MAX(0,(va!AN81-va!AM81))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN85" s="16">
         <f>MAX(0,(va!AO81-va!AN81))</f>
@@ -65650,7 +66154,7 @@
       </c>
       <c r="AM88" s="16">
         <f>MAX(0,(va!AN84-va!AM84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN88" s="16">
         <f>MAX(0,(va!AO84-va!AN84))</f>
@@ -67906,7 +68410,7 @@
       </c>
       <c r="AM96" s="16">
         <f>MAX(0,(va!AN92-va!AM92))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN96" s="16">
         <f>MAX(0,(va!AO92-va!AN92))</f>
@@ -68188,7 +68692,7 @@
       </c>
       <c r="AM97" s="16">
         <f>MAX(0,(va!AN93-va!AM93))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN97" s="16">
         <f>MAX(0,(va!AO93-va!AN93))</f>
@@ -68470,7 +68974,7 @@
       </c>
       <c r="AM98" s="16">
         <f>MAX(0,(va!AN94-va!AM94))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN98" s="16">
         <f>MAX(0,(va!AO94-va!AN94))</f>
@@ -68752,7 +69256,7 @@
       </c>
       <c r="AM99" s="16">
         <f>MAX(0,(va!AN95-va!AM95))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN99" s="16">
         <f>MAX(0,(va!AO95-va!AN95))</f>
@@ -69034,7 +69538,7 @@
       </c>
       <c r="AM100" s="16">
         <f>MAX(0,(va!AN96-va!AM96))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN100" s="16">
         <f>MAX(0,(va!AO96-va!AN96))</f>
@@ -69316,7 +69820,7 @@
       </c>
       <c r="AM101" s="16">
         <f>MAX(0,(va!AN97-va!AM97))</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AN101" s="16">
         <f>MAX(0,(va!AO97-va!AN97))</f>
@@ -69598,7 +70102,7 @@
       </c>
       <c r="AM102" s="16">
         <f>MAX(0,(va!AN98-va!AM98))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AN102" s="16">
         <f>MAX(0,(va!AO98-va!AN98))</f>
@@ -69880,7 +70384,7 @@
       </c>
       <c r="AM103" s="16">
         <f>MAX(0,(va!AN99-va!AM99))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AN103" s="16">
         <f>MAX(0,(va!AO99-va!AN99))</f>
@@ -70162,7 +70666,7 @@
       </c>
       <c r="AM104" s="16">
         <f>MAX(0,(va!AN100-va!AM100))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN104" s="16">
         <f>MAX(0,(va!AO100-va!AN100))</f>
@@ -70726,7 +71230,7 @@
       </c>
       <c r="AM106" s="16">
         <f>MAX(0,(va!AN102-va!AM102))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN106" s="16">
         <f>MAX(0,(va!AO102-va!AN102))</f>
@@ -71008,7 +71512,7 @@
       </c>
       <c r="AM107" s="16">
         <f>MAX(0,(va!AN103-va!AM103))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN107" s="16">
         <f>MAX(0,(va!AO103-va!AN103))</f>
@@ -71290,7 +71794,7 @@
       </c>
       <c r="AM108" s="16">
         <f>MAX(0,(va!AN104-va!AM104))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN108" s="16">
         <f>MAX(0,(va!AO104-va!AN104))</f>
@@ -71572,7 +72076,7 @@
       </c>
       <c r="AM109" s="16">
         <f>MAX(0,(va!AN105-va!AM105))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN109" s="16">
         <f>MAX(0,(va!AO105-va!AN105))</f>
@@ -71854,7 +72358,7 @@
       </c>
       <c r="AM110" s="16">
         <f>MAX(0,(va!AN106-va!AM106))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN110" s="16">
         <f>MAX(0,(va!AO106-va!AN106))</f>
@@ -72982,7 +73486,7 @@
       </c>
       <c r="AM114" s="16">
         <f>MAX(0,(va!AN110-va!AM110))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AN114" s="16">
         <f>MAX(0,(va!AO110-va!AN110))</f>
@@ -73264,7 +73768,7 @@
       </c>
       <c r="AM115" s="16">
         <f>MAX(0,(va!AN111-va!AM111))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AN115" s="16">
         <f>MAX(0,(va!AO111-va!AN111))</f>
@@ -73546,7 +74050,7 @@
       </c>
       <c r="AM116" s="16">
         <f>MAX(0,(va!AN112-va!AM112))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN116" s="16">
         <f>MAX(0,(va!AO112-va!AN112))</f>
@@ -74392,7 +74896,7 @@
       </c>
       <c r="AM119" s="16">
         <f>MAX(0,(va!AN115-va!AM115))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN119" s="16">
         <f>MAX(0,(va!AO115-va!AN115))</f>
@@ -74956,7 +75460,7 @@
       </c>
       <c r="AM121" s="16">
         <f>MAX(0,(va!AN117-va!AM117))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN121" s="16">
         <f>MAX(0,(va!AO117-va!AN117))</f>
@@ -75802,7 +76306,7 @@
       </c>
       <c r="AM124" s="16">
         <f>MAX(0,(va!AN120-va!AM120))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN124" s="16">
         <f>MAX(0,(va!AO120-va!AN120))</f>
@@ -76366,7 +76870,7 @@
       </c>
       <c r="AM126" s="16">
         <f>MAX(0,(va!AN122-va!AM122))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN126" s="16">
         <f>MAX(0,(va!AO122-va!AN122))</f>
@@ -78340,7 +78844,7 @@
       </c>
       <c r="AM133" s="16">
         <f>MAX(0,(va!AN129-va!AM129))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN133" s="16">
         <f>MAX(0,(va!AO129-va!AN129))</f>
@@ -78622,7 +79126,7 @@
       </c>
       <c r="AM134" s="16">
         <f>MAX(0,(va!AN130-va!AM130))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN134" s="16">
         <f>MAX(0,(va!AO130-va!AN130))</f>
@@ -78904,7 +79408,7 @@
       </c>
       <c r="AM135" s="16">
         <f>MAX(0,(va!AN131-va!AM131))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN135" s="16">
         <f>MAX(0,(va!AO131-va!AN131))</f>
@@ -79186,7 +79690,7 @@
       </c>
       <c r="AM136" s="16">
         <f>MAX(0,(va!AN132-va!AM132))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN136" s="16">
         <f>MAX(0,(va!AO132-va!AN132))</f>
@@ -80878,7 +81382,7 @@
       </c>
       <c r="AM142" s="16">
         <f>MAX(0,(va!AN138-va!AM138))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN142" s="16">
         <f>MAX(0,(va!AO138-va!AN138))</f>
@@ -81160,7 +81664,7 @@
       </c>
       <c r="AM143" s="16">
         <f>MAX(0,(va!AN139-va!AM139))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN143" s="16">
         <f>MAX(0,(va!AO139-va!AN139))</f>

</xml_diff>

<commit_message>
30 April data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB04DD1-4059-4111-A6D7-C7FCFAE19FF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2834A8-3B0E-4275-8794-3A6AA06061B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4018,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AV2" sqref="AV2"/>
+      <selection pane="bottomRight" activeCell="AW2" sqref="AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4179,6 +4179,9 @@
       <c r="AV2" s="12">
         <v>19229</v>
       </c>
+      <c r="AW2" s="12">
+        <v>20079</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4359,7 +4362,7 @@
       </c>
       <c r="AW3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4323</v>
       </c>
       <c r="AX3" s="10">
         <f t="shared" si="0"/>
@@ -4640,6 +4643,9 @@
       <c r="AV5" s="10">
         <v>205</v>
       </c>
+      <c r="AW5" s="10">
+        <v>224</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5031,6 +5037,9 @@
       <c r="AV7" s="10">
         <v>503</v>
       </c>
+      <c r="AW7" s="10">
+        <v>543</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5177,6 +5186,9 @@
       <c r="AV8" s="10">
         <v>284</v>
       </c>
+      <c r="AW8" s="10">
+        <v>291</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5323,6 +5335,9 @@
       <c r="AV9" s="10">
         <v>270</v>
       </c>
+      <c r="AW9" s="10">
+        <v>282</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5469,6 +5484,9 @@
       <c r="AV10" s="10">
         <v>727</v>
       </c>
+      <c r="AW10" s="10">
+        <v>774</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5615,6 +5633,9 @@
       <c r="AV11" s="10">
         <v>622</v>
       </c>
+      <c r="AW11" s="10">
+        <v>646</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5761,6 +5782,9 @@
       <c r="AV12" s="10">
         <v>433</v>
       </c>
+      <c r="AW12" s="10">
+        <v>450</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5907,6 +5931,9 @@
       <c r="AV13" s="10">
         <v>630</v>
       </c>
+      <c r="AW13" s="10">
+        <v>659</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6053,6 +6080,9 @@
       <c r="AV14" s="10">
         <v>597</v>
       </c>
+      <c r="AW14" s="10">
+        <v>632</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6198,6 +6228,9 @@
       </c>
       <c r="AV15" s="10">
         <v>40</v>
+      </c>
+      <c r="AW15" s="10">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6452,7 +6485,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
+      <selection pane="bottomRight" activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6581,7 +6614,7 @@
         <v>90080</v>
       </c>
       <c r="AL2" s="10">
-        <v>0</v>
+        <v>92617</v>
       </c>
       <c r="AM2" s="10">
         <v>0</v>
@@ -6822,7 +6855,7 @@
       </c>
       <c r="AL3" s="10">
         <f>SUM(md[30-Apr])</f>
-        <v>0</v>
+        <v>21742</v>
       </c>
       <c r="AM3" s="10">
         <f>SUM(md[1-May])</f>
@@ -7059,7 +7092,7 @@
         <v>4402</v>
       </c>
       <c r="AL4" s="10">
-        <v>0</v>
+        <v>4559</v>
       </c>
       <c r="AM4" s="10">
         <v>0</v>
@@ -7265,7 +7298,7 @@
         <v>985</v>
       </c>
       <c r="AL5" s="10">
-        <v>0</v>
+        <v>1047</v>
       </c>
       <c r="AM5" s="10">
         <v>0</v>
@@ -7682,6 +7715,9 @@
       <c r="AK7">
         <v>116</v>
       </c>
+      <c r="AL7">
+        <v>118</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7795,6 +7831,9 @@
       <c r="AK8" s="10">
         <v>1662</v>
       </c>
+      <c r="AL8" s="10">
+        <v>1725</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7908,6 +7947,9 @@
       <c r="AK9">
         <v>2014</v>
       </c>
+      <c r="AL9">
+        <v>2068</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -8021,6 +8063,9 @@
       <c r="AK10">
         <v>2740</v>
       </c>
+      <c r="AL10">
+        <v>2831</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8134,6 +8179,9 @@
       <c r="AK11">
         <v>142</v>
       </c>
+      <c r="AL11">
+        <v>150</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8247,6 +8295,9 @@
       <c r="AK12">
         <v>69</v>
       </c>
+      <c r="AL12">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8360,6 +8411,9 @@
       <c r="AK13">
         <v>421</v>
       </c>
+      <c r="AL13">
+        <v>436</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8473,6 +8527,9 @@
       <c r="AK14">
         <v>164</v>
       </c>
+      <c r="AL14">
+        <v>167</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8586,6 +8643,9 @@
       <c r="AK15">
         <v>551</v>
       </c>
+      <c r="AL15">
+        <v>564</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8699,8 +8759,11 @@
       <c r="AK16" s="10">
         <v>51</v>
       </c>
+      <c r="AL16" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8812,8 +8875,11 @@
       <c r="AK17">
         <v>893</v>
       </c>
+      <c r="AL17">
+        <v>918</v>
+      </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8925,8 +8991,11 @@
       <c r="AK18">
         <v>4</v>
       </c>
+      <c r="AL18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -9038,8 +9107,11 @@
       <c r="AK19">
         <v>371</v>
       </c>
+      <c r="AL19">
+        <v>414</v>
+      </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9151,8 +9223,11 @@
       <c r="AK20">
         <v>831</v>
       </c>
+      <c r="AL20">
+        <v>867</v>
+      </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9264,8 +9339,11 @@
       <c r="AK21">
         <v>73</v>
       </c>
+      <c r="AL21">
+        <v>79</v>
+      </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9377,8 +9455,11 @@
       <c r="AK22">
         <v>4152</v>
       </c>
+      <c r="AL22">
+        <v>4300</v>
+      </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9490,8 +9571,11 @@
       <c r="AK23">
         <v>5738</v>
       </c>
+      <c r="AL23">
+        <v>6043</v>
+      </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9603,8 +9687,11 @@
       <c r="AK24">
         <v>55</v>
       </c>
+      <c r="AL24">
+        <v>52</v>
+      </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9716,8 +9803,11 @@
       <c r="AK25">
         <v>145</v>
       </c>
+      <c r="AL25">
+        <v>150</v>
+      </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9829,8 +9919,11 @@
       <c r="AK26">
         <v>21</v>
       </c>
+      <c r="AL26">
+        <v>26</v>
+      </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -9942,8 +10035,11 @@
       <c r="AK27">
         <v>34</v>
       </c>
+      <c r="AL27">
+        <v>35</v>
+      </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -10055,8 +10151,11 @@
       <c r="AK28">
         <v>197</v>
       </c>
+      <c r="AL28">
+        <v>206</v>
+      </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -10168,8 +10267,11 @@
       <c r="AK29">
         <v>350</v>
       </c>
+      <c r="AL29">
+        <v>406</v>
+      </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10281,8 +10383,11 @@
       <c r="AK30">
         <v>55</v>
       </c>
+      <c r="AL30">
+        <v>61</v>
+      </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10376,7 +10481,7 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
@@ -10553,7 +10658,7 @@
       </c>
       <c r="AO2" s="10">
         <f>SUM(va[30-Apr])</f>
-        <v>0</v>
+        <v>15846</v>
       </c>
       <c r="AP2" s="10">
         <f>SUM(va[1-May])</f>
@@ -10793,7 +10898,7 @@
         <v>2259</v>
       </c>
       <c r="AO3" s="10">
-        <v>0</v>
+        <v>2322</v>
       </c>
       <c r="AP3" s="10">
         <v>0</v>
@@ -11002,7 +11107,7 @@
         <v>522</v>
       </c>
       <c r="AO4" s="10">
-        <v>0</v>
+        <v>552</v>
       </c>
       <c r="AP4" s="10">
         <v>0</v>
@@ -11211,7 +11316,7 @@
         <v>85307</v>
       </c>
       <c r="AO5" s="10">
-        <v>0</v>
+        <v>90843</v>
       </c>
       <c r="AP5" s="10">
         <v>0</v>
@@ -11646,9 +11751,12 @@
       <c r="AN7" s="10">
         <v>700</v>
       </c>
+      <c r="AO7" s="10">
+        <v>754</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11768,9 +11876,12 @@
       <c r="AN8" s="10">
         <v>6</v>
       </c>
+      <c r="AO8" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11888,9 +11999,12 @@
       <c r="AN9" s="10">
         <v>28</v>
       </c>
+      <c r="AO9" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -12008,9 +12122,12 @@
       <c r="AN10" s="10">
         <v>2</v>
       </c>
+      <c r="AO10" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -12128,9 +12245,12 @@
       <c r="AN11" s="10">
         <v>47</v>
       </c>
+      <c r="AO11" s="10">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -12248,9 +12368,12 @@
       <c r="AN12" s="10">
         <v>0</v>
       </c>
+      <c r="AO12" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -12367,6 +12490,9 @@
       </c>
       <c r="AN13" s="10">
         <v>16</v>
+      </c>
+      <c r="AO13" s="10">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
@@ -12490,9 +12616,12 @@
       <c r="AN14" s="10">
         <v>912</v>
       </c>
+      <c r="AO14" s="10">
+        <v>967</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12612,9 +12741,12 @@
       <c r="AN15" s="10">
         <v>41</v>
       </c>
+      <c r="AO15" s="10">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -12732,9 +12864,12 @@
       <c r="AN16" s="10">
         <v>0</v>
       </c>
+      <c r="AO16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12852,9 +12987,12 @@
       <c r="AN17" s="10">
         <v>2</v>
       </c>
+      <c r="AO17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -12972,9 +13110,12 @@
       <c r="AN18" s="10">
         <v>5</v>
       </c>
+      <c r="AO18" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -13092,9 +13233,12 @@
       <c r="AN19" s="10">
         <v>220</v>
       </c>
+      <c r="AO19" s="10">
+        <v>240</v>
+      </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -13212,9 +13356,12 @@
       <c r="AN20" s="10">
         <v>5</v>
       </c>
+      <c r="AO20" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -13332,9 +13479,12 @@
       <c r="AN21" s="10">
         <v>411</v>
       </c>
+      <c r="AO21" s="10">
+        <v>426</v>
+      </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -13452,9 +13602,12 @@
       <c r="AN22" s="10">
         <v>3</v>
       </c>
+      <c r="AO22" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -13572,9 +13725,12 @@
       <c r="AN23" s="10">
         <v>12</v>
       </c>
+      <c r="AO23" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -13692,9 +13848,12 @@
       <c r="AN24" s="10">
         <v>11</v>
       </c>
+      <c r="AO24" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -13814,9 +13973,12 @@
       <c r="AN25" s="10">
         <v>11</v>
       </c>
+      <c r="AO25" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -13934,9 +14096,12 @@
       <c r="AN26" s="10">
         <v>18</v>
       </c>
+      <c r="AO26" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -14054,9 +14219,12 @@
       <c r="AN27" s="10">
         <v>27</v>
       </c>
+      <c r="AO27" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -14174,9 +14342,12 @@
       <c r="AN28" s="10">
         <v>12</v>
       </c>
+      <c r="AO28" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -14294,8 +14465,11 @@
       <c r="AN29" s="10">
         <v>52</v>
       </c>
+      <c r="AO29" s="10">
+        <v>53</v>
+      </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -14416,9 +14590,12 @@
       <c r="AN30" s="10">
         <v>232</v>
       </c>
+      <c r="AO30" s="10">
+        <v>242</v>
+      </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -14538,9 +14715,12 @@
       <c r="AN31" s="10">
         <v>501</v>
       </c>
+      <c r="AO31" s="10">
+        <v>531</v>
+      </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -14658,9 +14838,12 @@
       <c r="AN32" s="10">
         <v>12</v>
       </c>
+      <c r="AO32" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -14778,9 +14961,12 @@
       <c r="AN33" s="10">
         <v>49</v>
       </c>
+      <c r="AO33" s="10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -14900,9 +15086,12 @@
       <c r="AN34" s="10">
         <v>13</v>
       </c>
+      <c r="AO34" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -15020,9 +15209,12 @@
       <c r="AN35" s="10">
         <v>74</v>
       </c>
+      <c r="AO35" s="10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -15140,9 +15332,12 @@
       <c r="AN36" s="10">
         <v>113</v>
       </c>
+      <c r="AO36" s="10">
+        <v>118</v>
+      </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -15260,9 +15455,12 @@
       <c r="AN37" s="10">
         <v>23</v>
       </c>
+      <c r="AO37" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -15382,9 +15580,12 @@
       <c r="AN38" s="10">
         <v>15</v>
       </c>
+      <c r="AO38" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -15502,9 +15703,12 @@
       <c r="AN39" s="10">
         <v>38</v>
       </c>
+      <c r="AO39" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -15622,9 +15826,12 @@
       <c r="AN40" s="10">
         <v>33</v>
       </c>
+      <c r="AO40" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -15742,9 +15949,12 @@
       <c r="AN41" s="10">
         <v>4</v>
       </c>
+      <c r="AO41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -15862,9 +16072,12 @@
       <c r="AN42" s="10">
         <v>30</v>
       </c>
+      <c r="AO42" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -15982,9 +16195,12 @@
       <c r="AN43" s="10">
         <v>22</v>
       </c>
+      <c r="AO43" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -16102,9 +16318,12 @@
       <c r="AN44" s="10">
         <v>24</v>
       </c>
+      <c r="AO44" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -16222,9 +16441,12 @@
       <c r="AN45" s="10">
         <v>31</v>
       </c>
+      <c r="AO45" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -16344,9 +16566,12 @@
       <c r="AN46" s="10">
         <v>16</v>
       </c>
+      <c r="AO46" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -16464,9 +16689,12 @@
       <c r="AN47" s="10">
         <v>0</v>
       </c>
+      <c r="AO47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -16584,9 +16812,12 @@
       <c r="AN48" s="10">
         <v>3</v>
       </c>
+      <c r="AO48" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -16704,9 +16935,12 @@
       <c r="AN49" s="10">
         <v>6</v>
       </c>
+      <c r="AO49" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -16826,9 +17060,12 @@
       <c r="AN50" s="10">
         <v>229</v>
       </c>
+      <c r="AO50" s="10">
+        <v>264</v>
+      </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -16946,9 +17183,12 @@
       <c r="AN51" s="10">
         <v>36</v>
       </c>
+      <c r="AO51" s="10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -17068,9 +17308,12 @@
       <c r="AN52" s="10">
         <v>3448</v>
       </c>
+      <c r="AO52" s="10">
+        <v>3611</v>
+      </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -17188,9 +17431,12 @@
       <c r="AN53" s="10">
         <v>27</v>
       </c>
+      <c r="AO53" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -17308,8 +17554,11 @@
       <c r="AN54" s="10">
         <v>26</v>
       </c>
+      <c r="AO54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -17430,8 +17679,11 @@
       <c r="AN55" s="10">
         <v>109</v>
       </c>
+      <c r="AO55" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -17552,9 +17804,12 @@
       <c r="AN56" s="10">
         <v>846</v>
       </c>
+      <c r="AO56" s="10">
+        <v>876</v>
+      </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -17674,9 +17929,12 @@
       <c r="AN57" s="10">
         <v>9</v>
       </c>
+      <c r="AO57" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -17794,9 +18052,12 @@
       <c r="AN58" s="10">
         <v>7</v>
       </c>
+      <c r="AO58" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -17914,9 +18175,12 @@
       <c r="AN59" s="10">
         <v>22</v>
       </c>
+      <c r="AO59" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -18034,9 +18298,12 @@
       <c r="AN60" s="10">
         <v>2</v>
       </c>
+      <c r="AO60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -18156,9 +18423,12 @@
       <c r="AN61" s="10">
         <v>8</v>
       </c>
+      <c r="AO61" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
+    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -18276,9 +18546,12 @@
       <c r="AN62" s="10">
         <v>101</v>
       </c>
+      <c r="AO62" s="10">
+        <v>105</v>
+      </c>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -18396,9 +18669,12 @@
       <c r="AN63" s="10">
         <v>91</v>
       </c>
+      <c r="AO63" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -18516,9 +18792,12 @@
       <c r="AN64" s="10">
         <v>95</v>
       </c>
+      <c r="AO64" s="10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -18636,9 +18915,12 @@
       <c r="AN65" s="10">
         <v>51</v>
       </c>
+      <c r="AO65" s="10">
+        <v>52</v>
+      </c>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -18756,8 +19038,11 @@
       <c r="AN66" s="10">
         <v>36</v>
       </c>
+      <c r="AO66" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -18878,9 +19163,12 @@
       <c r="AN67" s="10">
         <v>727</v>
       </c>
+      <c r="AO67" s="10">
+        <v>746</v>
+      </c>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -19000,9 +19288,12 @@
       <c r="AN68" s="10">
         <v>0</v>
       </c>
+      <c r="AO68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -19120,9 +19411,12 @@
       <c r="AN69" s="10">
         <v>9</v>
       </c>
+      <c r="AO69" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -19240,9 +19534,12 @@
       <c r="AN70" s="10">
         <v>1</v>
       </c>
+      <c r="AO70" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -19360,9 +19657,12 @@
       <c r="AN71" s="10">
         <v>13</v>
       </c>
+      <c r="AO71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -19480,9 +19780,12 @@
       <c r="AN72" s="10">
         <v>36</v>
       </c>
+      <c r="AO72" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -19600,9 +19903,12 @@
       <c r="AN73" s="10">
         <v>11</v>
       </c>
+      <c r="AO73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -19720,9 +20026,12 @@
       <c r="AN74" s="10">
         <v>1</v>
       </c>
+      <c r="AO74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -19840,9 +20149,12 @@
       <c r="AN75" s="10">
         <v>4</v>
       </c>
+      <c r="AO75" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="76" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -19962,9 +20274,12 @@
       <c r="AN76" s="10">
         <v>2</v>
       </c>
+      <c r="AO76" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -20082,9 +20397,12 @@
       <c r="AN77" s="10">
         <v>4</v>
       </c>
+      <c r="AO77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -20202,9 +20520,12 @@
       <c r="AN78" s="10">
         <v>55</v>
       </c>
+      <c r="AO78" s="10">
+        <v>56</v>
+      </c>
     </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -20322,9 +20643,12 @@
       <c r="AN79" s="10">
         <v>9</v>
       </c>
+      <c r="AO79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -20442,8 +20766,11 @@
       <c r="AN80" s="10">
         <v>3</v>
       </c>
+      <c r="AO80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -20564,9 +20891,12 @@
       <c r="AN81" s="10">
         <v>192</v>
       </c>
+      <c r="AO81" s="10">
+        <v>198</v>
+      </c>
     </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -20686,9 +21016,12 @@
       <c r="AN82" s="10">
         <v>155</v>
       </c>
+      <c r="AO82" s="10">
+        <v>158</v>
+      </c>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
+    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -20806,9 +21139,12 @@
       <c r="AN83" s="10">
         <v>45</v>
       </c>
+      <c r="AO83" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
+    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -20926,9 +21262,12 @@
       <c r="AN84" s="10">
         <v>114</v>
       </c>
+      <c r="AO84" s="10">
+        <v>118</v>
+      </c>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
+    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -21046,9 +21385,12 @@
       <c r="AN85" s="10">
         <v>6</v>
       </c>
+      <c r="AO85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
+    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -21166,9 +21508,12 @@
       <c r="AN86" s="10">
         <v>18</v>
       </c>
+      <c r="AO86" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A87" s="30" t="s">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -21288,9 +21633,12 @@
       <c r="AN87" s="10">
         <v>15</v>
       </c>
+      <c r="AO87" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -21408,9 +21756,12 @@
       <c r="AN88" s="10">
         <v>55</v>
       </c>
+      <c r="AO88" s="10">
+        <v>58</v>
+      </c>
     </row>
-    <row r="89" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -21528,9 +21879,12 @@
       <c r="AN89" s="10">
         <v>7</v>
       </c>
+      <c r="AO89" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -21648,9 +22002,12 @@
       <c r="AN90" s="10">
         <v>11</v>
       </c>
+      <c r="AO90" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="91" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -21768,9 +22125,12 @@
       <c r="AN91" s="10">
         <v>4</v>
       </c>
+      <c r="AO91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A92" s="31"/>
+    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -21888,9 +22248,12 @@
       <c r="AN92" s="10">
         <v>12</v>
       </c>
+      <c r="AO92" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
+    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -22008,9 +22371,12 @@
       <c r="AN93" s="10">
         <v>46</v>
       </c>
+      <c r="AO93" s="10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -22130,9 +22496,12 @@
       <c r="AN94" s="10">
         <v>12</v>
       </c>
+      <c r="AO94" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -22250,8 +22619,11 @@
       <c r="AN95" s="10">
         <v>34</v>
       </c>
+      <c r="AO95" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -22372,9 +22744,12 @@
       <c r="AN96" s="10">
         <v>150</v>
       </c>
+      <c r="AO96" s="10">
+        <v>158</v>
+      </c>
     </row>
-    <row r="97" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A97" s="33" t="s">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -22494,9 +22869,12 @@
       <c r="AN97" s="10">
         <v>1527</v>
       </c>
+      <c r="AO97" s="10">
+        <v>1645</v>
+      </c>
     </row>
-    <row r="98" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
+    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -22614,9 +22992,12 @@
       <c r="AN98" s="10">
         <v>196</v>
       </c>
+      <c r="AO98" s="10">
+        <v>216</v>
+      </c>
     </row>
-    <row r="99" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A99" s="35"/>
+    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -22734,9 +23115,12 @@
       <c r="AN99" s="10">
         <v>60</v>
       </c>
+      <c r="AO99" s="10">
+        <v>61</v>
+      </c>
     </row>
-    <row r="100" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -22856,9 +23240,12 @@
       <c r="AN100" s="10">
         <v>25</v>
       </c>
+      <c r="AO100" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="101" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -22976,9 +23363,12 @@
       <c r="AN101" s="10">
         <v>30</v>
       </c>
+      <c r="AO101" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="102" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -23096,9 +23486,12 @@
       <c r="AN102" s="10">
         <v>131</v>
       </c>
+      <c r="AO102" s="10">
+        <v>143</v>
+      </c>
     </row>
-    <row r="103" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -23216,9 +23609,12 @@
       <c r="AN103" s="10">
         <v>225</v>
       </c>
+      <c r="AO103" s="10">
+        <v>240</v>
+      </c>
     </row>
-    <row r="104" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
+    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -23336,9 +23732,12 @@
       <c r="AN104" s="10">
         <v>28</v>
       </c>
+      <c r="AO104" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="105" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -23458,9 +23857,12 @@
       <c r="AN105" s="10">
         <v>129</v>
       </c>
+      <c r="AO105" s="10">
+        <v>141</v>
+      </c>
     </row>
-    <row r="106" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
+    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -23578,9 +23980,12 @@
       <c r="AN106" s="10">
         <v>109</v>
       </c>
+      <c r="AO106" s="10">
+        <v>111</v>
+      </c>
     </row>
-    <row r="107" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
+    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -23698,9 +24103,12 @@
       <c r="AN107" s="10">
         <v>14</v>
       </c>
+      <c r="AO107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
+    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -23818,9 +24226,12 @@
       <c r="AN108" s="10">
         <v>27</v>
       </c>
+      <c r="AO108" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="109" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -23938,8 +24349,11 @@
       <c r="AN109" s="10">
         <v>3</v>
       </c>
+      <c r="AO109" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="110" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -24060,8 +24474,11 @@
       <c r="AN110" s="10">
         <v>323</v>
       </c>
+      <c r="AO110" s="10">
+        <v>339</v>
+      </c>
     </row>
-    <row r="111" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -24182,9 +24599,12 @@
       <c r="AN111" s="10">
         <v>57</v>
       </c>
+      <c r="AO111" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -24304,9 +24724,12 @@
       <c r="AN112" s="10">
         <v>14</v>
       </c>
+      <c r="AO112" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -24424,9 +24847,12 @@
       <c r="AN113" s="10">
         <v>17</v>
       </c>
+      <c r="AO113" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A114" s="32"/>
+    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -24544,9 +24970,12 @@
       <c r="AN114" s="10">
         <v>100</v>
       </c>
+      <c r="AO114" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A115" s="33" t="s">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -24666,9 +25095,12 @@
       <c r="AN115" s="10">
         <v>81</v>
       </c>
+      <c r="AO115" s="10">
+        <v>103</v>
+      </c>
     </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
+    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -24786,9 +25218,12 @@
       <c r="AN116" s="10">
         <v>73</v>
       </c>
+      <c r="AO116" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -24906,9 +25341,12 @@
       <c r="AN117" s="10">
         <v>10</v>
       </c>
+      <c r="AO117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
+    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -25026,9 +25464,12 @@
       <c r="AN118" s="10">
         <v>41</v>
       </c>
+      <c r="AO118" s="10">
+        <v>43</v>
+      </c>
     </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -25146,9 +25587,12 @@
       <c r="AN119" s="10">
         <v>7</v>
       </c>
+      <c r="AO119" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -25266,9 +25710,12 @@
       <c r="AN120" s="10">
         <v>52</v>
       </c>
+      <c r="AO120" s="10">
+        <v>56</v>
+      </c>
     </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="s">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -25388,9 +25835,12 @@
       <c r="AN121" s="10">
         <v>6</v>
       </c>
+      <c r="AO121" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
+    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -25508,9 +25958,12 @@
       <c r="AN122" s="10">
         <v>23</v>
       </c>
+      <c r="AO122" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A123" s="31"/>
+    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -25628,9 +26081,12 @@
       <c r="AN123" s="10">
         <v>2</v>
       </c>
+      <c r="AO123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A124" s="31"/>
+    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -25748,9 +26204,12 @@
       <c r="AN124" s="10">
         <v>5</v>
       </c>
+      <c r="AO124" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="125" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A125" s="31"/>
+    <row r="125" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -25868,9 +26327,12 @@
       <c r="AN125" s="10">
         <v>1</v>
       </c>
+      <c r="AO125" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="126" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A126" s="31"/>
+    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -25988,9 +26450,12 @@
       <c r="AN126" s="10">
         <v>4</v>
       </c>
+      <c r="AO126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A127" s="31"/>
+    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -26108,9 +26573,12 @@
       <c r="AN127" s="10">
         <v>4</v>
       </c>
+      <c r="AO127" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A128" s="31"/>
+    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -26228,9 +26696,12 @@
       <c r="AN128" s="10">
         <v>8</v>
       </c>
+      <c r="AO128" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A129" s="31"/>
+    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -26348,9 +26819,12 @@
       <c r="AN129" s="10">
         <v>143</v>
       </c>
+      <c r="AO129" s="10">
+        <v>144</v>
+      </c>
     </row>
-    <row r="130" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -26468,8 +26942,11 @@
       <c r="AN130" s="10">
         <v>22</v>
       </c>
+      <c r="AO130" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -26590,9 +27067,12 @@
       <c r="AN131" s="10">
         <v>365</v>
       </c>
+      <c r="AO131" s="10">
+        <v>385</v>
+      </c>
     </row>
-    <row r="132" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="s">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -26712,9 +27192,12 @@
       <c r="AN132" s="10">
         <v>21</v>
       </c>
+      <c r="AO132" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="133" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A133" s="31"/>
+    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -26832,9 +27315,12 @@
       <c r="AN133" s="10">
         <v>16</v>
       </c>
+      <c r="AO133" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="134" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A134" s="31"/>
+    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -26952,9 +27438,12 @@
       <c r="AN134" s="10">
         <v>2</v>
       </c>
+      <c r="AO134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A135" s="32"/>
+    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -27072,9 +27561,12 @@
       <c r="AN135" s="10">
         <v>2</v>
       </c>
+      <c r="AO135" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="136" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="s">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -27194,9 +27686,12 @@
       <c r="AN136" s="10">
         <v>96</v>
       </c>
+      <c r="AO136" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="137" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
+    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -27314,9 +27809,12 @@
       <c r="AN137" s="10">
         <v>115</v>
       </c>
+      <c r="AO137" s="10">
+        <v>125</v>
+      </c>
     </row>
-    <row r="138" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -27434,9 +27932,12 @@
       <c r="AN138" s="10">
         <v>19</v>
       </c>
+      <c r="AO138" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="139" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A139" s="35"/>
+    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -27553,10 +28054,25 @@
       </c>
       <c r="AN139" s="10">
         <v>154</v>
+      </c>
+      <c r="AO139" s="10">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -27569,18 +28085,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -27899,7 +28403,7 @@
       </c>
       <c r="AW2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25.529411764705884</v>
       </c>
       <c r="AX2" s="18">
         <f t="shared" si="1"/>
@@ -28549,7 +29053,7 @@
       </c>
       <c r="AW4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.7557603686635943</v>
       </c>
       <c r="AX4" s="10">
         <f t="shared" si="7"/>
@@ -28874,7 +29378,7 @@
       </c>
       <c r="AW6" s="12">
         <f>MAX(0, (dc!AW2-dc!AV2))</f>
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="AX6" s="12">
         <f>MAX(0, (dc!AX2-dc!AW2))</f>
@@ -29198,7 +29702,7 @@
       </c>
       <c r="AW7" s="12">
         <f>MAX(0, (dc!AW3-dc!AV3))</f>
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="AX7" s="12">
         <f>MAX(0, (dc!AX3-dc!AW3))</f>
@@ -29846,7 +30350,7 @@
       </c>
       <c r="AW9" s="12">
         <f>MAX(0, (dc!AW5-dc!AV5))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AX9" s="12">
         <f>MAX(0, (dc!AX5-dc!AW5))</f>
@@ -30398,7 +30902,7 @@
       </c>
       <c r="AW11" s="10">
         <f>MAX(0,(dc!AW7-dc!AV7))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AX11" s="10">
         <f>MAX(0,(dc!AX7-dc!AW7))</f>
@@ -30705,7 +31209,7 @@
       </c>
       <c r="AW12" s="10">
         <f>MAX(0,(dc!AW8-dc!AV8))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AX12" s="10">
         <f>MAX(0,(dc!AX8-dc!AW8))</f>
@@ -31012,7 +31516,7 @@
       </c>
       <c r="AW13" s="10">
         <f>MAX(0,(dc!AW9-dc!AV9))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AX13" s="10">
         <f>MAX(0,(dc!AX9-dc!AW9))</f>
@@ -31319,7 +31823,7 @@
       </c>
       <c r="AW14" s="10">
         <f>MAX(0,(dc!AW10-dc!AV10))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AX14" s="10">
         <f>MAX(0,(dc!AX10-dc!AW10))</f>
@@ -31626,7 +32130,7 @@
       </c>
       <c r="AW15" s="10">
         <f>MAX(0,(dc!AW11-dc!AV11))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AX15" s="10">
         <f>MAX(0,(dc!AX11-dc!AW11))</f>
@@ -31933,7 +32437,7 @@
       </c>
       <c r="AW16" s="10">
         <f>MAX(0,(dc!AW12-dc!AV12))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AX16" s="10">
         <f>MAX(0,(dc!AX12-dc!AW12))</f>
@@ -32240,7 +32744,7 @@
       </c>
       <c r="AW17" s="10">
         <f>MAX(0,(dc!AW13-dc!AV13))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AX17" s="10">
         <f>MAX(0,(dc!AX13-dc!AW13))</f>
@@ -32547,7 +33051,7 @@
       </c>
       <c r="AW18" s="10">
         <f>MAX(0,(dc!AW14-dc!AV14))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AX18" s="10">
         <f>MAX(0,(dc!AX14-dc!AW14))</f>
@@ -32854,7 +33358,7 @@
       </c>
       <c r="AW19" s="10">
         <f>MAX(0,(dc!AW15-dc!AV15))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AX19" s="10">
         <f>MAX(0,(dc!AX15-dc!AW15))</f>
@@ -33251,7 +33755,7 @@
       </c>
       <c r="AL2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.034985422740526</v>
       </c>
       <c r="AM2" s="20">
         <f t="shared" si="0"/>
@@ -33524,7 +34028,7 @@
       </c>
       <c r="AL3" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>17.581187010078388</v>
       </c>
       <c r="AM3" s="20">
         <f t="shared" si="3"/>
@@ -33797,7 +34301,7 @@
       </c>
       <c r="AL4" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6.9428891377379625</v>
       </c>
       <c r="AM4" s="20">
         <f t="shared" si="5"/>
@@ -34133,7 +34637,7 @@
       </c>
       <c r="AL6" s="14">
         <f>MAX(0,(md!AL2-md!AK2)+(md!AL3-md!AK3))</f>
-        <v>0</v>
+        <v>3430</v>
       </c>
       <c r="AM6" s="14">
         <f>MAX(0,(md!AM2-md!AL2)+(md!AM3-md!AL3))</f>
@@ -34405,7 +34909,7 @@
       </c>
       <c r="AL7" s="14">
         <f>MAX(0,(md!AL3-md!AK3))</f>
-        <v>0</v>
+        <v>893</v>
       </c>
       <c r="AM7" s="14">
         <f>MAX(0,(md!AM3-md!AL3))</f>
@@ -34677,7 +35181,7 @@
       </c>
       <c r="AL8" s="14">
         <f>MAX(0,(md!AL4-md!AK4))</f>
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="AM8" s="14">
         <f>MAX(0,(md!AM4-md!AL4))</f>
@@ -34949,7 +35453,7 @@
       </c>
       <c r="AL9" s="14">
         <f>MAX(0,(md!AL5-md!AK5))</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="AM9" s="14">
         <f>MAX(0,(md!AM5-md!AL5))</f>
@@ -35435,7 +35939,7 @@
       </c>
       <c r="AL11" s="14">
         <f>MAX(0,(md!AL7-md!AK7))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM11" s="14">
         <f>MAX(0,(md!AM7-md!AL7))</f>
@@ -35712,7 +36216,7 @@
       </c>
       <c r="AL12" s="14">
         <f>MAX(0,(md!AL8-md!AK8))</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="AM12" s="14">
         <f>MAX(0,(md!AM8-md!AL8))</f>
@@ -35989,7 +36493,7 @@
       </c>
       <c r="AL13" s="14">
         <f>MAX(0,(md!AL9-md!AK9))</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="AM13" s="14">
         <f>MAX(0,(md!AM9-md!AL9))</f>
@@ -36266,7 +36770,7 @@
       </c>
       <c r="AL14" s="14">
         <f>MAX(0,(md!AL10-md!AK10))</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="AM14" s="14">
         <f>MAX(0,(md!AM10-md!AL10))</f>
@@ -36543,7 +37047,7 @@
       </c>
       <c r="AL15" s="14">
         <f>MAX(0,(md!AL11-md!AK11))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM15" s="14">
         <f>MAX(0,(md!AM11-md!AL11))</f>
@@ -36820,7 +37324,7 @@
       </c>
       <c r="AL16" s="14">
         <f>MAX(0,(md!AL12-md!AK12))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM16" s="14">
         <f>MAX(0,(md!AM12-md!AL12))</f>
@@ -37097,7 +37601,7 @@
       </c>
       <c r="AL17" s="14">
         <f>MAX(0,(md!AL13-md!AK13))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AM17" s="14">
         <f>MAX(0,(md!AM13-md!AL13))</f>
@@ -37374,7 +37878,7 @@
       </c>
       <c r="AL18" s="14">
         <f>MAX(0,(md!AL14-md!AK14))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM18" s="14">
         <f>MAX(0,(md!AM14-md!AL14))</f>
@@ -37651,7 +38155,7 @@
       </c>
       <c r="AL19" s="14">
         <f>MAX(0,(md!AL15-md!AK15))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AM19" s="14">
         <f>MAX(0,(md!AM15-md!AL15))</f>
@@ -38205,7 +38709,7 @@
       </c>
       <c r="AL21" s="14">
         <f>MAX(0,(md!AL17-md!AK17))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AM21" s="14">
         <f>MAX(0,(md!AM17-md!AL17))</f>
@@ -38759,7 +39263,7 @@
       </c>
       <c r="AL23" s="14">
         <f>MAX(0,(md!AL19-md!AK19))</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AM23" s="14">
         <f>MAX(0,(md!AM19-md!AL19))</f>
@@ -39036,7 +39540,7 @@
       </c>
       <c r="AL24" s="14">
         <f>MAX(0,(md!AL20-md!AK20))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AM24" s="14">
         <f>MAX(0,(md!AM20-md!AL20))</f>
@@ -39313,7 +39817,7 @@
       </c>
       <c r="AL25" s="14">
         <f>MAX(0,(md!AL21-md!AK21))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM25" s="14">
         <f>MAX(0,(md!AM21-md!AL21))</f>
@@ -39590,7 +40094,7 @@
       </c>
       <c r="AL26" s="14">
         <f>MAX(0,(md!AL22-md!AK22))</f>
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AM26" s="14">
         <f>MAX(0,(md!AM22-md!AL22))</f>
@@ -39867,7 +40371,7 @@
       </c>
       <c r="AL27" s="14">
         <f>MAX(0,(md!AL23-md!AK23))</f>
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="AM27" s="14">
         <f>MAX(0,(md!AM23-md!AL23))</f>
@@ -40421,7 +40925,7 @@
       </c>
       <c r="AL29" s="14">
         <f>MAX(0,(md!AL25-md!AK25))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM29" s="14">
         <f>MAX(0,(md!AM25-md!AL25))</f>
@@ -40698,7 +41202,7 @@
       </c>
       <c r="AL30" s="14">
         <f>MAX(0,(md!AL26-md!AK26))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM30" s="14">
         <f>MAX(0,(md!AM26-md!AL26))</f>
@@ -40975,7 +41479,7 @@
       </c>
       <c r="AL31" s="14">
         <f>MAX(0,(md!AL27-md!AK27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM31" s="14">
         <f>MAX(0,(md!AM27-md!AL27))</f>
@@ -41252,7 +41756,7 @@
       </c>
       <c r="AL32" s="14">
         <f>MAX(0,(md!AL28-md!AK28))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AM32" s="14">
         <f>MAX(0,(md!AM28-md!AL28))</f>
@@ -41529,7 +42033,7 @@
       </c>
       <c r="AL33" s="14">
         <f>MAX(0,(md!AL29-md!AK29))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AM33" s="14">
         <f>MAX(0,(md!AM29-md!AL29))</f>
@@ -41806,7 +42310,7 @@
       </c>
       <c r="AL34" s="14">
         <f>MAX(0,(md!AL30-md!AK30))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM34" s="14">
         <f>MAX(0,(md!AM30-md!AL30))</f>
@@ -42285,7 +42789,7 @@
       </c>
       <c r="AN2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.986271676300579</v>
       </c>
       <c r="AO2" s="19">
         <f t="shared" si="1"/>
@@ -42562,7 +43066,7 @@
       </c>
       <c r="AN3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.1186440677966107</v>
       </c>
       <c r="AO3" s="19">
         <f t="shared" si="3"/>
@@ -42839,7 +43343,7 @@
       </c>
       <c r="AN4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.3898305084745761</v>
       </c>
       <c r="AO4" s="19">
         <f t="shared" si="5"/>
@@ -43116,7 +43620,7 @@
       </c>
       <c r="AN6" s="14">
         <f>MAX(0,(va!AO5-va!AN5))</f>
-        <v>0</v>
+        <v>5536</v>
       </c>
       <c r="AO6" s="14">
         <f>MAX(0,(va!AP5-va!AO5))</f>
@@ -43393,7 +43897,7 @@
       </c>
       <c r="AN7" s="14">
         <f>MAX(0,(va!AO2-va!AN2))</f>
-        <v>0</v>
+        <v>885</v>
       </c>
       <c r="AO7" s="14">
         <f>MAX(0,(va!AP2-va!AO2))</f>
@@ -43670,7 +44174,7 @@
       </c>
       <c r="AN8" s="14">
         <f>MAX(0,(va!AO3-va!AN3))</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="AO8" s="14">
         <f>MAX(0,(va!AP3-va!AO3))</f>
@@ -43947,7 +44451,7 @@
       </c>
       <c r="AN9" s="14">
         <f>MAX(0,(va!AO4-va!AN4))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AO9" s="14">
         <f>MAX(0,(va!AP4-va!AO4))</f>
@@ -44444,7 +44948,7 @@
       </c>
       <c r="AN11" s="16">
         <f>MAX(0,(va!AO7-va!AN7))</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="AO11" s="16">
         <f>MAX(0,(va!AP7-va!AO7))</f>
@@ -45290,7 +45794,7 @@
       </c>
       <c r="AN14" s="16">
         <f>MAX(0,(va!AO10-va!AN10))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO14" s="16">
         <f>MAX(0,(va!AP10-va!AO10))</f>
@@ -45572,7 +46076,7 @@
       </c>
       <c r="AN15" s="16">
         <f>MAX(0,(va!AO11-va!AN11))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO15" s="16">
         <f>MAX(0,(va!AP11-va!AO11))</f>
@@ -46136,7 +46640,7 @@
       </c>
       <c r="AN17" s="16">
         <f>MAX(0,(va!AO13-va!AN13))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO17" s="16">
         <f>MAX(0,(va!AP13-va!AO13))</f>
@@ -46418,7 +46922,7 @@
       </c>
       <c r="AN18" s="16">
         <f>MAX(0,(va!AO14-va!AN14))</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="AO18" s="16">
         <f>MAX(0,(va!AP14-va!AO14))</f>
@@ -46700,7 +47204,7 @@
       </c>
       <c r="AN19" s="16">
         <f>MAX(0,(va!AO15-va!AN15))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO19" s="16">
         <f>MAX(0,(va!AP15-va!AO15))</f>
@@ -47546,7 +48050,7 @@
       </c>
       <c r="AN22" s="16">
         <f>MAX(0,(va!AO18-va!AN18))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO22" s="16">
         <f>MAX(0,(va!AP18-va!AO18))</f>
@@ -47828,7 +48332,7 @@
       </c>
       <c r="AN23" s="16">
         <f>MAX(0,(va!AO19-va!AN19))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AO23" s="16">
         <f>MAX(0,(va!AP19-va!AO19))</f>
@@ -48110,7 +48614,7 @@
       </c>
       <c r="AN24" s="16">
         <f>MAX(0,(va!AO20-va!AN20))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO24" s="16">
         <f>MAX(0,(va!AP20-va!AO20))</f>
@@ -48392,7 +48896,7 @@
       </c>
       <c r="AN25" s="16">
         <f>MAX(0,(va!AO21-va!AN21))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AO25" s="16">
         <f>MAX(0,(va!AP21-va!AO21))</f>
@@ -49520,7 +50024,7 @@
       </c>
       <c r="AN29" s="16">
         <f>MAX(0,(va!AO25-va!AN25))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO29" s="16">
         <f>MAX(0,(va!AP25-va!AO25))</f>
@@ -49802,7 +50306,7 @@
       </c>
       <c r="AN30" s="16">
         <f>MAX(0,(va!AO26-va!AN26))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO30" s="16">
         <f>MAX(0,(va!AP26-va!AO26))</f>
@@ -50084,7 +50588,7 @@
       </c>
       <c r="AN31" s="16">
         <f>MAX(0,(va!AO27-va!AN27))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO31" s="16">
         <f>MAX(0,(va!AP27-va!AO27))</f>
@@ -50648,7 +51152,7 @@
       </c>
       <c r="AN33" s="16">
         <f>MAX(0,(va!AO29-va!AN29))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO33" s="16">
         <f>MAX(0,(va!AP29-va!AO29))</f>
@@ -50930,7 +51434,7 @@
       </c>
       <c r="AN34" s="16">
         <f>MAX(0,(va!AO30-va!AN30))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO34" s="16">
         <f>MAX(0,(va!AP30-va!AO30))</f>
@@ -51212,7 +51716,7 @@
       </c>
       <c r="AN35" s="16">
         <f>MAX(0,(va!AO31-va!AN31))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AO35" s="16">
         <f>MAX(0,(va!AP31-va!AO31))</f>
@@ -51494,7 +51998,7 @@
       </c>
       <c r="AN36" s="16">
         <f>MAX(0,(va!AO32-va!AN32))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO36" s="16">
         <f>MAX(0,(va!AP32-va!AO32))</f>
@@ -51776,7 +52280,7 @@
       </c>
       <c r="AN37" s="16">
         <f>MAX(0,(va!AO33-va!AN33))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO37" s="16">
         <f>MAX(0,(va!AP33-va!AO33))</f>
@@ -52340,7 +52844,7 @@
       </c>
       <c r="AN39" s="16">
         <f>MAX(0,(va!AO35-va!AN35))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO39" s="16">
         <f>MAX(0,(va!AP35-va!AO35))</f>
@@ -52622,7 +53126,7 @@
       </c>
       <c r="AN40" s="16">
         <f>MAX(0,(va!AO36-va!AN36))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO40" s="16">
         <f>MAX(0,(va!AP36-va!AO36))</f>
@@ -53186,7 +53690,7 @@
       </c>
       <c r="AN42" s="16">
         <f>MAX(0,(va!AO38-va!AN38))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO42" s="16">
         <f>MAX(0,(va!AP38-va!AO38))</f>
@@ -53468,7 +53972,7 @@
       </c>
       <c r="AN43" s="16">
         <f>MAX(0,(va!AO39-va!AN39))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO43" s="16">
         <f>MAX(0,(va!AP39-va!AO39))</f>
@@ -54314,7 +54818,7 @@
       </c>
       <c r="AN46" s="16">
         <f>MAX(0,(va!AO42-va!AN42))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO46" s="16">
         <f>MAX(0,(va!AP42-va!AO42))</f>
@@ -54596,7 +55100,7 @@
       </c>
       <c r="AN47" s="16">
         <f>MAX(0,(va!AO43-va!AN43))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO47" s="16">
         <f>MAX(0,(va!AP43-va!AO43))</f>
@@ -56570,7 +57074,7 @@
       </c>
       <c r="AN54" s="16">
         <f>MAX(0,(va!AO50-va!AN50))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AO54" s="16">
         <f>MAX(0,(va!AP50-va!AO50))</f>
@@ -56852,7 +57356,7 @@
       </c>
       <c r="AN55" s="16">
         <f>MAX(0,(va!AO51-va!AN51))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AO55" s="16">
         <f>MAX(0,(va!AP51-va!AO51))</f>
@@ -57134,7 +57638,7 @@
       </c>
       <c r="AN56" s="16">
         <f>MAX(0,(va!AO52-va!AN52))</f>
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="AO56" s="16">
         <f>MAX(0,(va!AP52-va!AO52))</f>
@@ -57980,7 +58484,7 @@
       </c>
       <c r="AN59" s="16">
         <f>MAX(0,(va!AO55-va!AN55))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AO59" s="16">
         <f>MAX(0,(va!AP55-va!AO55))</f>
@@ -58262,7 +58766,7 @@
       </c>
       <c r="AN60" s="16">
         <f>MAX(0,(va!AO56-va!AN56))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AO60" s="16">
         <f>MAX(0,(va!AP56-va!AO56))</f>
@@ -59954,7 +60458,7 @@
       </c>
       <c r="AN66" s="16">
         <f>MAX(0,(va!AO62-va!AN62))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO66" s="16">
         <f>MAX(0,(va!AP62-va!AO62))</f>
@@ -60236,7 +60740,7 @@
       </c>
       <c r="AN67" s="16">
         <f>MAX(0,(va!AO63-va!AN63))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AO67" s="16">
         <f>MAX(0,(va!AP63-va!AO63))</f>
@@ -60518,7 +61022,7 @@
       </c>
       <c r="AN68" s="16">
         <f>MAX(0,(va!AO64-va!AN64))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AO68" s="16">
         <f>MAX(0,(va!AP64-va!AO64))</f>
@@ -60800,7 +61304,7 @@
       </c>
       <c r="AN69" s="16">
         <f>MAX(0,(va!AO65-va!AN65))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO69" s="16">
         <f>MAX(0,(va!AP65-va!AO65))</f>
@@ -61082,7 +61586,7 @@
       </c>
       <c r="AN70" s="16">
         <f>MAX(0,(va!AO66-va!AN66))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO70" s="16">
         <f>MAX(0,(va!AP66-va!AO66))</f>
@@ -61364,7 +61868,7 @@
       </c>
       <c r="AN71" s="16">
         <f>MAX(0,(va!AO67-va!AN67))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AO71" s="16">
         <f>MAX(0,(va!AP67-va!AO67))</f>
@@ -61928,7 +62432,7 @@
       </c>
       <c r="AN73" s="16">
         <f>MAX(0,(va!AO69-va!AN69))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO73" s="16">
         <f>MAX(0,(va!AP69-va!AO69))</f>
@@ -62210,7 +62714,7 @@
       </c>
       <c r="AN74" s="16">
         <f>MAX(0,(va!AO70-va!AN70))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO74" s="16">
         <f>MAX(0,(va!AP70-va!AO70))</f>
@@ -64466,7 +64970,7 @@
       </c>
       <c r="AN82" s="16">
         <f>MAX(0,(va!AO78-va!AN78))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO82" s="16">
         <f>MAX(0,(va!AP78-va!AO78))</f>
@@ -65312,7 +65816,7 @@
       </c>
       <c r="AN85" s="16">
         <f>MAX(0,(va!AO81-va!AN81))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AO85" s="16">
         <f>MAX(0,(va!AP81-va!AO81))</f>
@@ -65594,7 +66098,7 @@
       </c>
       <c r="AN86" s="16">
         <f>MAX(0,(va!AO82-va!AN82))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO86" s="16">
         <f>MAX(0,(va!AP82-va!AO82))</f>
@@ -65876,7 +66380,7 @@
       </c>
       <c r="AN87" s="16">
         <f>MAX(0,(va!AO83-va!AN83))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO87" s="16">
         <f>MAX(0,(va!AP83-va!AO83))</f>
@@ -66158,7 +66662,7 @@
       </c>
       <c r="AN88" s="16">
         <f>MAX(0,(va!AO84-va!AN84))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO88" s="16">
         <f>MAX(0,(va!AP84-va!AO84))</f>
@@ -67286,7 +67790,7 @@
       </c>
       <c r="AN92" s="16">
         <f>MAX(0,(va!AO88-va!AN88))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO92" s="16">
         <f>MAX(0,(va!AP88-va!AO88))</f>
@@ -67850,7 +68354,7 @@
       </c>
       <c r="AN94" s="16">
         <f>MAX(0,(va!AO90-va!AN90))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO94" s="16">
         <f>MAX(0,(va!AP90-va!AO90))</f>
@@ -68696,7 +69200,7 @@
       </c>
       <c r="AN97" s="16">
         <f>MAX(0,(va!AO93-va!AN93))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO97" s="16">
         <f>MAX(0,(va!AP93-va!AO93))</f>
@@ -68978,7 +69482,7 @@
       </c>
       <c r="AN98" s="16">
         <f>MAX(0,(va!AO94-va!AN94))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO98" s="16">
         <f>MAX(0,(va!AP94-va!AO94))</f>
@@ -69260,7 +69764,7 @@
       </c>
       <c r="AN99" s="16">
         <f>MAX(0,(va!AO95-va!AN95))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO99" s="16">
         <f>MAX(0,(va!AP95-va!AO95))</f>
@@ -69542,7 +70046,7 @@
       </c>
       <c r="AN100" s="16">
         <f>MAX(0,(va!AO96-va!AN96))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AO100" s="16">
         <f>MAX(0,(va!AP96-va!AO96))</f>
@@ -69824,7 +70328,7 @@
       </c>
       <c r="AN101" s="16">
         <f>MAX(0,(va!AO97-va!AN97))</f>
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="AO101" s="16">
         <f>MAX(0,(va!AP97-va!AO97))</f>
@@ -70106,7 +70610,7 @@
       </c>
       <c r="AN102" s="16">
         <f>MAX(0,(va!AO98-va!AN98))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AO102" s="16">
         <f>MAX(0,(va!AP98-va!AO98))</f>
@@ -70388,7 +70892,7 @@
       </c>
       <c r="AN103" s="16">
         <f>MAX(0,(va!AO99-va!AN99))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO103" s="16">
         <f>MAX(0,(va!AP99-va!AO99))</f>
@@ -70670,7 +71174,7 @@
       </c>
       <c r="AN104" s="16">
         <f>MAX(0,(va!AO100-va!AN100))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO104" s="16">
         <f>MAX(0,(va!AP100-va!AO100))</f>
@@ -70952,7 +71456,7 @@
       </c>
       <c r="AN105" s="16">
         <f>MAX(0,(va!AO101-va!AN101))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO105" s="16">
         <f>MAX(0,(va!AP101-va!AO101))</f>
@@ -71234,7 +71738,7 @@
       </c>
       <c r="AN106" s="16">
         <f>MAX(0,(va!AO102-va!AN102))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AO106" s="16">
         <f>MAX(0,(va!AP102-va!AO102))</f>
@@ -71516,7 +72020,7 @@
       </c>
       <c r="AN107" s="16">
         <f>MAX(0,(va!AO103-va!AN103))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AO107" s="16">
         <f>MAX(0,(va!AP103-va!AO103))</f>
@@ -71798,7 +72302,7 @@
       </c>
       <c r="AN108" s="16">
         <f>MAX(0,(va!AO104-va!AN104))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO108" s="16">
         <f>MAX(0,(va!AP104-va!AO104))</f>
@@ -72080,7 +72584,7 @@
       </c>
       <c r="AN109" s="16">
         <f>MAX(0,(va!AO105-va!AN105))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AO109" s="16">
         <f>MAX(0,(va!AP105-va!AO105))</f>
@@ -72362,7 +72866,7 @@
       </c>
       <c r="AN110" s="16">
         <f>MAX(0,(va!AO106-va!AN106))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO110" s="16">
         <f>MAX(0,(va!AP106-va!AO106))</f>
@@ -72926,7 +73430,7 @@
       </c>
       <c r="AN112" s="16">
         <f>MAX(0,(va!AO108-va!AN108))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO112" s="16">
         <f>MAX(0,(va!AP108-va!AO108))</f>
@@ -73208,7 +73712,7 @@
       </c>
       <c r="AN113" s="16">
         <f>MAX(0,(va!AO109-va!AN109))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO113" s="16">
         <f>MAX(0,(va!AP109-va!AO109))</f>
@@ -73490,7 +73994,7 @@
       </c>
       <c r="AN114" s="16">
         <f>MAX(0,(va!AO110-va!AN110))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AO114" s="16">
         <f>MAX(0,(va!AP110-va!AO110))</f>
@@ -73772,7 +74276,7 @@
       </c>
       <c r="AN115" s="16">
         <f>MAX(0,(va!AO111-va!AN111))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AO115" s="16">
         <f>MAX(0,(va!AP111-va!AO111))</f>
@@ -74336,7 +74840,7 @@
       </c>
       <c r="AN117" s="16">
         <f>MAX(0,(va!AO113-va!AN113))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO117" s="16">
         <f>MAX(0,(va!AP113-va!AO113))</f>
@@ -74900,7 +75404,7 @@
       </c>
       <c r="AN119" s="16">
         <f>MAX(0,(va!AO115-va!AN115))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AO119" s="16">
         <f>MAX(0,(va!AP115-va!AO115))</f>
@@ -75746,7 +76250,7 @@
       </c>
       <c r="AN122" s="16">
         <f>MAX(0,(va!AO118-va!AN118))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO122" s="16">
         <f>MAX(0,(va!AP118-va!AO118))</f>
@@ -76028,7 +76532,7 @@
       </c>
       <c r="AN123" s="16">
         <f>MAX(0,(va!AO119-va!AN119))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO123" s="16">
         <f>MAX(0,(va!AP119-va!AO119))</f>
@@ -76310,7 +76814,7 @@
       </c>
       <c r="AN124" s="16">
         <f>MAX(0,(va!AO120-va!AN120))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO124" s="16">
         <f>MAX(0,(va!AP120-va!AO120))</f>
@@ -76592,7 +77096,7 @@
       </c>
       <c r="AN125" s="16">
         <f>MAX(0,(va!AO121-va!AN121))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO125" s="16">
         <f>MAX(0,(va!AP121-va!AO121))</f>
@@ -77720,7 +78224,7 @@
       </c>
       <c r="AN129" s="16">
         <f>MAX(0,(va!AO125-va!AN125))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO129" s="16">
         <f>MAX(0,(va!AP125-va!AO125))</f>
@@ -78284,7 +78788,7 @@
       </c>
       <c r="AN131" s="16">
         <f>MAX(0,(va!AO127-va!AN127))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO131" s="16">
         <f>MAX(0,(va!AP127-va!AO127))</f>
@@ -78566,7 +79070,7 @@
       </c>
       <c r="AN132" s="16">
         <f>MAX(0,(va!AO128-va!AN128))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO132" s="16">
         <f>MAX(0,(va!AP128-va!AO128))</f>
@@ -78848,7 +79352,7 @@
       </c>
       <c r="AN133" s="16">
         <f>MAX(0,(va!AO129-va!AN129))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO133" s="16">
         <f>MAX(0,(va!AP129-va!AO129))</f>
@@ -79412,7 +79916,7 @@
       </c>
       <c r="AN135" s="16">
         <f>MAX(0,(va!AO131-va!AN131))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AO135" s="16">
         <f>MAX(0,(va!AP131-va!AO131))</f>
@@ -80822,7 +81326,7 @@
       </c>
       <c r="AN140" s="16">
         <f>MAX(0,(va!AO136-va!AN136))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO140" s="16">
         <f>MAX(0,(va!AP136-va!AO136))</f>
@@ -81104,7 +81608,7 @@
       </c>
       <c r="AN141" s="16">
         <f>MAX(0,(va!AO137-va!AN137))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO141" s="16">
         <f>MAX(0,(va!AP137-va!AO137))</f>
@@ -81386,7 +81890,7 @@
       </c>
       <c r="AN142" s="16">
         <f>MAX(0,(va!AO138-va!AN138))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO142" s="16">
         <f>MAX(0,(va!AP138-va!AO138))</f>
@@ -81668,7 +82172,7 @@
       </c>
       <c r="AN143" s="16">
         <f>MAX(0,(va!AO139-va!AN139))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AO143" s="16">
         <f>MAX(0,(va!AP139-va!AO139))</f>

</xml_diff>

<commit_message>
01 May data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2834A8-3B0E-4275-8794-3A6AA06061B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF9050B-D384-4B20-A744-98330A6AA583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4018,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AW2" sqref="AW2"/>
+      <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4182,6 +4182,9 @@
       <c r="AW2" s="12">
         <v>20079</v>
       </c>
+      <c r="AX2" s="12">
+        <v>21135</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4366,7 +4369,7 @@
       </c>
       <c r="AX3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4323</v>
       </c>
       <c r="AY3" s="10">
         <f t="shared" si="0"/>
@@ -4646,6 +4649,9 @@
       <c r="AW5" s="10">
         <v>224</v>
       </c>
+      <c r="AX5" s="10">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5040,6 +5046,9 @@
       <c r="AW7" s="10">
         <v>543</v>
       </c>
+      <c r="AX7" s="10">
+        <v>543</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5189,6 +5198,9 @@
       <c r="AW8" s="10">
         <v>291</v>
       </c>
+      <c r="AX8" s="10">
+        <v>291</v>
+      </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5338,6 +5350,9 @@
       <c r="AW9" s="10">
         <v>282</v>
       </c>
+      <c r="AX9" s="10">
+        <v>282</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5487,6 +5502,9 @@
       <c r="AW10" s="10">
         <v>774</v>
       </c>
+      <c r="AX10" s="10">
+        <v>774</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5636,6 +5654,9 @@
       <c r="AW11" s="10">
         <v>646</v>
       </c>
+      <c r="AX11" s="10">
+        <v>646</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5785,6 +5806,9 @@
       <c r="AW12" s="10">
         <v>450</v>
       </c>
+      <c r="AX12" s="10">
+        <v>450</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5934,6 +5958,9 @@
       <c r="AW13" s="10">
         <v>659</v>
       </c>
+      <c r="AX13" s="10">
+        <v>659</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6083,6 +6110,9 @@
       <c r="AW14" s="10">
         <v>632</v>
       </c>
+      <c r="AX14" s="10">
+        <v>632</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6230,6 +6260,9 @@
         <v>40</v>
       </c>
       <c r="AW15" s="10">
+        <v>46</v>
+      </c>
+      <c r="AX15" s="10">
         <v>46</v>
       </c>
     </row>
@@ -6485,7 +6518,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AM2" sqref="AM2"/>
+      <selection pane="bottomRight" activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6617,7 +6650,7 @@
         <v>92617</v>
       </c>
       <c r="AM2" s="10">
-        <v>0</v>
+        <v>97511</v>
       </c>
       <c r="AN2" s="10">
         <v>0</v>
@@ -6859,7 +6892,7 @@
       </c>
       <c r="AM3" s="10">
         <f>SUM(md[1-May])</f>
-        <v>0</v>
+        <v>23472</v>
       </c>
       <c r="AN3" s="10">
         <f>SUM(md[2-May])</f>
@@ -7095,7 +7128,7 @@
         <v>4559</v>
       </c>
       <c r="AM4" s="10">
-        <v>0</v>
+        <v>4718</v>
       </c>
       <c r="AN4" s="10">
         <v>0</v>
@@ -7301,7 +7334,7 @@
         <v>1047</v>
       </c>
       <c r="AM5" s="10">
-        <v>0</v>
+        <v>1098</v>
       </c>
       <c r="AN5" s="10">
         <v>0</v>
@@ -7718,6 +7751,9 @@
       <c r="AL7">
         <v>118</v>
       </c>
+      <c r="AM7">
+        <v>118</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7834,6 +7870,9 @@
       <c r="AL8" s="10">
         <v>1725</v>
       </c>
+      <c r="AM8" s="10">
+        <v>1807</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7950,6 +7989,9 @@
       <c r="AL9">
         <v>2068</v>
       </c>
+      <c r="AM9">
+        <v>2162</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -8066,6 +8108,9 @@
       <c r="AL10">
         <v>2831</v>
       </c>
+      <c r="AM10">
+        <v>3013</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8182,6 +8227,9 @@
       <c r="AL11">
         <v>150</v>
       </c>
+      <c r="AM11">
+        <v>161</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8298,6 +8346,9 @@
       <c r="AL12">
         <v>71</v>
       </c>
+      <c r="AM12">
+        <v>74</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8414,6 +8465,9 @@
       <c r="AL13">
         <v>436</v>
       </c>
+      <c r="AM13">
+        <v>460</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8530,6 +8584,9 @@
       <c r="AL14">
         <v>167</v>
       </c>
+      <c r="AM14">
+        <v>176</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8646,6 +8703,9 @@
       <c r="AL15">
         <v>564</v>
       </c>
+      <c r="AM15">
+        <v>611</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8762,8 +8822,11 @@
       <c r="AL16" s="10">
         <v>51</v>
       </c>
+      <c r="AM16" s="10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8878,8 +8941,11 @@
       <c r="AL17">
         <v>918</v>
       </c>
+      <c r="AM17">
+        <v>942</v>
+      </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -8994,8 +9060,11 @@
       <c r="AL18">
         <v>4</v>
       </c>
+      <c r="AM18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -9110,8 +9179,11 @@
       <c r="AL19">
         <v>414</v>
       </c>
+      <c r="AM19">
+        <v>437</v>
+      </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9226,8 +9298,11 @@
       <c r="AL20">
         <v>867</v>
       </c>
+      <c r="AM20">
+        <v>896</v>
+      </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9342,8 +9417,11 @@
       <c r="AL21">
         <v>79</v>
       </c>
+      <c r="AM21">
+        <v>86</v>
+      </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9458,8 +9536,11 @@
       <c r="AL22">
         <v>4300</v>
       </c>
+      <c r="AM22">
+        <v>4754</v>
+      </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9574,8 +9655,11 @@
       <c r="AL23">
         <v>6043</v>
       </c>
+      <c r="AM23">
+        <v>6735</v>
+      </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9690,8 +9774,11 @@
       <c r="AL24">
         <v>52</v>
       </c>
+      <c r="AM24">
+        <v>52</v>
+      </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9806,8 +9893,11 @@
       <c r="AL25">
         <v>150</v>
       </c>
+      <c r="AM25">
+        <v>159</v>
+      </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -9922,8 +10012,11 @@
       <c r="AL26">
         <v>26</v>
       </c>
+      <c r="AM26">
+        <v>30</v>
+      </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -10038,8 +10131,11 @@
       <c r="AL27">
         <v>35</v>
       </c>
+      <c r="AM27">
+        <v>35</v>
+      </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -10154,8 +10250,11 @@
       <c r="AL28">
         <v>206</v>
       </c>
+      <c r="AM28">
+        <v>216</v>
+      </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -10270,8 +10369,11 @@
       <c r="AL29">
         <v>406</v>
       </c>
+      <c r="AM29">
+        <v>425</v>
+      </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10386,8 +10488,11 @@
       <c r="AL30">
         <v>61</v>
       </c>
+      <c r="AM30">
+        <v>65</v>
+      </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10481,10 +10586,10 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="AD6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10662,7 +10767,7 @@
       </c>
       <c r="AP2" s="10">
         <f>SUM(va[1-May])</f>
-        <v>0</v>
+        <v>16901</v>
       </c>
       <c r="AQ2" s="10">
         <f>SUM(va[2-May])</f>
@@ -10901,7 +11006,7 @@
         <v>2322</v>
       </c>
       <c r="AP3" s="10">
-        <v>0</v>
+        <v>2416</v>
       </c>
       <c r="AQ3" s="10">
         <v>0</v>
@@ -11110,7 +11215,7 @@
         <v>552</v>
       </c>
       <c r="AP4" s="10">
-        <v>0</v>
+        <v>581</v>
       </c>
       <c r="AQ4" s="10">
         <v>0</v>
@@ -11319,7 +11424,7 @@
         <v>90843</v>
       </c>
       <c r="AP5" s="10">
-        <v>0</v>
+        <v>105648</v>
       </c>
       <c r="AQ5" s="10">
         <v>0</v>
@@ -11754,9 +11859,12 @@
       <c r="AO7" s="10">
         <v>754</v>
       </c>
+      <c r="AP7" s="10">
+        <v>802</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11879,9 +11987,12 @@
       <c r="AO8" s="10">
         <v>6</v>
       </c>
+      <c r="AP8" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -12002,9 +12113,12 @@
       <c r="AO9" s="10">
         <v>28</v>
       </c>
+      <c r="AP9" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -12125,9 +12239,12 @@
       <c r="AO10" s="10">
         <v>3</v>
       </c>
+      <c r="AP10" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -12248,9 +12365,12 @@
       <c r="AO11" s="10">
         <v>51</v>
       </c>
+      <c r="AP11" s="10">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -12371,9 +12491,12 @@
       <c r="AO12" s="10">
         <v>0</v>
       </c>
+      <c r="AP12" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -12492,6 +12615,9 @@
         <v>16</v>
       </c>
       <c r="AO13" s="10">
+        <v>26</v>
+      </c>
+      <c r="AP13" s="10">
         <v>26</v>
       </c>
     </row>
@@ -12619,9 +12745,12 @@
       <c r="AO14" s="10">
         <v>967</v>
       </c>
+      <c r="AP14" s="10">
+        <v>1004</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12744,9 +12873,12 @@
       <c r="AO15" s="10">
         <v>43</v>
       </c>
+      <c r="AP15" s="10">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -12867,9 +12999,12 @@
       <c r="AO16" s="10">
         <v>0</v>
       </c>
+      <c r="AP16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12990,9 +13125,12 @@
       <c r="AO17" s="10">
         <v>2</v>
       </c>
+      <c r="AP17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -13113,9 +13251,12 @@
       <c r="AO18" s="10">
         <v>6</v>
       </c>
+      <c r="AP18" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -13236,9 +13377,12 @@
       <c r="AO19" s="10">
         <v>240</v>
       </c>
+      <c r="AP19" s="10">
+        <v>249</v>
+      </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -13359,9 +13503,12 @@
       <c r="AO20" s="10">
         <v>6</v>
       </c>
+      <c r="AP20" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -13482,9 +13629,12 @@
       <c r="AO21" s="10">
         <v>426</v>
       </c>
+      <c r="AP21" s="10">
+        <v>456</v>
+      </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -13605,9 +13755,12 @@
       <c r="AO22" s="10">
         <v>3</v>
       </c>
+      <c r="AP22" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -13728,9 +13881,12 @@
       <c r="AO23" s="10">
         <v>12</v>
       </c>
+      <c r="AP23" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -13851,9 +14007,12 @@
       <c r="AO24" s="10">
         <v>11</v>
       </c>
+      <c r="AP24" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -13976,9 +14135,12 @@
       <c r="AO25" s="10">
         <v>12</v>
       </c>
+      <c r="AP25" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -14099,9 +14261,12 @@
       <c r="AO26" s="10">
         <v>20</v>
       </c>
+      <c r="AP26" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -14222,9 +14387,12 @@
       <c r="AO27" s="10">
         <v>30</v>
       </c>
+      <c r="AP27" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -14345,9 +14513,12 @@
       <c r="AO28" s="10">
         <v>12</v>
       </c>
+      <c r="AP28" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -14468,8 +14639,11 @@
       <c r="AO29" s="10">
         <v>53</v>
       </c>
+      <c r="AP29" s="10">
+        <v>58</v>
+      </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -14593,9 +14767,12 @@
       <c r="AO30" s="10">
         <v>242</v>
       </c>
+      <c r="AP30" s="10">
+        <v>256</v>
+      </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -14718,9 +14895,12 @@
       <c r="AO31" s="10">
         <v>531</v>
       </c>
+      <c r="AP31" s="10">
+        <v>557</v>
+      </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -14841,9 +15021,12 @@
       <c r="AO32" s="10">
         <v>13</v>
       </c>
+      <c r="AP32" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -14964,9 +15147,12 @@
       <c r="AO33" s="10">
         <v>54</v>
       </c>
+      <c r="AP33" s="10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -15089,9 +15275,12 @@
       <c r="AO34" s="10">
         <v>13</v>
       </c>
+      <c r="AP34" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -15212,9 +15401,12 @@
       <c r="AO35" s="10">
         <v>76</v>
       </c>
+      <c r="AP35" s="10">
+        <v>78</v>
+      </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -15335,9 +15527,12 @@
       <c r="AO36" s="10">
         <v>118</v>
       </c>
+      <c r="AP36" s="10">
+        <v>132</v>
+      </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -15458,9 +15653,12 @@
       <c r="AO37" s="10">
         <v>23</v>
       </c>
+      <c r="AP37" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -15583,9 +15781,12 @@
       <c r="AO38" s="10">
         <v>16</v>
       </c>
+      <c r="AP38" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -15706,9 +15907,12 @@
       <c r="AO39" s="10">
         <v>39</v>
       </c>
+      <c r="AP39" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -15829,9 +16033,12 @@
       <c r="AO40" s="10">
         <v>33</v>
       </c>
+      <c r="AP40" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -15952,9 +16159,12 @@
       <c r="AO41" s="10">
         <v>4</v>
       </c>
+      <c r="AP41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -16075,9 +16285,12 @@
       <c r="AO42" s="10">
         <v>31</v>
       </c>
+      <c r="AP42" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -16198,9 +16411,12 @@
       <c r="AO43" s="10">
         <v>23</v>
       </c>
+      <c r="AP43" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -16321,9 +16537,12 @@
       <c r="AO44" s="10">
         <v>24</v>
       </c>
+      <c r="AP44" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -16444,9 +16663,12 @@
       <c r="AO45" s="10">
         <v>31</v>
       </c>
+      <c r="AP45" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -16569,9 +16791,12 @@
       <c r="AO46" s="10">
         <v>16</v>
       </c>
+      <c r="AP46" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -16692,9 +16917,12 @@
       <c r="AO47" s="10">
         <v>0</v>
       </c>
+      <c r="AP47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -16815,9 +17043,12 @@
       <c r="AO48" s="10">
         <v>3</v>
       </c>
+      <c r="AP48" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -16938,9 +17169,12 @@
       <c r="AO49" s="10">
         <v>6</v>
       </c>
+      <c r="AP49" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -17063,9 +17297,12 @@
       <c r="AO50" s="10">
         <v>264</v>
       </c>
+      <c r="AP50" s="10">
+        <v>303</v>
+      </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -17186,9 +17423,12 @@
       <c r="AO51" s="10">
         <v>64</v>
       </c>
+      <c r="AP51" s="10">
+        <v>82</v>
+      </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -17311,9 +17551,12 @@
       <c r="AO52" s="10">
         <v>3611</v>
       </c>
+      <c r="AP52" s="10">
+        <v>3897</v>
+      </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -17434,9 +17677,12 @@
       <c r="AO53" s="10">
         <v>27</v>
       </c>
+      <c r="AP53" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A54" s="32"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -17557,8 +17803,11 @@
       <c r="AO54" s="10">
         <v>26</v>
       </c>
+      <c r="AP54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -17682,8 +17931,11 @@
       <c r="AO55" s="10">
         <v>115</v>
       </c>
+      <c r="AP55" s="10">
+        <v>119</v>
+      </c>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -17807,9 +18059,12 @@
       <c r="AO56" s="10">
         <v>876</v>
       </c>
+      <c r="AP56" s="10">
+        <v>898</v>
+      </c>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -17932,9 +18187,12 @@
       <c r="AO57" s="10">
         <v>9</v>
       </c>
+      <c r="AP57" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -18055,9 +18313,12 @@
       <c r="AO58" s="10">
         <v>7</v>
       </c>
+      <c r="AP58" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -18178,9 +18439,12 @@
       <c r="AO59" s="10">
         <v>22</v>
       </c>
+      <c r="AP59" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -18301,9 +18565,12 @@
       <c r="AO60" s="10">
         <v>2</v>
       </c>
+      <c r="AP60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -18426,9 +18693,12 @@
       <c r="AO61" s="10">
         <v>8</v>
       </c>
+      <c r="AP61" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -18549,9 +18819,12 @@
       <c r="AO62" s="10">
         <v>105</v>
       </c>
+      <c r="AP62" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
+    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -18672,9 +18945,12 @@
       <c r="AO63" s="10">
         <v>100</v>
       </c>
+      <c r="AP63" s="10">
+        <v>104</v>
+      </c>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -18795,9 +19071,12 @@
       <c r="AO64" s="10">
         <v>108</v>
       </c>
+      <c r="AP64" s="10">
+        <v>120</v>
+      </c>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -18918,9 +19197,12 @@
       <c r="AO65" s="10">
         <v>52</v>
       </c>
+      <c r="AP65" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A66" s="32"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -19041,8 +19323,11 @@
       <c r="AO66" s="10">
         <v>37</v>
       </c>
+      <c r="AP66" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -19166,9 +19451,12 @@
       <c r="AO67" s="10">
         <v>746</v>
       </c>
+      <c r="AP67" s="10">
+        <v>832</v>
+      </c>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -19291,9 +19579,12 @@
       <c r="AO68" s="10">
         <v>0</v>
       </c>
+      <c r="AP68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -19414,9 +19705,12 @@
       <c r="AO69" s="10">
         <v>11</v>
       </c>
+      <c r="AP69" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -19537,9 +19831,12 @@
       <c r="AO70" s="10">
         <v>2</v>
       </c>
+      <c r="AP70" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A71" s="31"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -19660,9 +19957,12 @@
       <c r="AO71" s="10">
         <v>13</v>
       </c>
+      <c r="AP71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A72" s="31"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -19783,9 +20083,12 @@
       <c r="AO72" s="10">
         <v>36</v>
       </c>
+      <c r="AP72" s="10">
+        <v>38</v>
+      </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A73" s="31"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -19906,9 +20209,12 @@
       <c r="AO73" s="10">
         <v>11</v>
       </c>
+      <c r="AP73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
+    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A74" s="31"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -20029,9 +20335,12 @@
       <c r="AO74" s="10">
         <v>1</v>
       </c>
+      <c r="AP74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A75" s="32"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -20152,9 +20461,12 @@
       <c r="AO75" s="10">
         <v>4</v>
       </c>
+      <c r="AP75" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A76" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -20277,9 +20589,12 @@
       <c r="AO76" s="10">
         <v>2</v>
       </c>
+      <c r="AP76" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A77" s="34"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -20400,9 +20715,12 @@
       <c r="AO77" s="10">
         <v>4</v>
       </c>
+      <c r="AP77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
+    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A78" s="34"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -20523,9 +20841,12 @@
       <c r="AO78" s="10">
         <v>56</v>
       </c>
+      <c r="AP78" s="10">
+        <v>56</v>
+      </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
+    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A79" s="34"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -20646,9 +20967,12 @@
       <c r="AO79" s="10">
         <v>9</v>
       </c>
+      <c r="AP79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -20769,8 +21093,11 @@
       <c r="AO80" s="10">
         <v>3</v>
       </c>
+      <c r="AP80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -20894,9 +21221,12 @@
       <c r="AO81" s="10">
         <v>198</v>
       </c>
+      <c r="AP81" s="10">
+        <v>204</v>
+      </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A82" s="30" t="s">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -21019,9 +21349,12 @@
       <c r="AO82" s="10">
         <v>158</v>
       </c>
+      <c r="AP82" s="10">
+        <v>160</v>
+      </c>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
+    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A83" s="34"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -21142,9 +21475,12 @@
       <c r="AO83" s="10">
         <v>46</v>
       </c>
+      <c r="AP83" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A84" s="34"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -21265,9 +21601,12 @@
       <c r="AO84" s="10">
         <v>118</v>
       </c>
+      <c r="AP84" s="10">
+        <v>120</v>
+      </c>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A85" s="34"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -21388,9 +21727,12 @@
       <c r="AO85" s="10">
         <v>6</v>
       </c>
+      <c r="AP85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
+    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A86" s="35"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -21511,9 +21853,12 @@
       <c r="AO86" s="10">
         <v>18</v>
       </c>
+      <c r="AP86" s="10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A87" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -21636,9 +21981,12 @@
       <c r="AO87" s="10">
         <v>15</v>
       </c>
+      <c r="AP87" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -21759,9 +22107,12 @@
       <c r="AO88" s="10">
         <v>58</v>
       </c>
+      <c r="AP88" s="10">
+        <v>94</v>
+      </c>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
+    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -21882,9 +22233,12 @@
       <c r="AO89" s="10">
         <v>7</v>
       </c>
+      <c r="AP89" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
+    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -22005,9 +22359,12 @@
       <c r="AO90" s="10">
         <v>13</v>
       </c>
+      <c r="AP90" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
+    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -22128,9 +22485,12 @@
       <c r="AO91" s="10">
         <v>4</v>
       </c>
+      <c r="AP91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
+    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -22251,9 +22611,12 @@
       <c r="AO92" s="10">
         <v>12</v>
       </c>
+      <c r="AP92" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A93" s="32"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -22374,9 +22737,12 @@
       <c r="AO93" s="10">
         <v>49</v>
       </c>
+      <c r="AP93" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -22499,9 +22865,12 @@
       <c r="AO94" s="10">
         <v>13</v>
       </c>
+      <c r="AP94" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
+    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A95" s="35"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -22622,8 +22991,11 @@
       <c r="AO95" s="10">
         <v>35</v>
       </c>
+      <c r="AP95" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -22747,9 +23119,12 @@
       <c r="AO96" s="10">
         <v>158</v>
       </c>
+      <c r="AP96" s="10">
+        <v>170</v>
+      </c>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A97" s="33" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -22872,9 +23247,12 @@
       <c r="AO97" s="10">
         <v>1645</v>
       </c>
+      <c r="AP97" s="10">
+        <v>1781</v>
+      </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A98" s="34"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -22995,9 +23373,12 @@
       <c r="AO98" s="10">
         <v>216</v>
       </c>
+      <c r="AP98" s="10">
+        <v>222</v>
+      </c>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
+    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A99" s="35"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -23118,9 +23499,12 @@
       <c r="AO99" s="10">
         <v>61</v>
       </c>
+      <c r="AP99" s="10">
+        <v>68</v>
+      </c>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A100" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -23243,9 +23627,12 @@
       <c r="AO100" s="10">
         <v>27</v>
       </c>
+      <c r="AP100" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
+    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -23366,9 +23753,12 @@
       <c r="AO101" s="10">
         <v>32</v>
       </c>
+      <c r="AP101" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
+    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -23489,9 +23879,12 @@
       <c r="AO102" s="10">
         <v>143</v>
       </c>
+      <c r="AP102" s="10">
+        <v>155</v>
+      </c>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
+    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -23612,9 +24005,12 @@
       <c r="AO103" s="10">
         <v>240</v>
       </c>
+      <c r="AP103" s="10">
+        <v>251</v>
+      </c>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
+    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A104" s="32"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -23735,9 +24131,12 @@
       <c r="AO104" s="10">
         <v>33</v>
       </c>
+      <c r="AP104" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A105" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -23860,9 +24259,12 @@
       <c r="AO105" s="10">
         <v>141</v>
       </c>
+      <c r="AP105" s="10">
+        <v>162</v>
+      </c>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A106" s="34"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -23983,9 +24385,12 @@
       <c r="AO106" s="10">
         <v>111</v>
       </c>
+      <c r="AP106" s="10">
+        <v>128</v>
+      </c>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A107" s="34"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -24106,9 +24511,12 @@
       <c r="AO107" s="10">
         <v>14</v>
       </c>
+      <c r="AP107" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+    <row r="108" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A108" s="34"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -24229,9 +24637,12 @@
       <c r="AO108" s="10">
         <v>31</v>
       </c>
+      <c r="AP108" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A109" s="32"/>
+    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A109" s="35"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -24352,8 +24763,11 @@
       <c r="AO109" s="10">
         <v>5</v>
       </c>
+      <c r="AP109" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -24477,8 +24891,11 @@
       <c r="AO110" s="10">
         <v>339</v>
       </c>
+      <c r="AP110" s="10">
+        <v>364</v>
+      </c>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -24602,9 +25019,12 @@
       <c r="AO111" s="10">
         <v>73</v>
       </c>
+      <c r="AP111" s="10">
+        <v>80</v>
+      </c>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A112" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -24727,9 +25147,12 @@
       <c r="AO112" s="10">
         <v>14</v>
       </c>
+      <c r="AP112" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+    <row r="113" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -24850,9 +25273,12 @@
       <c r="AO113" s="10">
         <v>18</v>
       </c>
+      <c r="AP113" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+    <row r="114" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A114" s="32"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -24973,9 +25399,12 @@
       <c r="AO114" s="10">
         <v>100</v>
       </c>
+      <c r="AP114" s="10">
+        <v>103</v>
+      </c>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A115" s="30" t="s">
+    <row r="115" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A115" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -25098,9 +25527,12 @@
       <c r="AO115" s="10">
         <v>103</v>
       </c>
+      <c r="AP115" s="10">
+        <v>103</v>
+      </c>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A116" s="31"/>
+    <row r="116" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A116" s="34"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -25221,9 +25653,12 @@
       <c r="AO116" s="10">
         <v>73</v>
       </c>
+      <c r="AP116" s="10">
+        <v>74</v>
+      </c>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
+    <row r="117" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A117" s="34"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -25344,9 +25779,12 @@
       <c r="AO117" s="10">
         <v>10</v>
       </c>
+      <c r="AP117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
+    <row r="118" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A118" s="34"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -25467,9 +25905,12 @@
       <c r="AO118" s="10">
         <v>43</v>
       </c>
+      <c r="AP118" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
+    <row r="119" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A119" s="34"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -25590,9 +26031,12 @@
       <c r="AO119" s="10">
         <v>8</v>
       </c>
+      <c r="AP119" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+    <row r="120" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A120" s="35"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -25713,9 +26157,12 @@
       <c r="AO120" s="10">
         <v>56</v>
       </c>
+      <c r="AP120" s="10">
+        <v>58</v>
+      </c>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A121" s="33" t="s">
+    <row r="121" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A121" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -25838,9 +26285,12 @@
       <c r="AO121" s="10">
         <v>7</v>
       </c>
+      <c r="AP121" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
+    <row r="122" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -25961,9 +26411,12 @@
       <c r="AO122" s="10">
         <v>23</v>
       </c>
+      <c r="AP122" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+    <row r="123" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -26084,9 +26537,12 @@
       <c r="AO123" s="10">
         <v>2</v>
       </c>
+      <c r="AP123" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+    <row r="124" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -26207,9 +26663,12 @@
       <c r="AO124" s="10">
         <v>5</v>
       </c>
+      <c r="AP124" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="125" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
+    <row r="125" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -26330,9 +26789,12 @@
       <c r="AO125" s="10">
         <v>2</v>
       </c>
+      <c r="AP125" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+    <row r="126" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -26453,9 +26915,12 @@
       <c r="AO126" s="10">
         <v>4</v>
       </c>
+      <c r="AP126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+    <row r="127" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -26576,9 +27041,12 @@
       <c r="AO127" s="10">
         <v>8</v>
       </c>
+      <c r="AP127" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
+    <row r="128" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -26699,9 +27167,12 @@
       <c r="AO128" s="10">
         <v>9</v>
       </c>
+      <c r="AP128" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+    <row r="129" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A129" s="31"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -26822,9 +27293,12 @@
       <c r="AO129" s="10">
         <v>144</v>
       </c>
+      <c r="AP129" s="10">
+        <v>142</v>
+      </c>
     </row>
-    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+    <row r="130" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A130" s="32"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -26945,8 +27419,11 @@
       <c r="AO130" s="10">
         <v>21</v>
       </c>
+      <c r="AP130" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -27070,9 +27547,12 @@
       <c r="AO131" s="10">
         <v>385</v>
       </c>
+      <c r="AP131" s="10">
+        <v>396</v>
+      </c>
     </row>
-    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A132" s="33" t="s">
+    <row r="132" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A132" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -27195,9 +27675,12 @@
       <c r="AO132" s="10">
         <v>21</v>
       </c>
+      <c r="AP132" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+    <row r="133" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A133" s="31"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -27318,9 +27801,12 @@
       <c r="AO133" s="10">
         <v>16</v>
       </c>
+      <c r="AP133" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+    <row r="134" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A134" s="31"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -27441,9 +27927,12 @@
       <c r="AO134" s="10">
         <v>2</v>
       </c>
+      <c r="AP134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A135" s="35"/>
+    <row r="135" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A135" s="32"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -27564,9 +28053,12 @@
       <c r="AO135" s="10">
         <v>2</v>
       </c>
+      <c r="AP135" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+    <row r="136" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A136" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -27689,9 +28181,12 @@
       <c r="AO136" s="10">
         <v>99</v>
       </c>
+      <c r="AP136" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
+    <row r="137" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A137" s="34"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -27812,9 +28307,12 @@
       <c r="AO137" s="10">
         <v>125</v>
       </c>
+      <c r="AP137" s="10">
+        <v>125</v>
+      </c>
     </row>
-    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
+    <row r="138" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A138" s="34"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -27935,9 +28433,12 @@
       <c r="AO138" s="10">
         <v>20</v>
       </c>
+      <c r="AP138" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A139" s="32"/>
+    <row r="139" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A139" s="35"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -28057,10 +28558,25 @@
       </c>
       <c r="AO139" s="10">
         <v>169</v>
+      </c>
+      <c r="AP139" s="10">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -28073,18 +28589,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -29057,7 +29561,7 @@
       </c>
       <c r="AX4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="AY4" s="10">
         <f t="shared" si="7"/>
@@ -29382,7 +29886,7 @@
       </c>
       <c r="AX6" s="12">
         <f>MAX(0, (dc!AX2-dc!AW2))</f>
-        <v>0</v>
+        <v>1056</v>
       </c>
       <c r="AY6" s="12">
         <f>MAX(0, (dc!AY2-dc!AX2))</f>
@@ -30354,7 +30858,7 @@
       </c>
       <c r="AX9" s="12">
         <f>MAX(0, (dc!AX5-dc!AW5))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AY9" s="12">
         <f>MAX(0, (dc!AY5-dc!AX5))</f>
@@ -33759,7 +34263,7 @@
       </c>
       <c r="AM2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.117149758454104</v>
       </c>
       <c r="AN2" s="20">
         <f t="shared" si="0"/>
@@ -34032,7 +34536,7 @@
       </c>
       <c r="AM3" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.1907514450867041</v>
       </c>
       <c r="AN3" s="20">
         <f t="shared" si="3"/>
@@ -34305,7 +34809,7 @@
       </c>
       <c r="AM4" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.9479768786127165</v>
       </c>
       <c r="AN4" s="20">
         <f t="shared" si="5"/>
@@ -34641,7 +35145,7 @@
       </c>
       <c r="AM6" s="14">
         <f>MAX(0,(md!AM2-md!AL2)+(md!AM3-md!AL3))</f>
-        <v>0</v>
+        <v>6624</v>
       </c>
       <c r="AN6" s="14">
         <f>MAX(0,(md!AN2-md!AM2)+(md!AN3-md!AM3))</f>
@@ -34913,7 +35417,7 @@
       </c>
       <c r="AM7" s="14">
         <f>MAX(0,(md!AM3-md!AL3))</f>
-        <v>0</v>
+        <v>1730</v>
       </c>
       <c r="AN7" s="14">
         <f>MAX(0,(md!AN3-md!AM3))</f>
@@ -35185,7 +35689,7 @@
       </c>
       <c r="AM8" s="14">
         <f>MAX(0,(md!AM4-md!AL4))</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="AN8" s="14">
         <f>MAX(0,(md!AN4-md!AM4))</f>
@@ -35457,7 +35961,7 @@
       </c>
       <c r="AM9" s="14">
         <f>MAX(0,(md!AM5-md!AL5))</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="AN9" s="14">
         <f>MAX(0,(md!AN5-md!AM5))</f>
@@ -36220,7 +36724,7 @@
       </c>
       <c r="AM12" s="14">
         <f>MAX(0,(md!AM8-md!AL8))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="AN12" s="14">
         <f>MAX(0,(md!AN8-md!AM8))</f>
@@ -36497,7 +37001,7 @@
       </c>
       <c r="AM13" s="14">
         <f>MAX(0,(md!AM9-md!AL9))</f>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="AN13" s="14">
         <f>MAX(0,(md!AN9-md!AM9))</f>
@@ -36774,7 +37278,7 @@
       </c>
       <c r="AM14" s="14">
         <f>MAX(0,(md!AM10-md!AL10))</f>
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="AN14" s="14">
         <f>MAX(0,(md!AN10-md!AM10))</f>
@@ -37051,7 +37555,7 @@
       </c>
       <c r="AM15" s="14">
         <f>MAX(0,(md!AM11-md!AL11))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AN15" s="14">
         <f>MAX(0,(md!AN11-md!AM11))</f>
@@ -37328,7 +37832,7 @@
       </c>
       <c r="AM16" s="14">
         <f>MAX(0,(md!AM12-md!AL12))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN16" s="14">
         <f>MAX(0,(md!AN12-md!AM12))</f>
@@ -37605,7 +38109,7 @@
       </c>
       <c r="AM17" s="14">
         <f>MAX(0,(md!AM13-md!AL13))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AN17" s="14">
         <f>MAX(0,(md!AN13-md!AM13))</f>
@@ -37882,7 +38386,7 @@
       </c>
       <c r="AM18" s="14">
         <f>MAX(0,(md!AM14-md!AL14))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AN18" s="14">
         <f>MAX(0,(md!AN14-md!AM14))</f>
@@ -38159,7 +38663,7 @@
       </c>
       <c r="AM19" s="14">
         <f>MAX(0,(md!AM15-md!AL15))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AN19" s="14">
         <f>MAX(0,(md!AN15-md!AM15))</f>
@@ -38436,7 +38940,7 @@
       </c>
       <c r="AM20" s="14">
         <f>MAX(0,(md!AM16-md!AL16))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN20" s="14">
         <f>MAX(0,(md!AN16-md!AM16))</f>
@@ -38713,7 +39217,7 @@
       </c>
       <c r="AM21" s="14">
         <f>MAX(0,(md!AM17-md!AL17))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AN21" s="14">
         <f>MAX(0,(md!AN17-md!AM17))</f>
@@ -39267,7 +39771,7 @@
       </c>
       <c r="AM23" s="14">
         <f>MAX(0,(md!AM19-md!AL19))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AN23" s="14">
         <f>MAX(0,(md!AN19-md!AM19))</f>
@@ -39544,7 +40048,7 @@
       </c>
       <c r="AM24" s="14">
         <f>MAX(0,(md!AM20-md!AL20))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AN24" s="14">
         <f>MAX(0,(md!AN20-md!AM20))</f>
@@ -39821,7 +40325,7 @@
       </c>
       <c r="AM25" s="14">
         <f>MAX(0,(md!AM21-md!AL21))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AN25" s="14">
         <f>MAX(0,(md!AN21-md!AM21))</f>
@@ -40098,7 +40602,7 @@
       </c>
       <c r="AM26" s="14">
         <f>MAX(0,(md!AM22-md!AL22))</f>
-        <v>0</v>
+        <v>454</v>
       </c>
       <c r="AN26" s="14">
         <f>MAX(0,(md!AN22-md!AM22))</f>
@@ -40375,7 +40879,7 @@
       </c>
       <c r="AM27" s="14">
         <f>MAX(0,(md!AM23-md!AL23))</f>
-        <v>0</v>
+        <v>692</v>
       </c>
       <c r="AN27" s="14">
         <f>MAX(0,(md!AN23-md!AM23))</f>
@@ -40929,7 +41433,7 @@
       </c>
       <c r="AM29" s="14">
         <f>MAX(0,(md!AM25-md!AL25))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AN29" s="14">
         <f>MAX(0,(md!AN25-md!AM25))</f>
@@ -41206,7 +41710,7 @@
       </c>
       <c r="AM30" s="14">
         <f>MAX(0,(md!AM26-md!AL26))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN30" s="14">
         <f>MAX(0,(md!AN26-md!AM26))</f>
@@ -41760,7 +42264,7 @@
       </c>
       <c r="AM32" s="14">
         <f>MAX(0,(md!AM28-md!AL28))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AN32" s="14">
         <f>MAX(0,(md!AN28-md!AM28))</f>
@@ -42037,7 +42541,7 @@
       </c>
       <c r="AM33" s="14">
         <f>MAX(0,(md!AM29-md!AL29))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AN33" s="14">
         <f>MAX(0,(md!AN29-md!AM29))</f>
@@ -42314,7 +42818,7 @@
       </c>
       <c r="AM34" s="14">
         <f>MAX(0,(md!AM30-md!AL30))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN34" s="14">
         <f>MAX(0,(md!AN30-md!AM30))</f>
@@ -42793,7 +43297,7 @@
       </c>
       <c r="AO2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.1259709557581905</v>
       </c>
       <c r="AP2" s="19">
         <f t="shared" si="1"/>
@@ -43070,7 +43574,7 @@
       </c>
       <c r="AO3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8.9099526066350716</v>
       </c>
       <c r="AP3" s="19">
         <f t="shared" si="3"/>
@@ -43347,7 +43851,7 @@
       </c>
       <c r="AO4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.7488151658767772</v>
       </c>
       <c r="AP4" s="19">
         <f t="shared" si="5"/>
@@ -43624,7 +44128,7 @@
       </c>
       <c r="AO6" s="14">
         <f>MAX(0,(va!AP5-va!AO5))</f>
-        <v>0</v>
+        <v>14805</v>
       </c>
       <c r="AP6" s="14">
         <f>MAX(0,(va!AQ5-va!AP5))</f>
@@ -43901,7 +44405,7 @@
       </c>
       <c r="AO7" s="14">
         <f>MAX(0,(va!AP2-va!AO2))</f>
-        <v>0</v>
+        <v>1055</v>
       </c>
       <c r="AP7" s="14">
         <f>MAX(0,(va!AQ2-va!AP2))</f>
@@ -44178,7 +44682,7 @@
       </c>
       <c r="AO8" s="14">
         <f>MAX(0,(va!AP3-va!AO3))</f>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="AP8" s="14">
         <f>MAX(0,(va!AQ3-va!AP3))</f>
@@ -44455,7 +44959,7 @@
       </c>
       <c r="AO9" s="14">
         <f>MAX(0,(va!AP4-va!AO4))</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AP9" s="14">
         <f>MAX(0,(va!AQ4-va!AP4))</f>
@@ -44952,7 +45456,7 @@
       </c>
       <c r="AO11" s="16">
         <f>MAX(0,(va!AP7-va!AO7))</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="AP11" s="16">
         <f>MAX(0,(va!AQ7-va!AP7))</f>
@@ -46080,7 +46584,7 @@
       </c>
       <c r="AO15" s="16">
         <f>MAX(0,(va!AP11-va!AO11))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP15" s="16">
         <f>MAX(0,(va!AQ11-va!AP11))</f>
@@ -46926,7 +47430,7 @@
       </c>
       <c r="AO18" s="16">
         <f>MAX(0,(va!AP14-va!AO14))</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AP18" s="16">
         <f>MAX(0,(va!AQ14-va!AP14))</f>
@@ -47208,7 +47712,7 @@
       </c>
       <c r="AO19" s="16">
         <f>MAX(0,(va!AP15-va!AO15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP19" s="16">
         <f>MAX(0,(va!AQ15-va!AP15))</f>
@@ -48054,7 +48558,7 @@
       </c>
       <c r="AO22" s="16">
         <f>MAX(0,(va!AP18-va!AO18))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP22" s="16">
         <f>MAX(0,(va!AQ18-va!AP18))</f>
@@ -48336,7 +48840,7 @@
       </c>
       <c r="AO23" s="16">
         <f>MAX(0,(va!AP19-va!AO19))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AP23" s="16">
         <f>MAX(0,(va!AQ19-va!AP19))</f>
@@ -48900,7 +49404,7 @@
       </c>
       <c r="AO25" s="16">
         <f>MAX(0,(va!AP21-va!AO21))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AP25" s="16">
         <f>MAX(0,(va!AQ21-va!AP21))</f>
@@ -49182,7 +49686,7 @@
       </c>
       <c r="AO26" s="16">
         <f>MAX(0,(va!AP22-va!AO22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP26" s="16">
         <f>MAX(0,(va!AQ22-va!AP22))</f>
@@ -49746,7 +50250,7 @@
       </c>
       <c r="AO28" s="16">
         <f>MAX(0,(va!AP24-va!AO24))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP28" s="16">
         <f>MAX(0,(va!AQ24-va!AP24))</f>
@@ -50028,7 +50532,7 @@
       </c>
       <c r="AO29" s="16">
         <f>MAX(0,(va!AP25-va!AO25))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP29" s="16">
         <f>MAX(0,(va!AQ25-va!AP25))</f>
@@ -50592,7 +51096,7 @@
       </c>
       <c r="AO31" s="16">
         <f>MAX(0,(va!AP27-va!AO27))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP31" s="16">
         <f>MAX(0,(va!AQ27-va!AP27))</f>
@@ -51156,7 +51660,7 @@
       </c>
       <c r="AO33" s="16">
         <f>MAX(0,(va!AP29-va!AO29))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP33" s="16">
         <f>MAX(0,(va!AQ29-va!AP29))</f>
@@ -51438,7 +51942,7 @@
       </c>
       <c r="AO34" s="16">
         <f>MAX(0,(va!AP30-va!AO30))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AP34" s="16">
         <f>MAX(0,(va!AQ30-va!AP30))</f>
@@ -51720,7 +52224,7 @@
       </c>
       <c r="AO35" s="16">
         <f>MAX(0,(va!AP31-va!AO31))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AP35" s="16">
         <f>MAX(0,(va!AQ31-va!AP31))</f>
@@ -52002,7 +52506,7 @@
       </c>
       <c r="AO36" s="16">
         <f>MAX(0,(va!AP32-va!AO32))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP36" s="16">
         <f>MAX(0,(va!AQ32-va!AP32))</f>
@@ -52848,7 +53352,7 @@
       </c>
       <c r="AO39" s="16">
         <f>MAX(0,(va!AP35-va!AO35))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP39" s="16">
         <f>MAX(0,(va!AQ35-va!AP35))</f>
@@ -53130,7 +53634,7 @@
       </c>
       <c r="AO40" s="16">
         <f>MAX(0,(va!AP36-va!AO36))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AP40" s="16">
         <f>MAX(0,(va!AQ36-va!AP36))</f>
@@ -54258,7 +54762,7 @@
       </c>
       <c r="AO44" s="16">
         <f>MAX(0,(va!AP40-va!AO40))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP44" s="16">
         <f>MAX(0,(va!AQ40-va!AP40))</f>
@@ -55386,7 +55890,7 @@
       </c>
       <c r="AO48" s="16">
         <f>MAX(0,(va!AP44-va!AO44))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP48" s="16">
         <f>MAX(0,(va!AQ44-va!AP44))</f>
@@ -55668,7 +56172,7 @@
       </c>
       <c r="AO49" s="16">
         <f>MAX(0,(va!AP45-va!AO45))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP49" s="16">
         <f>MAX(0,(va!AQ45-va!AP45))</f>
@@ -56514,7 +57018,7 @@
       </c>
       <c r="AO52" s="16">
         <f>MAX(0,(va!AP48-va!AO48))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP52" s="16">
         <f>MAX(0,(va!AQ48-va!AP48))</f>
@@ -57078,7 +57582,7 @@
       </c>
       <c r="AO54" s="16">
         <f>MAX(0,(va!AP50-va!AO50))</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AP54" s="16">
         <f>MAX(0,(va!AQ50-va!AP50))</f>
@@ -57360,7 +57864,7 @@
       </c>
       <c r="AO55" s="16">
         <f>MAX(0,(va!AP51-va!AO51))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AP55" s="16">
         <f>MAX(0,(va!AQ51-va!AP51))</f>
@@ -57642,7 +58146,7 @@
       </c>
       <c r="AO56" s="16">
         <f>MAX(0,(va!AP52-va!AO52))</f>
-        <v>0</v>
+        <v>286</v>
       </c>
       <c r="AP56" s="16">
         <f>MAX(0,(va!AQ52-va!AP52))</f>
@@ -57924,7 +58428,7 @@
       </c>
       <c r="AO57" s="16">
         <f>MAX(0,(va!AP53-va!AO53))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP57" s="16">
         <f>MAX(0,(va!AQ53-va!AP53))</f>
@@ -58488,7 +58992,7 @@
       </c>
       <c r="AO59" s="16">
         <f>MAX(0,(va!AP55-va!AO55))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AP59" s="16">
         <f>MAX(0,(va!AQ55-va!AP55))</f>
@@ -58770,7 +59274,7 @@
       </c>
       <c r="AO60" s="16">
         <f>MAX(0,(va!AP56-va!AO56))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AP60" s="16">
         <f>MAX(0,(va!AQ56-va!AP56))</f>
@@ -59052,7 +59556,7 @@
       </c>
       <c r="AO61" s="16">
         <f>MAX(0,(va!AP57-va!AO57))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP61" s="16">
         <f>MAX(0,(va!AQ57-va!AP57))</f>
@@ -60180,7 +60684,7 @@
       </c>
       <c r="AO65" s="16">
         <f>MAX(0,(va!AP61-va!AO61))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP65" s="16">
         <f>MAX(0,(va!AQ61-va!AP61))</f>
@@ -60462,7 +60966,7 @@
       </c>
       <c r="AO66" s="16">
         <f>MAX(0,(va!AP62-va!AO62))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AP66" s="16">
         <f>MAX(0,(va!AQ62-va!AP62))</f>
@@ -60744,7 +61248,7 @@
       </c>
       <c r="AO67" s="16">
         <f>MAX(0,(va!AP63-va!AO63))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AP67" s="16">
         <f>MAX(0,(va!AQ63-va!AP63))</f>
@@ -61026,7 +61530,7 @@
       </c>
       <c r="AO68" s="16">
         <f>MAX(0,(va!AP64-va!AO64))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AP68" s="16">
         <f>MAX(0,(va!AQ64-va!AP64))</f>
@@ -61308,7 +61812,7 @@
       </c>
       <c r="AO69" s="16">
         <f>MAX(0,(va!AP65-va!AO65))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP69" s="16">
         <f>MAX(0,(va!AQ65-va!AP65))</f>
@@ -61590,7 +62094,7 @@
       </c>
       <c r="AO70" s="16">
         <f>MAX(0,(va!AP66-va!AO66))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AP70" s="16">
         <f>MAX(0,(va!AQ66-va!AP66))</f>
@@ -61872,7 +62376,7 @@
       </c>
       <c r="AO71" s="16">
         <f>MAX(0,(va!AP67-va!AO67))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="AP71" s="16">
         <f>MAX(0,(va!AQ67-va!AP67))</f>
@@ -62436,7 +62940,7 @@
       </c>
       <c r="AO73" s="16">
         <f>MAX(0,(va!AP69-va!AO69))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP73" s="16">
         <f>MAX(0,(va!AQ69-va!AP69))</f>
@@ -63282,7 +63786,7 @@
       </c>
       <c r="AO76" s="16">
         <f>MAX(0,(va!AP72-va!AO72))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP76" s="16">
         <f>MAX(0,(va!AQ72-va!AP72))</f>
@@ -64128,7 +64632,7 @@
       </c>
       <c r="AO79" s="16">
         <f>MAX(0,(va!AP75-va!AO75))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP79" s="16">
         <f>MAX(0,(va!AQ75-va!AP75))</f>
@@ -64410,7 +64914,7 @@
       </c>
       <c r="AO80" s="16">
         <f>MAX(0,(va!AP76-va!AO76))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP80" s="16">
         <f>MAX(0,(va!AQ76-va!AP76))</f>
@@ -65820,7 +66324,7 @@
       </c>
       <c r="AO85" s="16">
         <f>MAX(0,(va!AP81-va!AO81))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AP85" s="16">
         <f>MAX(0,(va!AQ81-va!AP81))</f>
@@ -66102,7 +66606,7 @@
       </c>
       <c r="AO86" s="16">
         <f>MAX(0,(va!AP82-va!AO82))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP86" s="16">
         <f>MAX(0,(va!AQ82-va!AP82))</f>
@@ -66666,7 +67170,7 @@
       </c>
       <c r="AO88" s="16">
         <f>MAX(0,(va!AP84-va!AO84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP88" s="16">
         <f>MAX(0,(va!AQ84-va!AP84))</f>
@@ -67230,7 +67734,7 @@
       </c>
       <c r="AO90" s="16">
         <f>MAX(0,(va!AP86-va!AO86))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP90" s="16">
         <f>MAX(0,(va!AQ86-va!AP86))</f>
@@ -67512,7 +68016,7 @@
       </c>
       <c r="AO91" s="16">
         <f>MAX(0,(va!AP87-va!AO87))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP91" s="16">
         <f>MAX(0,(va!AQ87-va!AP87))</f>
@@ -67794,7 +68298,7 @@
       </c>
       <c r="AO92" s="16">
         <f>MAX(0,(va!AP88-va!AO88))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AP92" s="16">
         <f>MAX(0,(va!AQ88-va!AP88))</f>
@@ -68076,7 +68580,7 @@
       </c>
       <c r="AO93" s="16">
         <f>MAX(0,(va!AP89-va!AO89))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP93" s="16">
         <f>MAX(0,(va!AQ89-va!AP89))</f>
@@ -68922,7 +69426,7 @@
       </c>
       <c r="AO96" s="16">
         <f>MAX(0,(va!AP92-va!AO92))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP96" s="16">
         <f>MAX(0,(va!AQ92-va!AP92))</f>
@@ -69204,7 +69708,7 @@
       </c>
       <c r="AO97" s="16">
         <f>MAX(0,(va!AP93-va!AO93))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP97" s="16">
         <f>MAX(0,(va!AQ93-va!AP93))</f>
@@ -70050,7 +70554,7 @@
       </c>
       <c r="AO100" s="16">
         <f>MAX(0,(va!AP96-va!AO96))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AP100" s="16">
         <f>MAX(0,(va!AQ96-va!AP96))</f>
@@ -70332,7 +70836,7 @@
       </c>
       <c r="AO101" s="16">
         <f>MAX(0,(va!AP97-va!AO97))</f>
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="AP101" s="16">
         <f>MAX(0,(va!AQ97-va!AP97))</f>
@@ -70614,7 +71118,7 @@
       </c>
       <c r="AO102" s="16">
         <f>MAX(0,(va!AP98-va!AO98))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AP102" s="16">
         <f>MAX(0,(va!AQ98-va!AP98))</f>
@@ -70896,7 +71400,7 @@
       </c>
       <c r="AO103" s="16">
         <f>MAX(0,(va!AP99-va!AO99))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AP103" s="16">
         <f>MAX(0,(va!AQ99-va!AP99))</f>
@@ -71178,7 +71682,7 @@
       </c>
       <c r="AO104" s="16">
         <f>MAX(0,(va!AP100-va!AO100))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP104" s="16">
         <f>MAX(0,(va!AQ100-va!AP100))</f>
@@ -71460,7 +71964,7 @@
       </c>
       <c r="AO105" s="16">
         <f>MAX(0,(va!AP101-va!AO101))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP105" s="16">
         <f>MAX(0,(va!AQ101-va!AP101))</f>
@@ -71742,7 +72246,7 @@
       </c>
       <c r="AO106" s="16">
         <f>MAX(0,(va!AP102-va!AO102))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AP106" s="16">
         <f>MAX(0,(va!AQ102-va!AP102))</f>
@@ -72024,7 +72528,7 @@
       </c>
       <c r="AO107" s="16">
         <f>MAX(0,(va!AP103-va!AO103))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AP107" s="16">
         <f>MAX(0,(va!AQ103-va!AP103))</f>
@@ -72306,7 +72810,7 @@
       </c>
       <c r="AO108" s="16">
         <f>MAX(0,(va!AP104-va!AO104))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP108" s="16">
         <f>MAX(0,(va!AQ104-va!AP104))</f>
@@ -72588,7 +73092,7 @@
       </c>
       <c r="AO109" s="16">
         <f>MAX(0,(va!AP105-va!AO105))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AP109" s="16">
         <f>MAX(0,(va!AQ105-va!AP105))</f>
@@ -72870,7 +73374,7 @@
       </c>
       <c r="AO110" s="16">
         <f>MAX(0,(va!AP106-va!AO106))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AP110" s="16">
         <f>MAX(0,(va!AQ106-va!AP106))</f>
@@ -73434,7 +73938,7 @@
       </c>
       <c r="AO112" s="16">
         <f>MAX(0,(va!AP108-va!AO108))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP112" s="16">
         <f>MAX(0,(va!AQ108-va!AP108))</f>
@@ -73998,7 +74502,7 @@
       </c>
       <c r="AO114" s="16">
         <f>MAX(0,(va!AP110-va!AO110))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AP114" s="16">
         <f>MAX(0,(va!AQ110-va!AP110))</f>
@@ -74280,7 +74784,7 @@
       </c>
       <c r="AO115" s="16">
         <f>MAX(0,(va!AP111-va!AO111))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AP115" s="16">
         <f>MAX(0,(va!AQ111-va!AP111))</f>
@@ -75126,7 +75630,7 @@
       </c>
       <c r="AO118" s="16">
         <f>MAX(0,(va!AP114-va!AO114))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP118" s="16">
         <f>MAX(0,(va!AQ114-va!AP114))</f>
@@ -75690,7 +76194,7 @@
       </c>
       <c r="AO120" s="16">
         <f>MAX(0,(va!AP116-va!AO116))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP120" s="16">
         <f>MAX(0,(va!AQ116-va!AP116))</f>
@@ -76254,7 +76758,7 @@
       </c>
       <c r="AO122" s="16">
         <f>MAX(0,(va!AP118-va!AO118))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP122" s="16">
         <f>MAX(0,(va!AQ118-va!AP118))</f>
@@ -76818,7 +77322,7 @@
       </c>
       <c r="AO124" s="16">
         <f>MAX(0,(va!AP120-va!AO120))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP124" s="16">
         <f>MAX(0,(va!AQ120-va!AP120))</f>
@@ -77100,7 +77604,7 @@
       </c>
       <c r="AO125" s="16">
         <f>MAX(0,(va!AP121-va!AO121))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP125" s="16">
         <f>MAX(0,(va!AQ121-va!AP121))</f>
@@ -77382,7 +77886,7 @@
       </c>
       <c r="AO126" s="16">
         <f>MAX(0,(va!AP122-va!AO122))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP126" s="16">
         <f>MAX(0,(va!AQ122-va!AP122))</f>
@@ -78228,7 +78732,7 @@
       </c>
       <c r="AO129" s="16">
         <f>MAX(0,(va!AP125-va!AO125))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP129" s="16">
         <f>MAX(0,(va!AQ125-va!AP125))</f>
@@ -79638,7 +80142,7 @@
       </c>
       <c r="AO134" s="16">
         <f>MAX(0,(va!AP130-va!AO130))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP134" s="16">
         <f>MAX(0,(va!AQ130-va!AP130))</f>
@@ -79920,7 +80424,7 @@
       </c>
       <c r="AO135" s="16">
         <f>MAX(0,(va!AP131-va!AO131))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AP135" s="16">
         <f>MAX(0,(va!AQ131-va!AP131))</f>
@@ -81894,7 +82398,7 @@
       </c>
       <c r="AO142" s="16">
         <f>MAX(0,(va!AP138-va!AO138))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP142" s="16">
         <f>MAX(0,(va!AQ138-va!AP138))</f>
@@ -82176,7 +82680,7 @@
       </c>
       <c r="AO143" s="16">
         <f>MAX(0,(va!AP139-va!AO139))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AP143" s="16">
         <f>MAX(0,(va!AQ139-va!AP139))</f>

</xml_diff>

<commit_message>
02 May data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF9050B-D384-4B20-A744-98330A6AA583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157912FB-C96E-4D22-A80F-C85CC05F43CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4018,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
+      <selection pane="bottomRight" activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4185,6 +4185,9 @@
       <c r="AX2" s="12">
         <v>21135</v>
       </c>
+      <c r="AY2" s="12">
+        <v>22004</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4373,7 +4376,7 @@
       </c>
       <c r="AY3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4797</v>
       </c>
       <c r="AZ3" s="10">
         <f t="shared" si="0"/>
@@ -4652,6 +4655,9 @@
       <c r="AX5" s="10">
         <v>231</v>
       </c>
+      <c r="AY5" s="10">
+        <v>240</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5049,6 +5055,9 @@
       <c r="AX7" s="10">
         <v>543</v>
       </c>
+      <c r="AY7" s="10">
+        <v>621</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5200,6 +5209,9 @@
       </c>
       <c r="AX8" s="10">
         <v>291</v>
+      </c>
+      <c r="AY8" s="10">
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
@@ -5353,6 +5365,9 @@
       <c r="AX9" s="10">
         <v>282</v>
       </c>
+      <c r="AY9" s="10">
+        <v>302</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5505,6 +5520,9 @@
       <c r="AX10" s="10">
         <v>774</v>
       </c>
+      <c r="AY10" s="10">
+        <v>889</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5657,6 +5675,9 @@
       <c r="AX11" s="10">
         <v>646</v>
       </c>
+      <c r="AY11" s="10">
+        <v>722</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5809,6 +5830,9 @@
       <c r="AX12" s="10">
         <v>450</v>
       </c>
+      <c r="AY12" s="10">
+        <v>476</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5961,6 +5985,9 @@
       <c r="AX13" s="10">
         <v>659</v>
       </c>
+      <c r="AY13" s="10">
+        <v>711</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6113,6 +6140,9 @@
       <c r="AX14" s="10">
         <v>632</v>
       </c>
+      <c r="AY14" s="10">
+        <v>692</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6264,6 +6294,9 @@
       </c>
       <c r="AX15" s="10">
         <v>46</v>
+      </c>
+      <c r="AY15" s="10">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6653,7 +6686,7 @@
         <v>97511</v>
       </c>
       <c r="AN2" s="10">
-        <v>0</v>
+        <v>101049</v>
       </c>
       <c r="AO2" s="10">
         <v>0</v>
@@ -6896,7 +6929,7 @@
       </c>
       <c r="AN3" s="10">
         <f>SUM(md[2-May])</f>
-        <v>0</v>
+        <v>24473</v>
       </c>
       <c r="AO3" s="10">
         <f>SUM(md[3-May])</f>
@@ -7131,7 +7164,7 @@
         <v>4718</v>
       </c>
       <c r="AN4" s="10">
-        <v>0</v>
+        <v>4910</v>
       </c>
       <c r="AO4" s="10">
         <v>0</v>
@@ -7337,7 +7370,7 @@
         <v>1098</v>
       </c>
       <c r="AN5" s="10">
-        <v>0</v>
+        <v>1156</v>
       </c>
       <c r="AO5" s="10">
         <v>0</v>
@@ -7754,6 +7787,9 @@
       <c r="AM7">
         <v>118</v>
       </c>
+      <c r="AN7">
+        <v>121</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7873,6 +7909,9 @@
       <c r="AM8" s="10">
         <v>1807</v>
       </c>
+      <c r="AN8" s="10">
+        <v>1885</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -7992,6 +8031,9 @@
       <c r="AM9">
         <v>2162</v>
       </c>
+      <c r="AN9">
+        <v>2237</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -8111,6 +8153,9 @@
       <c r="AM10">
         <v>3013</v>
       </c>
+      <c r="AN10">
+        <v>3183</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8230,6 +8275,9 @@
       <c r="AM11">
         <v>161</v>
       </c>
+      <c r="AN11">
+        <v>160</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8349,6 +8397,9 @@
       <c r="AM12">
         <v>74</v>
       </c>
+      <c r="AN12">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8468,6 +8519,9 @@
       <c r="AM13">
         <v>460</v>
       </c>
+      <c r="AN13">
+        <v>480</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8587,6 +8641,9 @@
       <c r="AM14">
         <v>176</v>
       </c>
+      <c r="AN14">
+        <v>187</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8706,6 +8763,9 @@
       <c r="AM15">
         <v>611</v>
       </c>
+      <c r="AN15">
+        <v>622</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8825,8 +8885,11 @@
       <c r="AM16" s="10">
         <v>54</v>
       </c>
+      <c r="AN16" s="10">
+        <v>59</v>
+      </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -8944,8 +9007,11 @@
       <c r="AM17">
         <v>942</v>
       </c>
+      <c r="AN17">
+        <v>976</v>
+      </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -9063,8 +9129,11 @@
       <c r="AM18">
         <v>4</v>
       </c>
+      <c r="AN18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -9182,8 +9251,11 @@
       <c r="AM19">
         <v>437</v>
       </c>
+      <c r="AN19">
+        <v>468</v>
+      </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9301,8 +9373,11 @@
       <c r="AM20">
         <v>896</v>
       </c>
+      <c r="AN20">
+        <v>931</v>
+      </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9420,8 +9495,11 @@
       <c r="AM21">
         <v>86</v>
       </c>
+      <c r="AN21">
+        <v>80</v>
+      </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9539,8 +9617,11 @@
       <c r="AM22">
         <v>4754</v>
       </c>
+      <c r="AN22">
+        <v>4919</v>
+      </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9658,8 +9739,11 @@
       <c r="AM23">
         <v>6735</v>
       </c>
+      <c r="AN23">
+        <v>7041</v>
+      </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9777,8 +9861,11 @@
       <c r="AM24">
         <v>52</v>
       </c>
+      <c r="AN24">
+        <v>57</v>
+      </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9896,8 +9983,11 @@
       <c r="AM25">
         <v>159</v>
       </c>
+      <c r="AN25">
+        <v>164</v>
+      </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -10015,8 +10105,11 @@
       <c r="AM26">
         <v>30</v>
       </c>
+      <c r="AN26">
+        <v>32</v>
+      </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -10134,8 +10227,11 @@
       <c r="AM27">
         <v>35</v>
       </c>
+      <c r="AN27">
+        <v>39</v>
+      </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -10253,8 +10349,11 @@
       <c r="AM28">
         <v>216</v>
       </c>
+      <c r="AN28">
+        <v>225</v>
+      </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -10372,8 +10471,11 @@
       <c r="AM29">
         <v>425</v>
       </c>
+      <c r="AN29">
+        <v>452</v>
+      </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10491,8 +10593,11 @@
       <c r="AM30">
         <v>65</v>
       </c>
+      <c r="AN30">
+        <v>72</v>
+      </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10589,7 +10694,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="AD6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AP2" sqref="AP2"/>
+      <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10771,7 +10876,7 @@
       </c>
       <c r="AQ2" s="10">
         <f>SUM(va[2-May])</f>
-        <v>0</v>
+        <v>17731</v>
       </c>
       <c r="AR2" s="10">
         <f>SUM(va[3-May])</f>
@@ -11009,7 +11114,7 @@
         <v>2416</v>
       </c>
       <c r="AQ3" s="10">
-        <v>0</v>
+        <v>2519</v>
       </c>
       <c r="AR3" s="10">
         <v>0</v>
@@ -11218,7 +11323,7 @@
         <v>581</v>
       </c>
       <c r="AQ4" s="10">
-        <v>0</v>
+        <v>616</v>
       </c>
       <c r="AR4" s="10">
         <v>0</v>
@@ -11427,7 +11532,7 @@
         <v>105648</v>
       </c>
       <c r="AQ5" s="10">
-        <v>0</v>
+        <v>112450</v>
       </c>
       <c r="AR5" s="10">
         <v>0</v>
@@ -11862,9 +11967,12 @@
       <c r="AP7" s="10">
         <v>802</v>
       </c>
+      <c r="AQ7" s="10">
+        <v>848</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -11990,9 +12098,12 @@
       <c r="AP8" s="10">
         <v>6</v>
       </c>
+      <c r="AQ8" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -12116,9 +12227,12 @@
       <c r="AP9" s="10">
         <v>28</v>
       </c>
+      <c r="AQ9" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -12242,9 +12356,12 @@
       <c r="AP10" s="10">
         <v>3</v>
       </c>
+      <c r="AQ10" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -12368,9 +12485,12 @@
       <c r="AP11" s="10">
         <v>53</v>
       </c>
+      <c r="AQ11" s="10">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -12494,9 +12614,12 @@
       <c r="AP12" s="10">
         <v>0</v>
       </c>
+      <c r="AQ12" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -12618,6 +12741,9 @@
         <v>26</v>
       </c>
       <c r="AP13" s="10">
+        <v>26</v>
+      </c>
+      <c r="AQ13" s="10">
         <v>26</v>
       </c>
     </row>
@@ -12748,9 +12874,12 @@
       <c r="AP14" s="10">
         <v>1004</v>
       </c>
+      <c r="AQ14" s="10">
+        <v>1044</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12876,9 +13005,12 @@
       <c r="AP15" s="10">
         <v>44</v>
       </c>
+      <c r="AQ15" s="10">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -13002,9 +13134,12 @@
       <c r="AP16" s="10">
         <v>0</v>
       </c>
+      <c r="AQ16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -13128,9 +13263,12 @@
       <c r="AP17" s="10">
         <v>2</v>
       </c>
+      <c r="AQ17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -13254,9 +13392,12 @@
       <c r="AP18" s="10">
         <v>7</v>
       </c>
+      <c r="AQ18" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -13380,9 +13521,12 @@
       <c r="AP19" s="10">
         <v>249</v>
       </c>
+      <c r="AQ19" s="10">
+        <v>259</v>
+      </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -13506,9 +13650,12 @@
       <c r="AP20" s="10">
         <v>6</v>
       </c>
+      <c r="AQ20" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -13632,9 +13779,12 @@
       <c r="AP21" s="10">
         <v>456</v>
       </c>
+      <c r="AQ21" s="10">
+        <v>470</v>
+      </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -13758,9 +13908,12 @@
       <c r="AP22" s="10">
         <v>4</v>
       </c>
+      <c r="AQ22" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -13884,9 +14037,12 @@
       <c r="AP23" s="10">
         <v>12</v>
       </c>
+      <c r="AQ23" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -14010,9 +14166,12 @@
       <c r="AP24" s="10">
         <v>13</v>
       </c>
+      <c r="AQ24" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -14138,9 +14297,12 @@
       <c r="AP25" s="10">
         <v>13</v>
       </c>
+      <c r="AQ25" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -14264,9 +14426,12 @@
       <c r="AP26" s="10">
         <v>20</v>
       </c>
+      <c r="AQ26" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -14390,9 +14555,12 @@
       <c r="AP27" s="10">
         <v>33</v>
       </c>
+      <c r="AQ27" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -14516,9 +14684,12 @@
       <c r="AP28" s="10">
         <v>12</v>
       </c>
+      <c r="AQ28" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -14642,8 +14813,11 @@
       <c r="AP29" s="10">
         <v>58</v>
       </c>
+      <c r="AQ29" s="10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -14770,9 +14944,12 @@
       <c r="AP30" s="10">
         <v>256</v>
       </c>
+      <c r="AQ30" s="10">
+        <v>263</v>
+      </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -14898,9 +15075,12 @@
       <c r="AP31" s="10">
         <v>557</v>
       </c>
+      <c r="AQ31" s="10">
+        <v>593</v>
+      </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -15024,9 +15204,12 @@
       <c r="AP32" s="10">
         <v>14</v>
       </c>
+      <c r="AQ32" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -15150,9 +15333,12 @@
       <c r="AP33" s="10">
         <v>54</v>
       </c>
+      <c r="AQ33" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -15278,9 +15464,12 @@
       <c r="AP34" s="10">
         <v>13</v>
       </c>
+      <c r="AQ34" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -15404,9 +15593,12 @@
       <c r="AP35" s="10">
         <v>78</v>
       </c>
+      <c r="AQ35" s="10">
+        <v>78</v>
+      </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -15530,9 +15722,12 @@
       <c r="AP36" s="10">
         <v>132</v>
       </c>
+      <c r="AQ36" s="10">
+        <v>133</v>
+      </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -15656,9 +15851,12 @@
       <c r="AP37" s="10">
         <v>23</v>
       </c>
+      <c r="AQ37" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -15784,9 +15982,12 @@
       <c r="AP38" s="10">
         <v>16</v>
       </c>
+      <c r="AQ38" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -15910,9 +16111,12 @@
       <c r="AP39" s="10">
         <v>39</v>
       </c>
+      <c r="AQ39" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -16036,9 +16240,12 @@
       <c r="AP40" s="10">
         <v>34</v>
       </c>
+      <c r="AQ40" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -16162,9 +16369,12 @@
       <c r="AP41" s="10">
         <v>4</v>
       </c>
+      <c r="AQ41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -16288,9 +16498,12 @@
       <c r="AP42" s="10">
         <v>31</v>
       </c>
+      <c r="AQ42" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -16414,9 +16627,12 @@
       <c r="AP43" s="10">
         <v>23</v>
       </c>
+      <c r="AQ43" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -16540,9 +16756,12 @@
       <c r="AP44" s="10">
         <v>25</v>
       </c>
+      <c r="AQ44" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -16666,9 +16885,12 @@
       <c r="AP45" s="10">
         <v>33</v>
       </c>
+      <c r="AQ45" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -16794,9 +17016,12 @@
       <c r="AP46" s="10">
         <v>16</v>
       </c>
+      <c r="AQ46" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -16920,9 +17145,12 @@
       <c r="AP47" s="10">
         <v>0</v>
       </c>
+      <c r="AQ47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A48" s="34"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -17046,9 +17274,12 @@
       <c r="AP48" s="10">
         <v>4</v>
       </c>
+      <c r="AQ48" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -17172,9 +17403,12 @@
       <c r="AP49" s="10">
         <v>6</v>
       </c>
+      <c r="AQ49" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -17300,9 +17534,12 @@
       <c r="AP50" s="10">
         <v>303</v>
       </c>
+      <c r="AQ50" s="10">
+        <v>353</v>
+      </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -17426,9 +17663,12 @@
       <c r="AP51" s="10">
         <v>82</v>
       </c>
+      <c r="AQ51" s="10">
+        <v>94</v>
+      </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -17554,9 +17794,12 @@
       <c r="AP52" s="10">
         <v>3897</v>
       </c>
+      <c r="AQ52" s="10">
+        <v>4046</v>
+      </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -17680,9 +17923,12 @@
       <c r="AP53" s="10">
         <v>29</v>
       </c>
+      <c r="AQ53" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -17806,8 +18052,11 @@
       <c r="AP54" s="10">
         <v>26</v>
       </c>
+      <c r="AQ54" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -17934,8 +18183,11 @@
       <c r="AP55" s="10">
         <v>119</v>
       </c>
+      <c r="AQ55" s="10">
+        <v>122</v>
+      </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -18062,9 +18314,12 @@
       <c r="AP56" s="10">
         <v>898</v>
       </c>
+      <c r="AQ56" s="10">
+        <v>926</v>
+      </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -18190,9 +18445,12 @@
       <c r="AP57" s="10">
         <v>10</v>
       </c>
+      <c r="AQ57" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -18316,9 +18574,12 @@
       <c r="AP58" s="10">
         <v>7</v>
       </c>
+      <c r="AQ58" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -18442,9 +18703,12 @@
       <c r="AP59" s="10">
         <v>22</v>
       </c>
+      <c r="AQ59" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -18568,9 +18832,12 @@
       <c r="AP60" s="10">
         <v>2</v>
       </c>
+      <c r="AQ60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -18696,9 +18963,12 @@
       <c r="AP61" s="10">
         <v>9</v>
       </c>
+      <c r="AQ61" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A62" s="34"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -18822,9 +19092,12 @@
       <c r="AP62" s="10">
         <v>115</v>
       </c>
+      <c r="AQ62" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -18948,9 +19221,12 @@
       <c r="AP63" s="10">
         <v>104</v>
       </c>
+      <c r="AQ63" s="10">
+        <v>107</v>
+      </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -19074,9 +19350,12 @@
       <c r="AP64" s="10">
         <v>120</v>
       </c>
+      <c r="AQ64" s="10">
+        <v>134</v>
+      </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A65" s="34"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -19200,9 +19479,12 @@
       <c r="AP65" s="10">
         <v>57</v>
       </c>
+      <c r="AQ65" s="10">
+        <v>61</v>
+      </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -19326,8 +19608,11 @@
       <c r="AP66" s="10">
         <v>41</v>
       </c>
+      <c r="AQ66" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -19454,9 +19739,12 @@
       <c r="AP67" s="10">
         <v>832</v>
       </c>
+      <c r="AQ67" s="10">
+        <v>881</v>
+      </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -19582,9 +19870,12 @@
       <c r="AP68" s="10">
         <v>0</v>
       </c>
+      <c r="AQ68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A69" s="34"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -19708,9 +19999,12 @@
       <c r="AP69" s="10">
         <v>12</v>
       </c>
+      <c r="AQ69" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A70" s="34"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -19834,9 +20128,12 @@
       <c r="AP70" s="10">
         <v>2</v>
       </c>
+      <c r="AQ70" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A71" s="34"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -19960,9 +20257,12 @@
       <c r="AP71" s="10">
         <v>13</v>
       </c>
+      <c r="AQ71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A72" s="34"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -20086,9 +20386,12 @@
       <c r="AP72" s="10">
         <v>38</v>
       </c>
+      <c r="AQ72" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A73" s="34"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -20212,9 +20515,12 @@
       <c r="AP73" s="10">
         <v>11</v>
       </c>
+      <c r="AQ73" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A74" s="34"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -20338,9 +20644,12 @@
       <c r="AP74" s="10">
         <v>1</v>
       </c>
+      <c r="AQ74" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A75" s="35"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -20464,9 +20773,12 @@
       <c r="AP75" s="10">
         <v>9</v>
       </c>
+      <c r="AQ75" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -20592,9 +20904,12 @@
       <c r="AP76" s="10">
         <v>3</v>
       </c>
+      <c r="AQ76" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -20718,9 +21033,12 @@
       <c r="AP77" s="10">
         <v>4</v>
       </c>
+      <c r="AQ77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -20844,9 +21162,12 @@
       <c r="AP78" s="10">
         <v>56</v>
       </c>
+      <c r="AQ78" s="10">
+        <v>56</v>
+      </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
+    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -20970,9 +21291,12 @@
       <c r="AP79" s="10">
         <v>9</v>
       </c>
+      <c r="AQ79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A80" s="32"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -21096,8 +21420,11 @@
       <c r="AP80" s="10">
         <v>3</v>
       </c>
+      <c r="AQ80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -21224,9 +21551,12 @@
       <c r="AP81" s="10">
         <v>204</v>
       </c>
+      <c r="AQ81" s="10">
+        <v>211</v>
+      </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -21352,9 +21682,12 @@
       <c r="AP82" s="10">
         <v>160</v>
       </c>
+      <c r="AQ82" s="10">
+        <v>161</v>
+      </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
+    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -21478,9 +21811,12 @@
       <c r="AP83" s="10">
         <v>46</v>
       </c>
+      <c r="AQ83" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
+    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -21604,9 +21940,12 @@
       <c r="AP84" s="10">
         <v>120</v>
       </c>
+      <c r="AQ84" s="10">
+        <v>123</v>
+      </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
+    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -21730,9 +22069,12 @@
       <c r="AP85" s="10">
         <v>6</v>
       </c>
+      <c r="AQ85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
+    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A86" s="32"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -21856,9 +22198,12 @@
       <c r="AP86" s="10">
         <v>20</v>
       </c>
+      <c r="AQ86" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A87" s="30" t="s">
+    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -21984,9 +22329,12 @@
       <c r="AP87" s="10">
         <v>16</v>
       </c>
+      <c r="AQ87" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A88" s="34"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -22110,9 +22458,12 @@
       <c r="AP88" s="10">
         <v>94</v>
       </c>
+      <c r="AQ88" s="10">
+        <v>137</v>
+      </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -22236,9 +22587,12 @@
       <c r="AP89" s="10">
         <v>8</v>
       </c>
+      <c r="AQ89" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A90" s="34"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -22362,9 +22716,12 @@
       <c r="AP90" s="10">
         <v>13</v>
       </c>
+      <c r="AQ90" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -22488,9 +22845,12 @@
       <c r="AP91" s="10">
         <v>4</v>
       </c>
+      <c r="AQ91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A92" s="31"/>
+    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -22614,9 +22974,12 @@
       <c r="AP92" s="10">
         <v>13</v>
       </c>
+      <c r="AQ92" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
+    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -22740,9 +23103,12 @@
       <c r="AP93" s="10">
         <v>51</v>
       </c>
+      <c r="AQ93" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -22868,9 +23234,12 @@
       <c r="AP94" s="10">
         <v>13</v>
       </c>
+      <c r="AQ94" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A95" s="32"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -22994,8 +23363,11 @@
       <c r="AP95" s="10">
         <v>35</v>
       </c>
+      <c r="AQ95" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -23122,9 +23494,12 @@
       <c r="AP96" s="10">
         <v>170</v>
       </c>
+      <c r="AQ96" s="10">
+        <v>173</v>
+      </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A97" s="33" t="s">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -23250,9 +23625,12 @@
       <c r="AP97" s="10">
         <v>1781</v>
       </c>
+      <c r="AQ97" s="10">
+        <v>1900</v>
+      </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
+    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -23376,9 +23754,12 @@
       <c r="AP98" s="10">
         <v>222</v>
       </c>
+      <c r="AQ98" s="10">
+        <v>258</v>
+      </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A99" s="35"/>
+    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A99" s="32"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -23502,9 +23883,12 @@
       <c r="AP99" s="10">
         <v>68</v>
       </c>
+      <c r="AQ99" s="10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -23630,9 +24014,12 @@
       <c r="AP100" s="10">
         <v>32</v>
       </c>
+      <c r="AQ100" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A101" s="34"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -23756,9 +24143,12 @@
       <c r="AP101" s="10">
         <v>34</v>
       </c>
+      <c r="AQ101" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A102" s="34"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -23882,9 +24272,12 @@
       <c r="AP102" s="10">
         <v>155</v>
       </c>
+      <c r="AQ102" s="10">
+        <v>174</v>
+      </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A103" s="34"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -24008,9 +24401,12 @@
       <c r="AP103" s="10">
         <v>251</v>
       </c>
+      <c r="AQ103" s="10">
+        <v>262</v>
+      </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
+    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -24134,9 +24530,12 @@
       <c r="AP104" s="10">
         <v>34</v>
       </c>
+      <c r="AQ104" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
+    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -24262,9 +24661,12 @@
       <c r="AP105" s="10">
         <v>162</v>
       </c>
+      <c r="AQ105" s="10">
+        <v>177</v>
+      </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
+    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -24388,9 +24790,12 @@
       <c r="AP106" s="10">
         <v>128</v>
       </c>
+      <c r="AQ106" s="10">
+        <v>128</v>
+      </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
+    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -24514,9 +24919,12 @@
       <c r="AP107" s="10">
         <v>14</v>
       </c>
+      <c r="AQ107" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="108" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
+    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -24640,9 +25048,12 @@
       <c r="AP108" s="10">
         <v>36</v>
       </c>
+      <c r="AQ108" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -24766,8 +25177,11 @@
       <c r="AP109" s="10">
         <v>5</v>
       </c>
+      <c r="AQ109" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -24894,8 +25308,11 @@
       <c r="AP110" s="10">
         <v>364</v>
       </c>
+      <c r="AQ110" s="10">
+        <v>382</v>
+      </c>
     </row>
-    <row r="111" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -25022,9 +25439,12 @@
       <c r="AP111" s="10">
         <v>80</v>
       </c>
+      <c r="AQ111" s="10">
+        <v>80</v>
+      </c>
     </row>
-    <row r="112" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
+    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A112" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -25150,9 +25570,12 @@
       <c r="AP112" s="10">
         <v>14</v>
       </c>
+      <c r="AQ112" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A113" s="34"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -25276,9 +25699,12 @@
       <c r="AP113" s="10">
         <v>18</v>
       </c>
+      <c r="AQ113" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A114" s="32"/>
+    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A114" s="35"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -25402,9 +25828,12 @@
       <c r="AP114" s="10">
         <v>103</v>
       </c>
+      <c r="AQ114" s="10">
+        <v>104</v>
+      </c>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A115" s="33" t="s">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A115" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -25530,9 +25959,12 @@
       <c r="AP115" s="10">
         <v>103</v>
       </c>
+      <c r="AQ115" s="10">
+        <v>105</v>
+      </c>
     </row>
-    <row r="116" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
+    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -25656,9 +26088,12 @@
       <c r="AP116" s="10">
         <v>74</v>
       </c>
+      <c r="AQ116" s="10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="117" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -25782,9 +26217,12 @@
       <c r="AP117" s="10">
         <v>10</v>
       </c>
+      <c r="AQ117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
+    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -25908,9 +26346,12 @@
       <c r="AP118" s="10">
         <v>45</v>
       </c>
+      <c r="AQ118" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="119" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -26034,9 +26475,12 @@
       <c r="AP119" s="10">
         <v>8</v>
       </c>
+      <c r="AQ119" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="120" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -26160,9 +26604,12 @@
       <c r="AP120" s="10">
         <v>58</v>
       </c>
+      <c r="AQ120" s="10">
+        <v>58</v>
+      </c>
     </row>
-    <row r="121" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="s">
+    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A121" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -26288,9 +26735,12 @@
       <c r="AP121" s="10">
         <v>8</v>
       </c>
+      <c r="AQ121" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="122" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
+    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A122" s="34"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -26414,9 +26864,12 @@
       <c r="AP122" s="10">
         <v>24</v>
       </c>
+      <c r="AQ122" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="123" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A123" s="31"/>
+    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A123" s="34"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -26540,9 +26993,12 @@
       <c r="AP123" s="10">
         <v>2</v>
       </c>
+      <c r="AQ123" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="124" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A124" s="31"/>
+    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A124" s="34"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -26666,9 +27122,12 @@
       <c r="AP124" s="10">
         <v>5</v>
       </c>
+      <c r="AQ124" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="125" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A125" s="31"/>
+    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A125" s="34"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -26792,9 +27251,12 @@
       <c r="AP125" s="10">
         <v>3</v>
       </c>
+      <c r="AQ125" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="126" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A126" s="31"/>
+    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A126" s="34"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -26918,9 +27380,12 @@
       <c r="AP126" s="10">
         <v>4</v>
       </c>
+      <c r="AQ126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A127" s="31"/>
+    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A127" s="34"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -27044,9 +27509,12 @@
       <c r="AP127" s="10">
         <v>7</v>
       </c>
+      <c r="AQ127" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="128" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A128" s="31"/>
+    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A128" s="34"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -27170,9 +27638,12 @@
       <c r="AP128" s="10">
         <v>9</v>
       </c>
+      <c r="AQ128" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="129" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A129" s="31"/>
+    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A129" s="34"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -27296,9 +27767,12 @@
       <c r="AP129" s="10">
         <v>142</v>
       </c>
+      <c r="AQ129" s="10">
+        <v>143</v>
+      </c>
     </row>
-    <row r="130" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A130" s="35"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -27422,8 +27896,11 @@
       <c r="AP130" s="10">
         <v>23</v>
       </c>
+      <c r="AQ130" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="131" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -27550,9 +28027,12 @@
       <c r="AP131" s="10">
         <v>396</v>
       </c>
+      <c r="AQ131" s="10">
+        <v>413</v>
+      </c>
     </row>
-    <row r="132" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="s">
+    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A132" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -27678,9 +28158,12 @@
       <c r="AP132" s="10">
         <v>21</v>
       </c>
+      <c r="AQ132" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="133" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A133" s="31"/>
+    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A133" s="34"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -27804,9 +28287,12 @@
       <c r="AP133" s="10">
         <v>16</v>
       </c>
+      <c r="AQ133" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="134" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A134" s="31"/>
+    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A134" s="34"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -27930,9 +28416,12 @@
       <c r="AP134" s="10">
         <v>2</v>
       </c>
+      <c r="AQ134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A135" s="32"/>
+    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A135" s="35"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -28056,9 +28545,12 @@
       <c r="AP135" s="10">
         <v>2</v>
       </c>
+      <c r="AQ135" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="136" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="s">
+    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A136" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -28184,9 +28676,12 @@
       <c r="AP136" s="10">
         <v>99</v>
       </c>
+      <c r="AQ136" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="137" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
+    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -28310,9 +28805,12 @@
       <c r="AP137" s="10">
         <v>125</v>
       </c>
+      <c r="AQ137" s="10">
+        <v>125</v>
+      </c>
     </row>
-    <row r="138" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A138" s="31"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -28436,9 +28934,12 @@
       <c r="AP138" s="10">
         <v>23</v>
       </c>
+      <c r="AQ138" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="139" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A139" s="35"/>
+    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A139" s="32"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -28561,10 +29062,25 @@
       </c>
       <c r="AP139" s="10">
         <v>175</v>
+      </c>
+      <c r="AQ139" s="10">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A82:A86"/>
@@ -28577,18 +29093,6 @@
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="A132:A135"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -28915,7 +29419,7 @@
       </c>
       <c r="AY2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>54.54545454545454</v>
       </c>
       <c r="AZ2" s="18">
         <f t="shared" si="1"/>
@@ -29565,7 +30069,7 @@
       </c>
       <c r="AY4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.89873417721519</v>
       </c>
       <c r="AZ4" s="10">
         <f t="shared" si="7"/>
@@ -29890,7 +30394,7 @@
       </c>
       <c r="AY6" s="12">
         <f>MAX(0, (dc!AY2-dc!AX2))</f>
-        <v>0</v>
+        <v>869</v>
       </c>
       <c r="AZ6" s="12">
         <f>MAX(0, (dc!AZ2-dc!AY2))</f>
@@ -30214,7 +30718,7 @@
       </c>
       <c r="AY7" s="12">
         <f>MAX(0, (dc!AY3-dc!AX3))</f>
-        <v>0</v>
+        <v>474</v>
       </c>
       <c r="AZ7" s="12">
         <f>MAX(0, (dc!AZ3-dc!AY3))</f>
@@ -30862,7 +31366,7 @@
       </c>
       <c r="AY9" s="12">
         <f>MAX(0, (dc!AY5-dc!AX5))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AZ9" s="12">
         <f>MAX(0, (dc!AZ5-dc!AY5))</f>
@@ -31414,7 +31918,7 @@
       </c>
       <c r="AY11" s="10">
         <f>MAX(0,(dc!AY7-dc!AX7))</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AZ11" s="10">
         <f>MAX(0,(dc!AZ7-dc!AY7))</f>
@@ -31721,7 +32225,7 @@
       </c>
       <c r="AY12" s="10">
         <f>MAX(0,(dc!AY8-dc!AX8))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AZ12" s="10">
         <f>MAX(0,(dc!AZ8-dc!AY8))</f>
@@ -32028,7 +32532,7 @@
       </c>
       <c r="AY13" s="10">
         <f>MAX(0,(dc!AY9-dc!AX9))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AZ13" s="10">
         <f>MAX(0,(dc!AZ9-dc!AY9))</f>
@@ -32335,7 +32839,7 @@
       </c>
       <c r="AY14" s="10">
         <f>MAX(0,(dc!AY10-dc!AX10))</f>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="AZ14" s="10">
         <f>MAX(0,(dc!AZ10-dc!AY10))</f>
@@ -32642,7 +33146,7 @@
       </c>
       <c r="AY15" s="10">
         <f>MAX(0,(dc!AY11-dc!AX11))</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AZ15" s="10">
         <f>MAX(0,(dc!AZ11-dc!AY11))</f>
@@ -32949,7 +33453,7 @@
       </c>
       <c r="AY16" s="10">
         <f>MAX(0,(dc!AY12-dc!AX12))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AZ16" s="10">
         <f>MAX(0,(dc!AZ12-dc!AY12))</f>
@@ -33256,7 +33760,7 @@
       </c>
       <c r="AY17" s="10">
         <f>MAX(0,(dc!AY13-dc!AX13))</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AZ17" s="10">
         <f>MAX(0,(dc!AZ13-dc!AY13))</f>
@@ -33563,7 +34067,7 @@
       </c>
       <c r="AY18" s="10">
         <f>MAX(0,(dc!AY14-dc!AX14))</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AZ18" s="10">
         <f>MAX(0,(dc!AZ14-dc!AY14))</f>
@@ -33870,7 +34374,7 @@
       </c>
       <c r="AY19" s="10">
         <f>MAX(0,(dc!AY15-dc!AX15))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AZ19" s="10">
         <f>MAX(0,(dc!AZ15-dc!AY15))</f>
@@ -34267,7 +34771,7 @@
       </c>
       <c r="AN2" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.053315708305792</v>
       </c>
       <c r="AO2" s="20">
         <f t="shared" ref="AO2:BQ2" si="1">(AO7/MAX(AO6,1))*100</f>
@@ -34540,7 +35044,7 @@
       </c>
       <c r="AN3" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>19.180819180819181</v>
       </c>
       <c r="AO3" s="20">
         <f t="shared" si="3"/>
@@ -34813,7 +35317,7 @@
       </c>
       <c r="AN4" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.7942057942057943</v>
       </c>
       <c r="AO4" s="20">
         <f t="shared" si="5"/>
@@ -35149,7 +35653,7 @@
       </c>
       <c r="AN6" s="14">
         <f>MAX(0,(md!AN2-md!AM2)+(md!AN3-md!AM3))</f>
-        <v>0</v>
+        <v>4539</v>
       </c>
       <c r="AO6" s="14">
         <f>MAX(0,(md!AO2-md!AN2)+(md!AO3-md!AN3))</f>
@@ -35421,7 +35925,7 @@
       </c>
       <c r="AN7" s="14">
         <f>MAX(0,(md!AN3-md!AM3))</f>
-        <v>0</v>
+        <v>1001</v>
       </c>
       <c r="AO7" s="14">
         <f>MAX(0,(md!AO3-md!AN3))</f>
@@ -35693,7 +36197,7 @@
       </c>
       <c r="AN8" s="14">
         <f>MAX(0,(md!AN4-md!AM4))</f>
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="AO8" s="14">
         <f>MAX(0,(md!AO4-md!AN4))</f>
@@ -35965,7 +36469,7 @@
       </c>
       <c r="AN9" s="14">
         <f>MAX(0,(md!AN5-md!AM5))</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="AO9" s="14">
         <f>MAX(0,(md!AO5-md!AN5))</f>
@@ -36451,7 +36955,7 @@
       </c>
       <c r="AN11" s="14">
         <f>MAX(0,(md!AN7-md!AM7))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO11" s="14">
         <f>MAX(0,(md!AO7-md!AN7))</f>
@@ -36728,7 +37232,7 @@
       </c>
       <c r="AN12" s="14">
         <f>MAX(0,(md!AN8-md!AM8))</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AO12" s="14">
         <f>MAX(0,(md!AO8-md!AN8))</f>
@@ -37005,7 +37509,7 @@
       </c>
       <c r="AN13" s="14">
         <f>MAX(0,(md!AN9-md!AM9))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AO13" s="14">
         <f>MAX(0,(md!AO9-md!AN9))</f>
@@ -37282,7 +37786,7 @@
       </c>
       <c r="AN14" s="14">
         <f>MAX(0,(md!AN10-md!AM10))</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="AO14" s="14">
         <f>MAX(0,(md!AO10-md!AN10))</f>
@@ -37836,7 +38340,7 @@
       </c>
       <c r="AN16" s="14">
         <f>MAX(0,(md!AN12-md!AM12))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO16" s="14">
         <f>MAX(0,(md!AO12-md!AN12))</f>
@@ -38113,7 +38617,7 @@
       </c>
       <c r="AN17" s="14">
         <f>MAX(0,(md!AN13-md!AM13))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AO17" s="14">
         <f>MAX(0,(md!AO13-md!AN13))</f>
@@ -38390,7 +38894,7 @@
       </c>
       <c r="AN18" s="14">
         <f>MAX(0,(md!AN14-md!AM14))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AO18" s="14">
         <f>MAX(0,(md!AO14-md!AN14))</f>
@@ -38667,7 +39171,7 @@
       </c>
       <c r="AN19" s="14">
         <f>MAX(0,(md!AN15-md!AM15))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AO19" s="14">
         <f>MAX(0,(md!AO15-md!AN15))</f>
@@ -38944,7 +39448,7 @@
       </c>
       <c r="AN20" s="14">
         <f>MAX(0,(md!AN16-md!AM16))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO20" s="14">
         <f>MAX(0,(md!AO16-md!AN16))</f>
@@ -39221,7 +39725,7 @@
       </c>
       <c r="AN21" s="14">
         <f>MAX(0,(md!AN17-md!AM17))</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AO21" s="14">
         <f>MAX(0,(md!AO17-md!AN17))</f>
@@ -39775,7 +40279,7 @@
       </c>
       <c r="AN23" s="14">
         <f>MAX(0,(md!AN19-md!AM19))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AO23" s="14">
         <f>MAX(0,(md!AO19-md!AN19))</f>
@@ -40052,7 +40556,7 @@
       </c>
       <c r="AN24" s="14">
         <f>MAX(0,(md!AN20-md!AM20))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AO24" s="14">
         <f>MAX(0,(md!AO20-md!AN20))</f>
@@ -40606,7 +41110,7 @@
       </c>
       <c r="AN26" s="14">
         <f>MAX(0,(md!AN22-md!AM22))</f>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="AO26" s="14">
         <f>MAX(0,(md!AO22-md!AN22))</f>
@@ -40883,7 +41387,7 @@
       </c>
       <c r="AN27" s="14">
         <f>MAX(0,(md!AN23-md!AM23))</f>
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="AO27" s="14">
         <f>MAX(0,(md!AO23-md!AN23))</f>
@@ -41160,7 +41664,7 @@
       </c>
       <c r="AN28" s="14">
         <f>MAX(0,(md!AN24-md!AM24))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO28" s="14">
         <f>MAX(0,(md!AO24-md!AN24))</f>
@@ -41437,7 +41941,7 @@
       </c>
       <c r="AN29" s="14">
         <f>MAX(0,(md!AN25-md!AM25))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO29" s="14">
         <f>MAX(0,(md!AO25-md!AN25))</f>
@@ -41714,7 +42218,7 @@
       </c>
       <c r="AN30" s="14">
         <f>MAX(0,(md!AN26-md!AM26))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO30" s="14">
         <f>MAX(0,(md!AO26-md!AN26))</f>
@@ -41991,7 +42495,7 @@
       </c>
       <c r="AN31" s="14">
         <f>MAX(0,(md!AN27-md!AM27))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO31" s="14">
         <f>MAX(0,(md!AO27-md!AN27))</f>
@@ -42268,7 +42772,7 @@
       </c>
       <c r="AN32" s="14">
         <f>MAX(0,(md!AN28-md!AM28))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AO32" s="14">
         <f>MAX(0,(md!AO28-md!AN28))</f>
@@ -42545,7 +43049,7 @@
       </c>
       <c r="AN33" s="14">
         <f>MAX(0,(md!AN29-md!AM29))</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AO33" s="14">
         <f>MAX(0,(md!AO29-md!AN29))</f>
@@ -42822,7 +43326,7 @@
       </c>
       <c r="AN34" s="14">
         <f>MAX(0,(md!AN30-md!AM30))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AO34" s="14">
         <f>MAX(0,(md!AO30-md!AN30))</f>
@@ -43301,7 +43805,7 @@
       </c>
       <c r="AP2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.202293443104969</v>
       </c>
       <c r="AQ2" s="19">
         <f t="shared" si="1"/>
@@ -43578,7 +44082,7 @@
       </c>
       <c r="AP3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12.409638554216867</v>
       </c>
       <c r="AQ3" s="19">
         <f t="shared" si="3"/>
@@ -43855,7 +44359,7 @@
       </c>
       <c r="AP4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.2168674698795181</v>
       </c>
       <c r="AQ4" s="19">
         <f t="shared" si="5"/>
@@ -44132,7 +44636,7 @@
       </c>
       <c r="AP6" s="14">
         <f>MAX(0,(va!AQ5-va!AP5))</f>
-        <v>0</v>
+        <v>6802</v>
       </c>
       <c r="AQ6" s="14">
         <f>MAX(0,(va!AR5-va!AQ5))</f>
@@ -44409,7 +44913,7 @@
       </c>
       <c r="AP7" s="14">
         <f>MAX(0,(va!AQ2-va!AP2))</f>
-        <v>0</v>
+        <v>830</v>
       </c>
       <c r="AQ7" s="14">
         <f>MAX(0,(va!AR2-va!AQ2))</f>
@@ -44686,7 +45190,7 @@
       </c>
       <c r="AP8" s="14">
         <f>MAX(0,(va!AQ3-va!AP3))</f>
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="AQ8" s="14">
         <f>MAX(0,(va!AR3-va!AQ3))</f>
@@ -44963,7 +45467,7 @@
       </c>
       <c r="AP9" s="14">
         <f>MAX(0,(va!AQ4-va!AP4))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AQ9" s="14">
         <f>MAX(0,(va!AR4-va!AQ4))</f>
@@ -45460,7 +45964,7 @@
       </c>
       <c r="AP11" s="16">
         <f>MAX(0,(va!AQ7-va!AP7))</f>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AQ11" s="16">
         <f>MAX(0,(va!AR7-va!AQ7))</f>
@@ -46588,7 +47092,7 @@
       </c>
       <c r="AP15" s="16">
         <f>MAX(0,(va!AQ11-va!AP11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ15" s="16">
         <f>MAX(0,(va!AR11-va!AQ11))</f>
@@ -47434,7 +47938,7 @@
       </c>
       <c r="AP18" s="16">
         <f>MAX(0,(va!AQ14-va!AP14))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AQ18" s="16">
         <f>MAX(0,(va!AR14-va!AQ14))</f>
@@ -47716,7 +48220,7 @@
       </c>
       <c r="AP19" s="16">
         <f>MAX(0,(va!AQ15-va!AP15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ19" s="16">
         <f>MAX(0,(va!AR15-va!AQ15))</f>
@@ -48844,7 +49348,7 @@
       </c>
       <c r="AP23" s="16">
         <f>MAX(0,(va!AQ19-va!AP19))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AQ23" s="16">
         <f>MAX(0,(va!AR19-va!AQ19))</f>
@@ -49408,7 +49912,7 @@
       </c>
       <c r="AP25" s="16">
         <f>MAX(0,(va!AQ21-va!AP21))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AQ25" s="16">
         <f>MAX(0,(va!AR21-va!AQ21))</f>
@@ -49690,7 +50194,7 @@
       </c>
       <c r="AP26" s="16">
         <f>MAX(0,(va!AQ22-va!AP22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ26" s="16">
         <f>MAX(0,(va!AR22-va!AQ22))</f>
@@ -49972,7 +50476,7 @@
       </c>
       <c r="AP27" s="16">
         <f>MAX(0,(va!AQ23-va!AP23))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ27" s="16">
         <f>MAX(0,(va!AR23-va!AQ23))</f>
@@ -50254,7 +50758,7 @@
       </c>
       <c r="AP28" s="16">
         <f>MAX(0,(va!AQ24-va!AP24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ28" s="16">
         <f>MAX(0,(va!AR24-va!AQ24))</f>
@@ -50818,7 +51322,7 @@
       </c>
       <c r="AP30" s="16">
         <f>MAX(0,(va!AQ26-va!AP26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ30" s="16">
         <f>MAX(0,(va!AR26-va!AQ26))</f>
@@ -51100,7 +51604,7 @@
       </c>
       <c r="AP31" s="16">
         <f>MAX(0,(va!AQ27-va!AP27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ31" s="16">
         <f>MAX(0,(va!AR27-va!AQ27))</f>
@@ -51382,7 +51886,7 @@
       </c>
       <c r="AP32" s="16">
         <f>MAX(0,(va!AQ28-va!AP28))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ32" s="16">
         <f>MAX(0,(va!AR28-va!AQ28))</f>
@@ -51664,7 +52168,7 @@
       </c>
       <c r="AP33" s="16">
         <f>MAX(0,(va!AQ29-va!AP29))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ33" s="16">
         <f>MAX(0,(va!AR29-va!AQ29))</f>
@@ -51946,7 +52450,7 @@
       </c>
       <c r="AP34" s="16">
         <f>MAX(0,(va!AQ30-va!AP30))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AQ34" s="16">
         <f>MAX(0,(va!AR30-va!AQ30))</f>
@@ -52228,7 +52732,7 @@
       </c>
       <c r="AP35" s="16">
         <f>MAX(0,(va!AQ31-va!AP31))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AQ35" s="16">
         <f>MAX(0,(va!AR31-va!AQ31))</f>
@@ -52792,7 +53296,7 @@
       </c>
       <c r="AP37" s="16">
         <f>MAX(0,(va!AQ33-va!AP33))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ37" s="16">
         <f>MAX(0,(va!AR33-va!AQ33))</f>
@@ -53638,7 +54142,7 @@
       </c>
       <c r="AP40" s="16">
         <f>MAX(0,(va!AQ36-va!AP36))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ40" s="16">
         <f>MAX(0,(va!AR36-va!AQ36))</f>
@@ -54202,7 +54706,7 @@
       </c>
       <c r="AP42" s="16">
         <f>MAX(0,(va!AQ38-va!AP38))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ42" s="16">
         <f>MAX(0,(va!AR38-va!AQ38))</f>
@@ -54766,7 +55270,7 @@
       </c>
       <c r="AP44" s="16">
         <f>MAX(0,(va!AQ40-va!AP40))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ44" s="16">
         <f>MAX(0,(va!AR40-va!AQ40))</f>
@@ -55894,7 +56398,7 @@
       </c>
       <c r="AP48" s="16">
         <f>MAX(0,(va!AQ44-va!AP44))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ48" s="16">
         <f>MAX(0,(va!AR44-va!AQ44))</f>
@@ -56176,7 +56680,7 @@
       </c>
       <c r="AP49" s="16">
         <f>MAX(0,(va!AQ45-va!AP45))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ49" s="16">
         <f>MAX(0,(va!AR45-va!AQ45))</f>
@@ -57022,7 +57526,7 @@
       </c>
       <c r="AP52" s="16">
         <f>MAX(0,(va!AQ48-va!AP48))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ52" s="16">
         <f>MAX(0,(va!AR48-va!AQ48))</f>
@@ -57586,7 +58090,7 @@
       </c>
       <c r="AP54" s="16">
         <f>MAX(0,(va!AQ50-va!AP50))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AQ54" s="16">
         <f>MAX(0,(va!AR50-va!AQ50))</f>
@@ -57868,7 +58372,7 @@
       </c>
       <c r="AP55" s="16">
         <f>MAX(0,(va!AQ51-va!AP51))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AQ55" s="16">
         <f>MAX(0,(va!AR51-va!AQ51))</f>
@@ -58150,7 +58654,7 @@
       </c>
       <c r="AP56" s="16">
         <f>MAX(0,(va!AQ52-va!AP52))</f>
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="AQ56" s="16">
         <f>MAX(0,(va!AR52-va!AQ52))</f>
@@ -58996,7 +59500,7 @@
       </c>
       <c r="AP59" s="16">
         <f>MAX(0,(va!AQ55-va!AP55))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ59" s="16">
         <f>MAX(0,(va!AR55-va!AQ55))</f>
@@ -59278,7 +59782,7 @@
       </c>
       <c r="AP60" s="16">
         <f>MAX(0,(va!AQ56-va!AP56))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AQ60" s="16">
         <f>MAX(0,(va!AR56-va!AQ56))</f>
@@ -60688,7 +61192,7 @@
       </c>
       <c r="AP65" s="16">
         <f>MAX(0,(va!AQ61-va!AP61))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ65" s="16">
         <f>MAX(0,(va!AR61-va!AQ61))</f>
@@ -61252,7 +61756,7 @@
       </c>
       <c r="AP67" s="16">
         <f>MAX(0,(va!AQ63-va!AP63))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ67" s="16">
         <f>MAX(0,(va!AR63-va!AQ63))</f>
@@ -61534,7 +62038,7 @@
       </c>
       <c r="AP68" s="16">
         <f>MAX(0,(va!AQ64-va!AP64))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AQ68" s="16">
         <f>MAX(0,(va!AR64-va!AQ64))</f>
@@ -61816,7 +62320,7 @@
       </c>
       <c r="AP69" s="16">
         <f>MAX(0,(va!AQ65-va!AP65))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ69" s="16">
         <f>MAX(0,(va!AR65-va!AQ65))</f>
@@ -62098,7 +62602,7 @@
       </c>
       <c r="AP70" s="16">
         <f>MAX(0,(va!AQ66-va!AP66))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AQ70" s="16">
         <f>MAX(0,(va!AR66-va!AQ66))</f>
@@ -62380,7 +62884,7 @@
       </c>
       <c r="AP71" s="16">
         <f>MAX(0,(va!AQ67-va!AP67))</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="AQ71" s="16">
         <f>MAX(0,(va!AR67-va!AQ67))</f>
@@ -62944,7 +63448,7 @@
       </c>
       <c r="AP73" s="16">
         <f>MAX(0,(va!AQ69-va!AP69))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ73" s="16">
         <f>MAX(0,(va!AR69-va!AQ69))</f>
@@ -63790,7 +64294,7 @@
       </c>
       <c r="AP76" s="16">
         <f>MAX(0,(va!AQ72-va!AP72))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ76" s="16">
         <f>MAX(0,(va!AR72-va!AQ72))</f>
@@ -64636,7 +65140,7 @@
       </c>
       <c r="AP79" s="16">
         <f>MAX(0,(va!AQ75-va!AP75))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ79" s="16">
         <f>MAX(0,(va!AR75-va!AQ75))</f>
@@ -66328,7 +66832,7 @@
       </c>
       <c r="AP85" s="16">
         <f>MAX(0,(va!AQ81-va!AP81))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AQ85" s="16">
         <f>MAX(0,(va!AR81-va!AQ81))</f>
@@ -66610,7 +67114,7 @@
       </c>
       <c r="AP86" s="16">
         <f>MAX(0,(va!AQ82-va!AP82))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ86" s="16">
         <f>MAX(0,(va!AR82-va!AQ82))</f>
@@ -67174,7 +67678,7 @@
       </c>
       <c r="AP88" s="16">
         <f>MAX(0,(va!AQ84-va!AP84))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ88" s="16">
         <f>MAX(0,(va!AR84-va!AQ84))</f>
@@ -67738,7 +68242,7 @@
       </c>
       <c r="AP90" s="16">
         <f>MAX(0,(va!AQ86-va!AP86))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ90" s="16">
         <f>MAX(0,(va!AR86-va!AQ86))</f>
@@ -68302,7 +68806,7 @@
       </c>
       <c r="AP92" s="16">
         <f>MAX(0,(va!AQ88-va!AP88))</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AQ92" s="16">
         <f>MAX(0,(va!AR88-va!AQ88))</f>
@@ -68584,7 +69088,7 @@
       </c>
       <c r="AP93" s="16">
         <f>MAX(0,(va!AQ89-va!AP89))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ93" s="16">
         <f>MAX(0,(va!AR89-va!AQ89))</f>
@@ -69712,7 +70216,7 @@
       </c>
       <c r="AP97" s="16">
         <f>MAX(0,(va!AQ93-va!AP93))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ97" s="16">
         <f>MAX(0,(va!AR93-va!AQ93))</f>
@@ -69994,7 +70498,7 @@
       </c>
       <c r="AP98" s="16">
         <f>MAX(0,(va!AQ94-va!AP94))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ98" s="16">
         <f>MAX(0,(va!AR94-va!AQ94))</f>
@@ -70276,7 +70780,7 @@
       </c>
       <c r="AP99" s="16">
         <f>MAX(0,(va!AQ95-va!AP95))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ99" s="16">
         <f>MAX(0,(va!AR95-va!AQ95))</f>
@@ -70558,7 +71062,7 @@
       </c>
       <c r="AP100" s="16">
         <f>MAX(0,(va!AQ96-va!AP96))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ100" s="16">
         <f>MAX(0,(va!AR96-va!AQ96))</f>
@@ -70840,7 +71344,7 @@
       </c>
       <c r="AP101" s="16">
         <f>MAX(0,(va!AQ97-va!AP97))</f>
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="AQ101" s="16">
         <f>MAX(0,(va!AR97-va!AQ97))</f>
@@ -71122,7 +71626,7 @@
       </c>
       <c r="AP102" s="16">
         <f>MAX(0,(va!AQ98-va!AP98))</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AQ102" s="16">
         <f>MAX(0,(va!AR98-va!AQ98))</f>
@@ -71404,7 +71908,7 @@
       </c>
       <c r="AP103" s="16">
         <f>MAX(0,(va!AQ99-va!AP99))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AQ103" s="16">
         <f>MAX(0,(va!AR99-va!AQ99))</f>
@@ -72250,7 +72754,7 @@
       </c>
       <c r="AP106" s="16">
         <f>MAX(0,(va!AQ102-va!AP102))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AQ106" s="16">
         <f>MAX(0,(va!AR102-va!AQ102))</f>
@@ -72532,7 +73036,7 @@
       </c>
       <c r="AP107" s="16">
         <f>MAX(0,(va!AQ103-va!AP103))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AQ107" s="16">
         <f>MAX(0,(va!AR103-va!AQ103))</f>
@@ -72814,7 +73318,7 @@
       </c>
       <c r="AP108" s="16">
         <f>MAX(0,(va!AQ104-va!AP104))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ108" s="16">
         <f>MAX(0,(va!AR104-va!AQ104))</f>
@@ -73096,7 +73600,7 @@
       </c>
       <c r="AP109" s="16">
         <f>MAX(0,(va!AQ105-va!AP105))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AQ109" s="16">
         <f>MAX(0,(va!AR105-va!AQ105))</f>
@@ -73660,7 +74164,7 @@
       </c>
       <c r="AP111" s="16">
         <f>MAX(0,(va!AQ107-va!AP107))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ111" s="16">
         <f>MAX(0,(va!AR107-va!AQ107))</f>
@@ -73942,7 +74446,7 @@
       </c>
       <c r="AP112" s="16">
         <f>MAX(0,(va!AQ108-va!AP108))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ112" s="16">
         <f>MAX(0,(va!AR108-va!AQ108))</f>
@@ -74224,7 +74728,7 @@
       </c>
       <c r="AP113" s="16">
         <f>MAX(0,(va!AQ109-va!AP109))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ113" s="16">
         <f>MAX(0,(va!AR109-va!AQ109))</f>
@@ -74506,7 +75010,7 @@
       </c>
       <c r="AP114" s="16">
         <f>MAX(0,(va!AQ110-va!AP110))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AQ114" s="16">
         <f>MAX(0,(va!AR110-va!AQ110))</f>
@@ -75070,7 +75574,7 @@
       </c>
       <c r="AP116" s="16">
         <f>MAX(0,(va!AQ112-va!AP112))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ116" s="16">
         <f>MAX(0,(va!AR112-va!AQ112))</f>
@@ -75352,7 +75856,7 @@
       </c>
       <c r="AP117" s="16">
         <f>MAX(0,(va!AQ113-va!AP113))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ117" s="16">
         <f>MAX(0,(va!AR113-va!AQ113))</f>
@@ -75634,7 +76138,7 @@
       </c>
       <c r="AP118" s="16">
         <f>MAX(0,(va!AQ114-va!AP114))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ118" s="16">
         <f>MAX(0,(va!AR114-va!AQ114))</f>
@@ -75916,7 +76420,7 @@
       </c>
       <c r="AP119" s="16">
         <f>MAX(0,(va!AQ115-va!AP115))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ119" s="16">
         <f>MAX(0,(va!AR115-va!AQ115))</f>
@@ -76198,7 +76702,7 @@
       </c>
       <c r="AP120" s="16">
         <f>MAX(0,(va!AQ116-va!AP116))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ120" s="16">
         <f>MAX(0,(va!AR116-va!AQ116))</f>
@@ -76762,7 +77266,7 @@
       </c>
       <c r="AP122" s="16">
         <f>MAX(0,(va!AQ118-va!AP118))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ122" s="16">
         <f>MAX(0,(va!AR118-va!AQ118))</f>
@@ -78172,7 +78676,7 @@
       </c>
       <c r="AP127" s="16">
         <f>MAX(0,(va!AQ123-va!AP123))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ127" s="16">
         <f>MAX(0,(va!AR123-va!AQ123))</f>
@@ -78454,7 +78958,7 @@
       </c>
       <c r="AP128" s="16">
         <f>MAX(0,(va!AQ124-va!AP124))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ128" s="16">
         <f>MAX(0,(va!AR124-va!AQ124))</f>
@@ -79864,7 +80368,7 @@
       </c>
       <c r="AP133" s="16">
         <f>MAX(0,(va!AQ129-va!AP129))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ133" s="16">
         <f>MAX(0,(va!AR129-va!AQ129))</f>
@@ -80146,7 +80650,7 @@
       </c>
       <c r="AP134" s="16">
         <f>MAX(0,(va!AQ130-va!AP130))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ134" s="16">
         <f>MAX(0,(va!AR130-va!AQ130))</f>
@@ -80428,7 +80932,7 @@
       </c>
       <c r="AP135" s="16">
         <f>MAX(0,(va!AQ131-va!AP131))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AQ135" s="16">
         <f>MAX(0,(va!AR131-va!AQ131))</f>
@@ -80710,7 +81214,7 @@
       </c>
       <c r="AP136" s="16">
         <f>MAX(0,(va!AQ132-va!AP132))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ136" s="16">
         <f>MAX(0,(va!AR132-va!AQ132))</f>
@@ -80992,7 +81496,7 @@
       </c>
       <c r="AP137" s="16">
         <f>MAX(0,(va!AQ133-va!AP133))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ137" s="16">
         <f>MAX(0,(va!AR133-va!AQ133))</f>
@@ -82684,7 +83188,7 @@
       </c>
       <c r="AP143" s="16">
         <f>MAX(0,(va!AQ139-va!AP139))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ143" s="16">
         <f>MAX(0,(va!AR139-va!AQ139))</f>

</xml_diff>

<commit_message>
03 May data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157912FB-C96E-4D22-A80F-C85CC05F43CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F57A93A-5F08-4EF3-B8EB-527C7128867D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4015,10 +4015,10 @@
   <dimension ref="A1:CC46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="AR6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AY2" sqref="AY2"/>
+      <selection pane="bottomRight" activeCell="AZ2" sqref="AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4188,6 +4188,9 @@
       <c r="AY2" s="12">
         <v>22004</v>
       </c>
+      <c r="AZ2" s="12">
+        <v>23102</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4380,7 +4383,7 @@
       </c>
       <c r="AZ3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5016</v>
       </c>
       <c r="BA3" s="10">
         <f t="shared" si="0"/>
@@ -4658,6 +4661,9 @@
       <c r="AY5" s="10">
         <v>240</v>
       </c>
+      <c r="AZ5" s="10">
+        <v>251</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5058,6 +5064,9 @@
       <c r="AY7" s="10">
         <v>621</v>
       </c>
+      <c r="AZ7" s="10">
+        <v>649</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5212,6 +5221,9 @@
       </c>
       <c r="AY8" s="10">
         <v>318</v>
+      </c>
+      <c r="AZ8" s="10">
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
@@ -5368,6 +5380,9 @@
       <c r="AY9" s="10">
         <v>302</v>
       </c>
+      <c r="AZ9" s="10">
+        <v>311</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5523,6 +5538,9 @@
       <c r="AY10" s="10">
         <v>889</v>
       </c>
+      <c r="AZ10" s="10">
+        <v>931</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5678,6 +5696,9 @@
       <c r="AY11" s="10">
         <v>722</v>
       </c>
+      <c r="AZ11" s="10">
+        <v>768</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5833,6 +5854,9 @@
       <c r="AY12" s="10">
         <v>476</v>
       </c>
+      <c r="AZ12" s="10">
+        <v>489</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -5988,6 +6012,9 @@
       <c r="AY13" s="10">
         <v>711</v>
       </c>
+      <c r="AZ13" s="10">
+        <v>751</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6143,6 +6170,9 @@
       <c r="AY14" s="10">
         <v>692</v>
       </c>
+      <c r="AZ14" s="10">
+        <v>713</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6297,6 +6327,9 @@
       </c>
       <c r="AY15" s="10">
         <v>66</v>
+      </c>
+      <c r="AZ15" s="10">
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6551,7 +6584,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AN2" sqref="AN2"/>
+      <selection pane="bottomRight" activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6689,7 +6722,7 @@
         <v>101049</v>
       </c>
       <c r="AO2" s="10">
-        <v>0</v>
+        <v>107332</v>
       </c>
       <c r="AP2" s="10">
         <v>0</v>
@@ -6933,7 +6966,7 @@
       </c>
       <c r="AO3" s="10">
         <f>SUM(md[3-May])</f>
-        <v>0</v>
+        <v>25462</v>
       </c>
       <c r="AP3" s="10">
         <f>SUM(md[4-May])</f>
@@ -7167,7 +7200,7 @@
         <v>4910</v>
       </c>
       <c r="AO4" s="10">
-        <v>0</v>
+        <v>5051</v>
       </c>
       <c r="AP4" s="10">
         <v>0</v>
@@ -7373,7 +7406,7 @@
         <v>1156</v>
       </c>
       <c r="AO5" s="10">
-        <v>0</v>
+        <v>1182</v>
       </c>
       <c r="AP5" s="10">
         <v>0</v>
@@ -7790,6 +7823,9 @@
       <c r="AN7">
         <v>121</v>
       </c>
+      <c r="AO7">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7912,6 +7948,9 @@
       <c r="AN8" s="10">
         <v>1885</v>
       </c>
+      <c r="AO8" s="10">
+        <v>1959</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -8034,6 +8073,9 @@
       <c r="AN9">
         <v>2237</v>
       </c>
+      <c r="AO9">
+        <v>2319</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -8156,6 +8198,9 @@
       <c r="AN10">
         <v>3183</v>
       </c>
+      <c r="AO10">
+        <v>3301</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8278,6 +8323,9 @@
       <c r="AN11">
         <v>160</v>
       </c>
+      <c r="AO11">
+        <v>162</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8400,6 +8448,9 @@
       <c r="AN12">
         <v>79</v>
       </c>
+      <c r="AO12">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8522,6 +8573,9 @@
       <c r="AN13">
         <v>480</v>
       </c>
+      <c r="AO13">
+        <v>494</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8644,6 +8698,9 @@
       <c r="AN14">
         <v>187</v>
       </c>
+      <c r="AO14">
+        <v>188</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8766,6 +8823,9 @@
       <c r="AN15">
         <v>622</v>
       </c>
+      <c r="AO15">
+        <v>637</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8888,8 +8948,11 @@
       <c r="AN16" s="10">
         <v>59</v>
       </c>
+      <c r="AO16" s="10">
+        <v>71</v>
+      </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -9010,8 +9073,11 @@
       <c r="AN17">
         <v>976</v>
       </c>
+      <c r="AO17">
+        <v>1004</v>
+      </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -9132,8 +9198,11 @@
       <c r="AN18">
         <v>4</v>
       </c>
+      <c r="AO18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -9254,8 +9323,11 @@
       <c r="AN19">
         <v>468</v>
       </c>
+      <c r="AO19">
+        <v>479</v>
+      </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9376,8 +9448,11 @@
       <c r="AN20">
         <v>931</v>
       </c>
+      <c r="AO20">
+        <v>969</v>
+      </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9498,8 +9573,11 @@
       <c r="AN21">
         <v>80</v>
       </c>
+      <c r="AO21">
+        <v>91</v>
+      </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9620,8 +9698,11 @@
       <c r="AN22">
         <v>4919</v>
       </c>
+      <c r="AO22">
+        <v>5150</v>
+      </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9742,8 +9823,11 @@
       <c r="AN23">
         <v>7041</v>
       </c>
+      <c r="AO23">
+        <v>7333</v>
+      </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9864,8 +9948,11 @@
       <c r="AN24">
         <v>57</v>
       </c>
+      <c r="AO24">
+        <v>60</v>
+      </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -9986,8 +10073,11 @@
       <c r="AN25">
         <v>164</v>
       </c>
+      <c r="AO25">
+        <v>165</v>
+      </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -10108,8 +10198,11 @@
       <c r="AN26">
         <v>32</v>
       </c>
+      <c r="AO26">
+        <v>33</v>
+      </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -10230,8 +10323,11 @@
       <c r="AN27">
         <v>39</v>
       </c>
+      <c r="AO27">
+        <v>44</v>
+      </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -10352,8 +10448,11 @@
       <c r="AN28">
         <v>225</v>
       </c>
+      <c r="AO28">
+        <v>232</v>
+      </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -10474,8 +10573,11 @@
       <c r="AN29">
         <v>452</v>
       </c>
+      <c r="AO29">
+        <v>473</v>
+      </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10596,8 +10698,11 @@
       <c r="AN30">
         <v>72</v>
       </c>
+      <c r="AO30">
+        <v>75</v>
+      </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10694,7 +10799,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="AD6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
+      <selection pane="bottomRight" activeCell="AR3" sqref="AR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10880,7 +10985,7 @@
       </c>
       <c r="AR2" s="10">
         <f>SUM(va[3-May])</f>
-        <v>0</v>
+        <v>18671</v>
       </c>
       <c r="AS2" s="10">
         <f>SUM(va[4-May])</f>
@@ -11117,7 +11222,7 @@
         <v>2519</v>
       </c>
       <c r="AR3" s="10">
-        <v>0</v>
+        <v>2627</v>
       </c>
       <c r="AS3" s="10">
         <v>0</v>
@@ -11326,7 +11431,7 @@
         <v>616</v>
       </c>
       <c r="AR4" s="10">
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="AS4" s="10">
         <v>0</v>
@@ -11535,7 +11640,7 @@
         <v>112450</v>
       </c>
       <c r="AR5" s="10">
-        <v>0</v>
+        <v>119065</v>
       </c>
       <c r="AS5" s="10">
         <v>0</v>
@@ -11970,9 +12075,12 @@
       <c r="AQ7" s="10">
         <v>848</v>
       </c>
+      <c r="AR7" s="10">
+        <v>899</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -12101,9 +12209,12 @@
       <c r="AQ8" s="10">
         <v>6</v>
       </c>
+      <c r="AR8" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -12230,9 +12341,12 @@
       <c r="AQ9" s="10">
         <v>28</v>
       </c>
+      <c r="AR9" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -12359,9 +12473,12 @@
       <c r="AQ10" s="10">
         <v>3</v>
       </c>
+      <c r="AR10" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -12488,9 +12605,12 @@
       <c r="AQ11" s="10">
         <v>54</v>
       </c>
+      <c r="AR11" s="10">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -12617,9 +12737,12 @@
       <c r="AQ12" s="10">
         <v>0</v>
       </c>
+      <c r="AR12" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -12744,6 +12867,9 @@
         <v>26</v>
       </c>
       <c r="AQ13" s="10">
+        <v>26</v>
+      </c>
+      <c r="AR13" s="10">
         <v>26</v>
       </c>
     </row>
@@ -12877,9 +13003,12 @@
       <c r="AQ14" s="10">
         <v>1044</v>
       </c>
+      <c r="AR14" s="10">
+        <v>1106</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -13008,9 +13137,12 @@
       <c r="AQ15" s="10">
         <v>45</v>
       </c>
+      <c r="AR15" s="10">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -13137,9 +13269,12 @@
       <c r="AQ16" s="10">
         <v>0</v>
       </c>
+      <c r="AR16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -13266,9 +13401,12 @@
       <c r="AQ17" s="10">
         <v>2</v>
       </c>
+      <c r="AR17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -13395,9 +13533,12 @@
       <c r="AQ18" s="10">
         <v>7</v>
       </c>
+      <c r="AR18" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -13524,9 +13665,12 @@
       <c r="AQ19" s="10">
         <v>259</v>
       </c>
+      <c r="AR19" s="10">
+        <v>265</v>
+      </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -13653,9 +13797,12 @@
       <c r="AQ20" s="10">
         <v>6</v>
       </c>
+      <c r="AR20" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -13782,9 +13929,12 @@
       <c r="AQ21" s="10">
         <v>470</v>
       </c>
+      <c r="AR21" s="10">
+        <v>478</v>
+      </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -13911,9 +14061,12 @@
       <c r="AQ22" s="10">
         <v>5</v>
       </c>
+      <c r="AR22" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -14040,9 +14193,12 @@
       <c r="AQ23" s="10">
         <v>13</v>
       </c>
+      <c r="AR23" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -14169,9 +14325,12 @@
       <c r="AQ24" s="10">
         <v>14</v>
       </c>
+      <c r="AR24" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -14300,9 +14459,12 @@
       <c r="AQ25" s="10">
         <v>12</v>
       </c>
+      <c r="AR25" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -14429,9 +14591,12 @@
       <c r="AQ26" s="10">
         <v>21</v>
       </c>
+      <c r="AR26" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -14558,9 +14723,12 @@
       <c r="AQ27" s="10">
         <v>34</v>
       </c>
+      <c r="AR27" s="10">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -14687,9 +14855,12 @@
       <c r="AQ28" s="10">
         <v>13</v>
       </c>
+      <c r="AR28" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -14816,8 +14987,11 @@
       <c r="AQ29" s="10">
         <v>62</v>
       </c>
+      <c r="AR29" s="10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -14947,9 +15121,12 @@
       <c r="AQ30" s="10">
         <v>263</v>
       </c>
+      <c r="AR30" s="10">
+        <v>279</v>
+      </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -15078,9 +15255,12 @@
       <c r="AQ31" s="10">
         <v>593</v>
       </c>
+      <c r="AR31" s="10">
+        <v>601</v>
+      </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -15207,9 +15387,12 @@
       <c r="AQ32" s="10">
         <v>14</v>
       </c>
+      <c r="AR32" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
@@ -15336,9 +15519,12 @@
       <c r="AQ33" s="10">
         <v>57</v>
       </c>
+      <c r="AR33" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -15467,9 +15653,12 @@
       <c r="AQ34" s="10">
         <v>13</v>
       </c>
+      <c r="AR34" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
@@ -15596,9 +15785,12 @@
       <c r="AQ35" s="10">
         <v>78</v>
       </c>
+      <c r="AR35" s="10">
+        <v>79</v>
+      </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -15725,9 +15917,12 @@
       <c r="AQ36" s="10">
         <v>133</v>
       </c>
+      <c r="AR36" s="10">
+        <v>137</v>
+      </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
@@ -15854,9 +16049,12 @@
       <c r="AQ37" s="10">
         <v>23</v>
       </c>
+      <c r="AR37" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -15985,9 +16183,12 @@
       <c r="AQ38" s="10">
         <v>18</v>
       </c>
+      <c r="AR38" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -16114,9 +16315,12 @@
       <c r="AQ39" s="10">
         <v>39</v>
       </c>
+      <c r="AR39" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
@@ -16243,9 +16447,12 @@
       <c r="AQ40" s="10">
         <v>35</v>
       </c>
+      <c r="AR40" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
@@ -16372,9 +16579,12 @@
       <c r="AQ41" s="10">
         <v>4</v>
       </c>
+      <c r="AR41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
@@ -16501,9 +16711,12 @@
       <c r="AQ42" s="10">
         <v>31</v>
       </c>
+      <c r="AR42" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
@@ -16630,9 +16843,12 @@
       <c r="AQ43" s="10">
         <v>23</v>
       </c>
+      <c r="AR43" s="10">
+        <v>24</v>
+      </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
@@ -16759,9 +16975,12 @@
       <c r="AQ44" s="10">
         <v>27</v>
       </c>
+      <c r="AR44" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
       </c>
@@ -16888,9 +17107,12 @@
       <c r="AQ45" s="10">
         <v>35</v>
       </c>
+      <c r="AR45" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -17019,9 +17241,12 @@
       <c r="AQ46" s="10">
         <v>16</v>
       </c>
+      <c r="AR46" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -17148,9 +17373,12 @@
       <c r="AQ47" s="10">
         <v>0</v>
       </c>
+      <c r="AR47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
@@ -17277,9 +17505,12 @@
       <c r="AQ48" s="10">
         <v>5</v>
       </c>
+      <c r="AR48" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
@@ -17406,9 +17637,12 @@
       <c r="AQ49" s="10">
         <v>6</v>
       </c>
+      <c r="AR49" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -17537,9 +17771,12 @@
       <c r="AQ50" s="10">
         <v>353</v>
       </c>
+      <c r="AR50" s="10">
+        <v>400</v>
+      </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
@@ -17666,9 +17903,12 @@
       <c r="AQ51" s="10">
         <v>94</v>
       </c>
+      <c r="AR51" s="10">
+        <v>134</v>
+      </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -17797,9 +18037,12 @@
       <c r="AQ52" s="10">
         <v>4046</v>
       </c>
+      <c r="AR52" s="10">
+        <v>4340</v>
+      </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
@@ -17926,9 +18169,12 @@
       <c r="AQ53" s="10">
         <v>29</v>
       </c>
+      <c r="AR53" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A54" s="32"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
@@ -18055,8 +18301,11 @@
       <c r="AQ54" s="10">
         <v>26</v>
       </c>
+      <c r="AR54" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -18186,8 +18435,11 @@
       <c r="AQ55" s="10">
         <v>122</v>
       </c>
+      <c r="AR55" s="10">
+        <v>123</v>
+      </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -18317,9 +18569,12 @@
       <c r="AQ56" s="10">
         <v>926</v>
       </c>
+      <c r="AR56" s="10">
+        <v>954</v>
+      </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -18448,9 +18703,12 @@
       <c r="AQ57" s="10">
         <v>10</v>
       </c>
+      <c r="AR57" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
@@ -18577,9 +18835,12 @@
       <c r="AQ58" s="10">
         <v>7</v>
       </c>
+      <c r="AR58" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
+    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
@@ -18706,9 +18967,12 @@
       <c r="AQ59" s="10">
         <v>22</v>
       </c>
+      <c r="AR59" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -18835,9 +19099,12 @@
       <c r="AQ60" s="10">
         <v>2</v>
       </c>
+      <c r="AR60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -18966,9 +19233,12 @@
       <c r="AQ61" s="10">
         <v>10</v>
       </c>
+      <c r="AR61" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
@@ -19095,9 +19365,12 @@
       <c r="AQ62" s="10">
         <v>115</v>
       </c>
+      <c r="AR62" s="10">
+        <v>121</v>
+      </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
+    <row r="63" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
@@ -19224,9 +19497,12 @@
       <c r="AQ63" s="10">
         <v>107</v>
       </c>
+      <c r="AR63" s="10">
+        <v>109</v>
+      </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
@@ -19353,9 +19629,12 @@
       <c r="AQ64" s="10">
         <v>134</v>
       </c>
+      <c r="AR64" s="10">
+        <v>145</v>
+      </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
@@ -19482,9 +19761,12 @@
       <c r="AQ65" s="10">
         <v>61</v>
       </c>
+      <c r="AR65" s="10">
+        <v>61</v>
+      </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A66" s="32"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
@@ -19611,8 +19893,11 @@
       <c r="AQ66" s="10">
         <v>46</v>
       </c>
+      <c r="AR66" s="10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -19742,9 +20027,12 @@
       <c r="AQ67" s="10">
         <v>881</v>
       </c>
+      <c r="AR67" s="10">
+        <v>931</v>
+      </c>
     </row>
-    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -19873,9 +20161,12 @@
       <c r="AQ68" s="10">
         <v>0</v>
       </c>
+      <c r="AR68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -20002,9 +20293,12 @@
       <c r="AQ69" s="10">
         <v>13</v>
       </c>
+      <c r="AR69" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -20131,9 +20425,12 @@
       <c r="AQ70" s="10">
         <v>2</v>
       </c>
+      <c r="AR70" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A71" s="31"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
@@ -20260,9 +20557,12 @@
       <c r="AQ71" s="10">
         <v>13</v>
       </c>
+      <c r="AR71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A72" s="31"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
       </c>
@@ -20389,9 +20689,12 @@
       <c r="AQ72" s="10">
         <v>39</v>
       </c>
+      <c r="AR72" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A73" s="31"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
@@ -20518,9 +20821,12 @@
       <c r="AQ73" s="10">
         <v>11</v>
       </c>
+      <c r="AR73" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
+    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A74" s="31"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
       </c>
@@ -20647,9 +20953,12 @@
       <c r="AQ74" s="10">
         <v>1</v>
       </c>
+      <c r="AR74" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A75" s="32"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -20776,9 +21085,12 @@
       <c r="AQ75" s="10">
         <v>10</v>
       </c>
+      <c r="AR75" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A76" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -20907,9 +21219,12 @@
       <c r="AQ76" s="10">
         <v>3</v>
       </c>
+      <c r="AR76" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A77" s="34"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
@@ -21036,9 +21351,12 @@
       <c r="AQ77" s="10">
         <v>4</v>
       </c>
+      <c r="AR77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
+    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A78" s="34"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
       </c>
@@ -21165,9 +21483,12 @@
       <c r="AQ78" s="10">
         <v>56</v>
       </c>
+      <c r="AR78" s="10">
+        <v>56</v>
+      </c>
     </row>
-    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
+    <row r="79" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A79" s="34"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
@@ -21294,9 +21615,12 @@
       <c r="AQ79" s="10">
         <v>9</v>
       </c>
+      <c r="AR79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+    <row r="80" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
       </c>
@@ -21423,8 +21747,11 @@
       <c r="AQ80" s="10">
         <v>3</v>
       </c>
+      <c r="AR80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -21554,9 +21881,12 @@
       <c r="AQ81" s="10">
         <v>211</v>
       </c>
+      <c r="AR81" s="10">
+        <v>221</v>
+      </c>
     </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A82" s="30" t="s">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -21685,9 +22015,12 @@
       <c r="AQ82" s="10">
         <v>161</v>
       </c>
+      <c r="AR82" s="10">
+        <v>163</v>
+      </c>
     </row>
-    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
+    <row r="83" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A83" s="34"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
@@ -21814,9 +22147,12 @@
       <c r="AQ83" s="10">
         <v>46</v>
       </c>
+      <c r="AR83" s="10">
+        <v>47</v>
+      </c>
     </row>
-    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+    <row r="84" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A84" s="34"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
       </c>
@@ -21943,9 +22279,12 @@
       <c r="AQ84" s="10">
         <v>123</v>
       </c>
+      <c r="AR84" s="10">
+        <v>125</v>
+      </c>
     </row>
-    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+    <row r="85" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A85" s="34"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
       </c>
@@ -22072,9 +22411,12 @@
       <c r="AQ85" s="10">
         <v>6</v>
       </c>
+      <c r="AR85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
+    <row r="86" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A86" s="35"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
       </c>
@@ -22201,9 +22543,12 @@
       <c r="AQ86" s="10">
         <v>21</v>
       </c>
+      <c r="AR86" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A87" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -22332,9 +22677,12 @@
       <c r="AQ87" s="10">
         <v>16</v>
       </c>
+      <c r="AR87" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+    <row r="88" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
       </c>
@@ -22461,9 +22809,12 @@
       <c r="AQ88" s="10">
         <v>137</v>
       </c>
+      <c r="AR88" s="10">
+        <v>137</v>
+      </c>
     </row>
-    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
+    <row r="89" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
@@ -22590,9 +22941,12 @@
       <c r="AQ89" s="10">
         <v>9</v>
       </c>
+      <c r="AR89" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
+    <row r="90" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
@@ -22719,9 +23073,12 @@
       <c r="AQ90" s="10">
         <v>12</v>
       </c>
+      <c r="AR90" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
+    <row r="91" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
@@ -22848,9 +23205,12 @@
       <c r="AQ91" s="10">
         <v>4</v>
       </c>
+      <c r="AR91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
+    <row r="92" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
       </c>
@@ -22977,9 +23337,12 @@
       <c r="AQ92" s="10">
         <v>13</v>
       </c>
+      <c r="AR92" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+    <row r="93" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A93" s="32"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
       </c>
@@ -23106,9 +23469,12 @@
       <c r="AQ93" s="10">
         <v>55</v>
       </c>
+      <c r="AR93" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
+    <row r="94" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -23237,9 +23603,12 @@
       <c r="AQ94" s="10">
         <v>14</v>
       </c>
+      <c r="AR94" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
+    <row r="95" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A95" s="35"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
       </c>
@@ -23366,8 +23735,11 @@
       <c r="AQ95" s="10">
         <v>37</v>
       </c>
+      <c r="AR95" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -23497,9 +23869,12 @@
       <c r="AQ96" s="10">
         <v>173</v>
       </c>
+      <c r="AR96" s="10">
+        <v>183</v>
+      </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+    <row r="97" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A97" s="33" t="s">
         <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -23628,9 +24003,12 @@
       <c r="AQ97" s="10">
         <v>1900</v>
       </c>
+      <c r="AR97" s="10">
+        <v>2026</v>
+      </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+    <row r="98" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A98" s="34"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
       </c>
@@ -23757,9 +24135,12 @@
       <c r="AQ98" s="10">
         <v>258</v>
       </c>
+      <c r="AR98" s="10">
+        <v>266</v>
+      </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
+    <row r="99" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A99" s="35"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
       </c>
@@ -23886,9 +24267,12 @@
       <c r="AQ99" s="10">
         <v>76</v>
       </c>
+      <c r="AR99" s="10">
+        <v>82</v>
+      </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+    <row r="100" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A100" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -24017,9 +24401,12 @@
       <c r="AQ100" s="10">
         <v>29</v>
       </c>
+      <c r="AR100" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
+    <row r="101" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
@@ -24146,9 +24533,12 @@
       <c r="AQ101" s="10">
         <v>33</v>
       </c>
+      <c r="AR101" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
+    <row r="102" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
       </c>
@@ -24275,9 +24665,12 @@
       <c r="AQ102" s="10">
         <v>174</v>
       </c>
+      <c r="AR102" s="10">
+        <v>186</v>
+      </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
+    <row r="103" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
@@ -24404,9 +24797,12 @@
       <c r="AQ103" s="10">
         <v>262</v>
       </c>
+      <c r="AR103" s="10">
+        <v>271</v>
+      </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
+    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A104" s="32"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
       </c>
@@ -24533,9 +24929,12 @@
       <c r="AQ104" s="10">
         <v>37</v>
       </c>
+      <c r="AR104" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+    <row r="105" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A105" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -24664,9 +25063,12 @@
       <c r="AQ105" s="10">
         <v>177</v>
       </c>
+      <c r="AR105" s="10">
+        <v>191</v>
+      </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+    <row r="106" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A106" s="34"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
       </c>
@@ -24793,9 +25195,12 @@
       <c r="AQ106" s="10">
         <v>128</v>
       </c>
+      <c r="AR106" s="10">
+        <v>133</v>
+      </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+    <row r="107" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A107" s="34"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
@@ -24922,9 +25327,12 @@
       <c r="AQ107" s="10">
         <v>15</v>
       </c>
+      <c r="AR107" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+    <row r="108" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A108" s="34"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
       </c>
@@ -25051,9 +25459,12 @@
       <c r="AQ108" s="10">
         <v>37</v>
       </c>
+      <c r="AR108" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A109" s="32"/>
+    <row r="109" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A109" s="35"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
@@ -25180,8 +25591,11 @@
       <c r="AQ109" s="10">
         <v>6</v>
       </c>
+      <c r="AR109" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -25311,8 +25725,11 @@
       <c r="AQ110" s="10">
         <v>382</v>
       </c>
+      <c r="AR110" s="10">
+        <v>403</v>
+      </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -25442,9 +25859,12 @@
       <c r="AQ111" s="10">
         <v>80</v>
       </c>
+      <c r="AR111" s="10">
+        <v>81</v>
+      </c>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+    <row r="112" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A112" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -25573,9 +25993,12 @@
       <c r="AQ112" s="10">
         <v>15</v>
       </c>
+      <c r="AR112" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+    <row r="113" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
@@ -25702,9 +26125,12 @@
       <c r="AQ113" s="10">
         <v>19</v>
       </c>
+      <c r="AR113" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+    <row r="114" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A114" s="32"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -25831,9 +26257,12 @@
       <c r="AQ114" s="10">
         <v>104</v>
       </c>
+      <c r="AR114" s="10">
+        <v>106</v>
+      </c>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A115" s="30" t="s">
+    <row r="115" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A115" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -25962,9 +26391,12 @@
       <c r="AQ115" s="10">
         <v>105</v>
       </c>
+      <c r="AR115" s="10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A116" s="31"/>
+    <row r="116" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A116" s="34"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
       </c>
@@ -26091,9 +26523,12 @@
       <c r="AQ116" s="10">
         <v>76</v>
       </c>
+      <c r="AR116" s="10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
+    <row r="117" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A117" s="34"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -26220,9 +26655,12 @@
       <c r="AQ117" s="10">
         <v>10</v>
       </c>
+      <c r="AR117" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
+    <row r="118" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A118" s="34"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
       </c>
@@ -26349,9 +26787,12 @@
       <c r="AQ118" s="10">
         <v>46</v>
       </c>
+      <c r="AR118" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
+    <row r="119" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A119" s="34"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
@@ -26478,9 +26919,12 @@
       <c r="AQ119" s="10">
         <v>8</v>
       </c>
+      <c r="AR119" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+    <row r="120" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A120" s="35"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
       </c>
@@ -26607,9 +27051,12 @@
       <c r="AQ120" s="10">
         <v>58</v>
       </c>
+      <c r="AR120" s="10">
+        <v>63</v>
+      </c>
     </row>
-    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A121" s="33" t="s">
+    <row r="121" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A121" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -26738,9 +27185,12 @@
       <c r="AQ121" s="10">
         <v>8</v>
       </c>
+      <c r="AR121" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
+    <row r="122" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
@@ -26867,9 +27317,12 @@
       <c r="AQ122" s="10">
         <v>24</v>
       </c>
+      <c r="AR122" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+    <row r="123" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
@@ -26996,9 +27449,12 @@
       <c r="AQ123" s="10">
         <v>3</v>
       </c>
+      <c r="AR123" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+    <row r="124" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
       </c>
@@ -27125,9 +27581,12 @@
       <c r="AQ124" s="10">
         <v>9</v>
       </c>
+      <c r="AR124" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
+    <row r="125" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
       </c>
@@ -27254,9 +27713,12 @@
       <c r="AQ125" s="10">
         <v>3</v>
       </c>
+      <c r="AR125" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+    <row r="126" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
       </c>
@@ -27383,9 +27845,12 @@
       <c r="AQ126" s="10">
         <v>4</v>
       </c>
+      <c r="AR126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+    <row r="127" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
       </c>
@@ -27512,9 +27977,12 @@
       <c r="AQ127" s="10">
         <v>7</v>
       </c>
+      <c r="AR127" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
+    <row r="128" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
       </c>
@@ -27641,9 +28109,12 @@
       <c r="AQ128" s="10">
         <v>9</v>
       </c>
+      <c r="AR128" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+    <row r="129" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A129" s="31"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
       </c>
@@ -27770,9 +28241,12 @@
       <c r="AQ129" s="10">
         <v>143</v>
       </c>
+      <c r="AR129" s="10">
+        <v>145</v>
+      </c>
     </row>
-    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+    <row r="130" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A130" s="32"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
       </c>
@@ -27899,8 +28373,11 @@
       <c r="AQ130" s="10">
         <v>25</v>
       </c>
+      <c r="AR130" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -28030,9 +28507,12 @@
       <c r="AQ131" s="10">
         <v>413</v>
       </c>
+      <c r="AR131" s="10">
+        <v>413</v>
+      </c>
     </row>
-    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A132" s="33" t="s">
+    <row r="132" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A132" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -28161,9 +28641,12 @@
       <c r="AQ132" s="10">
         <v>22</v>
       </c>
+      <c r="AR132" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+    <row r="133" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A133" s="31"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
       </c>
@@ -28290,9 +28773,12 @@
       <c r="AQ133" s="10">
         <v>19</v>
       </c>
+      <c r="AR133" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+    <row r="134" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A134" s="31"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
       </c>
@@ -28419,9 +28905,12 @@
       <c r="AQ134" s="10">
         <v>2</v>
       </c>
+      <c r="AR134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A135" s="35"/>
+    <row r="135" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A135" s="32"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
       </c>
@@ -28548,9 +29037,12 @@
       <c r="AQ135" s="10">
         <v>2</v>
       </c>
+      <c r="AR135" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+    <row r="136" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A136" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -28679,9 +29171,12 @@
       <c r="AQ136" s="10">
         <v>99</v>
       </c>
+      <c r="AR136" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
+    <row r="137" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A137" s="34"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
       </c>
@@ -28808,9 +29303,12 @@
       <c r="AQ137" s="10">
         <v>125</v>
       </c>
+      <c r="AR137" s="10">
+        <v>127</v>
+      </c>
     </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
+    <row r="138" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A138" s="34"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
       </c>
@@ -28937,9 +29435,12 @@
       <c r="AQ138" s="10">
         <v>23</v>
       </c>
+      <c r="AR138" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A139" s="32"/>
+    <row r="139" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A139" s="35"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
       </c>
@@ -29065,10 +29566,25 @@
       </c>
       <c r="AQ139" s="10">
         <v>178</v>
+      </c>
+      <c r="AR139" s="10">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A130"/>
+    <mergeCell ref="A132:A135"/>
     <mergeCell ref="A68:A75"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A15:A24"/>
@@ -29081,18 +29597,6 @@
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A130"/>
-    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="BC1:BR1">
     <cfRule type="colorScale" priority="6">
@@ -29423,7 +29927,7 @@
       </c>
       <c r="AZ2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19.94535519125683</v>
       </c>
       <c r="BA2" s="18">
         <f t="shared" si="1"/>
@@ -30073,7 +30577,7 @@
       </c>
       <c r="AZ4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.0228310502283104</v>
       </c>
       <c r="BA4" s="10">
         <f t="shared" si="7"/>
@@ -30398,7 +30902,7 @@
       </c>
       <c r="AZ6" s="12">
         <f>MAX(0, (dc!AZ2-dc!AY2))</f>
-        <v>0</v>
+        <v>1098</v>
       </c>
       <c r="BA6" s="12">
         <f>MAX(0, (dc!BA2-dc!AZ2))</f>
@@ -30722,7 +31226,7 @@
       </c>
       <c r="AZ7" s="12">
         <f>MAX(0, (dc!AZ3-dc!AY3))</f>
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="BA7" s="12">
         <f>MAX(0, (dc!BA3-dc!AZ3))</f>
@@ -31370,7 +31874,7 @@
       </c>
       <c r="AZ9" s="12">
         <f>MAX(0, (dc!AZ5-dc!AY5))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="BA9" s="12">
         <f>MAX(0, (dc!BA5-dc!AZ5))</f>
@@ -31922,7 +32426,7 @@
       </c>
       <c r="AZ11" s="10">
         <f>MAX(0,(dc!AZ7-dc!AY7))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="BA11" s="10">
         <f>MAX(0,(dc!BA7-dc!AZ7))</f>
@@ -32229,7 +32733,7 @@
       </c>
       <c r="AZ12" s="10">
         <f>MAX(0,(dc!AZ8-dc!AY8))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BA12" s="10">
         <f>MAX(0,(dc!BA8-dc!AZ8))</f>
@@ -32536,7 +33040,7 @@
       </c>
       <c r="AZ13" s="10">
         <f>MAX(0,(dc!AZ9-dc!AY9))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="BA13" s="10">
         <f>MAX(0,(dc!BA9-dc!AZ9))</f>
@@ -32843,7 +33347,7 @@
       </c>
       <c r="AZ14" s="10">
         <f>MAX(0,(dc!AZ10-dc!AY10))</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="BA14" s="10">
         <f>MAX(0,(dc!BA10-dc!AZ10))</f>
@@ -33150,7 +33654,7 @@
       </c>
       <c r="AZ15" s="10">
         <f>MAX(0,(dc!AZ11-dc!AY11))</f>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="BA15" s="10">
         <f>MAX(0,(dc!BA11-dc!AZ11))</f>
@@ -33457,7 +33961,7 @@
       </c>
       <c r="AZ16" s="10">
         <f>MAX(0,(dc!AZ12-dc!AY12))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="BA16" s="10">
         <f>MAX(0,(dc!BA12-dc!AZ12))</f>
@@ -33764,7 +34268,7 @@
       </c>
       <c r="AZ17" s="10">
         <f>MAX(0,(dc!AZ13-dc!AY13))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="BA17" s="10">
         <f>MAX(0,(dc!BA13-dc!AZ13))</f>
@@ -34071,7 +34575,7 @@
       </c>
       <c r="AZ18" s="10">
         <f>MAX(0,(dc!AZ14-dc!AY14))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="BA18" s="10">
         <f>MAX(0,(dc!BA14-dc!AZ14))</f>
@@ -34378,7 +34882,7 @@
       </c>
       <c r="AZ19" s="10">
         <f>MAX(0,(dc!AZ15-dc!AY15))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="BA19" s="10">
         <f>MAX(0,(dc!BA15-dc!AZ15))</f>
@@ -34775,7 +35279,7 @@
       </c>
       <c r="AO2" s="20">
         <f t="shared" ref="AO2:BQ2" si="1">(AO7/MAX(AO6,1))*100</f>
-        <v>0</v>
+        <v>13.600110011001101</v>
       </c>
       <c r="AP2" s="20">
         <f t="shared" si="1"/>
@@ -35048,7 +35552,7 @@
       </c>
       <c r="AO3" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14.256825075834175</v>
       </c>
       <c r="AP3" s="20">
         <f t="shared" si="3"/>
@@ -35321,7 +35825,7 @@
       </c>
       <c r="AO4" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.6289180990899901</v>
       </c>
       <c r="AP4" s="20">
         <f t="shared" si="5"/>
@@ -35657,7 +36161,7 @@
       </c>
       <c r="AO6" s="14">
         <f>MAX(0,(md!AO2-md!AN2)+(md!AO3-md!AN3))</f>
-        <v>0</v>
+        <v>7272</v>
       </c>
       <c r="AP6" s="14">
         <f>MAX(0,(md!AP2-md!AO2)+(md!AP3-md!AO3))</f>
@@ -35929,7 +36433,7 @@
       </c>
       <c r="AO7" s="14">
         <f>MAX(0,(md!AO3-md!AN3))</f>
-        <v>0</v>
+        <v>989</v>
       </c>
       <c r="AP7" s="14">
         <f>MAX(0,(md!AP3-md!AO3))</f>
@@ -36201,7 +36705,7 @@
       </c>
       <c r="AO8" s="14">
         <f>MAX(0,(md!AO4-md!AN4))</f>
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="AP8" s="14">
         <f>MAX(0,(md!AP4-md!AO4))</f>
@@ -36473,7 +36977,7 @@
       </c>
       <c r="AO9" s="14">
         <f>MAX(0,(md!AO5-md!AN5))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AP9" s="14">
         <f>MAX(0,(md!AP5-md!AO5))</f>
@@ -36959,7 +37463,7 @@
       </c>
       <c r="AO11" s="14">
         <f>MAX(0,(md!AO7-md!AN7))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP11" s="14">
         <f>MAX(0,(md!AP7-md!AO7))</f>
@@ -37236,7 +37740,7 @@
       </c>
       <c r="AO12" s="14">
         <f>MAX(0,(md!AO8-md!AN8))</f>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="AP12" s="14">
         <f>MAX(0,(md!AP8-md!AO8))</f>
@@ -37513,7 +38017,7 @@
       </c>
       <c r="AO13" s="14">
         <f>MAX(0,(md!AO9-md!AN9))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="AP13" s="14">
         <f>MAX(0,(md!AP9-md!AO9))</f>
@@ -37790,7 +38294,7 @@
       </c>
       <c r="AO14" s="14">
         <f>MAX(0,(md!AO10-md!AN10))</f>
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="AP14" s="14">
         <f>MAX(0,(md!AP10-md!AO10))</f>
@@ -38067,7 +38571,7 @@
       </c>
       <c r="AO15" s="14">
         <f>MAX(0,(md!AO11-md!AN11))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP15" s="14">
         <f>MAX(0,(md!AP11-md!AO11))</f>
@@ -38344,7 +38848,7 @@
       </c>
       <c r="AO16" s="14">
         <f>MAX(0,(md!AO12-md!AN12))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AP16" s="14">
         <f>MAX(0,(md!AP12-md!AO12))</f>
@@ -38621,7 +39125,7 @@
       </c>
       <c r="AO17" s="14">
         <f>MAX(0,(md!AO13-md!AN13))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AP17" s="14">
         <f>MAX(0,(md!AP13-md!AO13))</f>
@@ -38898,7 +39402,7 @@
       </c>
       <c r="AO18" s="14">
         <f>MAX(0,(md!AO14-md!AN14))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP18" s="14">
         <f>MAX(0,(md!AP14-md!AO14))</f>
@@ -39175,7 +39679,7 @@
       </c>
       <c r="AO19" s="14">
         <f>MAX(0,(md!AO15-md!AN15))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AP19" s="14">
         <f>MAX(0,(md!AP15-md!AO15))</f>
@@ -39452,7 +39956,7 @@
       </c>
       <c r="AO20" s="14">
         <f>MAX(0,(md!AO16-md!AN16))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AP20" s="14">
         <f>MAX(0,(md!AP16-md!AO16))</f>
@@ -39729,7 +40233,7 @@
       </c>
       <c r="AO21" s="14">
         <f>MAX(0,(md!AO17-md!AN17))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AP21" s="14">
         <f>MAX(0,(md!AP17-md!AO17))</f>
@@ -40283,7 +40787,7 @@
       </c>
       <c r="AO23" s="14">
         <f>MAX(0,(md!AO19-md!AN19))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AP23" s="14">
         <f>MAX(0,(md!AP19-md!AO19))</f>
@@ -40560,7 +41064,7 @@
       </c>
       <c r="AO24" s="14">
         <f>MAX(0,(md!AO20-md!AN20))</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AP24" s="14">
         <f>MAX(0,(md!AP20-md!AO20))</f>
@@ -40837,7 +41341,7 @@
       </c>
       <c r="AO25" s="14">
         <f>MAX(0,(md!AO21-md!AN21))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AP25" s="14">
         <f>MAX(0,(md!AP21-md!AO21))</f>
@@ -41114,7 +41618,7 @@
       </c>
       <c r="AO26" s="14">
         <f>MAX(0,(md!AO22-md!AN22))</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="AP26" s="14">
         <f>MAX(0,(md!AP22-md!AO22))</f>
@@ -41391,7 +41895,7 @@
       </c>
       <c r="AO27" s="14">
         <f>MAX(0,(md!AO23-md!AN23))</f>
-        <v>0</v>
+        <v>292</v>
       </c>
       <c r="AP27" s="14">
         <f>MAX(0,(md!AP23-md!AO23))</f>
@@ -41668,7 +42172,7 @@
       </c>
       <c r="AO28" s="14">
         <f>MAX(0,(md!AO24-md!AN24))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP28" s="14">
         <f>MAX(0,(md!AP24-md!AO24))</f>
@@ -41945,7 +42449,7 @@
       </c>
       <c r="AO29" s="14">
         <f>MAX(0,(md!AO25-md!AN25))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP29" s="14">
         <f>MAX(0,(md!AP25-md!AO25))</f>
@@ -42222,7 +42726,7 @@
       </c>
       <c r="AO30" s="14">
         <f>MAX(0,(md!AO26-md!AN26))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP30" s="14">
         <f>MAX(0,(md!AP26-md!AO26))</f>
@@ -42499,7 +43003,7 @@
       </c>
       <c r="AO31" s="14">
         <f>MAX(0,(md!AO27-md!AN27))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP31" s="14">
         <f>MAX(0,(md!AP27-md!AO27))</f>
@@ -42776,7 +43280,7 @@
       </c>
       <c r="AO32" s="14">
         <f>MAX(0,(md!AO28-md!AN28))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AP32" s="14">
         <f>MAX(0,(md!AP28-md!AO28))</f>
@@ -43053,7 +43557,7 @@
       </c>
       <c r="AO33" s="14">
         <f>MAX(0,(md!AO29-md!AN29))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AP33" s="14">
         <f>MAX(0,(md!AP29-md!AO29))</f>
@@ -43330,7 +43834,7 @@
       </c>
       <c r="AO34" s="14">
         <f>MAX(0,(md!AO30-md!AN30))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP34" s="14">
         <f>MAX(0,(md!AP30-md!AO30))</f>
@@ -43809,7 +44313,7 @@
       </c>
       <c r="AQ2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14.210128495842781</v>
       </c>
       <c r="AR2" s="19">
         <f t="shared" si="1"/>
@@ -44086,7 +44590,7 @@
       </c>
       <c r="AQ3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11.48936170212766</v>
       </c>
       <c r="AR3" s="19">
         <f t="shared" si="3"/>
@@ -44363,7 +44867,7 @@
       </c>
       <c r="AQ4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.6808510638297873</v>
       </c>
       <c r="AR4" s="19">
         <f t="shared" si="5"/>
@@ -44640,7 +45144,7 @@
       </c>
       <c r="AQ6" s="14">
         <f>MAX(0,(va!AR5-va!AQ5))</f>
-        <v>0</v>
+        <v>6615</v>
       </c>
       <c r="AR6" s="14">
         <f>MAX(0,(va!AS5-va!AR5))</f>
@@ -44917,7 +45421,7 @@
       </c>
       <c r="AQ7" s="14">
         <f>MAX(0,(va!AR2-va!AQ2))</f>
-        <v>0</v>
+        <v>940</v>
       </c>
       <c r="AR7" s="14">
         <f>MAX(0,(va!AS2-va!AR2))</f>
@@ -45194,7 +45698,7 @@
       </c>
       <c r="AQ8" s="14">
         <f>MAX(0,(va!AR3-va!AQ3))</f>
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="AR8" s="14">
         <f>MAX(0,(va!AS3-va!AR3))</f>
@@ -45471,7 +45975,7 @@
       </c>
       <c r="AQ9" s="14">
         <f>MAX(0,(va!AR4-va!AQ4))</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="AR9" s="14">
         <f>MAX(0,(va!AS4-va!AR4))</f>
@@ -45968,7 +46472,7 @@
       </c>
       <c r="AQ11" s="16">
         <f>MAX(0,(va!AR7-va!AQ7))</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="AR11" s="16">
         <f>MAX(0,(va!AS7-va!AR7))</f>
@@ -47096,7 +47600,7 @@
       </c>
       <c r="AQ15" s="16">
         <f>MAX(0,(va!AR11-va!AQ11))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR15" s="16">
         <f>MAX(0,(va!AS11-va!AR11))</f>
@@ -47942,7 +48446,7 @@
       </c>
       <c r="AQ18" s="16">
         <f>MAX(0,(va!AR14-va!AQ14))</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="AR18" s="16">
         <f>MAX(0,(va!AS14-va!AR14))</f>
@@ -48224,7 +48728,7 @@
       </c>
       <c r="AQ19" s="16">
         <f>MAX(0,(va!AR15-va!AQ15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR19" s="16">
         <f>MAX(0,(va!AS15-va!AR15))</f>
@@ -49352,7 +49856,7 @@
       </c>
       <c r="AQ23" s="16">
         <f>MAX(0,(va!AR19-va!AQ19))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR23" s="16">
         <f>MAX(0,(va!AS19-va!AR19))</f>
@@ -49916,7 +50420,7 @@
       </c>
       <c r="AQ25" s="16">
         <f>MAX(0,(va!AR21-va!AQ21))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AR25" s="16">
         <f>MAX(0,(va!AS21-va!AR21))</f>
@@ -50198,7 +50702,7 @@
       </c>
       <c r="AQ26" s="16">
         <f>MAX(0,(va!AR22-va!AQ22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR26" s="16">
         <f>MAX(0,(va!AS22-va!AR22))</f>
@@ -51044,7 +51548,7 @@
       </c>
       <c r="AQ29" s="16">
         <f>MAX(0,(va!AR25-va!AQ25))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR29" s="16">
         <f>MAX(0,(va!AS25-va!AR25))</f>
@@ -52172,7 +52676,7 @@
       </c>
       <c r="AQ33" s="16">
         <f>MAX(0,(va!AR29-va!AQ29))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR33" s="16">
         <f>MAX(0,(va!AS29-va!AR29))</f>
@@ -52454,7 +52958,7 @@
       </c>
       <c r="AQ34" s="16">
         <f>MAX(0,(va!AR30-va!AQ30))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AR34" s="16">
         <f>MAX(0,(va!AS30-va!AR30))</f>
@@ -52736,7 +53240,7 @@
       </c>
       <c r="AQ35" s="16">
         <f>MAX(0,(va!AR31-va!AQ31))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AR35" s="16">
         <f>MAX(0,(va!AS31-va!AR31))</f>
@@ -53018,7 +53522,7 @@
       </c>
       <c r="AQ36" s="16">
         <f>MAX(0,(va!AR32-va!AQ32))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR36" s="16">
         <f>MAX(0,(va!AS32-va!AR32))</f>
@@ -53582,7 +54086,7 @@
       </c>
       <c r="AQ38" s="16">
         <f>MAX(0,(va!AR34-va!AQ34))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AR38" s="16">
         <f>MAX(0,(va!AS34-va!AR34))</f>
@@ -53864,7 +54368,7 @@
       </c>
       <c r="AQ39" s="16">
         <f>MAX(0,(va!AR35-va!AQ35))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR39" s="16">
         <f>MAX(0,(va!AS35-va!AR35))</f>
@@ -54146,7 +54650,7 @@
       </c>
       <c r="AQ40" s="16">
         <f>MAX(0,(va!AR36-va!AQ36))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AR40" s="16">
         <f>MAX(0,(va!AS36-va!AR36))</f>
@@ -54428,7 +54932,7 @@
       </c>
       <c r="AQ41" s="16">
         <f>MAX(0,(va!AR37-va!AQ37))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR41" s="16">
         <f>MAX(0,(va!AS37-va!AR37))</f>
@@ -56120,7 +56624,7 @@
       </c>
       <c r="AQ47" s="16">
         <f>MAX(0,(va!AR43-va!AQ43))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR47" s="16">
         <f>MAX(0,(va!AS43-va!AR43))</f>
@@ -58094,7 +58598,7 @@
       </c>
       <c r="AQ54" s="16">
         <f>MAX(0,(va!AR50-va!AQ50))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AR54" s="16">
         <f>MAX(0,(va!AS50-va!AR50))</f>
@@ -58376,7 +58880,7 @@
       </c>
       <c r="AQ55" s="16">
         <f>MAX(0,(va!AR51-va!AQ51))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AR55" s="16">
         <f>MAX(0,(va!AS51-va!AR51))</f>
@@ -58658,7 +59162,7 @@
       </c>
       <c r="AQ56" s="16">
         <f>MAX(0,(va!AR52-va!AQ52))</f>
-        <v>0</v>
+        <v>294</v>
       </c>
       <c r="AR56" s="16">
         <f>MAX(0,(va!AS52-va!AR52))</f>
@@ -58940,7 +59444,7 @@
       </c>
       <c r="AQ57" s="16">
         <f>MAX(0,(va!AR53-va!AQ53))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR57" s="16">
         <f>MAX(0,(va!AS53-va!AR53))</f>
@@ -59222,7 +59726,7 @@
       </c>
       <c r="AQ58" s="16">
         <f>MAX(0,(va!AR54-va!AQ54))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AR58" s="16">
         <f>MAX(0,(va!AS54-va!AR54))</f>
@@ -59504,7 +60008,7 @@
       </c>
       <c r="AQ59" s="16">
         <f>MAX(0,(va!AR55-va!AQ55))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR59" s="16">
         <f>MAX(0,(va!AS55-va!AR55))</f>
@@ -59786,7 +60290,7 @@
       </c>
       <c r="AQ60" s="16">
         <f>MAX(0,(va!AR56-va!AQ56))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AR60" s="16">
         <f>MAX(0,(va!AS56-va!AR56))</f>
@@ -61478,7 +61982,7 @@
       </c>
       <c r="AQ66" s="16">
         <f>MAX(0,(va!AR62-va!AQ62))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR66" s="16">
         <f>MAX(0,(va!AS62-va!AR62))</f>
@@ -61760,7 +62264,7 @@
       </c>
       <c r="AQ67" s="16">
         <f>MAX(0,(va!AR63-va!AQ63))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR67" s="16">
         <f>MAX(0,(va!AS63-va!AR63))</f>
@@ -62042,7 +62546,7 @@
       </c>
       <c r="AQ68" s="16">
         <f>MAX(0,(va!AR64-va!AQ64))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AR68" s="16">
         <f>MAX(0,(va!AS64-va!AR64))</f>
@@ -62606,7 +63110,7 @@
       </c>
       <c r="AQ70" s="16">
         <f>MAX(0,(va!AR66-va!AQ66))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR70" s="16">
         <f>MAX(0,(va!AS66-va!AR66))</f>
@@ -62888,7 +63392,7 @@
       </c>
       <c r="AQ71" s="16">
         <f>MAX(0,(va!AR67-va!AQ67))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AR71" s="16">
         <f>MAX(0,(va!AS67-va!AR67))</f>
@@ -63452,7 +63956,7 @@
       </c>
       <c r="AQ73" s="16">
         <f>MAX(0,(va!AR69-va!AQ69))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR73" s="16">
         <f>MAX(0,(va!AS69-va!AR69))</f>
@@ -64580,7 +65084,7 @@
       </c>
       <c r="AQ77" s="16">
         <f>MAX(0,(va!AR73-va!AQ73))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR77" s="16">
         <f>MAX(0,(va!AS73-va!AR73))</f>
@@ -64862,7 +65366,7 @@
       </c>
       <c r="AQ78" s="16">
         <f>MAX(0,(va!AR74-va!AQ74))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR78" s="16">
         <f>MAX(0,(va!AS74-va!AR74))</f>
@@ -65144,7 +65648,7 @@
       </c>
       <c r="AQ79" s="16">
         <f>MAX(0,(va!AR75-va!AQ75))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR79" s="16">
         <f>MAX(0,(va!AS75-va!AR75))</f>
@@ -66836,7 +67340,7 @@
       </c>
       <c r="AQ85" s="16">
         <f>MAX(0,(va!AR81-va!AQ81))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AR85" s="16">
         <f>MAX(0,(va!AS81-va!AR81))</f>
@@ -67118,7 +67622,7 @@
       </c>
       <c r="AQ86" s="16">
         <f>MAX(0,(va!AR82-va!AQ82))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR86" s="16">
         <f>MAX(0,(va!AS82-va!AR82))</f>
@@ -67400,7 +67904,7 @@
       </c>
       <c r="AQ87" s="16">
         <f>MAX(0,(va!AR83-va!AQ83))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR87" s="16">
         <f>MAX(0,(va!AS83-va!AR83))</f>
@@ -67682,7 +68186,7 @@
       </c>
       <c r="AQ88" s="16">
         <f>MAX(0,(va!AR84-va!AQ84))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR88" s="16">
         <f>MAX(0,(va!AS84-va!AR84))</f>
@@ -68246,7 +68750,7 @@
       </c>
       <c r="AQ90" s="16">
         <f>MAX(0,(va!AR86-va!AQ86))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR90" s="16">
         <f>MAX(0,(va!AS86-va!AR86))</f>
@@ -71066,7 +71570,7 @@
       </c>
       <c r="AQ100" s="16">
         <f>MAX(0,(va!AR96-va!AQ96))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AR100" s="16">
         <f>MAX(0,(va!AS96-va!AR96))</f>
@@ -71348,7 +71852,7 @@
       </c>
       <c r="AQ101" s="16">
         <f>MAX(0,(va!AR97-va!AQ97))</f>
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="AR101" s="16">
         <f>MAX(0,(va!AS97-va!AR97))</f>
@@ -71630,7 +72134,7 @@
       </c>
       <c r="AQ102" s="16">
         <f>MAX(0,(va!AR98-va!AQ98))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AR102" s="16">
         <f>MAX(0,(va!AS98-va!AR98))</f>
@@ -71912,7 +72416,7 @@
       </c>
       <c r="AQ103" s="16">
         <f>MAX(0,(va!AR99-va!AQ99))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR103" s="16">
         <f>MAX(0,(va!AS99-va!AR99))</f>
@@ -72194,7 +72698,7 @@
       </c>
       <c r="AQ104" s="16">
         <f>MAX(0,(va!AR100-va!AQ100))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR104" s="16">
         <f>MAX(0,(va!AS100-va!AR100))</f>
@@ -72476,7 +72980,7 @@
       </c>
       <c r="AQ105" s="16">
         <f>MAX(0,(va!AR101-va!AQ101))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR105" s="16">
         <f>MAX(0,(va!AS101-va!AR101))</f>
@@ -72758,7 +73262,7 @@
       </c>
       <c r="AQ106" s="16">
         <f>MAX(0,(va!AR102-va!AQ102))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AR106" s="16">
         <f>MAX(0,(va!AS102-va!AR102))</f>
@@ -73040,7 +73544,7 @@
       </c>
       <c r="AQ107" s="16">
         <f>MAX(0,(va!AR103-va!AQ103))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AR107" s="16">
         <f>MAX(0,(va!AS103-va!AR103))</f>
@@ -73322,7 +73826,7 @@
       </c>
       <c r="AQ108" s="16">
         <f>MAX(0,(va!AR104-va!AQ104))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR108" s="16">
         <f>MAX(0,(va!AS104-va!AR104))</f>
@@ -73604,7 +74108,7 @@
       </c>
       <c r="AQ109" s="16">
         <f>MAX(0,(va!AR105-va!AQ105))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AR109" s="16">
         <f>MAX(0,(va!AS105-va!AR105))</f>
@@ -73886,7 +74390,7 @@
       </c>
       <c r="AQ110" s="16">
         <f>MAX(0,(va!AR106-va!AQ106))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR110" s="16">
         <f>MAX(0,(va!AS106-va!AR106))</f>
@@ -75014,7 +75518,7 @@
       </c>
       <c r="AQ114" s="16">
         <f>MAX(0,(va!AR110-va!AQ110))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AR114" s="16">
         <f>MAX(0,(va!AS110-va!AR110))</f>
@@ -75296,7 +75800,7 @@
       </c>
       <c r="AQ115" s="16">
         <f>MAX(0,(va!AR111-va!AQ111))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR115" s="16">
         <f>MAX(0,(va!AS111-va!AR111))</f>
@@ -76142,7 +76646,7 @@
       </c>
       <c r="AQ118" s="16">
         <f>MAX(0,(va!AR114-va!AQ114))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR118" s="16">
         <f>MAX(0,(va!AS114-va!AR114))</f>
@@ -76424,7 +76928,7 @@
       </c>
       <c r="AQ119" s="16">
         <f>MAX(0,(va!AR115-va!AQ115))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR119" s="16">
         <f>MAX(0,(va!AS115-va!AR115))</f>
@@ -77834,7 +78338,7 @@
       </c>
       <c r="AQ124" s="16">
         <f>MAX(0,(va!AR120-va!AQ120))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR124" s="16">
         <f>MAX(0,(va!AS120-va!AR120))</f>
@@ -78116,7 +78620,7 @@
       </c>
       <c r="AQ125" s="16">
         <f>MAX(0,(va!AR121-va!AQ121))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR125" s="16">
         <f>MAX(0,(va!AS121-va!AR121))</f>
@@ -78398,7 +78902,7 @@
       </c>
       <c r="AQ126" s="16">
         <f>MAX(0,(va!AR122-va!AQ122))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR126" s="16">
         <f>MAX(0,(va!AS122-va!AR122))</f>
@@ -79244,7 +79748,7 @@
       </c>
       <c r="AQ129" s="16">
         <f>MAX(0,(va!AR125-va!AQ125))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR129" s="16">
         <f>MAX(0,(va!AS125-va!AR125))</f>
@@ -80372,7 +80876,7 @@
       </c>
       <c r="AQ133" s="16">
         <f>MAX(0,(va!AR129-va!AQ129))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR133" s="16">
         <f>MAX(0,(va!AS129-va!AR129))</f>
@@ -80654,7 +81158,7 @@
       </c>
       <c r="AQ134" s="16">
         <f>MAX(0,(va!AR130-va!AQ130))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR134" s="16">
         <f>MAX(0,(va!AS130-va!AR130))</f>
@@ -81218,7 +81722,7 @@
       </c>
       <c r="AQ136" s="16">
         <f>MAX(0,(va!AR132-va!AQ132))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR136" s="16">
         <f>MAX(0,(va!AS132-va!AR132))</f>
@@ -82628,7 +83132,7 @@
       </c>
       <c r="AQ141" s="16">
         <f>MAX(0,(va!AR137-va!AQ137))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR141" s="16">
         <f>MAX(0,(va!AS137-va!AR137))</f>
@@ -83192,7 +83696,7 @@
       </c>
       <c r="AQ143" s="16">
         <f>MAX(0,(va!AR139-va!AQ139))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AR143" s="16">
         <f>MAX(0,(va!AS139-va!AR139))</f>

</xml_diff>

<commit_message>
04 May data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F57A93A-5F08-4EF3-B8EB-527C7128867D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7056E4-E093-4102-9333-1744044A8B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -4018,7 +4018,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="AR6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AZ2" sqref="AZ2"/>
+      <selection pane="bottomRight" activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4191,6 +4191,9 @@
       <c r="AZ2" s="12">
         <v>23102</v>
       </c>
+      <c r="BA2" s="12">
+        <v>23795</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4387,7 +4390,7 @@
       </c>
       <c r="BA3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5170</v>
       </c>
       <c r="BB3" s="10">
         <f t="shared" si="0"/>
@@ -4664,6 +4667,9 @@
       <c r="AZ5" s="10">
         <v>251</v>
       </c>
+      <c r="BA5" s="10">
+        <v>258</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5067,6 +5073,9 @@
       <c r="AZ7" s="10">
         <v>649</v>
       </c>
+      <c r="BA7" s="10">
+        <v>668</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5224,6 +5233,9 @@
       </c>
       <c r="AZ8" s="10">
         <v>325</v>
+      </c>
+      <c r="BA8" s="10">
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
@@ -5383,6 +5395,9 @@
       <c r="AZ9" s="10">
         <v>311</v>
       </c>
+      <c r="BA9" s="10">
+        <v>314</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5541,6 +5556,9 @@
       <c r="AZ10" s="10">
         <v>931</v>
       </c>
+      <c r="BA10" s="10">
+        <v>980</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5699,6 +5717,9 @@
       <c r="AZ11" s="10">
         <v>768</v>
       </c>
+      <c r="BA11" s="10">
+        <v>799</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5857,6 +5878,9 @@
       <c r="AZ12" s="10">
         <v>489</v>
       </c>
+      <c r="BA12" s="10">
+        <v>499</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -6015,6 +6039,9 @@
       <c r="AZ13" s="10">
         <v>751</v>
       </c>
+      <c r="BA13" s="10">
+        <v>769</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6173,6 +6200,9 @@
       <c r="AZ14" s="10">
         <v>713</v>
       </c>
+      <c r="BA14" s="10">
+        <v>737</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6330,6 +6360,9 @@
       </c>
       <c r="AZ15" s="10">
         <v>79</v>
+      </c>
+      <c r="BA15" s="10">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -6584,7 +6617,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AO2" sqref="AO2"/>
+      <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6725,7 +6758,7 @@
         <v>107332</v>
       </c>
       <c r="AP2" s="10">
-        <v>0</v>
+        <v>110587</v>
       </c>
       <c r="AQ2" s="10">
         <v>0</v>
@@ -6970,7 +7003,7 @@
       </c>
       <c r="AP3" s="10">
         <f>SUM(md[4-May])</f>
-        <v>0</v>
+        <v>26408</v>
       </c>
       <c r="AQ3" s="10">
         <f>SUM(md[5-May])</f>
@@ -7203,7 +7236,7 @@
         <v>5051</v>
       </c>
       <c r="AP4" s="10">
-        <v>0</v>
+        <v>5199</v>
       </c>
       <c r="AQ4" s="10">
         <v>0</v>
@@ -7409,7 +7442,7 @@
         <v>1182</v>
       </c>
       <c r="AP5" s="10">
-        <v>0</v>
+        <v>1216</v>
       </c>
       <c r="AQ5" s="10">
         <v>0</v>
@@ -7826,6 +7859,9 @@
       <c r="AO7">
         <v>124</v>
       </c>
+      <c r="AP7">
+        <v>126</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7951,6 +7987,9 @@
       <c r="AO8" s="10">
         <v>1959</v>
       </c>
+      <c r="AP8" s="10">
+        <v>2018</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -8076,6 +8115,9 @@
       <c r="AO9">
         <v>2319</v>
       </c>
+      <c r="AP9">
+        <v>2411</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -8201,6 +8243,9 @@
       <c r="AO10">
         <v>3301</v>
       </c>
+      <c r="AP10">
+        <v>3448</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8326,6 +8371,9 @@
       <c r="AO11">
         <v>162</v>
       </c>
+      <c r="AP11">
+        <v>171</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8451,6 +8499,9 @@
       <c r="AO12">
         <v>95</v>
       </c>
+      <c r="AP12">
+        <v>98</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8576,6 +8627,9 @@
       <c r="AO13">
         <v>494</v>
       </c>
+      <c r="AP13">
+        <v>506</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8701,6 +8755,9 @@
       <c r="AO14">
         <v>188</v>
       </c>
+      <c r="AP14">
+        <v>194</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8826,6 +8883,9 @@
       <c r="AO15">
         <v>637</v>
       </c>
+      <c r="AP15">
+        <v>651</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -8951,8 +9011,11 @@
       <c r="AO16" s="10">
         <v>71</v>
       </c>
+      <c r="AP16" s="10">
+        <v>75</v>
+      </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -9076,8 +9139,11 @@
       <c r="AO17">
         <v>1004</v>
       </c>
+      <c r="AP17">
+        <v>1038</v>
+      </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -9201,8 +9267,11 @@
       <c r="AO18">
         <v>4</v>
       </c>
+      <c r="AP18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -9326,8 +9395,11 @@
       <c r="AO19">
         <v>479</v>
       </c>
+      <c r="AP19">
+        <v>491</v>
+      </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9451,8 +9523,11 @@
       <c r="AO20">
         <v>969</v>
       </c>
+      <c r="AP20">
+        <v>992</v>
+      </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9576,8 +9651,11 @@
       <c r="AO21">
         <v>91</v>
       </c>
+      <c r="AP21">
+        <v>95</v>
+      </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9701,8 +9779,11 @@
       <c r="AO22">
         <v>5150</v>
       </c>
+      <c r="AP22">
+        <v>5384</v>
+      </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9826,8 +9907,11 @@
       <c r="AO23">
         <v>7333</v>
       </c>
+      <c r="AP23">
+        <v>7598</v>
+      </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -9951,8 +10035,11 @@
       <c r="AO24">
         <v>60</v>
       </c>
+      <c r="AP24">
+        <v>63</v>
+      </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -10076,8 +10163,11 @@
       <c r="AO25">
         <v>165</v>
       </c>
+      <c r="AP25">
+        <v>168</v>
+      </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -10201,8 +10291,11 @@
       <c r="AO26">
         <v>33</v>
       </c>
+      <c r="AP26">
+        <v>35</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -10326,8 +10419,11 @@
       <c r="AO27">
         <v>44</v>
       </c>
+      <c r="AP27">
+        <v>45</v>
+      </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -10451,8 +10547,11 @@
       <c r="AO28">
         <v>232</v>
       </c>
+      <c r="AP28">
+        <v>237</v>
+      </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -10576,8 +10675,11 @@
       <c r="AO29">
         <v>473</v>
       </c>
+      <c r="AP29">
+        <v>480</v>
+      </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10701,8 +10803,11 @@
       <c r="AO30">
         <v>75</v>
       </c>
+      <c r="AP30">
+        <v>80</v>
+      </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10799,7 +10904,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="AD6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AR3" sqref="AR3"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10989,7 +11094,7 @@
       </c>
       <c r="AS2" s="10">
         <f>SUM(va[4-May])</f>
-        <v>0</v>
+        <v>19492</v>
       </c>
       <c r="AT2" s="10">
         <f>SUM(va[5-May])</f>
@@ -11225,7 +11330,7 @@
         <v>2627</v>
       </c>
       <c r="AS3" s="10">
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="AT3" s="10">
         <v>0</v>
@@ -11434,7 +11539,7 @@
         <v>660</v>
       </c>
       <c r="AS4" s="10">
-        <v>0</v>
+        <v>684</v>
       </c>
       <c r="AT4" s="10">
         <v>0</v>
@@ -11643,7 +11748,7 @@
         <v>119065</v>
       </c>
       <c r="AS5" s="10">
-        <v>0</v>
+        <v>122788</v>
       </c>
       <c r="AT5" s="10">
         <v>0</v>
@@ -12078,6 +12183,9 @@
       <c r="AR7" s="10">
         <v>899</v>
       </c>
+      <c r="AS7" s="10">
+        <v>940</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
@@ -12210,6 +12318,9 @@
         <v>6</v>
       </c>
       <c r="AR8" s="10">
+        <v>6</v>
+      </c>
+      <c r="AS8" s="10">
         <v>6</v>
       </c>
     </row>
@@ -12344,6 +12455,9 @@
       <c r="AR9" s="10">
         <v>28</v>
       </c>
+      <c r="AS9" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
@@ -12476,6 +12590,9 @@
       <c r="AR10" s="10">
         <v>3</v>
       </c>
+      <c r="AS10" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
@@ -12608,6 +12725,9 @@
       <c r="AR11" s="10">
         <v>57</v>
       </c>
+      <c r="AS11" s="10">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
@@ -12740,6 +12860,9 @@
       <c r="AR12" s="10">
         <v>0</v>
       </c>
+      <c r="AS12" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
@@ -12872,6 +12995,9 @@
       <c r="AR13" s="10">
         <v>26</v>
       </c>
+      <c r="AS13" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -13006,6 +13132,9 @@
       <c r="AR14" s="10">
         <v>1106</v>
       </c>
+      <c r="AS14" s="10">
+        <v>1139</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
@@ -13139,6 +13268,9 @@
       </c>
       <c r="AR15" s="10">
         <v>46</v>
+      </c>
+      <c r="AS15" s="10">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
@@ -13272,8 +13404,11 @@
       <c r="AR16" s="10">
         <v>0</v>
       </c>
+      <c r="AS16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -13404,8 +13539,11 @@
       <c r="AR17" s="10">
         <v>2</v>
       </c>
+      <c r="AS17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
@@ -13536,8 +13674,11 @@
       <c r="AR18" s="10">
         <v>7</v>
       </c>
+      <c r="AS18" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
@@ -13668,8 +13809,11 @@
       <c r="AR19" s="10">
         <v>265</v>
       </c>
+      <c r="AS19" s="10">
+        <v>269</v>
+      </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
@@ -13800,8 +13944,11 @@
       <c r="AR20" s="10">
         <v>6</v>
       </c>
+      <c r="AS20" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
@@ -13932,8 +14079,11 @@
       <c r="AR21" s="10">
         <v>478</v>
       </c>
+      <c r="AS21" s="10">
+        <v>497</v>
+      </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
@@ -14064,8 +14214,11 @@
       <c r="AR22" s="10">
         <v>6</v>
       </c>
+      <c r="AS22" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
@@ -14196,8 +14349,11 @@
       <c r="AR23" s="10">
         <v>13</v>
       </c>
+      <c r="AS23" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="32"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
@@ -14328,8 +14484,11 @@
       <c r="AR24" s="10">
         <v>14</v>
       </c>
+      <c r="AS24" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>6</v>
       </c>
@@ -14462,8 +14621,11 @@
       <c r="AR25" s="10">
         <v>14</v>
       </c>
+      <c r="AS25" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
@@ -14594,8 +14756,11 @@
       <c r="AR26" s="10">
         <v>21</v>
       </c>
+      <c r="AS26" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
@@ -14726,8 +14891,11 @@
       <c r="AR27" s="10">
         <v>34</v>
       </c>
+      <c r="AS27" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
@@ -14858,8 +15026,11 @@
       <c r="AR28" s="10">
         <v>13</v>
       </c>
+      <c r="AS28" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" s="35"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
@@ -14990,8 +15161,11 @@
       <c r="AR29" s="10">
         <v>64</v>
       </c>
+      <c r="AS29" s="10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -15124,8 +15298,11 @@
       <c r="AR30" s="10">
         <v>279</v>
       </c>
+      <c r="AS30" s="10">
+        <v>284</v>
+      </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
         <v>62</v>
       </c>
@@ -15258,8 +15435,11 @@
       <c r="AR31" s="10">
         <v>601</v>
       </c>
+      <c r="AS31" s="10">
+        <v>601</v>
+      </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
@@ -15390,8 +15570,11 @@
       <c r="AR32" s="10">
         <v>15</v>
       </c>
+      <c r="AS32" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
@@ -15522,8 +15705,11 @@
       <c r="AR33" s="10">
         <v>57</v>
       </c>
+      <c r="AS33" s="10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>25</v>
       </c>
@@ -15656,8 +15842,11 @@
       <c r="AR34" s="10">
         <v>17</v>
       </c>
+      <c r="AS34" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>107</v>
@@ -15788,8 +15977,11 @@
       <c r="AR35" s="10">
         <v>79</v>
       </c>
+      <c r="AS35" s="10">
+        <v>80</v>
+      </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
@@ -15920,8 +16112,11 @@
       <c r="AR36" s="10">
         <v>137</v>
       </c>
+      <c r="AS36" s="10">
+        <v>141</v>
+      </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="32"/>
       <c r="B37" s="1" t="s">
         <v>53</v>
@@ -16052,8 +16247,11 @@
       <c r="AR37" s="10">
         <v>25</v>
       </c>
+      <c r="AS37" s="10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>33</v>
       </c>
@@ -16186,8 +16384,11 @@
       <c r="AR38" s="10">
         <v>18</v>
       </c>
+      <c r="AS38" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
@@ -16318,8 +16519,11 @@
       <c r="AR39" s="10">
         <v>39</v>
       </c>
+      <c r="AS39" s="10">
+        <v>41</v>
+      </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
       <c r="B40" s="1" t="s">
         <v>63</v>
@@ -16450,8 +16654,11 @@
       <c r="AR40" s="10">
         <v>35</v>
       </c>
+      <c r="AS40" s="10">
+        <v>40</v>
+      </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" s="34"/>
       <c r="B41" s="1" t="s">
         <v>129</v>
@@ -16582,8 +16789,11 @@
       <c r="AR41" s="10">
         <v>4</v>
       </c>
+      <c r="AS41" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
       <c r="B42" s="1" t="s">
         <v>130</v>
@@ -16714,8 +16924,11 @@
       <c r="AR42" s="10">
         <v>31</v>
       </c>
+      <c r="AS42" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" s="34"/>
       <c r="B43" s="1" t="s">
         <v>137</v>
@@ -16846,8 +17059,11 @@
       <c r="AR43" s="10">
         <v>24</v>
       </c>
+      <c r="AS43" s="10">
+        <v>46</v>
+      </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" s="34"/>
       <c r="B44" s="1" t="s">
         <v>142</v>
@@ -16978,8 +17194,11 @@
       <c r="AR44" s="10">
         <v>27</v>
       </c>
+      <c r="AS44" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" s="35"/>
       <c r="B45" s="1" t="s">
         <v>146</v>
@@ -17110,8 +17329,11 @@
       <c r="AR45" s="10">
         <v>35</v>
       </c>
+      <c r="AS45" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
         <v>17</v>
       </c>
@@ -17244,8 +17466,11 @@
       <c r="AR46" s="10">
         <v>16</v>
       </c>
+      <c r="AS46" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>99</v>
@@ -17376,8 +17601,11 @@
       <c r="AR47" s="10">
         <v>0</v>
       </c>
+      <c r="AS47" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>69</v>
@@ -17508,8 +17736,11 @@
       <c r="AR48" s="10">
         <v>5</v>
       </c>
+      <c r="AS48" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="32"/>
       <c r="B49" s="1" t="s">
         <v>70</v>
@@ -17640,8 +17871,11 @@
       <c r="AR49" s="10">
         <v>6</v>
       </c>
+      <c r="AS49" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
         <v>55</v>
       </c>
@@ -17774,8 +18008,11 @@
       <c r="AR50" s="10">
         <v>400</v>
       </c>
+      <c r="AS50" s="10">
+        <v>425</v>
+      </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
       <c r="B51" s="1" t="s">
         <v>54</v>
@@ -17906,8 +18143,11 @@
       <c r="AR51" s="10">
         <v>134</v>
       </c>
+      <c r="AS51" s="10">
+        <v>139</v>
+      </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
         <v>81</v>
       </c>
@@ -18040,8 +18280,11 @@
       <c r="AR52" s="10">
         <v>4340</v>
       </c>
+      <c r="AS52" s="10">
+        <v>4615</v>
+      </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
@@ -18172,8 +18415,11 @@
       <c r="AR53" s="10">
         <v>32</v>
       </c>
+      <c r="AS53" s="10">
+        <v>33</v>
+      </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="32"/>
       <c r="B54" s="1" t="s">
         <v>138</v>
@@ -18304,8 +18550,11 @@
       <c r="AR54" s="10">
         <v>35</v>
       </c>
+      <c r="AS54" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>141</v>
       </c>
@@ -18438,8 +18687,11 @@
       <c r="AR55" s="10">
         <v>123</v>
       </c>
+      <c r="AS55" s="10">
+        <v>128</v>
+      </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -18572,8 +18824,11 @@
       <c r="AR56" s="10">
         <v>954</v>
       </c>
+      <c r="AS56" s="10">
+        <v>964</v>
+      </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
         <v>47</v>
       </c>
@@ -18706,8 +18961,11 @@
       <c r="AR57" s="10">
         <v>10</v>
       </c>
+      <c r="AS57" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="34"/>
       <c r="B58" s="1" t="s">
         <v>123</v>
@@ -18838,8 +19096,11 @@
       <c r="AR58" s="10">
         <v>7</v>
       </c>
+      <c r="AS58" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="34"/>
       <c r="B59" s="1" t="s">
         <v>132</v>
@@ -18970,8 +19231,11 @@
       <c r="AR59" s="10">
         <v>22</v>
       </c>
+      <c r="AS59" s="10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" s="35"/>
       <c r="B60" s="1" t="s">
         <v>145</v>
@@ -19102,8 +19366,11 @@
       <c r="AR60" s="10">
         <v>2</v>
       </c>
+      <c r="AS60" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>28</v>
       </c>
@@ -19236,8 +19503,11 @@
       <c r="AR61" s="10">
         <v>10</v>
       </c>
+      <c r="AS61" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" s="31"/>
       <c r="B62" s="1" t="s">
         <v>104</v>
@@ -19368,8 +19638,11 @@
       <c r="AR62" s="10">
         <v>121</v>
       </c>
+      <c r="AS62" s="10">
+        <v>126</v>
+      </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" s="31"/>
       <c r="B63" s="1" t="s">
         <v>119</v>
@@ -19500,8 +19773,11 @@
       <c r="AR63" s="10">
         <v>109</v>
       </c>
+      <c r="AS63" s="10">
+        <v>113</v>
+      </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A64" s="31"/>
       <c r="B64" s="1" t="s">
         <v>124</v>
@@ -19632,8 +19908,11 @@
       <c r="AR64" s="10">
         <v>145</v>
       </c>
+      <c r="AS64" s="10">
+        <v>149</v>
+      </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A65" s="31"/>
       <c r="B65" s="1" t="s">
         <v>71</v>
@@ -19764,8 +20043,11 @@
       <c r="AR65" s="10">
         <v>61</v>
       </c>
+      <c r="AS65" s="10">
+        <v>63</v>
+      </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A66" s="32"/>
       <c r="B66" s="1" t="s">
         <v>93</v>
@@ -19896,8 +20178,11 @@
       <c r="AR66" s="10">
         <v>49</v>
       </c>
+      <c r="AS66" s="10">
+        <v>50</v>
+      </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>113</v>
       </c>
@@ -20030,8 +20315,11 @@
       <c r="AR67" s="10">
         <v>931</v>
       </c>
+      <c r="AS67" s="10">
+        <v>961</v>
+      </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>13</v>
       </c>
@@ -20164,8 +20452,11 @@
       <c r="AR68" s="10">
         <v>0</v>
       </c>
+      <c r="AS68" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" s="31"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
@@ -20296,8 +20587,11 @@
       <c r="AR69" s="10">
         <v>15</v>
       </c>
+      <c r="AS69" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="31"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
@@ -20428,8 +20722,11 @@
       <c r="AR70" s="10">
         <v>2</v>
       </c>
+      <c r="AS70" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" s="31"/>
       <c r="B71" s="1" t="s">
         <v>125</v>
@@ -20560,8 +20857,11 @@
       <c r="AR71" s="10">
         <v>13</v>
       </c>
+      <c r="AS71" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="31"/>
       <c r="B72" s="1" t="s">
         <v>131</v>
@@ -20692,8 +20992,11 @@
       <c r="AR72" s="10">
         <v>39</v>
       </c>
+      <c r="AS72" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="31"/>
       <c r="B73" s="1" t="s">
         <v>73</v>
@@ -20824,8 +21127,11 @@
       <c r="AR73" s="10">
         <v>12</v>
       </c>
+      <c r="AS73" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="31"/>
       <c r="B74" s="1" t="s">
         <v>77</v>
@@ -20956,8 +21262,11 @@
       <c r="AR74" s="10">
         <v>2</v>
       </c>
+      <c r="AS74" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75" s="32"/>
       <c r="B75" s="1" t="s">
         <v>140</v>
@@ -21088,8 +21397,11 @@
       <c r="AR75" s="10">
         <v>12</v>
       </c>
+      <c r="AS75" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
         <v>66</v>
       </c>
@@ -21222,8 +21534,11 @@
       <c r="AR76" s="10">
         <v>3</v>
       </c>
+      <c r="AS76" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A77" s="34"/>
       <c r="B77" s="1" t="s">
         <v>105</v>
@@ -21354,8 +21669,11 @@
       <c r="AR77" s="10">
         <v>4</v>
       </c>
+      <c r="AS77" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A78" s="34"/>
       <c r="B78" s="1" t="s">
         <v>115</v>
@@ -21486,8 +21804,11 @@
       <c r="AR78" s="10">
         <v>56</v>
       </c>
+      <c r="AS78" s="10">
+        <v>59</v>
+      </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A79" s="34"/>
       <c r="B79" s="1" t="s">
         <v>65</v>
@@ -21618,8 +21939,11 @@
       <c r="AR79" s="10">
         <v>9</v>
       </c>
+      <c r="AS79" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A80" s="35"/>
       <c r="B80" s="1" t="s">
         <v>149</v>
@@ -21750,8 +22074,11 @@
       <c r="AR80" s="10">
         <v>3</v>
       </c>
+      <c r="AS80" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>88</v>
       </c>
@@ -21884,8 +22211,11 @@
       <c r="AR81" s="10">
         <v>221</v>
       </c>
+      <c r="AS81" s="10">
+        <v>239</v>
+      </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A82" s="33" t="s">
         <v>75</v>
       </c>
@@ -22018,8 +22348,11 @@
       <c r="AR82" s="10">
         <v>163</v>
       </c>
+      <c r="AS82" s="10">
+        <v>167</v>
+      </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A83" s="34"/>
       <c r="B83" s="1" t="s">
         <v>74</v>
@@ -22150,8 +22483,11 @@
       <c r="AR83" s="10">
         <v>47</v>
       </c>
+      <c r="AS83" s="10">
+        <v>47</v>
+      </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A84" s="34"/>
       <c r="B84" s="1" t="s">
         <v>87</v>
@@ -22282,8 +22618,11 @@
       <c r="AR84" s="10">
         <v>125</v>
       </c>
+      <c r="AS84" s="10">
+        <v>132</v>
+      </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A85" s="34"/>
       <c r="B85" s="1" t="s">
         <v>147</v>
@@ -22414,8 +22753,11 @@
       <c r="AR85" s="10">
         <v>6</v>
       </c>
+      <c r="AS85" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A86" s="35"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
@@ -22546,8 +22888,11 @@
       <c r="AR86" s="10">
         <v>22</v>
       </c>
+      <c r="AS86" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
         <v>19</v>
       </c>
@@ -22680,8 +23025,11 @@
       <c r="AR87" s="10">
         <v>16</v>
       </c>
+      <c r="AS87" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A88" s="31"/>
       <c r="B88" s="1" t="s">
         <v>18</v>
@@ -22812,8 +23160,11 @@
       <c r="AR88" s="10">
         <v>137</v>
       </c>
+      <c r="AS88" s="10">
+        <v>137</v>
+      </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A89" s="31"/>
       <c r="B89" s="1" t="s">
         <v>26</v>
@@ -22944,8 +23295,11 @@
       <c r="AR89" s="10">
         <v>9</v>
       </c>
+      <c r="AS89" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A90" s="31"/>
       <c r="B90" s="1" t="s">
         <v>31</v>
@@ -23076,8 +23430,11 @@
       <c r="AR90" s="10">
         <v>12</v>
       </c>
+      <c r="AS90" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A91" s="31"/>
       <c r="B91" s="1" t="s">
         <v>49</v>
@@ -23208,8 +23565,11 @@
       <c r="AR91" s="10">
         <v>4</v>
       </c>
+      <c r="AS91" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A92" s="31"/>
       <c r="B92" s="1" t="s">
         <v>117</v>
@@ -23340,8 +23700,11 @@
       <c r="AR92" s="10">
         <v>13</v>
       </c>
+      <c r="AS92" s="10">
+        <v>14</v>
+      </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A93" s="32"/>
       <c r="B93" s="1" t="s">
         <v>120</v>
@@ -23472,8 +23835,11 @@
       <c r="AR93" s="10">
         <v>55</v>
       </c>
+      <c r="AS93" s="10">
+        <v>55</v>
+      </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A94" s="33" t="s">
         <v>60</v>
       </c>
@@ -23606,8 +23972,11 @@
       <c r="AR94" s="10">
         <v>14</v>
       </c>
+      <c r="AS94" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A95" s="35"/>
       <c r="B95" s="1" t="s">
         <v>79</v>
@@ -23738,8 +24107,11 @@
       <c r="AR95" s="10">
         <v>37</v>
       </c>
+      <c r="AS95" s="10">
+        <v>37</v>
+      </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
@@ -23872,8 +24244,11 @@
       <c r="AR96" s="10">
         <v>183</v>
       </c>
+      <c r="AS96" s="10">
+        <v>183</v>
+      </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A97" s="33" t="s">
         <v>64</v>
       </c>
@@ -24006,8 +24381,11 @@
       <c r="AR97" s="10">
         <v>2026</v>
       </c>
+      <c r="AS97" s="10">
+        <v>2146</v>
+      </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A98" s="34"/>
       <c r="B98" s="1" t="s">
         <v>144</v>
@@ -24138,8 +24516,11 @@
       <c r="AR98" s="10">
         <v>266</v>
       </c>
+      <c r="AS98" s="10">
+        <v>273</v>
+      </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A99" s="35"/>
       <c r="B99" s="1" t="s">
         <v>85</v>
@@ -24270,8 +24651,11 @@
       <c r="AR99" s="10">
         <v>82</v>
       </c>
+      <c r="AS99" s="10">
+        <v>88</v>
+      </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
         <v>22</v>
       </c>
@@ -24404,8 +24788,11 @@
       <c r="AR100" s="10">
         <v>31</v>
       </c>
+      <c r="AS100" s="10">
+        <v>32</v>
+      </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A101" s="31"/>
       <c r="B101" s="1" t="s">
         <v>110</v>
@@ -24536,8 +24923,11 @@
       <c r="AR101" s="10">
         <v>35</v>
       </c>
+      <c r="AS101" s="10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A102" s="31"/>
       <c r="B102" s="1" t="s">
         <v>127</v>
@@ -24668,8 +25058,11 @@
       <c r="AR102" s="10">
         <v>186</v>
       </c>
+      <c r="AS102" s="10">
+        <v>195</v>
+      </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A103" s="31"/>
       <c r="B103" s="1" t="s">
         <v>128</v>
@@ -24800,8 +25193,11 @@
       <c r="AR103" s="10">
         <v>271</v>
       </c>
+      <c r="AS103" s="10">
+        <v>288</v>
+      </c>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A104" s="32"/>
       <c r="B104" s="1" t="s">
         <v>139</v>
@@ -24932,8 +25328,11 @@
       <c r="AR104" s="10">
         <v>39</v>
       </c>
+      <c r="AS104" s="10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A105" s="33" t="s">
         <v>30</v>
       </c>
@@ -25066,8 +25465,11 @@
       <c r="AR105" s="10">
         <v>191</v>
       </c>
+      <c r="AS105" s="10">
+        <v>196</v>
+      </c>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A106" s="34"/>
       <c r="B106" s="1" t="s">
         <v>100</v>
@@ -25198,8 +25600,11 @@
       <c r="AR106" s="10">
         <v>133</v>
       </c>
+      <c r="AS106" s="10">
+        <v>140</v>
+      </c>
     </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A107" s="34"/>
       <c r="B107" s="1" t="s">
         <v>50</v>
@@ -25330,8 +25735,11 @@
       <c r="AR107" s="10">
         <v>15</v>
       </c>
+      <c r="AS107" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A108" s="34"/>
       <c r="B108" s="1" t="s">
         <v>118</v>
@@ -25462,8 +25870,11 @@
       <c r="AR108" s="10">
         <v>37</v>
       </c>
+      <c r="AS108" s="10">
+        <v>39</v>
+      </c>
     </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A109" s="35"/>
       <c r="B109" s="1" t="s">
         <v>22</v>
@@ -25594,8 +26005,11 @@
       <c r="AR109" s="10">
         <v>6</v>
       </c>
+      <c r="AS109" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>151</v>
       </c>
@@ -25728,8 +26142,11 @@
       <c r="AR110" s="10">
         <v>403</v>
       </c>
+      <c r="AS110" s="10">
+        <v>419</v>
+      </c>
     </row>
-    <row r="111" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>153</v>
       </c>
@@ -25862,8 +26279,11 @@
       <c r="AR111" s="10">
         <v>81</v>
       </c>
+      <c r="AS111" s="10">
+        <v>81</v>
+      </c>
     </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A112" s="30" t="s">
         <v>15</v>
       </c>
@@ -25996,8 +26416,11 @@
       <c r="AR112" s="10">
         <v>15</v>
       </c>
+      <c r="AS112" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="113" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A113" s="31"/>
       <c r="B113" s="1" t="s">
         <v>39</v>
@@ -26128,8 +26551,11 @@
       <c r="AR113" s="10">
         <v>19</v>
       </c>
+      <c r="AS113" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="114" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A114" s="32"/>
       <c r="B114" s="1" t="s">
         <v>114</v>
@@ -26260,8 +26686,11 @@
       <c r="AR114" s="10">
         <v>106</v>
       </c>
+      <c r="AS114" s="10">
+        <v>106</v>
+      </c>
     </row>
-    <row r="115" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A115" s="33" t="s">
         <v>4</v>
       </c>
@@ -26394,8 +26823,11 @@
       <c r="AR115" s="10">
         <v>108</v>
       </c>
+      <c r="AS115" s="10">
+        <v>110</v>
+      </c>
     </row>
-    <row r="116" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A116" s="34"/>
       <c r="B116" s="1" t="s">
         <v>102</v>
@@ -26526,8 +26958,11 @@
       <c r="AR116" s="10">
         <v>76</v>
       </c>
+      <c r="AS116" s="10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="117" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A117" s="34"/>
       <c r="B117" s="1" t="s">
         <v>37</v>
@@ -26658,8 +27093,11 @@
       <c r="AR117" s="10">
         <v>10</v>
       </c>
+      <c r="AS117" s="10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="118" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A118" s="34"/>
       <c r="B118" s="1" t="s">
         <v>48</v>
@@ -26790,8 +27228,11 @@
       <c r="AR118" s="10">
         <v>46</v>
       </c>
+      <c r="AS118" s="10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="119" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A119" s="34"/>
       <c r="B119" s="1" t="s">
         <v>116</v>
@@ -26922,8 +27363,11 @@
       <c r="AR119" s="10">
         <v>8</v>
       </c>
+      <c r="AS119" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="120" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A120" s="35"/>
       <c r="B120" s="1" t="s">
         <v>134</v>
@@ -27054,8 +27498,11 @@
       <c r="AR120" s="10">
         <v>63</v>
       </c>
+      <c r="AS120" s="10">
+        <v>63</v>
+      </c>
     </row>
-    <row r="121" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A121" s="30" t="s">
         <v>35</v>
       </c>
@@ -27188,8 +27635,11 @@
       <c r="AR121" s="10">
         <v>11</v>
       </c>
+      <c r="AS121" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="122" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A122" s="31"/>
       <c r="B122" s="1" t="s">
         <v>106</v>
@@ -27320,8 +27770,11 @@
       <c r="AR122" s="10">
         <v>25</v>
       </c>
+      <c r="AS122" s="10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="123" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A123" s="31"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
@@ -27452,8 +27905,11 @@
       <c r="AR123" s="10">
         <v>3</v>
       </c>
+      <c r="AS123" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="124" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A124" s="31"/>
       <c r="B124" s="1" t="s">
         <v>111</v>
@@ -27584,8 +28040,11 @@
       <c r="AR124" s="10">
         <v>9</v>
       </c>
+      <c r="AS124" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="125" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A125" s="31"/>
       <c r="B125" s="1" t="s">
         <v>112</v>
@@ -27716,8 +28175,11 @@
       <c r="AR125" s="10">
         <v>4</v>
       </c>
+      <c r="AS125" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="126" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A126" s="31"/>
       <c r="B126" s="1" t="s">
         <v>51</v>
@@ -27848,8 +28310,11 @@
       <c r="AR126" s="10">
         <v>4</v>
       </c>
+      <c r="AS126" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A127" s="31"/>
       <c r="B127" s="1" t="s">
         <v>52</v>
@@ -27980,8 +28445,11 @@
       <c r="AR127" s="10">
         <v>7</v>
       </c>
+      <c r="AS127" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="128" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A128" s="31"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
@@ -28112,8 +28580,11 @@
       <c r="AR128" s="10">
         <v>9</v>
       </c>
+      <c r="AS128" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="129" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A129" s="31"/>
       <c r="B129" s="1" t="s">
         <v>121</v>
@@ -28244,8 +28715,11 @@
       <c r="AR129" s="10">
         <v>145</v>
       </c>
+      <c r="AS129" s="10">
+        <v>145</v>
+      </c>
     </row>
-    <row r="130" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A130" s="32"/>
       <c r="B130" s="1" t="s">
         <v>72</v>
@@ -28376,8 +28850,11 @@
       <c r="AR130" s="10">
         <v>26</v>
       </c>
+      <c r="AS130" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="131" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>156</v>
       </c>
@@ -28510,8 +28987,11 @@
       <c r="AR131" s="10">
         <v>413</v>
       </c>
+      <c r="AS131" s="10">
+        <v>439</v>
+      </c>
     </row>
-    <row r="132" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A132" s="30" t="s">
         <v>58</v>
       </c>
@@ -28644,8 +29124,11 @@
       <c r="AR132" s="10">
         <v>23</v>
       </c>
+      <c r="AS132" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="133" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A133" s="31"/>
       <c r="B133" s="1" t="s">
         <v>108</v>
@@ -28776,8 +29259,11 @@
       <c r="AR133" s="10">
         <v>19</v>
       </c>
+      <c r="AS133" s="10">
+        <v>19</v>
+      </c>
     </row>
-    <row r="134" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A134" s="31"/>
       <c r="B134" s="1" t="s">
         <v>57</v>
@@ -28908,8 +29394,11 @@
       <c r="AR134" s="10">
         <v>2</v>
       </c>
+      <c r="AS134" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="135" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A135" s="32"/>
       <c r="B135" s="1" t="s">
         <v>86</v>
@@ -29040,8 +29529,11 @@
       <c r="AR135" s="10">
         <v>2</v>
       </c>
+      <c r="AS135" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="136" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A136" s="33" t="s">
         <v>44</v>
       </c>
@@ -29174,8 +29666,11 @@
       <c r="AR136" s="10">
         <v>99</v>
       </c>
+      <c r="AS136" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="137" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A137" s="34"/>
       <c r="B137" s="1" t="s">
         <v>126</v>
@@ -29306,8 +29801,11 @@
       <c r="AR137" s="10">
         <v>127</v>
       </c>
+      <c r="AS137" s="10">
+        <v>127</v>
+      </c>
     </row>
-    <row r="138" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A138" s="34"/>
       <c r="B138" s="1" t="s">
         <v>82</v>
@@ -29438,8 +29936,11 @@
       <c r="AR138" s="10">
         <v>23</v>
       </c>
+      <c r="AS138" s="10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="139" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A139" s="35"/>
       <c r="B139" s="1" t="s">
         <v>155</v>
@@ -29568,6 +30069,9 @@
         <v>178</v>
       </c>
       <c r="AR139" s="10">
+        <v>190</v>
+      </c>
+      <c r="AS139" s="10">
         <v>190</v>
       </c>
     </row>
@@ -29931,7 +30435,7 @@
       </c>
       <c r="BA2" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>22.222222222222221</v>
       </c>
       <c r="BB2" s="18">
         <f t="shared" si="1"/>
@@ -30581,7 +31085,7 @@
       </c>
       <c r="BA4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.5454545454545459</v>
       </c>
       <c r="BB4" s="10">
         <f t="shared" si="7"/>
@@ -30906,7 +31410,7 @@
       </c>
       <c r="BA6" s="12">
         <f>MAX(0, (dc!BA2-dc!AZ2))</f>
-        <v>0</v>
+        <v>693</v>
       </c>
       <c r="BB6" s="12">
         <f>MAX(0, (dc!BB2-dc!BA2))</f>
@@ -31230,7 +31734,7 @@
       </c>
       <c r="BA7" s="12">
         <f>MAX(0, (dc!BA3-dc!AZ3))</f>
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="BB7" s="12">
         <f>MAX(0, (dc!BB3-dc!BA3))</f>
@@ -31878,7 +32382,7 @@
       </c>
       <c r="BA9" s="12">
         <f>MAX(0, (dc!BA5-dc!AZ5))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BB9" s="12">
         <f>MAX(0, (dc!BB5-dc!BA5))</f>
@@ -32430,7 +32934,7 @@
       </c>
       <c r="BA11" s="10">
         <f>MAX(0,(dc!BA7-dc!AZ7))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="BB11" s="10">
         <f>MAX(0,(dc!BB7-dc!BA7))</f>
@@ -32737,7 +33241,7 @@
       </c>
       <c r="BA12" s="10">
         <f>MAX(0,(dc!BA8-dc!AZ8))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BB12" s="10">
         <f>MAX(0,(dc!BB8-dc!BA8))</f>
@@ -33044,7 +33548,7 @@
       </c>
       <c r="BA13" s="10">
         <f>MAX(0,(dc!BA9-dc!AZ9))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB13" s="10">
         <f>MAX(0,(dc!BB9-dc!BA9))</f>
@@ -33351,7 +33855,7 @@
       </c>
       <c r="BA14" s="10">
         <f>MAX(0,(dc!BA10-dc!AZ10))</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="BB14" s="10">
         <f>MAX(0,(dc!BB10-dc!BA10))</f>
@@ -33658,7 +34162,7 @@
       </c>
       <c r="BA15" s="10">
         <f>MAX(0,(dc!BA11-dc!AZ11))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="BB15" s="10">
         <f>MAX(0,(dc!BB11-dc!BA11))</f>
@@ -33965,7 +34469,7 @@
       </c>
       <c r="BA16" s="10">
         <f>MAX(0,(dc!BA12-dc!AZ12))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BB16" s="10">
         <f>MAX(0,(dc!BB12-dc!BA12))</f>
@@ -34272,7 +34776,7 @@
       </c>
       <c r="BA17" s="10">
         <f>MAX(0,(dc!BA13-dc!AZ13))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="BB17" s="10">
         <f>MAX(0,(dc!BB13-dc!BA13))</f>
@@ -34579,7 +35083,7 @@
       </c>
       <c r="BA18" s="10">
         <f>MAX(0,(dc!BA14-dc!AZ14))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="BB18" s="10">
         <f>MAX(0,(dc!BB14-dc!BA14))</f>
@@ -35283,7 +35787,7 @@
       </c>
       <c r="AP2" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>22.518447988574149</v>
       </c>
       <c r="AQ2" s="20">
         <f t="shared" si="1"/>
@@ -35556,7 +36060,7 @@
       </c>
       <c r="AP3" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15.644820295983086</v>
       </c>
       <c r="AQ3" s="20">
         <f t="shared" si="3"/>
@@ -35829,7 +36333,7 @@
       </c>
       <c r="AP4" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.5940803382663846</v>
       </c>
       <c r="AQ4" s="20">
         <f t="shared" si="5"/>
@@ -36165,7 +36669,7 @@
       </c>
       <c r="AP6" s="14">
         <f>MAX(0,(md!AP2-md!AO2)+(md!AP3-md!AO3))</f>
-        <v>0</v>
+        <v>4201</v>
       </c>
       <c r="AQ6" s="14">
         <f>MAX(0,(md!AQ2-md!AP2)+(md!AQ3-md!AP3))</f>
@@ -36437,7 +36941,7 @@
       </c>
       <c r="AP7" s="14">
         <f>MAX(0,(md!AP3-md!AO3))</f>
-        <v>0</v>
+        <v>946</v>
       </c>
       <c r="AQ7" s="14">
         <f>MAX(0,(md!AQ3-md!AP3))</f>
@@ -36709,7 +37213,7 @@
       </c>
       <c r="AP8" s="14">
         <f>MAX(0,(md!AP4-md!AO4))</f>
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AQ8" s="14">
         <f>MAX(0,(md!AQ4-md!AP4))</f>
@@ -36981,7 +37485,7 @@
       </c>
       <c r="AP9" s="14">
         <f>MAX(0,(md!AP5-md!AO5))</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AQ9" s="14">
         <f>MAX(0,(md!AQ5-md!AP5))</f>
@@ -37467,7 +37971,7 @@
       </c>
       <c r="AP11" s="14">
         <f>MAX(0,(md!AP7-md!AO7))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ11" s="14">
         <f>MAX(0,(md!AQ7-md!AP7))</f>
@@ -37744,7 +38248,7 @@
       </c>
       <c r="AP12" s="14">
         <f>MAX(0,(md!AP8-md!AO8))</f>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="AQ12" s="14">
         <f>MAX(0,(md!AQ8-md!AP8))</f>
@@ -38021,7 +38525,7 @@
       </c>
       <c r="AP13" s="14">
         <f>MAX(0,(md!AP9-md!AO9))</f>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="AQ13" s="14">
         <f>MAX(0,(md!AQ9-md!AP9))</f>
@@ -38298,7 +38802,7 @@
       </c>
       <c r="AP14" s="14">
         <f>MAX(0,(md!AP10-md!AO10))</f>
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="AQ14" s="14">
         <f>MAX(0,(md!AQ10-md!AP10))</f>
@@ -38575,7 +39079,7 @@
       </c>
       <c r="AP15" s="14">
         <f>MAX(0,(md!AP11-md!AO11))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AQ15" s="14">
         <f>MAX(0,(md!AQ11-md!AP11))</f>
@@ -38852,7 +39356,7 @@
       </c>
       <c r="AP16" s="14">
         <f>MAX(0,(md!AP12-md!AO12))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ16" s="14">
         <f>MAX(0,(md!AQ12-md!AP12))</f>
@@ -39129,7 +39633,7 @@
       </c>
       <c r="AP17" s="14">
         <f>MAX(0,(md!AP13-md!AO13))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AQ17" s="14">
         <f>MAX(0,(md!AQ13-md!AP13))</f>
@@ -39406,7 +39910,7 @@
       </c>
       <c r="AP18" s="14">
         <f>MAX(0,(md!AP14-md!AO14))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AQ18" s="14">
         <f>MAX(0,(md!AQ14-md!AP14))</f>
@@ -39683,7 +40187,7 @@
       </c>
       <c r="AP19" s="14">
         <f>MAX(0,(md!AP15-md!AO15))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AQ19" s="14">
         <f>MAX(0,(md!AQ15-md!AP15))</f>
@@ -39960,7 +40464,7 @@
       </c>
       <c r="AP20" s="14">
         <f>MAX(0,(md!AP16-md!AO16))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ20" s="14">
         <f>MAX(0,(md!AQ16-md!AP16))</f>
@@ -40237,7 +40741,7 @@
       </c>
       <c r="AP21" s="14">
         <f>MAX(0,(md!AP17-md!AO17))</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AQ21" s="14">
         <f>MAX(0,(md!AQ17-md!AP17))</f>
@@ -40791,7 +41295,7 @@
       </c>
       <c r="AP23" s="14">
         <f>MAX(0,(md!AP19-md!AO19))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AQ23" s="14">
         <f>MAX(0,(md!AQ19-md!AP19))</f>
@@ -41068,7 +41572,7 @@
       </c>
       <c r="AP24" s="14">
         <f>MAX(0,(md!AP20-md!AO20))</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AQ24" s="14">
         <f>MAX(0,(md!AQ20-md!AP20))</f>
@@ -41345,7 +41849,7 @@
       </c>
       <c r="AP25" s="14">
         <f>MAX(0,(md!AP21-md!AO21))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ25" s="14">
         <f>MAX(0,(md!AQ21-md!AP21))</f>
@@ -41622,7 +42126,7 @@
       </c>
       <c r="AP26" s="14">
         <f>MAX(0,(md!AP22-md!AO22))</f>
-        <v>0</v>
+        <v>234</v>
       </c>
       <c r="AQ26" s="14">
         <f>MAX(0,(md!AQ22-md!AP22))</f>
@@ -41899,7 +42403,7 @@
       </c>
       <c r="AP27" s="14">
         <f>MAX(0,(md!AP23-md!AO23))</f>
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="AQ27" s="14">
         <f>MAX(0,(md!AQ23-md!AP23))</f>
@@ -42176,7 +42680,7 @@
       </c>
       <c r="AP28" s="14">
         <f>MAX(0,(md!AP24-md!AO24))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ28" s="14">
         <f>MAX(0,(md!AQ24-md!AP24))</f>
@@ -42453,7 +42957,7 @@
       </c>
       <c r="AP29" s="14">
         <f>MAX(0,(md!AP25-md!AO25))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ29" s="14">
         <f>MAX(0,(md!AQ25-md!AP25))</f>
@@ -42730,7 +43234,7 @@
       </c>
       <c r="AP30" s="14">
         <f>MAX(0,(md!AP26-md!AO26))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ30" s="14">
         <f>MAX(0,(md!AQ26-md!AP26))</f>
@@ -43007,7 +43511,7 @@
       </c>
       <c r="AP31" s="14">
         <f>MAX(0,(md!AP27-md!AO27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ31" s="14">
         <f>MAX(0,(md!AQ27-md!AP27))</f>
@@ -43284,7 +43788,7 @@
       </c>
       <c r="AP32" s="14">
         <f>MAX(0,(md!AP28-md!AO28))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AQ32" s="14">
         <f>MAX(0,(md!AQ28-md!AP28))</f>
@@ -43561,7 +44065,7 @@
       </c>
       <c r="AP33" s="14">
         <f>MAX(0,(md!AP29-md!AO29))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AQ33" s="14">
         <f>MAX(0,(md!AQ29-md!AP29))</f>
@@ -43838,7 +44342,7 @@
       </c>
       <c r="AP34" s="14">
         <f>MAX(0,(md!AP30-md!AO30))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AQ34" s="14">
         <f>MAX(0,(md!AQ30-md!AP30))</f>
@@ -44130,7 +44634,7 @@
   </sheetPr>
   <dimension ref="A1:BS143"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A102" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -44317,7 +44821,7 @@
       </c>
       <c r="AR2" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>22.052108514638732</v>
       </c>
       <c r="AS2" s="19">
         <f t="shared" si="1"/>
@@ -44594,7 +45098,7 @@
       </c>
       <c r="AR3" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8.8915956151035331</v>
       </c>
       <c r="AS3" s="19">
         <f t="shared" si="3"/>
@@ -44871,7 +45375,7 @@
       </c>
       <c r="AR4" s="19">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.9232643118148598</v>
       </c>
       <c r="AS4" s="19">
         <f t="shared" si="5"/>
@@ -45148,7 +45652,7 @@
       </c>
       <c r="AR6" s="14">
         <f>MAX(0,(va!AS5-va!AR5))</f>
-        <v>0</v>
+        <v>3723</v>
       </c>
       <c r="AS6" s="14">
         <f>MAX(0,(va!AT5-va!AS5))</f>
@@ -45425,7 +45929,7 @@
       </c>
       <c r="AR7" s="14">
         <f>MAX(0,(va!AS2-va!AR2))</f>
-        <v>0</v>
+        <v>821</v>
       </c>
       <c r="AS7" s="14">
         <f>MAX(0,(va!AT2-va!AS2))</f>
@@ -45702,7 +46206,7 @@
       </c>
       <c r="AR8" s="14">
         <f>MAX(0,(va!AS3-va!AR3))</f>
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="AS8" s="14">
         <f>MAX(0,(va!AT3-va!AS3))</f>
@@ -45979,7 +46483,7 @@
       </c>
       <c r="AR9" s="14">
         <f>MAX(0,(va!AS4-va!AR4))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AS9" s="14">
         <f>MAX(0,(va!AT4-va!AS4))</f>
@@ -46476,7 +46980,7 @@
       </c>
       <c r="AR11" s="16">
         <f>MAX(0,(va!AS7-va!AR7))</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="AS11" s="16">
         <f>MAX(0,(va!AT7-va!AS7))</f>
@@ -48168,7 +48672,7 @@
       </c>
       <c r="AR17" s="16">
         <f>MAX(0,(va!AS13-va!AR13))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS17" s="16">
         <f>MAX(0,(va!AT13-va!AS13))</f>
@@ -48450,7 +48954,7 @@
       </c>
       <c r="AR18" s="16">
         <f>MAX(0,(va!AS14-va!AR14))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AS18" s="16">
         <f>MAX(0,(va!AT14-va!AS14))</f>
@@ -48732,7 +49236,7 @@
       </c>
       <c r="AR19" s="16">
         <f>MAX(0,(va!AS15-va!AR15))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS19" s="16">
         <f>MAX(0,(va!AT15-va!AS15))</f>
@@ -49860,7 +50364,7 @@
       </c>
       <c r="AR23" s="16">
         <f>MAX(0,(va!AS19-va!AR19))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS23" s="16">
         <f>MAX(0,(va!AT19-va!AS19))</f>
@@ -50424,7 +50928,7 @@
       </c>
       <c r="AR25" s="16">
         <f>MAX(0,(va!AS21-va!AR21))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AS25" s="16">
         <f>MAX(0,(va!AT21-va!AS21))</f>
@@ -52116,7 +52620,7 @@
       </c>
       <c r="AR31" s="16">
         <f>MAX(0,(va!AS27-va!AR27))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS31" s="16">
         <f>MAX(0,(va!AT27-va!AS27))</f>
@@ -52962,7 +53466,7 @@
       </c>
       <c r="AR34" s="16">
         <f>MAX(0,(va!AS30-va!AR30))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS34" s="16">
         <f>MAX(0,(va!AT30-va!AS30))</f>
@@ -54372,7 +54876,7 @@
       </c>
       <c r="AR39" s="16">
         <f>MAX(0,(va!AS35-va!AR35))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS39" s="16">
         <f>MAX(0,(va!AT35-va!AS35))</f>
@@ -54654,7 +55158,7 @@
       </c>
       <c r="AR40" s="16">
         <f>MAX(0,(va!AS36-va!AR36))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS40" s="16">
         <f>MAX(0,(va!AT36-va!AS36))</f>
@@ -54936,7 +55440,7 @@
       </c>
       <c r="AR41" s="16">
         <f>MAX(0,(va!AS37-va!AR37))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS41" s="16">
         <f>MAX(0,(va!AT37-va!AS37))</f>
@@ -55218,7 +55722,7 @@
       </c>
       <c r="AR42" s="16">
         <f>MAX(0,(va!AS38-va!AR38))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS42" s="16">
         <f>MAX(0,(va!AT38-va!AS38))</f>
@@ -55500,7 +56004,7 @@
       </c>
       <c r="AR43" s="16">
         <f>MAX(0,(va!AS39-va!AR39))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS43" s="16">
         <f>MAX(0,(va!AT39-va!AS39))</f>
@@ -55782,7 +56286,7 @@
       </c>
       <c r="AR44" s="16">
         <f>MAX(0,(va!AS40-va!AR40))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS44" s="16">
         <f>MAX(0,(va!AT40-va!AS40))</f>
@@ -56346,7 +56850,7 @@
       </c>
       <c r="AR46" s="16">
         <f>MAX(0,(va!AS42-va!AR42))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS46" s="16">
         <f>MAX(0,(va!AT42-va!AS42))</f>
@@ -56628,7 +57132,7 @@
       </c>
       <c r="AR47" s="16">
         <f>MAX(0,(va!AS43-va!AR43))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AS47" s="16">
         <f>MAX(0,(va!AT43-va!AS43))</f>
@@ -56910,7 +57414,7 @@
       </c>
       <c r="AR48" s="16">
         <f>MAX(0,(va!AS44-va!AR44))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS48" s="16">
         <f>MAX(0,(va!AT44-va!AS44))</f>
@@ -57192,7 +57696,7 @@
       </c>
       <c r="AR49" s="16">
         <f>MAX(0,(va!AS45-va!AR45))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS49" s="16">
         <f>MAX(0,(va!AT45-va!AS45))</f>
@@ -58602,7 +59106,7 @@
       </c>
       <c r="AR54" s="16">
         <f>MAX(0,(va!AS50-va!AR50))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AS54" s="16">
         <f>MAX(0,(va!AT50-va!AS50))</f>
@@ -58884,7 +59388,7 @@
       </c>
       <c r="AR55" s="16">
         <f>MAX(0,(va!AS51-va!AR51))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS55" s="16">
         <f>MAX(0,(va!AT51-va!AS51))</f>
@@ -59166,7 +59670,7 @@
       </c>
       <c r="AR56" s="16">
         <f>MAX(0,(va!AS52-va!AR52))</f>
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="AS56" s="16">
         <f>MAX(0,(va!AT52-va!AS52))</f>
@@ -59448,7 +59952,7 @@
       </c>
       <c r="AR57" s="16">
         <f>MAX(0,(va!AS53-va!AR53))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS57" s="16">
         <f>MAX(0,(va!AT53-va!AS53))</f>
@@ -59730,7 +60234,7 @@
       </c>
       <c r="AR58" s="16">
         <f>MAX(0,(va!AS54-va!AR54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS58" s="16">
         <f>MAX(0,(va!AT54-va!AS54))</f>
@@ -60012,7 +60516,7 @@
       </c>
       <c r="AR59" s="16">
         <f>MAX(0,(va!AS55-va!AR55))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS59" s="16">
         <f>MAX(0,(va!AT55-va!AS55))</f>
@@ -60294,7 +60798,7 @@
       </c>
       <c r="AR60" s="16">
         <f>MAX(0,(va!AS56-va!AR56))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AS60" s="16">
         <f>MAX(0,(va!AT56-va!AS56))</f>
@@ -61986,7 +62490,7 @@
       </c>
       <c r="AR66" s="16">
         <f>MAX(0,(va!AS62-va!AR62))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS66" s="16">
         <f>MAX(0,(va!AT62-va!AS62))</f>
@@ -62268,7 +62772,7 @@
       </c>
       <c r="AR67" s="16">
         <f>MAX(0,(va!AS63-va!AR63))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS67" s="16">
         <f>MAX(0,(va!AT63-va!AS63))</f>
@@ -62550,7 +63054,7 @@
       </c>
       <c r="AR68" s="16">
         <f>MAX(0,(va!AS64-va!AR64))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS68" s="16">
         <f>MAX(0,(va!AT64-va!AS64))</f>
@@ -62832,7 +63336,7 @@
       </c>
       <c r="AR69" s="16">
         <f>MAX(0,(va!AS65-va!AR65))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS69" s="16">
         <f>MAX(0,(va!AT65-va!AS65))</f>
@@ -63114,7 +63618,7 @@
       </c>
       <c r="AR70" s="16">
         <f>MAX(0,(va!AS66-va!AR66))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS70" s="16">
         <f>MAX(0,(va!AT66-va!AS66))</f>
@@ -63396,7 +63900,7 @@
       </c>
       <c r="AR71" s="16">
         <f>MAX(0,(va!AS67-va!AR67))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AS71" s="16">
         <f>MAX(0,(va!AT67-va!AS67))</f>
@@ -63960,7 +64464,7 @@
       </c>
       <c r="AR73" s="16">
         <f>MAX(0,(va!AS69-va!AR69))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS73" s="16">
         <f>MAX(0,(va!AT69-va!AS69))</f>
@@ -64242,7 +64746,7 @@
       </c>
       <c r="AR74" s="16">
         <f>MAX(0,(va!AS70-va!AR70))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS74" s="16">
         <f>MAX(0,(va!AT70-va!AS70))</f>
@@ -65652,7 +66156,7 @@
       </c>
       <c r="AR79" s="16">
         <f>MAX(0,(va!AS75-va!AR75))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AS79" s="16">
         <f>MAX(0,(va!AT75-va!AS75))</f>
@@ -66498,7 +67002,7 @@
       </c>
       <c r="AR82" s="16">
         <f>MAX(0,(va!AS78-va!AR78))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS82" s="16">
         <f>MAX(0,(va!AT78-va!AS78))</f>
@@ -67344,7 +67848,7 @@
       </c>
       <c r="AR85" s="16">
         <f>MAX(0,(va!AS81-va!AR81))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AS85" s="16">
         <f>MAX(0,(va!AT81-va!AS81))</f>
@@ -67626,7 +68130,7 @@
       </c>
       <c r="AR86" s="16">
         <f>MAX(0,(va!AS82-va!AR82))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AS86" s="16">
         <f>MAX(0,(va!AT82-va!AS82))</f>
@@ -68190,7 +68694,7 @@
       </c>
       <c r="AR88" s="16">
         <f>MAX(0,(va!AS84-va!AR84))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AS88" s="16">
         <f>MAX(0,(va!AT84-va!AS84))</f>
@@ -68754,7 +69258,7 @@
       </c>
       <c r="AR90" s="16">
         <f>MAX(0,(va!AS86-va!AR86))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS90" s="16">
         <f>MAX(0,(va!AT86-va!AS86))</f>
@@ -69600,7 +70104,7 @@
       </c>
       <c r="AR93" s="16">
         <f>MAX(0,(va!AS89-va!AR89))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS93" s="16">
         <f>MAX(0,(va!AT89-va!AS89))</f>
@@ -70446,7 +70950,7 @@
       </c>
       <c r="AR96" s="16">
         <f>MAX(0,(va!AS92-va!AR92))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS96" s="16">
         <f>MAX(0,(va!AT92-va!AS92))</f>
@@ -71010,7 +71514,7 @@
       </c>
       <c r="AR98" s="16">
         <f>MAX(0,(va!AS94-va!AR94))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS98" s="16">
         <f>MAX(0,(va!AT94-va!AS94))</f>
@@ -71856,7 +72360,7 @@
       </c>
       <c r="AR101" s="16">
         <f>MAX(0,(va!AS97-va!AR97))</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AS101" s="16">
         <f>MAX(0,(va!AT97-va!AS97))</f>
@@ -72138,7 +72642,7 @@
       </c>
       <c r="AR102" s="16">
         <f>MAX(0,(va!AS98-va!AR98))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AS102" s="16">
         <f>MAX(0,(va!AT98-va!AS98))</f>
@@ -72420,7 +72924,7 @@
       </c>
       <c r="AR103" s="16">
         <f>MAX(0,(va!AS99-va!AR99))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AS103" s="16">
         <f>MAX(0,(va!AT99-va!AS99))</f>
@@ -72702,7 +73206,7 @@
       </c>
       <c r="AR104" s="16">
         <f>MAX(0,(va!AS100-va!AR100))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS104" s="16">
         <f>MAX(0,(va!AT100-va!AS100))</f>
@@ -73266,7 +73770,7 @@
       </c>
       <c r="AR106" s="16">
         <f>MAX(0,(va!AS102-va!AR102))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AS106" s="16">
         <f>MAX(0,(va!AT102-va!AS102))</f>
@@ -73548,7 +74052,7 @@
       </c>
       <c r="AR107" s="16">
         <f>MAX(0,(va!AS103-va!AR103))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AS107" s="16">
         <f>MAX(0,(va!AT103-va!AS103))</f>
@@ -73830,7 +74334,7 @@
       </c>
       <c r="AR108" s="16">
         <f>MAX(0,(va!AS104-va!AR104))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AS108" s="16">
         <f>MAX(0,(va!AT104-va!AS104))</f>
@@ -74112,7 +74616,7 @@
       </c>
       <c r="AR109" s="16">
         <f>MAX(0,(va!AS105-va!AR105))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS109" s="16">
         <f>MAX(0,(va!AT105-va!AS105))</f>
@@ -74394,7 +74898,7 @@
       </c>
       <c r="AR110" s="16">
         <f>MAX(0,(va!AS106-va!AR106))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AS110" s="16">
         <f>MAX(0,(va!AT106-va!AS106))</f>
@@ -74676,7 +75180,7 @@
       </c>
       <c r="AR111" s="16">
         <f>MAX(0,(va!AS107-va!AR107))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS111" s="16">
         <f>MAX(0,(va!AT107-va!AS107))</f>
@@ -74958,7 +75462,7 @@
       </c>
       <c r="AR112" s="16">
         <f>MAX(0,(va!AS108-va!AR108))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS112" s="16">
         <f>MAX(0,(va!AT108-va!AS108))</f>
@@ -75522,7 +76026,7 @@
       </c>
       <c r="AR114" s="16">
         <f>MAX(0,(va!AS110-va!AR110))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AS114" s="16">
         <f>MAX(0,(va!AT110-va!AS110))</f>
@@ -76932,7 +77436,7 @@
       </c>
       <c r="AR119" s="16">
         <f>MAX(0,(va!AS115-va!AR115))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS119" s="16">
         <f>MAX(0,(va!AT115-va!AS115))</f>
@@ -77496,7 +78000,7 @@
       </c>
       <c r="AR121" s="16">
         <f>MAX(0,(va!AS117-va!AR117))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS121" s="16">
         <f>MAX(0,(va!AT117-va!AS117))</f>
@@ -77778,7 +78282,7 @@
       </c>
       <c r="AR122" s="16">
         <f>MAX(0,(va!AS118-va!AR118))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS122" s="16">
         <f>MAX(0,(va!AT118-va!AS118))</f>
@@ -78060,7 +78564,7 @@
       </c>
       <c r="AR123" s="16">
         <f>MAX(0,(va!AS119-va!AR119))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS123" s="16">
         <f>MAX(0,(va!AT119-va!AS119))</f>
@@ -78624,7 +79128,7 @@
       </c>
       <c r="AR125" s="16">
         <f>MAX(0,(va!AS121-va!AR121))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS125" s="16">
         <f>MAX(0,(va!AT121-va!AS121))</f>
@@ -78906,7 +79410,7 @@
       </c>
       <c r="AR126" s="16">
         <f>MAX(0,(va!AS122-va!AR122))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS126" s="16">
         <f>MAX(0,(va!AT122-va!AS122))</f>
@@ -79752,7 +80256,7 @@
       </c>
       <c r="AR129" s="16">
         <f>MAX(0,(va!AS125-va!AR125))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS129" s="16">
         <f>MAX(0,(va!AT125-va!AS125))</f>
@@ -81162,7 +81666,7 @@
       </c>
       <c r="AR134" s="16">
         <f>MAX(0,(va!AS130-va!AR130))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS134" s="16">
         <f>MAX(0,(va!AT130-va!AS130))</f>
@@ -81444,7 +81948,7 @@
       </c>
       <c r="AR135" s="16">
         <f>MAX(0,(va!AS131-va!AR131))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AS135" s="16">
         <f>MAX(0,(va!AT131-va!AS131))</f>

</xml_diff>

<commit_message>
05 May data update
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7056E4-E093-4102-9333-1744044A8B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDBBC4D-634A-4384-9C39-51773A78137E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
+    <workbookView xWindow="5400" yWindow="4020" windowWidth="16200" windowHeight="9480" tabRatio="685" xr2:uid="{00D9CD8D-2A36-4016-83EC-C5F4A2780280}"/>
   </bookViews>
   <sheets>
     <sheet name="dc" sheetId="8" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4194,6 +4194,9 @@
       <c r="BA2" s="12">
         <v>23795</v>
       </c>
+      <c r="BB2" s="12">
+        <v>24329</v>
+      </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4394,7 +4397,7 @@
       </c>
       <c r="BB3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5322</v>
       </c>
       <c r="BC3" s="10">
         <f t="shared" si="0"/>
@@ -4670,6 +4673,9 @@
       <c r="BA5" s="10">
         <v>258</v>
       </c>
+      <c r="BB5" s="10">
+        <v>264</v>
+      </c>
     </row>
     <row r="6" spans="1:81" ht="39.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5076,6 +5082,9 @@
       <c r="BA7" s="10">
         <v>668</v>
       </c>
+      <c r="BB7" s="10">
+        <v>694</v>
+      </c>
     </row>
     <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -5236,6 +5245,9 @@
       </c>
       <c r="BA8" s="10">
         <v>333</v>
+      </c>
+      <c r="BB8" s="10">
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
@@ -5398,6 +5410,9 @@
       <c r="BA9" s="10">
         <v>314</v>
       </c>
+      <c r="BB9" s="10">
+        <v>317</v>
+      </c>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -5559,6 +5574,9 @@
       <c r="BA10" s="10">
         <v>980</v>
       </c>
+      <c r="BB10" s="10">
+        <v>1009</v>
+      </c>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
@@ -5720,6 +5738,9 @@
       <c r="BA11" s="10">
         <v>799</v>
       </c>
+      <c r="BB11" s="10">
+        <v>819</v>
+      </c>
     </row>
     <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -5881,6 +5902,9 @@
       <c r="BA12" s="10">
         <v>499</v>
       </c>
+      <c r="BB12" s="10">
+        <v>525</v>
+      </c>
     </row>
     <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -6042,6 +6066,9 @@
       <c r="BA13" s="10">
         <v>769</v>
       </c>
+      <c r="BB13" s="10">
+        <v>791</v>
+      </c>
     </row>
     <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6203,6 +6230,9 @@
       <c r="BA14" s="10">
         <v>737</v>
       </c>
+      <c r="BB14" s="10">
+        <v>751</v>
+      </c>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -6362,6 +6392,9 @@
         <v>79</v>
       </c>
       <c r="BA15" s="10">
+        <v>71</v>
+      </c>
+      <c r="BB15" s="10">
         <v>71</v>
       </c>
     </row>
@@ -6617,7 +6650,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
+      <selection pane="bottomRight" activeCell="AQ3" sqref="AQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6761,7 +6794,7 @@
         <v>110587</v>
       </c>
       <c r="AQ2" s="10">
-        <v>0</v>
+        <v>112986</v>
       </c>
       <c r="AR2" s="10">
         <v>0</v>
@@ -7007,7 +7040,7 @@
       </c>
       <c r="AQ3" s="10">
         <f>SUM(md[5-May])</f>
-        <v>0</v>
+        <v>27117</v>
       </c>
       <c r="AR3" s="10">
         <f>SUM(md[6-May])</f>
@@ -7239,7 +7272,7 @@
         <v>5199</v>
       </c>
       <c r="AQ4" s="10">
-        <v>0</v>
+        <v>5337</v>
       </c>
       <c r="AR4" s="10">
         <v>0</v>
@@ -7445,7 +7478,7 @@
         <v>1216</v>
       </c>
       <c r="AQ5" s="10">
-        <v>0</v>
+        <v>1290</v>
       </c>
       <c r="AR5" s="10">
         <v>0</v>
@@ -7862,6 +7895,9 @@
       <c r="AP7">
         <v>126</v>
       </c>
+      <c r="AQ7">
+        <v>129</v>
+      </c>
     </row>
     <row r="8" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -7990,6 +8026,9 @@
       <c r="AP8" s="10">
         <v>2018</v>
       </c>
+      <c r="AQ8" s="10">
+        <v>2045</v>
+      </c>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -8118,6 +8157,9 @@
       <c r="AP9">
         <v>2411</v>
       </c>
+      <c r="AQ9">
+        <v>2609</v>
+      </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -8246,6 +8288,9 @@
       <c r="AP10">
         <v>3448</v>
       </c>
+      <c r="AQ10">
+        <v>3430</v>
+      </c>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -8374,6 +8419,9 @@
       <c r="AP11">
         <v>171</v>
       </c>
+      <c r="AQ11">
+        <v>174</v>
+      </c>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -8502,6 +8550,9 @@
       <c r="AP12">
         <v>98</v>
       </c>
+      <c r="AQ12">
+        <v>99</v>
+      </c>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -8630,6 +8681,9 @@
       <c r="AP13">
         <v>506</v>
       </c>
+      <c r="AQ13">
+        <v>513</v>
+      </c>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -8758,6 +8812,9 @@
       <c r="AP14">
         <v>194</v>
       </c>
+      <c r="AQ14">
+        <v>195</v>
+      </c>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -8886,6 +8943,9 @@
       <c r="AP15">
         <v>651</v>
       </c>
+      <c r="AQ15">
+        <v>660</v>
+      </c>
     </row>
     <row r="16" spans="1:69" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -9014,8 +9074,11 @@
       <c r="AP16" s="10">
         <v>75</v>
       </c>
+      <c r="AQ16" s="10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -9142,8 +9205,11 @@
       <c r="AP17">
         <v>1038</v>
       </c>
+      <c r="AQ17">
+        <v>1071</v>
+      </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -9270,8 +9336,11 @@
       <c r="AP18">
         <v>4</v>
       </c>
+      <c r="AQ18">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -9398,8 +9467,11 @@
       <c r="AP19">
         <v>491</v>
       </c>
+      <c r="AQ19">
+        <v>499</v>
+      </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -9526,8 +9598,11 @@
       <c r="AP20">
         <v>992</v>
       </c>
+      <c r="AQ20">
+        <v>1010</v>
+      </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>170</v>
       </c>
@@ -9654,8 +9729,11 @@
       <c r="AP21">
         <v>95</v>
       </c>
+      <c r="AQ21">
+        <v>95</v>
+      </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -9782,8 +9860,11 @@
       <c r="AP22">
         <v>5384</v>
       </c>
+      <c r="AQ22">
+        <v>5541</v>
+      </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -9910,8 +9991,11 @@
       <c r="AP23">
         <v>7598</v>
       </c>
+      <c r="AQ23">
+        <v>7831</v>
+      </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -10038,8 +10122,11 @@
       <c r="AP24">
         <v>63</v>
       </c>
+      <c r="AQ24">
+        <v>65</v>
+      </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -10166,8 +10253,11 @@
       <c r="AP25">
         <v>168</v>
       </c>
+      <c r="AQ25">
+        <v>170</v>
+      </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -10294,8 +10384,11 @@
       <c r="AP26">
         <v>35</v>
       </c>
+      <c r="AQ26">
+        <v>37</v>
+      </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>175</v>
       </c>
@@ -10422,8 +10515,11 @@
       <c r="AP27">
         <v>45</v>
       </c>
+      <c r="AQ27">
+        <v>45</v>
+      </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -10550,8 +10646,11 @@
       <c r="AP28">
         <v>237</v>
       </c>
+      <c r="AQ28">
+        <v>238</v>
+      </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>176</v>
       </c>
@@ -10678,8 +10777,11 @@
       <c r="AP29">
         <v>480</v>
       </c>
+      <c r="AQ29">
+        <v>500</v>
+      </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>177</v>
       </c>
@@ -10806,8 +10908,11 @@
       <c r="AP30">
         <v>80</v>
       </c>
+      <c r="AQ30">
+        <v>81</v>
+      </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
@@ -10901,10 +11006,10 @@
   <dimension ref="A1:BT139"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AD6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="AH6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11098,7 +11203,7 @@
       </c>
       <c r="AT2" s="10">
         <f>SUM(va[5-May])</f>
-        <v>0</v>
+        <v>20256</v>
       </c>
       <c r="AU2" s="10">
         <f>SUM(va[6-May])</f>
@@ -11333,7 +11438,7 @@
         <v>2700</v>
       </c>
       <c r="AT3" s="10">
-        <v>0</v>
+        <v>2773</v>
       </c>
       <c r="AU3" s="10">
         <v>0</v>
@@ -11542,7 +11647,7 @@
         <v>684</v>
       </c>
       <c r="AT4" s="10">
-        <v>0</v>
+        <v>713</v>
       </c>
       <c r="AU4" s="10">
         <v>0</v>
@@ -11751,7 +11856,7 @@
         <v>122788</v>
       </c>
       <c r="AT5" s="10">
-        <v>0</v>
+        <v>127938</v>
       </c>
       <c r="AU5" s="10">
         <v>0</v>
@@ -12186,9 +12291,12 @@
       <c r="AS7" s="10">
         <v>940</v>
       </c>
+      <c r="AT7" s="10">
+        <v>983</v>
+      </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -12323,9 +12431,12 @@
       <c r="AS8" s="10">
         <v>6</v>
       </c>
+      <c r="AT8" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
@@ -12458,9 +12569,12 @@
       <c r="AS9" s="10">
         <v>28</v>
       </c>
+      <c r="AT9" s="10">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
@@ -12593,9 +12707,12 @@
       <c r="AS10" s="10">
         <v>3</v>
       </c>
+      <c r="AT10" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>122</v>
       </c>
@@ -12728,9 +12845,12 @@
       <c r="AS11" s="10">
         <v>57</v>
       </c>
+      <c r="AT11" s="10">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>136</v>
       </c>
@@ -12863,9 +12983,12 @@
       <c r="AS12" s="10">
         <v>0</v>
       </c>
+      <c r="AT12" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
@@ -12997,6 +13120,9 @@
       </c>
       <c r="AS13" s="10">
         <v>27</v>
+      </c>
+      <c r="AT13" s="10">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
@@ -13135,9 +13261,12 @@
       <c r="AS14" s="10">
         <v>1139</v>
       </c>
+      <c r="AT14" s="10">
+        <v>1169</v>
+      </c>
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -13272,9 +13401,12 @@
       <c r="AS15" s="10">
         <v>47</v>
       </c>
+      <c r="AT15" s="10">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
@@ -13407,9 +13539,12 @@
       <c r="AS16" s="10">
         <v>0</v>
       </c>
+      <c r="AT16" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
@@ -13542,9 +13677,12 @@
       <c r="AS17" s="10">
         <v>2</v>
       </c>
+      <c r="AT17" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
@@ -13677,9 +13815,12 @@
       <c r="AS18" s="10">
         <v>7</v>
       </c>
+      <c r="AT18" s="10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -13812,9 +13953,12 @@
       <c r="AS19" s="10">
         <v>269</v>
       </c>
+      <c r="AT19" s="10">
+        <v>282</v>
+      </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>133</v>
       </c>
@@ -13947,9 +14091,12 @@
       <c r="AS20" s="10">
         <v>6</v>
       </c>
+      <c r="AT20" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
@@ -14082,9 +14229,12 @@
       <c r="AS21" s="10">
         <v>497</v>
       </c>
+      <c r="AT21" s="10">
+        <v>525</v>
+      </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
@@ -14217,9 +14367,12 @@
       <c r="AS22" s="10">
         <v>6</v>
       </c>
+      <c r="AT22" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>154</v>
       </c>
@@ -14352,9 +14505,12 @@
       <c r="AS23" s="10">
         <v>13</v>
       </c>
+      <c r="AT23" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -14487,9 +14643,12 @@
       <c r="AS24" s="10">
         <v>14</v>
       </c>
+      <c r="AT24" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -14624,9 +14783,12 @@
       <c r="AS25" s="10">
         <v>14</v>
       </c>
+      <c r="AT25" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -14759,9 +14921,12 @@
       <c r="AS26" s="10">
         <v>21</v>
       </c>
+      <c r="AT26" s="10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -14894,9 +15059,12 @@
       <c r="AS27" s="10">
         <v>35</v>
       </c>
+      <c r="AT27" s="10">
+        <v>36</v>
+      </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
@@ -15029,9 +15197,12 @@
       <c r="AS28" s="10">
         <v>13</v>
       </c>
+      <c r="AT28" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -15164,8 +15335,11 @@
       <c r="AS29" s="10">
         <v>64</v>
       </c>
+      <c r="AT29" s="10">
+        <v>65</v>
+      </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>78</v>
       </c>
@@ -15301,9 +15475,12 @@
       <c r="AS30" s="10">
         <v>284</v>
       </c>
+      <c r="AT30" s="10">
+        <v>293</v>
+      </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25"